<commit_message>
#8 Time Tracking.xlsx: updated to mid-September 2023.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="709" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="870" uniqueCount="356">
   <si>
     <t>Year</t>
   </si>
@@ -987,10 +987,109 @@
     <t>2023-08-18</t>
   </si>
   <si>
-    <t>nwtimetrackingmanager</t>
-  </si>
-  <si>
     <t>IsReleaseDate</t>
+  </si>
+  <si>
+    <t>2023-08-21</t>
+  </si>
+  <si>
+    <t>2023-08-22</t>
+  </si>
+  <si>
+    <t>2023-08-28</t>
+  </si>
+  <si>
+    <t>08:00</t>
+  </si>
+  <si>
+    <t>08:30</t>
+  </si>
+  <si>
+    <t>2023-08-29</t>
+  </si>
+  <si>
+    <t>08:20</t>
+  </si>
+  <si>
+    <t>08:35</t>
+  </si>
+  <si>
+    <t>0h 15m</t>
+  </si>
+  <si>
+    <t>2023-08-30</t>
+  </si>
+  <si>
+    <t>08:15</t>
+  </si>
+  <si>
+    <t>2023-08-31</t>
+  </si>
+  <si>
+    <t>18:15</t>
+  </si>
+  <si>
+    <t>md-numbworks.</t>
+  </si>
+  <si>
+    <t>2023-09-01</t>
+  </si>
+  <si>
+    <t>2023-09-02</t>
+  </si>
+  <si>
+    <t>2023-09-04</t>
+  </si>
+  <si>
+    <t>08:05</t>
+  </si>
+  <si>
+    <t>2023-09-05</t>
+  </si>
+  <si>
+    <t>2023-09-06</t>
+  </si>
+  <si>
+    <t>2023-09-07</t>
+  </si>
+  <si>
+    <t>2023-09-08</t>
+  </si>
+  <si>
+    <t>08:10</t>
+  </si>
+  <si>
+    <t>08:40</t>
+  </si>
+  <si>
+    <t>2023-09-11</t>
+  </si>
+  <si>
+    <t>08:45</t>
+  </si>
+  <si>
+    <t>2023-09-12</t>
+  </si>
+  <si>
+    <t>17:45</t>
+  </si>
+  <si>
+    <t>2023-09-13</t>
+  </si>
+  <si>
+    <t>2023-09-14</t>
+  </si>
+  <si>
+    <t>2023-09-15</t>
+  </si>
+  <si>
+    <t>22:45</t>
+  </si>
+  <si>
+    <t>4h 45m</t>
+  </si>
+  <si>
+    <t>v1.5.0</t>
   </si>
 </sst>
 </file>
@@ -1387,10 +1486,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K167"/>
+  <dimension ref="A1:K197"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+    <sheetView tabSelected="1" topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="F170" sqref="F170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -1435,7 +1534,7 @@
         <v>11</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>0</v>
@@ -4990,11 +5089,11 @@
         <v>4</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" ref="J131:J152" si="4">YEAR(A131)</f>
+        <f t="shared" ref="J131:J178" si="4">YEAR(A131)</f>
         <v>2023</v>
       </c>
       <c r="K131" s="4">
-        <f t="shared" ref="K131:K152" si="5">MONTH(A131)</f>
+        <f t="shared" ref="K131:K178" si="5">MONTH(A131)</f>
         <v>7</v>
       </c>
     </row>
@@ -5692,7 +5791,7 @@
       </c>
       <c r="F152" s="3"/>
       <c r="G152" s="3" t="s">
-        <v>321</v>
+        <v>282</v>
       </c>
       <c r="H152" s="3" t="s">
         <v>228</v>
@@ -5710,199 +5809,1067 @@
       </c>
     </row>
     <row r="153" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A153" s="3"/>
-      <c r="B153" s="3"/>
-      <c r="C153" s="3"/>
-      <c r="D153" s="3"/>
-      <c r="E153" s="3"/>
+      <c r="A153" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B153" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="D153" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E153" s="3" t="s">
+        <v>196</v>
+      </c>
       <c r="F153" s="3"/>
-      <c r="G153" s="3"/>
-      <c r="H153" s="3"/>
-      <c r="I153" s="3"/>
-      <c r="J153" s="4"/>
-      <c r="K153" s="4"/>
+      <c r="G153" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H153" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="I153" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="J153" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K153" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="154" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A154" s="3"/>
-      <c r="B154" s="3"/>
-      <c r="C154" s="3"/>
-      <c r="D154" s="3"/>
-      <c r="E154" s="3"/>
-      <c r="F154" s="3"/>
+      <c r="A154" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="B154" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D154" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E154" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G154" s="3"/>
       <c r="H154" s="3"/>
       <c r="I154" s="3"/>
-      <c r="J154" s="4"/>
-      <c r="K154" s="4"/>
+      <c r="J154" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K154" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="155" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A155" s="3"/>
-      <c r="B155" s="3"/>
-      <c r="C155" s="3"/>
-      <c r="D155" s="3"/>
-      <c r="E155" s="3"/>
-      <c r="F155" s="3"/>
+      <c r="A155" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B155" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D155" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E155" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F155" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G155" s="3"/>
       <c r="H155" s="3"/>
       <c r="I155" s="3"/>
-      <c r="J155" s="4"/>
-      <c r="K155" s="4"/>
+      <c r="J155" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K155" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="156" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A156" s="3"/>
-      <c r="B156" s="3"/>
-      <c r="C156" s="3"/>
-      <c r="D156" s="3"/>
-      <c r="E156" s="3"/>
-      <c r="F156" s="3"/>
+      <c r="A156" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="B156" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D156" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E156" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F156" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G156" s="3"/>
       <c r="H156" s="3"/>
       <c r="I156" s="3"/>
-      <c r="J156" s="4"/>
-      <c r="K156" s="4"/>
+      <c r="J156" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K156" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="157" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A157" s="3"/>
-      <c r="B157" s="3"/>
-      <c r="C157" s="3"/>
-      <c r="D157" s="3"/>
-      <c r="E157" s="3"/>
-      <c r="F157" s="3"/>
+      <c r="A157" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="B157" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D157" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E157" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F157" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G157" s="3"/>
       <c r="H157" s="3"/>
       <c r="I157" s="3"/>
-      <c r="J157" s="4"/>
-      <c r="K157" s="4"/>
+      <c r="J157" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K157" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="158" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A158" s="3"/>
-      <c r="B158" s="3"/>
-      <c r="C158" s="3"/>
-      <c r="D158" s="3"/>
-      <c r="E158" s="3"/>
-      <c r="F158" s="3"/>
+      <c r="A158" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B158" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D158" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E158" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F158" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G158" s="3"/>
       <c r="H158" s="3"/>
       <c r="I158" s="3"/>
-      <c r="J158" s="4"/>
-      <c r="K158" s="4"/>
+      <c r="J158" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K158" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="159" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A159" s="3"/>
-      <c r="B159" s="3"/>
-      <c r="C159" s="3"/>
-      <c r="D159" s="3"/>
-      <c r="E159" s="3"/>
-      <c r="F159" s="3"/>
+      <c r="A159" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="B159" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D159" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E159" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F159" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G159" s="3"/>
       <c r="H159" s="3"/>
       <c r="I159" s="3"/>
-      <c r="J159" s="4"/>
-      <c r="K159" s="4"/>
+      <c r="J159" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K159" s="4">
+        <f t="shared" si="5"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="160" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A160" s="3"/>
-      <c r="B160" s="3"/>
-      <c r="C160" s="3"/>
-      <c r="D160" s="3"/>
-      <c r="E160" s="3"/>
-      <c r="F160" s="3"/>
+      <c r="A160" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B160" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>247</v>
+      </c>
+      <c r="D160" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E160" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>335</v>
+      </c>
       <c r="G160" s="3"/>
       <c r="H160" s="3"/>
       <c r="I160" s="3"/>
-      <c r="J160" s="4"/>
-      <c r="K160" s="4"/>
+      <c r="J160" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K160" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="161" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A161" s="3"/>
-      <c r="B161" s="3"/>
-      <c r="C161" s="3"/>
-      <c r="D161" s="3"/>
-      <c r="E161" s="3"/>
-      <c r="F161" s="3"/>
+      <c r="A161" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="D161" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E161" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F161" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G161" s="3"/>
       <c r="H161" s="3"/>
       <c r="I161" s="3"/>
-      <c r="J161" s="4"/>
-      <c r="K161" s="4"/>
+      <c r="J161" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K161" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="162" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A162" s="3"/>
-      <c r="B162" s="3"/>
-      <c r="C162" s="3"/>
-      <c r="D162" s="3"/>
-      <c r="E162" s="3"/>
-      <c r="F162" s="3"/>
+      <c r="A162" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B162" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D162" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E162" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F162" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G162" s="3"/>
       <c r="H162" s="3"/>
       <c r="I162" s="3"/>
-      <c r="J162" s="4"/>
-      <c r="K162" s="4"/>
+      <c r="J162" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K162" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="163" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A163" s="3"/>
-      <c r="B163" s="3"/>
-      <c r="C163" s="3"/>
-      <c r="D163" s="3"/>
-      <c r="E163" s="3"/>
-      <c r="F163" s="3"/>
+      <c r="A163" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="B163" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D163" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E163" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F163" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G163" s="3"/>
       <c r="H163" s="3"/>
       <c r="I163" s="3"/>
-      <c r="J163" s="4"/>
-      <c r="K163" s="4"/>
+      <c r="J163" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K163" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="164" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A164" s="3"/>
-      <c r="B164" s="3"/>
-      <c r="C164" s="3"/>
-      <c r="D164" s="3"/>
-      <c r="E164" s="3"/>
-      <c r="F164" s="3"/>
+      <c r="A164" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="B164" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D164" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E164" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F164" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G164" s="3"/>
       <c r="H164" s="3"/>
       <c r="I164" s="3"/>
-      <c r="J164" s="4"/>
-      <c r="K164" s="4"/>
+      <c r="J164" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K164" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="165" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A165" s="3"/>
-      <c r="B165" s="3"/>
-      <c r="C165" s="3"/>
-      <c r="D165" s="3"/>
-      <c r="E165" s="3"/>
-      <c r="F165" s="3"/>
+      <c r="A165" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B165" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D165" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E165" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F165" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G165" s="3"/>
       <c r="H165" s="3"/>
       <c r="I165" s="3"/>
-      <c r="J165" s="4"/>
-      <c r="K165" s="4"/>
+      <c r="J165" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K165" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="166" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A166" s="3"/>
-      <c r="B166" s="3"/>
-      <c r="C166" s="3"/>
-      <c r="D166" s="3"/>
-      <c r="E166" s="3"/>
-      <c r="F166" s="3"/>
+      <c r="A166" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="B166" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D166" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="E166" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F166" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G166" s="3"/>
       <c r="H166" s="3"/>
       <c r="I166" s="3"/>
-      <c r="J166" s="4"/>
-      <c r="K166" s="4"/>
+      <c r="J166" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K166" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="167" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A167" s="3"/>
-      <c r="B167" s="3"/>
-      <c r="C167" s="3"/>
-      <c r="D167" s="3"/>
-      <c r="E167" s="3"/>
-      <c r="F167" s="3"/>
+      <c r="A167" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B167" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D167" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E167" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F167" s="3" t="s">
+        <v>261</v>
+      </c>
       <c r="G167" s="3"/>
       <c r="H167" s="3"/>
       <c r="I167" s="3"/>
-      <c r="J167" s="4"/>
-      <c r="K167" s="4"/>
+      <c r="J167" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K167" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="B168" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D168" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E168" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F168" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G168" s="3"/>
+      <c r="H168" s="3"/>
+      <c r="I168" s="3"/>
+      <c r="J168" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K168" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>343</v>
+      </c>
+      <c r="B169" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="D169" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E169" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F169" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G169" s="3"/>
+      <c r="H169" s="3"/>
+      <c r="I169" s="3"/>
+      <c r="J169" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K169" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A170" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B170" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="D170" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E170" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F170" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G170" s="3"/>
+      <c r="H170" s="3"/>
+      <c r="I170" s="3"/>
+      <c r="J170" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K170" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B171" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="D171" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E171" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F171" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G171" s="3"/>
+      <c r="H171" s="3"/>
+      <c r="I171" s="3"/>
+      <c r="J171" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K171" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B172" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="D172" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E172" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F172" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G172" s="3"/>
+      <c r="H172" s="3"/>
+      <c r="I172" s="3"/>
+      <c r="J172" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K172" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A173" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="B173" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D173" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E173" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F173" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G173" s="3"/>
+      <c r="H173" s="3"/>
+      <c r="I173" s="3"/>
+      <c r="J173" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K173" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B174" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="D174" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="E174" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F174" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G174" s="3"/>
+      <c r="H174" s="3"/>
+      <c r="I174" s="3"/>
+      <c r="J174" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K174" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="B175" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="D175" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="E175" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F175" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="G175" s="3"/>
+      <c r="H175" s="3"/>
+      <c r="I175" s="3"/>
+      <c r="J175" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K175" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="B176" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>349</v>
+      </c>
+      <c r="D176" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E176" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="F176" s="3"/>
+      <c r="G176" s="3"/>
+      <c r="H176" s="3"/>
+      <c r="I176" s="3"/>
+      <c r="J176" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K176" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A177" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C177" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D177" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E177" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F177" s="3"/>
+      <c r="G177" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H177" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I177" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J177" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K177" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A178" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="B178" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C178" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D178" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="E178" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="F178" s="3"/>
+      <c r="G178" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H178" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="I178" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="J178" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="K178" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A179" s="3"/>
+      <c r="B179" s="3"/>
+      <c r="C179" s="3"/>
+      <c r="D179" s="3"/>
+      <c r="E179" s="3"/>
+      <c r="F179" s="3"/>
+      <c r="G179" s="3"/>
+      <c r="H179" s="3"/>
+      <c r="I179" s="3"/>
+      <c r="J179" s="4"/>
+      <c r="K179" s="4"/>
+    </row>
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A180" s="3"/>
+      <c r="B180" s="3"/>
+      <c r="C180" s="3"/>
+      <c r="D180" s="3"/>
+      <c r="E180" s="3"/>
+      <c r="F180" s="3"/>
+      <c r="G180" s="3"/>
+      <c r="H180" s="3"/>
+      <c r="I180" s="3"/>
+      <c r="J180" s="4"/>
+      <c r="K180" s="4"/>
+    </row>
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A181" s="3"/>
+      <c r="B181" s="3"/>
+      <c r="C181" s="3"/>
+      <c r="D181" s="3"/>
+      <c r="E181" s="3"/>
+      <c r="F181" s="3"/>
+      <c r="G181" s="3"/>
+      <c r="H181" s="3"/>
+      <c r="I181" s="3"/>
+      <c r="J181" s="4"/>
+      <c r="K181" s="4"/>
+    </row>
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A182" s="3"/>
+      <c r="B182" s="3"/>
+      <c r="C182" s="3"/>
+      <c r="D182" s="3"/>
+      <c r="E182" s="3"/>
+      <c r="F182" s="3"/>
+      <c r="G182" s="3"/>
+      <c r="H182" s="3"/>
+      <c r="I182" s="3"/>
+      <c r="J182" s="4"/>
+      <c r="K182" s="4"/>
+    </row>
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A183" s="3"/>
+      <c r="B183" s="3"/>
+      <c r="C183" s="3"/>
+      <c r="D183" s="3"/>
+      <c r="E183" s="3"/>
+      <c r="F183" s="3"/>
+      <c r="G183" s="3"/>
+      <c r="H183" s="3"/>
+      <c r="I183" s="3"/>
+      <c r="J183" s="4"/>
+      <c r="K183" s="4"/>
+    </row>
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A184" s="3"/>
+      <c r="B184" s="3"/>
+      <c r="C184" s="3"/>
+      <c r="D184" s="3"/>
+      <c r="E184" s="3"/>
+      <c r="F184" s="3"/>
+      <c r="G184" s="3"/>
+      <c r="H184" s="3"/>
+      <c r="I184" s="3"/>
+      <c r="J184" s="4"/>
+      <c r="K184" s="4"/>
+    </row>
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A185" s="3"/>
+      <c r="B185" s="3"/>
+      <c r="C185" s="3"/>
+      <c r="D185" s="3"/>
+      <c r="E185" s="3"/>
+      <c r="F185" s="3"/>
+      <c r="G185" s="3"/>
+      <c r="H185" s="3"/>
+      <c r="I185" s="3"/>
+      <c r="J185" s="4"/>
+      <c r="K185" s="4"/>
+    </row>
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A186" s="3"/>
+      <c r="B186" s="3"/>
+      <c r="C186" s="3"/>
+      <c r="D186" s="3"/>
+      <c r="E186" s="3"/>
+      <c r="F186" s="3"/>
+      <c r="G186" s="3"/>
+      <c r="H186" s="3"/>
+      <c r="I186" s="3"/>
+      <c r="J186" s="4"/>
+      <c r="K186" s="4"/>
+    </row>
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A187" s="3"/>
+      <c r="B187" s="3"/>
+      <c r="C187" s="3"/>
+      <c r="D187" s="3"/>
+      <c r="E187" s="3"/>
+      <c r="F187" s="3"/>
+      <c r="G187" s="3"/>
+      <c r="H187" s="3"/>
+      <c r="I187" s="3"/>
+      <c r="J187" s="4"/>
+      <c r="K187" s="4"/>
+    </row>
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A188" s="3"/>
+      <c r="B188" s="3"/>
+      <c r="C188" s="3"/>
+      <c r="D188" s="3"/>
+      <c r="E188" s="3"/>
+      <c r="F188" s="3"/>
+      <c r="G188" s="3"/>
+      <c r="H188" s="3"/>
+      <c r="I188" s="3"/>
+      <c r="J188" s="4"/>
+      <c r="K188" s="4"/>
+    </row>
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A189" s="3"/>
+      <c r="B189" s="3"/>
+      <c r="C189" s="3"/>
+      <c r="D189" s="3"/>
+      <c r="E189" s="3"/>
+      <c r="F189" s="3"/>
+      <c r="G189" s="3"/>
+      <c r="H189" s="3"/>
+      <c r="I189" s="3"/>
+      <c r="J189" s="4"/>
+      <c r="K189" s="4"/>
+    </row>
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A190" s="3"/>
+      <c r="B190" s="3"/>
+      <c r="C190" s="3"/>
+      <c r="D190" s="3"/>
+      <c r="E190" s="3"/>
+      <c r="F190" s="3"/>
+      <c r="G190" s="3"/>
+      <c r="H190" s="3"/>
+      <c r="I190" s="3"/>
+      <c r="J190" s="4"/>
+      <c r="K190" s="4"/>
+    </row>
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A191" s="3"/>
+      <c r="B191" s="3"/>
+      <c r="C191" s="3"/>
+      <c r="D191" s="3"/>
+      <c r="E191" s="3"/>
+      <c r="F191" s="3"/>
+      <c r="G191" s="3"/>
+      <c r="H191" s="3"/>
+      <c r="I191" s="3"/>
+      <c r="J191" s="4"/>
+      <c r="K191" s="4"/>
+    </row>
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A192" s="3"/>
+      <c r="B192" s="3"/>
+      <c r="C192" s="3"/>
+      <c r="D192" s="3"/>
+      <c r="E192" s="3"/>
+      <c r="F192" s="3"/>
+      <c r="G192" s="3"/>
+      <c r="H192" s="3"/>
+      <c r="I192" s="3"/>
+      <c r="J192" s="4"/>
+      <c r="K192" s="4"/>
+    </row>
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A193" s="3"/>
+      <c r="B193" s="3"/>
+      <c r="C193" s="3"/>
+      <c r="D193" s="3"/>
+      <c r="E193" s="3"/>
+      <c r="F193" s="3"/>
+      <c r="G193" s="3"/>
+      <c r="H193" s="3"/>
+      <c r="I193" s="3"/>
+      <c r="J193" s="4"/>
+      <c r="K193" s="4"/>
+    </row>
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A194" s="3"/>
+      <c r="B194" s="3"/>
+      <c r="C194" s="3"/>
+      <c r="D194" s="3"/>
+      <c r="E194" s="3"/>
+      <c r="F194" s="3"/>
+      <c r="G194" s="3"/>
+      <c r="H194" s="3"/>
+      <c r="I194" s="3"/>
+      <c r="J194" s="4"/>
+      <c r="K194" s="4"/>
+    </row>
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A195" s="3"/>
+      <c r="B195" s="3"/>
+      <c r="C195" s="3"/>
+      <c r="D195" s="3"/>
+      <c r="E195" s="3"/>
+      <c r="F195" s="3"/>
+      <c r="G195" s="3"/>
+      <c r="H195" s="3"/>
+      <c r="I195" s="3"/>
+      <c r="J195" s="4"/>
+      <c r="K195" s="4"/>
+    </row>
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A196" s="3"/>
+      <c r="B196" s="3"/>
+      <c r="C196" s="3"/>
+      <c r="D196" s="3"/>
+      <c r="E196" s="3"/>
+      <c r="F196" s="3"/>
+      <c r="G196" s="3"/>
+      <c r="H196" s="3"/>
+      <c r="I196" s="3"/>
+      <c r="J196" s="4"/>
+      <c r="K196" s="4"/>
+    </row>
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A197" s="3"/>
+      <c r="B197" s="3"/>
+      <c r="C197" s="3"/>
+      <c r="D197" s="3"/>
+      <c r="E197" s="3"/>
+      <c r="F197" s="3"/>
+      <c r="G197" s="3"/>
+      <c r="H197" s="3"/>
+      <c r="I197" s="3"/>
+      <c r="J197" s="4"/>
+      <c r="K197" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#8 Time Tracking.xlsx: updated to 2023-09-28.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1155" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="364">
   <si>
     <t>Year</t>
   </si>
@@ -1081,6 +1081,39 @@
   </si>
   <si>
     <t>False</t>
+  </si>
+  <si>
+    <t>2023-09-19</t>
+  </si>
+  <si>
+    <t>2023-09-20</t>
+  </si>
+  <si>
+    <t>2023-09-21</t>
+  </si>
+  <si>
+    <t>2023-09-22</t>
+  </si>
+  <si>
+    <t>21:45</t>
+  </si>
+  <si>
+    <t>2023-09-23</t>
+  </si>
+  <si>
+    <t>10:15</t>
+  </si>
+  <si>
+    <t>13:15</t>
+  </si>
+  <si>
+    <t>2023-09-27</t>
+  </si>
+  <si>
+    <t>nwtimetrackingmanager v1.0.0</t>
+  </si>
+  <si>
+    <t>2023-09-28</t>
   </si>
 </sst>
 </file>
@@ -1483,8 +1516,8 @@
   <dimension ref="A1:J197"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H175" sqref="H175"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E177" sqref="E177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5406,11 +5439,11 @@
         <v>352</v>
       </c>
       <c r="I131" s="4">
-        <f t="shared" ref="I131:I178" si="4">YEAR(A131)</f>
+        <f t="shared" ref="I131:I187" si="4">YEAR(A131)</f>
         <v>2023</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" ref="J131:J178" si="5">MONTH(A131)</f>
+        <f t="shared" ref="J131:J187" si="5">MONTH(A131)</f>
         <v>7</v>
       </c>
     </row>
@@ -7011,112 +7044,310 @@
       </c>
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A179" s="3"/>
-      <c r="B179" s="3"/>
-      <c r="C179" s="3"/>
-      <c r="D179" s="3"/>
-      <c r="E179" s="3"/>
-      <c r="F179" s="3"/>
-      <c r="G179" s="3"/>
-      <c r="H179" s="3"/>
-      <c r="I179" s="4"/>
-      <c r="J179" s="4"/>
+      <c r="A179" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="B179" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C179" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D179" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F179" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G179" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H179" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I179" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J179" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A180" s="3"/>
-      <c r="B180" s="3"/>
-      <c r="C180" s="3"/>
-      <c r="D180" s="3"/>
-      <c r="E180" s="3"/>
-      <c r="F180" s="3"/>
-      <c r="G180" s="3"/>
-      <c r="H180" s="3"/>
-      <c r="I180" s="4"/>
-      <c r="J180" s="4"/>
+      <c r="A180" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="B180" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C180" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D180" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E180" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F180" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G180" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H180" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I180" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J180" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A181" s="3"/>
-      <c r="B181" s="3"/>
-      <c r="C181" s="3"/>
-      <c r="D181" s="3"/>
-      <c r="E181" s="3"/>
-      <c r="F181" s="3"/>
-      <c r="G181" s="3"/>
-      <c r="H181" s="3"/>
-      <c r="I181" s="4"/>
-      <c r="J181" s="4"/>
+      <c r="A181" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B181" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="C181" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D181" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="E181" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F181" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G181" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H181" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I181" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J181" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A182" s="3"/>
-      <c r="B182" s="3"/>
-      <c r="C182" s="3"/>
-      <c r="D182" s="3"/>
-      <c r="E182" s="3"/>
-      <c r="F182" s="3"/>
-      <c r="G182" s="3"/>
-      <c r="H182" s="3"/>
-      <c r="I182" s="4"/>
-      <c r="J182" s="4"/>
+      <c r="A182" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B182" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="C182" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D182" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E182" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F182" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G182" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H182" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I182" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J182" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A183" s="3"/>
-      <c r="B183" s="3"/>
-      <c r="C183" s="3"/>
-      <c r="D183" s="3"/>
-      <c r="E183" s="3"/>
-      <c r="F183" s="3"/>
-      <c r="G183" s="3"/>
-      <c r="H183" s="3"/>
-      <c r="I183" s="4"/>
-      <c r="J183" s="4"/>
+      <c r="A183" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="B183" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="C183" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="D183" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="E183" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F183" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G183" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H183" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I183" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J183" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A184" s="3"/>
-      <c r="B184" s="3"/>
-      <c r="C184" s="3"/>
-      <c r="D184" s="3"/>
-      <c r="E184" s="3"/>
-      <c r="F184" s="3"/>
-      <c r="G184" s="3"/>
-      <c r="H184" s="3"/>
-      <c r="I184" s="4"/>
-      <c r="J184" s="4"/>
+      <c r="A184" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B184" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C184" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D184" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E184" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F184" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G184" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H184" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I184" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J184" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A185" s="3"/>
-      <c r="B185" s="3"/>
-      <c r="C185" s="3"/>
-      <c r="D185" s="3"/>
-      <c r="E185" s="3"/>
-      <c r="F185" s="3"/>
-      <c r="G185" s="3"/>
-      <c r="H185" s="3"/>
-      <c r="I185" s="4"/>
-      <c r="J185" s="4"/>
+      <c r="A185" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B185" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C185" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D185" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="E185" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F185" s="3" t="s">
+        <v>345</v>
+      </c>
+      <c r="G185" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H185" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I185" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J185" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A186" s="3"/>
-      <c r="B186" s="3"/>
-      <c r="C186" s="3"/>
-      <c r="D186" s="3"/>
-      <c r="E186" s="3"/>
-      <c r="F186" s="3"/>
-      <c r="G186" s="3"/>
-      <c r="H186" s="3"/>
-      <c r="I186" s="4"/>
-      <c r="J186" s="4"/>
+      <c r="A186" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B186" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="C186" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D186" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="E186" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F186" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="G186" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H186" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I186" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J186" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A187" s="3"/>
-      <c r="B187" s="3"/>
-      <c r="C187" s="3"/>
-      <c r="D187" s="3"/>
-      <c r="E187" s="3"/>
-      <c r="F187" s="3"/>
-      <c r="G187" s="3"/>
-      <c r="H187" s="3"/>
-      <c r="I187" s="4"/>
-      <c r="J187" s="4"/>
+      <c r="A187" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B187" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="C187" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="D187" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E187" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F187" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="G187" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="H187" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="I187" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J187" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" s="3"/>

</xml_diff>

<commit_message>
#9 Time Tracking.xlsx: added missing 2023-09-24.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1227" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="366">
   <si>
     <t>Year</t>
   </si>
@@ -1114,6 +1114,12 @@
   </si>
   <si>
     <t>Effort</t>
+  </si>
+  <si>
+    <t>2023-09-24</t>
+  </si>
+  <si>
+    <t>nwreadinglistmanager v1.6.0</t>
   </si>
 </sst>
 </file>
@@ -1513,11 +1519,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J197"/>
+  <dimension ref="A1:J198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A176" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E191" sqref="E191"/>
+      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F192" sqref="F192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5439,11 +5445,11 @@
         <v>351</v>
       </c>
       <c r="I131" s="4">
-        <f t="shared" ref="I131:I187" si="4">YEAR(A131)</f>
+        <f t="shared" ref="I131:I188" si="4">YEAR(A131)</f>
         <v>2023</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" ref="J131:J187" si="5">MONTH(A131)</f>
+        <f t="shared" ref="J131:J188" si="5">MONTH(A131)</f>
         <v>7</v>
       </c>
     </row>
@@ -7283,28 +7289,28 @@
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" s="3" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="B186" s="3" t="s">
-        <v>213</v>
+        <v>224</v>
       </c>
       <c r="C186" s="3" t="s">
-        <v>175</v>
+        <v>260</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>188</v>
+        <v>207</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>190</v>
       </c>
       <c r="F186" s="3" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="G186" s="8" t="s">
         <v>350</v>
       </c>
       <c r="H186" s="8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="I186" s="4">
         <f t="shared" si="4"/>
@@ -7317,16 +7323,16 @@
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B187" s="3" t="s">
-        <v>336</v>
+        <v>213</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>321</v>
+        <v>175</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>257</v>
+        <v>188</v>
       </c>
       <c r="E187" s="3" t="s">
         <v>190</v>
@@ -7350,16 +7356,38 @@
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A188" s="3"/>
-      <c r="B188" s="3"/>
-      <c r="C188" s="3"/>
-      <c r="D188" s="3"/>
-      <c r="E188" s="3"/>
-      <c r="F188" s="3"/>
-      <c r="G188" s="3"/>
-      <c r="H188" s="3"/>
-      <c r="I188" s="4"/>
-      <c r="J188" s="4"/>
+      <c r="A188" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B188" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C188" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="D188" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E188" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F188" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G188" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H188" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I188" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J188" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" s="3"/>
@@ -7469,6 +7497,18 @@
       <c r="I197" s="4"/>
       <c r="J197" s="4"/>
     </row>
+    <row r="198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A198" s="3"/>
+      <c r="B198" s="3"/>
+      <c r="C198" s="3"/>
+      <c r="D198" s="3"/>
+      <c r="E198" s="3"/>
+      <c r="F198" s="3"/>
+      <c r="G198" s="3"/>
+      <c r="H198" s="3"/>
+      <c r="I198" s="4"/>
+      <c r="J198" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#9 Time Tracking.xlsx: added missing 2023-09-29.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="368">
   <si>
     <t>Year</t>
   </si>
@@ -1120,6 +1120,12 @@
   </si>
   <si>
     <t>nwreadinglistmanager v1.6.0</t>
+  </si>
+  <si>
+    <t>2023-09-29</t>
+  </si>
+  <si>
+    <t>03:15</t>
   </si>
 </sst>
 </file>
@@ -1523,7 +1529,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F192" sqref="F192"/>
+      <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5445,11 +5451,11 @@
         <v>351</v>
       </c>
       <c r="I131" s="4">
-        <f t="shared" ref="I131:I188" si="4">YEAR(A131)</f>
+        <f t="shared" ref="I131:I190" si="4">YEAR(A131)</f>
         <v>2023</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" ref="J131:J188" si="5">MONTH(A131)</f>
+        <f t="shared" ref="J131:J190" si="5">MONTH(A131)</f>
         <v>7</v>
       </c>
     </row>
@@ -7390,28 +7396,72 @@
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A189" s="3"/>
-      <c r="B189" s="3"/>
-      <c r="C189" s="3"/>
-      <c r="D189" s="3"/>
-      <c r="E189" s="3"/>
-      <c r="F189" s="3"/>
-      <c r="G189" s="3"/>
-      <c r="H189" s="3"/>
-      <c r="I189" s="4"/>
-      <c r="J189" s="4"/>
+      <c r="A189" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B189" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C189" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D189" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="E189" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F189" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G189" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H189" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I189" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J189" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A190" s="3"/>
-      <c r="B190" s="3"/>
-      <c r="C190" s="3"/>
-      <c r="D190" s="3"/>
-      <c r="E190" s="3"/>
-      <c r="F190" s="3"/>
-      <c r="G190" s="3"/>
-      <c r="H190" s="3"/>
-      <c r="I190" s="4"/>
-      <c r="J190" s="4"/>
+      <c r="A190" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B190" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C190" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="D190" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="E190" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F190" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G190" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H190" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I190" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J190" s="4">
+        <f t="shared" si="5"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" s="3"/>

</xml_diff>

<commit_message>
#11 Time Tracking.xlsx: updated to 2023-10-05.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1251" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="372">
   <si>
     <t>Year</t>
   </si>
@@ -1126,6 +1126,18 @@
   </si>
   <si>
     <t>03:15</t>
+  </si>
+  <si>
+    <t>2023-10-02</t>
+  </si>
+  <si>
+    <t>2023-10-05</t>
+  </si>
+  <si>
+    <t>01:15</t>
+  </si>
+  <si>
+    <t>3h 15m</t>
   </si>
 </sst>
 </file>
@@ -1528,8 +1540,8 @@
   <dimension ref="A1:J198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E190" sqref="E190"/>
+      <pane ySplit="1" topLeftCell="A165" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F199" sqref="F199"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -5451,11 +5463,11 @@
         <v>351</v>
       </c>
       <c r="I131" s="4">
-        <f t="shared" ref="I131:I190" si="4">YEAR(A131)</f>
+        <f t="shared" ref="I131:I194" si="4">YEAR(A131)</f>
         <v>2023</v>
       </c>
       <c r="J131" s="4">
-        <f t="shared" ref="J131:J190" si="5">MONTH(A131)</f>
+        <f t="shared" ref="J131:J194" si="5">MONTH(A131)</f>
         <v>7</v>
       </c>
     </row>
@@ -7464,52 +7476,140 @@
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A191" s="3"/>
-      <c r="B191" s="3"/>
-      <c r="C191" s="3"/>
-      <c r="D191" s="3"/>
-      <c r="E191" s="3"/>
-      <c r="F191" s="3"/>
-      <c r="G191" s="3"/>
-      <c r="H191" s="3"/>
-      <c r="I191" s="4"/>
-      <c r="J191" s="4"/>
+      <c r="A191" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B191" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C191" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D191" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="E191" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F191" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G191" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H191" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I191" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J191" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A192" s="3"/>
-      <c r="B192" s="3"/>
-      <c r="C192" s="3"/>
-      <c r="D192" s="3"/>
-      <c r="E192" s="3"/>
-      <c r="F192" s="3"/>
-      <c r="G192" s="3"/>
-      <c r="H192" s="3"/>
-      <c r="I192" s="4"/>
-      <c r="J192" s="4"/>
+      <c r="A192" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="B192" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C192" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D192" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="E192" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F192" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G192" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H192" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I192" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J192" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A193" s="3"/>
-      <c r="B193" s="3"/>
-      <c r="C193" s="3"/>
-      <c r="D193" s="3"/>
-      <c r="E193" s="3"/>
-      <c r="F193" s="3"/>
-      <c r="G193" s="3"/>
-      <c r="H193" s="3"/>
-      <c r="I193" s="4"/>
-      <c r="J193" s="4"/>
+      <c r="A193" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B193" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C193" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="D193" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="E193" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G193" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H193" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I193" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J193" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A194" s="3"/>
-      <c r="B194" s="3"/>
-      <c r="C194" s="3"/>
-      <c r="D194" s="3"/>
-      <c r="E194" s="3"/>
-      <c r="F194" s="3"/>
-      <c r="G194" s="3"/>
-      <c r="H194" s="3"/>
-      <c r="I194" s="4"/>
-      <c r="J194" s="4"/>
+      <c r="A194" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="B194" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="C194" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="D194" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="E194" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F194" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="G194" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="H194" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="I194" s="4">
+        <f t="shared" si="4"/>
+        <v>2023</v>
+      </c>
+      <c r="J194" s="4">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" s="3"/>

</xml_diff>

<commit_message>
#11 Time Tracking.xlsx: updated up to 2023-10-20.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6824" uniqueCount="980">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6928" uniqueCount="988">
   <si>
     <t>Year</t>
   </si>
@@ -2962,6 +2962,30 @@
   </si>
   <si>
     <t>2021-05-30</t>
+  </si>
+  <si>
+    <t>2023-10-09</t>
+  </si>
+  <si>
+    <t>2023-10-10</t>
+  </si>
+  <si>
+    <t>2023-10-11</t>
+  </si>
+  <si>
+    <t>2023-10-16</t>
+  </si>
+  <si>
+    <t>2023-10-17</t>
+  </si>
+  <si>
+    <t>2023-10-18</t>
+  </si>
+  <si>
+    <t>2023-10-19</t>
+  </si>
+  <si>
+    <t>2023-10-20</t>
   </si>
 </sst>
 </file>
@@ -3361,11 +3385,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J871"/>
+  <dimension ref="A1:J901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F43" sqref="F43"/>
+      <pane ySplit="1" topLeftCell="A864" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E887" sqref="E887"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -29229,11 +29253,11 @@
         <v>290</v>
       </c>
       <c r="I769" s="4">
-        <f>YEAR(A769)</f>
+        <f t="shared" ref="I769:I807" si="36">YEAR(A769)</f>
         <v>2023</v>
       </c>
       <c r="J769" s="4">
-        <f>MONTH(A769)</f>
+        <f t="shared" ref="J769:J807" si="37">MONTH(A769)</f>
         <v>4</v>
       </c>
     </row>
@@ -29263,11 +29287,11 @@
         <v>290</v>
       </c>
       <c r="I770" s="4">
-        <f>YEAR(A770)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J770" s="4">
-        <f>MONTH(A770)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29297,11 +29321,11 @@
         <v>290</v>
       </c>
       <c r="I771" s="4">
-        <f>YEAR(A771)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J771" s="4">
-        <f>MONTH(A771)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29331,11 +29355,11 @@
         <v>290</v>
       </c>
       <c r="I772" s="4">
-        <f>YEAR(A772)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J772" s="4">
-        <f>MONTH(A772)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29365,11 +29389,11 @@
         <v>290</v>
       </c>
       <c r="I773" s="4">
-        <f>YEAR(A773)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J773" s="4">
-        <f>MONTH(A773)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29399,11 +29423,11 @@
         <v>290</v>
       </c>
       <c r="I774" s="4">
-        <f>YEAR(A774)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J774" s="4">
-        <f>MONTH(A774)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29433,11 +29457,11 @@
         <v>290</v>
       </c>
       <c r="I775" s="4">
-        <f>YEAR(A775)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J775" s="4">
-        <f>MONTH(A775)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29467,11 +29491,11 @@
         <v>290</v>
       </c>
       <c r="I776" s="4">
-        <f>YEAR(A776)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J776" s="4">
-        <f>MONTH(A776)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29501,11 +29525,11 @@
         <v>289</v>
       </c>
       <c r="I777" s="4">
-        <f>YEAR(A777)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J777" s="4">
-        <f>MONTH(A777)</f>
+        <f t="shared" si="37"/>
         <v>4</v>
       </c>
     </row>
@@ -29535,11 +29559,11 @@
         <v>290</v>
       </c>
       <c r="I778" s="4">
-        <f>YEAR(A778)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J778" s="4">
-        <f>MONTH(A778)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29569,11 +29593,11 @@
         <v>290</v>
       </c>
       <c r="I779" s="4">
-        <f>YEAR(A779)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J779" s="4">
-        <f>MONTH(A779)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29603,11 +29627,11 @@
         <v>290</v>
       </c>
       <c r="I780" s="4">
-        <f>YEAR(A780)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J780" s="4">
-        <f>MONTH(A780)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29637,11 +29661,11 @@
         <v>290</v>
       </c>
       <c r="I781" s="4">
-        <f>YEAR(A781)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J781" s="4">
-        <f>MONTH(A781)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29671,11 +29695,11 @@
         <v>290</v>
       </c>
       <c r="I782" s="4">
-        <f>YEAR(A782)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J782" s="4">
-        <f>MONTH(A782)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29705,11 +29729,11 @@
         <v>290</v>
       </c>
       <c r="I783" s="4">
-        <f>YEAR(A783)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J783" s="4">
-        <f>MONTH(A783)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29739,11 +29763,11 @@
         <v>290</v>
       </c>
       <c r="I784" s="4">
-        <f>YEAR(A784)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J784" s="4">
-        <f>MONTH(A784)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29773,11 +29797,11 @@
         <v>290</v>
       </c>
       <c r="I785" s="4">
-        <f>YEAR(A785)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J785" s="4">
-        <f>MONTH(A785)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29807,11 +29831,11 @@
         <v>290</v>
       </c>
       <c r="I786" s="4">
-        <f>YEAR(A786)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J786" s="4">
-        <f>MONTH(A786)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29841,11 +29865,11 @@
         <v>290</v>
       </c>
       <c r="I787" s="4">
-        <f>YEAR(A787)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J787" s="4">
-        <f>MONTH(A787)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29875,11 +29899,11 @@
         <v>290</v>
       </c>
       <c r="I788" s="4">
-        <f>YEAR(A788)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J788" s="4">
-        <f>MONTH(A788)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29909,11 +29933,11 @@
         <v>290</v>
       </c>
       <c r="I789" s="4">
-        <f>YEAR(A789)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J789" s="4">
-        <f>MONTH(A789)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29943,11 +29967,11 @@
         <v>290</v>
       </c>
       <c r="I790" s="4">
-        <f>YEAR(A790)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J790" s="4">
-        <f>MONTH(A790)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -29977,11 +30001,11 @@
         <v>290</v>
       </c>
       <c r="I791" s="4">
-        <f>YEAR(A791)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J791" s="4">
-        <f>MONTH(A791)</f>
+        <f t="shared" si="37"/>
         <v>5</v>
       </c>
     </row>
@@ -30011,11 +30035,11 @@
         <v>290</v>
       </c>
       <c r="I792" s="4">
-        <f>YEAR(A792)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J792" s="4">
-        <f>MONTH(A792)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30045,11 +30069,11 @@
         <v>290</v>
       </c>
       <c r="I793" s="4">
-        <f>YEAR(A793)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J793" s="4">
-        <f>MONTH(A793)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30079,11 +30103,11 @@
         <v>290</v>
       </c>
       <c r="I794" s="4">
-        <f>YEAR(A794)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J794" s="4">
-        <f>MONTH(A794)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30113,11 +30137,11 @@
         <v>290</v>
       </c>
       <c r="I795" s="4">
-        <f>YEAR(A795)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J795" s="4">
-        <f>MONTH(A795)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30147,11 +30171,11 @@
         <v>290</v>
       </c>
       <c r="I796" s="4">
-        <f>YEAR(A796)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J796" s="4">
-        <f>MONTH(A796)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30181,11 +30205,11 @@
         <v>290</v>
       </c>
       <c r="I797" s="4">
-        <f>YEAR(A797)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J797" s="4">
-        <f>MONTH(A797)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30215,11 +30239,11 @@
         <v>290</v>
       </c>
       <c r="I798" s="4">
-        <f>YEAR(A798)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J798" s="4">
-        <f>MONTH(A798)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30249,11 +30273,11 @@
         <v>289</v>
       </c>
       <c r="I799" s="4">
-        <f>YEAR(A799)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J799" s="4">
-        <f>MONTH(A799)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30283,11 +30307,11 @@
         <v>290</v>
       </c>
       <c r="I800" s="4">
-        <f>YEAR(A800)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J800" s="4">
-        <f>MONTH(A800)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30317,11 +30341,11 @@
         <v>290</v>
       </c>
       <c r="I801" s="4">
-        <f>YEAR(A801)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J801" s="4">
-        <f>MONTH(A801)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30351,11 +30375,11 @@
         <v>290</v>
       </c>
       <c r="I802" s="4">
-        <f>YEAR(A802)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J802" s="4">
-        <f>MONTH(A802)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30385,11 +30409,11 @@
         <v>290</v>
       </c>
       <c r="I803" s="4">
-        <f>YEAR(A803)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J803" s="4">
-        <f>MONTH(A803)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30419,11 +30443,11 @@
         <v>290</v>
       </c>
       <c r="I804" s="4">
-        <f>YEAR(A804)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J804" s="4">
-        <f>MONTH(A804)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30453,11 +30477,11 @@
         <v>290</v>
       </c>
       <c r="I805" s="4">
-        <f>YEAR(A805)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J805" s="4">
-        <f>MONTH(A805)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30487,11 +30511,11 @@
         <v>290</v>
       </c>
       <c r="I806" s="4">
-        <f>YEAR(A806)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J806" s="4">
-        <f>MONTH(A806)</f>
+        <f t="shared" si="37"/>
         <v>6</v>
       </c>
     </row>
@@ -30521,11 +30545,11 @@
         <v>290</v>
       </c>
       <c r="I807" s="4">
-        <f>YEAR(A807)</f>
+        <f t="shared" si="36"/>
         <v>2023</v>
       </c>
       <c r="J807" s="4">
-        <f>MONTH(A807)</f>
+        <f t="shared" si="37"/>
         <v>7</v>
       </c>
     </row>
@@ -30555,11 +30579,11 @@
         <v>290</v>
       </c>
       <c r="I808" s="4">
-        <f t="shared" ref="I808:I871" si="36">YEAR(A808)</f>
+        <f t="shared" ref="I808:I871" si="38">YEAR(A808)</f>
         <v>2023</v>
       </c>
       <c r="J808" s="4">
-        <f t="shared" ref="J808:J871" si="37">MONTH(A808)</f>
+        <f t="shared" ref="J808:J871" si="39">MONTH(A808)</f>
         <v>7</v>
       </c>
     </row>
@@ -30589,11 +30613,11 @@
         <v>290</v>
       </c>
       <c r="I809" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J809" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
     </row>
@@ -30623,11 +30647,11 @@
         <v>290</v>
       </c>
       <c r="I810" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J810" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
     </row>
@@ -30657,11 +30681,11 @@
         <v>290</v>
       </c>
       <c r="I811" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J811" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
     </row>
@@ -30691,11 +30715,11 @@
         <v>290</v>
       </c>
       <c r="I812" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J812" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
     </row>
@@ -30725,11 +30749,11 @@
         <v>290</v>
       </c>
       <c r="I813" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J813" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
     </row>
@@ -30759,11 +30783,11 @@
         <v>290</v>
       </c>
       <c r="I814" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J814" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>7</v>
       </c>
     </row>
@@ -30793,11 +30817,11 @@
         <v>290</v>
       </c>
       <c r="I815" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J815" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -30827,11 +30851,11 @@
         <v>290</v>
       </c>
       <c r="I816" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J816" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -30861,11 +30885,11 @@
         <v>290</v>
       </c>
       <c r="I817" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J817" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -30895,11 +30919,11 @@
         <v>290</v>
       </c>
       <c r="I818" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J818" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -30929,11 +30953,11 @@
         <v>290</v>
       </c>
       <c r="I819" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J819" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -30963,11 +30987,11 @@
         <v>290</v>
       </c>
       <c r="I820" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J820" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -30997,11 +31021,11 @@
         <v>290</v>
       </c>
       <c r="I821" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J821" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31031,11 +31055,11 @@
         <v>289</v>
       </c>
       <c r="I822" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J822" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31065,11 +31089,11 @@
         <v>290</v>
       </c>
       <c r="I823" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J823" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31099,11 +31123,11 @@
         <v>290</v>
       </c>
       <c r="I824" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J824" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31133,11 +31157,11 @@
         <v>290</v>
       </c>
       <c r="I825" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J825" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31167,11 +31191,11 @@
         <v>290</v>
       </c>
       <c r="I826" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J826" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31201,11 +31225,11 @@
         <v>290</v>
       </c>
       <c r="I827" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J827" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31235,11 +31259,11 @@
         <v>290</v>
       </c>
       <c r="I828" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J828" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31269,11 +31293,11 @@
         <v>290</v>
       </c>
       <c r="I829" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J829" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31303,11 +31327,11 @@
         <v>289</v>
       </c>
       <c r="I830" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J830" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31337,11 +31361,11 @@
         <v>290</v>
       </c>
       <c r="I831" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J831" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31371,11 +31395,11 @@
         <v>290</v>
       </c>
       <c r="I832" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J832" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31405,11 +31429,11 @@
         <v>290</v>
       </c>
       <c r="I833" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J833" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31439,11 +31463,11 @@
         <v>290</v>
       </c>
       <c r="I834" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J834" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31473,11 +31497,11 @@
         <v>290</v>
       </c>
       <c r="I835" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J835" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31507,11 +31531,11 @@
         <v>290</v>
       </c>
       <c r="I836" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J836" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>8</v>
       </c>
     </row>
@@ -31541,11 +31565,11 @@
         <v>290</v>
       </c>
       <c r="I837" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J837" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31575,11 +31599,11 @@
         <v>290</v>
       </c>
       <c r="I838" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J838" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31609,11 +31633,11 @@
         <v>290</v>
       </c>
       <c r="I839" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J839" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31643,11 +31667,11 @@
         <v>290</v>
       </c>
       <c r="I840" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J840" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31677,11 +31701,11 @@
         <v>290</v>
       </c>
       <c r="I841" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J841" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31711,11 +31735,11 @@
         <v>290</v>
       </c>
       <c r="I842" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J842" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31745,11 +31769,11 @@
         <v>290</v>
       </c>
       <c r="I843" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J843" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31779,11 +31803,11 @@
         <v>290</v>
       </c>
       <c r="I844" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J844" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31813,11 +31837,11 @@
         <v>290</v>
       </c>
       <c r="I845" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J845" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31847,11 +31871,11 @@
         <v>290</v>
       </c>
       <c r="I846" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J846" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31881,11 +31905,11 @@
         <v>290</v>
       </c>
       <c r="I847" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J847" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31915,11 +31939,11 @@
         <v>290</v>
       </c>
       <c r="I848" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J848" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31949,11 +31973,11 @@
         <v>290</v>
       </c>
       <c r="I849" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J849" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -31983,11 +32007,11 @@
         <v>290</v>
       </c>
       <c r="I850" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J850" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32017,11 +32041,11 @@
         <v>290</v>
       </c>
       <c r="I851" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J851" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32051,11 +32075,11 @@
         <v>290</v>
       </c>
       <c r="I852" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J852" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32083,11 +32107,11 @@
         <v>290</v>
       </c>
       <c r="I853" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J853" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32117,11 +32141,11 @@
         <v>290</v>
       </c>
       <c r="I854" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J854" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32151,11 +32175,11 @@
         <v>290</v>
       </c>
       <c r="I855" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J855" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32185,11 +32209,11 @@
         <v>290</v>
       </c>
       <c r="I856" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J856" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32219,11 +32243,11 @@
         <v>290</v>
       </c>
       <c r="I857" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J857" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32253,11 +32277,11 @@
         <v>290</v>
       </c>
       <c r="I858" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J858" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32287,11 +32311,11 @@
         <v>290</v>
       </c>
       <c r="I859" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J859" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32321,11 +32345,11 @@
         <v>290</v>
       </c>
       <c r="I860" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J860" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32355,11 +32379,11 @@
         <v>289</v>
       </c>
       <c r="I861" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J861" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32389,11 +32413,11 @@
         <v>289</v>
       </c>
       <c r="I862" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J862" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32423,11 +32447,11 @@
         <v>289</v>
       </c>
       <c r="I863" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J863" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32457,11 +32481,11 @@
         <v>290</v>
       </c>
       <c r="I864" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J864" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32491,11 +32515,11 @@
         <v>290</v>
       </c>
       <c r="I865" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J865" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32525,11 +32549,11 @@
         <v>290</v>
       </c>
       <c r="I866" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J866" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32559,11 +32583,11 @@
         <v>290</v>
       </c>
       <c r="I867" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J867" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>9</v>
       </c>
     </row>
@@ -32593,11 +32617,11 @@
         <v>290</v>
       </c>
       <c r="I868" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J868" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
     </row>
@@ -32627,11 +32651,11 @@
         <v>290</v>
       </c>
       <c r="I869" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J869" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
     </row>
@@ -32661,11 +32685,11 @@
         <v>290</v>
       </c>
       <c r="I870" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J870" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
     </row>
@@ -32695,13 +32719,659 @@
         <v>290</v>
       </c>
       <c r="I871" s="4">
-        <f t="shared" si="36"/>
+        <f t="shared" si="38"/>
         <v>2023</v>
       </c>
       <c r="J871" s="4">
-        <f t="shared" si="37"/>
+        <f t="shared" si="39"/>
         <v>10</v>
       </c>
+    </row>
+    <row r="872" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A872" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="B872" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C872" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D872" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="E872" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F872" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G872" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H872" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I872" s="4">
+        <f t="shared" ref="I872" si="40">YEAR(A872)</f>
+        <v>2023</v>
+      </c>
+      <c r="J872" s="4">
+        <f t="shared" ref="J872" si="41">MONTH(A872)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="873" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A873" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B873" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="C873" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="D873" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E873" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F873" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G873" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H873" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I873" s="4">
+        <f t="shared" ref="I873" si="42">YEAR(A873)</f>
+        <v>2023</v>
+      </c>
+      <c r="J873" s="4">
+        <f t="shared" ref="J873" si="43">MONTH(A873)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="874" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A874" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="B874" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C874" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D874" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E874" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F874" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G874" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H874" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I874" s="4">
+        <f t="shared" ref="I874:I875" si="44">YEAR(A874)</f>
+        <v>2023</v>
+      </c>
+      <c r="J874" s="4">
+        <f t="shared" ref="J874:J875" si="45">MONTH(A874)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="875" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A875" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="B875" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C875" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D875" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E875" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F875" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G875" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H875" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I875" s="4">
+        <f t="shared" si="44"/>
+        <v>2023</v>
+      </c>
+      <c r="J875" s="4">
+        <f t="shared" si="45"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="876" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A876" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="B876" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C876" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="D876" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E876" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F876" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G876" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H876" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I876" s="4">
+        <f t="shared" ref="I876:I877" si="46">YEAR(A876)</f>
+        <v>2023</v>
+      </c>
+      <c r="J876" s="4">
+        <f t="shared" ref="J876:J877" si="47">MONTH(A876)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="877" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A877" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="B877" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C877" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D877" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E877" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F877" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G877" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H877" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I877" s="4">
+        <f t="shared" si="46"/>
+        <v>2023</v>
+      </c>
+      <c r="J877" s="4">
+        <f t="shared" si="47"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="878" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A878" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="B878" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="C878" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D878" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E878" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F878" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G878" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H878" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I878" s="4">
+        <f t="shared" ref="I878:I884" si="48">YEAR(A878)</f>
+        <v>2023</v>
+      </c>
+      <c r="J878" s="4">
+        <f t="shared" ref="J878:J884" si="49">MONTH(A878)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="879" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A879" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="B879" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C879" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D879" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E879" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F879" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G879" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H879" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I879" s="4">
+        <f t="shared" si="48"/>
+        <v>2023</v>
+      </c>
+      <c r="J879" s="4">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="880" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A880" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="B880" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C880" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D880" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E880" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F880" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G880" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H880" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I880" s="4">
+        <f t="shared" si="48"/>
+        <v>2023</v>
+      </c>
+      <c r="J880" s="4">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="881" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A881" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="B881" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C881" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D881" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E881" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F881" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G881" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H881" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I881" s="4">
+        <f t="shared" si="48"/>
+        <v>2023</v>
+      </c>
+      <c r="J881" s="4">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="882" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A882" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="B882" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C882" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D882" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="E882" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F882" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G882" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H882" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I882" s="4">
+        <f t="shared" si="48"/>
+        <v>2023</v>
+      </c>
+      <c r="J882" s="4">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="883" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A883" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B883" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="C883" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="D883" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="E883" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F883" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G883" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H883" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I883" s="4">
+        <f t="shared" si="48"/>
+        <v>2023</v>
+      </c>
+      <c r="J883" s="4">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="884" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A884" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B884" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C884" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D884" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E884" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F884" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G884" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H884" s="8" t="s">
+        <v>290</v>
+      </c>
+      <c r="I884" s="4">
+        <f t="shared" si="48"/>
+        <v>2023</v>
+      </c>
+      <c r="J884" s="4">
+        <f t="shared" si="49"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="885" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A885" s="3"/>
+      <c r="B885" s="3"/>
+      <c r="C885" s="3"/>
+      <c r="D885" s="3"/>
+      <c r="E885" s="3"/>
+      <c r="F885" s="3"/>
+      <c r="G885" s="3"/>
+      <c r="H885" s="3"/>
+      <c r="I885" s="4"/>
+      <c r="J885" s="4"/>
+    </row>
+    <row r="886" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A886" s="3"/>
+      <c r="B886" s="3"/>
+      <c r="C886" s="3"/>
+      <c r="D886" s="3"/>
+      <c r="E886" s="3"/>
+      <c r="F886" s="3"/>
+      <c r="G886" s="3"/>
+      <c r="H886" s="3"/>
+      <c r="I886" s="4"/>
+      <c r="J886" s="4"/>
+    </row>
+    <row r="887" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A887" s="3"/>
+      <c r="B887" s="3"/>
+      <c r="C887" s="3"/>
+      <c r="D887" s="3"/>
+      <c r="E887" s="3"/>
+      <c r="F887" s="3"/>
+      <c r="G887" s="3"/>
+      <c r="H887" s="3"/>
+      <c r="I887" s="4"/>
+      <c r="J887" s="4"/>
+    </row>
+    <row r="888" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A888" s="3"/>
+      <c r="B888" s="3"/>
+      <c r="C888" s="3"/>
+      <c r="D888" s="3"/>
+      <c r="E888" s="3"/>
+      <c r="F888" s="3"/>
+      <c r="G888" s="3"/>
+      <c r="H888" s="3"/>
+      <c r="I888" s="4"/>
+      <c r="J888" s="4"/>
+    </row>
+    <row r="889" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A889" s="3"/>
+      <c r="B889" s="3"/>
+      <c r="C889" s="3"/>
+      <c r="D889" s="3"/>
+      <c r="E889" s="3"/>
+      <c r="F889" s="3"/>
+      <c r="G889" s="3"/>
+      <c r="H889" s="3"/>
+      <c r="I889" s="4"/>
+      <c r="J889" s="4"/>
+    </row>
+    <row r="890" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A890" s="3"/>
+      <c r="B890" s="3"/>
+      <c r="C890" s="3"/>
+      <c r="D890" s="3"/>
+      <c r="E890" s="3"/>
+      <c r="F890" s="3"/>
+      <c r="G890" s="3"/>
+      <c r="H890" s="3"/>
+      <c r="I890" s="4"/>
+      <c r="J890" s="4"/>
+    </row>
+    <row r="891" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A891" s="3"/>
+      <c r="B891" s="3"/>
+      <c r="C891" s="3"/>
+      <c r="D891" s="3"/>
+      <c r="E891" s="3"/>
+      <c r="F891" s="3"/>
+      <c r="G891" s="3"/>
+      <c r="H891" s="3"/>
+      <c r="I891" s="4"/>
+      <c r="J891" s="4"/>
+    </row>
+    <row r="892" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A892" s="3"/>
+      <c r="B892" s="3"/>
+      <c r="C892" s="3"/>
+      <c r="D892" s="3"/>
+      <c r="E892" s="3"/>
+      <c r="F892" s="3"/>
+      <c r="G892" s="3"/>
+      <c r="H892" s="3"/>
+      <c r="I892" s="4"/>
+      <c r="J892" s="4"/>
+    </row>
+    <row r="893" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A893" s="3"/>
+      <c r="B893" s="3"/>
+      <c r="C893" s="3"/>
+      <c r="D893" s="3"/>
+      <c r="E893" s="3"/>
+      <c r="F893" s="3"/>
+      <c r="G893" s="3"/>
+      <c r="H893" s="3"/>
+      <c r="I893" s="4"/>
+      <c r="J893" s="4"/>
+    </row>
+    <row r="894" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A894" s="3"/>
+      <c r="B894" s="3"/>
+      <c r="C894" s="3"/>
+      <c r="D894" s="3"/>
+      <c r="E894" s="3"/>
+      <c r="F894" s="3"/>
+      <c r="G894" s="3"/>
+      <c r="H894" s="3"/>
+      <c r="I894" s="4"/>
+      <c r="J894" s="4"/>
+    </row>
+    <row r="895" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A895" s="3"/>
+      <c r="B895" s="3"/>
+      <c r="C895" s="3"/>
+      <c r="D895" s="3"/>
+      <c r="E895" s="3"/>
+      <c r="F895" s="3"/>
+      <c r="G895" s="3"/>
+      <c r="H895" s="3"/>
+      <c r="I895" s="4"/>
+      <c r="J895" s="4"/>
+    </row>
+    <row r="896" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A896" s="3"/>
+      <c r="B896" s="3"/>
+      <c r="C896" s="3"/>
+      <c r="D896" s="3"/>
+      <c r="E896" s="3"/>
+      <c r="F896" s="3"/>
+      <c r="G896" s="3"/>
+      <c r="H896" s="3"/>
+      <c r="I896" s="4"/>
+      <c r="J896" s="4"/>
+    </row>
+    <row r="897" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A897" s="3"/>
+      <c r="B897" s="3"/>
+      <c r="C897" s="3"/>
+      <c r="D897" s="3"/>
+      <c r="E897" s="3"/>
+      <c r="F897" s="3"/>
+      <c r="G897" s="3"/>
+      <c r="H897" s="3"/>
+      <c r="I897" s="4"/>
+      <c r="J897" s="4"/>
+    </row>
+    <row r="898" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A898" s="3"/>
+      <c r="B898" s="3"/>
+      <c r="C898" s="3"/>
+      <c r="D898" s="3"/>
+      <c r="E898" s="3"/>
+      <c r="F898" s="3"/>
+      <c r="G898" s="3"/>
+      <c r="H898" s="3"/>
+      <c r="I898" s="4"/>
+      <c r="J898" s="4"/>
+    </row>
+    <row r="899" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A899" s="3"/>
+      <c r="B899" s="3"/>
+      <c r="C899" s="3"/>
+      <c r="D899" s="3"/>
+      <c r="E899" s="3"/>
+      <c r="F899" s="3"/>
+      <c r="G899" s="3"/>
+      <c r="H899" s="3"/>
+      <c r="I899" s="4"/>
+      <c r="J899" s="4"/>
+    </row>
+    <row r="900" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A900" s="3"/>
+      <c r="B900" s="3"/>
+      <c r="C900" s="3"/>
+      <c r="D900" s="3"/>
+      <c r="E900" s="3"/>
+      <c r="F900" s="3"/>
+      <c r="G900" s="3"/>
+      <c r="H900" s="3"/>
+      <c r="I900" s="4"/>
+      <c r="J900" s="4"/>
+    </row>
+    <row r="901" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A901" s="3"/>
+      <c r="B901" s="3"/>
+      <c r="C901" s="3"/>
+      <c r="D901" s="3"/>
+      <c r="E901" s="3"/>
+      <c r="F901" s="3"/>
+      <c r="G901" s="3"/>
+      <c r="H901" s="3"/>
+      <c r="I901" s="4"/>
+      <c r="J901" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#11 Time Tracking.xlsx: updated to 2023-10-31.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6928" uniqueCount="988">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6936" uniqueCount="989">
   <si>
     <t>Year</t>
   </si>
@@ -2986,6 +2986,9 @@
   </si>
   <si>
     <t>2023-10-20</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
   </si>
 </sst>
 </file>
@@ -3388,8 +3391,8 @@
   <dimension ref="A1:J901"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A864" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E887" sqref="E887"/>
+      <pane ySplit="1" topLeftCell="A866" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A885" sqref="A885"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -33170,16 +33173,38 @@
       </c>
     </row>
     <row r="885" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A885" s="3"/>
-      <c r="B885" s="3"/>
-      <c r="C885" s="3"/>
-      <c r="D885" s="3"/>
-      <c r="E885" s="3"/>
-      <c r="F885" s="3"/>
-      <c r="G885" s="3"/>
-      <c r="H885" s="3"/>
-      <c r="I885" s="4"/>
-      <c r="J885" s="4"/>
+      <c r="A885" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="B885" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C885" s="3" t="s">
+        <v>275</v>
+      </c>
+      <c r="D885" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="E885" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F885" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="G885" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="H885" s="8" t="s">
+        <v>289</v>
+      </c>
+      <c r="I885" s="4">
+        <f t="shared" ref="I885" si="50">YEAR(A885)</f>
+        <v>2023</v>
+      </c>
+      <c r="J885" s="4">
+        <f t="shared" ref="J885" si="51">MONTH(A885)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="886" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A886" s="3"/>

</xml_diff>

<commit_message>
#13 Time Tracking.*: updated to 11/21/2023.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6936" uniqueCount="981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7040" uniqueCount="991">
   <si>
     <t>Year</t>
   </si>
@@ -2965,6 +2965,36 @@
   </si>
   <si>
     <t>9h 15m</t>
+  </si>
+  <si>
+    <t>2023-11-06</t>
+  </si>
+  <si>
+    <t>nwtimetrackingmanager v1.1.0</t>
+  </si>
+  <si>
+    <t>2023-11-08</t>
+  </si>
+  <si>
+    <t>2023-11-13</t>
+  </si>
+  <si>
+    <t>2023-11-14</t>
+  </si>
+  <si>
+    <t>2023-11-15</t>
+  </si>
+  <si>
+    <t>2023-11-16</t>
+  </si>
+  <si>
+    <t>2023-11-17</t>
+  </si>
+  <si>
+    <t>2023-11-20</t>
+  </si>
+  <si>
+    <t>2023-11-21</t>
   </si>
 </sst>
 </file>
@@ -3364,11 +3394,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J901"/>
+  <dimension ref="A1:J919"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A831" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D853" sqref="D853"/>
+      <pane ySplit="1" topLeftCell="A881" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D903" sqref="D903"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -33174,169 +33204,455 @@
         <v>282</v>
       </c>
       <c r="I885" s="4">
-        <f t="shared" ref="I885" si="50">YEAR(A885)</f>
+        <f t="shared" ref="I885:I886" si="50">YEAR(A885)</f>
         <v>2023</v>
       </c>
       <c r="J885" s="4">
-        <f t="shared" ref="J885" si="51">MONTH(A885)</f>
+        <f t="shared" ref="J885:J886" si="51">MONTH(A885)</f>
         <v>10</v>
       </c>
     </row>
     <row r="886" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A886" s="3"/>
-      <c r="B886" s="3"/>
-      <c r="C886" s="3"/>
-      <c r="D886" s="3"/>
-      <c r="E886" s="3"/>
-      <c r="F886" s="3"/>
-      <c r="G886" s="3"/>
-      <c r="H886" s="3"/>
-      <c r="I886" s="4"/>
-      <c r="J886" s="4"/>
+      <c r="A886" s="3" t="s">
+        <v>981</v>
+      </c>
+      <c r="B886" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C886" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D886" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E886" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F886" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G886" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H886" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I886" s="4">
+        <f t="shared" si="50"/>
+        <v>2023</v>
+      </c>
+      <c r="J886" s="4">
+        <f t="shared" si="51"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="887" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A887" s="3"/>
-      <c r="B887" s="3"/>
-      <c r="C887" s="3"/>
-      <c r="D887" s="3"/>
-      <c r="E887" s="3"/>
-      <c r="F887" s="3"/>
-      <c r="G887" s="3"/>
-      <c r="H887" s="3"/>
-      <c r="I887" s="4"/>
-      <c r="J887" s="4"/>
+      <c r="A887" s="3" t="s">
+        <v>983</v>
+      </c>
+      <c r="B887" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C887" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D887" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E887" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F887" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G887" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H887" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I887" s="4">
+        <f t="shared" ref="I887:I898" si="52">YEAR(A887)</f>
+        <v>2023</v>
+      </c>
+      <c r="J887" s="4">
+        <f t="shared" ref="J887:J898" si="53">MONTH(A887)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="888" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A888" s="3"/>
-      <c r="B888" s="3"/>
-      <c r="C888" s="3"/>
-      <c r="D888" s="3"/>
-      <c r="E888" s="3"/>
-      <c r="F888" s="3"/>
-      <c r="G888" s="3"/>
-      <c r="H888" s="3"/>
-      <c r="I888" s="4"/>
-      <c r="J888" s="4"/>
+      <c r="A888" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="B888" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C888" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D888" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="E888" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F888" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G888" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H888" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I888" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J888" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="889" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A889" s="3"/>
-      <c r="B889" s="3"/>
-      <c r="C889" s="3"/>
-      <c r="D889" s="3"/>
-      <c r="E889" s="3"/>
-      <c r="F889" s="3"/>
-      <c r="G889" s="3"/>
-      <c r="H889" s="3"/>
-      <c r="I889" s="4"/>
-      <c r="J889" s="4"/>
+      <c r="A889" s="3" t="s">
+        <v>985</v>
+      </c>
+      <c r="B889" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C889" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="D889" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E889" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F889" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G889" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H889" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I889" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J889" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="890" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A890" s="3"/>
-      <c r="B890" s="3"/>
-      <c r="C890" s="3"/>
-      <c r="D890" s="3"/>
-      <c r="E890" s="3"/>
-      <c r="F890" s="3"/>
-      <c r="G890" s="3"/>
-      <c r="H890" s="3"/>
-      <c r="I890" s="4"/>
-      <c r="J890" s="4"/>
+      <c r="A890" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="B890" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C890" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D890" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E890" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F890" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G890" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H890" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I890" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J890" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="891" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A891" s="3"/>
-      <c r="B891" s="3"/>
-      <c r="C891" s="3"/>
-      <c r="D891" s="3"/>
-      <c r="E891" s="3"/>
-      <c r="F891" s="3"/>
-      <c r="G891" s="3"/>
-      <c r="H891" s="3"/>
-      <c r="I891" s="4"/>
-      <c r="J891" s="4"/>
+      <c r="A891" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="B891" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C891" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D891" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E891" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F891" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G891" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H891" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I891" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J891" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="892" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A892" s="3"/>
-      <c r="B892" s="3"/>
-      <c r="C892" s="3"/>
-      <c r="D892" s="3"/>
-      <c r="E892" s="3"/>
-      <c r="F892" s="3"/>
-      <c r="G892" s="3"/>
-      <c r="H892" s="3"/>
-      <c r="I892" s="4"/>
-      <c r="J892" s="4"/>
+      <c r="A892" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="B892" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C892" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="D892" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E892" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F892" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G892" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H892" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I892" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J892" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="893" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A893" s="3"/>
-      <c r="B893" s="3"/>
-      <c r="C893" s="3"/>
-      <c r="D893" s="3"/>
-      <c r="E893" s="3"/>
-      <c r="F893" s="3"/>
-      <c r="G893" s="3"/>
-      <c r="H893" s="3"/>
-      <c r="I893" s="4"/>
-      <c r="J893" s="4"/>
+      <c r="A893" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="B893" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C893" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D893" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="E893" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F893" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G893" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H893" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I893" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J893" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="894" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A894" s="3"/>
-      <c r="B894" s="3"/>
-      <c r="C894" s="3"/>
-      <c r="D894" s="3"/>
-      <c r="E894" s="3"/>
-      <c r="F894" s="3"/>
-      <c r="G894" s="3"/>
-      <c r="H894" s="3"/>
-      <c r="I894" s="4"/>
-      <c r="J894" s="4"/>
+      <c r="A894" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B894" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C894" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D894" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E894" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F894" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G894" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H894" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I894" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J894" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="895" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A895" s="3"/>
-      <c r="B895" s="3"/>
-      <c r="C895" s="3"/>
-      <c r="D895" s="3"/>
-      <c r="E895" s="3"/>
-      <c r="F895" s="3"/>
-      <c r="G895" s="3"/>
-      <c r="H895" s="3"/>
-      <c r="I895" s="4"/>
-      <c r="J895" s="4"/>
+      <c r="A895" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B895" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C895" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D895" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E895" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F895" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G895" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H895" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I895" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J895" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="896" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A896" s="3"/>
-      <c r="B896" s="3"/>
-      <c r="C896" s="3"/>
-      <c r="D896" s="3"/>
-      <c r="E896" s="3"/>
-      <c r="F896" s="3"/>
-      <c r="G896" s="3"/>
-      <c r="H896" s="3"/>
-      <c r="I896" s="4"/>
-      <c r="J896" s="4"/>
+      <c r="A896" s="3" t="s">
+        <v>989</v>
+      </c>
+      <c r="B896" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C896" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="D896" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E896" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F896" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G896" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H896" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I896" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J896" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="897" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A897" s="3"/>
-      <c r="B897" s="3"/>
-      <c r="C897" s="3"/>
-      <c r="D897" s="3"/>
-      <c r="E897" s="3"/>
-      <c r="F897" s="3"/>
-      <c r="G897" s="3"/>
-      <c r="H897" s="3"/>
-      <c r="I897" s="4"/>
-      <c r="J897" s="4"/>
+      <c r="A897" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="B897" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C897" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D897" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E897" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F897" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G897" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H897" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I897" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J897" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="898" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A898" s="3"/>
-      <c r="B898" s="3"/>
-      <c r="C898" s="3"/>
-      <c r="D898" s="3"/>
-      <c r="E898" s="3"/>
-      <c r="F898" s="3"/>
-      <c r="G898" s="3"/>
-      <c r="H898" s="3"/>
-      <c r="I898" s="4"/>
-      <c r="J898" s="4"/>
+      <c r="A898" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="B898" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="C898" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="D898" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E898" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F898" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G898" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H898" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I898" s="4">
+        <f t="shared" si="52"/>
+        <v>2023</v>
+      </c>
+      <c r="J898" s="4">
+        <f t="shared" si="53"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="899" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A899" s="3"/>
@@ -33374,6 +33690,222 @@
       <c r="I901" s="4"/>
       <c r="J901" s="4"/>
     </row>
+    <row r="902" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A902" s="3"/>
+      <c r="B902" s="3"/>
+      <c r="C902" s="3"/>
+      <c r="D902" s="3"/>
+      <c r="E902" s="3"/>
+      <c r="F902" s="3"/>
+      <c r="G902" s="3"/>
+      <c r="H902" s="3"/>
+      <c r="I902" s="4"/>
+      <c r="J902" s="4"/>
+    </row>
+    <row r="903" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A903" s="3"/>
+      <c r="B903" s="3"/>
+      <c r="C903" s="3"/>
+      <c r="D903" s="3"/>
+      <c r="E903" s="3"/>
+      <c r="F903" s="3"/>
+      <c r="G903" s="3"/>
+      <c r="H903" s="3"/>
+      <c r="I903" s="4"/>
+      <c r="J903" s="4"/>
+    </row>
+    <row r="904" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A904" s="3"/>
+      <c r="B904" s="3"/>
+      <c r="C904" s="3"/>
+      <c r="D904" s="3"/>
+      <c r="E904" s="3"/>
+      <c r="F904" s="3"/>
+      <c r="G904" s="3"/>
+      <c r="H904" s="3"/>
+      <c r="I904" s="4"/>
+      <c r="J904" s="4"/>
+    </row>
+    <row r="905" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A905" s="3"/>
+      <c r="B905" s="3"/>
+      <c r="C905" s="3"/>
+      <c r="D905" s="3"/>
+      <c r="E905" s="3"/>
+      <c r="F905" s="3"/>
+      <c r="G905" s="3"/>
+      <c r="H905" s="3"/>
+      <c r="I905" s="4"/>
+      <c r="J905" s="4"/>
+    </row>
+    <row r="906" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A906" s="3"/>
+      <c r="B906" s="3"/>
+      <c r="C906" s="3"/>
+      <c r="D906" s="3"/>
+      <c r="E906" s="3"/>
+      <c r="F906" s="3"/>
+      <c r="G906" s="3"/>
+      <c r="H906" s="3"/>
+      <c r="I906" s="4"/>
+      <c r="J906" s="4"/>
+    </row>
+    <row r="907" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A907" s="3"/>
+      <c r="B907" s="3"/>
+      <c r="C907" s="3"/>
+      <c r="D907" s="3"/>
+      <c r="E907" s="3"/>
+      <c r="F907" s="3"/>
+      <c r="G907" s="3"/>
+      <c r="H907" s="3"/>
+      <c r="I907" s="4"/>
+      <c r="J907" s="4"/>
+    </row>
+    <row r="908" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A908" s="3"/>
+      <c r="B908" s="3"/>
+      <c r="C908" s="3"/>
+      <c r="D908" s="3"/>
+      <c r="E908" s="3"/>
+      <c r="F908" s="3"/>
+      <c r="G908" s="3"/>
+      <c r="H908" s="3"/>
+      <c r="I908" s="4"/>
+      <c r="J908" s="4"/>
+    </row>
+    <row r="909" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A909" s="3"/>
+      <c r="B909" s="3"/>
+      <c r="C909" s="3"/>
+      <c r="D909" s="3"/>
+      <c r="E909" s="3"/>
+      <c r="F909" s="3"/>
+      <c r="G909" s="3"/>
+      <c r="H909" s="3"/>
+      <c r="I909" s="4"/>
+      <c r="J909" s="4"/>
+    </row>
+    <row r="910" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A910" s="3"/>
+      <c r="B910" s="3"/>
+      <c r="C910" s="3"/>
+      <c r="D910" s="3"/>
+      <c r="E910" s="3"/>
+      <c r="F910" s="3"/>
+      <c r="G910" s="3"/>
+      <c r="H910" s="3"/>
+      <c r="I910" s="4"/>
+      <c r="J910" s="4"/>
+    </row>
+    <row r="911" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A911" s="3"/>
+      <c r="B911" s="3"/>
+      <c r="C911" s="3"/>
+      <c r="D911" s="3"/>
+      <c r="E911" s="3"/>
+      <c r="F911" s="3"/>
+      <c r="G911" s="3"/>
+      <c r="H911" s="3"/>
+      <c r="I911" s="4"/>
+      <c r="J911" s="4"/>
+    </row>
+    <row r="912" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A912" s="3"/>
+      <c r="B912" s="3"/>
+      <c r="C912" s="3"/>
+      <c r="D912" s="3"/>
+      <c r="E912" s="3"/>
+      <c r="F912" s="3"/>
+      <c r="G912" s="3"/>
+      <c r="H912" s="3"/>
+      <c r="I912" s="4"/>
+      <c r="J912" s="4"/>
+    </row>
+    <row r="913" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A913" s="3"/>
+      <c r="B913" s="3"/>
+      <c r="C913" s="3"/>
+      <c r="D913" s="3"/>
+      <c r="E913" s="3"/>
+      <c r="F913" s="3"/>
+      <c r="G913" s="3"/>
+      <c r="H913" s="3"/>
+      <c r="I913" s="4"/>
+      <c r="J913" s="4"/>
+    </row>
+    <row r="914" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A914" s="3"/>
+      <c r="B914" s="3"/>
+      <c r="C914" s="3"/>
+      <c r="D914" s="3"/>
+      <c r="E914" s="3"/>
+      <c r="F914" s="3"/>
+      <c r="G914" s="3"/>
+      <c r="H914" s="3"/>
+      <c r="I914" s="4"/>
+      <c r="J914" s="4"/>
+    </row>
+    <row r="915" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A915" s="3"/>
+      <c r="B915" s="3"/>
+      <c r="C915" s="3"/>
+      <c r="D915" s="3"/>
+      <c r="E915" s="3"/>
+      <c r="F915" s="3"/>
+      <c r="G915" s="3"/>
+      <c r="H915" s="3"/>
+      <c r="I915" s="4"/>
+      <c r="J915" s="4"/>
+    </row>
+    <row r="916" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A916" s="3"/>
+      <c r="B916" s="3"/>
+      <c r="C916" s="3"/>
+      <c r="D916" s="3"/>
+      <c r="E916" s="3"/>
+      <c r="F916" s="3"/>
+      <c r="G916" s="3"/>
+      <c r="H916" s="3"/>
+      <c r="I916" s="4"/>
+      <c r="J916" s="4"/>
+    </row>
+    <row r="917" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A917" s="3"/>
+      <c r="B917" s="3"/>
+      <c r="C917" s="3"/>
+      <c r="D917" s="3"/>
+      <c r="E917" s="3"/>
+      <c r="F917" s="3"/>
+      <c r="G917" s="3"/>
+      <c r="H917" s="3"/>
+      <c r="I917" s="4"/>
+      <c r="J917" s="4"/>
+    </row>
+    <row r="918" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A918" s="3"/>
+      <c r="B918" s="3"/>
+      <c r="C918" s="3"/>
+      <c r="D918" s="3"/>
+      <c r="E918" s="3"/>
+      <c r="F918" s="3"/>
+      <c r="G918" s="3"/>
+      <c r="H918" s="3"/>
+      <c r="I918" s="4"/>
+      <c r="J918" s="4"/>
+    </row>
+    <row r="919" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A919" s="3"/>
+      <c r="B919" s="3"/>
+      <c r="C919" s="3"/>
+      <c r="D919" s="3"/>
+      <c r="E919" s="3"/>
+      <c r="F919" s="3"/>
+      <c r="G919" s="3"/>
+      <c r="H919" s="3"/>
+      <c r="I919" s="4"/>
+      <c r="J919" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#13 Time Tracking.*: updated to 11/22/2023.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7040" uniqueCount="991">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7056" uniqueCount="992">
   <si>
     <t>Year</t>
   </si>
@@ -2995,6 +2995,9 @@
   </si>
   <si>
     <t>2023-11-21</t>
+  </si>
+  <si>
+    <t>2023-11-22</t>
   </si>
 </sst>
 </file>
@@ -3398,7 +3401,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A881" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D903" sqref="D903"/>
+      <selection pane="bottomLeft" activeCell="B901" sqref="B901"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -33646,37 +33649,81 @@
         <v>283</v>
       </c>
       <c r="I898" s="4">
-        <f t="shared" si="52"/>
+        <f t="shared" ref="I898:I899" si="54">YEAR(A898)</f>
         <v>2023</v>
       </c>
       <c r="J898" s="4">
-        <f t="shared" si="53"/>
+        <f t="shared" ref="J898:J899" si="55">MONTH(A898)</f>
         <v>11</v>
       </c>
     </row>
     <row r="899" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A899" s="3"/>
-      <c r="B899" s="3"/>
-      <c r="C899" s="3"/>
-      <c r="D899" s="3"/>
-      <c r="E899" s="3"/>
-      <c r="F899" s="3"/>
-      <c r="G899" s="3"/>
-      <c r="H899" s="3"/>
-      <c r="I899" s="4"/>
-      <c r="J899" s="4"/>
+      <c r="A899" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="B899" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C899" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D899" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E899" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F899" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G899" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H899" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I899" s="4">
+        <f t="shared" si="54"/>
+        <v>2023</v>
+      </c>
+      <c r="J899" s="4">
+        <f t="shared" si="55"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="900" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A900" s="3"/>
-      <c r="B900" s="3"/>
-      <c r="C900" s="3"/>
-      <c r="D900" s="3"/>
-      <c r="E900" s="3"/>
-      <c r="F900" s="3"/>
-      <c r="G900" s="3"/>
-      <c r="H900" s="3"/>
-      <c r="I900" s="4"/>
-      <c r="J900" s="4"/>
+      <c r="A900" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="B900" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="C900" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="D900" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E900" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F900" s="3" t="s">
+        <v>982</v>
+      </c>
+      <c r="G900" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H900" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I900" s="4">
+        <f t="shared" ref="I900" si="56">YEAR(A900)</f>
+        <v>2023</v>
+      </c>
+      <c r="J900" s="4">
+        <f t="shared" ref="J900" si="57">MONTH(A900)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="901" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A901" s="3"/>

</xml_diff>

<commit_message>
#15 Time Tracking.*: updated to 2023-11-24.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7056" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7088" uniqueCount="995">
   <si>
     <t>Year</t>
   </si>
@@ -2998,6 +2998,15 @@
   </si>
   <si>
     <t>2023-11-22</t>
+  </si>
+  <si>
+    <t>2023-11-23</t>
+  </si>
+  <si>
+    <t>2023-11-24</t>
+  </si>
+  <si>
+    <t>nwtimetrackingmanager v1.2.0</t>
   </si>
 </sst>
 </file>
@@ -3401,7 +3410,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A881" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B901" sqref="B901"/>
+      <selection pane="bottomLeft" activeCell="C906" sqref="C906"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -33275,11 +33284,11 @@
         <v>283</v>
       </c>
       <c r="I887" s="4">
-        <f t="shared" ref="I887:I898" si="52">YEAR(A887)</f>
+        <f t="shared" ref="I887:I897" si="52">YEAR(A887)</f>
         <v>2023</v>
       </c>
       <c r="J887" s="4">
-        <f t="shared" ref="J887:J898" si="53">MONTH(A887)</f>
+        <f t="shared" ref="J887:J897" si="53">MONTH(A887)</f>
         <v>11</v>
       </c>
     </row>
@@ -33717,61 +33726,149 @@
         <v>282</v>
       </c>
       <c r="I900" s="4">
-        <f t="shared" ref="I900" si="56">YEAR(A900)</f>
+        <f t="shared" ref="I900:I902" si="56">YEAR(A900)</f>
         <v>2023</v>
       </c>
       <c r="J900" s="4">
-        <f t="shared" ref="J900" si="57">MONTH(A900)</f>
+        <f t="shared" ref="J900:J902" si="57">MONTH(A900)</f>
         <v>11</v>
       </c>
     </row>
     <row r="901" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A901" s="3"/>
-      <c r="B901" s="3"/>
-      <c r="C901" s="3"/>
-      <c r="D901" s="3"/>
-      <c r="E901" s="3"/>
-      <c r="F901" s="3"/>
-      <c r="G901" s="3"/>
-      <c r="H901" s="3"/>
-      <c r="I901" s="4"/>
-      <c r="J901" s="4"/>
+      <c r="A901" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B901" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C901" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D901" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E901" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F901" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="G901" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H901" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I901" s="4">
+        <f t="shared" si="56"/>
+        <v>2023</v>
+      </c>
+      <c r="J901" s="4">
+        <f t="shared" si="57"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="902" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A902" s="3"/>
-      <c r="B902" s="3"/>
-      <c r="C902" s="3"/>
-      <c r="D902" s="3"/>
-      <c r="E902" s="3"/>
-      <c r="F902" s="3"/>
-      <c r="G902" s="3"/>
-      <c r="H902" s="3"/>
-      <c r="I902" s="4"/>
-      <c r="J902" s="4"/>
+      <c r="A902" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B902" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C902" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D902" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E902" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F902" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="G902" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H902" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I902" s="4">
+        <f t="shared" si="56"/>
+        <v>2023</v>
+      </c>
+      <c r="J902" s="4">
+        <f t="shared" si="57"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="903" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A903" s="3"/>
-      <c r="B903" s="3"/>
-      <c r="C903" s="3"/>
-      <c r="D903" s="3"/>
-      <c r="E903" s="3"/>
-      <c r="F903" s="3"/>
-      <c r="G903" s="3"/>
-      <c r="H903" s="3"/>
-      <c r="I903" s="4"/>
-      <c r="J903" s="4"/>
+      <c r="A903" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="B903" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C903" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="D903" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E903" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F903" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="G903" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H903" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I903" s="4">
+        <f t="shared" ref="I903:I904" si="58">YEAR(A903)</f>
+        <v>2023</v>
+      </c>
+      <c r="J903" s="4">
+        <f t="shared" ref="J903:J904" si="59">MONTH(A903)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="904" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A904" s="3"/>
-      <c r="B904" s="3"/>
-      <c r="C904" s="3"/>
-      <c r="D904" s="3"/>
-      <c r="E904" s="3"/>
-      <c r="F904" s="3"/>
-      <c r="G904" s="3"/>
-      <c r="H904" s="3"/>
-      <c r="I904" s="4"/>
-      <c r="J904" s="4"/>
+      <c r="A904" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="B904" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C904" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="D904" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="E904" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F904" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="G904" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H904" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="I904" s="4">
+        <f t="shared" si="58"/>
+        <v>2023</v>
+      </c>
+      <c r="J904" s="4">
+        <f t="shared" si="59"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="905" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A905" s="3"/>

</xml_diff>

<commit_message>
#17 Time Tracking.*: updated to 2023-11-27.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7088" uniqueCount="992">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7120" uniqueCount="993">
   <si>
     <t>Year</t>
   </si>
@@ -2998,6 +2998,9 @@
   </si>
   <si>
     <t>nwtimetrackingmanager v1.2.0</t>
+  </si>
+  <si>
+    <t>2023-11-27</t>
   </si>
 </sst>
 </file>
@@ -3401,7 +3404,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A890" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F906" sqref="F906"/>
+      <selection pane="bottomLeft" activeCell="E910" sqref="E910"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -33862,52 +33865,140 @@
       </c>
     </row>
     <row r="905" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A905" s="3"/>
-      <c r="B905" s="3"/>
-      <c r="C905" s="3"/>
-      <c r="D905" s="3"/>
-      <c r="E905" s="3"/>
-      <c r="F905" s="3"/>
-      <c r="G905" s="3"/>
-      <c r="H905" s="3"/>
-      <c r="I905" s="4"/>
-      <c r="J905" s="4"/>
+      <c r="A905" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B905" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C905" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D905" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E905" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F905" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="G905" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H905" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I905" s="4">
+        <f t="shared" ref="I905:I906" si="60">YEAR(A905)</f>
+        <v>2023</v>
+      </c>
+      <c r="J905" s="4">
+        <f t="shared" ref="J905:J906" si="61">MONTH(A905)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="906" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A906" s="3"/>
-      <c r="B906" s="3"/>
-      <c r="C906" s="3"/>
-      <c r="D906" s="3"/>
-      <c r="E906" s="3"/>
-      <c r="F906" s="3"/>
-      <c r="G906" s="3"/>
-      <c r="H906" s="3"/>
-      <c r="I906" s="4"/>
-      <c r="J906" s="4"/>
+      <c r="A906" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B906" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C906" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D906" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E906" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F906" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="G906" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H906" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I906" s="4">
+        <f t="shared" ref="I906:I908" si="62">YEAR(A906)</f>
+        <v>2023</v>
+      </c>
+      <c r="J906" s="4">
+        <f t="shared" ref="J906:J908" si="63">MONTH(A906)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="907" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A907" s="3"/>
-      <c r="B907" s="3"/>
-      <c r="C907" s="3"/>
-      <c r="D907" s="3"/>
-      <c r="E907" s="3"/>
-      <c r="F907" s="3"/>
-      <c r="G907" s="3"/>
-      <c r="H907" s="3"/>
-      <c r="I907" s="4"/>
-      <c r="J907" s="4"/>
+      <c r="A907" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B907" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C907" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D907" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E907" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F907" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="G907" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H907" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I907" s="4">
+        <f t="shared" si="62"/>
+        <v>2023</v>
+      </c>
+      <c r="J907" s="4">
+        <f t="shared" si="63"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="908" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A908" s="3"/>
-      <c r="B908" s="3"/>
-      <c r="C908" s="3"/>
-      <c r="D908" s="3"/>
-      <c r="E908" s="3"/>
-      <c r="F908" s="3"/>
-      <c r="G908" s="3"/>
-      <c r="H908" s="3"/>
-      <c r="I908" s="4"/>
-      <c r="J908" s="4"/>
+      <c r="A908" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="B908" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C908" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D908" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E908" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F908" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="G908" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H908" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I908" s="4">
+        <f t="shared" si="62"/>
+        <v>2023</v>
+      </c>
+      <c r="J908" s="4">
+        <f t="shared" si="63"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="909" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A909" s="3"/>

</xml_diff>

<commit_message>
Time Tracking.xlsx: updated to 2023-12-30.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7120" uniqueCount="993">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7191" uniqueCount="1003">
   <si>
     <t>Year</t>
   </si>
@@ -3001,6 +3001,36 @@
   </si>
   <si>
     <t>2023-11-27</t>
+  </si>
+  <si>
+    <t>2023-11-28</t>
+  </si>
+  <si>
+    <t>2023-12-01</t>
+  </si>
+  <si>
+    <t>nwtimetrackingmanager v1.3.0</t>
+  </si>
+  <si>
+    <t>2023-12-02</t>
+  </si>
+  <si>
+    <t>2023-12-11</t>
+  </si>
+  <si>
+    <t>Overtime.</t>
+  </si>
+  <si>
+    <t>2023-12-12</t>
+  </si>
+  <si>
+    <t>2023-12-13</t>
+  </si>
+  <si>
+    <t>2023-12-14</t>
+  </si>
+  <si>
+    <t>2023-12-16</t>
   </si>
 </sst>
 </file>
@@ -3400,11 +3430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J919"/>
+  <dimension ref="A1:J928"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A890" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E910" sqref="E910"/>
+      <selection pane="bottomLeft" activeCell="E916" sqref="E916"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -33890,11 +33920,11 @@
         <v>281</v>
       </c>
       <c r="I905" s="4">
-        <f t="shared" ref="I905:I906" si="60">YEAR(A905)</f>
+        <f t="shared" ref="I905" si="60">YEAR(A905)</f>
         <v>2023</v>
       </c>
       <c r="J905" s="4">
-        <f t="shared" ref="J905:J906" si="61">MONTH(A905)</f>
+        <f t="shared" ref="J905" si="61">MONTH(A905)</f>
         <v>11</v>
       </c>
     </row>
@@ -33924,11 +33954,11 @@
         <v>281</v>
       </c>
       <c r="I906" s="4">
-        <f t="shared" ref="I906:I908" si="62">YEAR(A906)</f>
+        <f t="shared" ref="I906:I911" si="62">YEAR(A906)</f>
         <v>2023</v>
       </c>
       <c r="J906" s="4">
-        <f t="shared" ref="J906:J908" si="63">MONTH(A906)</f>
+        <f t="shared" ref="J906:J911" si="63">MONTH(A906)</f>
         <v>11</v>
       </c>
     </row>
@@ -34001,112 +34031,308 @@
       </c>
     </row>
     <row r="909" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A909" s="3"/>
-      <c r="B909" s="3"/>
-      <c r="C909" s="3"/>
-      <c r="D909" s="3"/>
-      <c r="E909" s="3"/>
+      <c r="A909" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="B909" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C909" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D909" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E909" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F909" s="3"/>
-      <c r="G909" s="3"/>
-      <c r="H909" s="3"/>
-      <c r="I909" s="4"/>
-      <c r="J909" s="4"/>
+      <c r="G909" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H909" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I909" s="4">
+        <f t="shared" si="62"/>
+        <v>2023</v>
+      </c>
+      <c r="J909" s="4">
+        <f t="shared" si="63"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="910" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A910" s="3"/>
-      <c r="B910" s="3"/>
-      <c r="C910" s="3"/>
-      <c r="D910" s="3"/>
-      <c r="E910" s="3"/>
-      <c r="F910" s="3"/>
-      <c r="G910" s="3"/>
-      <c r="H910" s="3"/>
-      <c r="I910" s="4"/>
-      <c r="J910" s="4"/>
+      <c r="A910" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="B910" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C910" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="D910" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E910" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F910" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G910" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H910" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I910" s="4">
+        <f t="shared" si="62"/>
+        <v>2023</v>
+      </c>
+      <c r="J910" s="4">
+        <f t="shared" si="63"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="911" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A911" s="3"/>
-      <c r="B911" s="3"/>
-      <c r="C911" s="3"/>
-      <c r="D911" s="3"/>
-      <c r="E911" s="3"/>
-      <c r="F911" s="3"/>
-      <c r="G911" s="3"/>
-      <c r="H911" s="3"/>
-      <c r="I911" s="4"/>
-      <c r="J911" s="4"/>
+      <c r="A911" s="3" t="s">
+        <v>994</v>
+      </c>
+      <c r="B911" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C911" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D911" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E911" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F911" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G911" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H911" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I911" s="4">
+        <f t="shared" si="62"/>
+        <v>2023</v>
+      </c>
+      <c r="J911" s="4">
+        <f t="shared" si="63"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="912" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A912" s="3"/>
-      <c r="B912" s="3"/>
-      <c r="C912" s="3"/>
-      <c r="D912" s="3"/>
-      <c r="E912" s="3"/>
-      <c r="F912" s="3"/>
-      <c r="G912" s="3"/>
-      <c r="H912" s="3"/>
-      <c r="I912" s="4"/>
-      <c r="J912" s="4"/>
+      <c r="A912" s="3" t="s">
+        <v>996</v>
+      </c>
+      <c r="B912" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C912" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D912" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E912" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F912" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G912" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H912" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I912" s="4">
+        <f t="shared" ref="I912" si="64">YEAR(A912)</f>
+        <v>2023</v>
+      </c>
+      <c r="J912" s="4">
+        <f t="shared" ref="J912" si="65">MONTH(A912)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="913" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A913" s="3"/>
-      <c r="B913" s="3"/>
-      <c r="C913" s="3"/>
-      <c r="D913" s="3"/>
-      <c r="E913" s="3"/>
-      <c r="F913" s="3"/>
-      <c r="G913" s="3"/>
-      <c r="H913" s="3"/>
-      <c r="I913" s="4"/>
-      <c r="J913" s="4"/>
+      <c r="A913" s="3" t="s">
+        <v>997</v>
+      </c>
+      <c r="B913" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C913" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D913" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E913" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F913" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="G913" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H913" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I913" s="4">
+        <f t="shared" ref="I913" si="66">YEAR(A913)</f>
+        <v>2023</v>
+      </c>
+      <c r="J913" s="4">
+        <f t="shared" ref="J913" si="67">MONTH(A913)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="914" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A914" s="3"/>
-      <c r="B914" s="3"/>
-      <c r="C914" s="3"/>
-      <c r="D914" s="3"/>
-      <c r="E914" s="3"/>
-      <c r="F914" s="3"/>
-      <c r="G914" s="3"/>
-      <c r="H914" s="3"/>
-      <c r="I914" s="4"/>
-      <c r="J914" s="4"/>
+      <c r="A914" s="3" t="s">
+        <v>999</v>
+      </c>
+      <c r="B914" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C914" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D914" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E914" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F914" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="G914" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H914" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I914" s="4">
+        <f t="shared" ref="I914" si="68">YEAR(A914)</f>
+        <v>2023</v>
+      </c>
+      <c r="J914" s="4">
+        <f t="shared" ref="J914" si="69">MONTH(A914)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="915" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A915" s="3"/>
-      <c r="B915" s="3"/>
-      <c r="C915" s="3"/>
-      <c r="D915" s="3"/>
-      <c r="E915" s="3"/>
-      <c r="F915" s="3"/>
-      <c r="G915" s="3"/>
-      <c r="H915" s="3"/>
-      <c r="I915" s="4"/>
-      <c r="J915" s="4"/>
+      <c r="A915" s="3" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B915" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C915" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D915" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E915" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F915" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="G915" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H915" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I915" s="4">
+        <f t="shared" ref="I915" si="70">YEAR(A915)</f>
+        <v>2023</v>
+      </c>
+      <c r="J915" s="4">
+        <f t="shared" ref="J915" si="71">MONTH(A915)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="916" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A916" s="3"/>
-      <c r="B916" s="3"/>
-      <c r="C916" s="3"/>
-      <c r="D916" s="3"/>
-      <c r="E916" s="3"/>
-      <c r="F916" s="3"/>
-      <c r="G916" s="3"/>
-      <c r="H916" s="3"/>
-      <c r="I916" s="4"/>
-      <c r="J916" s="4"/>
+      <c r="A916" s="3" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B916" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C916" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D916" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E916" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F916" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="G916" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H916" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I916" s="4">
+        <f t="shared" ref="I916" si="72">YEAR(A916)</f>
+        <v>2023</v>
+      </c>
+      <c r="J916" s="4">
+        <f t="shared" ref="J916" si="73">MONTH(A916)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="917" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A917" s="3"/>
-      <c r="B917" s="3"/>
-      <c r="C917" s="3"/>
-      <c r="D917" s="3"/>
-      <c r="E917" s="3"/>
-      <c r="F917" s="3"/>
-      <c r="G917" s="3"/>
-      <c r="H917" s="3"/>
-      <c r="I917" s="4"/>
-      <c r="J917" s="4"/>
+      <c r="A917" s="3" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B917" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C917" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D917" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E917" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F917" s="3" t="s">
+        <v>998</v>
+      </c>
+      <c r="G917" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H917" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I917" s="4">
+        <f t="shared" ref="I917" si="74">YEAR(A917)</f>
+        <v>2023</v>
+      </c>
+      <c r="J917" s="4">
+        <f t="shared" ref="J917" si="75">MONTH(A917)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="918" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A918" s="3"/>
@@ -34132,6 +34358,114 @@
       <c r="I919" s="4"/>
       <c r="J919" s="4"/>
     </row>
+    <row r="920" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A920" s="3"/>
+      <c r="B920" s="3"/>
+      <c r="C920" s="3"/>
+      <c r="D920" s="3"/>
+      <c r="E920" s="3"/>
+      <c r="F920" s="3"/>
+      <c r="G920" s="3"/>
+      <c r="H920" s="3"/>
+      <c r="I920" s="4"/>
+      <c r="J920" s="4"/>
+    </row>
+    <row r="921" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A921" s="3"/>
+      <c r="B921" s="3"/>
+      <c r="C921" s="3"/>
+      <c r="D921" s="3"/>
+      <c r="E921" s="3"/>
+      <c r="F921" s="3"/>
+      <c r="G921" s="3"/>
+      <c r="H921" s="3"/>
+      <c r="I921" s="4"/>
+      <c r="J921" s="4"/>
+    </row>
+    <row r="922" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A922" s="3"/>
+      <c r="B922" s="3"/>
+      <c r="C922" s="3"/>
+      <c r="D922" s="3"/>
+      <c r="E922" s="3"/>
+      <c r="F922" s="3"/>
+      <c r="G922" s="3"/>
+      <c r="H922" s="3"/>
+      <c r="I922" s="4"/>
+      <c r="J922" s="4"/>
+    </row>
+    <row r="923" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A923" s="3"/>
+      <c r="B923" s="3"/>
+      <c r="C923" s="3"/>
+      <c r="D923" s="3"/>
+      <c r="E923" s="3"/>
+      <c r="F923" s="3"/>
+      <c r="G923" s="3"/>
+      <c r="H923" s="3"/>
+      <c r="I923" s="4"/>
+      <c r="J923" s="4"/>
+    </row>
+    <row r="924" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A924" s="3"/>
+      <c r="B924" s="3"/>
+      <c r="C924" s="3"/>
+      <c r="D924" s="3"/>
+      <c r="E924" s="3"/>
+      <c r="F924" s="3"/>
+      <c r="G924" s="3"/>
+      <c r="H924" s="3"/>
+      <c r="I924" s="4"/>
+      <c r="J924" s="4"/>
+    </row>
+    <row r="925" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A925" s="3"/>
+      <c r="B925" s="3"/>
+      <c r="C925" s="3"/>
+      <c r="D925" s="3"/>
+      <c r="E925" s="3"/>
+      <c r="F925" s="3"/>
+      <c r="G925" s="3"/>
+      <c r="H925" s="3"/>
+      <c r="I925" s="4"/>
+      <c r="J925" s="4"/>
+    </row>
+    <row r="926" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A926" s="3"/>
+      <c r="B926" s="3"/>
+      <c r="C926" s="3"/>
+      <c r="D926" s="3"/>
+      <c r="E926" s="3"/>
+      <c r="F926" s="3"/>
+      <c r="G926" s="3"/>
+      <c r="H926" s="3"/>
+      <c r="I926" s="4"/>
+      <c r="J926" s="4"/>
+    </row>
+    <row r="927" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A927" s="3"/>
+      <c r="B927" s="3"/>
+      <c r="C927" s="3"/>
+      <c r="D927" s="3"/>
+      <c r="E927" s="3"/>
+      <c r="F927" s="3"/>
+      <c r="G927" s="3"/>
+      <c r="H927" s="3"/>
+      <c r="I927" s="4"/>
+      <c r="J927" s="4"/>
+    </row>
+    <row r="928" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A928" s="3"/>
+      <c r="B928" s="3"/>
+      <c r="C928" s="3"/>
+      <c r="D928" s="3"/>
+      <c r="E928" s="3"/>
+      <c r="F928" s="3"/>
+      <c r="G928" s="3"/>
+      <c r="H928" s="3"/>
+      <c r="I928" s="4"/>
+      <c r="J928" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Time Tracking.xlsx: updated to 2023-12-31.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7198" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7214" uniqueCount="1005">
   <si>
     <t>Year</t>
   </si>
@@ -3034,6 +3034,9 @@
   </si>
   <si>
     <t>2023-12-30</t>
+  </si>
+  <si>
+    <t>2023-12-31</t>
   </si>
 </sst>
 </file>
@@ -3436,8 +3439,8 @@
   <dimension ref="A1:J928"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A890" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F921" sqref="F921"/>
+      <pane ySplit="1" topLeftCell="A896" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D922" sqref="D922"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -34329,11 +34332,11 @@
         <v>282</v>
       </c>
       <c r="I917" s="4">
-        <f t="shared" ref="I917:I918" si="74">YEAR(A917)</f>
+        <f t="shared" ref="I917:I920" si="74">YEAR(A917)</f>
         <v>2023</v>
       </c>
       <c r="J917" s="4">
-        <f t="shared" ref="J917:J918" si="75">MONTH(A917)</f>
+        <f t="shared" ref="J917:J920" si="75">MONTH(A917)</f>
         <v>12</v>
       </c>
     </row>
@@ -34370,28 +34373,72 @@
       </c>
     </row>
     <row r="919" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A919" s="3"/>
-      <c r="B919" s="3"/>
-      <c r="C919" s="3"/>
-      <c r="D919" s="3"/>
-      <c r="E919" s="3"/>
-      <c r="F919" s="3"/>
-      <c r="G919" s="3"/>
-      <c r="H919" s="3"/>
-      <c r="I919" s="4"/>
-      <c r="J919" s="4"/>
+      <c r="A919" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B919" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C919" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D919" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E919" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F919" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G919" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H919" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I919" s="4">
+        <f t="shared" si="74"/>
+        <v>2023</v>
+      </c>
+      <c r="J919" s="4">
+        <f t="shared" si="75"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="920" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A920" s="3"/>
-      <c r="B920" s="3"/>
-      <c r="C920" s="3"/>
-      <c r="D920" s="3"/>
-      <c r="E920" s="3"/>
-      <c r="F920" s="3"/>
-      <c r="G920" s="3"/>
-      <c r="H920" s="3"/>
-      <c r="I920" s="4"/>
-      <c r="J920" s="4"/>
+      <c r="A920" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B920" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C920" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D920" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E920" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F920" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G920" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H920" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I920" s="4">
+        <f t="shared" si="74"/>
+        <v>2023</v>
+      </c>
+      <c r="J920" s="4">
+        <f t="shared" si="75"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="921" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A921" s="3"/>

</xml_diff>

<commit_message>
Time Tracking*: update 08.01.2024.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7214" uniqueCount="1005">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7267" uniqueCount="1010">
   <si>
     <t>Year</t>
   </si>
@@ -3037,6 +3037,21 @@
   </si>
   <si>
     <t>2023-12-31</t>
+  </si>
+  <si>
+    <t>2024-01-03</t>
+  </si>
+  <si>
+    <t>2024-01-04</t>
+  </si>
+  <si>
+    <t>2024-01-05</t>
+  </si>
+  <si>
+    <t>2024-01-06</t>
+  </si>
+  <si>
+    <t>2024-01-07</t>
   </si>
 </sst>
 </file>
@@ -3436,11 +3451,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J928"/>
+  <dimension ref="A1:J935"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A896" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D922" sqref="D922"/>
+      <pane ySplit="1" topLeftCell="A908" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A928" sqref="A928"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -34441,88 +34456,236 @@
       </c>
     </row>
     <row r="921" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A921" s="3"/>
-      <c r="B921" s="3"/>
-      <c r="C921" s="3"/>
-      <c r="D921" s="3"/>
-      <c r="E921" s="3"/>
-      <c r="F921" s="3"/>
-      <c r="G921" s="3"/>
-      <c r="H921" s="3"/>
-      <c r="I921" s="4"/>
-      <c r="J921" s="4"/>
+      <c r="A921" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B921" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C921" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D921" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E921" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F921" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G921" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H921" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I921" s="4">
+        <f t="shared" ref="I921" si="76">YEAR(A921)</f>
+        <v>2024</v>
+      </c>
+      <c r="J921" s="4">
+        <f t="shared" ref="J921" si="77">MONTH(A921)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="922" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A922" s="3"/>
-      <c r="B922" s="3"/>
-      <c r="C922" s="3"/>
-      <c r="D922" s="3"/>
-      <c r="E922" s="3"/>
-      <c r="F922" s="3"/>
-      <c r="G922" s="3"/>
-      <c r="H922" s="3"/>
-      <c r="I922" s="4"/>
-      <c r="J922" s="4"/>
+      <c r="A922" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B922" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C922" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D922" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E922" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F922" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G922" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H922" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I922" s="4">
+        <f t="shared" ref="I922" si="78">YEAR(A922)</f>
+        <v>2024</v>
+      </c>
+      <c r="J922" s="4">
+        <f t="shared" ref="J922" si="79">MONTH(A922)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="923" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A923" s="3"/>
-      <c r="B923" s="3"/>
-      <c r="C923" s="3"/>
-      <c r="D923" s="3"/>
-      <c r="E923" s="3"/>
-      <c r="F923" s="3"/>
-      <c r="G923" s="3"/>
-      <c r="H923" s="3"/>
-      <c r="I923" s="4"/>
-      <c r="J923" s="4"/>
+      <c r="A923" s="3" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B923" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C923" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D923" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E923" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F923" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G923" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H923" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I923" s="4">
+        <f t="shared" ref="I923" si="80">YEAR(A923)</f>
+        <v>2024</v>
+      </c>
+      <c r="J923" s="4">
+        <f t="shared" ref="J923" si="81">MONTH(A923)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="924" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A924" s="3"/>
-      <c r="B924" s="3"/>
-      <c r="C924" s="3"/>
-      <c r="D924" s="3"/>
-      <c r="E924" s="3"/>
-      <c r="F924" s="3"/>
-      <c r="G924" s="3"/>
-      <c r="H924" s="3"/>
-      <c r="I924" s="4"/>
-      <c r="J924" s="4"/>
+      <c r="A924" s="3" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B924" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C924" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D924" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E924" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F924" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G924" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H924" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I924" s="4">
+        <f t="shared" ref="I924:I926" si="82">YEAR(A924)</f>
+        <v>2024</v>
+      </c>
+      <c r="J924" s="4">
+        <f t="shared" ref="J924:J926" si="83">MONTH(A924)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="925" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A925" s="3"/>
-      <c r="B925" s="3"/>
-      <c r="C925" s="3"/>
-      <c r="D925" s="3"/>
-      <c r="E925" s="3"/>
+      <c r="A925" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B925" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C925" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D925" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E925" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F925" s="3"/>
-      <c r="G925" s="3"/>
-      <c r="H925" s="3"/>
-      <c r="I925" s="4"/>
-      <c r="J925" s="4"/>
+      <c r="G925" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H925" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I925" s="4">
+        <f t="shared" si="82"/>
+        <v>2024</v>
+      </c>
+      <c r="J925" s="4">
+        <f t="shared" si="83"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="926" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A926" s="3"/>
-      <c r="B926" s="3"/>
-      <c r="C926" s="3"/>
-      <c r="D926" s="3"/>
-      <c r="E926" s="3"/>
+      <c r="A926" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B926" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C926" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="D926" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E926" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F926" s="3"/>
-      <c r="G926" s="3"/>
-      <c r="H926" s="3"/>
-      <c r="I926" s="4"/>
-      <c r="J926" s="4"/>
+      <c r="G926" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H926" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I926" s="4">
+        <f t="shared" si="82"/>
+        <v>2024</v>
+      </c>
+      <c r="J926" s="4">
+        <f t="shared" si="83"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="927" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A927" s="3"/>
-      <c r="B927" s="3"/>
-      <c r="C927" s="3"/>
-      <c r="D927" s="3"/>
-      <c r="E927" s="3"/>
+      <c r="A927" s="3" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B927" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C927" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D927" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E927" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F927" s="3"/>
-      <c r="G927" s="3"/>
-      <c r="H927" s="3"/>
-      <c r="I927" s="4"/>
-      <c r="J927" s="4"/>
+      <c r="G927" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H927" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I927" s="4">
+        <f t="shared" ref="I927" si="84">YEAR(A927)</f>
+        <v>2024</v>
+      </c>
+      <c r="J927" s="4">
+        <f t="shared" ref="J927" si="85">MONTH(A927)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="928" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A928" s="3"/>
@@ -34536,6 +34699,90 @@
       <c r="I928" s="4"/>
       <c r="J928" s="4"/>
     </row>
+    <row r="929" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A929" s="3"/>
+      <c r="B929" s="3"/>
+      <c r="C929" s="3"/>
+      <c r="D929" s="3"/>
+      <c r="E929" s="3"/>
+      <c r="F929" s="3"/>
+      <c r="G929" s="3"/>
+      <c r="H929" s="3"/>
+      <c r="I929" s="4"/>
+      <c r="J929" s="4"/>
+    </row>
+    <row r="930" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A930" s="3"/>
+      <c r="B930" s="3"/>
+      <c r="C930" s="3"/>
+      <c r="D930" s="3"/>
+      <c r="E930" s="3"/>
+      <c r="F930" s="3"/>
+      <c r="G930" s="3"/>
+      <c r="H930" s="3"/>
+      <c r="I930" s="4"/>
+      <c r="J930" s="4"/>
+    </row>
+    <row r="931" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A931" s="3"/>
+      <c r="B931" s="3"/>
+      <c r="C931" s="3"/>
+      <c r="D931" s="3"/>
+      <c r="E931" s="3"/>
+      <c r="F931" s="3"/>
+      <c r="G931" s="3"/>
+      <c r="H931" s="3"/>
+      <c r="I931" s="4"/>
+      <c r="J931" s="4"/>
+    </row>
+    <row r="932" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A932" s="3"/>
+      <c r="B932" s="3"/>
+      <c r="C932" s="3"/>
+      <c r="D932" s="3"/>
+      <c r="E932" s="3"/>
+      <c r="F932" s="3"/>
+      <c r="G932" s="3"/>
+      <c r="H932" s="3"/>
+      <c r="I932" s="4"/>
+      <c r="J932" s="4"/>
+    </row>
+    <row r="933" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A933" s="3"/>
+      <c r="B933" s="3"/>
+      <c r="C933" s="3"/>
+      <c r="D933" s="3"/>
+      <c r="E933" s="3"/>
+      <c r="F933" s="3"/>
+      <c r="G933" s="3"/>
+      <c r="H933" s="3"/>
+      <c r="I933" s="4"/>
+      <c r="J933" s="4"/>
+    </row>
+    <row r="934" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A934" s="3"/>
+      <c r="B934" s="3"/>
+      <c r="C934" s="3"/>
+      <c r="D934" s="3"/>
+      <c r="E934" s="3"/>
+      <c r="F934" s="3"/>
+      <c r="G934" s="3"/>
+      <c r="H934" s="3"/>
+      <c r="I934" s="4"/>
+      <c r="J934" s="4"/>
+    </row>
+    <row r="935" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A935" s="3"/>
+      <c r="B935" s="3"/>
+      <c r="C935" s="3"/>
+      <c r="D935" s="3"/>
+      <c r="E935" s="3"/>
+      <c r="F935" s="3"/>
+      <c r="G935" s="3"/>
+      <c r="H935" s="3"/>
+      <c r="I935" s="4"/>
+      <c r="J935" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#18 Time Tracking.xlsx: updated to 2024-01-16.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7267" uniqueCount="1010">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7352" uniqueCount="1015">
   <si>
     <t>Year</t>
   </si>
@@ -3052,6 +3052,21 @@
   </si>
   <si>
     <t>2024-01-07</t>
+  </si>
+  <si>
+    <t>2024-01-11</t>
+  </si>
+  <si>
+    <t>2024-01-12</t>
+  </si>
+  <si>
+    <t>2024-01-14</t>
+  </si>
+  <si>
+    <t>2024-01-15</t>
+  </si>
+  <si>
+    <t>2024-01-16</t>
   </si>
 </sst>
 </file>
@@ -3451,11 +3466,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J935"/>
+  <dimension ref="A1:J947"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A908" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A928" sqref="A928"/>
+      <pane ySplit="1" topLeftCell="A922" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B939" sqref="B939"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -34679,109 +34694,489 @@
         <v>282</v>
       </c>
       <c r="I927" s="4">
-        <f t="shared" ref="I927" si="84">YEAR(A927)</f>
+        <f t="shared" ref="I927:I929" si="84">YEAR(A927)</f>
         <v>2024</v>
       </c>
       <c r="J927" s="4">
-        <f t="shared" ref="J927" si="85">MONTH(A927)</f>
+        <f t="shared" ref="J927:J929" si="85">MONTH(A927)</f>
         <v>1</v>
       </c>
     </row>
     <row r="928" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A928" s="3"/>
-      <c r="B928" s="3"/>
-      <c r="C928" s="3"/>
-      <c r="D928" s="3"/>
-      <c r="E928" s="3"/>
-      <c r="F928" s="3"/>
-      <c r="G928" s="3"/>
-      <c r="H928" s="3"/>
-      <c r="I928" s="4"/>
-      <c r="J928" s="4"/>
+      <c r="A928" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B928" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C928" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D928" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E928" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F928" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G928" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H928" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I928" s="4">
+        <f t="shared" si="84"/>
+        <v>2024</v>
+      </c>
+      <c r="J928" s="4">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="929" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A929" s="3"/>
-      <c r="B929" s="3"/>
-      <c r="C929" s="3"/>
-      <c r="D929" s="3"/>
-      <c r="E929" s="3"/>
-      <c r="F929" s="3"/>
-      <c r="G929" s="3"/>
-      <c r="H929" s="3"/>
-      <c r="I929" s="4"/>
-      <c r="J929" s="4"/>
+      <c r="A929" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B929" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C929" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D929" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E929" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F929" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G929" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H929" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I929" s="4">
+        <f t="shared" si="84"/>
+        <v>2024</v>
+      </c>
+      <c r="J929" s="4">
+        <f t="shared" si="85"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="930" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A930" s="3"/>
-      <c r="B930" s="3"/>
-      <c r="C930" s="3"/>
-      <c r="D930" s="3"/>
-      <c r="E930" s="3"/>
-      <c r="F930" s="3"/>
-      <c r="G930" s="3"/>
-      <c r="H930" s="3"/>
-      <c r="I930" s="4"/>
-      <c r="J930" s="4"/>
+      <c r="A930" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B930" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C930" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D930" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E930" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F930" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G930" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H930" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I930" s="4">
+        <f t="shared" ref="I930:I933" si="86">YEAR(A930)</f>
+        <v>2024</v>
+      </c>
+      <c r="J930" s="4">
+        <f t="shared" ref="J930:J933" si="87">MONTH(A930)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="931" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A931" s="3"/>
-      <c r="B931" s="3"/>
-      <c r="C931" s="3"/>
-      <c r="D931" s="3"/>
-      <c r="E931" s="3"/>
-      <c r="F931" s="3"/>
-      <c r="G931" s="3"/>
-      <c r="H931" s="3"/>
-      <c r="I931" s="4"/>
-      <c r="J931" s="4"/>
+      <c r="A931" s="3" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B931" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C931" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D931" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E931" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F931" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G931" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H931" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I931" s="4">
+        <f t="shared" si="86"/>
+        <v>2024</v>
+      </c>
+      <c r="J931" s="4">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="932" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A932" s="3"/>
-      <c r="B932" s="3"/>
-      <c r="C932" s="3"/>
-      <c r="D932" s="3"/>
-      <c r="E932" s="3"/>
+      <c r="A932" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B932" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C932" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D932" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E932" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F932" s="3"/>
-      <c r="G932" s="3"/>
-      <c r="H932" s="3"/>
-      <c r="I932" s="4"/>
-      <c r="J932" s="4"/>
+      <c r="G932" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H932" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I932" s="4">
+        <f t="shared" si="86"/>
+        <v>2024</v>
+      </c>
+      <c r="J932" s="4">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="933" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A933" s="3"/>
-      <c r="B933" s="3"/>
-      <c r="C933" s="3"/>
-      <c r="D933" s="3"/>
-      <c r="E933" s="3"/>
+      <c r="A933" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B933" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C933" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D933" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E933" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F933" s="3"/>
-      <c r="G933" s="3"/>
-      <c r="H933" s="3"/>
-      <c r="I933" s="4"/>
-      <c r="J933" s="4"/>
+      <c r="G933" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H933" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I933" s="4">
+        <f t="shared" si="86"/>
+        <v>2024</v>
+      </c>
+      <c r="J933" s="4">
+        <f t="shared" si="87"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="934" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A934" s="3"/>
-      <c r="B934" s="3"/>
-      <c r="C934" s="3"/>
-      <c r="D934" s="3"/>
-      <c r="E934" s="3"/>
-      <c r="F934" s="3"/>
-      <c r="G934" s="3"/>
-      <c r="H934" s="3"/>
-      <c r="I934" s="4"/>
-      <c r="J934" s="4"/>
+      <c r="A934" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B934" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C934" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D934" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E934" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F934" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G934" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H934" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I934" s="4">
+        <f t="shared" ref="I934" si="88">YEAR(A934)</f>
+        <v>2024</v>
+      </c>
+      <c r="J934" s="4">
+        <f t="shared" ref="J934" si="89">MONTH(A934)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="935" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A935" s="3"/>
-      <c r="B935" s="3"/>
-      <c r="C935" s="3"/>
-      <c r="D935" s="3"/>
-      <c r="E935" s="3"/>
+      <c r="A935" s="3" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B935" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C935" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D935" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E935" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F935" s="3"/>
-      <c r="G935" s="3"/>
-      <c r="H935" s="3"/>
-      <c r="I935" s="4"/>
-      <c r="J935" s="4"/>
+      <c r="G935" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H935" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I935" s="4">
+        <f t="shared" ref="I935:I938" si="90">YEAR(A935)</f>
+        <v>2024</v>
+      </c>
+      <c r="J935" s="4">
+        <f t="shared" ref="J935:J938" si="91">MONTH(A935)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="936" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A936" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B936" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C936" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D936" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E936" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F936" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G936" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H936" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I936" s="4">
+        <f t="shared" si="90"/>
+        <v>2024</v>
+      </c>
+      <c r="J936" s="4">
+        <f t="shared" si="91"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="937" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A937" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B937" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C937" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D937" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E937" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F937" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G937" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H937" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I937" s="4">
+        <f t="shared" si="90"/>
+        <v>2024</v>
+      </c>
+      <c r="J937" s="4">
+        <f t="shared" si="91"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="938" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A938" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B938" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C938" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D938" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E938" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F938" s="3" t="s">
+        <v>995</v>
+      </c>
+      <c r="G938" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H938" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I938" s="4">
+        <f t="shared" si="90"/>
+        <v>2024</v>
+      </c>
+      <c r="J938" s="4">
+        <f t="shared" si="91"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="939" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A939" s="3"/>
+      <c r="B939" s="3"/>
+      <c r="C939" s="3"/>
+      <c r="D939" s="3"/>
+      <c r="E939" s="3"/>
+      <c r="F939" s="3"/>
+      <c r="G939" s="3"/>
+      <c r="H939" s="3"/>
+      <c r="I939" s="4"/>
+      <c r="J939" s="4"/>
+    </row>
+    <row r="940" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A940" s="3"/>
+      <c r="B940" s="3"/>
+      <c r="C940" s="3"/>
+      <c r="D940" s="3"/>
+      <c r="E940" s="3"/>
+      <c r="F940" s="3"/>
+      <c r="G940" s="3"/>
+      <c r="H940" s="3"/>
+      <c r="I940" s="4"/>
+      <c r="J940" s="4"/>
+    </row>
+    <row r="941" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A941" s="3"/>
+      <c r="B941" s="3"/>
+      <c r="C941" s="3"/>
+      <c r="D941" s="3"/>
+      <c r="E941" s="3"/>
+      <c r="F941" s="3"/>
+      <c r="G941" s="3"/>
+      <c r="H941" s="3"/>
+      <c r="I941" s="4"/>
+      <c r="J941" s="4"/>
+    </row>
+    <row r="942" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A942" s="3"/>
+      <c r="B942" s="3"/>
+      <c r="C942" s="3"/>
+      <c r="D942" s="3"/>
+      <c r="E942" s="3"/>
+      <c r="F942" s="3"/>
+      <c r="G942" s="3"/>
+      <c r="H942" s="3"/>
+      <c r="I942" s="4"/>
+      <c r="J942" s="4"/>
+    </row>
+    <row r="943" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A943" s="3"/>
+      <c r="B943" s="3"/>
+      <c r="C943" s="3"/>
+      <c r="D943" s="3"/>
+      <c r="E943" s="3"/>
+      <c r="F943" s="3"/>
+      <c r="G943" s="3"/>
+      <c r="H943" s="3"/>
+      <c r="I943" s="4"/>
+      <c r="J943" s="4"/>
+    </row>
+    <row r="944" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A944" s="3"/>
+      <c r="B944" s="3"/>
+      <c r="C944" s="3"/>
+      <c r="D944" s="3"/>
+      <c r="E944" s="3"/>
+      <c r="F944" s="3"/>
+      <c r="G944" s="3"/>
+      <c r="H944" s="3"/>
+      <c r="I944" s="4"/>
+      <c r="J944" s="4"/>
+    </row>
+    <row r="945" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A945" s="3"/>
+      <c r="B945" s="3"/>
+      <c r="C945" s="3"/>
+      <c r="D945" s="3"/>
+      <c r="E945" s="3"/>
+      <c r="F945" s="3"/>
+      <c r="G945" s="3"/>
+      <c r="H945" s="3"/>
+      <c r="I945" s="4"/>
+      <c r="J945" s="4"/>
+    </row>
+    <row r="946" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A946" s="3"/>
+      <c r="B946" s="3"/>
+      <c r="C946" s="3"/>
+      <c r="D946" s="3"/>
+      <c r="E946" s="3"/>
+      <c r="F946" s="3"/>
+      <c r="G946" s="3"/>
+      <c r="H946" s="3"/>
+      <c r="I946" s="4"/>
+      <c r="J946" s="4"/>
+    </row>
+    <row r="947" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A947" s="3"/>
+      <c r="B947" s="3"/>
+      <c r="C947" s="3"/>
+      <c r="D947" s="3"/>
+      <c r="E947" s="3"/>
+      <c r="F947" s="3"/>
+      <c r="G947" s="3"/>
+      <c r="H947" s="3"/>
+      <c r="I947" s="4"/>
+      <c r="J947" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#20 Time Tracking.xlsx updated to 2024-01-21.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7352" uniqueCount="1015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7413" uniqueCount="1021">
   <si>
     <t>Year</t>
   </si>
@@ -3067,6 +3067,24 @@
   </si>
   <si>
     <t>2024-01-16</t>
+  </si>
+  <si>
+    <t>2024-01-17</t>
+  </si>
+  <si>
+    <t>2024-01-18</t>
+  </si>
+  <si>
+    <t>NW.MarkdownTables v3.0.0</t>
+  </si>
+  <si>
+    <t>2024-01-21</t>
+  </si>
+  <si>
+    <t>nwreadinglistmanager v2.0.0</t>
+  </si>
+  <si>
+    <t>nwtimetrackingmanager v2.0.0</t>
   </si>
 </sst>
 </file>
@@ -3466,11 +3484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J947"/>
+  <dimension ref="A1:J960"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A922" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B939" sqref="B939"/>
+      <pane ySplit="1" topLeftCell="A932" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F949" sqref="F949"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -35071,100 +35089,270 @@
       </c>
     </row>
     <row r="939" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A939" s="3"/>
-      <c r="B939" s="3"/>
-      <c r="C939" s="3"/>
-      <c r="D939" s="3"/>
-      <c r="E939" s="3"/>
+      <c r="A939" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B939" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C939" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D939" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E939" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F939" s="3"/>
-      <c r="G939" s="3"/>
-      <c r="H939" s="3"/>
-      <c r="I939" s="4"/>
-      <c r="J939" s="4"/>
+      <c r="G939" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H939" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I939" s="4">
+        <f t="shared" ref="I939:I942" si="92">YEAR(A939)</f>
+        <v>2024</v>
+      </c>
+      <c r="J939" s="4">
+        <f t="shared" ref="J939:J942" si="93">MONTH(A939)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="940" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A940" s="3"/>
-      <c r="B940" s="3"/>
-      <c r="C940" s="3"/>
-      <c r="D940" s="3"/>
-      <c r="E940" s="3"/>
+      <c r="A940" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B940" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C940" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D940" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E940" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F940" s="3"/>
-      <c r="G940" s="3"/>
-      <c r="H940" s="3"/>
-      <c r="I940" s="4"/>
-      <c r="J940" s="4"/>
+      <c r="G940" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H940" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I940" s="4">
+        <f t="shared" si="92"/>
+        <v>2024</v>
+      </c>
+      <c r="J940" s="4">
+        <f t="shared" si="93"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="941" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A941" s="3"/>
-      <c r="B941" s="3"/>
-      <c r="C941" s="3"/>
-      <c r="D941" s="3"/>
-      <c r="E941" s="3"/>
-      <c r="F941" s="3"/>
-      <c r="G941" s="3"/>
-      <c r="H941" s="3"/>
-      <c r="I941" s="4"/>
-      <c r="J941" s="4"/>
+      <c r="A941" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B941" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C941" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D941" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E941" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F941" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G941" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H941" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I941" s="4">
+        <f t="shared" si="92"/>
+        <v>2024</v>
+      </c>
+      <c r="J941" s="4">
+        <f t="shared" si="93"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="942" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A942" s="3"/>
-      <c r="B942" s="3"/>
-      <c r="C942" s="3"/>
-      <c r="D942" s="3"/>
-      <c r="E942" s="3"/>
-      <c r="F942" s="3"/>
-      <c r="G942" s="3"/>
-      <c r="H942" s="3"/>
-      <c r="I942" s="4"/>
-      <c r="J942" s="4"/>
+      <c r="A942" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B942" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C942" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D942" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E942" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F942" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G942" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H942" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I942" s="4">
+        <f t="shared" si="92"/>
+        <v>2024</v>
+      </c>
+      <c r="J942" s="4">
+        <f t="shared" si="93"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="943" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A943" s="3"/>
-      <c r="B943" s="3"/>
-      <c r="C943" s="3"/>
-      <c r="D943" s="3"/>
-      <c r="E943" s="3"/>
-      <c r="F943" s="3"/>
-      <c r="G943" s="3"/>
-      <c r="H943" s="3"/>
-      <c r="I943" s="4"/>
-      <c r="J943" s="4"/>
+      <c r="A943" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B943" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="C943" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D943" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E943" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F943" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="G943" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H943" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I943" s="4">
+        <f t="shared" ref="I943:I944" si="94">YEAR(A943)</f>
+        <v>2024</v>
+      </c>
+      <c r="J943" s="4">
+        <f t="shared" ref="J943:J944" si="95">MONTH(A943)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="944" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A944" s="3"/>
-      <c r="B944" s="3"/>
-      <c r="C944" s="3"/>
-      <c r="D944" s="3"/>
-      <c r="E944" s="3"/>
+      <c r="A944" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B944" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C944" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D944" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E944" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F944" s="3"/>
-      <c r="G944" s="3"/>
-      <c r="H944" s="3"/>
-      <c r="I944" s="4"/>
-      <c r="J944" s="4"/>
+      <c r="G944" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H944" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I944" s="4">
+        <f t="shared" si="94"/>
+        <v>2024</v>
+      </c>
+      <c r="J944" s="4">
+        <f t="shared" si="95"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="945" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A945" s="3"/>
-      <c r="B945" s="3"/>
-      <c r="C945" s="3"/>
-      <c r="D945" s="3"/>
-      <c r="E945" s="3"/>
-      <c r="F945" s="3"/>
-      <c r="G945" s="3"/>
-      <c r="H945" s="3"/>
-      <c r="I945" s="4"/>
-      <c r="J945" s="4"/>
+      <c r="A945" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B945" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C945" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D945" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E945" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F945" s="3" t="s">
+        <v>1019</v>
+      </c>
+      <c r="G945" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H945" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I945" s="4">
+        <f t="shared" ref="I945:I946" si="96">YEAR(A945)</f>
+        <v>2024</v>
+      </c>
+      <c r="J945" s="4">
+        <f t="shared" ref="J945:J946" si="97">MONTH(A945)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="946" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A946" s="3"/>
-      <c r="B946" s="3"/>
-      <c r="C946" s="3"/>
-      <c r="D946" s="3"/>
-      <c r="E946" s="3"/>
-      <c r="F946" s="3"/>
-      <c r="G946" s="3"/>
-      <c r="H946" s="3"/>
-      <c r="I946" s="4"/>
-      <c r="J946" s="4"/>
+      <c r="A946" s="3" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B946" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C946" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D946" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E946" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F946" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G946" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H946" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="I946" s="4">
+        <f t="shared" si="96"/>
+        <v>2024</v>
+      </c>
+      <c r="J946" s="4">
+        <f t="shared" si="97"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="947" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A947" s="3"/>
@@ -35178,6 +35366,162 @@
       <c r="I947" s="4"/>
       <c r="J947" s="4"/>
     </row>
+    <row r="948" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A948" s="3"/>
+      <c r="B948" s="3"/>
+      <c r="C948" s="3"/>
+      <c r="D948" s="3"/>
+      <c r="E948" s="3"/>
+      <c r="F948" s="3"/>
+      <c r="G948" s="3"/>
+      <c r="H948" s="3"/>
+      <c r="I948" s="4"/>
+      <c r="J948" s="4"/>
+    </row>
+    <row r="949" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A949" s="3"/>
+      <c r="B949" s="3"/>
+      <c r="C949" s="3"/>
+      <c r="D949" s="3"/>
+      <c r="E949" s="3"/>
+      <c r="F949" s="3"/>
+      <c r="G949" s="3"/>
+      <c r="H949" s="3"/>
+      <c r="I949" s="4"/>
+      <c r="J949" s="4"/>
+    </row>
+    <row r="950" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A950" s="3"/>
+      <c r="B950" s="3"/>
+      <c r="C950" s="3"/>
+      <c r="D950" s="3"/>
+      <c r="E950" s="3"/>
+      <c r="F950" s="3"/>
+      <c r="G950" s="3"/>
+      <c r="H950" s="3"/>
+      <c r="I950" s="4"/>
+      <c r="J950" s="4"/>
+    </row>
+    <row r="951" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A951" s="3"/>
+      <c r="B951" s="3"/>
+      <c r="C951" s="3"/>
+      <c r="D951" s="3"/>
+      <c r="E951" s="3"/>
+      <c r="F951" s="3"/>
+      <c r="G951" s="3"/>
+      <c r="H951" s="3"/>
+      <c r="I951" s="4"/>
+      <c r="J951" s="4"/>
+    </row>
+    <row r="952" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A952" s="3"/>
+      <c r="B952" s="3"/>
+      <c r="C952" s="3"/>
+      <c r="D952" s="3"/>
+      <c r="E952" s="3"/>
+      <c r="F952" s="3"/>
+      <c r="G952" s="3"/>
+      <c r="H952" s="3"/>
+      <c r="I952" s="4"/>
+      <c r="J952" s="4"/>
+    </row>
+    <row r="953" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A953" s="3"/>
+      <c r="B953" s="3"/>
+      <c r="C953" s="3"/>
+      <c r="D953" s="3"/>
+      <c r="E953" s="3"/>
+      <c r="F953" s="3"/>
+      <c r="G953" s="3"/>
+      <c r="H953" s="3"/>
+      <c r="I953" s="4"/>
+      <c r="J953" s="4"/>
+    </row>
+    <row r="954" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A954" s="3"/>
+      <c r="B954" s="3"/>
+      <c r="C954" s="3"/>
+      <c r="D954" s="3"/>
+      <c r="E954" s="3"/>
+      <c r="F954" s="3"/>
+      <c r="G954" s="3"/>
+      <c r="H954" s="3"/>
+      <c r="I954" s="4"/>
+      <c r="J954" s="4"/>
+    </row>
+    <row r="955" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A955" s="3"/>
+      <c r="B955" s="3"/>
+      <c r="C955" s="3"/>
+      <c r="D955" s="3"/>
+      <c r="E955" s="3"/>
+      <c r="F955" s="3"/>
+      <c r="G955" s="3"/>
+      <c r="H955" s="3"/>
+      <c r="I955" s="4"/>
+      <c r="J955" s="4"/>
+    </row>
+    <row r="956" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A956" s="3"/>
+      <c r="B956" s="3"/>
+      <c r="C956" s="3"/>
+      <c r="D956" s="3"/>
+      <c r="E956" s="3"/>
+      <c r="F956" s="3"/>
+      <c r="G956" s="3"/>
+      <c r="H956" s="3"/>
+      <c r="I956" s="4"/>
+      <c r="J956" s="4"/>
+    </row>
+    <row r="957" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A957" s="3"/>
+      <c r="B957" s="3"/>
+      <c r="C957" s="3"/>
+      <c r="D957" s="3"/>
+      <c r="E957" s="3"/>
+      <c r="F957" s="3"/>
+      <c r="G957" s="3"/>
+      <c r="H957" s="3"/>
+      <c r="I957" s="4"/>
+      <c r="J957" s="4"/>
+    </row>
+    <row r="958" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A958" s="3"/>
+      <c r="B958" s="3"/>
+      <c r="C958" s="3"/>
+      <c r="D958" s="3"/>
+      <c r="E958" s="3"/>
+      <c r="F958" s="3"/>
+      <c r="G958" s="3"/>
+      <c r="H958" s="3"/>
+      <c r="I958" s="4"/>
+      <c r="J958" s="4"/>
+    </row>
+    <row r="959" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A959" s="3"/>
+      <c r="B959" s="3"/>
+      <c r="C959" s="3"/>
+      <c r="D959" s="3"/>
+      <c r="E959" s="3"/>
+      <c r="F959" s="3"/>
+      <c r="G959" s="3"/>
+      <c r="H959" s="3"/>
+      <c r="I959" s="4"/>
+      <c r="J959" s="4"/>
+    </row>
+    <row r="960" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A960" s="3"/>
+      <c r="B960" s="3"/>
+      <c r="C960" s="3"/>
+      <c r="D960" s="3"/>
+      <c r="E960" s="3"/>
+      <c r="F960" s="3"/>
+      <c r="G960" s="3"/>
+      <c r="H960" s="3"/>
+      <c r="I960" s="4"/>
+      <c r="J960" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#20 Time Tracking.xlsx updated to 2024-01-23.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7413" uniqueCount="1021">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7437" uniqueCount="1023">
   <si>
     <t>Year</t>
   </si>
@@ -3085,6 +3085,12 @@
   </si>
   <si>
     <t>nwtimetrackingmanager v2.0.0</t>
+  </si>
+  <si>
+    <t>2024-01-22</t>
+  </si>
+  <si>
+    <t>2024-01-23</t>
   </si>
 </sst>
 </file>
@@ -3488,7 +3494,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A932" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F949" sqref="F949"/>
+      <selection pane="bottomLeft" activeCell="A950" sqref="A950"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -35342,8 +35348,8 @@
       <c r="G946" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="H946" s="3" t="s">
-        <v>281</v>
+      <c r="H946" s="8" t="s">
+        <v>282</v>
       </c>
       <c r="I946" s="4">
         <f t="shared" si="96"/>
@@ -35355,40 +35361,106 @@
       </c>
     </row>
     <row r="947" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A947" s="3"/>
-      <c r="B947" s="3"/>
-      <c r="C947" s="3"/>
-      <c r="D947" s="3"/>
-      <c r="E947" s="3"/>
-      <c r="F947" s="3"/>
-      <c r="G947" s="3"/>
-      <c r="H947" s="3"/>
-      <c r="I947" s="4"/>
-      <c r="J947" s="4"/>
+      <c r="A947" s="3" t="s">
+        <v>1021</v>
+      </c>
+      <c r="B947" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C947" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D947" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E947" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F947" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G947" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H947" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I947" s="4">
+        <f t="shared" ref="I947:I949" si="98">YEAR(A947)</f>
+        <v>2024</v>
+      </c>
+      <c r="J947" s="4">
+        <f t="shared" ref="J947:J949" si="99">MONTH(A947)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="948" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A948" s="3"/>
-      <c r="B948" s="3"/>
-      <c r="C948" s="3"/>
-      <c r="D948" s="3"/>
-      <c r="E948" s="3"/>
-      <c r="F948" s="3"/>
-      <c r="G948" s="3"/>
-      <c r="H948" s="3"/>
-      <c r="I948" s="4"/>
-      <c r="J948" s="4"/>
+      <c r="A948" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B948" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C948" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D948" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E948" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F948" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G948" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H948" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I948" s="4">
+        <f t="shared" si="98"/>
+        <v>2024</v>
+      </c>
+      <c r="J948" s="4">
+        <f t="shared" si="99"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="949" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A949" s="3"/>
-      <c r="B949" s="3"/>
-      <c r="C949" s="3"/>
-      <c r="D949" s="3"/>
-      <c r="E949" s="3"/>
-      <c r="F949" s="3"/>
-      <c r="G949" s="3"/>
-      <c r="H949" s="3"/>
-      <c r="I949" s="4"/>
-      <c r="J949" s="4"/>
+      <c r="A949" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B949" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C949" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D949" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E949" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F949" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G949" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H949" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I949" s="4">
+        <f t="shared" si="98"/>
+        <v>2024</v>
+      </c>
+      <c r="J949" s="4">
+        <f t="shared" si="99"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="950" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A950" s="3"/>

</xml_diff>

<commit_message>
#20 Time Tracking: updated to 2024-01-28.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7437" uniqueCount="1023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7504" uniqueCount="1029">
   <si>
     <t>Year</t>
   </si>
@@ -3091,6 +3091,24 @@
   </si>
   <si>
     <t>2024-01-23</t>
+  </si>
+  <si>
+    <t>2024-01-08</t>
+  </si>
+  <si>
+    <t>2024-01-24</t>
+  </si>
+  <si>
+    <t>2024-01-25</t>
+  </si>
+  <si>
+    <t>NW.NGramTextClassification v4.0.0</t>
+  </si>
+  <si>
+    <t>2024-01-26</t>
+  </si>
+  <si>
+    <t>2024-01-28</t>
   </si>
 </sst>
 </file>
@@ -3490,11 +3508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J960"/>
+  <dimension ref="A1:J962"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A932" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A950" sqref="A950"/>
+      <pane ySplit="1" topLeftCell="A923" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C941" sqref="C941"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -34718,37 +34736,35 @@
         <v>282</v>
       </c>
       <c r="I927" s="4">
-        <f t="shared" ref="I927:I929" si="84">YEAR(A927)</f>
+        <f t="shared" ref="I927:I931" si="84">YEAR(A927)</f>
         <v>2024</v>
       </c>
       <c r="J927" s="4">
-        <f t="shared" ref="J927:J929" si="85">MONTH(A927)</f>
+        <f t="shared" ref="J927:J931" si="85">MONTH(A927)</f>
         <v>1</v>
       </c>
     </row>
     <row r="928" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A928" s="3" t="s">
-        <v>1010</v>
+        <v>1023</v>
       </c>
       <c r="B928" s="3" t="s">
         <v>248</v>
       </c>
       <c r="C928" s="3" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="D928" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="E928" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F928" s="3" t="s">
-        <v>995</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F928" s="3"/>
       <c r="G928" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H928" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H928" s="8" t="s">
         <v>282</v>
       </c>
       <c r="I928" s="4">
@@ -34762,7 +34778,7 @@
     </row>
     <row r="929" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A929" s="3" t="s">
-        <v>1010</v>
+        <v>1023</v>
       </c>
       <c r="B929" s="3" t="s">
         <v>118</v>
@@ -34774,63 +34790,61 @@
         <v>193</v>
       </c>
       <c r="E929" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F929" s="3"/>
+      <c r="G929" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H929" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I929" s="4">
+        <f t="shared" ref="I929" si="86">YEAR(A929)</f>
+        <v>2024</v>
+      </c>
+      <c r="J929" s="4">
+        <f t="shared" ref="J929" si="87">MONTH(A929)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="930" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A930" s="3" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B930" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C930" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D930" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E930" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="F929" s="3" t="s">
+      <c r="F930" s="3" t="s">
         <v>995</v>
       </c>
-      <c r="G929" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H929" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="I929" s="4">
+      <c r="G930" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H930" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="I930" s="4">
         <f t="shared" si="84"/>
         <v>2024</v>
       </c>
-      <c r="J929" s="4">
+      <c r="J930" s="4">
         <f t="shared" si="85"/>
         <v>1</v>
       </c>
     </row>
-    <row r="930" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A930" s="3" t="s">
-        <v>1011</v>
-      </c>
-      <c r="B930" s="3" t="s">
-        <v>248</v>
-      </c>
-      <c r="C930" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="D930" s="3" t="s">
-        <v>184</v>
-      </c>
-      <c r="E930" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F930" s="3" t="s">
-        <v>995</v>
-      </c>
-      <c r="G930" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H930" s="3" t="s">
-        <v>282</v>
-      </c>
-      <c r="I930" s="4">
-        <f t="shared" ref="I930:I933" si="86">YEAR(A930)</f>
-        <v>2024</v>
-      </c>
-      <c r="J930" s="4">
-        <f t="shared" ref="J930:J933" si="87">MONTH(A930)</f>
-        <v>1</v>
-      </c>
-    </row>
     <row r="931" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A931" s="3" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B931" s="3" t="s">
         <v>118</v>
@@ -34854,75 +34868,79 @@
         <v>282</v>
       </c>
       <c r="I931" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="84"/>
         <v>2024</v>
       </c>
       <c r="J931" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" si="85"/>
         <v>1</v>
       </c>
     </row>
     <row r="932" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A932" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B932" s="3" t="s">
-        <v>202</v>
+        <v>248</v>
       </c>
       <c r="C932" s="3" t="s">
-        <v>337</v>
+        <v>265</v>
       </c>
       <c r="D932" s="3" t="s">
-        <v>126</v>
+        <v>184</v>
       </c>
       <c r="E932" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F932" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="F932" s="3" t="s">
+        <v>995</v>
+      </c>
       <c r="G932" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="H932" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H932" s="3" t="s">
         <v>282</v>
       </c>
       <c r="I932" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" ref="I932:I935" si="88">YEAR(A932)</f>
         <v>2024</v>
       </c>
       <c r="J932" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" ref="J932:J935" si="89">MONTH(A932)</f>
         <v>1</v>
       </c>
     </row>
     <row r="933" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A933" s="3" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B933" s="3" t="s">
-        <v>160</v>
+        <v>118</v>
       </c>
       <c r="C933" s="3" t="s">
-        <v>123</v>
+        <v>150</v>
       </c>
       <c r="D933" s="3" t="s">
-        <v>115</v>
+        <v>193</v>
       </c>
       <c r="E933" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F933" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="F933" s="3" t="s">
+        <v>995</v>
+      </c>
       <c r="G933" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="H933" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H933" s="3" t="s">
         <v>282</v>
       </c>
       <c r="I933" s="4">
-        <f t="shared" si="86"/>
+        <f t="shared" si="88"/>
         <v>2024</v>
       </c>
       <c r="J933" s="4">
-        <f t="shared" si="87"/>
+        <f t="shared" si="89"/>
         <v>1</v>
       </c>
     </row>
@@ -34931,32 +34949,30 @@
         <v>1012</v>
       </c>
       <c r="B934" s="3" t="s">
-        <v>123</v>
+        <v>202</v>
       </c>
       <c r="C934" s="3" t="s">
-        <v>150</v>
+        <v>337</v>
       </c>
       <c r="D934" s="3" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="E934" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F934" s="3" t="s">
-        <v>995</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F934" s="3"/>
       <c r="G934" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H934" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H934" s="8" t="s">
         <v>282</v>
       </c>
       <c r="I934" s="4">
-        <f t="shared" ref="I934" si="88">YEAR(A934)</f>
+        <f t="shared" si="88"/>
         <v>2024</v>
       </c>
       <c r="J934" s="4">
-        <f t="shared" ref="J934" si="89">MONTH(A934)</f>
+        <f t="shared" si="89"/>
         <v>1</v>
       </c>
     </row>
@@ -34965,13 +34981,13 @@
         <v>1012</v>
       </c>
       <c r="B935" s="3" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="C935" s="3" t="s">
-        <v>113</v>
+        <v>123</v>
       </c>
       <c r="D935" s="3" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="E935" s="3" t="s">
         <v>140</v>
@@ -34984,26 +35000,26 @@
         <v>282</v>
       </c>
       <c r="I935" s="4">
-        <f t="shared" ref="I935:I938" si="90">YEAR(A935)</f>
+        <f t="shared" si="88"/>
         <v>2024</v>
       </c>
       <c r="J935" s="4">
-        <f t="shared" ref="J935:J938" si="91">MONTH(A935)</f>
+        <f t="shared" si="89"/>
         <v>1</v>
       </c>
     </row>
     <row r="936" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A936" s="3" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B936" s="3" t="s">
-        <v>267</v>
+        <v>123</v>
       </c>
       <c r="C936" s="3" t="s">
-        <v>255</v>
+        <v>150</v>
       </c>
       <c r="D936" s="3" t="s">
-        <v>193</v>
+        <v>111</v>
       </c>
       <c r="E936" s="3" t="s">
         <v>127</v>
@@ -35018,60 +35034,58 @@
         <v>282</v>
       </c>
       <c r="I936" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="I936" si="90">YEAR(A936)</f>
         <v>2024</v>
       </c>
       <c r="J936" s="4">
-        <f t="shared" si="91"/>
+        <f t="shared" ref="J936" si="91">MONTH(A936)</f>
         <v>1</v>
       </c>
     </row>
     <row r="937" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A937" s="3" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="B937" s="3" t="s">
-        <v>253</v>
+        <v>150</v>
       </c>
       <c r="C937" s="3" t="s">
-        <v>265</v>
+        <v>113</v>
       </c>
       <c r="D937" s="3" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="E937" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F937" s="3" t="s">
-        <v>995</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F937" s="3"/>
       <c r="G937" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H937" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I937" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" ref="I937:I940" si="92">YEAR(A937)</f>
         <v>2024</v>
       </c>
       <c r="J937" s="4">
-        <f t="shared" si="91"/>
+        <f t="shared" ref="J937:J940" si="93">MONTH(A937)</f>
         <v>1</v>
       </c>
     </row>
     <row r="938" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A938" s="3" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B938" s="3" t="s">
-        <v>149</v>
+        <v>267</v>
       </c>
       <c r="C938" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D938" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="E938" s="3" t="s">
         <v>127</v>
@@ -35082,72 +35096,76 @@
       <c r="G938" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="H938" s="8" t="s">
-        <v>281</v>
+      <c r="H938" s="3" t="s">
+        <v>282</v>
       </c>
       <c r="I938" s="4">
-        <f t="shared" si="90"/>
+        <f t="shared" si="92"/>
         <v>2024</v>
       </c>
       <c r="J938" s="4">
-        <f t="shared" si="91"/>
+        <f t="shared" si="93"/>
         <v>1</v>
       </c>
     </row>
     <row r="939" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A939" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B939" s="3" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C939" s="3" t="s">
         <v>265</v>
       </c>
       <c r="D939" s="3" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="E939" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F939" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="F939" s="3" t="s">
+        <v>995</v>
+      </c>
       <c r="G939" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H939" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I939" s="4">
-        <f t="shared" ref="I939:I942" si="92">YEAR(A939)</f>
+        <f t="shared" si="92"/>
         <v>2024</v>
       </c>
       <c r="J939" s="4">
-        <f t="shared" ref="J939:J942" si="93">MONTH(A939)</f>
+        <f t="shared" si="93"/>
         <v>1</v>
       </c>
     </row>
     <row r="940" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A940" s="3" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="B940" s="3" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="C940" s="3" t="s">
-        <v>150</v>
+        <v>267</v>
       </c>
       <c r="D940" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E940" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F940" s="3"/>
+        <v>127</v>
+      </c>
+      <c r="F940" s="3" t="s">
+        <v>995</v>
+      </c>
       <c r="G940" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H940" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="I940" s="4">
         <f t="shared" si="92"/>
@@ -35160,84 +35178,80 @@
     </row>
     <row r="941" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A941" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B941" s="3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C941" s="3" t="s">
-        <v>179</v>
+        <v>265</v>
       </c>
       <c r="D941" s="3" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="E941" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F941" s="3" t="s">
-        <v>1017</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F941" s="3"/>
       <c r="G941" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H941" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H941" s="8" t="s">
         <v>282</v>
       </c>
       <c r="I941" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" ref="I941:I944" si="94">YEAR(A941)</f>
         <v>2024</v>
       </c>
       <c r="J941" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" ref="J941:J944" si="95">MONTH(A941)</f>
         <v>1</v>
       </c>
     </row>
     <row r="942" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A942" s="3" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="B942" s="3" t="s">
-        <v>267</v>
+        <v>118</v>
       </c>
       <c r="C942" s="3" t="s">
-        <v>255</v>
+        <v>150</v>
       </c>
       <c r="D942" s="3" t="s">
         <v>193</v>
       </c>
       <c r="E942" s="3" t="s">
-        <v>155</v>
-      </c>
-      <c r="F942" s="3" t="s">
-        <v>1017</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F942" s="3"/>
       <c r="G942" s="8" t="s">
-        <v>281</v>
-      </c>
-      <c r="H942" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="H942" s="8" t="s">
         <v>282</v>
       </c>
       <c r="I942" s="4">
-        <f t="shared" si="92"/>
+        <f t="shared" si="94"/>
         <v>2024</v>
       </c>
       <c r="J942" s="4">
-        <f t="shared" si="93"/>
+        <f t="shared" si="95"/>
         <v>1</v>
       </c>
     </row>
     <row r="943" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A943" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B943" s="3" t="s">
-        <v>463</v>
+        <v>249</v>
       </c>
       <c r="C943" s="3" t="s">
-        <v>171</v>
+        <v>179</v>
       </c>
       <c r="D943" s="3" t="s">
-        <v>126</v>
+        <v>193</v>
       </c>
       <c r="E943" s="3" t="s">
         <v>155</v>
@@ -35249,38 +35263,40 @@
         <v>281</v>
       </c>
       <c r="H943" s="3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I943" s="4">
-        <f t="shared" ref="I943:I944" si="94">YEAR(A943)</f>
+        <f t="shared" si="94"/>
         <v>2024</v>
       </c>
       <c r="J943" s="4">
-        <f t="shared" ref="J943:J944" si="95">MONTH(A943)</f>
+        <f t="shared" si="95"/>
         <v>1</v>
       </c>
     </row>
     <row r="944" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A944" s="3" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="B944" s="3" t="s">
-        <v>171</v>
+        <v>267</v>
       </c>
       <c r="C944" s="3" t="s">
-        <v>267</v>
+        <v>255</v>
       </c>
       <c r="D944" s="3" t="s">
-        <v>105</v>
+        <v>193</v>
       </c>
       <c r="E944" s="3" t="s">
-        <v>140</v>
-      </c>
-      <c r="F944" s="3"/>
+        <v>155</v>
+      </c>
+      <c r="F944" s="3" t="s">
+        <v>1017</v>
+      </c>
       <c r="G944" s="8" t="s">
-        <v>282</v>
-      </c>
-      <c r="H944" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H944" s="3" t="s">
         <v>282</v>
       </c>
       <c r="I944" s="4">
@@ -35297,19 +35313,19 @@
         <v>1018</v>
       </c>
       <c r="B945" s="3" t="s">
-        <v>267</v>
+        <v>463</v>
       </c>
       <c r="C945" s="3" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D945" s="3" t="s">
-        <v>115</v>
+        <v>126</v>
       </c>
       <c r="E945" s="3" t="s">
-        <v>127</v>
+        <v>155</v>
       </c>
       <c r="F945" s="3" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="G945" s="8" t="s">
         <v>281</v>
@@ -35331,22 +35347,20 @@
         <v>1018</v>
       </c>
       <c r="B946" s="3" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C946" s="3" t="s">
-        <v>192</v>
+        <v>267</v>
       </c>
       <c r="D946" s="3" t="s">
         <v>105</v>
       </c>
       <c r="E946" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="F946" s="3" t="s">
-        <v>1020</v>
-      </c>
+        <v>140</v>
+      </c>
+      <c r="F946" s="3"/>
       <c r="G946" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="H946" s="8" t="s">
         <v>282</v>
@@ -35362,50 +35376,50 @@
     </row>
     <row r="947" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A947" s="3" t="s">
-        <v>1021</v>
+        <v>1018</v>
       </c>
       <c r="B947" s="3" t="s">
-        <v>249</v>
+        <v>267</v>
       </c>
       <c r="C947" s="3" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
       <c r="D947" s="3" t="s">
-        <v>193</v>
+        <v>115</v>
       </c>
       <c r="E947" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F947" s="3" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="G947" s="8" t="s">
         <v>281</v>
       </c>
-      <c r="H947" s="8" t="s">
-        <v>282</v>
+      <c r="H947" s="3" t="s">
+        <v>281</v>
       </c>
       <c r="I947" s="4">
-        <f t="shared" ref="I947:I949" si="98">YEAR(A947)</f>
+        <f t="shared" ref="I947:I948" si="98">YEAR(A947)</f>
         <v>2024</v>
       </c>
       <c r="J947" s="4">
-        <f t="shared" ref="J947:J949" si="99">MONTH(A947)</f>
+        <f t="shared" ref="J947:J948" si="99">MONTH(A947)</f>
         <v>1</v>
       </c>
     </row>
     <row r="948" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A948" s="3" t="s">
-        <v>1022</v>
+        <v>1018</v>
       </c>
       <c r="B948" s="3" t="s">
-        <v>253</v>
+        <v>183</v>
       </c>
       <c r="C948" s="3" t="s">
-        <v>265</v>
+        <v>192</v>
       </c>
       <c r="D948" s="3" t="s">
-        <v>193</v>
+        <v>105</v>
       </c>
       <c r="E948" s="3" t="s">
         <v>127</v>
@@ -35417,7 +35431,7 @@
         <v>281</v>
       </c>
       <c r="H948" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I948" s="4">
         <f t="shared" si="98"/>
@@ -35430,13 +35444,13 @@
     </row>
     <row r="949" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A949" s="3" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B949" s="3" t="s">
-        <v>118</v>
+        <v>249</v>
       </c>
       <c r="C949" s="3" t="s">
-        <v>150</v>
+        <v>179</v>
       </c>
       <c r="D949" s="3" t="s">
         <v>193</v>
@@ -35451,124 +35465,316 @@
         <v>281</v>
       </c>
       <c r="H949" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I949" s="4">
-        <f t="shared" si="98"/>
+        <f t="shared" ref="I949:I953" si="100">YEAR(A949)</f>
         <v>2024</v>
       </c>
       <c r="J949" s="4">
-        <f t="shared" si="99"/>
+        <f t="shared" ref="J949:J953" si="101">MONTH(A949)</f>
         <v>1</v>
       </c>
     </row>
     <row r="950" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A950" s="3"/>
-      <c r="B950" s="3"/>
-      <c r="C950" s="3"/>
-      <c r="D950" s="3"/>
-      <c r="E950" s="3"/>
-      <c r="F950" s="3"/>
-      <c r="G950" s="3"/>
-      <c r="H950" s="3"/>
-      <c r="I950" s="4"/>
-      <c r="J950" s="4"/>
+      <c r="A950" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B950" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C950" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D950" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E950" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F950" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G950" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H950" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I950" s="4">
+        <f t="shared" si="100"/>
+        <v>2024</v>
+      </c>
+      <c r="J950" s="4">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="951" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A951" s="3"/>
-      <c r="B951" s="3"/>
-      <c r="C951" s="3"/>
-      <c r="D951" s="3"/>
-      <c r="E951" s="3"/>
-      <c r="F951" s="3"/>
-      <c r="G951" s="3"/>
-      <c r="H951" s="3"/>
-      <c r="I951" s="4"/>
-      <c r="J951" s="4"/>
+      <c r="A951" s="3" t="s">
+        <v>1022</v>
+      </c>
+      <c r="B951" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C951" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D951" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E951" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F951" s="3" t="s">
+        <v>1020</v>
+      </c>
+      <c r="G951" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H951" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I951" s="4">
+        <f t="shared" si="100"/>
+        <v>2024</v>
+      </c>
+      <c r="J951" s="4">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="952" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A952" s="3"/>
-      <c r="B952" s="3"/>
-      <c r="C952" s="3"/>
-      <c r="D952" s="3"/>
-      <c r="E952" s="3"/>
+      <c r="A952" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B952" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C952" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D952" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E952" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F952" s="3"/>
-      <c r="G952" s="3"/>
-      <c r="H952" s="3"/>
-      <c r="I952" s="4"/>
-      <c r="J952" s="4"/>
+      <c r="G952" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H952" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I952" s="4">
+        <f t="shared" si="100"/>
+        <v>2024</v>
+      </c>
+      <c r="J952" s="4">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="953" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A953" s="3"/>
-      <c r="B953" s="3"/>
-      <c r="C953" s="3"/>
-      <c r="D953" s="3"/>
-      <c r="E953" s="3"/>
-      <c r="F953" s="3"/>
-      <c r="G953" s="3"/>
-      <c r="H953" s="3"/>
-      <c r="I953" s="4"/>
-      <c r="J953" s="4"/>
+      <c r="A953" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B953" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C953" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D953" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E953" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F953" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G953" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H953" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I953" s="4">
+        <f t="shared" si="100"/>
+        <v>2024</v>
+      </c>
+      <c r="J953" s="4">
+        <f t="shared" si="101"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="954" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A954" s="3"/>
-      <c r="B954" s="3"/>
-      <c r="C954" s="3"/>
-      <c r="D954" s="3"/>
-      <c r="E954" s="3"/>
-      <c r="F954" s="3"/>
-      <c r="G954" s="3"/>
-      <c r="H954" s="3"/>
-      <c r="I954" s="4"/>
-      <c r="J954" s="4"/>
+      <c r="A954" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="B954" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C954" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D954" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E954" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F954" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G954" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H954" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I954" s="4">
+        <f t="shared" ref="I954:I955" si="102">YEAR(A954)</f>
+        <v>2024</v>
+      </c>
+      <c r="J954" s="4">
+        <f t="shared" ref="J954:J955" si="103">MONTH(A954)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="955" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A955" s="3"/>
-      <c r="B955" s="3"/>
-      <c r="C955" s="3"/>
-      <c r="D955" s="3"/>
-      <c r="E955" s="3"/>
-      <c r="F955" s="3"/>
-      <c r="G955" s="3"/>
-      <c r="H955" s="3"/>
-      <c r="I955" s="4"/>
-      <c r="J955" s="4"/>
+      <c r="A955" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B955" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C955" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D955" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E955" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F955" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G955" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H955" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I955" s="4">
+        <f t="shared" si="102"/>
+        <v>2024</v>
+      </c>
+      <c r="J955" s="4">
+        <f t="shared" si="103"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="956" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A956" s="3"/>
-      <c r="B956" s="3"/>
-      <c r="C956" s="3"/>
-      <c r="D956" s="3"/>
-      <c r="E956" s="3"/>
-      <c r="F956" s="3"/>
-      <c r="G956" s="3"/>
-      <c r="H956" s="3"/>
-      <c r="I956" s="4"/>
-      <c r="J956" s="4"/>
+      <c r="A956" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="B956" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C956" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D956" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E956" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F956" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G956" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H956" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I956" s="4">
+        <f t="shared" ref="I956:I958" si="104">YEAR(A956)</f>
+        <v>2024</v>
+      </c>
+      <c r="J956" s="4">
+        <f t="shared" ref="J956:J958" si="105">MONTH(A956)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="957" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A957" s="3"/>
-      <c r="B957" s="3"/>
-      <c r="C957" s="3"/>
-      <c r="D957" s="3"/>
-      <c r="E957" s="3"/>
+      <c r="A957" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B957" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C957" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D957" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E957" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F957" s="3"/>
-      <c r="G957" s="3"/>
-      <c r="H957" s="3"/>
-      <c r="I957" s="4"/>
-      <c r="J957" s="4"/>
+      <c r="G957" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H957" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I957" s="4">
+        <f t="shared" si="104"/>
+        <v>2024</v>
+      </c>
+      <c r="J957" s="4">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="958" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A958" s="3"/>
-      <c r="B958" s="3"/>
-      <c r="C958" s="3"/>
-      <c r="D958" s="3"/>
-      <c r="E958" s="3"/>
+      <c r="A958" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="B958" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C958" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D958" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="E958" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F958" s="3"/>
-      <c r="G958" s="3"/>
-      <c r="H958" s="3"/>
-      <c r="I958" s="4"/>
-      <c r="J958" s="4"/>
+      <c r="G958" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H958" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I958" s="4">
+        <f t="shared" si="104"/>
+        <v>2024</v>
+      </c>
+      <c r="J958" s="4">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="959" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A959" s="3"/>
@@ -35594,6 +35800,30 @@
       <c r="I960" s="4"/>
       <c r="J960" s="4"/>
     </row>
+    <row r="961" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A961" s="3"/>
+      <c r="B961" s="3"/>
+      <c r="C961" s="3"/>
+      <c r="D961" s="3"/>
+      <c r="E961" s="3"/>
+      <c r="F961" s="3"/>
+      <c r="G961" s="3"/>
+      <c r="H961" s="3"/>
+      <c r="I961" s="4"/>
+      <c r="J961" s="4"/>
+    </row>
+    <row r="962" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A962" s="3"/>
+      <c r="B962" s="3"/>
+      <c r="C962" s="3"/>
+      <c r="D962" s="3"/>
+      <c r="E962" s="3"/>
+      <c r="F962" s="3"/>
+      <c r="G962" s="3"/>
+      <c r="H962" s="3"/>
+      <c r="I962" s="4"/>
+      <c r="J962" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#20 Time Tracking.xlsx updated to 2024-02-06.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7504" uniqueCount="1029">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7606" uniqueCount="1035">
   <si>
     <t>Year</t>
   </si>
@@ -3109,6 +3109,24 @@
   </si>
   <si>
     <t>2024-01-28</t>
+  </si>
+  <si>
+    <t>2024-01-29</t>
+  </si>
+  <si>
+    <t>2024-01-30</t>
+  </si>
+  <si>
+    <t>2024-01-31</t>
+  </si>
+  <si>
+    <t>2024-02-01</t>
+  </si>
+  <si>
+    <t>2024-02-05</t>
+  </si>
+  <si>
+    <t>2024-02-06</t>
   </si>
 </sst>
 </file>
@@ -3508,11 +3526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J962"/>
+  <dimension ref="A1:J980"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A923" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C941" sqref="C941"/>
+      <pane ySplit="1" topLeftCell="A955" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D974" sqref="D974"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -35704,11 +35722,11 @@
         <v>282</v>
       </c>
       <c r="I956" s="4">
-        <f t="shared" ref="I956:I958" si="104">YEAR(A956)</f>
+        <f t="shared" ref="I956:I959" si="104">YEAR(A956)</f>
         <v>2024</v>
       </c>
       <c r="J956" s="4">
-        <f t="shared" ref="J956:J958" si="105">MONTH(A956)</f>
+        <f t="shared" ref="J956:J959" si="105">MONTH(A956)</f>
         <v>1</v>
       </c>
     </row>
@@ -35777,52 +35795,550 @@
       </c>
     </row>
     <row r="959" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A959" s="3"/>
-      <c r="B959" s="3"/>
-      <c r="C959" s="3"/>
-      <c r="D959" s="3"/>
-      <c r="E959" s="3"/>
-      <c r="F959" s="3"/>
-      <c r="G959" s="3"/>
-      <c r="H959" s="3"/>
-      <c r="I959" s="4"/>
-      <c r="J959" s="4"/>
+      <c r="A959" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B959" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C959" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D959" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E959" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F959" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G959" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H959" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I959" s="4">
+        <f t="shared" si="104"/>
+        <v>2024</v>
+      </c>
+      <c r="J959" s="4">
+        <f t="shared" si="105"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="960" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A960" s="3"/>
-      <c r="B960" s="3"/>
-      <c r="C960" s="3"/>
-      <c r="D960" s="3"/>
-      <c r="E960" s="3"/>
-      <c r="F960" s="3"/>
-      <c r="G960" s="3"/>
-      <c r="H960" s="3"/>
-      <c r="I960" s="4"/>
-      <c r="J960" s="4"/>
+      <c r="A960" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="B960" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C960" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D960" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E960" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F960" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G960" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H960" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I960" s="4">
+        <f t="shared" ref="I960:I961" si="106">YEAR(A960)</f>
+        <v>2024</v>
+      </c>
+      <c r="J960" s="4">
+        <f t="shared" ref="J960:J961" si="107">MONTH(A960)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="961" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A961" s="3"/>
-      <c r="B961" s="3"/>
-      <c r="C961" s="3"/>
-      <c r="D961" s="3"/>
-      <c r="E961" s="3"/>
-      <c r="F961" s="3"/>
-      <c r="G961" s="3"/>
-      <c r="H961" s="3"/>
-      <c r="I961" s="4"/>
-      <c r="J961" s="4"/>
+      <c r="A961" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B961" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C961" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D961" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E961" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F961" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G961" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H961" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I961" s="4">
+        <f t="shared" si="106"/>
+        <v>2024</v>
+      </c>
+      <c r="J961" s="4">
+        <f t="shared" si="107"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="962" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A962" s="3"/>
-      <c r="B962" s="3"/>
-      <c r="C962" s="3"/>
-      <c r="D962" s="3"/>
-      <c r="E962" s="3"/>
-      <c r="F962" s="3"/>
-      <c r="G962" s="3"/>
-      <c r="H962" s="3"/>
-      <c r="I962" s="4"/>
-      <c r="J962" s="4"/>
+      <c r="A962" s="3" t="s">
+        <v>1030</v>
+      </c>
+      <c r="B962" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C962" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D962" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E962" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F962" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G962" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H962" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I962" s="4">
+        <f t="shared" ref="I962:I963" si="108">YEAR(A962)</f>
+        <v>2024</v>
+      </c>
+      <c r="J962" s="4">
+        <f t="shared" ref="J962:J963" si="109">MONTH(A962)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="963" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A963" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B963" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C963" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D963" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E963" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F963" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G963" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H963" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I963" s="4">
+        <f t="shared" si="108"/>
+        <v>2024</v>
+      </c>
+      <c r="J963" s="4">
+        <f t="shared" si="109"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="964" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A964" s="3" t="s">
+        <v>1031</v>
+      </c>
+      <c r="B964" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C964" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D964" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E964" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F964" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G964" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H964" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I964" s="4">
+        <f t="shared" ref="I964:I965" si="110">YEAR(A964)</f>
+        <v>2024</v>
+      </c>
+      <c r="J964" s="4">
+        <f t="shared" ref="J964:J965" si="111">MONTH(A964)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="965" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A965" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B965" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C965" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D965" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E965" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F965" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G965" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H965" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I965" s="4">
+        <f t="shared" si="110"/>
+        <v>2024</v>
+      </c>
+      <c r="J965" s="4">
+        <f t="shared" si="111"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="966" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A966" s="3" t="s">
+        <v>1032</v>
+      </c>
+      <c r="B966" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C966" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D966" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E966" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F966" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G966" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H966" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I966" s="4">
+        <f t="shared" ref="I966:I968" si="112">YEAR(A966)</f>
+        <v>2024</v>
+      </c>
+      <c r="J966" s="4">
+        <f t="shared" ref="J966:J968" si="113">MONTH(A966)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="967" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A967" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B967" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C967" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D967" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E967" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F967" s="3"/>
+      <c r="G967" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H967" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I967" s="4">
+        <f t="shared" si="112"/>
+        <v>2024</v>
+      </c>
+      <c r="J967" s="4">
+        <f t="shared" si="113"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="968" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A968" s="3" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B968" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C968" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D968" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E968" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F968" s="3"/>
+      <c r="G968" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H968" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I968" s="4">
+        <f t="shared" si="112"/>
+        <v>2024</v>
+      </c>
+      <c r="J968" s="4">
+        <f t="shared" si="113"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="969" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A969" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B969" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C969" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D969" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E969" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F969" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G969" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H969" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I969" s="4">
+        <f t="shared" ref="I969:I971" si="114">YEAR(A969)</f>
+        <v>2024</v>
+      </c>
+      <c r="J969" s="4">
+        <f t="shared" ref="J969:J971" si="115">MONTH(A969)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="970" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A970" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B970" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C970" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D970" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E970" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F970" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G970" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H970" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I970" s="4">
+        <f t="shared" si="114"/>
+        <v>2024</v>
+      </c>
+      <c r="J970" s="4">
+        <f t="shared" si="115"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="971" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A971" s="3" t="s">
+        <v>1034</v>
+      </c>
+      <c r="B971" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C971" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D971" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E971" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F971" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G971" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H971" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I971" s="4">
+        <f t="shared" si="114"/>
+        <v>2024</v>
+      </c>
+      <c r="J971" s="4">
+        <f t="shared" si="115"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="972" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A972" s="3"/>
+      <c r="B972" s="3"/>
+      <c r="C972" s="3"/>
+      <c r="D972" s="3"/>
+      <c r="E972" s="3"/>
+      <c r="F972" s="3"/>
+      <c r="G972" s="3"/>
+      <c r="H972" s="3"/>
+      <c r="I972" s="4"/>
+      <c r="J972" s="4"/>
+    </row>
+    <row r="973" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A973" s="3"/>
+      <c r="B973" s="3"/>
+      <c r="C973" s="3"/>
+      <c r="D973" s="3"/>
+      <c r="E973" s="3"/>
+      <c r="F973" s="3"/>
+      <c r="G973" s="3"/>
+      <c r="H973" s="3"/>
+      <c r="I973" s="4"/>
+      <c r="J973" s="4"/>
+    </row>
+    <row r="974" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A974" s="3"/>
+      <c r="B974" s="3"/>
+      <c r="C974" s="3"/>
+      <c r="D974" s="3"/>
+      <c r="E974" s="3"/>
+      <c r="F974" s="3"/>
+      <c r="G974" s="3"/>
+      <c r="H974" s="3"/>
+      <c r="I974" s="4"/>
+      <c r="J974" s="4"/>
+    </row>
+    <row r="975" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A975" s="3"/>
+      <c r="B975" s="3"/>
+      <c r="C975" s="3"/>
+      <c r="D975" s="3"/>
+      <c r="E975" s="3"/>
+      <c r="F975" s="3"/>
+      <c r="G975" s="3"/>
+      <c r="H975" s="3"/>
+      <c r="I975" s="4"/>
+      <c r="J975" s="4"/>
+    </row>
+    <row r="976" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A976" s="3"/>
+      <c r="B976" s="3"/>
+      <c r="C976" s="3"/>
+      <c r="D976" s="3"/>
+      <c r="E976" s="3"/>
+      <c r="F976" s="3"/>
+      <c r="G976" s="3"/>
+      <c r="H976" s="3"/>
+      <c r="I976" s="4"/>
+      <c r="J976" s="4"/>
+    </row>
+    <row r="977" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A977" s="3"/>
+      <c r="B977" s="3"/>
+      <c r="C977" s="3"/>
+      <c r="D977" s="3"/>
+      <c r="E977" s="3"/>
+      <c r="F977" s="3"/>
+      <c r="G977" s="3"/>
+      <c r="H977" s="3"/>
+      <c r="I977" s="4"/>
+      <c r="J977" s="4"/>
+    </row>
+    <row r="978" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A978" s="3"/>
+      <c r="B978" s="3"/>
+      <c r="C978" s="3"/>
+      <c r="D978" s="3"/>
+      <c r="E978" s="3"/>
+      <c r="F978" s="3"/>
+      <c r="G978" s="3"/>
+      <c r="H978" s="3"/>
+      <c r="I978" s="4"/>
+      <c r="J978" s="4"/>
+    </row>
+    <row r="979" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A979" s="3"/>
+      <c r="B979" s="3"/>
+      <c r="C979" s="3"/>
+      <c r="D979" s="3"/>
+      <c r="E979" s="3"/>
+      <c r="F979" s="3"/>
+      <c r="G979" s="3"/>
+      <c r="H979" s="3"/>
+      <c r="I979" s="4"/>
+      <c r="J979" s="4"/>
+    </row>
+    <row r="980" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A980" s="3"/>
+      <c r="B980" s="3"/>
+      <c r="C980" s="3"/>
+      <c r="D980" s="3"/>
+      <c r="E980" s="3"/>
+      <c r="F980" s="3"/>
+      <c r="G980" s="3"/>
+      <c r="H980" s="3"/>
+      <c r="I980" s="4"/>
+      <c r="J980" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#20 Time Tracking.xlsx updated to 2024-02-18.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7606" uniqueCount="1035">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7775" uniqueCount="1052">
   <si>
     <t>Year</t>
   </si>
@@ -3127,6 +3127,57 @@
   </si>
   <si>
     <t>2024-02-06</t>
+  </si>
+  <si>
+    <t>2024-02-08</t>
+  </si>
+  <si>
+    <t>2024-02-09</t>
+  </si>
+  <si>
+    <t>NW.Shared.Files v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-02-10</t>
+  </si>
+  <si>
+    <t>NW.Shared.Validation v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-02-11</t>
+  </si>
+  <si>
+    <t>NW.UnivariateForecasting v4.1.0</t>
+  </si>
+  <si>
+    <t>2024-02-12</t>
+  </si>
+  <si>
+    <t>NW.NGramTextClassification v4.1.0</t>
+  </si>
+  <si>
+    <t>2024-02-13</t>
+  </si>
+  <si>
+    <t>NW.Shared.Serialization v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-02-14</t>
+  </si>
+  <si>
+    <t>NW.NGramTextClassification v4.2.0</t>
+  </si>
+  <si>
+    <t>NW.UnivariateForecasting v4.2.0</t>
+  </si>
+  <si>
+    <t>2024-02-15</t>
+  </si>
+  <si>
+    <t>2024-02-18</t>
+  </si>
+  <si>
+    <t>nwreadinglistmanager v2.1.0</t>
   </si>
 </sst>
 </file>
@@ -3526,11 +3577,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J980"/>
+  <dimension ref="A1:J1007"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A955" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D974" sqref="D974"/>
+      <pane ySplit="1" topLeftCell="A967" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G998" sqref="G998"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -36153,7 +36204,7 @@
         <v>281</v>
       </c>
       <c r="H969" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I969" s="4">
         <f t="shared" ref="I969:I971" si="114">YEAR(A969)</f>
@@ -36187,7 +36238,7 @@
         <v>281</v>
       </c>
       <c r="H970" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I970" s="4">
         <f t="shared" si="114"/>
@@ -36221,7 +36272,7 @@
         <v>281</v>
       </c>
       <c r="H971" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I971" s="4">
         <f t="shared" si="114"/>
@@ -36233,112 +36284,906 @@
       </c>
     </row>
     <row r="972" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A972" s="3"/>
-      <c r="B972" s="3"/>
-      <c r="C972" s="3"/>
-      <c r="D972" s="3"/>
-      <c r="E972" s="3"/>
-      <c r="F972" s="3"/>
-      <c r="G972" s="3"/>
-      <c r="H972" s="3"/>
-      <c r="I972" s="4"/>
-      <c r="J972" s="4"/>
+      <c r="A972" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B972" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C972" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D972" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E972" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F972" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G972" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H972" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I972" s="4">
+        <f t="shared" ref="I972:I974" si="116">YEAR(A972)</f>
+        <v>2024</v>
+      </c>
+      <c r="J972" s="4">
+        <f t="shared" ref="J972:J974" si="117">MONTH(A972)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="973" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A973" s="3"/>
-      <c r="B973" s="3"/>
-      <c r="C973" s="3"/>
-      <c r="D973" s="3"/>
-      <c r="E973" s="3"/>
-      <c r="F973" s="3"/>
-      <c r="G973" s="3"/>
-      <c r="H973" s="3"/>
-      <c r="I973" s="4"/>
-      <c r="J973" s="4"/>
+      <c r="A973" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B973" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C973" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D973" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E973" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F973" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G973" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H973" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I973" s="4">
+        <f t="shared" si="116"/>
+        <v>2024</v>
+      </c>
+      <c r="J973" s="4">
+        <f t="shared" si="117"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="974" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A974" s="3"/>
-      <c r="B974" s="3"/>
-      <c r="C974" s="3"/>
-      <c r="D974" s="3"/>
-      <c r="E974" s="3"/>
-      <c r="F974" s="3"/>
-      <c r="G974" s="3"/>
-      <c r="H974" s="3"/>
-      <c r="I974" s="4"/>
-      <c r="J974" s="4"/>
+      <c r="A974" s="3" t="s">
+        <v>1035</v>
+      </c>
+      <c r="B974" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C974" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D974" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E974" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F974" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G974" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H974" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I974" s="4">
+        <f t="shared" si="116"/>
+        <v>2024</v>
+      </c>
+      <c r="J974" s="4">
+        <f t="shared" si="117"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="975" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A975" s="3"/>
-      <c r="B975" s="3"/>
-      <c r="C975" s="3"/>
-      <c r="D975" s="3"/>
-      <c r="E975" s="3"/>
-      <c r="F975" s="3"/>
-      <c r="G975" s="3"/>
-      <c r="H975" s="3"/>
-      <c r="I975" s="4"/>
-      <c r="J975" s="4"/>
+      <c r="A975" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B975" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C975" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D975" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E975" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F975" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="G975" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H975" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I975" s="4">
+        <f t="shared" ref="I975:I976" si="118">YEAR(A975)</f>
+        <v>2024</v>
+      </c>
+      <c r="J975" s="4">
+        <f t="shared" ref="J975:J976" si="119">MONTH(A975)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="976" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A976" s="3"/>
-      <c r="B976" s="3"/>
-      <c r="C976" s="3"/>
-      <c r="D976" s="3"/>
-      <c r="E976" s="3"/>
-      <c r="F976" s="3"/>
-      <c r="G976" s="3"/>
-      <c r="H976" s="3"/>
-      <c r="I976" s="4"/>
-      <c r="J976" s="4"/>
+      <c r="A976" s="3" t="s">
+        <v>1036</v>
+      </c>
+      <c r="B976" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C976" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="D976" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E976" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F976" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G976" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H976" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I976" s="4">
+        <f t="shared" si="118"/>
+        <v>2024</v>
+      </c>
+      <c r="J976" s="4">
+        <f t="shared" si="119"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="977" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A977" s="3"/>
-      <c r="B977" s="3"/>
-      <c r="C977" s="3"/>
-      <c r="D977" s="3"/>
-      <c r="E977" s="3"/>
-      <c r="F977" s="3"/>
-      <c r="G977" s="3"/>
-      <c r="H977" s="3"/>
-      <c r="I977" s="4"/>
-      <c r="J977" s="4"/>
+      <c r="A977" s="3" t="s">
+        <v>1038</v>
+      </c>
+      <c r="B977" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C977" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D977" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E977" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F977" s="3" t="s">
+        <v>1039</v>
+      </c>
+      <c r="G977" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H977" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I977" s="4">
+        <f t="shared" ref="I977" si="120">YEAR(A977)</f>
+        <v>2024</v>
+      </c>
+      <c r="J977" s="4">
+        <f t="shared" ref="J977" si="121">MONTH(A977)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="978" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A978" s="3"/>
-      <c r="B978" s="3"/>
-      <c r="C978" s="3"/>
-      <c r="D978" s="3"/>
-      <c r="E978" s="3"/>
-      <c r="F978" s="3"/>
-      <c r="G978" s="3"/>
-      <c r="H978" s="3"/>
-      <c r="I978" s="4"/>
-      <c r="J978" s="4"/>
+      <c r="A978" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B978" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C978" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D978" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E978" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F978" s="3" t="s">
+        <v>1037</v>
+      </c>
+      <c r="G978" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H978" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I978" s="4">
+        <f t="shared" ref="I978:I979" si="122">YEAR(A978)</f>
+        <v>2024</v>
+      </c>
+      <c r="J978" s="4">
+        <f t="shared" ref="J978:J979" si="123">MONTH(A978)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="979" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A979" s="3"/>
-      <c r="B979" s="3"/>
-      <c r="C979" s="3"/>
-      <c r="D979" s="3"/>
-      <c r="E979" s="3"/>
-      <c r="F979" s="3"/>
-      <c r="G979" s="3"/>
-      <c r="H979" s="3"/>
-      <c r="I979" s="4"/>
-      <c r="J979" s="4"/>
+      <c r="A979" s="3" t="s">
+        <v>1040</v>
+      </c>
+      <c r="B979" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C979" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D979" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E979" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F979" s="3" t="s">
+        <v>1041</v>
+      </c>
+      <c r="G979" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H979" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I979" s="4">
+        <f t="shared" si="122"/>
+        <v>2024</v>
+      </c>
+      <c r="J979" s="4">
+        <f t="shared" si="123"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="980" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A980" s="3"/>
-      <c r="B980" s="3"/>
-      <c r="C980" s="3"/>
-      <c r="D980" s="3"/>
-      <c r="E980" s="3"/>
-      <c r="F980" s="3"/>
-      <c r="G980" s="3"/>
-      <c r="H980" s="3"/>
-      <c r="I980" s="4"/>
-      <c r="J980" s="4"/>
+      <c r="A980" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B980" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C980" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="D980" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E980" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F980" s="3" t="s">
+        <v>1043</v>
+      </c>
+      <c r="G980" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H980" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I980" s="4">
+        <f t="shared" ref="I980:I981" si="124">YEAR(A980)</f>
+        <v>2024</v>
+      </c>
+      <c r="J980" s="4">
+        <f t="shared" ref="J980:J981" si="125">MONTH(A980)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="981" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A981" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B981" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C981" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D981" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E981" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F981" s="3"/>
+      <c r="G981" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H981" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I981" s="4">
+        <f t="shared" si="124"/>
+        <v>2024</v>
+      </c>
+      <c r="J981" s="4">
+        <f t="shared" si="125"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="982" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A982" s="3" t="s">
+        <v>1042</v>
+      </c>
+      <c r="B982" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C982" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D982" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E982" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F982" s="3"/>
+      <c r="G982" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H982" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I982" s="4">
+        <f t="shared" ref="I982:I984" si="126">YEAR(A982)</f>
+        <v>2024</v>
+      </c>
+      <c r="J982" s="4">
+        <f t="shared" ref="J982:J984" si="127">MONTH(A982)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="983" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A983" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B983" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C983" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D983" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E983" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F983" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G983" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H983" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I983" s="4">
+        <f t="shared" si="126"/>
+        <v>2024</v>
+      </c>
+      <c r="J983" s="4">
+        <f t="shared" si="127"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="984" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A984" s="3" t="s">
+        <v>1044</v>
+      </c>
+      <c r="B984" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C984" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D984" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E984" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F984" s="3" t="s">
+        <v>1045</v>
+      </c>
+      <c r="G984" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H984" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I984" s="4">
+        <f t="shared" si="126"/>
+        <v>2024</v>
+      </c>
+      <c r="J984" s="4">
+        <f t="shared" si="127"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="985" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A985" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B985" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C985" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D985" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E985" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F985" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="G985" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H985" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I985" s="4">
+        <f t="shared" ref="I985:I987" si="128">YEAR(A985)</f>
+        <v>2024</v>
+      </c>
+      <c r="J985" s="4">
+        <f t="shared" ref="J985:J987" si="129">MONTH(A985)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="986" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A986" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B986" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C986" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D986" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E986" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F986" s="3" t="s">
+        <v>1047</v>
+      </c>
+      <c r="G986" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H986" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I986" s="4">
+        <f t="shared" si="128"/>
+        <v>2024</v>
+      </c>
+      <c r="J986" s="4">
+        <f t="shared" si="129"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="987" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A987" s="3" t="s">
+        <v>1046</v>
+      </c>
+      <c r="B987" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C987" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D987" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E987" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F987" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G987" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H987" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I987" s="4">
+        <f t="shared" si="128"/>
+        <v>2024</v>
+      </c>
+      <c r="J987" s="4">
+        <f t="shared" si="129"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="988" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A988" s="3" t="s">
+        <v>1049</v>
+      </c>
+      <c r="B988" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C988" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D988" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E988" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="F988" s="3" t="s">
+        <v>1048</v>
+      </c>
+      <c r="G988" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H988" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I988" s="4">
+        <f t="shared" ref="I988:I992" si="130">YEAR(A988)</f>
+        <v>2024</v>
+      </c>
+      <c r="J988" s="4">
+        <f t="shared" ref="J988:J992" si="131">MONTH(A988)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="989" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A989" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B989" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C989" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D989" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E989" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F989" s="3"/>
+      <c r="G989" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H989" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I989" s="4">
+        <f t="shared" si="130"/>
+        <v>2024</v>
+      </c>
+      <c r="J989" s="4">
+        <f t="shared" si="131"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="990" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A990" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B990" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C990" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D990" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E990" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F990" s="3"/>
+      <c r="G990" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H990" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I990" s="4">
+        <f t="shared" si="130"/>
+        <v>2024</v>
+      </c>
+      <c r="J990" s="4">
+        <f t="shared" si="131"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="991" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A991" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B991" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C991" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D991" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E991" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F991" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G991" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H991" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I991" s="4">
+        <f t="shared" si="130"/>
+        <v>2024</v>
+      </c>
+      <c r="J991" s="4">
+        <f t="shared" si="131"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="992" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A992" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B992" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C992" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D992" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E992" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F992" s="3" t="s">
+        <v>1051</v>
+      </c>
+      <c r="G992" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H992" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I992" s="4">
+        <f t="shared" si="130"/>
+        <v>2024</v>
+      </c>
+      <c r="J992" s="4">
+        <f t="shared" si="131"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="993" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A993" s="3" t="s">
+        <v>1050</v>
+      </c>
+      <c r="B993" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C993" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D993" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E993" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F993" s="3"/>
+      <c r="G993" s="3"/>
+      <c r="H993" s="3"/>
+      <c r="I993" s="4">
+        <f t="shared" ref="I993" si="132">YEAR(A993)</f>
+        <v>2024</v>
+      </c>
+      <c r="J993" s="4">
+        <f t="shared" ref="J993" si="133">MONTH(A993)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="994" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A994" s="3"/>
+      <c r="B994" s="3"/>
+      <c r="C994" s="3"/>
+      <c r="D994" s="3"/>
+      <c r="E994" s="3"/>
+      <c r="F994" s="3"/>
+      <c r="G994" s="3"/>
+      <c r="H994" s="3"/>
+      <c r="I994" s="4"/>
+      <c r="J994" s="4"/>
+    </row>
+    <row r="995" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A995" s="3"/>
+      <c r="B995" s="3"/>
+      <c r="C995" s="3"/>
+      <c r="D995" s="3"/>
+      <c r="E995" s="3"/>
+      <c r="F995" s="3"/>
+      <c r="G995" s="3"/>
+      <c r="H995" s="3"/>
+      <c r="I995" s="4"/>
+      <c r="J995" s="4"/>
+    </row>
+    <row r="996" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A996" s="3"/>
+      <c r="B996" s="3"/>
+      <c r="C996" s="3"/>
+      <c r="D996" s="3"/>
+      <c r="E996" s="3"/>
+      <c r="F996" s="3"/>
+      <c r="G996" s="3"/>
+      <c r="H996" s="3"/>
+      <c r="I996" s="4"/>
+      <c r="J996" s="4"/>
+    </row>
+    <row r="997" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A997" s="3"/>
+      <c r="B997" s="3"/>
+      <c r="C997" s="3"/>
+      <c r="D997" s="3"/>
+      <c r="E997" s="3"/>
+      <c r="F997" s="3"/>
+      <c r="G997" s="3"/>
+      <c r="H997" s="3"/>
+      <c r="I997" s="4"/>
+      <c r="J997" s="4"/>
+    </row>
+    <row r="998" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A998" s="3"/>
+      <c r="B998" s="3"/>
+      <c r="C998" s="3"/>
+      <c r="D998" s="3"/>
+      <c r="E998" s="3"/>
+      <c r="F998" s="3"/>
+      <c r="G998" s="3"/>
+      <c r="H998" s="3"/>
+      <c r="I998" s="4"/>
+      <c r="J998" s="4"/>
+    </row>
+    <row r="999" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A999" s="3"/>
+      <c r="B999" s="3"/>
+      <c r="C999" s="3"/>
+      <c r="D999" s="3"/>
+      <c r="E999" s="3"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="4"/>
+      <c r="J999" s="4"/>
+    </row>
+    <row r="1000" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1000" s="3"/>
+      <c r="B1000" s="3"/>
+      <c r="C1000" s="3"/>
+      <c r="D1000" s="3"/>
+      <c r="E1000" s="3"/>
+      <c r="F1000" s="3"/>
+      <c r="G1000" s="3"/>
+      <c r="H1000" s="3"/>
+      <c r="I1000" s="4"/>
+      <c r="J1000" s="4"/>
+    </row>
+    <row r="1001" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1001" s="3"/>
+      <c r="B1001" s="3"/>
+      <c r="C1001" s="3"/>
+      <c r="D1001" s="3"/>
+      <c r="E1001" s="3"/>
+      <c r="F1001" s="3"/>
+      <c r="G1001" s="3"/>
+      <c r="H1001" s="3"/>
+      <c r="I1001" s="4"/>
+      <c r="J1001" s="4"/>
+    </row>
+    <row r="1002" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1002" s="3"/>
+      <c r="B1002" s="3"/>
+      <c r="C1002" s="3"/>
+      <c r="D1002" s="3"/>
+      <c r="E1002" s="3"/>
+      <c r="F1002" s="3"/>
+      <c r="G1002" s="3"/>
+      <c r="H1002" s="3"/>
+      <c r="I1002" s="4"/>
+      <c r="J1002" s="4"/>
+    </row>
+    <row r="1003" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1003" s="3"/>
+      <c r="B1003" s="3"/>
+      <c r="C1003" s="3"/>
+      <c r="D1003" s="3"/>
+      <c r="E1003" s="3"/>
+      <c r="F1003" s="3"/>
+      <c r="G1003" s="3"/>
+      <c r="H1003" s="3"/>
+      <c r="I1003" s="4"/>
+      <c r="J1003" s="4"/>
+    </row>
+    <row r="1004" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1004" s="3"/>
+      <c r="B1004" s="3"/>
+      <c r="C1004" s="3"/>
+      <c r="D1004" s="3"/>
+      <c r="E1004" s="3"/>
+      <c r="F1004" s="3"/>
+      <c r="G1004" s="3"/>
+      <c r="H1004" s="3"/>
+      <c r="I1004" s="4"/>
+      <c r="J1004" s="4"/>
+    </row>
+    <row r="1005" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1005" s="3"/>
+      <c r="B1005" s="3"/>
+      <c r="C1005" s="3"/>
+      <c r="D1005" s="3"/>
+      <c r="E1005" s="3"/>
+      <c r="F1005" s="3"/>
+      <c r="G1005" s="3"/>
+      <c r="H1005" s="3"/>
+      <c r="I1005" s="4"/>
+      <c r="J1005" s="4"/>
+    </row>
+    <row r="1006" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1006" s="3"/>
+      <c r="B1006" s="3"/>
+      <c r="C1006" s="3"/>
+      <c r="D1006" s="3"/>
+      <c r="E1006" s="3"/>
+      <c r="F1006" s="3"/>
+      <c r="G1006" s="3"/>
+      <c r="H1006" s="3"/>
+      <c r="I1006" s="4"/>
+      <c r="J1006" s="4"/>
+    </row>
+    <row r="1007" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1007" s="3"/>
+      <c r="B1007" s="3"/>
+      <c r="C1007" s="3"/>
+      <c r="D1007" s="3"/>
+      <c r="E1007" s="3"/>
+      <c r="F1007" s="3"/>
+      <c r="G1007" s="3"/>
+      <c r="H1007" s="3"/>
+      <c r="I1007" s="4"/>
+      <c r="J1007" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#20 Time Tracking.xlsx updated to 2024-02-26.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7775" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7869" uniqueCount="1056">
   <si>
     <t>Year</t>
   </si>
@@ -3178,6 +3178,18 @@
   </si>
   <si>
     <t>nwreadinglistmanager v2.1.0</t>
+  </si>
+  <si>
+    <t>2024-02-19</t>
+  </si>
+  <si>
+    <t>2024-02-20</t>
+  </si>
+  <si>
+    <t>2024-02-25</t>
+  </si>
+  <si>
+    <t>2024-02-26</t>
   </si>
 </sst>
 </file>
@@ -3577,11 +3589,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1007"/>
+  <dimension ref="A1:J1025"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A967" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G998" sqref="G998"/>
+      <pane ySplit="1" topLeftCell="A979" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1007" sqref="D1007"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -37009,157 +37021,417 @@
       <c r="G993" s="3"/>
       <c r="H993" s="3"/>
       <c r="I993" s="4">
-        <f t="shared" ref="I993" si="132">YEAR(A993)</f>
+        <f t="shared" ref="I993:I996" si="132">YEAR(A993)</f>
         <v>2024</v>
       </c>
       <c r="J993" s="4">
-        <f t="shared" ref="J993" si="133">MONTH(A993)</f>
+        <f t="shared" ref="J993:J996" si="133">MONTH(A993)</f>
         <v>2</v>
       </c>
     </row>
     <row r="994" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A994" s="3"/>
-      <c r="B994" s="3"/>
-      <c r="C994" s="3"/>
-      <c r="D994" s="3"/>
-      <c r="E994" s="3"/>
-      <c r="F994" s="3"/>
-      <c r="G994" s="3"/>
-      <c r="H994" s="3"/>
-      <c r="I994" s="4"/>
-      <c r="J994" s="4"/>
+      <c r="A994" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B994" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C994" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D994" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E994" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F994" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G994" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H994" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I994" s="4">
+        <f t="shared" si="132"/>
+        <v>2024</v>
+      </c>
+      <c r="J994" s="4">
+        <f t="shared" si="133"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="995" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A995" s="3"/>
-      <c r="B995" s="3"/>
-      <c r="C995" s="3"/>
-      <c r="D995" s="3"/>
-      <c r="E995" s="3"/>
-      <c r="F995" s="3"/>
-      <c r="G995" s="3"/>
-      <c r="H995" s="3"/>
-      <c r="I995" s="4"/>
-      <c r="J995" s="4"/>
+      <c r="A995" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B995" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C995" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D995" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E995" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F995" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G995" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H995" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I995" s="4">
+        <f t="shared" si="132"/>
+        <v>2024</v>
+      </c>
+      <c r="J995" s="4">
+        <f t="shared" si="133"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="996" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A996" s="3"/>
-      <c r="B996" s="3"/>
-      <c r="C996" s="3"/>
-      <c r="D996" s="3"/>
-      <c r="E996" s="3"/>
-      <c r="F996" s="3"/>
-      <c r="G996" s="3"/>
-      <c r="H996" s="3"/>
-      <c r="I996" s="4"/>
-      <c r="J996" s="4"/>
+      <c r="A996" s="3" t="s">
+        <v>1052</v>
+      </c>
+      <c r="B996" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C996" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D996" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E996" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F996" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G996" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H996" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I996" s="4">
+        <f t="shared" si="132"/>
+        <v>2024</v>
+      </c>
+      <c r="J996" s="4">
+        <f t="shared" si="133"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="997" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A997" s="3"/>
-      <c r="B997" s="3"/>
-      <c r="C997" s="3"/>
-      <c r="D997" s="3"/>
-      <c r="E997" s="3"/>
-      <c r="F997" s="3"/>
-      <c r="G997" s="3"/>
-      <c r="H997" s="3"/>
-      <c r="I997" s="4"/>
-      <c r="J997" s="4"/>
+      <c r="A997" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B997" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C997" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D997" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E997" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F997" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G997" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H997" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I997" s="4">
+        <f t="shared" ref="I997:I999" si="134">YEAR(A997)</f>
+        <v>2024</v>
+      </c>
+      <c r="J997" s="4">
+        <f t="shared" ref="J997:J999" si="135">MONTH(A997)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="998" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A998" s="3"/>
-      <c r="B998" s="3"/>
-      <c r="C998" s="3"/>
-      <c r="D998" s="3"/>
-      <c r="E998" s="3"/>
-      <c r="F998" s="3"/>
-      <c r="G998" s="3"/>
-      <c r="H998" s="3"/>
-      <c r="I998" s="4"/>
-      <c r="J998" s="4"/>
+      <c r="A998" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B998" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C998" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D998" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E998" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F998" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G998" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H998" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I998" s="4">
+        <f t="shared" si="134"/>
+        <v>2024</v>
+      </c>
+      <c r="J998" s="4">
+        <f t="shared" si="135"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="999" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A999" s="3"/>
-      <c r="B999" s="3"/>
-      <c r="C999" s="3"/>
-      <c r="D999" s="3"/>
-      <c r="E999" s="3"/>
-      <c r="F999" s="3"/>
-      <c r="G999" s="3"/>
-      <c r="H999" s="3"/>
-      <c r="I999" s="4"/>
-      <c r="J999" s="4"/>
+      <c r="A999" s="3" t="s">
+        <v>1053</v>
+      </c>
+      <c r="B999" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C999" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D999" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E999" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F999" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G999" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H999" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I999" s="4">
+        <f t="shared" si="134"/>
+        <v>2024</v>
+      </c>
+      <c r="J999" s="4">
+        <f t="shared" si="135"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="1000" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1000" s="3"/>
-      <c r="B1000" s="3"/>
-      <c r="C1000" s="3"/>
-      <c r="D1000" s="3"/>
-      <c r="E1000" s="3"/>
-      <c r="F1000" s="3"/>
-      <c r="G1000" s="3"/>
-      <c r="H1000" s="3"/>
-      <c r="I1000" s="4"/>
-      <c r="J1000" s="4"/>
+      <c r="A1000" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B1000" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="C1000" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1000" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1000" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1000" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1000" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1000" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1000" s="4">
+        <f t="shared" ref="I1000:I1001" si="136">YEAR(A1000)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1000" s="4">
+        <f t="shared" ref="J1000:J1001" si="137">MONTH(A1000)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="1001" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1001" s="3"/>
-      <c r="B1001" s="3"/>
-      <c r="C1001" s="3"/>
-      <c r="D1001" s="3"/>
-      <c r="E1001" s="3"/>
-      <c r="F1001" s="3"/>
-      <c r="G1001" s="3"/>
-      <c r="H1001" s="3"/>
-      <c r="I1001" s="4"/>
-      <c r="J1001" s="4"/>
+      <c r="A1001" s="3" t="s">
+        <v>1054</v>
+      </c>
+      <c r="B1001" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1001" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1001" s="3" t="s">
+        <v>879</v>
+      </c>
+      <c r="E1001" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1001" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1001" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1001" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1001" s="4">
+        <f t="shared" si="136"/>
+        <v>2024</v>
+      </c>
+      <c r="J1001" s="4">
+        <f t="shared" si="137"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="1002" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1002" s="3"/>
-      <c r="B1002" s="3"/>
-      <c r="C1002" s="3"/>
-      <c r="D1002" s="3"/>
-      <c r="E1002" s="3"/>
-      <c r="F1002" s="3"/>
-      <c r="G1002" s="3"/>
-      <c r="H1002" s="3"/>
-      <c r="I1002" s="4"/>
-      <c r="J1002" s="4"/>
+      <c r="A1002" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1002" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1002" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1002" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1002" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1002" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1002" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1002" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1002" s="4">
+        <f t="shared" ref="I1002:I1005" si="138">YEAR(A1002)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1002" s="4">
+        <f t="shared" ref="J1002:J1005" si="139">MONTH(A1002)</f>
+        <v>2</v>
+      </c>
     </row>
     <row r="1003" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1003" s="3"/>
-      <c r="B1003" s="3"/>
-      <c r="C1003" s="3"/>
-      <c r="D1003" s="3"/>
-      <c r="E1003" s="3"/>
-      <c r="F1003" s="3"/>
-      <c r="G1003" s="3"/>
-      <c r="H1003" s="3"/>
-      <c r="I1003" s="4"/>
-      <c r="J1003" s="4"/>
+      <c r="A1003" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1003" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1003" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1003" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1003" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1003" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="G1003" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1003" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1003" s="4">
+        <f t="shared" si="138"/>
+        <v>2024</v>
+      </c>
+      <c r="J1003" s="4">
+        <f t="shared" si="139"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="1004" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1004" s="3"/>
-      <c r="B1004" s="3"/>
-      <c r="C1004" s="3"/>
-      <c r="D1004" s="3"/>
-      <c r="E1004" s="3"/>
+      <c r="A1004" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1004" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1004" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1004" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1004" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1004" s="3"/>
-      <c r="G1004" s="3"/>
-      <c r="H1004" s="3"/>
-      <c r="I1004" s="4"/>
-      <c r="J1004" s="4"/>
+      <c r="G1004" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1004" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1004" s="4">
+        <f t="shared" si="138"/>
+        <v>2024</v>
+      </c>
+      <c r="J1004" s="4">
+        <f t="shared" si="139"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="1005" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1005" s="3"/>
-      <c r="B1005" s="3"/>
-      <c r="C1005" s="3"/>
-      <c r="D1005" s="3"/>
-      <c r="E1005" s="3"/>
+      <c r="A1005" s="3" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1005" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1005" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1005" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1005" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1005" s="3"/>
-      <c r="G1005" s="3"/>
-      <c r="H1005" s="3"/>
-      <c r="I1005" s="4"/>
-      <c r="J1005" s="4"/>
+      <c r="G1005" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1005" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1005" s="4">
+        <f t="shared" si="138"/>
+        <v>2024</v>
+      </c>
+      <c r="J1005" s="4">
+        <f t="shared" si="139"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="1006" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1006" s="3"/>
@@ -37185,6 +37457,222 @@
       <c r="I1007" s="4"/>
       <c r="J1007" s="4"/>
     </row>
+    <row r="1008" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1008" s="3"/>
+      <c r="B1008" s="3"/>
+      <c r="C1008" s="3"/>
+      <c r="D1008" s="3"/>
+      <c r="E1008" s="3"/>
+      <c r="F1008" s="3"/>
+      <c r="G1008" s="3"/>
+      <c r="H1008" s="3"/>
+      <c r="I1008" s="4"/>
+      <c r="J1008" s="4"/>
+    </row>
+    <row r="1009" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1009" s="3"/>
+      <c r="B1009" s="3"/>
+      <c r="C1009" s="3"/>
+      <c r="D1009" s="3"/>
+      <c r="E1009" s="3"/>
+      <c r="F1009" s="3"/>
+      <c r="G1009" s="3"/>
+      <c r="H1009" s="3"/>
+      <c r="I1009" s="4"/>
+      <c r="J1009" s="4"/>
+    </row>
+    <row r="1010" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1010" s="3"/>
+      <c r="B1010" s="3"/>
+      <c r="C1010" s="3"/>
+      <c r="D1010" s="3"/>
+      <c r="E1010" s="3"/>
+      <c r="F1010" s="3"/>
+      <c r="G1010" s="3"/>
+      <c r="H1010" s="3"/>
+      <c r="I1010" s="4"/>
+      <c r="J1010" s="4"/>
+    </row>
+    <row r="1011" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1011" s="3"/>
+      <c r="B1011" s="3"/>
+      <c r="C1011" s="3"/>
+      <c r="D1011" s="3"/>
+      <c r="E1011" s="3"/>
+      <c r="F1011" s="3"/>
+      <c r="G1011" s="3"/>
+      <c r="H1011" s="3"/>
+      <c r="I1011" s="4"/>
+      <c r="J1011" s="4"/>
+    </row>
+    <row r="1012" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1012" s="3"/>
+      <c r="B1012" s="3"/>
+      <c r="C1012" s="3"/>
+      <c r="D1012" s="3"/>
+      <c r="E1012" s="3"/>
+      <c r="F1012" s="3"/>
+      <c r="G1012" s="3"/>
+      <c r="H1012" s="3"/>
+      <c r="I1012" s="4"/>
+      <c r="J1012" s="4"/>
+    </row>
+    <row r="1013" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1013" s="3"/>
+      <c r="B1013" s="3"/>
+      <c r="C1013" s="3"/>
+      <c r="D1013" s="3"/>
+      <c r="E1013" s="3"/>
+      <c r="F1013" s="3"/>
+      <c r="G1013" s="3"/>
+      <c r="H1013" s="3"/>
+      <c r="I1013" s="4"/>
+      <c r="J1013" s="4"/>
+    </row>
+    <row r="1014" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1014" s="3"/>
+      <c r="B1014" s="3"/>
+      <c r="C1014" s="3"/>
+      <c r="D1014" s="3"/>
+      <c r="E1014" s="3"/>
+      <c r="F1014" s="3"/>
+      <c r="G1014" s="3"/>
+      <c r="H1014" s="3"/>
+      <c r="I1014" s="4"/>
+      <c r="J1014" s="4"/>
+    </row>
+    <row r="1015" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1015" s="3"/>
+      <c r="B1015" s="3"/>
+      <c r="C1015" s="3"/>
+      <c r="D1015" s="3"/>
+      <c r="E1015" s="3"/>
+      <c r="F1015" s="3"/>
+      <c r="G1015" s="3"/>
+      <c r="H1015" s="3"/>
+      <c r="I1015" s="4"/>
+      <c r="J1015" s="4"/>
+    </row>
+    <row r="1016" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1016" s="3"/>
+      <c r="B1016" s="3"/>
+      <c r="C1016" s="3"/>
+      <c r="D1016" s="3"/>
+      <c r="E1016" s="3"/>
+      <c r="F1016" s="3"/>
+      <c r="G1016" s="3"/>
+      <c r="H1016" s="3"/>
+      <c r="I1016" s="4"/>
+      <c r="J1016" s="4"/>
+    </row>
+    <row r="1017" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1017" s="3"/>
+      <c r="B1017" s="3"/>
+      <c r="C1017" s="3"/>
+      <c r="D1017" s="3"/>
+      <c r="E1017" s="3"/>
+      <c r="F1017" s="3"/>
+      <c r="G1017" s="3"/>
+      <c r="H1017" s="3"/>
+      <c r="I1017" s="4"/>
+      <c r="J1017" s="4"/>
+    </row>
+    <row r="1018" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1018" s="3"/>
+      <c r="B1018" s="3"/>
+      <c r="C1018" s="3"/>
+      <c r="D1018" s="3"/>
+      <c r="E1018" s="3"/>
+      <c r="F1018" s="3"/>
+      <c r="G1018" s="3"/>
+      <c r="H1018" s="3"/>
+      <c r="I1018" s="4"/>
+      <c r="J1018" s="4"/>
+    </row>
+    <row r="1019" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1019" s="3"/>
+      <c r="B1019" s="3"/>
+      <c r="C1019" s="3"/>
+      <c r="D1019" s="3"/>
+      <c r="E1019" s="3"/>
+      <c r="F1019" s="3"/>
+      <c r="G1019" s="3"/>
+      <c r="H1019" s="3"/>
+      <c r="I1019" s="4"/>
+      <c r="J1019" s="4"/>
+    </row>
+    <row r="1020" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1020" s="3"/>
+      <c r="B1020" s="3"/>
+      <c r="C1020" s="3"/>
+      <c r="D1020" s="3"/>
+      <c r="E1020" s="3"/>
+      <c r="F1020" s="3"/>
+      <c r="G1020" s="3"/>
+      <c r="H1020" s="3"/>
+      <c r="I1020" s="4"/>
+      <c r="J1020" s="4"/>
+    </row>
+    <row r="1021" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1021" s="3"/>
+      <c r="B1021" s="3"/>
+      <c r="C1021" s="3"/>
+      <c r="D1021" s="3"/>
+      <c r="E1021" s="3"/>
+      <c r="F1021" s="3"/>
+      <c r="G1021" s="3"/>
+      <c r="H1021" s="3"/>
+      <c r="I1021" s="4"/>
+      <c r="J1021" s="4"/>
+    </row>
+    <row r="1022" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1022" s="3"/>
+      <c r="B1022" s="3"/>
+      <c r="C1022" s="3"/>
+      <c r="D1022" s="3"/>
+      <c r="E1022" s="3"/>
+      <c r="F1022" s="3"/>
+      <c r="G1022" s="3"/>
+      <c r="H1022" s="3"/>
+      <c r="I1022" s="4"/>
+      <c r="J1022" s="4"/>
+    </row>
+    <row r="1023" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1023" s="3"/>
+      <c r="B1023" s="3"/>
+      <c r="C1023" s="3"/>
+      <c r="D1023" s="3"/>
+      <c r="E1023" s="3"/>
+      <c r="F1023" s="3"/>
+      <c r="G1023" s="3"/>
+      <c r="H1023" s="3"/>
+      <c r="I1023" s="4"/>
+      <c r="J1023" s="4"/>
+    </row>
+    <row r="1024" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1024" s="3"/>
+      <c r="B1024" s="3"/>
+      <c r="C1024" s="3"/>
+      <c r="D1024" s="3"/>
+      <c r="E1024" s="3"/>
+      <c r="F1024" s="3"/>
+      <c r="G1024" s="3"/>
+      <c r="H1024" s="3"/>
+      <c r="I1024" s="4"/>
+      <c r="J1024" s="4"/>
+    </row>
+    <row r="1025" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1025" s="3"/>
+      <c r="B1025" s="3"/>
+      <c r="C1025" s="3"/>
+      <c r="D1025" s="3"/>
+      <c r="E1025" s="3"/>
+      <c r="F1025" s="3"/>
+      <c r="G1025" s="3"/>
+      <c r="H1025" s="3"/>
+      <c r="I1025" s="4"/>
+      <c r="J1025" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#20 notebook: updated to 2024-02-26.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -3592,8 +3592,8 @@
   <dimension ref="A1:J1025"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A979" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1007" sqref="D1007"/>
+      <pane ySplit="1" topLeftCell="A955" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E979" sqref="E979"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -36442,7 +36442,7 @@
         <v>463</v>
       </c>
       <c r="D976" s="3" t="s">
-        <v>111</v>
+        <v>168</v>
       </c>
       <c r="E976" s="3" t="s">
         <v>155</v>

</xml_diff>

<commit_message>
#24 Time Tracking.xlsx: updated to 3/19/2024.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7933" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8092" uniqueCount="1075">
   <si>
     <t>Year</t>
   </si>
@@ -3208,6 +3208,45 @@
   </si>
   <si>
     <t>2024-03-04</t>
+  </si>
+  <si>
+    <t>2024-03-05</t>
+  </si>
+  <si>
+    <t>8h 15m</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v3.0.0</t>
+  </si>
+  <si>
+    <t>2024-03-08</t>
+  </si>
+  <si>
+    <t>2024-03-09</t>
+  </si>
+  <si>
+    <t>2024-03-10</t>
+  </si>
+  <si>
+    <t>2024-03-11</t>
+  </si>
+  <si>
+    <t>2024-03-12</t>
+  </si>
+  <si>
+    <t>2024-03-14</t>
+  </si>
+  <si>
+    <t>2024-03-15</t>
+  </si>
+  <si>
+    <t>2024-03-16</t>
+  </si>
+  <si>
+    <t>2024-03-18</t>
+  </si>
+  <si>
+    <t>2024-03-19</t>
   </si>
 </sst>
 </file>
@@ -3607,11 +3646,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1025"/>
+  <dimension ref="A1:J1048"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A988" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1017" sqref="F1017"/>
+      <pane ySplit="1" topLeftCell="A1016" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1040" sqref="G1040"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -37542,7 +37581,7 @@
         <v>281</v>
       </c>
       <c r="H1008" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I1008" s="4">
         <f t="shared" ref="I1008" si="140">YEAR(A1008)</f>
@@ -37573,10 +37612,10 @@
         <v>1059</v>
       </c>
       <c r="G1009" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H1009" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I1009" s="4">
         <f t="shared" ref="I1009" si="142">YEAR(A1009)</f>
@@ -37607,10 +37646,10 @@
         <v>1059</v>
       </c>
       <c r="G1010" s="8" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H1010" s="8" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="I1010" s="4">
         <f t="shared" ref="I1010:I1013" si="144">YEAR(A1010)</f>
@@ -37724,148 +37763,862 @@
       </c>
     </row>
     <row r="1014" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1014" s="3"/>
-      <c r="B1014" s="3"/>
-      <c r="C1014" s="3"/>
-      <c r="D1014" s="3"/>
-      <c r="E1014" s="3"/>
-      <c r="F1014" s="3"/>
-      <c r="G1014" s="3"/>
-      <c r="H1014" s="3"/>
-      <c r="I1014" s="4"/>
-      <c r="J1014" s="4"/>
+      <c r="A1014" s="3" t="s">
+        <v>1062</v>
+      </c>
+      <c r="B1014" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1014" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1014" s="3" t="s">
+        <v>1063</v>
+      </c>
+      <c r="E1014" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1014" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1014" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1014" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1014" s="4">
+        <f t="shared" ref="I1014" si="146">YEAR(A1014)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1014" s="4">
+        <f t="shared" ref="J1014" si="147">MONTH(A1014)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1015" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1015" s="3"/>
-      <c r="B1015" s="3"/>
-      <c r="C1015" s="3"/>
-      <c r="D1015" s="3"/>
-      <c r="E1015" s="3"/>
-      <c r="F1015" s="3"/>
-      <c r="G1015" s="3"/>
-      <c r="H1015" s="3"/>
-      <c r="I1015" s="4"/>
-      <c r="J1015" s="4"/>
+      <c r="A1015" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1015" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1015" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1015" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1015" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1015" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1015" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1015" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1015" s="4">
+        <f t="shared" ref="I1015:I1017" si="148">YEAR(A1015)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1015" s="4">
+        <f t="shared" ref="J1015:J1017" si="149">MONTH(A1015)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1016" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1016" s="3"/>
-      <c r="B1016" s="3"/>
-      <c r="C1016" s="3"/>
-      <c r="D1016" s="3"/>
-      <c r="E1016" s="3"/>
-      <c r="F1016" s="3"/>
-      <c r="G1016" s="3"/>
-      <c r="H1016" s="3"/>
-      <c r="I1016" s="4"/>
-      <c r="J1016" s="4"/>
+      <c r="A1016" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1016" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1016" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1016" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1016" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1016" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1016" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1016" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1016" s="4">
+        <f t="shared" si="148"/>
+        <v>2024</v>
+      </c>
+      <c r="J1016" s="4">
+        <f t="shared" si="149"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1017" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1017" s="3"/>
-      <c r="B1017" s="3"/>
-      <c r="C1017" s="3"/>
-      <c r="D1017" s="3"/>
-      <c r="E1017" s="3"/>
-      <c r="F1017" s="3"/>
-      <c r="G1017" s="3"/>
-      <c r="H1017" s="3"/>
-      <c r="I1017" s="4"/>
-      <c r="J1017" s="4"/>
+      <c r="A1017" s="3" t="s">
+        <v>1065</v>
+      </c>
+      <c r="B1017" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1017" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1017" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1017" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1017" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1017" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1017" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1017" s="4">
+        <f t="shared" si="148"/>
+        <v>2024</v>
+      </c>
+      <c r="J1017" s="4">
+        <f t="shared" si="149"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1018" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1018" s="3"/>
-      <c r="B1018" s="3"/>
-      <c r="C1018" s="3"/>
-      <c r="D1018" s="3"/>
-      <c r="E1018" s="3"/>
-      <c r="F1018" s="3"/>
-      <c r="G1018" s="3"/>
-      <c r="H1018" s="3"/>
-      <c r="I1018" s="4"/>
-      <c r="J1018" s="4"/>
+      <c r="A1018" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1018" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1018" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1018" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1018" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1018" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1018" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1018" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1018" s="4">
+        <f t="shared" ref="I1018:I1020" si="150">YEAR(A1018)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1018" s="4">
+        <f t="shared" ref="J1018:J1020" si="151">MONTH(A1018)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1019" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1019" s="3"/>
-      <c r="B1019" s="3"/>
-      <c r="C1019" s="3"/>
-      <c r="D1019" s="3"/>
-      <c r="E1019" s="3"/>
-      <c r="F1019" s="3"/>
-      <c r="G1019" s="3"/>
-      <c r="H1019" s="3"/>
-      <c r="I1019" s="4"/>
-      <c r="J1019" s="4"/>
+      <c r="A1019" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1019" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1019" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1019" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1019" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1019" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1019" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1019" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1019" s="4">
+        <f t="shared" si="150"/>
+        <v>2024</v>
+      </c>
+      <c r="J1019" s="4">
+        <f t="shared" si="151"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1020" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1020" s="3"/>
-      <c r="B1020" s="3"/>
-      <c r="C1020" s="3"/>
-      <c r="D1020" s="3"/>
-      <c r="E1020" s="3"/>
-      <c r="F1020" s="3"/>
-      <c r="G1020" s="3"/>
-      <c r="H1020" s="3"/>
-      <c r="I1020" s="4"/>
-      <c r="J1020" s="4"/>
+      <c r="A1020" s="3" t="s">
+        <v>1066</v>
+      </c>
+      <c r="B1020" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1020" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="D1020" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1020" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1020" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1020" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1020" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1020" s="4">
+        <f t="shared" si="150"/>
+        <v>2024</v>
+      </c>
+      <c r="J1020" s="4">
+        <f t="shared" si="151"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1021" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1021" s="3"/>
-      <c r="B1021" s="3"/>
-      <c r="C1021" s="3"/>
-      <c r="D1021" s="3"/>
-      <c r="E1021" s="3"/>
-      <c r="F1021" s="3"/>
-      <c r="G1021" s="3"/>
-      <c r="H1021" s="3"/>
-      <c r="I1021" s="4"/>
-      <c r="J1021" s="4"/>
+      <c r="A1021" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1021" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="C1021" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1021" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1021" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1021" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1021" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1021" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1021" s="4">
+        <f t="shared" ref="I1021:I1022" si="152">YEAR(A1021)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1021" s="4">
+        <f t="shared" ref="J1021:J1022" si="153">MONTH(A1021)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1022" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1022" s="3"/>
-      <c r="B1022" s="3"/>
-      <c r="C1022" s="3"/>
-      <c r="D1022" s="3"/>
-      <c r="E1022" s="3"/>
-      <c r="F1022" s="3"/>
-      <c r="G1022" s="3"/>
-      <c r="H1022" s="3"/>
-      <c r="I1022" s="4"/>
-      <c r="J1022" s="4"/>
+      <c r="A1022" s="3" t="s">
+        <v>1067</v>
+      </c>
+      <c r="B1022" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1022" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1022" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="E1022" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1022" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1022" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1022" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1022" s="4">
+        <f t="shared" si="152"/>
+        <v>2024</v>
+      </c>
+      <c r="J1022" s="4">
+        <f t="shared" si="153"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1023" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1023" s="3"/>
-      <c r="B1023" s="3"/>
-      <c r="C1023" s="3"/>
-      <c r="D1023" s="3"/>
-      <c r="E1023" s="3"/>
-      <c r="F1023" s="3"/>
-      <c r="G1023" s="3"/>
-      <c r="H1023" s="3"/>
-      <c r="I1023" s="4"/>
-      <c r="J1023" s="4"/>
+      <c r="A1023" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1023" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1023" s="3" t="s">
+        <v>337</v>
+      </c>
+      <c r="D1023" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1023" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1023" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1023" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1023" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1023" s="4">
+        <f t="shared" ref="I1023:I1024" si="154">YEAR(A1023)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1023" s="4">
+        <f t="shared" ref="J1023:J1024" si="155">MONTH(A1023)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1024" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1024" s="3"/>
-      <c r="B1024" s="3"/>
-      <c r="C1024" s="3"/>
-      <c r="D1024" s="3"/>
-      <c r="E1024" s="3"/>
-      <c r="F1024" s="3"/>
-      <c r="G1024" s="3"/>
-      <c r="H1024" s="3"/>
-      <c r="I1024" s="4"/>
-      <c r="J1024" s="4"/>
+      <c r="A1024" s="3" t="s">
+        <v>1068</v>
+      </c>
+      <c r="B1024" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="C1024" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1024" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1024" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1024" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1024" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1024" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1024" s="4">
+        <f t="shared" si="154"/>
+        <v>2024</v>
+      </c>
+      <c r="J1024" s="4">
+        <f t="shared" si="155"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1025" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1025" s="3"/>
-      <c r="B1025" s="3"/>
-      <c r="C1025" s="3"/>
-      <c r="D1025" s="3"/>
-      <c r="E1025" s="3"/>
-      <c r="F1025" s="3"/>
-      <c r="G1025" s="3"/>
-      <c r="H1025" s="3"/>
-      <c r="I1025" s="4"/>
-      <c r="J1025" s="4"/>
+      <c r="A1025" s="3" t="s">
+        <v>1069</v>
+      </c>
+      <c r="B1025" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1025" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1025" s="3" t="s">
+        <v>351</v>
+      </c>
+      <c r="E1025" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1025" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1025" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1025" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1025" s="4">
+        <f t="shared" ref="I1025:I1028" si="156">YEAR(A1025)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1025" s="4">
+        <f t="shared" ref="J1025:J1028" si="157">MONTH(A1025)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1026" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1026" s="3" t="s">
+        <v>1070</v>
+      </c>
+      <c r="B1026" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1026" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1026" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1026" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1026" s="3"/>
+      <c r="G1026" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="H1026" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1026" s="4">
+        <f t="shared" si="156"/>
+        <v>2024</v>
+      </c>
+      <c r="J1026" s="4">
+        <f t="shared" si="157"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1027" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1027" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1027" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1027" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1027" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1027" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1027" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1027" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1027" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1027" s="4">
+        <f t="shared" si="156"/>
+        <v>2024</v>
+      </c>
+      <c r="J1027" s="4">
+        <f t="shared" si="157"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1028" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1028" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1028" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1028" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1028" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1028" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1028" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1028" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1028" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1028" s="4">
+        <f t="shared" si="156"/>
+        <v>2024</v>
+      </c>
+      <c r="J1028" s="4">
+        <f t="shared" si="157"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1029" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1029" s="3" t="s">
+        <v>1071</v>
+      </c>
+      <c r="B1029" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1029" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1029" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1029" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1029" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1029" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1029" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1029" s="4">
+        <f t="shared" ref="I1029:I1030" si="158">YEAR(A1029)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1029" s="4">
+        <f t="shared" ref="J1029:J1030" si="159">MONTH(A1029)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1030" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1030" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1030" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1030" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1030" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1030" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1030" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1030" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1030" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1030" s="4">
+        <f t="shared" si="158"/>
+        <v>2024</v>
+      </c>
+      <c r="J1030" s="4">
+        <f t="shared" si="159"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1031" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1031" s="3" t="s">
+        <v>1072</v>
+      </c>
+      <c r="B1031" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1031" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1031" s="3" t="s">
+        <v>976</v>
+      </c>
+      <c r="E1031" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1031" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1031" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1031" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1031" s="4">
+        <f t="shared" ref="I1031" si="160">YEAR(A1031)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1031" s="4">
+        <f t="shared" ref="J1031" si="161">MONTH(A1031)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1032" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1032" s="3" t="s">
+        <v>1073</v>
+      </c>
+      <c r="B1032" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1032" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1032" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="E1032" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1032" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1032" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1032" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1032" s="4">
+        <f t="shared" ref="I1032" si="162">YEAR(A1032)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1032" s="4">
+        <f t="shared" ref="J1032" si="163">MONTH(A1032)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1033" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1033" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1033" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1033" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="D1033" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1033" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1033" s="3" t="s">
+        <v>1064</v>
+      </c>
+      <c r="G1033" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1033" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1033" s="4">
+        <f t="shared" ref="I1033" si="164">YEAR(A1033)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1033" s="4">
+        <f t="shared" ref="J1033" si="165">MONTH(A1033)</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="1034" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1034" s="3"/>
+      <c r="B1034" s="3"/>
+      <c r="C1034" s="3"/>
+      <c r="D1034" s="3"/>
+      <c r="E1034" s="3"/>
+      <c r="F1034" s="3"/>
+      <c r="G1034" s="3"/>
+      <c r="H1034" s="3"/>
+      <c r="I1034" s="4"/>
+      <c r="J1034" s="4"/>
+    </row>
+    <row r="1035" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1035" s="3"/>
+      <c r="B1035" s="3"/>
+      <c r="C1035" s="3"/>
+      <c r="D1035" s="3"/>
+      <c r="E1035" s="3"/>
+      <c r="F1035" s="3"/>
+      <c r="G1035" s="3"/>
+      <c r="H1035" s="3"/>
+      <c r="I1035" s="4"/>
+      <c r="J1035" s="4"/>
+    </row>
+    <row r="1036" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1036" s="3"/>
+      <c r="B1036" s="3"/>
+      <c r="C1036" s="3"/>
+      <c r="D1036" s="3"/>
+      <c r="E1036" s="3"/>
+      <c r="F1036" s="3"/>
+      <c r="G1036" s="3"/>
+      <c r="H1036" s="3"/>
+      <c r="I1036" s="4"/>
+      <c r="J1036" s="4"/>
+    </row>
+    <row r="1037" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1037" s="3"/>
+      <c r="B1037" s="3"/>
+      <c r="C1037" s="3"/>
+      <c r="D1037" s="3"/>
+      <c r="E1037" s="3"/>
+      <c r="F1037" s="3"/>
+      <c r="G1037" s="3"/>
+      <c r="H1037" s="3"/>
+      <c r="I1037" s="4"/>
+      <c r="J1037" s="4"/>
+    </row>
+    <row r="1038" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1038" s="3"/>
+      <c r="B1038" s="3"/>
+      <c r="C1038" s="3"/>
+      <c r="D1038" s="3"/>
+      <c r="E1038" s="3"/>
+      <c r="F1038" s="3"/>
+      <c r="G1038" s="3"/>
+      <c r="H1038" s="3"/>
+      <c r="I1038" s="4"/>
+      <c r="J1038" s="4"/>
+    </row>
+    <row r="1039" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1039" s="3"/>
+      <c r="B1039" s="3"/>
+      <c r="C1039" s="3"/>
+      <c r="D1039" s="3"/>
+      <c r="E1039" s="3"/>
+      <c r="F1039" s="3"/>
+      <c r="G1039" s="3"/>
+      <c r="H1039" s="3"/>
+      <c r="I1039" s="4"/>
+      <c r="J1039" s="4"/>
+    </row>
+    <row r="1040" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1040" s="3"/>
+      <c r="B1040" s="3"/>
+      <c r="C1040" s="3"/>
+      <c r="D1040" s="3"/>
+      <c r="E1040" s="3"/>
+      <c r="F1040" s="3"/>
+      <c r="G1040" s="3"/>
+      <c r="H1040" s="3"/>
+      <c r="I1040" s="4"/>
+      <c r="J1040" s="4"/>
+    </row>
+    <row r="1041" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1041" s="3"/>
+      <c r="B1041" s="3"/>
+      <c r="C1041" s="3"/>
+      <c r="D1041" s="3"/>
+      <c r="E1041" s="3"/>
+      <c r="F1041" s="3"/>
+      <c r="G1041" s="3"/>
+      <c r="H1041" s="3"/>
+      <c r="I1041" s="4"/>
+      <c r="J1041" s="4"/>
+    </row>
+    <row r="1042" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1042" s="3"/>
+      <c r="B1042" s="3"/>
+      <c r="C1042" s="3"/>
+      <c r="D1042" s="3"/>
+      <c r="E1042" s="3"/>
+      <c r="F1042" s="3"/>
+      <c r="G1042" s="3"/>
+      <c r="H1042" s="3"/>
+      <c r="I1042" s="4"/>
+      <c r="J1042" s="4"/>
+    </row>
+    <row r="1043" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1043" s="3"/>
+      <c r="B1043" s="3"/>
+      <c r="C1043" s="3"/>
+      <c r="D1043" s="3"/>
+      <c r="E1043" s="3"/>
+      <c r="F1043" s="3"/>
+      <c r="G1043" s="3"/>
+      <c r="H1043" s="3"/>
+      <c r="I1043" s="4"/>
+      <c r="J1043" s="4"/>
+    </row>
+    <row r="1044" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1044" s="3"/>
+      <c r="B1044" s="3"/>
+      <c r="C1044" s="3"/>
+      <c r="D1044" s="3"/>
+      <c r="E1044" s="3"/>
+      <c r="F1044" s="3"/>
+      <c r="G1044" s="3"/>
+      <c r="H1044" s="3"/>
+      <c r="I1044" s="4"/>
+      <c r="J1044" s="4"/>
+    </row>
+    <row r="1045" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1045" s="3"/>
+      <c r="B1045" s="3"/>
+      <c r="C1045" s="3"/>
+      <c r="D1045" s="3"/>
+      <c r="E1045" s="3"/>
+      <c r="F1045" s="3"/>
+      <c r="G1045" s="3"/>
+      <c r="H1045" s="3"/>
+      <c r="I1045" s="4"/>
+      <c r="J1045" s="4"/>
+    </row>
+    <row r="1046" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1046" s="3"/>
+      <c r="B1046" s="3"/>
+      <c r="C1046" s="3"/>
+      <c r="D1046" s="3"/>
+      <c r="E1046" s="3"/>
+      <c r="F1046" s="3"/>
+      <c r="G1046" s="3"/>
+      <c r="H1046" s="3"/>
+      <c r="I1046" s="4"/>
+      <c r="J1046" s="4"/>
+    </row>
+    <row r="1047" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1047" s="3"/>
+      <c r="B1047" s="3"/>
+      <c r="C1047" s="3"/>
+      <c r="D1047" s="3"/>
+      <c r="E1047" s="3"/>
+      <c r="F1047" s="3"/>
+      <c r="G1047" s="3"/>
+      <c r="H1047" s="3"/>
+      <c r="I1047" s="4"/>
+      <c r="J1047" s="4"/>
+    </row>
+    <row r="1048" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1048" s="3"/>
+      <c r="B1048" s="3"/>
+      <c r="C1048" s="3"/>
+      <c r="D1048" s="3"/>
+      <c r="E1048" s="3"/>
+      <c r="F1048" s="3"/>
+      <c r="G1048" s="3"/>
+      <c r="H1048" s="3"/>
+      <c r="I1048" s="4"/>
+      <c r="J1048" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#24 Time Tracking*: updated to 2024-03-28.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8092" uniqueCount="1075">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8196" uniqueCount="1083">
   <si>
     <t>Year</t>
   </si>
@@ -3247,6 +3247,30 @@
   </si>
   <si>
     <t>2024-03-19</t>
+  </si>
+  <si>
+    <t>nwtimetrackingmanager v3.0.0</t>
+  </si>
+  <si>
+    <t>2024-03-21</t>
+  </si>
+  <si>
+    <t>nwreadinglistmanager v3.0.0</t>
+  </si>
+  <si>
+    <t>2024-03-22</t>
+  </si>
+  <si>
+    <t>2024-03-23</t>
+  </si>
+  <si>
+    <t>2024-03-24</t>
+  </si>
+  <si>
+    <t>nwreadinglistmanager v3.1.0</t>
+  </si>
+  <si>
+    <t>2024-03-28</t>
   </si>
 </sst>
 </file>
@@ -3646,11 +3670,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1048"/>
+  <dimension ref="A1:J1063"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1016" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1040" sqref="G1040"/>
+      <pane ySplit="1" topLeftCell="A1021" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1047" sqref="A1047"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -38441,160 +38465,446 @@
       </c>
     </row>
     <row r="1034" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1034" s="3"/>
-      <c r="B1034" s="3"/>
-      <c r="C1034" s="3"/>
-      <c r="D1034" s="3"/>
-      <c r="E1034" s="3"/>
-      <c r="F1034" s="3"/>
-      <c r="G1034" s="3"/>
-      <c r="H1034" s="3"/>
-      <c r="I1034" s="4"/>
-      <c r="J1034" s="4"/>
+      <c r="A1034" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1034" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C1034" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1034" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1034" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1034" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G1034" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1034" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1034" s="4">
+        <f t="shared" ref="I1034:I1035" si="166">YEAR(A1034)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1034" s="4">
+        <f t="shared" ref="J1034:J1035" si="167">MONTH(A1034)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1035" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1035" s="3"/>
-      <c r="B1035" s="3"/>
-      <c r="C1035" s="3"/>
-      <c r="D1035" s="3"/>
-      <c r="E1035" s="3"/>
-      <c r="F1035" s="3"/>
-      <c r="G1035" s="3"/>
-      <c r="H1035" s="3"/>
-      <c r="I1035" s="4"/>
-      <c r="J1035" s="4"/>
+      <c r="A1035" s="3" t="s">
+        <v>1074</v>
+      </c>
+      <c r="B1035" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1035" s="3" t="s">
+        <v>357</v>
+      </c>
+      <c r="D1035" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1035" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1035" s="3" t="s">
+        <v>1075</v>
+      </c>
+      <c r="G1035" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1035" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1035" s="4">
+        <f t="shared" si="166"/>
+        <v>2024</v>
+      </c>
+      <c r="J1035" s="4">
+        <f t="shared" si="167"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1036" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1036" s="3"/>
-      <c r="B1036" s="3"/>
-      <c r="C1036" s="3"/>
-      <c r="D1036" s="3"/>
-      <c r="E1036" s="3"/>
-      <c r="F1036" s="3"/>
-      <c r="G1036" s="3"/>
-      <c r="H1036" s="3"/>
-      <c r="I1036" s="4"/>
-      <c r="J1036" s="4"/>
+      <c r="A1036" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1036" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1036" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1036" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1036" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1036" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1036" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1036" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1036" s="4">
+        <f t="shared" ref="I1036:I1037" si="168">YEAR(A1036)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1036" s="4">
+        <f t="shared" ref="J1036:J1037" si="169">MONTH(A1036)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1037" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1037" s="3"/>
-      <c r="B1037" s="3"/>
-      <c r="C1037" s="3"/>
-      <c r="D1037" s="3"/>
-      <c r="E1037" s="3"/>
-      <c r="F1037" s="3"/>
-      <c r="G1037" s="3"/>
-      <c r="H1037" s="3"/>
-      <c r="I1037" s="4"/>
-      <c r="J1037" s="4"/>
+      <c r="A1037" s="3" t="s">
+        <v>1076</v>
+      </c>
+      <c r="B1037" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1037" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1037" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1037" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1037" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1037" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1037" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1037" s="4">
+        <f t="shared" si="168"/>
+        <v>2024</v>
+      </c>
+      <c r="J1037" s="4">
+        <f t="shared" si="169"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1038" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1038" s="3"/>
-      <c r="B1038" s="3"/>
-      <c r="C1038" s="3"/>
-      <c r="D1038" s="3"/>
-      <c r="E1038" s="3"/>
-      <c r="F1038" s="3"/>
-      <c r="G1038" s="3"/>
-      <c r="H1038" s="3"/>
-      <c r="I1038" s="4"/>
-      <c r="J1038" s="4"/>
+      <c r="A1038" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1038" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1038" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1038" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1038" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1038" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1038" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1038" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1038" s="4">
+        <f t="shared" ref="I1038:I1039" si="170">YEAR(A1038)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1038" s="4">
+        <f t="shared" ref="J1038:J1039" si="171">MONTH(A1038)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1039" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1039" s="3"/>
-      <c r="B1039" s="3"/>
-      <c r="C1039" s="3"/>
-      <c r="D1039" s="3"/>
-      <c r="E1039" s="3"/>
-      <c r="F1039" s="3"/>
-      <c r="G1039" s="3"/>
-      <c r="H1039" s="3"/>
-      <c r="I1039" s="4"/>
-      <c r="J1039" s="4"/>
+      <c r="A1039" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1039" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1039" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1039" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1039" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1039" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1039" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1039" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1039" s="4">
+        <f t="shared" si="170"/>
+        <v>2024</v>
+      </c>
+      <c r="J1039" s="4">
+        <f t="shared" si="171"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1040" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1040" s="3"/>
-      <c r="B1040" s="3"/>
-      <c r="C1040" s="3"/>
-      <c r="D1040" s="3"/>
-      <c r="E1040" s="3"/>
-      <c r="F1040" s="3"/>
-      <c r="G1040" s="3"/>
-      <c r="H1040" s="3"/>
-      <c r="I1040" s="4"/>
-      <c r="J1040" s="4"/>
+      <c r="A1040" s="3" t="s">
+        <v>1078</v>
+      </c>
+      <c r="B1040" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C1040" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1040" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1040" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1040" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1040" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1040" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1040" s="4">
+        <f t="shared" ref="I1040:I1042" si="172">YEAR(A1040)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1040" s="4">
+        <f t="shared" ref="J1040:J1042" si="173">MONTH(A1040)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1041" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1041" s="3"/>
-      <c r="B1041" s="3"/>
-      <c r="C1041" s="3"/>
-      <c r="D1041" s="3"/>
-      <c r="E1041" s="3"/>
-      <c r="F1041" s="3"/>
-      <c r="G1041" s="3"/>
-      <c r="H1041" s="3"/>
-      <c r="I1041" s="4"/>
-      <c r="J1041" s="4"/>
+      <c r="A1041" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1041" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="C1041" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1041" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1041" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1041" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1041" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1041" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1041" s="4">
+        <f t="shared" si="172"/>
+        <v>2024</v>
+      </c>
+      <c r="J1041" s="4">
+        <f t="shared" si="173"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1042" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1042" s="3"/>
-      <c r="B1042" s="3"/>
-      <c r="C1042" s="3"/>
-      <c r="D1042" s="3"/>
-      <c r="E1042" s="3"/>
-      <c r="F1042" s="3"/>
-      <c r="G1042" s="3"/>
-      <c r="H1042" s="3"/>
-      <c r="I1042" s="4"/>
-      <c r="J1042" s="4"/>
+      <c r="A1042" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1042" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1042" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1042" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1042" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1042" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1042" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1042" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1042" s="4">
+        <f t="shared" si="172"/>
+        <v>2024</v>
+      </c>
+      <c r="J1042" s="4">
+        <f t="shared" si="173"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1043" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1043" s="3"/>
-      <c r="B1043" s="3"/>
-      <c r="C1043" s="3"/>
-      <c r="D1043" s="3"/>
-      <c r="E1043" s="3"/>
-      <c r="F1043" s="3"/>
-      <c r="G1043" s="3"/>
-      <c r="H1043" s="3"/>
-      <c r="I1043" s="4"/>
-      <c r="J1043" s="4"/>
+      <c r="A1043" s="3" t="s">
+        <v>1079</v>
+      </c>
+      <c r="B1043" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1043" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="D1043" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1043" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1043" s="3" t="s">
+        <v>1077</v>
+      </c>
+      <c r="G1043" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1043" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1043" s="4">
+        <f t="shared" ref="I1043:I1045" si="174">YEAR(A1043)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1043" s="4">
+        <f t="shared" ref="J1043:J1045" si="175">MONTH(A1043)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1044" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1044" s="3"/>
-      <c r="B1044" s="3"/>
-      <c r="C1044" s="3"/>
-      <c r="D1044" s="3"/>
-      <c r="E1044" s="3"/>
-      <c r="F1044" s="3"/>
-      <c r="G1044" s="3"/>
-      <c r="H1044" s="3"/>
-      <c r="I1044" s="4"/>
-      <c r="J1044" s="4"/>
+      <c r="A1044" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B1044" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1044" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="D1044" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1044" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1044" s="3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G1044" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1044" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1044" s="4">
+        <f t="shared" si="174"/>
+        <v>2024</v>
+      </c>
+      <c r="J1044" s="4">
+        <f t="shared" si="175"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1045" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1045" s="3"/>
-      <c r="B1045" s="3"/>
-      <c r="C1045" s="3"/>
-      <c r="D1045" s="3"/>
-      <c r="E1045" s="3"/>
-      <c r="F1045" s="3"/>
-      <c r="G1045" s="3"/>
-      <c r="H1045" s="3"/>
-      <c r="I1045" s="4"/>
-      <c r="J1045" s="4"/>
+      <c r="A1045" s="3" t="s">
+        <v>1080</v>
+      </c>
+      <c r="B1045" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1045" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1045" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1045" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1045" s="3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G1045" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1045" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="I1045" s="4">
+        <f t="shared" si="174"/>
+        <v>2024</v>
+      </c>
+      <c r="J1045" s="4">
+        <f t="shared" si="175"/>
+        <v>3</v>
+      </c>
     </row>
     <row r="1046" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1046" s="3"/>
-      <c r="B1046" s="3"/>
-      <c r="C1046" s="3"/>
-      <c r="D1046" s="3"/>
-      <c r="E1046" s="3"/>
-      <c r="F1046" s="3"/>
-      <c r="G1046" s="3"/>
-      <c r="H1046" s="3"/>
-      <c r="I1046" s="4"/>
-      <c r="J1046" s="4"/>
+      <c r="A1046" s="3" t="s">
+        <v>1082</v>
+      </c>
+      <c r="B1046" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1046" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1046" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1046" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1046" s="3" t="s">
+        <v>1081</v>
+      </c>
+      <c r="G1046" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="H1046" s="8" t="s">
+        <v>281</v>
+      </c>
+      <c r="I1046" s="4">
+        <f t="shared" ref="I1046" si="176">YEAR(A1046)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1046" s="4">
+        <f t="shared" ref="J1046" si="177">MONTH(A1046)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1047" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1047" s="3"/>
@@ -38620,6 +38930,186 @@
       <c r="I1048" s="4"/>
       <c r="J1048" s="4"/>
     </row>
+    <row r="1049" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1049" s="3"/>
+      <c r="B1049" s="3"/>
+      <c r="C1049" s="3"/>
+      <c r="D1049" s="3"/>
+      <c r="E1049" s="3"/>
+      <c r="F1049" s="3"/>
+      <c r="G1049" s="3"/>
+      <c r="H1049" s="3"/>
+      <c r="I1049" s="4"/>
+      <c r="J1049" s="4"/>
+    </row>
+    <row r="1050" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1050" s="3"/>
+      <c r="B1050" s="3"/>
+      <c r="C1050" s="3"/>
+      <c r="D1050" s="3"/>
+      <c r="E1050" s="3"/>
+      <c r="F1050" s="3"/>
+      <c r="G1050" s="3"/>
+      <c r="H1050" s="3"/>
+      <c r="I1050" s="4"/>
+      <c r="J1050" s="4"/>
+    </row>
+    <row r="1051" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1051" s="3"/>
+      <c r="B1051" s="3"/>
+      <c r="C1051" s="3"/>
+      <c r="D1051" s="3"/>
+      <c r="E1051" s="3"/>
+      <c r="F1051" s="3"/>
+      <c r="G1051" s="3"/>
+      <c r="H1051" s="3"/>
+      <c r="I1051" s="4"/>
+      <c r="J1051" s="4"/>
+    </row>
+    <row r="1052" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1052" s="3"/>
+      <c r="B1052" s="3"/>
+      <c r="C1052" s="3"/>
+      <c r="D1052" s="3"/>
+      <c r="E1052" s="3"/>
+      <c r="F1052" s="3"/>
+      <c r="G1052" s="3"/>
+      <c r="H1052" s="3"/>
+      <c r="I1052" s="4"/>
+      <c r="J1052" s="4"/>
+    </row>
+    <row r="1053" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1053" s="3"/>
+      <c r="B1053" s="3"/>
+      <c r="C1053" s="3"/>
+      <c r="D1053" s="3"/>
+      <c r="E1053" s="3"/>
+      <c r="F1053" s="3"/>
+      <c r="G1053" s="3"/>
+      <c r="H1053" s="3"/>
+      <c r="I1053" s="4"/>
+      <c r="J1053" s="4"/>
+    </row>
+    <row r="1054" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1054" s="3"/>
+      <c r="B1054" s="3"/>
+      <c r="C1054" s="3"/>
+      <c r="D1054" s="3"/>
+      <c r="E1054" s="3"/>
+      <c r="F1054" s="3"/>
+      <c r="G1054" s="3"/>
+      <c r="H1054" s="3"/>
+      <c r="I1054" s="4"/>
+      <c r="J1054" s="4"/>
+    </row>
+    <row r="1055" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1055" s="3"/>
+      <c r="B1055" s="3"/>
+      <c r="C1055" s="3"/>
+      <c r="D1055" s="3"/>
+      <c r="E1055" s="3"/>
+      <c r="F1055" s="3"/>
+      <c r="G1055" s="3"/>
+      <c r="H1055" s="3"/>
+      <c r="I1055" s="4"/>
+      <c r="J1055" s="4"/>
+    </row>
+    <row r="1056" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1056" s="3"/>
+      <c r="B1056" s="3"/>
+      <c r="C1056" s="3"/>
+      <c r="D1056" s="3"/>
+      <c r="E1056" s="3"/>
+      <c r="F1056" s="3"/>
+      <c r="G1056" s="3"/>
+      <c r="H1056" s="3"/>
+      <c r="I1056" s="4"/>
+      <c r="J1056" s="4"/>
+    </row>
+    <row r="1057" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1057" s="3"/>
+      <c r="B1057" s="3"/>
+      <c r="C1057" s="3"/>
+      <c r="D1057" s="3"/>
+      <c r="E1057" s="3"/>
+      <c r="F1057" s="3"/>
+      <c r="G1057" s="3"/>
+      <c r="H1057" s="3"/>
+      <c r="I1057" s="4"/>
+      <c r="J1057" s="4"/>
+    </row>
+    <row r="1058" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1058" s="3"/>
+      <c r="B1058" s="3"/>
+      <c r="C1058" s="3"/>
+      <c r="D1058" s="3"/>
+      <c r="E1058" s="3"/>
+      <c r="F1058" s="3"/>
+      <c r="G1058" s="3"/>
+      <c r="H1058" s="3"/>
+      <c r="I1058" s="4"/>
+      <c r="J1058" s="4"/>
+    </row>
+    <row r="1059" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1059" s="3"/>
+      <c r="B1059" s="3"/>
+      <c r="C1059" s="3"/>
+      <c r="D1059" s="3"/>
+      <c r="E1059" s="3"/>
+      <c r="F1059" s="3"/>
+      <c r="G1059" s="3"/>
+      <c r="H1059" s="3"/>
+      <c r="I1059" s="4"/>
+      <c r="J1059" s="4"/>
+    </row>
+    <row r="1060" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1060" s="3"/>
+      <c r="B1060" s="3"/>
+      <c r="C1060" s="3"/>
+      <c r="D1060" s="3"/>
+      <c r="E1060" s="3"/>
+      <c r="F1060" s="3"/>
+      <c r="G1060" s="3"/>
+      <c r="H1060" s="3"/>
+      <c r="I1060" s="4"/>
+      <c r="J1060" s="4"/>
+    </row>
+    <row r="1061" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1061" s="3"/>
+      <c r="B1061" s="3"/>
+      <c r="C1061" s="3"/>
+      <c r="D1061" s="3"/>
+      <c r="E1061" s="3"/>
+      <c r="F1061" s="3"/>
+      <c r="G1061" s="3"/>
+      <c r="H1061" s="3"/>
+      <c r="I1061" s="4"/>
+      <c r="J1061" s="4"/>
+    </row>
+    <row r="1062" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1062" s="3"/>
+      <c r="B1062" s="3"/>
+      <c r="C1062" s="3"/>
+      <c r="D1062" s="3"/>
+      <c r="E1062" s="3"/>
+      <c r="F1062" s="3"/>
+      <c r="G1062" s="3"/>
+      <c r="H1062" s="3"/>
+      <c r="I1062" s="4"/>
+      <c r="J1062" s="4"/>
+    </row>
+    <row r="1063" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1063" s="3"/>
+      <c r="B1063" s="3"/>
+      <c r="C1063" s="3"/>
+      <c r="D1063" s="3"/>
+      <c r="E1063" s="3"/>
+      <c r="F1063" s="3"/>
+      <c r="G1063" s="3"/>
+      <c r="H1063" s="3"/>
+      <c r="I1063" s="4"/>
+      <c r="J1063" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-06-07.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8265" uniqueCount="1091">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8535" uniqueCount="1111">
   <si>
     <t>Year</t>
   </si>
@@ -3295,6 +3295,66 @@
   </si>
   <si>
     <t>2024-05-14</t>
+  </si>
+  <si>
+    <t>2024-05-19</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.2.0</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.2.0</t>
+  </si>
+  <si>
+    <t>nwshared v1.1.0</t>
+  </si>
+  <si>
+    <t>2024-05-20</t>
+  </si>
+  <si>
+    <t>2024-05-21</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.3.0</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.3.0</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.0.0</t>
+  </si>
+  <si>
+    <t>2024-05-26</t>
+  </si>
+  <si>
+    <t>2024-05-27</t>
+  </si>
+  <si>
+    <t>2024-05-31</t>
+  </si>
+  <si>
+    <t>2024-05-28</t>
+  </si>
+  <si>
+    <t>2024-05-29</t>
+  </si>
+  <si>
+    <t>2024-05-30</t>
+  </si>
+  <si>
+    <t>2024-06-01</t>
+  </si>
+  <si>
+    <t>2024-06-02</t>
+  </si>
+  <si>
+    <t>2024-06-04</t>
+  </si>
+  <si>
+    <t>2024-06-06</t>
+  </si>
+  <si>
+    <t>2024-06-07</t>
   </si>
 </sst>
 </file>
@@ -3694,11 +3754,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1075"/>
+  <dimension ref="A1:J1104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1032" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1060" sqref="C1060"/>
+      <pane ySplit="1" topLeftCell="A1053" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1068" sqref="D1068"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -39231,244 +39291,1336 @@
       </c>
     </row>
     <row r="1056" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1056" s="3"/>
-      <c r="B1056" s="3"/>
-      <c r="C1056" s="3"/>
-      <c r="D1056" s="3"/>
-      <c r="E1056" s="3"/>
+      <c r="A1056" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1056" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1056" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1056" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1056" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1056" s="3"/>
-      <c r="G1056" s="3"/>
-      <c r="H1056" s="3"/>
-      <c r="I1056" s="4"/>
-      <c r="J1056" s="4"/>
+      <c r="G1056" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1056" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1056" s="4">
+        <f t="shared" ref="I1056:I1058" si="182">YEAR(A1056)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1056" s="4">
+        <f t="shared" ref="J1056:J1058" si="183">MONTH(A1056)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1057" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1057" s="3"/>
-      <c r="B1057" s="3"/>
-      <c r="C1057" s="3"/>
-      <c r="D1057" s="3"/>
-      <c r="E1057" s="3"/>
+      <c r="A1057" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1057" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1057" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1057" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1057" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1057" s="3"/>
-      <c r="G1057" s="3"/>
-      <c r="H1057" s="3"/>
-      <c r="I1057" s="4"/>
-      <c r="J1057" s="4"/>
+      <c r="G1057" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1057" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1057" s="4">
+        <f t="shared" si="182"/>
+        <v>2024</v>
+      </c>
+      <c r="J1057" s="4">
+        <f t="shared" si="183"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1058" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1058" s="3"/>
-      <c r="B1058" s="3"/>
-      <c r="C1058" s="3"/>
-      <c r="D1058" s="3"/>
-      <c r="E1058" s="3"/>
-      <c r="F1058" s="3"/>
-      <c r="G1058" s="3"/>
-      <c r="H1058" s="3"/>
-      <c r="I1058" s="4"/>
-      <c r="J1058" s="4"/>
+      <c r="A1058" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1058" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1058" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1058" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1058" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1058" s="3" t="s">
+        <v>1092</v>
+      </c>
+      <c r="G1058" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1058" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1058" s="4">
+        <f t="shared" si="182"/>
+        <v>2024</v>
+      </c>
+      <c r="J1058" s="4">
+        <f t="shared" si="183"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1059" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1059" s="3"/>
-      <c r="B1059" s="3"/>
-      <c r="C1059" s="3"/>
-      <c r="D1059" s="3"/>
-      <c r="E1059" s="3"/>
-      <c r="F1059" s="3"/>
-      <c r="G1059" s="3"/>
-      <c r="H1059" s="3"/>
-      <c r="I1059" s="4"/>
-      <c r="J1059" s="4"/>
+      <c r="A1059" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1059" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1059" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1059" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1059" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1059" s="3" t="s">
+        <v>1093</v>
+      </c>
+      <c r="G1059" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1059" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1059" s="4">
+        <f t="shared" ref="I1059:I1062" si="184">YEAR(A1059)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1059" s="4">
+        <f t="shared" ref="J1059:J1062" si="185">MONTH(A1059)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1060" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1060" s="3"/>
-      <c r="B1060" s="3"/>
-      <c r="C1060" s="3"/>
-      <c r="D1060" s="3"/>
-      <c r="E1060" s="3"/>
-      <c r="F1060" s="3"/>
-      <c r="G1060" s="3"/>
-      <c r="H1060" s="3"/>
-      <c r="I1060" s="4"/>
-      <c r="J1060" s="4"/>
+      <c r="A1060" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1060" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1060" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1060" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1060" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1060" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G1060" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1060" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1060" s="4">
+        <f t="shared" si="184"/>
+        <v>2024</v>
+      </c>
+      <c r="J1060" s="4">
+        <f t="shared" si="185"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1061" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1061" s="3"/>
-      <c r="B1061" s="3"/>
-      <c r="C1061" s="3"/>
-      <c r="D1061" s="3"/>
-      <c r="E1061" s="3"/>
-      <c r="F1061" s="3"/>
-      <c r="G1061" s="3"/>
-      <c r="H1061" s="3"/>
-      <c r="I1061" s="4"/>
-      <c r="J1061" s="4"/>
+      <c r="A1061" s="3" t="s">
+        <v>1091</v>
+      </c>
+      <c r="B1061" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1061" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1061" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1061" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1061" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G1061" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1061" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1061" s="4">
+        <f t="shared" si="184"/>
+        <v>2024</v>
+      </c>
+      <c r="J1061" s="4">
+        <f t="shared" si="185"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1062" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1062" s="3"/>
-      <c r="B1062" s="3"/>
-      <c r="C1062" s="3"/>
-      <c r="D1062" s="3"/>
-      <c r="E1062" s="3"/>
-      <c r="F1062" s="3"/>
-      <c r="G1062" s="3"/>
-      <c r="H1062" s="3"/>
-      <c r="I1062" s="4"/>
-      <c r="J1062" s="4"/>
+      <c r="A1062" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B1062" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1062" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1062" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1062" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1062" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G1062" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1062" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1062" s="4">
+        <f t="shared" si="184"/>
+        <v>2024</v>
+      </c>
+      <c r="J1062" s="4">
+        <f t="shared" si="185"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1063" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1063" s="3"/>
-      <c r="B1063" s="3"/>
-      <c r="C1063" s="3"/>
-      <c r="D1063" s="3"/>
-      <c r="E1063" s="3"/>
-      <c r="F1063" s="3"/>
-      <c r="G1063" s="3"/>
-      <c r="H1063" s="3"/>
-      <c r="I1063" s="4"/>
-      <c r="J1063" s="4"/>
+      <c r="A1063" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B1063" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1063" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1063" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1063" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1063" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G1063" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1063" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1063" s="4">
+        <f t="shared" ref="I1063" si="186">YEAR(A1063)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1063" s="4">
+        <f t="shared" ref="J1063" si="187">MONTH(A1063)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1064" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1064" s="3"/>
-      <c r="B1064" s="3"/>
-      <c r="C1064" s="3"/>
-      <c r="D1064" s="3"/>
-      <c r="E1064" s="3"/>
-      <c r="F1064" s="3"/>
-      <c r="G1064" s="3"/>
-      <c r="H1064" s="3"/>
-      <c r="I1064" s="4"/>
-      <c r="J1064" s="4"/>
+      <c r="A1064" s="3" t="s">
+        <v>1095</v>
+      </c>
+      <c r="B1064" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1064" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1064" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1064" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1064" s="3" t="s">
+        <v>1094</v>
+      </c>
+      <c r="G1064" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1064" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1064" s="4">
+        <f t="shared" ref="I1064" si="188">YEAR(A1064)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1064" s="4">
+        <f t="shared" ref="J1064" si="189">MONTH(A1064)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1065" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1065" s="3"/>
-      <c r="B1065" s="3"/>
-      <c r="C1065" s="3"/>
-      <c r="D1065" s="3"/>
-      <c r="E1065" s="3"/>
-      <c r="F1065" s="3"/>
-      <c r="G1065" s="3"/>
-      <c r="H1065" s="3"/>
-      <c r="I1065" s="4"/>
-      <c r="J1065" s="4"/>
+      <c r="A1065" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B1065" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1065" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1065" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1065" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1065" s="3" t="s">
+        <v>1097</v>
+      </c>
+      <c r="G1065" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1065" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1065" s="4">
+        <f t="shared" ref="I1065" si="190">YEAR(A1065)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1065" s="4">
+        <f t="shared" ref="J1065" si="191">MONTH(A1065)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1066" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1066" s="3"/>
-      <c r="B1066" s="3"/>
-      <c r="C1066" s="3"/>
-      <c r="D1066" s="3"/>
-      <c r="E1066" s="3"/>
-      <c r="F1066" s="3"/>
-      <c r="G1066" s="3"/>
-      <c r="H1066" s="3"/>
-      <c r="I1066" s="4"/>
-      <c r="J1066" s="4"/>
+      <c r="A1066" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B1066" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1066" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1066" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1066" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1066" s="3" t="s">
+        <v>1098</v>
+      </c>
+      <c r="G1066" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1066" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1066" s="4">
+        <f t="shared" ref="I1066" si="192">YEAR(A1066)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1066" s="4">
+        <f t="shared" ref="J1066" si="193">MONTH(A1066)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1067" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1067" s="3"/>
-      <c r="B1067" s="3"/>
-      <c r="C1067" s="3"/>
-      <c r="D1067" s="3"/>
-      <c r="E1067" s="3"/>
-      <c r="F1067" s="3"/>
-      <c r="G1067" s="3"/>
-      <c r="H1067" s="3"/>
-      <c r="I1067" s="4"/>
-      <c r="J1067" s="4"/>
+      <c r="A1067" s="3" t="s">
+        <v>1096</v>
+      </c>
+      <c r="B1067" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1067" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1067" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1067" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1067" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1067" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1067" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1067" s="4">
+        <f t="shared" ref="I1067" si="194">YEAR(A1067)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1067" s="4">
+        <f t="shared" ref="J1067" si="195">MONTH(A1067)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1068" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1068" s="3"/>
-      <c r="B1068" s="3"/>
-      <c r="C1068" s="3"/>
-      <c r="D1068" s="3"/>
-      <c r="E1068" s="3"/>
-      <c r="F1068" s="3"/>
-      <c r="G1068" s="3"/>
-      <c r="H1068" s="3"/>
-      <c r="I1068" s="4"/>
-      <c r="J1068" s="4"/>
+      <c r="A1068" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B1068" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1068" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1068" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1068" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1068" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1068" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1068" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1068" s="4">
+        <f t="shared" ref="I1068:I1070" si="196">YEAR(A1068)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1068" s="4">
+        <f t="shared" ref="J1068:J1070" si="197">MONTH(A1068)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1069" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1069" s="3"/>
-      <c r="B1069" s="3"/>
-      <c r="C1069" s="3"/>
-      <c r="D1069" s="3"/>
-      <c r="E1069" s="3"/>
-      <c r="F1069" s="3"/>
-      <c r="G1069" s="3"/>
-      <c r="H1069" s="3"/>
-      <c r="I1069" s="4"/>
-      <c r="J1069" s="4"/>
+      <c r="A1069" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B1069" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1069" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1069" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1069" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1069" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1069" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1069" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1069" s="4">
+        <f t="shared" si="196"/>
+        <v>2024</v>
+      </c>
+      <c r="J1069" s="4">
+        <f t="shared" si="197"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1070" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1070" s="3"/>
-      <c r="B1070" s="3"/>
-      <c r="C1070" s="3"/>
-      <c r="D1070" s="3"/>
-      <c r="E1070" s="3"/>
-      <c r="F1070" s="3"/>
-      <c r="G1070" s="3"/>
-      <c r="H1070" s="3"/>
-      <c r="I1070" s="4"/>
-      <c r="J1070" s="4"/>
+      <c r="A1070" s="3" t="s">
+        <v>1100</v>
+      </c>
+      <c r="B1070" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1070" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1070" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1070" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1070" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1070" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1070" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1070" s="4">
+        <f t="shared" si="196"/>
+        <v>2024</v>
+      </c>
+      <c r="J1070" s="4">
+        <f t="shared" si="197"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1071" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1071" s="3"/>
-      <c r="B1071" s="3"/>
-      <c r="C1071" s="3"/>
-      <c r="D1071" s="3"/>
-      <c r="E1071" s="3"/>
-      <c r="F1071" s="3"/>
-      <c r="G1071" s="3"/>
-      <c r="H1071" s="3"/>
-      <c r="I1071" s="4"/>
-      <c r="J1071" s="4"/>
+      <c r="A1071" s="3" t="s">
+        <v>1101</v>
+      </c>
+      <c r="B1071" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1071" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1071" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1071" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1071" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1071" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1071" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1071" s="4">
+        <f t="shared" ref="I1071:I1073" si="198">YEAR(A1071)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1071" s="4">
+        <f t="shared" ref="J1071:J1073" si="199">MONTH(A1071)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1072" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1072" s="3"/>
-      <c r="B1072" s="3"/>
-      <c r="C1072" s="3"/>
-      <c r="D1072" s="3"/>
-      <c r="E1072" s="3"/>
-      <c r="F1072" s="3"/>
-      <c r="G1072" s="3"/>
-      <c r="H1072" s="3"/>
-      <c r="I1072" s="4"/>
-      <c r="J1072" s="4"/>
+      <c r="A1072" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1072" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1072" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1072" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1072" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1072" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1072" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1072" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1072" s="4">
+        <f t="shared" si="198"/>
+        <v>2024</v>
+      </c>
+      <c r="J1072" s="4">
+        <f t="shared" si="199"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1073" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1073" s="3"/>
-      <c r="B1073" s="3"/>
-      <c r="C1073" s="3"/>
-      <c r="D1073" s="3"/>
-      <c r="E1073" s="3"/>
-      <c r="F1073" s="3"/>
-      <c r="G1073" s="3"/>
-      <c r="H1073" s="3"/>
-      <c r="I1073" s="4"/>
-      <c r="J1073" s="4"/>
+      <c r="A1073" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1073" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1073" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1073" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1073" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1073" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1073" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1073" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1073" s="4">
+        <f t="shared" si="198"/>
+        <v>2024</v>
+      </c>
+      <c r="J1073" s="4">
+        <f t="shared" si="199"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1074" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1074" s="3"/>
-      <c r="B1074" s="3"/>
-      <c r="C1074" s="3"/>
-      <c r="D1074" s="3"/>
-      <c r="E1074" s="3"/>
-      <c r="F1074" s="3"/>
-      <c r="G1074" s="3"/>
-      <c r="H1074" s="3"/>
-      <c r="I1074" s="4"/>
-      <c r="J1074" s="4"/>
+      <c r="A1074" s="3" t="s">
+        <v>1103</v>
+      </c>
+      <c r="B1074" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1074" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1074" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1074" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1074" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1074" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1074" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1074" s="4">
+        <f t="shared" ref="I1074:I1075" si="200">YEAR(A1074)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1074" s="4">
+        <f t="shared" ref="J1074:J1075" si="201">MONTH(A1074)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1075" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1075" s="3"/>
-      <c r="B1075" s="3"/>
-      <c r="C1075" s="3"/>
-      <c r="D1075" s="3"/>
-      <c r="E1075" s="3"/>
-      <c r="F1075" s="3"/>
-      <c r="G1075" s="3"/>
-      <c r="H1075" s="3"/>
-      <c r="I1075" s="4"/>
-      <c r="J1075" s="4"/>
+      <c r="A1075" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B1075" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1075" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1075" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1075" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1075" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1075" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1075" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1075" s="4">
+        <f t="shared" si="200"/>
+        <v>2024</v>
+      </c>
+      <c r="J1075" s="4">
+        <f t="shared" si="201"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1076" s="3" t="s">
+        <v>1104</v>
+      </c>
+      <c r="B1076" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1076" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1076" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1076" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1076" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1076" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1076" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1076" s="4">
+        <f t="shared" ref="I1076:I1077" si="202">YEAR(A1076)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1076" s="4">
+        <f t="shared" ref="J1076:J1077" si="203">MONTH(A1076)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1077" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B1077" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1077" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1077" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1077" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1077" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1077" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1077" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1077" s="4">
+        <f t="shared" si="202"/>
+        <v>2024</v>
+      </c>
+      <c r="J1077" s="4">
+        <f t="shared" si="203"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1078" s="3" t="s">
+        <v>1105</v>
+      </c>
+      <c r="B1078" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1078" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1078" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1078" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1078" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1078" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1078" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1078" s="4">
+        <f t="shared" ref="I1078:I1079" si="204">YEAR(A1078)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1078" s="4">
+        <f t="shared" ref="J1078:J1079" si="205">MONTH(A1078)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1079" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B1079" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1079" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1079" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1079" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1079" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1079" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1079" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1079" s="4">
+        <f t="shared" si="204"/>
+        <v>2024</v>
+      </c>
+      <c r="J1079" s="4">
+        <f t="shared" si="205"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1080" s="3" t="s">
+        <v>1102</v>
+      </c>
+      <c r="B1080" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1080" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1080" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1080" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1080" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1080" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1080" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1080" s="4">
+        <f t="shared" ref="I1080:I1081" si="206">YEAR(A1080)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1080" s="4">
+        <f t="shared" ref="J1080:J1081" si="207">MONTH(A1080)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1081" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B1081" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1081" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1081" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1081" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1081" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1081" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1081" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1081" s="4">
+        <f t="shared" si="206"/>
+        <v>2024</v>
+      </c>
+      <c r="J1081" s="4">
+        <f t="shared" si="207"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1082" s="3" t="s">
+        <v>1106</v>
+      </c>
+      <c r="B1082" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1082" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1082" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1082" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1082" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1082" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1082" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1082" s="4">
+        <f t="shared" ref="I1082:I1083" si="208">YEAR(A1082)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1082" s="4">
+        <f t="shared" ref="J1082:J1083" si="209">MONTH(A1082)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1083" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1083" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1083" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1083" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1083" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1083" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1083" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1083" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1083" s="4">
+        <f t="shared" si="208"/>
+        <v>2024</v>
+      </c>
+      <c r="J1083" s="4">
+        <f t="shared" si="209"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1084" s="3" t="s">
+        <v>1107</v>
+      </c>
+      <c r="B1084" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1084" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1084" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1084" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1084" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1084" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1084" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1084" s="4">
+        <f t="shared" ref="I1084" si="210">YEAR(A1084)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1084" s="4">
+        <f t="shared" ref="J1084" si="211">MONTH(A1084)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1085" s="3" t="s">
+        <v>1108</v>
+      </c>
+      <c r="B1085" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="C1085" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1085" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1085" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1085" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1085" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1085" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1085" s="4">
+        <f t="shared" ref="I1085:I1086" si="212">YEAR(A1085)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1085" s="4">
+        <f t="shared" ref="J1085:J1086" si="213">MONTH(A1085)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1086" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B1086" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1086" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1086" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1086" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1086" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1086" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1086" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1086" s="4">
+        <f t="shared" si="212"/>
+        <v>2024</v>
+      </c>
+      <c r="J1086" s="4">
+        <f t="shared" si="213"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1087" s="3" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B1087" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1087" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1087" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1087" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1087" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1087" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1087" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1087" s="4">
+        <f t="shared" ref="I1087:I1088" si="214">YEAR(A1087)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1087" s="4">
+        <f t="shared" ref="J1087:J1088" si="215">MONTH(A1087)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1088" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B1088" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1088" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1088" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1088" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1088" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1088" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1088" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1088" s="4">
+        <f t="shared" si="214"/>
+        <v>2024</v>
+      </c>
+      <c r="J1088" s="4">
+        <f t="shared" si="215"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1089" s="3" t="s">
+        <v>1110</v>
+      </c>
+      <c r="B1089" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1089" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1089" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1089" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1089" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1089" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1089" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1089" s="4">
+        <f t="shared" ref="I1089" si="216">YEAR(A1089)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1089" s="4">
+        <f t="shared" ref="J1089" si="217">MONTH(A1089)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1090" s="3"/>
+      <c r="B1090" s="3"/>
+      <c r="C1090" s="3"/>
+      <c r="D1090" s="3"/>
+      <c r="E1090" s="3"/>
+      <c r="F1090" s="3"/>
+      <c r="G1090" s="3"/>
+      <c r="H1090" s="3"/>
+      <c r="I1090" s="4"/>
+      <c r="J1090" s="4"/>
+    </row>
+    <row r="1091" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1091" s="3"/>
+      <c r="B1091" s="3"/>
+      <c r="C1091" s="3"/>
+      <c r="D1091" s="3"/>
+      <c r="E1091" s="3"/>
+      <c r="F1091" s="3"/>
+      <c r="G1091" s="3"/>
+      <c r="H1091" s="3"/>
+      <c r="I1091" s="4"/>
+      <c r="J1091" s="4"/>
+    </row>
+    <row r="1092" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1092" s="3"/>
+      <c r="B1092" s="3"/>
+      <c r="C1092" s="3"/>
+      <c r="D1092" s="3"/>
+      <c r="E1092" s="3"/>
+      <c r="F1092" s="3"/>
+      <c r="G1092" s="3"/>
+      <c r="H1092" s="3"/>
+      <c r="I1092" s="4"/>
+      <c r="J1092" s="4"/>
+    </row>
+    <row r="1093" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1093" s="3"/>
+      <c r="B1093" s="3"/>
+      <c r="C1093" s="3"/>
+      <c r="D1093" s="3"/>
+      <c r="E1093" s="3"/>
+      <c r="F1093" s="3"/>
+      <c r="G1093" s="3"/>
+      <c r="H1093" s="3"/>
+      <c r="I1093" s="4"/>
+      <c r="J1093" s="4"/>
+    </row>
+    <row r="1094" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1094" s="3"/>
+      <c r="B1094" s="3"/>
+      <c r="C1094" s="3"/>
+      <c r="D1094" s="3"/>
+      <c r="E1094" s="3"/>
+      <c r="F1094" s="3"/>
+      <c r="G1094" s="3"/>
+      <c r="H1094" s="3"/>
+      <c r="I1094" s="4"/>
+      <c r="J1094" s="4"/>
+    </row>
+    <row r="1095" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1095" s="3"/>
+      <c r="B1095" s="3"/>
+      <c r="C1095" s="3"/>
+      <c r="D1095" s="3"/>
+      <c r="E1095" s="3"/>
+      <c r="F1095" s="3"/>
+      <c r="G1095" s="3"/>
+      <c r="H1095" s="3"/>
+      <c r="I1095" s="4"/>
+      <c r="J1095" s="4"/>
+    </row>
+    <row r="1096" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1096" s="3"/>
+      <c r="B1096" s="3"/>
+      <c r="C1096" s="3"/>
+      <c r="D1096" s="3"/>
+      <c r="E1096" s="3"/>
+      <c r="F1096" s="3"/>
+      <c r="G1096" s="3"/>
+      <c r="H1096" s="3"/>
+      <c r="I1096" s="4"/>
+      <c r="J1096" s="4"/>
+    </row>
+    <row r="1097" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1097" s="3"/>
+      <c r="B1097" s="3"/>
+      <c r="C1097" s="3"/>
+      <c r="D1097" s="3"/>
+      <c r="E1097" s="3"/>
+      <c r="F1097" s="3"/>
+      <c r="G1097" s="3"/>
+      <c r="H1097" s="3"/>
+      <c r="I1097" s="4"/>
+      <c r="J1097" s="4"/>
+    </row>
+    <row r="1098" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1098" s="3"/>
+      <c r="B1098" s="3"/>
+      <c r="C1098" s="3"/>
+      <c r="D1098" s="3"/>
+      <c r="E1098" s="3"/>
+      <c r="F1098" s="3"/>
+      <c r="G1098" s="3"/>
+      <c r="H1098" s="3"/>
+      <c r="I1098" s="4"/>
+      <c r="J1098" s="4"/>
+    </row>
+    <row r="1099" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1099" s="3"/>
+      <c r="B1099" s="3"/>
+      <c r="C1099" s="3"/>
+      <c r="D1099" s="3"/>
+      <c r="E1099" s="3"/>
+      <c r="F1099" s="3"/>
+      <c r="G1099" s="3"/>
+      <c r="H1099" s="3"/>
+      <c r="I1099" s="4"/>
+      <c r="J1099" s="4"/>
+    </row>
+    <row r="1100" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1100" s="3"/>
+      <c r="B1100" s="3"/>
+      <c r="C1100" s="3"/>
+      <c r="D1100" s="3"/>
+      <c r="E1100" s="3"/>
+      <c r="F1100" s="3"/>
+      <c r="G1100" s="3"/>
+      <c r="H1100" s="3"/>
+      <c r="I1100" s="4"/>
+      <c r="J1100" s="4"/>
+    </row>
+    <row r="1101" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1101" s="3"/>
+      <c r="B1101" s="3"/>
+      <c r="C1101" s="3"/>
+      <c r="D1101" s="3"/>
+      <c r="E1101" s="3"/>
+      <c r="F1101" s="3"/>
+      <c r="G1101" s="3"/>
+      <c r="H1101" s="3"/>
+      <c r="I1101" s="4"/>
+      <c r="J1101" s="4"/>
+    </row>
+    <row r="1102" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1102" s="3"/>
+      <c r="B1102" s="3"/>
+      <c r="C1102" s="3"/>
+      <c r="D1102" s="3"/>
+      <c r="E1102" s="3"/>
+      <c r="F1102" s="3"/>
+      <c r="G1102" s="3"/>
+      <c r="H1102" s="3"/>
+      <c r="I1102" s="4"/>
+      <c r="J1102" s="4"/>
+    </row>
+    <row r="1103" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1103" s="3"/>
+      <c r="B1103" s="3"/>
+      <c r="C1103" s="3"/>
+      <c r="D1103" s="3"/>
+      <c r="E1103" s="3"/>
+      <c r="F1103" s="3"/>
+      <c r="G1103" s="3"/>
+      <c r="H1103" s="3"/>
+      <c r="I1103" s="4"/>
+      <c r="J1103" s="4"/>
+    </row>
+    <row r="1104" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1104" s="3"/>
+      <c r="B1104" s="3"/>
+      <c r="C1104" s="3"/>
+      <c r="D1104" s="3"/>
+      <c r="E1104" s="3"/>
+      <c r="F1104" s="3"/>
+      <c r="G1104" s="3"/>
+      <c r="H1104" s="3"/>
+      <c r="I1104" s="4"/>
+      <c r="J1104" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-06-24.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8535" uniqueCount="1111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8685" uniqueCount="1118">
   <si>
     <t>Year</t>
   </si>
@@ -3355,6 +3355,27 @@
   </si>
   <si>
     <t>2024-06-07</t>
+  </si>
+  <si>
+    <t>2024-06-16</t>
+  </si>
+  <si>
+    <t>2024-06-17</t>
+  </si>
+  <si>
+    <t>2024-06-18</t>
+  </si>
+  <si>
+    <t>2024-06-20</t>
+  </si>
+  <si>
+    <t>2024-06-21</t>
+  </si>
+  <si>
+    <t>2024-06-23</t>
+  </si>
+  <si>
+    <t>2024-06-24</t>
   </si>
 </sst>
 </file>
@@ -3754,11 +3775,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1104"/>
+  <dimension ref="A1:J1126"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1053" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1068" sqref="D1068"/>
+      <pane ySplit="1" topLeftCell="A1085" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1101" sqref="F1101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -40443,184 +40464,862 @@
       </c>
     </row>
     <row r="1090" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1090" s="3"/>
-      <c r="B1090" s="3"/>
-      <c r="C1090" s="3"/>
-      <c r="D1090" s="3"/>
-      <c r="E1090" s="3"/>
+      <c r="A1090" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B1090" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1090" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1090" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1090" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1090" s="3"/>
-      <c r="G1090" s="3"/>
-      <c r="H1090" s="3"/>
-      <c r="I1090" s="4"/>
-      <c r="J1090" s="4"/>
+      <c r="G1090" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1090" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1090" s="4">
+        <f t="shared" ref="I1090" si="218">YEAR(A1090)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1090" s="4">
+        <f t="shared" ref="J1090" si="219">MONTH(A1090)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1091" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1091" s="3"/>
-      <c r="B1091" s="3"/>
-      <c r="C1091" s="3"/>
-      <c r="D1091" s="3"/>
-      <c r="E1091" s="3"/>
-      <c r="F1091" s="3"/>
-      <c r="G1091" s="3"/>
-      <c r="H1091" s="3"/>
-      <c r="I1091" s="4"/>
-      <c r="J1091" s="4"/>
+      <c r="A1091" s="3" t="s">
+        <v>1111</v>
+      </c>
+      <c r="B1091" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1091" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1091" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1091" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1091" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1091" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1091" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1091" s="4">
+        <f t="shared" ref="I1091:I1097" si="220">YEAR(A1091)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1091" s="4">
+        <f t="shared" ref="J1091:J1097" si="221">MONTH(A1091)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1092" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1092" s="3"/>
-      <c r="B1092" s="3"/>
-      <c r="C1092" s="3"/>
-      <c r="D1092" s="3"/>
-      <c r="E1092" s="3"/>
-      <c r="F1092" s="3"/>
-      <c r="G1092" s="3"/>
-      <c r="H1092" s="3"/>
-      <c r="I1092" s="4"/>
-      <c r="J1092" s="4"/>
+      <c r="A1092" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1092" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1092" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1092" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1092" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1092" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1092" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1092" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1092" s="4">
+        <f t="shared" si="220"/>
+        <v>2024</v>
+      </c>
+      <c r="J1092" s="4">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1093" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1093" s="3"/>
-      <c r="B1093" s="3"/>
-      <c r="C1093" s="3"/>
-      <c r="D1093" s="3"/>
-      <c r="E1093" s="3"/>
-      <c r="F1093" s="3"/>
-      <c r="G1093" s="3"/>
-      <c r="H1093" s="3"/>
-      <c r="I1093" s="4"/>
-      <c r="J1093" s="4"/>
+      <c r="A1093" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1093" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1093" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1093" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1093" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1093" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1093" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1093" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1093" s="4">
+        <f t="shared" si="220"/>
+        <v>2024</v>
+      </c>
+      <c r="J1093" s="4">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1094" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1094" s="3"/>
-      <c r="B1094" s="3"/>
-      <c r="C1094" s="3"/>
-      <c r="D1094" s="3"/>
-      <c r="E1094" s="3"/>
-      <c r="F1094" s="3"/>
-      <c r="G1094" s="3"/>
-      <c r="H1094" s="3"/>
-      <c r="I1094" s="4"/>
-      <c r="J1094" s="4"/>
+      <c r="A1094" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1094" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1094" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1094" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1094" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1094" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1094" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1094" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1094" s="4">
+        <f t="shared" si="220"/>
+        <v>2024</v>
+      </c>
+      <c r="J1094" s="4">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1095" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1095" s="3"/>
-      <c r="B1095" s="3"/>
-      <c r="C1095" s="3"/>
-      <c r="D1095" s="3"/>
-      <c r="E1095" s="3"/>
-      <c r="F1095" s="3"/>
-      <c r="G1095" s="3"/>
-      <c r="H1095" s="3"/>
-      <c r="I1095" s="4"/>
-      <c r="J1095" s="4"/>
+      <c r="A1095" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1095" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1095" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1095" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1095" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1095" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1095" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1095" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1095" s="4">
+        <f t="shared" si="220"/>
+        <v>2024</v>
+      </c>
+      <c r="J1095" s="4">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1096" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1096" s="3"/>
-      <c r="B1096" s="3"/>
-      <c r="C1096" s="3"/>
-      <c r="D1096" s="3"/>
-      <c r="E1096" s="3"/>
-      <c r="F1096" s="3"/>
-      <c r="G1096" s="3"/>
-      <c r="H1096" s="3"/>
-      <c r="I1096" s="4"/>
-      <c r="J1096" s="4"/>
+      <c r="A1096" s="3" t="s">
+        <v>1112</v>
+      </c>
+      <c r="B1096" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1096" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1096" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1096" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1096" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1096" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1096" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1096" s="4">
+        <f t="shared" si="220"/>
+        <v>2024</v>
+      </c>
+      <c r="J1096" s="4">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1097" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1097" s="3"/>
-      <c r="B1097" s="3"/>
-      <c r="C1097" s="3"/>
-      <c r="D1097" s="3"/>
-      <c r="E1097" s="3"/>
+      <c r="A1097" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1097" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1097" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1097" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1097" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1097" s="3"/>
-      <c r="G1097" s="3"/>
-      <c r="H1097" s="3"/>
-      <c r="I1097" s="4"/>
-      <c r="J1097" s="4"/>
+      <c r="G1097" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1097" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1097" s="4">
+        <f t="shared" si="220"/>
+        <v>2024</v>
+      </c>
+      <c r="J1097" s="4">
+        <f t="shared" si="221"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1098" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1098" s="3"/>
-      <c r="B1098" s="3"/>
-      <c r="C1098" s="3"/>
-      <c r="D1098" s="3"/>
-      <c r="E1098" s="3"/>
-      <c r="F1098" s="3"/>
-      <c r="G1098" s="3"/>
-      <c r="H1098" s="3"/>
-      <c r="I1098" s="4"/>
-      <c r="J1098" s="4"/>
+      <c r="A1098" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1098" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1098" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1098" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1098" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1098" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1098" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1098" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1098" s="4">
+        <f t="shared" ref="I1098:I1099" si="222">YEAR(A1098)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1098" s="4">
+        <f t="shared" ref="J1098:J1099" si="223">MONTH(A1098)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1099" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1099" s="3"/>
-      <c r="B1099" s="3"/>
-      <c r="C1099" s="3"/>
-      <c r="D1099" s="3"/>
-      <c r="E1099" s="3"/>
-      <c r="F1099" s="3"/>
-      <c r="G1099" s="3"/>
-      <c r="H1099" s="3"/>
-      <c r="I1099" s="4"/>
-      <c r="J1099" s="4"/>
+      <c r="A1099" s="3" t="s">
+        <v>1113</v>
+      </c>
+      <c r="B1099" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1099" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1099" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1099" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1099" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1099" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1099" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1099" s="4">
+        <f t="shared" si="222"/>
+        <v>2024</v>
+      </c>
+      <c r="J1099" s="4">
+        <f t="shared" si="223"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1100" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1100" s="3"/>
-      <c r="B1100" s="3"/>
-      <c r="C1100" s="3"/>
-      <c r="D1100" s="3"/>
-      <c r="E1100" s="3"/>
-      <c r="F1100" s="3"/>
-      <c r="G1100" s="3"/>
-      <c r="H1100" s="3"/>
-      <c r="I1100" s="4"/>
-      <c r="J1100" s="4"/>
+      <c r="A1100" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B1100" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1100" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1100" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1100" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1100" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1100" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1100" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1100" s="4">
+        <f t="shared" ref="I1100:I1102" si="224">YEAR(A1100)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1100" s="4">
+        <f t="shared" ref="J1100:J1102" si="225">MONTH(A1100)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1101" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1101" s="3"/>
-      <c r="B1101" s="3"/>
-      <c r="C1101" s="3"/>
-      <c r="D1101" s="3"/>
-      <c r="E1101" s="3"/>
-      <c r="F1101" s="3"/>
-      <c r="G1101" s="3"/>
-      <c r="H1101" s="3"/>
-      <c r="I1101" s="4"/>
-      <c r="J1101" s="4"/>
+      <c r="A1101" s="3" t="s">
+        <v>1114</v>
+      </c>
+      <c r="B1101" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1101" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1101" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1101" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1101" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1101" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1101" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1101" s="4">
+        <f t="shared" si="224"/>
+        <v>2024</v>
+      </c>
+      <c r="J1101" s="4">
+        <f t="shared" si="225"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1102" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1102" s="3"/>
-      <c r="B1102" s="3"/>
-      <c r="C1102" s="3"/>
-      <c r="D1102" s="3"/>
-      <c r="E1102" s="3"/>
-      <c r="F1102" s="3"/>
-      <c r="G1102" s="3"/>
-      <c r="H1102" s="3"/>
-      <c r="I1102" s="4"/>
-      <c r="J1102" s="4"/>
+      <c r="A1102" s="3" t="s">
+        <v>1115</v>
+      </c>
+      <c r="B1102" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1102" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1102" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1102" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1102" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1102" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1102" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1102" s="4">
+        <f t="shared" si="224"/>
+        <v>2024</v>
+      </c>
+      <c r="J1102" s="4">
+        <f t="shared" si="225"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1103" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1103" s="3"/>
-      <c r="B1103" s="3"/>
-      <c r="C1103" s="3"/>
-      <c r="D1103" s="3"/>
-      <c r="E1103" s="3"/>
-      <c r="F1103" s="3"/>
-      <c r="G1103" s="3"/>
-      <c r="H1103" s="3"/>
-      <c r="I1103" s="4"/>
-      <c r="J1103" s="4"/>
+      <c r="A1103" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1103" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1103" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1103" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1103" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1103" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1103" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1103" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1103" s="4">
+        <f t="shared" ref="I1103:I1105" si="226">YEAR(A1103)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1103" s="4">
+        <f t="shared" ref="J1103:J1105" si="227">MONTH(A1103)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1104" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1104" s="3"/>
-      <c r="B1104" s="3"/>
-      <c r="C1104" s="3"/>
-      <c r="D1104" s="3"/>
-      <c r="E1104" s="3"/>
-      <c r="F1104" s="3"/>
-      <c r="G1104" s="3"/>
-      <c r="H1104" s="3"/>
-      <c r="I1104" s="4"/>
-      <c r="J1104" s="4"/>
+      <c r="A1104" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1104" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1104" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1104" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1104" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1104" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1104" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1104" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1104" s="4">
+        <f t="shared" si="226"/>
+        <v>2024</v>
+      </c>
+      <c r="J1104" s="4">
+        <f t="shared" si="227"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1105" s="3" t="s">
+        <v>1116</v>
+      </c>
+      <c r="B1105" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1105" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1105" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1105" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1105" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1105" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1105" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1105" s="4">
+        <f t="shared" si="226"/>
+        <v>2024</v>
+      </c>
+      <c r="J1105" s="4">
+        <f t="shared" si="227"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1106" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1106" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1106" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="D1106" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1106" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1106" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1106" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1106" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1106" s="4">
+        <f t="shared" ref="I1106:I1108" si="228">YEAR(A1106)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1106" s="4">
+        <f t="shared" ref="J1106:J1108" si="229">MONTH(A1106)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1107" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1107" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1107" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D1107" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1107" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1107" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1107" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1107" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1107" s="4">
+        <f t="shared" si="228"/>
+        <v>2024</v>
+      </c>
+      <c r="J1107" s="4">
+        <f t="shared" si="229"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1108" s="3" t="s">
+        <v>1117</v>
+      </c>
+      <c r="B1108" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1108" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1108" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1108" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1108" s="3" t="s">
+        <v>1099</v>
+      </c>
+      <c r="G1108" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1108" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1108" s="4">
+        <f t="shared" si="228"/>
+        <v>2024</v>
+      </c>
+      <c r="J1108" s="4">
+        <f t="shared" si="229"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1109" s="3"/>
+      <c r="B1109" s="3"/>
+      <c r="C1109" s="3"/>
+      <c r="D1109" s="3"/>
+      <c r="E1109" s="3"/>
+      <c r="F1109" s="3"/>
+      <c r="G1109" s="3"/>
+      <c r="H1109" s="3"/>
+      <c r="I1109" s="4"/>
+      <c r="J1109" s="4"/>
+    </row>
+    <row r="1110" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1110" s="3"/>
+      <c r="B1110" s="3"/>
+      <c r="C1110" s="3"/>
+      <c r="D1110" s="3"/>
+      <c r="E1110" s="3"/>
+      <c r="F1110" s="3"/>
+      <c r="G1110" s="3"/>
+      <c r="H1110" s="3"/>
+      <c r="I1110" s="4"/>
+      <c r="J1110" s="4"/>
+    </row>
+    <row r="1111" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1111" s="3"/>
+      <c r="B1111" s="3"/>
+      <c r="C1111" s="3"/>
+      <c r="D1111" s="3"/>
+      <c r="E1111" s="3"/>
+      <c r="F1111" s="3"/>
+      <c r="G1111" s="3"/>
+      <c r="H1111" s="3"/>
+      <c r="I1111" s="4"/>
+      <c r="J1111" s="4"/>
+    </row>
+    <row r="1112" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1112" s="3"/>
+      <c r="B1112" s="3"/>
+      <c r="C1112" s="3"/>
+      <c r="D1112" s="3"/>
+      <c r="E1112" s="3"/>
+      <c r="F1112" s="3"/>
+      <c r="G1112" s="3"/>
+      <c r="H1112" s="3"/>
+      <c r="I1112" s="4"/>
+      <c r="J1112" s="4"/>
+    </row>
+    <row r="1113" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1113" s="3"/>
+      <c r="B1113" s="3"/>
+      <c r="C1113" s="3"/>
+      <c r="D1113" s="3"/>
+      <c r="E1113" s="3"/>
+      <c r="F1113" s="3"/>
+      <c r="G1113" s="3"/>
+      <c r="H1113" s="3"/>
+      <c r="I1113" s="4"/>
+      <c r="J1113" s="4"/>
+    </row>
+    <row r="1114" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1114" s="3"/>
+      <c r="B1114" s="3"/>
+      <c r="C1114" s="3"/>
+      <c r="D1114" s="3"/>
+      <c r="E1114" s="3"/>
+      <c r="F1114" s="3"/>
+      <c r="G1114" s="3"/>
+      <c r="H1114" s="3"/>
+      <c r="I1114" s="4"/>
+      <c r="J1114" s="4"/>
+    </row>
+    <row r="1115" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1115" s="3"/>
+      <c r="B1115" s="3"/>
+      <c r="C1115" s="3"/>
+      <c r="D1115" s="3"/>
+      <c r="E1115" s="3"/>
+      <c r="F1115" s="3"/>
+      <c r="G1115" s="3"/>
+      <c r="H1115" s="3"/>
+      <c r="I1115" s="4"/>
+      <c r="J1115" s="4"/>
+    </row>
+    <row r="1116" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1116" s="3"/>
+      <c r="B1116" s="3"/>
+      <c r="C1116" s="3"/>
+      <c r="D1116" s="3"/>
+      <c r="E1116" s="3"/>
+      <c r="F1116" s="3"/>
+      <c r="G1116" s="3"/>
+      <c r="H1116" s="3"/>
+      <c r="I1116" s="4"/>
+      <c r="J1116" s="4"/>
+    </row>
+    <row r="1117" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1117" s="3"/>
+      <c r="B1117" s="3"/>
+      <c r="C1117" s="3"/>
+      <c r="D1117" s="3"/>
+      <c r="E1117" s="3"/>
+      <c r="F1117" s="3"/>
+      <c r="G1117" s="3"/>
+      <c r="H1117" s="3"/>
+      <c r="I1117" s="4"/>
+      <c r="J1117" s="4"/>
+    </row>
+    <row r="1118" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1118" s="3"/>
+      <c r="B1118" s="3"/>
+      <c r="C1118" s="3"/>
+      <c r="D1118" s="3"/>
+      <c r="E1118" s="3"/>
+      <c r="F1118" s="3"/>
+      <c r="G1118" s="3"/>
+      <c r="H1118" s="3"/>
+      <c r="I1118" s="4"/>
+      <c r="J1118" s="4"/>
+    </row>
+    <row r="1119" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1119" s="3"/>
+      <c r="B1119" s="3"/>
+      <c r="C1119" s="3"/>
+      <c r="D1119" s="3"/>
+      <c r="E1119" s="3"/>
+      <c r="F1119" s="3"/>
+      <c r="G1119" s="3"/>
+      <c r="H1119" s="3"/>
+      <c r="I1119" s="4"/>
+      <c r="J1119" s="4"/>
+    </row>
+    <row r="1120" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1120" s="3"/>
+      <c r="B1120" s="3"/>
+      <c r="C1120" s="3"/>
+      <c r="D1120" s="3"/>
+      <c r="E1120" s="3"/>
+      <c r="F1120" s="3"/>
+      <c r="G1120" s="3"/>
+      <c r="H1120" s="3"/>
+      <c r="I1120" s="4"/>
+      <c r="J1120" s="4"/>
+    </row>
+    <row r="1121" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1121" s="3"/>
+      <c r="B1121" s="3"/>
+      <c r="C1121" s="3"/>
+      <c r="D1121" s="3"/>
+      <c r="E1121" s="3"/>
+      <c r="F1121" s="3"/>
+      <c r="G1121" s="3"/>
+      <c r="H1121" s="3"/>
+      <c r="I1121" s="4"/>
+      <c r="J1121" s="4"/>
+    </row>
+    <row r="1122" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1122" s="3"/>
+      <c r="B1122" s="3"/>
+      <c r="C1122" s="3"/>
+      <c r="D1122" s="3"/>
+      <c r="E1122" s="3"/>
+      <c r="F1122" s="3"/>
+      <c r="G1122" s="3"/>
+      <c r="H1122" s="3"/>
+      <c r="I1122" s="4"/>
+      <c r="J1122" s="4"/>
+    </row>
+    <row r="1123" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1123" s="3"/>
+      <c r="B1123" s="3"/>
+      <c r="C1123" s="3"/>
+      <c r="D1123" s="3"/>
+      <c r="E1123" s="3"/>
+      <c r="F1123" s="3"/>
+      <c r="G1123" s="3"/>
+      <c r="H1123" s="3"/>
+      <c r="I1123" s="4"/>
+      <c r="J1123" s="4"/>
+    </row>
+    <row r="1124" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1124" s="3"/>
+      <c r="B1124" s="3"/>
+      <c r="C1124" s="3"/>
+      <c r="D1124" s="3"/>
+      <c r="E1124" s="3"/>
+      <c r="F1124" s="3"/>
+      <c r="G1124" s="3"/>
+      <c r="H1124" s="3"/>
+      <c r="I1124" s="4"/>
+      <c r="J1124" s="4"/>
+    </row>
+    <row r="1125" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1125" s="3"/>
+      <c r="B1125" s="3"/>
+      <c r="C1125" s="3"/>
+      <c r="D1125" s="3"/>
+      <c r="E1125" s="3"/>
+      <c r="F1125" s="3"/>
+      <c r="G1125" s="3"/>
+      <c r="H1125" s="3"/>
+      <c r="I1125" s="4"/>
+      <c r="J1125" s="4"/>
+    </row>
+    <row r="1126" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1126" s="3"/>
+      <c r="B1126" s="3"/>
+      <c r="C1126" s="3"/>
+      <c r="D1126" s="3"/>
+      <c r="E1126" s="3"/>
+      <c r="F1126" s="3"/>
+      <c r="G1126" s="3"/>
+      <c r="H1126" s="3"/>
+      <c r="I1126" s="4"/>
+      <c r="J1126" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-07-06.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8685" uniqueCount="1118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8769" uniqueCount="1122">
   <si>
     <t>Year</t>
   </si>
@@ -3376,6 +3376,18 @@
   </si>
   <si>
     <t>2024-06-24</t>
+  </si>
+  <si>
+    <t>2024-06-27</t>
+  </si>
+  <si>
+    <t>2024-07-04</t>
+  </si>
+  <si>
+    <t>2024-07-05</t>
+  </si>
+  <si>
+    <t>2024-07-06</t>
   </si>
 </sst>
 </file>
@@ -3775,11 +3787,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1126"/>
+  <dimension ref="A1:J1149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1085" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1101" sqref="F1101"/>
+      <pane ySplit="1" topLeftCell="A1103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1123" sqref="F1123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -41029,11 +41041,11 @@
         <v>279</v>
       </c>
       <c r="I1106" s="4">
-        <f t="shared" ref="I1106:I1108" si="228">YEAR(A1106)</f>
+        <f t="shared" ref="I1106:I1110" si="228">YEAR(A1106)</f>
         <v>2024</v>
       </c>
       <c r="J1106" s="4">
-        <f t="shared" ref="J1106:J1108" si="229">MONTH(A1106)</f>
+        <f t="shared" ref="J1106:J1110" si="229">MONTH(A1106)</f>
         <v>6</v>
       </c>
     </row>
@@ -41106,148 +41118,388 @@
       </c>
     </row>
     <row r="1109" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1109" s="3"/>
-      <c r="B1109" s="3"/>
-      <c r="C1109" s="3"/>
-      <c r="D1109" s="3"/>
-      <c r="E1109" s="3"/>
+      <c r="A1109" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B1109" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1109" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1109" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1109" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1109" s="3"/>
-      <c r="G1109" s="3"/>
-      <c r="H1109" s="3"/>
-      <c r="I1109" s="4"/>
-      <c r="J1109" s="4"/>
+      <c r="G1109" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1109" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1109" s="4">
+        <f t="shared" si="228"/>
+        <v>2024</v>
+      </c>
+      <c r="J1109" s="4">
+        <f t="shared" si="229"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1110" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1110" s="3"/>
-      <c r="B1110" s="3"/>
-      <c r="C1110" s="3"/>
-      <c r="D1110" s="3"/>
-      <c r="E1110" s="3"/>
+      <c r="A1110" s="3" t="s">
+        <v>1118</v>
+      </c>
+      <c r="B1110" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1110" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1110" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1110" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1110" s="3"/>
-      <c r="G1110" s="3"/>
-      <c r="H1110" s="3"/>
-      <c r="I1110" s="4"/>
-      <c r="J1110" s="4"/>
+      <c r="G1110" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1110" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1110" s="4">
+        <f t="shared" si="228"/>
+        <v>2024</v>
+      </c>
+      <c r="J1110" s="4">
+        <f t="shared" si="229"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1111" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1111" s="3"/>
-      <c r="B1111" s="3"/>
-      <c r="C1111" s="3"/>
-      <c r="D1111" s="3"/>
-      <c r="E1111" s="3"/>
+      <c r="A1111" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1111" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1111" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1111" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1111" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1111" s="3"/>
-      <c r="G1111" s="3"/>
-      <c r="H1111" s="3"/>
-      <c r="I1111" s="4"/>
-      <c r="J1111" s="4"/>
+      <c r="G1111" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1111" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1111" s="4">
+        <f t="shared" ref="I1111:I1112" si="230">YEAR(A1111)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1111" s="4">
+        <f t="shared" ref="J1111:J1112" si="231">MONTH(A1111)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1112" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1112" s="3"/>
-      <c r="B1112" s="3"/>
-      <c r="C1112" s="3"/>
-      <c r="D1112" s="3"/>
-      <c r="E1112" s="3"/>
+      <c r="A1112" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1112" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1112" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1112" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1112" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1112" s="3"/>
-      <c r="G1112" s="3"/>
-      <c r="H1112" s="3"/>
-      <c r="I1112" s="4"/>
-      <c r="J1112" s="4"/>
+      <c r="G1112" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1112" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1112" s="4">
+        <f t="shared" si="230"/>
+        <v>2024</v>
+      </c>
+      <c r="J1112" s="4">
+        <f t="shared" si="231"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1113" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1113" s="3"/>
-      <c r="B1113" s="3"/>
-      <c r="C1113" s="3"/>
-      <c r="D1113" s="3"/>
-      <c r="E1113" s="3"/>
+      <c r="A1113" s="3" t="s">
+        <v>1119</v>
+      </c>
+      <c r="B1113" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1113" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1113" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1113" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1113" s="3"/>
-      <c r="G1113" s="3"/>
-      <c r="H1113" s="3"/>
-      <c r="I1113" s="4"/>
-      <c r="J1113" s="4"/>
+      <c r="G1113" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1113" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1113" s="4">
+        <f t="shared" ref="I1113:I1114" si="232">YEAR(A1113)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1113" s="4">
+        <f t="shared" ref="J1113:J1114" si="233">MONTH(A1113)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1114" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1114" s="3"/>
-      <c r="B1114" s="3"/>
-      <c r="C1114" s="3"/>
-      <c r="D1114" s="3"/>
-      <c r="E1114" s="3"/>
+      <c r="A1114" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1114" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1114" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1114" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1114" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1114" s="3"/>
-      <c r="G1114" s="3"/>
-      <c r="H1114" s="3"/>
-      <c r="I1114" s="4"/>
-      <c r="J1114" s="4"/>
+      <c r="G1114" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1114" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1114" s="4">
+        <f t="shared" si="232"/>
+        <v>2024</v>
+      </c>
+      <c r="J1114" s="4">
+        <f t="shared" si="233"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1115" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1115" s="3"/>
-      <c r="B1115" s="3"/>
-      <c r="C1115" s="3"/>
-      <c r="D1115" s="3"/>
-      <c r="E1115" s="3"/>
+      <c r="A1115" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1115" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1115" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1115" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1115" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1115" s="3"/>
-      <c r="G1115" s="3"/>
-      <c r="H1115" s="3"/>
-      <c r="I1115" s="4"/>
-      <c r="J1115" s="4"/>
+      <c r="G1115" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1115" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1115" s="4">
+        <f t="shared" ref="I1115" si="234">YEAR(A1115)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1115" s="4">
+        <f t="shared" ref="J1115" si="235">MONTH(A1115)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1116" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1116" s="3"/>
-      <c r="B1116" s="3"/>
-      <c r="C1116" s="3"/>
-      <c r="D1116" s="3"/>
-      <c r="E1116" s="3"/>
+      <c r="A1116" s="3" t="s">
+        <v>1120</v>
+      </c>
+      <c r="B1116" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1116" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1116" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1116" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1116" s="3"/>
-      <c r="G1116" s="3"/>
-      <c r="H1116" s="3"/>
-      <c r="I1116" s="4"/>
-      <c r="J1116" s="4"/>
+      <c r="G1116" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1116" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1116" s="4">
+        <f t="shared" ref="I1116:I1119" si="236">YEAR(A1116)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1116" s="4">
+        <f t="shared" ref="J1116:J1119" si="237">MONTH(A1116)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1117" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1117" s="3"/>
-      <c r="B1117" s="3"/>
-      <c r="C1117" s="3"/>
-      <c r="D1117" s="3"/>
-      <c r="E1117" s="3"/>
+      <c r="A1117" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1117" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1117" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1117" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1117" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1117" s="3"/>
-      <c r="G1117" s="3"/>
-      <c r="H1117" s="3"/>
-      <c r="I1117" s="4"/>
-      <c r="J1117" s="4"/>
+      <c r="G1117" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1117" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1117" s="4">
+        <f t="shared" si="236"/>
+        <v>2024</v>
+      </c>
+      <c r="J1117" s="4">
+        <f t="shared" si="237"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1118" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1118" s="3"/>
-      <c r="B1118" s="3"/>
-      <c r="C1118" s="3"/>
-      <c r="D1118" s="3"/>
-      <c r="E1118" s="3"/>
+      <c r="A1118" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1118" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1118" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1118" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1118" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1118" s="3"/>
-      <c r="G1118" s="3"/>
-      <c r="H1118" s="3"/>
-      <c r="I1118" s="4"/>
-      <c r="J1118" s="4"/>
+      <c r="G1118" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1118" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1118" s="4">
+        <f t="shared" si="236"/>
+        <v>2024</v>
+      </c>
+      <c r="J1118" s="4">
+        <f t="shared" si="237"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1119" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1119" s="3"/>
-      <c r="B1119" s="3"/>
-      <c r="C1119" s="3"/>
-      <c r="D1119" s="3"/>
-      <c r="E1119" s="3"/>
+      <c r="A1119" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1119" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1119" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1119" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1119" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1119" s="3"/>
-      <c r="G1119" s="3"/>
-      <c r="H1119" s="3"/>
-      <c r="I1119" s="4"/>
-      <c r="J1119" s="4"/>
+      <c r="G1119" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1119" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1119" s="4">
+        <f t="shared" si="236"/>
+        <v>2024</v>
+      </c>
+      <c r="J1119" s="4">
+        <f t="shared" si="237"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1120" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1120" s="3"/>
-      <c r="B1120" s="3"/>
-      <c r="C1120" s="3"/>
-      <c r="D1120" s="3"/>
-      <c r="E1120" s="3"/>
+      <c r="A1120" s="3" t="s">
+        <v>1121</v>
+      </c>
+      <c r="B1120" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1120" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1120" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1120" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1120" s="3"/>
-      <c r="G1120" s="3"/>
-      <c r="H1120" s="3"/>
-      <c r="I1120" s="4"/>
-      <c r="J1120" s="4"/>
+      <c r="G1120" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1120" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1120" s="4">
+        <f t="shared" ref="I1120" si="238">YEAR(A1120)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1120" s="4">
+        <f t="shared" ref="J1120" si="239">MONTH(A1120)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1121" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1121" s="3"/>
@@ -41321,6 +41573,282 @@
       <c r="I1126" s="4"/>
       <c r="J1126" s="4"/>
     </row>
+    <row r="1127" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1127" s="3"/>
+      <c r="B1127" s="3"/>
+      <c r="C1127" s="3"/>
+      <c r="D1127" s="3"/>
+      <c r="E1127" s="3"/>
+      <c r="F1127" s="3"/>
+      <c r="G1127" s="3"/>
+      <c r="H1127" s="3"/>
+      <c r="I1127" s="4"/>
+      <c r="J1127" s="4"/>
+    </row>
+    <row r="1128" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1128" s="3"/>
+      <c r="B1128" s="3"/>
+      <c r="C1128" s="3"/>
+      <c r="D1128" s="3"/>
+      <c r="E1128" s="3"/>
+      <c r="F1128" s="3"/>
+      <c r="G1128" s="3"/>
+      <c r="H1128" s="3"/>
+      <c r="I1128" s="4"/>
+      <c r="J1128" s="4"/>
+    </row>
+    <row r="1129" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1129" s="3"/>
+      <c r="B1129" s="3"/>
+      <c r="C1129" s="3"/>
+      <c r="D1129" s="3"/>
+      <c r="E1129" s="3"/>
+      <c r="F1129" s="3"/>
+      <c r="G1129" s="3"/>
+      <c r="H1129" s="3"/>
+      <c r="I1129" s="4"/>
+      <c r="J1129" s="4"/>
+    </row>
+    <row r="1130" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1130" s="3"/>
+      <c r="B1130" s="3"/>
+      <c r="C1130" s="3"/>
+      <c r="D1130" s="3"/>
+      <c r="E1130" s="3"/>
+      <c r="F1130" s="3"/>
+      <c r="G1130" s="3"/>
+      <c r="H1130" s="3"/>
+      <c r="I1130" s="4"/>
+      <c r="J1130" s="4"/>
+    </row>
+    <row r="1131" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1131" s="3"/>
+      <c r="B1131" s="3"/>
+      <c r="C1131" s="3"/>
+      <c r="D1131" s="3"/>
+      <c r="E1131" s="3"/>
+      <c r="F1131" s="3"/>
+      <c r="G1131" s="3"/>
+      <c r="H1131" s="3"/>
+      <c r="I1131" s="4"/>
+      <c r="J1131" s="4"/>
+    </row>
+    <row r="1132" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1132" s="3"/>
+      <c r="B1132" s="3"/>
+      <c r="C1132" s="3"/>
+      <c r="D1132" s="3"/>
+      <c r="E1132" s="3"/>
+      <c r="F1132" s="3"/>
+      <c r="G1132" s="3"/>
+      <c r="H1132" s="3"/>
+      <c r="I1132" s="4"/>
+      <c r="J1132" s="4"/>
+    </row>
+    <row r="1133" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1133" s="3"/>
+      <c r="B1133" s="3"/>
+      <c r="C1133" s="3"/>
+      <c r="D1133" s="3"/>
+      <c r="E1133" s="3"/>
+      <c r="F1133" s="3"/>
+      <c r="G1133" s="3"/>
+      <c r="H1133" s="3"/>
+      <c r="I1133" s="4"/>
+      <c r="J1133" s="4"/>
+    </row>
+    <row r="1134" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1134" s="3"/>
+      <c r="B1134" s="3"/>
+      <c r="C1134" s="3"/>
+      <c r="D1134" s="3"/>
+      <c r="E1134" s="3"/>
+      <c r="F1134" s="3"/>
+      <c r="G1134" s="3"/>
+      <c r="H1134" s="3"/>
+      <c r="I1134" s="4"/>
+      <c r="J1134" s="4"/>
+    </row>
+    <row r="1135" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1135" s="3"/>
+      <c r="B1135" s="3"/>
+      <c r="C1135" s="3"/>
+      <c r="D1135" s="3"/>
+      <c r="E1135" s="3"/>
+      <c r="F1135" s="3"/>
+      <c r="G1135" s="3"/>
+      <c r="H1135" s="3"/>
+      <c r="I1135" s="4"/>
+      <c r="J1135" s="4"/>
+    </row>
+    <row r="1136" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1136" s="3"/>
+      <c r="B1136" s="3"/>
+      <c r="C1136" s="3"/>
+      <c r="D1136" s="3"/>
+      <c r="E1136" s="3"/>
+      <c r="F1136" s="3"/>
+      <c r="G1136" s="3"/>
+      <c r="H1136" s="3"/>
+      <c r="I1136" s="4"/>
+      <c r="J1136" s="4"/>
+    </row>
+    <row r="1137" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1137" s="3"/>
+      <c r="B1137" s="3"/>
+      <c r="C1137" s="3"/>
+      <c r="D1137" s="3"/>
+      <c r="E1137" s="3"/>
+      <c r="F1137" s="3"/>
+      <c r="G1137" s="3"/>
+      <c r="H1137" s="3"/>
+      <c r="I1137" s="4"/>
+      <c r="J1137" s="4"/>
+    </row>
+    <row r="1138" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1138" s="3"/>
+      <c r="B1138" s="3"/>
+      <c r="C1138" s="3"/>
+      <c r="D1138" s="3"/>
+      <c r="E1138" s="3"/>
+      <c r="F1138" s="3"/>
+      <c r="G1138" s="3"/>
+      <c r="H1138" s="3"/>
+      <c r="I1138" s="4"/>
+      <c r="J1138" s="4"/>
+    </row>
+    <row r="1139" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1139" s="3"/>
+      <c r="B1139" s="3"/>
+      <c r="C1139" s="3"/>
+      <c r="D1139" s="3"/>
+      <c r="E1139" s="3"/>
+      <c r="F1139" s="3"/>
+      <c r="G1139" s="3"/>
+      <c r="H1139" s="3"/>
+      <c r="I1139" s="4"/>
+      <c r="J1139" s="4"/>
+    </row>
+    <row r="1140" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1140" s="3"/>
+      <c r="B1140" s="3"/>
+      <c r="C1140" s="3"/>
+      <c r="D1140" s="3"/>
+      <c r="E1140" s="3"/>
+      <c r="F1140" s="3"/>
+      <c r="G1140" s="3"/>
+      <c r="H1140" s="3"/>
+      <c r="I1140" s="4"/>
+      <c r="J1140" s="4"/>
+    </row>
+    <row r="1141" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1141" s="3"/>
+      <c r="B1141" s="3"/>
+      <c r="C1141" s="3"/>
+      <c r="D1141" s="3"/>
+      <c r="E1141" s="3"/>
+      <c r="F1141" s="3"/>
+      <c r="G1141" s="3"/>
+      <c r="H1141" s="3"/>
+      <c r="I1141" s="4"/>
+      <c r="J1141" s="4"/>
+    </row>
+    <row r="1142" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1142" s="3"/>
+      <c r="B1142" s="3"/>
+      <c r="C1142" s="3"/>
+      <c r="D1142" s="3"/>
+      <c r="E1142" s="3"/>
+      <c r="F1142" s="3"/>
+      <c r="G1142" s="3"/>
+      <c r="H1142" s="3"/>
+      <c r="I1142" s="4"/>
+      <c r="J1142" s="4"/>
+    </row>
+    <row r="1143" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1143" s="3"/>
+      <c r="B1143" s="3"/>
+      <c r="C1143" s="3"/>
+      <c r="D1143" s="3"/>
+      <c r="E1143" s="3"/>
+      <c r="F1143" s="3"/>
+      <c r="G1143" s="3"/>
+      <c r="H1143" s="3"/>
+      <c r="I1143" s="4"/>
+      <c r="J1143" s="4"/>
+    </row>
+    <row r="1144" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1144" s="3"/>
+      <c r="B1144" s="3"/>
+      <c r="C1144" s="3"/>
+      <c r="D1144" s="3"/>
+      <c r="E1144" s="3"/>
+      <c r="F1144" s="3"/>
+      <c r="G1144" s="3"/>
+      <c r="H1144" s="3"/>
+      <c r="I1144" s="4"/>
+      <c r="J1144" s="4"/>
+    </row>
+    <row r="1145" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1145" s="3"/>
+      <c r="B1145" s="3"/>
+      <c r="C1145" s="3"/>
+      <c r="D1145" s="3"/>
+      <c r="E1145" s="3"/>
+      <c r="F1145" s="3"/>
+      <c r="G1145" s="3"/>
+      <c r="H1145" s="3"/>
+      <c r="I1145" s="4"/>
+      <c r="J1145" s="4"/>
+    </row>
+    <row r="1146" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1146" s="3"/>
+      <c r="B1146" s="3"/>
+      <c r="C1146" s="3"/>
+      <c r="D1146" s="3"/>
+      <c r="E1146" s="3"/>
+      <c r="F1146" s="3"/>
+      <c r="G1146" s="3"/>
+      <c r="H1146" s="3"/>
+      <c r="I1146" s="4"/>
+      <c r="J1146" s="4"/>
+    </row>
+    <row r="1147" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1147" s="3"/>
+      <c r="B1147" s="3"/>
+      <c r="C1147" s="3"/>
+      <c r="D1147" s="3"/>
+      <c r="E1147" s="3"/>
+      <c r="F1147" s="3"/>
+      <c r="G1147" s="3"/>
+      <c r="H1147" s="3"/>
+      <c r="I1147" s="4"/>
+      <c r="J1147" s="4"/>
+    </row>
+    <row r="1148" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1148" s="3"/>
+      <c r="B1148" s="3"/>
+      <c r="C1148" s="3"/>
+      <c r="D1148" s="3"/>
+      <c r="E1148" s="3"/>
+      <c r="F1148" s="3"/>
+      <c r="G1148" s="3"/>
+      <c r="H1148" s="3"/>
+      <c r="I1148" s="4"/>
+      <c r="J1148" s="4"/>
+    </row>
+    <row r="1149" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1149" s="3"/>
+      <c r="B1149" s="3"/>
+      <c r="C1149" s="3"/>
+      <c r="D1149" s="3"/>
+      <c r="E1149" s="3"/>
+      <c r="F1149" s="3"/>
+      <c r="G1149" s="3"/>
+      <c r="H1149" s="3"/>
+      <c r="I1149" s="4"/>
+      <c r="J1149" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-07-09.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8769" uniqueCount="1122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8811" uniqueCount="1125">
   <si>
     <t>Year</t>
   </si>
@@ -3388,6 +3388,15 @@
   </si>
   <si>
     <t>2024-07-06</t>
+  </si>
+  <si>
+    <t>2024-07-07</t>
+  </si>
+  <si>
+    <t>2024-07-08</t>
+  </si>
+  <si>
+    <t>2024-07-09</t>
   </si>
 </sst>
 </file>
@@ -3790,8 +3799,8 @@
   <dimension ref="A1:J1149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1103" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1123" sqref="F1123"/>
+      <pane ySplit="1" topLeftCell="A1094" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1126" sqref="D1126"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -41493,85 +41502,205 @@
         <v>280</v>
       </c>
       <c r="I1120" s="4">
-        <f t="shared" ref="I1120" si="238">YEAR(A1120)</f>
+        <f t="shared" ref="I1120:I1122" si="238">YEAR(A1120)</f>
         <v>2024</v>
       </c>
       <c r="J1120" s="4">
-        <f t="shared" ref="J1120" si="239">MONTH(A1120)</f>
+        <f t="shared" ref="J1120:J1122" si="239">MONTH(A1120)</f>
         <v>7</v>
       </c>
     </row>
     <row r="1121" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1121" s="3"/>
-      <c r="B1121" s="3"/>
-      <c r="C1121" s="3"/>
-      <c r="D1121" s="3"/>
-      <c r="E1121" s="3"/>
+      <c r="A1121" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B1121" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1121" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1121" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1121" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1121" s="3"/>
-      <c r="G1121" s="3"/>
-      <c r="H1121" s="3"/>
-      <c r="I1121" s="4"/>
-      <c r="J1121" s="4"/>
+      <c r="G1121" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1121" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1121" s="4">
+        <f t="shared" si="238"/>
+        <v>2024</v>
+      </c>
+      <c r="J1121" s="4">
+        <f t="shared" si="239"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1122" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1122" s="3"/>
-      <c r="B1122" s="3"/>
-      <c r="C1122" s="3"/>
-      <c r="D1122" s="3"/>
-      <c r="E1122" s="3"/>
+      <c r="A1122" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B1122" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1122" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1122" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1122" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1122" s="3"/>
-      <c r="G1122" s="3"/>
-      <c r="H1122" s="3"/>
-      <c r="I1122" s="4"/>
-      <c r="J1122" s="4"/>
+      <c r="G1122" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1122" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1122" s="4">
+        <f t="shared" si="238"/>
+        <v>2024</v>
+      </c>
+      <c r="J1122" s="4">
+        <f t="shared" si="239"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1123" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1123" s="3"/>
-      <c r="B1123" s="3"/>
-      <c r="C1123" s="3"/>
-      <c r="D1123" s="3"/>
-      <c r="E1123" s="3"/>
+      <c r="A1123" s="3" t="s">
+        <v>1122</v>
+      </c>
+      <c r="B1123" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1123" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1123" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1123" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1123" s="3"/>
-      <c r="G1123" s="3"/>
-      <c r="H1123" s="3"/>
-      <c r="I1123" s="4"/>
-      <c r="J1123" s="4"/>
+      <c r="G1123" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1123" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1123" s="4">
+        <f t="shared" ref="I1123" si="240">YEAR(A1123)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1123" s="4">
+        <f t="shared" ref="J1123" si="241">MONTH(A1123)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1124" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1124" s="3"/>
-      <c r="B1124" s="3"/>
-      <c r="C1124" s="3"/>
-      <c r="D1124" s="3"/>
-      <c r="E1124" s="3"/>
+      <c r="A1124" s="3" t="s">
+        <v>1123</v>
+      </c>
+      <c r="B1124" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1124" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1124" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1124" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1124" s="3"/>
-      <c r="G1124" s="3"/>
-      <c r="H1124" s="3"/>
-      <c r="I1124" s="4"/>
-      <c r="J1124" s="4"/>
+      <c r="G1124" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1124" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1124" s="4">
+        <f t="shared" ref="I1124" si="242">YEAR(A1124)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1124" s="4">
+        <f t="shared" ref="J1124" si="243">MONTH(A1124)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1125" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1125" s="3"/>
-      <c r="B1125" s="3"/>
-      <c r="C1125" s="3"/>
-      <c r="D1125" s="3"/>
-      <c r="E1125" s="3"/>
+      <c r="A1125" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1125" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1125" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1125" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1125" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1125" s="3"/>
-      <c r="G1125" s="3"/>
-      <c r="H1125" s="3"/>
-      <c r="I1125" s="4"/>
-      <c r="J1125" s="4"/>
+      <c r="G1125" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1125" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1125" s="4">
+        <f t="shared" ref="I1125:I1126" si="244">YEAR(A1125)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1125" s="4">
+        <f t="shared" ref="J1125:J1126" si="245">MONTH(A1125)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1126" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1126" s="3"/>
-      <c r="B1126" s="3"/>
-      <c r="C1126" s="3"/>
-      <c r="D1126" s="3"/>
-      <c r="E1126" s="3"/>
+      <c r="A1126" s="3" t="s">
+        <v>1124</v>
+      </c>
+      <c r="B1126" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1126" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1126" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1126" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1126" s="3"/>
-      <c r="G1126" s="3"/>
-      <c r="H1126" s="3"/>
-      <c r="I1126" s="4"/>
-      <c r="J1126" s="4"/>
+      <c r="G1126" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1126" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1126" s="4">
+        <f t="shared" si="244"/>
+        <v>2024</v>
+      </c>
+      <c r="J1126" s="4">
+        <f t="shared" si="245"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1127" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1127" s="3"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-07-13.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8811" uniqueCount="1125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8853" uniqueCount="1128">
   <si>
     <t>Year</t>
   </si>
@@ -3397,6 +3397,15 @@
   </si>
   <si>
     <t>2024-07-09</t>
+  </si>
+  <si>
+    <t>2024-07-11</t>
+  </si>
+  <si>
+    <t>2024-07-12</t>
+  </si>
+  <si>
+    <t>2024-07-13</t>
   </si>
 </sst>
 </file>
@@ -3799,8 +3808,8 @@
   <dimension ref="A1:J1149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1094" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1126" sqref="D1126"/>
+      <pane ySplit="1" topLeftCell="A1106" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1130" sqref="F1130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -41703,76 +41712,196 @@
       </c>
     </row>
     <row r="1127" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1127" s="3"/>
-      <c r="B1127" s="3"/>
-      <c r="C1127" s="3"/>
-      <c r="D1127" s="3"/>
-      <c r="E1127" s="3"/>
+      <c r="A1127" s="3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1127" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1127" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1127" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1127" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1127" s="3"/>
-      <c r="G1127" s="3"/>
-      <c r="H1127" s="3"/>
-      <c r="I1127" s="4"/>
-      <c r="J1127" s="4"/>
+      <c r="G1127" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1127" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1127" s="4">
+        <f t="shared" ref="I1127:I1128" si="246">YEAR(A1127)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1127" s="4">
+        <f t="shared" ref="J1127:J1128" si="247">MONTH(A1127)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1128" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1128" s="3"/>
-      <c r="B1128" s="3"/>
-      <c r="C1128" s="3"/>
-      <c r="D1128" s="3"/>
-      <c r="E1128" s="3"/>
+      <c r="A1128" s="3" t="s">
+        <v>1125</v>
+      </c>
+      <c r="B1128" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1128" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1128" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1128" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1128" s="3"/>
-      <c r="G1128" s="3"/>
-      <c r="H1128" s="3"/>
-      <c r="I1128" s="4"/>
-      <c r="J1128" s="4"/>
+      <c r="G1128" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1128" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1128" s="4">
+        <f t="shared" si="246"/>
+        <v>2024</v>
+      </c>
+      <c r="J1128" s="4">
+        <f t="shared" si="247"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1129" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1129" s="3"/>
-      <c r="B1129" s="3"/>
-      <c r="C1129" s="3"/>
-      <c r="D1129" s="3"/>
-      <c r="E1129" s="3"/>
+      <c r="A1129" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B1129" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1129" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1129" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1129" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1129" s="3"/>
-      <c r="G1129" s="3"/>
-      <c r="H1129" s="3"/>
-      <c r="I1129" s="4"/>
-      <c r="J1129" s="4"/>
+      <c r="G1129" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1129" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1129" s="4">
+        <f t="shared" ref="I1129:I1130" si="248">YEAR(A1129)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1129" s="4">
+        <f t="shared" ref="J1129:J1130" si="249">MONTH(A1129)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1130" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1130" s="3"/>
-      <c r="B1130" s="3"/>
-      <c r="C1130" s="3"/>
-      <c r="D1130" s="3"/>
-      <c r="E1130" s="3"/>
+      <c r="A1130" s="3" t="s">
+        <v>1126</v>
+      </c>
+      <c r="B1130" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1130" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1130" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1130" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1130" s="3"/>
-      <c r="G1130" s="3"/>
-      <c r="H1130" s="3"/>
-      <c r="I1130" s="4"/>
-      <c r="J1130" s="4"/>
+      <c r="G1130" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1130" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1130" s="4">
+        <f t="shared" si="248"/>
+        <v>2024</v>
+      </c>
+      <c r="J1130" s="4">
+        <f t="shared" si="249"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1131" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1131" s="3"/>
-      <c r="B1131" s="3"/>
-      <c r="C1131" s="3"/>
-      <c r="D1131" s="3"/>
-      <c r="E1131" s="3"/>
+      <c r="A1131" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B1131" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1131" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1131" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1131" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1131" s="3"/>
-      <c r="G1131" s="3"/>
-      <c r="H1131" s="3"/>
-      <c r="I1131" s="4"/>
-      <c r="J1131" s="4"/>
+      <c r="G1131" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1131" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1131" s="4">
+        <f t="shared" ref="I1131:I1132" si="250">YEAR(A1131)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1131" s="4">
+        <f t="shared" ref="J1131:J1132" si="251">MONTH(A1131)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1132" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1132" s="3"/>
-      <c r="B1132" s="3"/>
-      <c r="C1132" s="3"/>
-      <c r="D1132" s="3"/>
-      <c r="E1132" s="3"/>
+      <c r="A1132" s="3" t="s">
+        <v>1127</v>
+      </c>
+      <c r="B1132" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1132" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1132" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1132" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1132" s="3"/>
-      <c r="G1132" s="3"/>
-      <c r="H1132" s="3"/>
-      <c r="I1132" s="4"/>
-      <c r="J1132" s="4"/>
+      <c r="G1132" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1132" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1132" s="4">
+        <f t="shared" si="250"/>
+        <v>2024</v>
+      </c>
+      <c r="J1132" s="4">
+        <f t="shared" si="251"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1133" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1133" s="3"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-07-19.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8853" uniqueCount="1128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8909" uniqueCount="1134">
   <si>
     <t>Year</t>
   </si>
@@ -3406,6 +3406,24 @@
   </si>
   <si>
     <t>2024-07-13</t>
+  </si>
+  <si>
+    <t>2024-07-14</t>
+  </si>
+  <si>
+    <t>2024-07-15</t>
+  </si>
+  <si>
+    <t>2024-07-16</t>
+  </si>
+  <si>
+    <t>2024-07-17</t>
+  </si>
+  <si>
+    <t>2024-07-18</t>
+  </si>
+  <si>
+    <t>2024-07-19</t>
   </si>
 </sst>
 </file>
@@ -3808,8 +3826,8 @@
   <dimension ref="A1:J1149"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1106" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1130" sqref="F1130"/>
+      <pane ySplit="1" topLeftCell="A1109" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1145" sqref="C1145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -41904,100 +41922,260 @@
       </c>
     </row>
     <row r="1133" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1133" s="3"/>
-      <c r="B1133" s="3"/>
-      <c r="C1133" s="3"/>
-      <c r="D1133" s="3"/>
-      <c r="E1133" s="3"/>
+      <c r="A1133" s="3" t="s">
+        <v>1128</v>
+      </c>
+      <c r="B1133" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1133" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1133" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1133" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1133" s="3"/>
-      <c r="G1133" s="3"/>
-      <c r="H1133" s="3"/>
-      <c r="I1133" s="4"/>
-      <c r="J1133" s="4"/>
+      <c r="G1133" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1133" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1133" s="4">
+        <f t="shared" ref="I1133" si="252">YEAR(A1133)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1133" s="4">
+        <f t="shared" ref="J1133" si="253">MONTH(A1133)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1134" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1134" s="3"/>
-      <c r="B1134" s="3"/>
-      <c r="C1134" s="3"/>
-      <c r="D1134" s="3"/>
-      <c r="E1134" s="3"/>
+      <c r="A1134" s="3" t="s">
+        <v>1129</v>
+      </c>
+      <c r="B1134" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1134" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1134" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1134" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1134" s="3"/>
-      <c r="G1134" s="3"/>
-      <c r="H1134" s="3"/>
-      <c r="I1134" s="4"/>
-      <c r="J1134" s="4"/>
+      <c r="G1134" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1134" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1134" s="4">
+        <f t="shared" ref="I1134:I1135" si="254">YEAR(A1134)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1134" s="4">
+        <f t="shared" ref="J1134:J1135" si="255">MONTH(A1134)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1135" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1135" s="3"/>
-      <c r="B1135" s="3"/>
-      <c r="C1135" s="3"/>
-      <c r="D1135" s="3"/>
-      <c r="E1135" s="3"/>
+      <c r="A1135" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B1135" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1135" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1135" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1135" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1135" s="3"/>
-      <c r="G1135" s="3"/>
-      <c r="H1135" s="3"/>
-      <c r="I1135" s="4"/>
-      <c r="J1135" s="4"/>
+      <c r="G1135" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1135" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1135" s="4">
+        <f t="shared" si="254"/>
+        <v>2024</v>
+      </c>
+      <c r="J1135" s="4">
+        <f t="shared" si="255"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1136" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1136" s="3"/>
-      <c r="B1136" s="3"/>
-      <c r="C1136" s="3"/>
-      <c r="D1136" s="3"/>
-      <c r="E1136" s="3"/>
+      <c r="A1136" s="3" t="s">
+        <v>1130</v>
+      </c>
+      <c r="B1136" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1136" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1136" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1136" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1136" s="3"/>
-      <c r="G1136" s="3"/>
-      <c r="H1136" s="3"/>
-      <c r="I1136" s="4"/>
-      <c r="J1136" s="4"/>
+      <c r="G1136" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1136" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1136" s="4">
+        <f t="shared" ref="I1136" si="256">YEAR(A1136)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1136" s="4">
+        <f t="shared" ref="J1136" si="257">MONTH(A1136)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1137" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1137" s="3"/>
-      <c r="B1137" s="3"/>
-      <c r="C1137" s="3"/>
-      <c r="D1137" s="3"/>
-      <c r="E1137" s="3"/>
+      <c r="A1137" s="3" t="s">
+        <v>1131</v>
+      </c>
+      <c r="B1137" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1137" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1137" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1137" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1137" s="3"/>
-      <c r="G1137" s="3"/>
-      <c r="H1137" s="3"/>
-      <c r="I1137" s="4"/>
-      <c r="J1137" s="4"/>
+      <c r="G1137" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1137" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1137" s="4">
+        <f t="shared" ref="I1137" si="258">YEAR(A1137)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1137" s="4">
+        <f t="shared" ref="J1137" si="259">MONTH(A1137)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1138" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1138" s="3"/>
-      <c r="B1138" s="3"/>
-      <c r="C1138" s="3"/>
-      <c r="D1138" s="3"/>
-      <c r="E1138" s="3"/>
+      <c r="A1138" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B1138" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1138" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1138" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1138" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1138" s="3"/>
-      <c r="G1138" s="3"/>
-      <c r="H1138" s="3"/>
-      <c r="I1138" s="4"/>
-      <c r="J1138" s="4"/>
+      <c r="G1138" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1138" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1138" s="4">
+        <f t="shared" ref="I1138" si="260">YEAR(A1138)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1138" s="4">
+        <f t="shared" ref="J1138" si="261">MONTH(A1138)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1139" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1139" s="3"/>
-      <c r="B1139" s="3"/>
-      <c r="C1139" s="3"/>
-      <c r="D1139" s="3"/>
-      <c r="E1139" s="3"/>
+      <c r="A1139" s="3" t="s">
+        <v>1132</v>
+      </c>
+      <c r="B1139" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1139" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1139" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1139" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1139" s="3"/>
-      <c r="G1139" s="3"/>
-      <c r="H1139" s="3"/>
-      <c r="I1139" s="4"/>
-      <c r="J1139" s="4"/>
+      <c r="G1139" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1139" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1139" s="4">
+        <f t="shared" ref="I1139:I1140" si="262">YEAR(A1139)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1139" s="4">
+        <f t="shared" ref="J1139:J1140" si="263">MONTH(A1139)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1140" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1140" s="3"/>
-      <c r="B1140" s="3"/>
-      <c r="C1140" s="3"/>
-      <c r="D1140" s="3"/>
-      <c r="E1140" s="3"/>
+      <c r="A1140" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="B1140" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1140" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1140" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1140" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1140" s="3"/>
-      <c r="G1140" s="3"/>
-      <c r="H1140" s="3"/>
-      <c r="I1140" s="4"/>
-      <c r="J1140" s="4"/>
+      <c r="G1140" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1140" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1140" s="4">
+        <f t="shared" si="262"/>
+        <v>2024</v>
+      </c>
+      <c r="J1140" s="4">
+        <f t="shared" si="263"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1141" s="3"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated to 2024-07-23.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8909" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8944" uniqueCount="1136">
   <si>
     <t>Year</t>
   </si>
@@ -3424,6 +3424,12 @@
   </si>
   <si>
     <t>2024-07-19</t>
+  </si>
+  <si>
+    <t>2024-07-22</t>
+  </si>
+  <si>
+    <t>2024-07-23</t>
   </si>
 </sst>
 </file>
@@ -3823,11 +3829,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1149"/>
+  <dimension ref="A1:J1159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1109" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1145" sqref="C1145"/>
+      <pane ySplit="1" topLeftCell="A1124" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1147" sqref="D1147"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -42178,64 +42184,164 @@
       </c>
     </row>
     <row r="1141" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1141" s="3"/>
-      <c r="B1141" s="3"/>
-      <c r="C1141" s="3"/>
-      <c r="D1141" s="3"/>
-      <c r="E1141" s="3"/>
+      <c r="A1141" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B1141" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1141" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1141" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1141" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1141" s="3"/>
-      <c r="G1141" s="3"/>
-      <c r="H1141" s="3"/>
-      <c r="I1141" s="4"/>
-      <c r="J1141" s="4"/>
+      <c r="G1141" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1141" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1141" s="4">
+        <f t="shared" ref="I1141:I1143" si="264">YEAR(A1141)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1141" s="4">
+        <f t="shared" ref="J1141:J1143" si="265">MONTH(A1141)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1142" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1142" s="3"/>
-      <c r="B1142" s="3"/>
-      <c r="C1142" s="3"/>
-      <c r="D1142" s="3"/>
-      <c r="E1142" s="3"/>
+      <c r="A1142" s="3" t="s">
+        <v>1134</v>
+      </c>
+      <c r="B1142" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1142" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1142" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1142" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1142" s="3"/>
-      <c r="G1142" s="3"/>
-      <c r="H1142" s="3"/>
-      <c r="I1142" s="4"/>
-      <c r="J1142" s="4"/>
+      <c r="G1142" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1142" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1142" s="4">
+        <f t="shared" si="264"/>
+        <v>2024</v>
+      </c>
+      <c r="J1142" s="4">
+        <f t="shared" si="265"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1143" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1143" s="3"/>
-      <c r="B1143" s="3"/>
-      <c r="C1143" s="3"/>
-      <c r="D1143" s="3"/>
-      <c r="E1143" s="3"/>
+      <c r="A1143" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1143" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1143" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1143" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1143" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1143" s="3"/>
-      <c r="G1143" s="3"/>
-      <c r="H1143" s="3"/>
-      <c r="I1143" s="4"/>
-      <c r="J1143" s="4"/>
+      <c r="G1143" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1143" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1143" s="4">
+        <f t="shared" si="264"/>
+        <v>2024</v>
+      </c>
+      <c r="J1143" s="4">
+        <f t="shared" si="265"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1144" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1144" s="3"/>
-      <c r="B1144" s="3"/>
-      <c r="C1144" s="3"/>
-      <c r="D1144" s="3"/>
-      <c r="E1144" s="3"/>
+      <c r="A1144" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1144" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1144" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1144" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1144" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1144" s="3"/>
-      <c r="G1144" s="3"/>
-      <c r="H1144" s="3"/>
-      <c r="I1144" s="4"/>
-      <c r="J1144" s="4"/>
+      <c r="G1144" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1144" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1144" s="4">
+        <f t="shared" ref="I1144:I1145" si="266">YEAR(A1144)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1144" s="4">
+        <f t="shared" ref="J1144:J1145" si="267">MONTH(A1144)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1145" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1145" s="3"/>
-      <c r="B1145" s="3"/>
-      <c r="C1145" s="3"/>
-      <c r="D1145" s="3"/>
-      <c r="E1145" s="3"/>
+      <c r="A1145" s="3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="B1145" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1145" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1145" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1145" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1145" s="3"/>
-      <c r="G1145" s="3"/>
-      <c r="H1145" s="3"/>
-      <c r="I1145" s="4"/>
-      <c r="J1145" s="4"/>
+      <c r="G1145" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1145" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1145" s="4">
+        <f t="shared" si="266"/>
+        <v>2024</v>
+      </c>
+      <c r="J1145" s="4">
+        <f t="shared" si="267"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1146" s="3"/>
@@ -42285,6 +42391,126 @@
       <c r="I1149" s="4"/>
       <c r="J1149" s="4"/>
     </row>
+    <row r="1150" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1150" s="3"/>
+      <c r="B1150" s="3"/>
+      <c r="C1150" s="3"/>
+      <c r="D1150" s="3"/>
+      <c r="E1150" s="3"/>
+      <c r="F1150" s="3"/>
+      <c r="G1150" s="3"/>
+      <c r="H1150" s="3"/>
+      <c r="I1150" s="4"/>
+      <c r="J1150" s="4"/>
+    </row>
+    <row r="1151" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1151" s="3"/>
+      <c r="B1151" s="3"/>
+      <c r="C1151" s="3"/>
+      <c r="D1151" s="3"/>
+      <c r="E1151" s="3"/>
+      <c r="F1151" s="3"/>
+      <c r="G1151" s="3"/>
+      <c r="H1151" s="3"/>
+      <c r="I1151" s="4"/>
+      <c r="J1151" s="4"/>
+    </row>
+    <row r="1152" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1152" s="3"/>
+      <c r="B1152" s="3"/>
+      <c r="C1152" s="3"/>
+      <c r="D1152" s="3"/>
+      <c r="E1152" s="3"/>
+      <c r="F1152" s="3"/>
+      <c r="G1152" s="3"/>
+      <c r="H1152" s="3"/>
+      <c r="I1152" s="4"/>
+      <c r="J1152" s="4"/>
+    </row>
+    <row r="1153" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1153" s="3"/>
+      <c r="B1153" s="3"/>
+      <c r="C1153" s="3"/>
+      <c r="D1153" s="3"/>
+      <c r="E1153" s="3"/>
+      <c r="F1153" s="3"/>
+      <c r="G1153" s="3"/>
+      <c r="H1153" s="3"/>
+      <c r="I1153" s="4"/>
+      <c r="J1153" s="4"/>
+    </row>
+    <row r="1154" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1154" s="3"/>
+      <c r="B1154" s="3"/>
+      <c r="C1154" s="3"/>
+      <c r="D1154" s="3"/>
+      <c r="E1154" s="3"/>
+      <c r="F1154" s="3"/>
+      <c r="G1154" s="3"/>
+      <c r="H1154" s="3"/>
+      <c r="I1154" s="4"/>
+      <c r="J1154" s="4"/>
+    </row>
+    <row r="1155" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1155" s="3"/>
+      <c r="B1155" s="3"/>
+      <c r="C1155" s="3"/>
+      <c r="D1155" s="3"/>
+      <c r="E1155" s="3"/>
+      <c r="F1155" s="3"/>
+      <c r="G1155" s="3"/>
+      <c r="H1155" s="3"/>
+      <c r="I1155" s="4"/>
+      <c r="J1155" s="4"/>
+    </row>
+    <row r="1156" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1156" s="3"/>
+      <c r="B1156" s="3"/>
+      <c r="C1156" s="3"/>
+      <c r="D1156" s="3"/>
+      <c r="E1156" s="3"/>
+      <c r="F1156" s="3"/>
+      <c r="G1156" s="3"/>
+      <c r="H1156" s="3"/>
+      <c r="I1156" s="4"/>
+      <c r="J1156" s="4"/>
+    </row>
+    <row r="1157" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1157" s="3"/>
+      <c r="B1157" s="3"/>
+      <c r="C1157" s="3"/>
+      <c r="D1157" s="3"/>
+      <c r="E1157" s="3"/>
+      <c r="F1157" s="3"/>
+      <c r="G1157" s="3"/>
+      <c r="H1157" s="3"/>
+      <c r="I1157" s="4"/>
+      <c r="J1157" s="4"/>
+    </row>
+    <row r="1158" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1158" s="3"/>
+      <c r="B1158" s="3"/>
+      <c r="C1158" s="3"/>
+      <c r="D1158" s="3"/>
+      <c r="E1158" s="3"/>
+      <c r="F1158" s="3"/>
+      <c r="G1158" s="3"/>
+      <c r="H1158" s="3"/>
+      <c r="I1158" s="4"/>
+      <c r="J1158" s="4"/>
+    </row>
+    <row r="1159" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1159" s="3"/>
+      <c r="B1159" s="3"/>
+      <c r="C1159" s="3"/>
+      <c r="D1159" s="3"/>
+      <c r="E1159" s="3"/>
+      <c r="F1159" s="3"/>
+      <c r="G1159" s="3"/>
+      <c r="H1159" s="3"/>
+      <c r="I1159" s="4"/>
+      <c r="J1159" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated up to 2024-08-03.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8944" uniqueCount="1136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9037" uniqueCount="1144">
   <si>
     <t>Year</t>
   </si>
@@ -3430,6 +3430,30 @@
   </si>
   <si>
     <t>2024-07-23</t>
+  </si>
+  <si>
+    <t>2024-07-26</t>
+  </si>
+  <si>
+    <t>2024-07-25</t>
+  </si>
+  <si>
+    <t>2024-07-29</t>
+  </si>
+  <si>
+    <t>nwragagent v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-07-30</t>
+  </si>
+  <si>
+    <t>2024-08-01</t>
+  </si>
+  <si>
+    <t>2024-08-02</t>
+  </si>
+  <si>
+    <t>2024-08-03</t>
   </si>
 </sst>
 </file>
@@ -3829,11 +3853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1159"/>
+  <dimension ref="A1:J1171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1124" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1147" sqref="D1147"/>
+      <pane ySplit="1" topLeftCell="A1127" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1157" sqref="F1157"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -42344,160 +42368,424 @@
       </c>
     </row>
     <row r="1146" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1146" s="3"/>
-      <c r="B1146" s="3"/>
-      <c r="C1146" s="3"/>
-      <c r="D1146" s="3"/>
-      <c r="E1146" s="3"/>
+      <c r="A1146" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B1146" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1146" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1146" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1146" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1146" s="3"/>
-      <c r="G1146" s="3"/>
-      <c r="H1146" s="3"/>
-      <c r="I1146" s="4"/>
-      <c r="J1146" s="4"/>
+      <c r="G1146" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1146" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1146" s="4">
+        <f t="shared" ref="I1146:I1147" si="268">YEAR(A1146)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1146" s="4">
+        <f t="shared" ref="J1146:J1147" si="269">MONTH(A1146)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1147" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1147" s="3"/>
-      <c r="B1147" s="3"/>
-      <c r="C1147" s="3"/>
-      <c r="D1147" s="3"/>
-      <c r="E1147" s="3"/>
+      <c r="A1147" s="3" t="s">
+        <v>1137</v>
+      </c>
+      <c r="B1147" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1147" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1147" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1147" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1147" s="3"/>
-      <c r="G1147" s="3"/>
-      <c r="H1147" s="3"/>
-      <c r="I1147" s="4"/>
-      <c r="J1147" s="4"/>
+      <c r="G1147" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1147" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1147" s="4">
+        <f t="shared" si="268"/>
+        <v>2024</v>
+      </c>
+      <c r="J1147" s="4">
+        <f t="shared" si="269"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1148" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1148" s="3"/>
-      <c r="B1148" s="3"/>
-      <c r="C1148" s="3"/>
-      <c r="D1148" s="3"/>
-      <c r="E1148" s="3"/>
+      <c r="A1148" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B1148" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1148" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1148" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1148" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1148" s="3"/>
-      <c r="G1148" s="3"/>
-      <c r="H1148" s="3"/>
-      <c r="I1148" s="4"/>
-      <c r="J1148" s="4"/>
+      <c r="G1148" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1148" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1148" s="4">
+        <f t="shared" ref="I1148:I1149" si="270">YEAR(A1148)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1148" s="4">
+        <f t="shared" ref="J1148:J1149" si="271">MONTH(A1148)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1149" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1149" s="3"/>
-      <c r="B1149" s="3"/>
-      <c r="C1149" s="3"/>
-      <c r="D1149" s="3"/>
-      <c r="E1149" s="3"/>
+      <c r="A1149" s="3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="B1149" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1149" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1149" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1149" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1149" s="3"/>
-      <c r="G1149" s="3"/>
-      <c r="H1149" s="3"/>
-      <c r="I1149" s="4"/>
-      <c r="J1149" s="4"/>
+      <c r="G1149" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1149" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1149" s="4">
+        <f t="shared" si="270"/>
+        <v>2024</v>
+      </c>
+      <c r="J1149" s="4">
+        <f t="shared" si="271"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1150" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1150" s="3"/>
-      <c r="B1150" s="3"/>
-      <c r="C1150" s="3"/>
-      <c r="D1150" s="3"/>
-      <c r="E1150" s="3"/>
-      <c r="F1150" s="3"/>
-      <c r="G1150" s="3"/>
-      <c r="H1150" s="3"/>
-      <c r="I1150" s="4"/>
-      <c r="J1150" s="4"/>
+      <c r="A1150" s="3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B1150" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1150" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1150" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1150" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1150" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G1150" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1150" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1150" s="4">
+        <f t="shared" ref="I1150:I1152" si="272">YEAR(A1150)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1150" s="4">
+        <f t="shared" ref="J1150:J1152" si="273">MONTH(A1150)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1151" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1151" s="3"/>
-      <c r="B1151" s="3"/>
-      <c r="C1151" s="3"/>
-      <c r="D1151" s="3"/>
-      <c r="E1151" s="3"/>
-      <c r="F1151" s="3"/>
-      <c r="G1151" s="3"/>
-      <c r="H1151" s="3"/>
-      <c r="I1151" s="4"/>
-      <c r="J1151" s="4"/>
+      <c r="A1151" s="3" t="s">
+        <v>1138</v>
+      </c>
+      <c r="B1151" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1151" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1151" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1151" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1151" s="3" t="s">
+        <v>1139</v>
+      </c>
+      <c r="G1151" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1151" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1151" s="4">
+        <f t="shared" si="272"/>
+        <v>2024</v>
+      </c>
+      <c r="J1151" s="4">
+        <f t="shared" si="273"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1152" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1152" s="3"/>
-      <c r="B1152" s="3"/>
-      <c r="C1152" s="3"/>
-      <c r="D1152" s="3"/>
-      <c r="E1152" s="3"/>
+      <c r="A1152" s="3" t="s">
+        <v>1140</v>
+      </c>
+      <c r="B1152" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1152" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1152" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1152" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1152" s="3"/>
-      <c r="G1152" s="3"/>
-      <c r="H1152" s="3"/>
-      <c r="I1152" s="4"/>
-      <c r="J1152" s="4"/>
+      <c r="G1152" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1152" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1152" s="4">
+        <f t="shared" si="272"/>
+        <v>2024</v>
+      </c>
+      <c r="J1152" s="4">
+        <f t="shared" si="273"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1153" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1153" s="3"/>
-      <c r="B1153" s="3"/>
-      <c r="C1153" s="3"/>
-      <c r="D1153" s="3"/>
-      <c r="E1153" s="3"/>
+      <c r="A1153" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1153" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1153" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1153" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1153" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1153" s="3"/>
-      <c r="G1153" s="3"/>
-      <c r="H1153" s="3"/>
-      <c r="I1153" s="4"/>
-      <c r="J1153" s="4"/>
+      <c r="G1153" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1153" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1153" s="4">
+        <f t="shared" ref="I1153:I1154" si="274">YEAR(A1153)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1153" s="4">
+        <f t="shared" ref="J1153:J1154" si="275">MONTH(A1153)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1154" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1154" s="3"/>
-      <c r="B1154" s="3"/>
-      <c r="C1154" s="3"/>
-      <c r="D1154" s="3"/>
-      <c r="E1154" s="3"/>
+      <c r="A1154" s="3" t="s">
+        <v>1141</v>
+      </c>
+      <c r="B1154" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1154" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1154" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1154" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1154" s="3"/>
-      <c r="G1154" s="3"/>
-      <c r="H1154" s="3"/>
-      <c r="I1154" s="4"/>
-      <c r="J1154" s="4"/>
+      <c r="G1154" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1154" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1154" s="4">
+        <f t="shared" si="274"/>
+        <v>2024</v>
+      </c>
+      <c r="J1154" s="4">
+        <f t="shared" si="275"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1155" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1155" s="3"/>
-      <c r="B1155" s="3"/>
-      <c r="C1155" s="3"/>
-      <c r="D1155" s="3"/>
-      <c r="E1155" s="3"/>
+      <c r="A1155" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B1155" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1155" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1155" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1155" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1155" s="3"/>
-      <c r="G1155" s="3"/>
-      <c r="H1155" s="3"/>
-      <c r="I1155" s="4"/>
-      <c r="J1155" s="4"/>
+      <c r="G1155" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1155" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1155" s="4">
+        <f t="shared" ref="I1155:I1156" si="276">YEAR(A1155)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1155" s="4">
+        <f t="shared" ref="J1155:J1156" si="277">MONTH(A1155)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1156" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1156" s="3"/>
-      <c r="B1156" s="3"/>
-      <c r="C1156" s="3"/>
-      <c r="D1156" s="3"/>
-      <c r="E1156" s="3"/>
+      <c r="A1156" s="3" t="s">
+        <v>1142</v>
+      </c>
+      <c r="B1156" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1156" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1156" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1156" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1156" s="3"/>
-      <c r="G1156" s="3"/>
-      <c r="H1156" s="3"/>
-      <c r="I1156" s="4"/>
-      <c r="J1156" s="4"/>
+      <c r="G1156" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1156" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1156" s="4">
+        <f t="shared" si="276"/>
+        <v>2024</v>
+      </c>
+      <c r="J1156" s="4">
+        <f t="shared" si="277"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1157" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1157" s="3"/>
-      <c r="B1157" s="3"/>
-      <c r="C1157" s="3"/>
-      <c r="D1157" s="3"/>
-      <c r="E1157" s="3"/>
+      <c r="A1157" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1157" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1157" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1157" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1157" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1157" s="3"/>
-      <c r="G1157" s="3"/>
-      <c r="H1157" s="3"/>
-      <c r="I1157" s="4"/>
-      <c r="J1157" s="4"/>
+      <c r="G1157" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1157" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1157" s="4">
+        <f t="shared" ref="I1157" si="278">YEAR(A1157)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1157" s="4">
+        <f t="shared" ref="J1157" si="279">MONTH(A1157)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1158" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1158" s="3"/>
-      <c r="B1158" s="3"/>
-      <c r="C1158" s="3"/>
-      <c r="D1158" s="3"/>
-      <c r="E1158" s="3"/>
+      <c r="A1158" s="3" t="s">
+        <v>1143</v>
+      </c>
+      <c r="B1158" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1158" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1158" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1158" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1158" s="3"/>
-      <c r="G1158" s="3"/>
-      <c r="H1158" s="3"/>
-      <c r="I1158" s="4"/>
-      <c r="J1158" s="4"/>
+      <c r="G1158" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1158" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1158" s="4">
+        <f t="shared" ref="I1158" si="280">YEAR(A1158)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1158" s="4">
+        <f t="shared" ref="J1158" si="281">MONTH(A1158)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1159" s="3"/>
@@ -42511,6 +42799,150 @@
       <c r="I1159" s="4"/>
       <c r="J1159" s="4"/>
     </row>
+    <row r="1160" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1160" s="3"/>
+      <c r="B1160" s="3"/>
+      <c r="C1160" s="3"/>
+      <c r="D1160" s="3"/>
+      <c r="E1160" s="3"/>
+      <c r="F1160" s="3"/>
+      <c r="G1160" s="3"/>
+      <c r="H1160" s="3"/>
+      <c r="I1160" s="4"/>
+      <c r="J1160" s="4"/>
+    </row>
+    <row r="1161" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1161" s="3"/>
+      <c r="B1161" s="3"/>
+      <c r="C1161" s="3"/>
+      <c r="D1161" s="3"/>
+      <c r="E1161" s="3"/>
+      <c r="F1161" s="3"/>
+      <c r="G1161" s="3"/>
+      <c r="H1161" s="3"/>
+      <c r="I1161" s="4"/>
+      <c r="J1161" s="4"/>
+    </row>
+    <row r="1162" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1162" s="3"/>
+      <c r="B1162" s="3"/>
+      <c r="C1162" s="3"/>
+      <c r="D1162" s="3"/>
+      <c r="E1162" s="3"/>
+      <c r="F1162" s="3"/>
+      <c r="G1162" s="3"/>
+      <c r="H1162" s="3"/>
+      <c r="I1162" s="4"/>
+      <c r="J1162" s="4"/>
+    </row>
+    <row r="1163" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1163" s="3"/>
+      <c r="B1163" s="3"/>
+      <c r="C1163" s="3"/>
+      <c r="D1163" s="3"/>
+      <c r="E1163" s="3"/>
+      <c r="F1163" s="3"/>
+      <c r="G1163" s="3"/>
+      <c r="H1163" s="3"/>
+      <c r="I1163" s="4"/>
+      <c r="J1163" s="4"/>
+    </row>
+    <row r="1164" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1164" s="3"/>
+      <c r="B1164" s="3"/>
+      <c r="C1164" s="3"/>
+      <c r="D1164" s="3"/>
+      <c r="E1164" s="3"/>
+      <c r="F1164" s="3"/>
+      <c r="G1164" s="3"/>
+      <c r="H1164" s="3"/>
+      <c r="I1164" s="4"/>
+      <c r="J1164" s="4"/>
+    </row>
+    <row r="1165" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1165" s="3"/>
+      <c r="B1165" s="3"/>
+      <c r="C1165" s="3"/>
+      <c r="D1165" s="3"/>
+      <c r="E1165" s="3"/>
+      <c r="F1165" s="3"/>
+      <c r="G1165" s="3"/>
+      <c r="H1165" s="3"/>
+      <c r="I1165" s="4"/>
+      <c r="J1165" s="4"/>
+    </row>
+    <row r="1166" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1166" s="3"/>
+      <c r="B1166" s="3"/>
+      <c r="C1166" s="3"/>
+      <c r="D1166" s="3"/>
+      <c r="E1166" s="3"/>
+      <c r="F1166" s="3"/>
+      <c r="G1166" s="3"/>
+      <c r="H1166" s="3"/>
+      <c r="I1166" s="4"/>
+      <c r="J1166" s="4"/>
+    </row>
+    <row r="1167" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1167" s="3"/>
+      <c r="B1167" s="3"/>
+      <c r="C1167" s="3"/>
+      <c r="D1167" s="3"/>
+      <c r="E1167" s="3"/>
+      <c r="F1167" s="3"/>
+      <c r="G1167" s="3"/>
+      <c r="H1167" s="3"/>
+      <c r="I1167" s="4"/>
+      <c r="J1167" s="4"/>
+    </row>
+    <row r="1168" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1168" s="3"/>
+      <c r="B1168" s="3"/>
+      <c r="C1168" s="3"/>
+      <c r="D1168" s="3"/>
+      <c r="E1168" s="3"/>
+      <c r="F1168" s="3"/>
+      <c r="G1168" s="3"/>
+      <c r="H1168" s="3"/>
+      <c r="I1168" s="4"/>
+      <c r="J1168" s="4"/>
+    </row>
+    <row r="1169" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1169" s="3"/>
+      <c r="B1169" s="3"/>
+      <c r="C1169" s="3"/>
+      <c r="D1169" s="3"/>
+      <c r="E1169" s="3"/>
+      <c r="F1169" s="3"/>
+      <c r="G1169" s="3"/>
+      <c r="H1169" s="3"/>
+      <c r="I1169" s="4"/>
+      <c r="J1169" s="4"/>
+    </row>
+    <row r="1170" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1170" s="3"/>
+      <c r="B1170" s="3"/>
+      <c r="C1170" s="3"/>
+      <c r="D1170" s="3"/>
+      <c r="E1170" s="3"/>
+      <c r="F1170" s="3"/>
+      <c r="G1170" s="3"/>
+      <c r="H1170" s="3"/>
+      <c r="I1170" s="4"/>
+      <c r="J1170" s="4"/>
+    </row>
+    <row r="1171" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1171" s="3"/>
+      <c r="B1171" s="3"/>
+      <c r="C1171" s="3"/>
+      <c r="D1171" s="3"/>
+      <c r="E1171" s="3"/>
+      <c r="F1171" s="3"/>
+      <c r="G1171" s="3"/>
+      <c r="H1171" s="3"/>
+      <c r="I1171" s="4"/>
+      <c r="J1171" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#28 Time Tracking.xlsx: updated up to 2024-08-11.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9037" uniqueCount="1144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9100" uniqueCount="1147">
   <si>
     <t>Year</t>
   </si>
@@ -3454,6 +3454,15 @@
   </si>
   <si>
     <t>2024-08-03</t>
+  </si>
+  <si>
+    <t>2024-08-08</t>
+  </si>
+  <si>
+    <t>2024-08-09</t>
+  </si>
+  <si>
+    <t>2024-08-11</t>
   </si>
 </sst>
 </file>
@@ -3853,11 +3862,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1171"/>
+  <dimension ref="A1:J1181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1127" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1157" sqref="F1157"/>
+      <pane ySplit="1" topLeftCell="A1142" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1171" sqref="B1171"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -42779,121 +42788,301 @@
         <v>280</v>
       </c>
       <c r="I1158" s="4">
-        <f t="shared" ref="I1158" si="280">YEAR(A1158)</f>
+        <f t="shared" ref="I1158:I1159" si="280">YEAR(A1158)</f>
         <v>2024</v>
       </c>
       <c r="J1158" s="4">
-        <f t="shared" ref="J1158" si="281">MONTH(A1158)</f>
+        <f t="shared" ref="J1158:J1159" si="281">MONTH(A1158)</f>
         <v>8</v>
       </c>
     </row>
     <row r="1159" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1159" s="3"/>
-      <c r="B1159" s="3"/>
-      <c r="C1159" s="3"/>
-      <c r="D1159" s="3"/>
-      <c r="E1159" s="3"/>
+      <c r="A1159" s="3" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1159" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1159" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1159" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1159" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1159" s="3"/>
-      <c r="G1159" s="3"/>
-      <c r="H1159" s="3"/>
-      <c r="I1159" s="4"/>
-      <c r="J1159" s="4"/>
+      <c r="G1159" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1159" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1159" s="4">
+        <f t="shared" si="280"/>
+        <v>2024</v>
+      </c>
+      <c r="J1159" s="4">
+        <f t="shared" si="281"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1160" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1160" s="3"/>
-      <c r="B1160" s="3"/>
-      <c r="C1160" s="3"/>
-      <c r="D1160" s="3"/>
-      <c r="E1160" s="3"/>
+      <c r="A1160" s="3" t="s">
+        <v>1144</v>
+      </c>
+      <c r="B1160" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1160" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1160" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1160" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1160" s="3"/>
-      <c r="G1160" s="3"/>
-      <c r="H1160" s="3"/>
-      <c r="I1160" s="4"/>
-      <c r="J1160" s="4"/>
+      <c r="G1160" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1160" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1160" s="4">
+        <f t="shared" ref="I1160:I1161" si="282">YEAR(A1160)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1160" s="4">
+        <f t="shared" ref="J1160:J1161" si="283">MONTH(A1160)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1161" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1161" s="3"/>
-      <c r="B1161" s="3"/>
-      <c r="C1161" s="3"/>
-      <c r="D1161" s="3"/>
-      <c r="E1161" s="3"/>
+      <c r="A1161" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1161" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1161" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1161" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1161" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1161" s="3"/>
-      <c r="G1161" s="3"/>
-      <c r="H1161" s="3"/>
-      <c r="I1161" s="4"/>
-      <c r="J1161" s="4"/>
+      <c r="G1161" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1161" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1161" s="4">
+        <f t="shared" si="282"/>
+        <v>2024</v>
+      </c>
+      <c r="J1161" s="4">
+        <f t="shared" si="283"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1162" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1162" s="3"/>
-      <c r="B1162" s="3"/>
-      <c r="C1162" s="3"/>
-      <c r="D1162" s="3"/>
-      <c r="E1162" s="3"/>
+      <c r="A1162" s="3" t="s">
+        <v>1145</v>
+      </c>
+      <c r="B1162" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1162" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1162" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1162" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1162" s="3"/>
-      <c r="G1162" s="3"/>
-      <c r="H1162" s="3"/>
-      <c r="I1162" s="4"/>
-      <c r="J1162" s="4"/>
+      <c r="G1162" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1162" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1162" s="4">
+        <f t="shared" ref="I1162:I1166" si="284">YEAR(A1162)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1162" s="4">
+        <f t="shared" ref="J1162:J1166" si="285">MONTH(A1162)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1163" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1163" s="3"/>
-      <c r="B1163" s="3"/>
-      <c r="C1163" s="3"/>
-      <c r="D1163" s="3"/>
-      <c r="E1163" s="3"/>
+      <c r="A1163" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1163" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1163" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="D1163" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1163" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1163" s="3"/>
-      <c r="G1163" s="3"/>
-      <c r="H1163" s="3"/>
-      <c r="I1163" s="4"/>
-      <c r="J1163" s="4"/>
+      <c r="G1163" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1163" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1163" s="4">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="J1163" s="4">
+        <f t="shared" si="285"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1164" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1164" s="3"/>
-      <c r="B1164" s="3"/>
-      <c r="C1164" s="3"/>
-      <c r="D1164" s="3"/>
-      <c r="E1164" s="3"/>
+      <c r="A1164" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1164" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1164" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1164" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1164" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1164" s="3"/>
-      <c r="G1164" s="3"/>
-      <c r="H1164" s="3"/>
-      <c r="I1164" s="4"/>
-      <c r="J1164" s="4"/>
+      <c r="G1164" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1164" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1164" s="4">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="J1164" s="4">
+        <f t="shared" si="285"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1165" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1165" s="3"/>
-      <c r="B1165" s="3"/>
-      <c r="C1165" s="3"/>
-      <c r="D1165" s="3"/>
-      <c r="E1165" s="3"/>
+      <c r="A1165" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1165" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1165" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1165" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1165" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1165" s="3"/>
-      <c r="G1165" s="3"/>
-      <c r="H1165" s="3"/>
-      <c r="I1165" s="4"/>
-      <c r="J1165" s="4"/>
+      <c r="G1165" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1165" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1165" s="4">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="J1165" s="4">
+        <f t="shared" si="285"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1166" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1166" s="3"/>
-      <c r="B1166" s="3"/>
-      <c r="C1166" s="3"/>
-      <c r="D1166" s="3"/>
-      <c r="E1166" s="3"/>
+      <c r="A1166" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1166" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1166" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1166" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1166" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1166" s="3"/>
-      <c r="G1166" s="3"/>
-      <c r="H1166" s="3"/>
-      <c r="I1166" s="4"/>
-      <c r="J1166" s="4"/>
+      <c r="G1166" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1166" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1166" s="4">
+        <f t="shared" si="284"/>
+        <v>2024</v>
+      </c>
+      <c r="J1166" s="4">
+        <f t="shared" si="285"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1167" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1167" s="3"/>
-      <c r="B1167" s="3"/>
-      <c r="C1167" s="3"/>
-      <c r="D1167" s="3"/>
-      <c r="E1167" s="3"/>
+      <c r="A1167" s="3" t="s">
+        <v>1146</v>
+      </c>
+      <c r="B1167" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1167" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1167" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1167" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1167" s="3"/>
-      <c r="G1167" s="3"/>
-      <c r="H1167" s="3"/>
-      <c r="I1167" s="4"/>
-      <c r="J1167" s="4"/>
+      <c r="G1167" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1167" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1167" s="4">
+        <f t="shared" ref="I1167" si="286">YEAR(A1167)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1167" s="4">
+        <f t="shared" ref="J1167" si="287">MONTH(A1167)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1168" s="3"/>
@@ -42943,6 +43132,126 @@
       <c r="I1171" s="4"/>
       <c r="J1171" s="4"/>
     </row>
+    <row r="1172" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1172" s="3"/>
+      <c r="B1172" s="3"/>
+      <c r="C1172" s="3"/>
+      <c r="D1172" s="3"/>
+      <c r="E1172" s="3"/>
+      <c r="F1172" s="3"/>
+      <c r="G1172" s="3"/>
+      <c r="H1172" s="3"/>
+      <c r="I1172" s="4"/>
+      <c r="J1172" s="4"/>
+    </row>
+    <row r="1173" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1173" s="3"/>
+      <c r="B1173" s="3"/>
+      <c r="C1173" s="3"/>
+      <c r="D1173" s="3"/>
+      <c r="E1173" s="3"/>
+      <c r="F1173" s="3"/>
+      <c r="G1173" s="3"/>
+      <c r="H1173" s="3"/>
+      <c r="I1173" s="4"/>
+      <c r="J1173" s="4"/>
+    </row>
+    <row r="1174" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1174" s="3"/>
+      <c r="B1174" s="3"/>
+      <c r="C1174" s="3"/>
+      <c r="D1174" s="3"/>
+      <c r="E1174" s="3"/>
+      <c r="F1174" s="3"/>
+      <c r="G1174" s="3"/>
+      <c r="H1174" s="3"/>
+      <c r="I1174" s="4"/>
+      <c r="J1174" s="4"/>
+    </row>
+    <row r="1175" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1175" s="3"/>
+      <c r="B1175" s="3"/>
+      <c r="C1175" s="3"/>
+      <c r="D1175" s="3"/>
+      <c r="E1175" s="3"/>
+      <c r="F1175" s="3"/>
+      <c r="G1175" s="3"/>
+      <c r="H1175" s="3"/>
+      <c r="I1175" s="4"/>
+      <c r="J1175" s="4"/>
+    </row>
+    <row r="1176" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1176" s="3"/>
+      <c r="B1176" s="3"/>
+      <c r="C1176" s="3"/>
+      <c r="D1176" s="3"/>
+      <c r="E1176" s="3"/>
+      <c r="F1176" s="3"/>
+      <c r="G1176" s="3"/>
+      <c r="H1176" s="3"/>
+      <c r="I1176" s="4"/>
+      <c r="J1176" s="4"/>
+    </row>
+    <row r="1177" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1177" s="3"/>
+      <c r="B1177" s="3"/>
+      <c r="C1177" s="3"/>
+      <c r="D1177" s="3"/>
+      <c r="E1177" s="3"/>
+      <c r="F1177" s="3"/>
+      <c r="G1177" s="3"/>
+      <c r="H1177" s="3"/>
+      <c r="I1177" s="4"/>
+      <c r="J1177" s="4"/>
+    </row>
+    <row r="1178" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1178" s="3"/>
+      <c r="B1178" s="3"/>
+      <c r="C1178" s="3"/>
+      <c r="D1178" s="3"/>
+      <c r="E1178" s="3"/>
+      <c r="F1178" s="3"/>
+      <c r="G1178" s="3"/>
+      <c r="H1178" s="3"/>
+      <c r="I1178" s="4"/>
+      <c r="J1178" s="4"/>
+    </row>
+    <row r="1179" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1179" s="3"/>
+      <c r="B1179" s="3"/>
+      <c r="C1179" s="3"/>
+      <c r="D1179" s="3"/>
+      <c r="E1179" s="3"/>
+      <c r="F1179" s="3"/>
+      <c r="G1179" s="3"/>
+      <c r="H1179" s="3"/>
+      <c r="I1179" s="4"/>
+      <c r="J1179" s="4"/>
+    </row>
+    <row r="1180" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1180" s="3"/>
+      <c r="B1180" s="3"/>
+      <c r="C1180" s="3"/>
+      <c r="D1180" s="3"/>
+      <c r="E1180" s="3"/>
+      <c r="F1180" s="3"/>
+      <c r="G1180" s="3"/>
+      <c r="H1180" s="3"/>
+      <c r="I1180" s="4"/>
+      <c r="J1180" s="4"/>
+    </row>
+    <row r="1181" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1181" s="3"/>
+      <c r="B1181" s="3"/>
+      <c r="C1181" s="3"/>
+      <c r="D1181" s="3"/>
+      <c r="E1181" s="3"/>
+      <c r="F1181" s="3"/>
+      <c r="G1181" s="3"/>
+      <c r="H1181" s="3"/>
+      <c r="I1181" s="4"/>
+      <c r="J1181" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#30 Time Tracking.xlsx: updated up to 2024-08-19.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9100" uniqueCount="1147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9160" uniqueCount="1155">
   <si>
     <t>Year</t>
   </si>
@@ -3463,6 +3463,30 @@
   </si>
   <si>
     <t>2024-08-11</t>
+  </si>
+  <si>
+    <t>2024-08-12</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.4.0</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.4.0</t>
+  </si>
+  <si>
+    <t>2024-08-13</t>
+  </si>
+  <si>
+    <t>nwshared v1.2.0</t>
+  </si>
+  <si>
+    <t>2024-08-16</t>
+  </si>
+  <si>
+    <t>2024-08-18</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.1.0</t>
   </si>
 </sst>
 </file>
@@ -3862,11 +3886,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1181"/>
+  <dimension ref="A1:J1191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1142" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1171" sqref="B1171"/>
+      <pane ySplit="1" topLeftCell="A1163" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1178" sqref="F1178"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -43085,100 +43109,268 @@
       </c>
     </row>
     <row r="1168" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1168" s="3"/>
-      <c r="B1168" s="3"/>
-      <c r="C1168" s="3"/>
-      <c r="D1168" s="3"/>
-      <c r="E1168" s="3"/>
+      <c r="A1168" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1168" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1168" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1168" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1168" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1168" s="3"/>
-      <c r="G1168" s="3"/>
-      <c r="H1168" s="3"/>
-      <c r="I1168" s="4"/>
-      <c r="J1168" s="4"/>
+      <c r="G1168" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1168" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1168" s="4">
+        <f t="shared" ref="I1168:I1170" si="288">YEAR(A1168)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1168" s="4">
+        <f t="shared" ref="J1168:J1170" si="289">MONTH(A1168)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1169" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1169" s="3"/>
-      <c r="B1169" s="3"/>
-      <c r="C1169" s="3"/>
-      <c r="D1169" s="3"/>
-      <c r="E1169" s="3"/>
-      <c r="F1169" s="3"/>
-      <c r="G1169" s="3"/>
-      <c r="H1169" s="3"/>
-      <c r="I1169" s="4"/>
-      <c r="J1169" s="4"/>
+      <c r="A1169" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1169" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="C1169" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1169" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1169" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1169" s="3" t="s">
+        <v>1148</v>
+      </c>
+      <c r="G1169" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1169" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1169" s="4">
+        <f t="shared" si="288"/>
+        <v>2024</v>
+      </c>
+      <c r="J1169" s="4">
+        <f t="shared" si="289"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1170" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1170" s="3"/>
-      <c r="B1170" s="3"/>
-      <c r="C1170" s="3"/>
-      <c r="D1170" s="3"/>
-      <c r="E1170" s="3"/>
-      <c r="F1170" s="3"/>
-      <c r="G1170" s="3"/>
-      <c r="H1170" s="3"/>
-      <c r="I1170" s="4"/>
-      <c r="J1170" s="4"/>
+      <c r="A1170" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1170" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1170" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1170" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1170" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1170" s="3" t="s">
+        <v>1149</v>
+      </c>
+      <c r="G1170" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1170" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1170" s="4">
+        <f t="shared" si="288"/>
+        <v>2024</v>
+      </c>
+      <c r="J1170" s="4">
+        <f t="shared" si="289"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1171" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1171" s="3"/>
-      <c r="B1171" s="3"/>
-      <c r="C1171" s="3"/>
-      <c r="D1171" s="3"/>
-      <c r="E1171" s="3"/>
+      <c r="A1171" s="3" t="s">
+        <v>1147</v>
+      </c>
+      <c r="B1171" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1171" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1171" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1171" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1171" s="3"/>
-      <c r="G1171" s="3"/>
-      <c r="H1171" s="3"/>
-      <c r="I1171" s="4"/>
-      <c r="J1171" s="4"/>
+      <c r="G1171" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1171" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1171" s="4">
+        <f t="shared" ref="I1171:I1173" si="290">YEAR(A1171)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1171" s="4">
+        <f t="shared" ref="J1171:J1173" si="291">MONTH(A1171)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1172" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1172" s="3"/>
-      <c r="B1172" s="3"/>
-      <c r="C1172" s="3"/>
-      <c r="D1172" s="3"/>
-      <c r="E1172" s="3"/>
-      <c r="F1172" s="3"/>
-      <c r="G1172" s="3"/>
-      <c r="H1172" s="3"/>
-      <c r="I1172" s="4"/>
-      <c r="J1172" s="4"/>
+      <c r="A1172" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B1172" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1172" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1172" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1172" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1172" s="3" t="s">
+        <v>1151</v>
+      </c>
+      <c r="G1172" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1172" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1172" s="4">
+        <f t="shared" si="290"/>
+        <v>2024</v>
+      </c>
+      <c r="J1172" s="4">
+        <f t="shared" si="291"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1173" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1173" s="3"/>
-      <c r="B1173" s="3"/>
-      <c r="C1173" s="3"/>
-      <c r="D1173" s="3"/>
-      <c r="E1173" s="3"/>
-      <c r="F1173" s="3"/>
-      <c r="G1173" s="3"/>
-      <c r="H1173" s="3"/>
-      <c r="I1173" s="4"/>
-      <c r="J1173" s="4"/>
+      <c r="A1173" s="3" t="s">
+        <v>1150</v>
+      </c>
+      <c r="B1173" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1173" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1173" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1173" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1173" s="3" t="s">
+        <v>1154</v>
+      </c>
+      <c r="G1173" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1173" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1173" s="4">
+        <f t="shared" si="290"/>
+        <v>2024</v>
+      </c>
+      <c r="J1173" s="4">
+        <f t="shared" si="291"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1174" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1174" s="3"/>
-      <c r="B1174" s="3"/>
-      <c r="C1174" s="3"/>
-      <c r="D1174" s="3"/>
-      <c r="E1174" s="3"/>
+      <c r="A1174" s="3" t="s">
+        <v>1152</v>
+      </c>
+      <c r="B1174" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1174" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1174" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1174" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1174" s="3"/>
-      <c r="G1174" s="3"/>
-      <c r="H1174" s="3"/>
-      <c r="I1174" s="4"/>
-      <c r="J1174" s="4"/>
+      <c r="G1174" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1174" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1174" s="4">
+        <f t="shared" ref="I1174" si="292">YEAR(A1174)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1174" s="4">
+        <f t="shared" ref="J1174" si="293">MONTH(A1174)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1175" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1175" s="3"/>
-      <c r="B1175" s="3"/>
-      <c r="C1175" s="3"/>
-      <c r="D1175" s="3"/>
-      <c r="E1175" s="3"/>
+      <c r="A1175" s="3" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1175" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1175" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1175" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1175" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1175" s="3"/>
-      <c r="G1175" s="3"/>
-      <c r="H1175" s="3"/>
-      <c r="I1175" s="4"/>
-      <c r="J1175" s="4"/>
+      <c r="G1175" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1175" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1175" s="4">
+        <f t="shared" ref="I1175" si="294">YEAR(A1175)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1175" s="4">
+        <f t="shared" ref="J1175" si="295">MONTH(A1175)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1176" s="3"/>
@@ -43252,6 +43444,126 @@
       <c r="I1181" s="4"/>
       <c r="J1181" s="4"/>
     </row>
+    <row r="1182" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1182" s="3"/>
+      <c r="B1182" s="3"/>
+      <c r="C1182" s="3"/>
+      <c r="D1182" s="3"/>
+      <c r="E1182" s="3"/>
+      <c r="F1182" s="3"/>
+      <c r="G1182" s="3"/>
+      <c r="H1182" s="3"/>
+      <c r="I1182" s="4"/>
+      <c r="J1182" s="4"/>
+    </row>
+    <row r="1183" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1183" s="3"/>
+      <c r="B1183" s="3"/>
+      <c r="C1183" s="3"/>
+      <c r="D1183" s="3"/>
+      <c r="E1183" s="3"/>
+      <c r="F1183" s="3"/>
+      <c r="G1183" s="3"/>
+      <c r="H1183" s="3"/>
+      <c r="I1183" s="4"/>
+      <c r="J1183" s="4"/>
+    </row>
+    <row r="1184" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1184" s="3"/>
+      <c r="B1184" s="3"/>
+      <c r="C1184" s="3"/>
+      <c r="D1184" s="3"/>
+      <c r="E1184" s="3"/>
+      <c r="F1184" s="3"/>
+      <c r="G1184" s="3"/>
+      <c r="H1184" s="3"/>
+      <c r="I1184" s="4"/>
+      <c r="J1184" s="4"/>
+    </row>
+    <row r="1185" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1185" s="3"/>
+      <c r="B1185" s="3"/>
+      <c r="C1185" s="3"/>
+      <c r="D1185" s="3"/>
+      <c r="E1185" s="3"/>
+      <c r="F1185" s="3"/>
+      <c r="G1185" s="3"/>
+      <c r="H1185" s="3"/>
+      <c r="I1185" s="4"/>
+      <c r="J1185" s="4"/>
+    </row>
+    <row r="1186" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1186" s="3"/>
+      <c r="B1186" s="3"/>
+      <c r="C1186" s="3"/>
+      <c r="D1186" s="3"/>
+      <c r="E1186" s="3"/>
+      <c r="F1186" s="3"/>
+      <c r="G1186" s="3"/>
+      <c r="H1186" s="3"/>
+      <c r="I1186" s="4"/>
+      <c r="J1186" s="4"/>
+    </row>
+    <row r="1187" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1187" s="3"/>
+      <c r="B1187" s="3"/>
+      <c r="C1187" s="3"/>
+      <c r="D1187" s="3"/>
+      <c r="E1187" s="3"/>
+      <c r="F1187" s="3"/>
+      <c r="G1187" s="3"/>
+      <c r="H1187" s="3"/>
+      <c r="I1187" s="4"/>
+      <c r="J1187" s="4"/>
+    </row>
+    <row r="1188" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1188" s="3"/>
+      <c r="B1188" s="3"/>
+      <c r="C1188" s="3"/>
+      <c r="D1188" s="3"/>
+      <c r="E1188" s="3"/>
+      <c r="F1188" s="3"/>
+      <c r="G1188" s="3"/>
+      <c r="H1188" s="3"/>
+      <c r="I1188" s="4"/>
+      <c r="J1188" s="4"/>
+    </row>
+    <row r="1189" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1189" s="3"/>
+      <c r="B1189" s="3"/>
+      <c r="C1189" s="3"/>
+      <c r="D1189" s="3"/>
+      <c r="E1189" s="3"/>
+      <c r="F1189" s="3"/>
+      <c r="G1189" s="3"/>
+      <c r="H1189" s="3"/>
+      <c r="I1189" s="4"/>
+      <c r="J1189" s="4"/>
+    </row>
+    <row r="1190" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1190" s="3"/>
+      <c r="B1190" s="3"/>
+      <c r="C1190" s="3"/>
+      <c r="D1190" s="3"/>
+      <c r="E1190" s="3"/>
+      <c r="F1190" s="3"/>
+      <c r="G1190" s="3"/>
+      <c r="H1190" s="3"/>
+      <c r="I1190" s="4"/>
+      <c r="J1190" s="4"/>
+    </row>
+    <row r="1191" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1191" s="3"/>
+      <c r="B1191" s="3"/>
+      <c r="C1191" s="3"/>
+      <c r="D1191" s="3"/>
+      <c r="E1191" s="3"/>
+      <c r="F1191" s="3"/>
+      <c r="G1191" s="3"/>
+      <c r="H1191" s="3"/>
+      <c r="I1191" s="4"/>
+      <c r="J1191" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#30 Time Tracking.xlsx: updated up to 2024-09-06.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9160" uniqueCount="1155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9262" uniqueCount="1165">
   <si>
     <t>Year</t>
   </si>
@@ -3487,6 +3487,36 @@
   </si>
   <si>
     <t>nwtraderaanalytics v4.1.0</t>
+  </si>
+  <si>
+    <t>2024-08-19</t>
+  </si>
+  <si>
+    <t>2024-08-23</t>
+  </si>
+  <si>
+    <t>nwragmate v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-08-24</t>
+  </si>
+  <si>
+    <t>2024-08-31</t>
+  </si>
+  <si>
+    <t>pycaretlab v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-09-02</t>
+  </si>
+  <si>
+    <t>2024-09-03</t>
+  </si>
+  <si>
+    <t>2024-09-05</t>
+  </si>
+  <si>
+    <t>2024-09-06</t>
   </si>
 </sst>
 </file>
@@ -3886,11 +3916,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1191"/>
+  <dimension ref="A1:J1202"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1178" sqref="F1178"/>
+      <pane ySplit="1" topLeftCell="A1172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1197" sqref="F1197"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -43373,160 +43403,442 @@
       </c>
     </row>
     <row r="1176" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1176" s="3"/>
-      <c r="B1176" s="3"/>
-      <c r="C1176" s="3"/>
-      <c r="D1176" s="3"/>
-      <c r="E1176" s="3"/>
+      <c r="A1176" s="3" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B1176" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1176" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="D1176" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1176" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1176" s="3"/>
-      <c r="G1176" s="3"/>
-      <c r="H1176" s="3"/>
-      <c r="I1176" s="4"/>
-      <c r="J1176" s="4"/>
+      <c r="G1176" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1176" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1176" s="4">
+        <f t="shared" ref="I1176:I1177" si="296">YEAR(A1176)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1176" s="4">
+        <f t="shared" ref="J1176:J1177" si="297">MONTH(A1176)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1177" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1177" s="3"/>
-      <c r="B1177" s="3"/>
-      <c r="C1177" s="3"/>
-      <c r="D1177" s="3"/>
-      <c r="E1177" s="3"/>
-      <c r="F1177" s="3"/>
-      <c r="G1177" s="3"/>
-      <c r="H1177" s="3"/>
-      <c r="I1177" s="4"/>
-      <c r="J1177" s="4"/>
+      <c r="A1177" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B1177" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1177" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1177" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1177" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1177" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1177" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1177" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1177" s="4">
+        <f t="shared" si="296"/>
+        <v>2024</v>
+      </c>
+      <c r="J1177" s="4">
+        <f t="shared" si="297"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1178" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1178" s="3"/>
-      <c r="B1178" s="3"/>
-      <c r="C1178" s="3"/>
-      <c r="D1178" s="3"/>
-      <c r="E1178" s="3"/>
-      <c r="F1178" s="3"/>
-      <c r="G1178" s="3"/>
-      <c r="H1178" s="3"/>
-      <c r="I1178" s="4"/>
-      <c r="J1178" s="4"/>
+      <c r="A1178" s="3" t="s">
+        <v>1156</v>
+      </c>
+      <c r="B1178" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1178" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1178" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1178" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1178" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1178" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1178" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1178" s="4">
+        <f t="shared" ref="I1178:I1179" si="298">YEAR(A1178)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1178" s="4">
+        <f t="shared" ref="J1178:J1179" si="299">MONTH(A1178)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1179" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1179" s="3"/>
-      <c r="B1179" s="3"/>
-      <c r="C1179" s="3"/>
-      <c r="D1179" s="3"/>
-      <c r="E1179" s="3"/>
+      <c r="A1179" s="3" t="s">
+        <v>1158</v>
+      </c>
+      <c r="B1179" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1179" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1179" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1179" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1179" s="3"/>
-      <c r="G1179" s="3"/>
-      <c r="H1179" s="3"/>
-      <c r="I1179" s="4"/>
-      <c r="J1179" s="4"/>
+      <c r="G1179" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1179" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1179" s="4">
+        <f t="shared" si="298"/>
+        <v>2024</v>
+      </c>
+      <c r="J1179" s="4">
+        <f t="shared" si="299"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1180" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1180" s="3"/>
-      <c r="B1180" s="3"/>
-      <c r="C1180" s="3"/>
-      <c r="D1180" s="3"/>
-      <c r="E1180" s="3"/>
-      <c r="F1180" s="3"/>
-      <c r="G1180" s="3"/>
-      <c r="H1180" s="3"/>
-      <c r="I1180" s="4"/>
-      <c r="J1180" s="4"/>
+      <c r="A1180" s="3" t="s">
+        <v>1159</v>
+      </c>
+      <c r="B1180" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1180" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1180" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1180" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1180" s="3" t="s">
+        <v>1160</v>
+      </c>
+      <c r="G1180" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1180" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1180" s="4">
+        <f t="shared" ref="I1180:I1182" si="300">YEAR(A1180)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1180" s="4">
+        <f t="shared" ref="J1180:J1182" si="301">MONTH(A1180)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1181" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1181" s="3"/>
-      <c r="B1181" s="3"/>
-      <c r="C1181" s="3"/>
-      <c r="D1181" s="3"/>
-      <c r="E1181" s="3"/>
-      <c r="F1181" s="3"/>
-      <c r="G1181" s="3"/>
-      <c r="H1181" s="3"/>
-      <c r="I1181" s="4"/>
-      <c r="J1181" s="4"/>
+      <c r="A1181" s="3" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B1181" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1181" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1181" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1181" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1181" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1181" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1181" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1181" s="4">
+        <f t="shared" si="300"/>
+        <v>2024</v>
+      </c>
+      <c r="J1181" s="4">
+        <f t="shared" si="301"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1182" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1182" s="3"/>
-      <c r="B1182" s="3"/>
-      <c r="C1182" s="3"/>
-      <c r="D1182" s="3"/>
-      <c r="E1182" s="3"/>
-      <c r="F1182" s="3"/>
-      <c r="G1182" s="3"/>
-      <c r="H1182" s="3"/>
-      <c r="I1182" s="4"/>
-      <c r="J1182" s="4"/>
+      <c r="A1182" s="3" t="s">
+        <v>1161</v>
+      </c>
+      <c r="B1182" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1182" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1182" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1182" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1182" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1182" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1182" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1182" s="4">
+        <f t="shared" si="300"/>
+        <v>2024</v>
+      </c>
+      <c r="J1182" s="4">
+        <f t="shared" si="301"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1183" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1183" s="3"/>
-      <c r="B1183" s="3"/>
-      <c r="C1183" s="3"/>
-      <c r="D1183" s="3"/>
-      <c r="E1183" s="3"/>
-      <c r="F1183" s="3"/>
-      <c r="G1183" s="3"/>
-      <c r="H1183" s="3"/>
-      <c r="I1183" s="4"/>
-      <c r="J1183" s="4"/>
+      <c r="A1183" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B1183" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1183" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1183" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1183" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1183" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1183" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1183" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1183" s="4">
+        <f t="shared" ref="I1183:I1186" si="302">YEAR(A1183)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1183" s="4">
+        <f t="shared" ref="J1183:J1186" si="303">MONTH(A1183)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1184" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1184" s="3"/>
-      <c r="B1184" s="3"/>
-      <c r="C1184" s="3"/>
-      <c r="D1184" s="3"/>
-      <c r="E1184" s="3"/>
-      <c r="F1184" s="3"/>
-      <c r="G1184" s="3"/>
-      <c r="H1184" s="3"/>
-      <c r="I1184" s="4"/>
-      <c r="J1184" s="4"/>
+      <c r="A1184" s="3" t="s">
+        <v>1162</v>
+      </c>
+      <c r="B1184" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1184" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1184" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1184" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1184" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1184" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1184" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1184" s="4">
+        <f t="shared" si="302"/>
+        <v>2024</v>
+      </c>
+      <c r="J1184" s="4">
+        <f t="shared" si="303"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1185" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1185" s="3"/>
-      <c r="B1185" s="3"/>
-      <c r="C1185" s="3"/>
-      <c r="D1185" s="3"/>
-      <c r="E1185" s="3"/>
-      <c r="F1185" s="3"/>
-      <c r="G1185" s="3"/>
-      <c r="H1185" s="3"/>
-      <c r="I1185" s="4"/>
-      <c r="J1185" s="4"/>
+      <c r="A1185" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B1185" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1185" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1185" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1185" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1185" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1185" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1185" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1185" s="4">
+        <f t="shared" si="302"/>
+        <v>2024</v>
+      </c>
+      <c r="J1185" s="4">
+        <f t="shared" si="303"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1186" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1186" s="3"/>
-      <c r="B1186" s="3"/>
-      <c r="C1186" s="3"/>
-      <c r="D1186" s="3"/>
-      <c r="E1186" s="3"/>
-      <c r="F1186" s="3"/>
-      <c r="G1186" s="3"/>
-      <c r="H1186" s="3"/>
-      <c r="I1186" s="4"/>
-      <c r="J1186" s="4"/>
+      <c r="A1186" s="3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B1186" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1186" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1186" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1186" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1186" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1186" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1186" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1186" s="4">
+        <f t="shared" si="302"/>
+        <v>2024</v>
+      </c>
+      <c r="J1186" s="4">
+        <f t="shared" si="303"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1187" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1187" s="3"/>
-      <c r="B1187" s="3"/>
-      <c r="C1187" s="3"/>
-      <c r="D1187" s="3"/>
-      <c r="E1187" s="3"/>
-      <c r="F1187" s="3"/>
-      <c r="G1187" s="3"/>
-      <c r="H1187" s="3"/>
-      <c r="I1187" s="4"/>
-      <c r="J1187" s="4"/>
+      <c r="A1187" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B1187" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1187" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1187" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1187" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1187" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1187" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1187" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1187" s="4">
+        <f t="shared" ref="I1187:I1188" si="304">YEAR(A1187)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1187" s="4">
+        <f t="shared" ref="J1187:J1188" si="305">MONTH(A1187)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1188" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1188" s="3"/>
-      <c r="B1188" s="3"/>
-      <c r="C1188" s="3"/>
-      <c r="D1188" s="3"/>
-      <c r="E1188" s="3"/>
-      <c r="F1188" s="3"/>
-      <c r="G1188" s="3"/>
-      <c r="H1188" s="3"/>
-      <c r="I1188" s="4"/>
-      <c r="J1188" s="4"/>
+      <c r="A1188" s="3" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B1188" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1188" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1188" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1188" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1188" s="3" t="s">
+        <v>1157</v>
+      </c>
+      <c r="G1188" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1188" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1188" s="4">
+        <f t="shared" si="304"/>
+        <v>2024</v>
+      </c>
+      <c r="J1188" s="4">
+        <f t="shared" si="305"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1189" s="3"/>
@@ -43564,6 +43876,138 @@
       <c r="I1191" s="4"/>
       <c r="J1191" s="4"/>
     </row>
+    <row r="1192" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1192" s="3"/>
+      <c r="B1192" s="3"/>
+      <c r="C1192" s="3"/>
+      <c r="D1192" s="3"/>
+      <c r="E1192" s="3"/>
+      <c r="F1192" s="3"/>
+      <c r="G1192" s="3"/>
+      <c r="H1192" s="3"/>
+      <c r="I1192" s="4"/>
+      <c r="J1192" s="4"/>
+    </row>
+    <row r="1193" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1193" s="3"/>
+      <c r="B1193" s="3"/>
+      <c r="C1193" s="3"/>
+      <c r="D1193" s="3"/>
+      <c r="E1193" s="3"/>
+      <c r="F1193" s="3"/>
+      <c r="G1193" s="3"/>
+      <c r="H1193" s="3"/>
+      <c r="I1193" s="4"/>
+      <c r="J1193" s="4"/>
+    </row>
+    <row r="1194" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1194" s="3"/>
+      <c r="B1194" s="3"/>
+      <c r="C1194" s="3"/>
+      <c r="D1194" s="3"/>
+      <c r="E1194" s="3"/>
+      <c r="F1194" s="3"/>
+      <c r="G1194" s="3"/>
+      <c r="H1194" s="3"/>
+      <c r="I1194" s="4"/>
+      <c r="J1194" s="4"/>
+    </row>
+    <row r="1195" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1195" s="3"/>
+      <c r="B1195" s="3"/>
+      <c r="C1195" s="3"/>
+      <c r="D1195" s="3"/>
+      <c r="E1195" s="3"/>
+      <c r="F1195" s="3"/>
+      <c r="G1195" s="3"/>
+      <c r="H1195" s="3"/>
+      <c r="I1195" s="4"/>
+      <c r="J1195" s="4"/>
+    </row>
+    <row r="1196" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1196" s="3"/>
+      <c r="B1196" s="3"/>
+      <c r="C1196" s="3"/>
+      <c r="D1196" s="3"/>
+      <c r="E1196" s="3"/>
+      <c r="F1196" s="3"/>
+      <c r="G1196" s="3"/>
+      <c r="H1196" s="3"/>
+      <c r="I1196" s="4"/>
+      <c r="J1196" s="4"/>
+    </row>
+    <row r="1197" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1197" s="3"/>
+      <c r="B1197" s="3"/>
+      <c r="C1197" s="3"/>
+      <c r="D1197" s="3"/>
+      <c r="E1197" s="3"/>
+      <c r="F1197" s="3"/>
+      <c r="G1197" s="3"/>
+      <c r="H1197" s="3"/>
+      <c r="I1197" s="4"/>
+      <c r="J1197" s="4"/>
+    </row>
+    <row r="1198" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1198" s="3"/>
+      <c r="B1198" s="3"/>
+      <c r="C1198" s="3"/>
+      <c r="D1198" s="3"/>
+      <c r="E1198" s="3"/>
+      <c r="F1198" s="3"/>
+      <c r="G1198" s="3"/>
+      <c r="H1198" s="3"/>
+      <c r="I1198" s="4"/>
+      <c r="J1198" s="4"/>
+    </row>
+    <row r="1199" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1199" s="3"/>
+      <c r="B1199" s="3"/>
+      <c r="C1199" s="3"/>
+      <c r="D1199" s="3"/>
+      <c r="E1199" s="3"/>
+      <c r="F1199" s="3"/>
+      <c r="G1199" s="3"/>
+      <c r="H1199" s="3"/>
+      <c r="I1199" s="4"/>
+      <c r="J1199" s="4"/>
+    </row>
+    <row r="1200" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1200" s="3"/>
+      <c r="B1200" s="3"/>
+      <c r="C1200" s="3"/>
+      <c r="D1200" s="3"/>
+      <c r="E1200" s="3"/>
+      <c r="F1200" s="3"/>
+      <c r="G1200" s="3"/>
+      <c r="H1200" s="3"/>
+      <c r="I1200" s="4"/>
+      <c r="J1200" s="4"/>
+    </row>
+    <row r="1201" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1201" s="3"/>
+      <c r="B1201" s="3"/>
+      <c r="C1201" s="3"/>
+      <c r="D1201" s="3"/>
+      <c r="E1201" s="3"/>
+      <c r="F1201" s="3"/>
+      <c r="G1201" s="3"/>
+      <c r="H1201" s="3"/>
+      <c r="I1201" s="4"/>
+      <c r="J1201" s="4"/>
+    </row>
+    <row r="1202" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1202" s="3"/>
+      <c r="B1202" s="3"/>
+      <c r="C1202" s="3"/>
+      <c r="D1202" s="3"/>
+      <c r="E1202" s="3"/>
+      <c r="F1202" s="3"/>
+      <c r="G1202" s="3"/>
+      <c r="H1202" s="3"/>
+      <c r="I1202" s="4"/>
+      <c r="J1202" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#32 Time Tracking.xlxs: updated until 2024-09-20.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9262" uniqueCount="1165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9302" uniqueCount="1170">
   <si>
     <t>Year</t>
   </si>
@@ -3517,6 +3517,21 @@
   </si>
   <si>
     <t>2024-09-06</t>
+  </si>
+  <si>
+    <t>nwshared v1.3.0</t>
+  </si>
+  <si>
+    <t>2024-09-17</t>
+  </si>
+  <si>
+    <t>2024-09-19</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.5.0</t>
+  </si>
+  <si>
+    <t>2024-09-20</t>
   </si>
 </sst>
 </file>
@@ -3920,7 +3935,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1197" sqref="F1197"/>
+      <selection pane="bottomLeft" activeCell="D1198" sqref="D1198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -43841,64 +43856,174 @@
       </c>
     </row>
     <row r="1189" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1189" s="3"/>
-      <c r="B1189" s="3"/>
-      <c r="C1189" s="3"/>
-      <c r="D1189" s="3"/>
-      <c r="E1189" s="3"/>
-      <c r="F1189" s="3"/>
-      <c r="G1189" s="3"/>
-      <c r="H1189" s="3"/>
-      <c r="I1189" s="4"/>
-      <c r="J1189" s="4"/>
+      <c r="A1189" s="3" t="s">
+        <v>1166</v>
+      </c>
+      <c r="B1189" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1189" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1189" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1189" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1189" s="3" t="s">
+        <v>1165</v>
+      </c>
+      <c r="G1189" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1189" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1189" s="4">
+        <f t="shared" ref="I1189:I1191" si="306">YEAR(A1189)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1189" s="4">
+        <f t="shared" ref="J1189:J1191" si="307">MONTH(A1189)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1190" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1190" s="3"/>
-      <c r="B1190" s="3"/>
-      <c r="C1190" s="3"/>
-      <c r="D1190" s="3"/>
-      <c r="E1190" s="3"/>
-      <c r="F1190" s="3"/>
-      <c r="G1190" s="3"/>
-      <c r="H1190" s="3"/>
-      <c r="I1190" s="4"/>
-      <c r="J1190" s="4"/>
+      <c r="A1190" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B1190" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1190" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1190" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1190" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1190" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G1190" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1190" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1190" s="4">
+        <f t="shared" si="306"/>
+        <v>2024</v>
+      </c>
+      <c r="J1190" s="4">
+        <f t="shared" si="307"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1191" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1191" s="3"/>
-      <c r="B1191" s="3"/>
-      <c r="C1191" s="3"/>
-      <c r="D1191" s="3"/>
-      <c r="E1191" s="3"/>
-      <c r="F1191" s="3"/>
-      <c r="G1191" s="3"/>
-      <c r="H1191" s="3"/>
-      <c r="I1191" s="4"/>
-      <c r="J1191" s="4"/>
+      <c r="A1191" s="3" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B1191" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1191" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1191" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1191" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1191" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G1191" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1191" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1191" s="4">
+        <f t="shared" si="306"/>
+        <v>2024</v>
+      </c>
+      <c r="J1191" s="4">
+        <f t="shared" si="307"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1192" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1192" s="3"/>
-      <c r="B1192" s="3"/>
-      <c r="C1192" s="3"/>
-      <c r="D1192" s="3"/>
-      <c r="E1192" s="3"/>
-      <c r="F1192" s="3"/>
-      <c r="G1192" s="3"/>
-      <c r="H1192" s="3"/>
-      <c r="I1192" s="4"/>
-      <c r="J1192" s="4"/>
+      <c r="A1192" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B1192" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1192" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1192" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1192" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1192" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G1192" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1192" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1192" s="4">
+        <f t="shared" ref="I1192:I1193" si="308">YEAR(A1192)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1192" s="4">
+        <f t="shared" ref="J1192:J1193" si="309">MONTH(A1192)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1193" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1193" s="3"/>
-      <c r="B1193" s="3"/>
-      <c r="C1193" s="3"/>
-      <c r="D1193" s="3"/>
-      <c r="E1193" s="3"/>
-      <c r="F1193" s="3"/>
-      <c r="G1193" s="3"/>
-      <c r="H1193" s="3"/>
-      <c r="I1193" s="4"/>
-      <c r="J1193" s="4"/>
+      <c r="A1193" s="3" t="s">
+        <v>1169</v>
+      </c>
+      <c r="B1193" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1193" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1193" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1193" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1193" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G1193" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1193" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1193" s="4">
+        <f t="shared" si="308"/>
+        <v>2024</v>
+      </c>
+      <c r="J1193" s="4">
+        <f t="shared" si="309"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1194" s="3"/>

</xml_diff>

<commit_message>
#30 Time Tracking.xlsx: updated up to 2024-09-30.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9302" uniqueCount="1170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9382" uniqueCount="1183">
   <si>
     <t>Year</t>
   </si>
@@ -3532,6 +3532,45 @@
   </si>
   <si>
     <t>2024-09-20</t>
+  </si>
+  <si>
+    <t>2024-09-21</t>
+  </si>
+  <si>
+    <t>2024-09-22</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.5.0</t>
+  </si>
+  <si>
+    <t>2024-09-23</t>
+  </si>
+  <si>
+    <t>2024-09-24</t>
+  </si>
+  <si>
+    <t>nwshared v1.4.0</t>
+  </si>
+  <si>
+    <t>2024-09-25</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.6.0</t>
+  </si>
+  <si>
+    <t>2024-09-26</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.7.0</t>
+  </si>
+  <si>
+    <t>2024-09-27</t>
+  </si>
+  <si>
+    <t>2024-09-29</t>
+  </si>
+  <si>
+    <t>2024-09-30</t>
   </si>
 </sst>
 </file>
@@ -3931,11 +3970,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1202"/>
+  <dimension ref="A1:J1217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1172" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1198" sqref="D1198"/>
+      <pane ySplit="1" topLeftCell="A1181" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B1205" sqref="B1205"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44026,112 +44065,512 @@
       </c>
     </row>
     <row r="1194" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1194" s="3"/>
-      <c r="B1194" s="3"/>
-      <c r="C1194" s="3"/>
-      <c r="D1194" s="3"/>
-      <c r="E1194" s="3"/>
-      <c r="F1194" s="3"/>
-      <c r="G1194" s="3"/>
-      <c r="H1194" s="3"/>
-      <c r="I1194" s="4"/>
-      <c r="J1194" s="4"/>
+      <c r="A1194" s="3" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B1194" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1194" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1194" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1194" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1194" s="3" t="s">
+        <v>1168</v>
+      </c>
+      <c r="G1194" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1194" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1194" s="4">
+        <f t="shared" ref="I1194:I1195" si="310">YEAR(A1194)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1194" s="4">
+        <f t="shared" ref="J1194:J1195" si="311">MONTH(A1194)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1195" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1195" s="3"/>
-      <c r="B1195" s="3"/>
-      <c r="C1195" s="3"/>
-      <c r="D1195" s="3"/>
-      <c r="E1195" s="3"/>
-      <c r="F1195" s="3"/>
-      <c r="G1195" s="3"/>
-      <c r="H1195" s="3"/>
-      <c r="I1195" s="4"/>
-      <c r="J1195" s="4"/>
+      <c r="A1195" s="3" t="s">
+        <v>1171</v>
+      </c>
+      <c r="B1195" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1195" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1195" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1195" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1195" s="3" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G1195" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1195" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1195" s="4">
+        <f t="shared" si="310"/>
+        <v>2024</v>
+      </c>
+      <c r="J1195" s="4">
+        <f t="shared" si="311"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1196" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1196" s="3"/>
-      <c r="B1196" s="3"/>
-      <c r="C1196" s="3"/>
-      <c r="D1196" s="3"/>
-      <c r="E1196" s="3"/>
-      <c r="F1196" s="3"/>
-      <c r="G1196" s="3"/>
-      <c r="H1196" s="3"/>
-      <c r="I1196" s="4"/>
-      <c r="J1196" s="4"/>
+      <c r="A1196" s="3" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B1196" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1196" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1196" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1196" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1196" s="3" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G1196" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1196" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1196" s="4">
+        <f t="shared" ref="I1196:I1197" si="312">YEAR(A1196)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1196" s="4">
+        <f t="shared" ref="J1196:J1197" si="313">MONTH(A1196)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1197" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1197" s="3"/>
-      <c r="B1197" s="3"/>
-      <c r="C1197" s="3"/>
-      <c r="D1197" s="3"/>
-      <c r="E1197" s="3"/>
-      <c r="F1197" s="3"/>
-      <c r="G1197" s="3"/>
-      <c r="H1197" s="3"/>
-      <c r="I1197" s="4"/>
-      <c r="J1197" s="4"/>
+      <c r="A1197" s="3" t="s">
+        <v>1173</v>
+      </c>
+      <c r="B1197" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1197" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1197" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1197" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1197" s="3" t="s">
+        <v>1172</v>
+      </c>
+      <c r="G1197" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1197" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1197" s="4">
+        <f t="shared" si="312"/>
+        <v>2024</v>
+      </c>
+      <c r="J1197" s="4">
+        <f t="shared" si="313"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1198" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1198" s="3"/>
-      <c r="B1198" s="3"/>
-      <c r="C1198" s="3"/>
-      <c r="D1198" s="3"/>
-      <c r="E1198" s="3"/>
-      <c r="F1198" s="3"/>
-      <c r="G1198" s="3"/>
-      <c r="H1198" s="3"/>
-      <c r="I1198" s="4"/>
-      <c r="J1198" s="4"/>
+      <c r="A1198" s="3" t="s">
+        <v>1174</v>
+      </c>
+      <c r="B1198" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1198" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1198" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1198" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1198" s="3" t="s">
+        <v>1175</v>
+      </c>
+      <c r="G1198" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1198" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1198" s="4">
+        <f t="shared" ref="I1198" si="314">YEAR(A1198)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1198" s="4">
+        <f t="shared" ref="J1198" si="315">MONTH(A1198)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1199" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1199" s="3"/>
-      <c r="B1199" s="3"/>
-      <c r="C1199" s="3"/>
-      <c r="D1199" s="3"/>
-      <c r="E1199" s="3"/>
-      <c r="F1199" s="3"/>
-      <c r="G1199" s="3"/>
-      <c r="H1199" s="3"/>
-      <c r="I1199" s="4"/>
-      <c r="J1199" s="4"/>
+      <c r="A1199" s="3" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B1199" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1199" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1199" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1199" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1199" s="3" t="s">
+        <v>1177</v>
+      </c>
+      <c r="G1199" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1199" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1199" s="4">
+        <f t="shared" ref="I1199:I1200" si="316">YEAR(A1199)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1199" s="4">
+        <f t="shared" ref="J1199:J1200" si="317">MONTH(A1199)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1200" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1200" s="3"/>
-      <c r="B1200" s="3"/>
-      <c r="C1200" s="3"/>
-      <c r="D1200" s="3"/>
-      <c r="E1200" s="3"/>
-      <c r="F1200" s="3"/>
-      <c r="G1200" s="3"/>
-      <c r="H1200" s="3"/>
-      <c r="I1200" s="4"/>
-      <c r="J1200" s="4"/>
+      <c r="A1200" s="3" t="s">
+        <v>1178</v>
+      </c>
+      <c r="B1200" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1200" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1200" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1200" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1200" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1200" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1200" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1200" s="4">
+        <f t="shared" si="316"/>
+        <v>2024</v>
+      </c>
+      <c r="J1200" s="4">
+        <f t="shared" si="317"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1201" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1201" s="3"/>
-      <c r="B1201" s="3"/>
-      <c r="C1201" s="3"/>
-      <c r="D1201" s="3"/>
-      <c r="E1201" s="3"/>
-      <c r="F1201" s="3"/>
-      <c r="G1201" s="3"/>
-      <c r="H1201" s="3"/>
-      <c r="I1201" s="4"/>
-      <c r="J1201" s="4"/>
+      <c r="A1201" s="3" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B1201" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1201" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1201" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1201" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1201" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1201" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1201" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1201" s="4">
+        <f t="shared" ref="I1201" si="318">YEAR(A1201)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1201" s="4">
+        <f t="shared" ref="J1201" si="319">MONTH(A1201)</f>
+        <v>9</v>
+      </c>
     </row>
     <row r="1202" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1202" s="3"/>
-      <c r="B1202" s="3"/>
-      <c r="C1202" s="3"/>
-      <c r="D1202" s="3"/>
-      <c r="E1202" s="3"/>
-      <c r="F1202" s="3"/>
-      <c r="G1202" s="3"/>
-      <c r="H1202" s="3"/>
-      <c r="I1202" s="4"/>
-      <c r="J1202" s="4"/>
+      <c r="A1202" s="3" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B1202" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1202" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1202" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1202" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1202" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1202" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1202" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1202" s="4">
+        <f t="shared" ref="I1202" si="320">YEAR(A1202)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1202" s="4">
+        <f t="shared" ref="J1202" si="321">MONTH(A1202)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1203" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B1203" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1203" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1203" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1203" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1203" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1203" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1203" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1203" s="4">
+        <f t="shared" ref="I1203" si="322">YEAR(A1203)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1203" s="4">
+        <f t="shared" ref="J1203" si="323">MONTH(A1203)</f>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1204" s="3"/>
+      <c r="B1204" s="3"/>
+      <c r="C1204" s="3"/>
+      <c r="D1204" s="3"/>
+      <c r="E1204" s="3"/>
+      <c r="F1204" s="3"/>
+      <c r="G1204" s="3"/>
+      <c r="H1204" s="3"/>
+      <c r="I1204" s="4"/>
+      <c r="J1204" s="4"/>
+    </row>
+    <row r="1205" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1205" s="3"/>
+      <c r="B1205" s="3"/>
+      <c r="C1205" s="3"/>
+      <c r="D1205" s="3"/>
+      <c r="E1205" s="3"/>
+      <c r="F1205" s="3"/>
+      <c r="G1205" s="3"/>
+      <c r="H1205" s="3"/>
+      <c r="I1205" s="4"/>
+      <c r="J1205" s="4"/>
+    </row>
+    <row r="1206" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1206" s="3"/>
+      <c r="B1206" s="3"/>
+      <c r="C1206" s="3"/>
+      <c r="D1206" s="3"/>
+      <c r="E1206" s="3"/>
+      <c r="F1206" s="3"/>
+      <c r="G1206" s="3"/>
+      <c r="H1206" s="3"/>
+      <c r="I1206" s="4"/>
+      <c r="J1206" s="4"/>
+    </row>
+    <row r="1207" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1207" s="3"/>
+      <c r="B1207" s="3"/>
+      <c r="C1207" s="3"/>
+      <c r="D1207" s="3"/>
+      <c r="E1207" s="3"/>
+      <c r="F1207" s="3"/>
+      <c r="G1207" s="3"/>
+      <c r="H1207" s="3"/>
+      <c r="I1207" s="4"/>
+      <c r="J1207" s="4"/>
+    </row>
+    <row r="1208" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1208" s="3"/>
+      <c r="B1208" s="3"/>
+      <c r="C1208" s="3"/>
+      <c r="D1208" s="3"/>
+      <c r="E1208" s="3"/>
+      <c r="F1208" s="3"/>
+      <c r="G1208" s="3"/>
+      <c r="H1208" s="3"/>
+      <c r="I1208" s="4"/>
+      <c r="J1208" s="4"/>
+    </row>
+    <row r="1209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1209" s="3"/>
+      <c r="B1209" s="3"/>
+      <c r="C1209" s="3"/>
+      <c r="D1209" s="3"/>
+      <c r="E1209" s="3"/>
+      <c r="F1209" s="3"/>
+      <c r="G1209" s="3"/>
+      <c r="H1209" s="3"/>
+      <c r="I1209" s="4"/>
+      <c r="J1209" s="4"/>
+    </row>
+    <row r="1210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1210" s="3"/>
+      <c r="B1210" s="3"/>
+      <c r="C1210" s="3"/>
+      <c r="D1210" s="3"/>
+      <c r="E1210" s="3"/>
+      <c r="F1210" s="3"/>
+      <c r="G1210" s="3"/>
+      <c r="H1210" s="3"/>
+      <c r="I1210" s="4"/>
+      <c r="J1210" s="4"/>
+    </row>
+    <row r="1211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1211" s="3"/>
+      <c r="B1211" s="3"/>
+      <c r="C1211" s="3"/>
+      <c r="D1211" s="3"/>
+      <c r="E1211" s="3"/>
+      <c r="F1211" s="3"/>
+      <c r="G1211" s="3"/>
+      <c r="H1211" s="3"/>
+      <c r="I1211" s="4"/>
+      <c r="J1211" s="4"/>
+    </row>
+    <row r="1212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1212" s="3"/>
+      <c r="B1212" s="3"/>
+      <c r="C1212" s="3"/>
+      <c r="D1212" s="3"/>
+      <c r="E1212" s="3"/>
+      <c r="F1212" s="3"/>
+      <c r="G1212" s="3"/>
+      <c r="H1212" s="3"/>
+      <c r="I1212" s="4"/>
+      <c r="J1212" s="4"/>
+    </row>
+    <row r="1213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1213" s="3"/>
+      <c r="B1213" s="3"/>
+      <c r="C1213" s="3"/>
+      <c r="D1213" s="3"/>
+      <c r="E1213" s="3"/>
+      <c r="F1213" s="3"/>
+      <c r="G1213" s="3"/>
+      <c r="H1213" s="3"/>
+      <c r="I1213" s="4"/>
+      <c r="J1213" s="4"/>
+    </row>
+    <row r="1214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1214" s="3"/>
+      <c r="B1214" s="3"/>
+      <c r="C1214" s="3"/>
+      <c r="D1214" s="3"/>
+      <c r="E1214" s="3"/>
+      <c r="F1214" s="3"/>
+      <c r="G1214" s="3"/>
+      <c r="H1214" s="3"/>
+      <c r="I1214" s="4"/>
+      <c r="J1214" s="4"/>
+    </row>
+    <row r="1215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1215" s="3"/>
+      <c r="B1215" s="3"/>
+      <c r="C1215" s="3"/>
+      <c r="D1215" s="3"/>
+      <c r="E1215" s="3"/>
+      <c r="F1215" s="3"/>
+      <c r="G1215" s="3"/>
+      <c r="H1215" s="3"/>
+      <c r="I1215" s="4"/>
+      <c r="J1215" s="4"/>
+    </row>
+    <row r="1216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1216" s="3"/>
+      <c r="B1216" s="3"/>
+      <c r="C1216" s="3"/>
+      <c r="D1216" s="3"/>
+      <c r="E1216" s="3"/>
+      <c r="F1216" s="3"/>
+      <c r="G1216" s="3"/>
+      <c r="H1216" s="3"/>
+      <c r="I1216" s="4"/>
+      <c r="J1216" s="4"/>
+    </row>
+    <row r="1217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1217" s="3"/>
+      <c r="B1217" s="3"/>
+      <c r="C1217" s="3"/>
+      <c r="D1217" s="3"/>
+      <c r="E1217" s="3"/>
+      <c r="F1217" s="3"/>
+      <c r="G1217" s="3"/>
+      <c r="H1217" s="3"/>
+      <c r="I1217" s="4"/>
+      <c r="J1217" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#32 Time Tracking.xlxs: updated until 2024-09-30.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9382" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9389" uniqueCount="1183">
   <si>
     <t>Year</t>
   </si>
@@ -3973,8 +3973,8 @@
   <dimension ref="A1:J1217"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1181" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B1205" sqref="B1205"/>
+      <pane ySplit="1" topLeftCell="A1175" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1209" sqref="F1209"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44396,25 +44396,45 @@
         <v>279</v>
       </c>
       <c r="I1203" s="4">
-        <f t="shared" ref="I1203" si="322">YEAR(A1203)</f>
+        <f t="shared" ref="I1203:I1204" si="322">YEAR(A1203)</f>
         <v>2024</v>
       </c>
       <c r="J1203" s="4">
-        <f t="shared" ref="J1203" si="323">MONTH(A1203)</f>
+        <f t="shared" ref="J1203:J1204" si="323">MONTH(A1203)</f>
         <v>9</v>
       </c>
     </row>
     <row r="1204" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1204" s="3"/>
-      <c r="B1204" s="3"/>
-      <c r="C1204" s="3"/>
-      <c r="D1204" s="3"/>
-      <c r="E1204" s="3"/>
+      <c r="A1204" s="3" t="s">
+        <v>1182</v>
+      </c>
+      <c r="B1204" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1204" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1204" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1204" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1204" s="3"/>
-      <c r="G1204" s="3"/>
-      <c r="H1204" s="3"/>
-      <c r="I1204" s="4"/>
-      <c r="J1204" s="4"/>
+      <c r="G1204" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1204" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1204" s="4">
+        <f t="shared" si="322"/>
+        <v>2024</v>
+      </c>
+      <c r="J1204" s="4">
+        <f t="shared" si="323"/>
+        <v>9</v>
+      </c>
     </row>
     <row r="1205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1205" s="3"/>

</xml_diff>

<commit_message>
#34 Time Tracking.xlsx: updated up to 2024-10-13.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9389" uniqueCount="1183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9493" uniqueCount="1192">
   <si>
     <t>Year</t>
   </si>
@@ -3571,6 +3571,33 @@
   </si>
   <si>
     <t>2024-09-30</t>
+  </si>
+  <si>
+    <t>2024-10-01</t>
+  </si>
+  <si>
+    <t>nwtraderanalytics v4.2.0</t>
+  </si>
+  <si>
+    <t>2024-10-04</t>
+  </si>
+  <si>
+    <t>2024-10-06</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.0.0</t>
+  </si>
+  <si>
+    <t>2024-10-07</t>
+  </si>
+  <si>
+    <t>2024-10-08</t>
+  </si>
+  <si>
+    <t>2024-10-10</t>
+  </si>
+  <si>
+    <t>2024-10-11</t>
   </si>
 </sst>
 </file>
@@ -3970,11 +3997,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1217"/>
+  <dimension ref="A1:J1229"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1175" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1209" sqref="F1209"/>
+      <pane ySplit="1" topLeftCell="A1196" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1219" sqref="D1219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44437,160 +44464,590 @@
       </c>
     </row>
     <row r="1205" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1205" s="3"/>
-      <c r="B1205" s="3"/>
-      <c r="C1205" s="3"/>
-      <c r="D1205" s="3"/>
-      <c r="E1205" s="3"/>
-      <c r="F1205" s="3"/>
-      <c r="G1205" s="3"/>
-      <c r="H1205" s="3"/>
-      <c r="I1205" s="4"/>
-      <c r="J1205" s="4"/>
+      <c r="A1205" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B1205" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1205" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1205" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1205" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1205" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1205" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1205" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1205" s="4">
+        <f t="shared" ref="I1205:I1208" si="324">YEAR(A1205)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1205" s="4">
+        <f t="shared" ref="J1205:J1208" si="325">MONTH(A1205)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1206" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1206" s="3"/>
-      <c r="B1206" s="3"/>
-      <c r="C1206" s="3"/>
-      <c r="D1206" s="3"/>
-      <c r="E1206" s="3"/>
-      <c r="F1206" s="3"/>
-      <c r="G1206" s="3"/>
-      <c r="H1206" s="3"/>
-      <c r="I1206" s="4"/>
-      <c r="J1206" s="4"/>
+      <c r="A1206" s="3" t="s">
+        <v>1183</v>
+      </c>
+      <c r="B1206" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1206" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1206" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1206" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1206" s="3" t="s">
+        <v>1179</v>
+      </c>
+      <c r="G1206" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1206" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1206" s="4">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="J1206" s="4">
+        <f t="shared" si="325"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1207" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1207" s="3"/>
-      <c r="B1207" s="3"/>
-      <c r="C1207" s="3"/>
-      <c r="D1207" s="3"/>
-      <c r="E1207" s="3"/>
-      <c r="F1207" s="3"/>
-      <c r="G1207" s="3"/>
-      <c r="H1207" s="3"/>
-      <c r="I1207" s="4"/>
-      <c r="J1207" s="4"/>
+      <c r="A1207" s="3" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B1207" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1207" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1207" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1207" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1207" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G1207" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1207" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1207" s="4">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="J1207" s="4">
+        <f t="shared" si="325"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1208" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1208" s="3"/>
-      <c r="B1208" s="3"/>
-      <c r="C1208" s="3"/>
-      <c r="D1208" s="3"/>
-      <c r="E1208" s="3"/>
-      <c r="F1208" s="3"/>
-      <c r="G1208" s="3"/>
-      <c r="H1208" s="3"/>
-      <c r="I1208" s="4"/>
-      <c r="J1208" s="4"/>
+      <c r="A1208" s="3" t="s">
+        <v>1185</v>
+      </c>
+      <c r="B1208" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1208" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1208" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1208" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1208" s="3" t="s">
+        <v>1184</v>
+      </c>
+      <c r="G1208" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1208" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1208" s="4">
+        <f t="shared" si="324"/>
+        <v>2024</v>
+      </c>
+      <c r="J1208" s="4">
+        <f t="shared" si="325"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1209" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1209" s="3"/>
-      <c r="B1209" s="3"/>
-      <c r="C1209" s="3"/>
-      <c r="D1209" s="3"/>
-      <c r="E1209" s="3"/>
-      <c r="F1209" s="3"/>
-      <c r="G1209" s="3"/>
-      <c r="H1209" s="3"/>
-      <c r="I1209" s="4"/>
-      <c r="J1209" s="4"/>
+      <c r="A1209" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B1209" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1209" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1209" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1209" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1209" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1209" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1209" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1209" s="4">
+        <f t="shared" ref="I1209:I1210" si="326">YEAR(A1209)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1209" s="4">
+        <f t="shared" ref="J1209:J1210" si="327">MONTH(A1209)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1210" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1210" s="3"/>
-      <c r="B1210" s="3"/>
-      <c r="C1210" s="3"/>
-      <c r="D1210" s="3"/>
-      <c r="E1210" s="3"/>
-      <c r="F1210" s="3"/>
-      <c r="G1210" s="3"/>
-      <c r="H1210" s="3"/>
-      <c r="I1210" s="4"/>
-      <c r="J1210" s="4"/>
+      <c r="A1210" s="3" t="s">
+        <v>1186</v>
+      </c>
+      <c r="B1210" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1210" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1210" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1210" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1210" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1210" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1210" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1210" s="4">
+        <f t="shared" si="326"/>
+        <v>2024</v>
+      </c>
+      <c r="J1210" s="4">
+        <f t="shared" si="327"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1211" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1211" s="3"/>
-      <c r="B1211" s="3"/>
-      <c r="C1211" s="3"/>
-      <c r="D1211" s="3"/>
-      <c r="E1211" s="3"/>
-      <c r="F1211" s="3"/>
-      <c r="G1211" s="3"/>
-      <c r="H1211" s="3"/>
-      <c r="I1211" s="4"/>
-      <c r="J1211" s="4"/>
+      <c r="A1211" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B1211" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1211" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1211" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1211" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1211" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1211" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1211" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1211" s="4">
+        <f t="shared" ref="I1211:I1212" si="328">YEAR(A1211)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1211" s="4">
+        <f t="shared" ref="J1211:J1212" si="329">MONTH(A1211)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1212" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1212" s="3"/>
-      <c r="B1212" s="3"/>
-      <c r="C1212" s="3"/>
-      <c r="D1212" s="3"/>
-      <c r="E1212" s="3"/>
-      <c r="F1212" s="3"/>
-      <c r="G1212" s="3"/>
-      <c r="H1212" s="3"/>
-      <c r="I1212" s="4"/>
-      <c r="J1212" s="4"/>
+      <c r="A1212" s="3" t="s">
+        <v>1188</v>
+      </c>
+      <c r="B1212" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1212" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1212" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1212" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1212" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1212" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1212" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1212" s="4">
+        <f t="shared" si="328"/>
+        <v>2024</v>
+      </c>
+      <c r="J1212" s="4">
+        <f t="shared" si="329"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1213" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1213" s="3"/>
-      <c r="B1213" s="3"/>
-      <c r="C1213" s="3"/>
-      <c r="D1213" s="3"/>
-      <c r="E1213" s="3"/>
-      <c r="F1213" s="3"/>
-      <c r="G1213" s="3"/>
-      <c r="H1213" s="3"/>
-      <c r="I1213" s="4"/>
-      <c r="J1213" s="4"/>
+      <c r="A1213" s="3" t="s">
+        <v>1189</v>
+      </c>
+      <c r="B1213" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1213" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1213" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1213" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1213" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1213" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1213" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1213" s="4">
+        <f t="shared" ref="I1213:I1214" si="330">YEAR(A1213)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1213" s="4">
+        <f t="shared" ref="J1213:J1214" si="331">MONTH(A1213)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1214" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1214" s="3"/>
-      <c r="B1214" s="3"/>
-      <c r="C1214" s="3"/>
-      <c r="D1214" s="3"/>
-      <c r="E1214" s="3"/>
-      <c r="F1214" s="3"/>
-      <c r="G1214" s="3"/>
-      <c r="H1214" s="3"/>
-      <c r="I1214" s="4"/>
-      <c r="J1214" s="4"/>
+      <c r="A1214" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B1214" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1214" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1214" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1214" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1214" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1214" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1214" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1214" s="4">
+        <f t="shared" si="330"/>
+        <v>2024</v>
+      </c>
+      <c r="J1214" s="4">
+        <f t="shared" si="331"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1215" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1215" s="3"/>
-      <c r="B1215" s="3"/>
-      <c r="C1215" s="3"/>
-      <c r="D1215" s="3"/>
-      <c r="E1215" s="3"/>
-      <c r="F1215" s="3"/>
-      <c r="G1215" s="3"/>
-      <c r="H1215" s="3"/>
-      <c r="I1215" s="4"/>
-      <c r="J1215" s="4"/>
+      <c r="A1215" s="3" t="s">
+        <v>1190</v>
+      </c>
+      <c r="B1215" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1215" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1215" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1215" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1215" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1215" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1215" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1215" s="4">
+        <f t="shared" ref="I1215:I1216" si="332">YEAR(A1215)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1215" s="4">
+        <f t="shared" ref="J1215:J1216" si="333">MONTH(A1215)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1216" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1216" s="3"/>
-      <c r="B1216" s="3"/>
-      <c r="C1216" s="3"/>
-      <c r="D1216" s="3"/>
-      <c r="E1216" s="3"/>
-      <c r="F1216" s="3"/>
-      <c r="G1216" s="3"/>
-      <c r="H1216" s="3"/>
-      <c r="I1216" s="4"/>
-      <c r="J1216" s="4"/>
+      <c r="A1216" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B1216" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1216" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1216" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1216" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1216" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1216" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1216" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1216" s="4">
+        <f t="shared" si="332"/>
+        <v>2024</v>
+      </c>
+      <c r="J1216" s="4">
+        <f t="shared" si="333"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1217" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1217" s="3"/>
-      <c r="B1217" s="3"/>
-      <c r="C1217" s="3"/>
-      <c r="D1217" s="3"/>
-      <c r="E1217" s="3"/>
-      <c r="F1217" s="3"/>
-      <c r="G1217" s="3"/>
-      <c r="H1217" s="3"/>
-      <c r="I1217" s="4"/>
-      <c r="J1217" s="4"/>
+      <c r="A1217" s="3" t="s">
+        <v>1191</v>
+      </c>
+      <c r="B1217" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1217" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1217" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1217" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1217" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1217" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1217" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1217" s="4">
+        <f t="shared" ref="I1217" si="334">YEAR(A1217)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1217" s="4">
+        <f t="shared" ref="J1217" si="335">MONTH(A1217)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1218" s="3"/>
+      <c r="B1218" s="3"/>
+      <c r="C1218" s="3"/>
+      <c r="D1218" s="3"/>
+      <c r="E1218" s="3"/>
+      <c r="F1218" s="3"/>
+      <c r="G1218" s="3"/>
+      <c r="H1218" s="3"/>
+      <c r="I1218" s="4"/>
+      <c r="J1218" s="4"/>
+    </row>
+    <row r="1219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1219" s="3"/>
+      <c r="B1219" s="3"/>
+      <c r="C1219" s="3"/>
+      <c r="D1219" s="3"/>
+      <c r="E1219" s="3"/>
+      <c r="F1219" s="3"/>
+      <c r="G1219" s="3"/>
+      <c r="H1219" s="3"/>
+      <c r="I1219" s="4"/>
+      <c r="J1219" s="4"/>
+    </row>
+    <row r="1220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1220" s="3"/>
+      <c r="B1220" s="3"/>
+      <c r="C1220" s="3"/>
+      <c r="D1220" s="3"/>
+      <c r="E1220" s="3"/>
+      <c r="F1220" s="3"/>
+      <c r="G1220" s="3"/>
+      <c r="H1220" s="3"/>
+      <c r="I1220" s="4"/>
+      <c r="J1220" s="4"/>
+    </row>
+    <row r="1221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1221" s="3"/>
+      <c r="B1221" s="3"/>
+      <c r="C1221" s="3"/>
+      <c r="D1221" s="3"/>
+      <c r="E1221" s="3"/>
+      <c r="F1221" s="3"/>
+      <c r="G1221" s="3"/>
+      <c r="H1221" s="3"/>
+      <c r="I1221" s="4"/>
+      <c r="J1221" s="4"/>
+    </row>
+    <row r="1222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1222" s="3"/>
+      <c r="B1222" s="3"/>
+      <c r="C1222" s="3"/>
+      <c r="D1222" s="3"/>
+      <c r="E1222" s="3"/>
+      <c r="F1222" s="3"/>
+      <c r="G1222" s="3"/>
+      <c r="H1222" s="3"/>
+      <c r="I1222" s="4"/>
+      <c r="J1222" s="4"/>
+    </row>
+    <row r="1223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1223" s="3"/>
+      <c r="B1223" s="3"/>
+      <c r="C1223" s="3"/>
+      <c r="D1223" s="3"/>
+      <c r="E1223" s="3"/>
+      <c r="F1223" s="3"/>
+      <c r="G1223" s="3"/>
+      <c r="H1223" s="3"/>
+      <c r="I1223" s="4"/>
+      <c r="J1223" s="4"/>
+    </row>
+    <row r="1224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1224" s="3"/>
+      <c r="B1224" s="3"/>
+      <c r="C1224" s="3"/>
+      <c r="D1224" s="3"/>
+      <c r="E1224" s="3"/>
+      <c r="F1224" s="3"/>
+      <c r="G1224" s="3"/>
+      <c r="H1224" s="3"/>
+      <c r="I1224" s="4"/>
+      <c r="J1224" s="4"/>
+    </row>
+    <row r="1225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1225" s="3"/>
+      <c r="B1225" s="3"/>
+      <c r="C1225" s="3"/>
+      <c r="D1225" s="3"/>
+      <c r="E1225" s="3"/>
+      <c r="F1225" s="3"/>
+      <c r="G1225" s="3"/>
+      <c r="H1225" s="3"/>
+      <c r="I1225" s="4"/>
+      <c r="J1225" s="4"/>
+    </row>
+    <row r="1226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1226" s="3"/>
+      <c r="B1226" s="3"/>
+      <c r="C1226" s="3"/>
+      <c r="D1226" s="3"/>
+      <c r="E1226" s="3"/>
+      <c r="F1226" s="3"/>
+      <c r="G1226" s="3"/>
+      <c r="H1226" s="3"/>
+      <c r="I1226" s="4"/>
+      <c r="J1226" s="4"/>
+    </row>
+    <row r="1227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1227" s="3"/>
+      <c r="B1227" s="3"/>
+      <c r="C1227" s="3"/>
+      <c r="D1227" s="3"/>
+      <c r="E1227" s="3"/>
+      <c r="F1227" s="3"/>
+      <c r="G1227" s="3"/>
+      <c r="H1227" s="3"/>
+      <c r="I1227" s="4"/>
+      <c r="J1227" s="4"/>
+    </row>
+    <row r="1228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1228" s="3"/>
+      <c r="B1228" s="3"/>
+      <c r="C1228" s="3"/>
+      <c r="D1228" s="3"/>
+      <c r="E1228" s="3"/>
+      <c r="F1228" s="3"/>
+      <c r="G1228" s="3"/>
+      <c r="H1228" s="3"/>
+      <c r="I1228" s="4"/>
+      <c r="J1228" s="4"/>
+    </row>
+    <row r="1229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1229" s="3"/>
+      <c r="B1229" s="3"/>
+      <c r="C1229" s="3"/>
+      <c r="D1229" s="3"/>
+      <c r="E1229" s="3"/>
+      <c r="F1229" s="3"/>
+      <c r="G1229" s="3"/>
+      <c r="H1229" s="3"/>
+      <c r="I1229" s="4"/>
+      <c r="J1229" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#34 Time Tracking.xlsx: updated up to 2024-10-18.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9493" uniqueCount="1192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9541" uniqueCount="1195">
   <si>
     <t>Year</t>
   </si>
@@ -3598,6 +3598,15 @@
   </si>
   <si>
     <t>2024-10-11</t>
+  </si>
+  <si>
+    <t>2024-10-13</t>
+  </si>
+  <si>
+    <t>2024-10-14</t>
+  </si>
+  <si>
+    <t>2024-10-15</t>
   </si>
 </sst>
 </file>
@@ -3997,11 +4006,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1229"/>
+  <dimension ref="A1:J1235"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1196" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1219" sqref="D1219"/>
+      <pane ySplit="1" topLeftCell="A1202" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1225" sqref="C1225"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44897,85 +44906,217 @@
         <v>280</v>
       </c>
       <c r="I1217" s="4">
-        <f t="shared" ref="I1217" si="334">YEAR(A1217)</f>
+        <f t="shared" ref="I1217:I1219" si="334">YEAR(A1217)</f>
         <v>2024</v>
       </c>
       <c r="J1217" s="4">
-        <f t="shared" ref="J1217" si="335">MONTH(A1217)</f>
+        <f t="shared" ref="J1217:J1219" si="335">MONTH(A1217)</f>
         <v>10</v>
       </c>
     </row>
     <row r="1218" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1218" s="3"/>
-      <c r="B1218" s="3"/>
-      <c r="C1218" s="3"/>
-      <c r="D1218" s="3"/>
-      <c r="E1218" s="3"/>
-      <c r="F1218" s="3"/>
-      <c r="G1218" s="3"/>
-      <c r="H1218" s="3"/>
-      <c r="I1218" s="4"/>
-      <c r="J1218" s="4"/>
+      <c r="A1218" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B1218" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1218" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1218" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1218" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1218" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1218" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1218" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1218" s="4">
+        <f t="shared" si="334"/>
+        <v>2024</v>
+      </c>
+      <c r="J1218" s="4">
+        <f t="shared" si="335"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1219" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1219" s="3"/>
-      <c r="B1219" s="3"/>
-      <c r="C1219" s="3"/>
-      <c r="D1219" s="3"/>
-      <c r="E1219" s="3"/>
-      <c r="F1219" s="3"/>
-      <c r="G1219" s="3"/>
-      <c r="H1219" s="3"/>
-      <c r="I1219" s="4"/>
-      <c r="J1219" s="4"/>
+      <c r="A1219" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B1219" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1219" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1219" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1219" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1219" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1219" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1219" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1219" s="4">
+        <f t="shared" si="334"/>
+        <v>2024</v>
+      </c>
+      <c r="J1219" s="4">
+        <f t="shared" si="335"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1220" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1220" s="3"/>
-      <c r="B1220" s="3"/>
-      <c r="C1220" s="3"/>
-      <c r="D1220" s="3"/>
-      <c r="E1220" s="3"/>
-      <c r="F1220" s="3"/>
-      <c r="G1220" s="3"/>
-      <c r="H1220" s="3"/>
-      <c r="I1220" s="4"/>
-      <c r="J1220" s="4"/>
+      <c r="A1220" s="3" t="s">
+        <v>1192</v>
+      </c>
+      <c r="B1220" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1220" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1220" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1220" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1220" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1220" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1220" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1220" s="4">
+        <f t="shared" ref="I1220:I1221" si="336">YEAR(A1220)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1220" s="4">
+        <f t="shared" ref="J1220:J1221" si="337">MONTH(A1220)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1221" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1221" s="3"/>
-      <c r="B1221" s="3"/>
-      <c r="C1221" s="3"/>
-      <c r="D1221" s="3"/>
-      <c r="E1221" s="3"/>
-      <c r="F1221" s="3"/>
-      <c r="G1221" s="3"/>
-      <c r="H1221" s="3"/>
-      <c r="I1221" s="4"/>
-      <c r="J1221" s="4"/>
+      <c r="A1221" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B1221" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1221" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1221" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1221" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1221" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1221" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1221" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1221" s="4">
+        <f t="shared" si="336"/>
+        <v>2024</v>
+      </c>
+      <c r="J1221" s="4">
+        <f t="shared" si="337"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1222" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1222" s="3"/>
-      <c r="B1222" s="3"/>
-      <c r="C1222" s="3"/>
-      <c r="D1222" s="3"/>
-      <c r="E1222" s="3"/>
-      <c r="F1222" s="3"/>
-      <c r="G1222" s="3"/>
-      <c r="H1222" s="3"/>
-      <c r="I1222" s="4"/>
-      <c r="J1222" s="4"/>
+      <c r="A1222" s="3" t="s">
+        <v>1193</v>
+      </c>
+      <c r="B1222" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1222" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1222" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1222" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1222" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1222" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1222" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1222" s="4">
+        <f t="shared" ref="I1222" si="338">YEAR(A1222)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1222" s="4">
+        <f t="shared" ref="J1222" si="339">MONTH(A1222)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1223" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1223" s="3"/>
-      <c r="B1223" s="3"/>
-      <c r="C1223" s="3"/>
-      <c r="D1223" s="3"/>
-      <c r="E1223" s="3"/>
-      <c r="F1223" s="3"/>
-      <c r="G1223" s="3"/>
-      <c r="H1223" s="3"/>
-      <c r="I1223" s="4"/>
-      <c r="J1223" s="4"/>
+      <c r="A1223" s="3" t="s">
+        <v>1194</v>
+      </c>
+      <c r="B1223" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1223" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1223" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1223" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1223" s="3" t="s">
+        <v>1187</v>
+      </c>
+      <c r="G1223" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1223" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1223" s="4">
+        <f t="shared" ref="I1223" si="340">YEAR(A1223)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1223" s="4">
+        <f t="shared" ref="J1223" si="341">MONTH(A1223)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1224" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1224" s="3"/>
@@ -45049,6 +45190,78 @@
       <c r="I1229" s="4"/>
       <c r="J1229" s="4"/>
     </row>
+    <row r="1230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1230" s="3"/>
+      <c r="B1230" s="3"/>
+      <c r="C1230" s="3"/>
+      <c r="D1230" s="3"/>
+      <c r="E1230" s="3"/>
+      <c r="F1230" s="3"/>
+      <c r="G1230" s="3"/>
+      <c r="H1230" s="3"/>
+      <c r="I1230" s="4"/>
+      <c r="J1230" s="4"/>
+    </row>
+    <row r="1231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1231" s="3"/>
+      <c r="B1231" s="3"/>
+      <c r="C1231" s="3"/>
+      <c r="D1231" s="3"/>
+      <c r="E1231" s="3"/>
+      <c r="F1231" s="3"/>
+      <c r="G1231" s="3"/>
+      <c r="H1231" s="3"/>
+      <c r="I1231" s="4"/>
+      <c r="J1231" s="4"/>
+    </row>
+    <row r="1232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1232" s="3"/>
+      <c r="B1232" s="3"/>
+      <c r="C1232" s="3"/>
+      <c r="D1232" s="3"/>
+      <c r="E1232" s="3"/>
+      <c r="F1232" s="3"/>
+      <c r="G1232" s="3"/>
+      <c r="H1232" s="3"/>
+      <c r="I1232" s="4"/>
+      <c r="J1232" s="4"/>
+    </row>
+    <row r="1233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1233" s="3"/>
+      <c r="B1233" s="3"/>
+      <c r="C1233" s="3"/>
+      <c r="D1233" s="3"/>
+      <c r="E1233" s="3"/>
+      <c r="F1233" s="3"/>
+      <c r="G1233" s="3"/>
+      <c r="H1233" s="3"/>
+      <c r="I1233" s="4"/>
+      <c r="J1233" s="4"/>
+    </row>
+    <row r="1234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1234" s="3"/>
+      <c r="B1234" s="3"/>
+      <c r="C1234" s="3"/>
+      <c r="D1234" s="3"/>
+      <c r="E1234" s="3"/>
+      <c r="F1234" s="3"/>
+      <c r="G1234" s="3"/>
+      <c r="H1234" s="3"/>
+      <c r="I1234" s="4"/>
+      <c r="J1234" s="4"/>
+    </row>
+    <row r="1235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1235" s="3"/>
+      <c r="B1235" s="3"/>
+      <c r="C1235" s="3"/>
+      <c r="D1235" s="3"/>
+      <c r="E1235" s="3"/>
+      <c r="F1235" s="3"/>
+      <c r="G1235" s="3"/>
+      <c r="H1235" s="3"/>
+      <c r="I1235" s="4"/>
+      <c r="J1235" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#34 Time Tracking.xlsx: updated up to 2024-10-22.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9541" uniqueCount="1195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9612" uniqueCount="1201">
   <si>
     <t>Year</t>
   </si>
@@ -3607,6 +3607,24 @@
   </si>
   <si>
     <t>2024-10-15</t>
+  </si>
+  <si>
+    <t>2024-10-18</t>
+  </si>
+  <si>
+    <t>2024-10-19</t>
+  </si>
+  <si>
+    <t>2024-10-20</t>
+  </si>
+  <si>
+    <t>2024-10-21</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.2.0</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.7.0</t>
   </si>
 </sst>
 </file>
@@ -4006,11 +4024,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1235"/>
+  <dimension ref="A1:J1253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1202" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1225" sqref="C1225"/>
+      <pane ySplit="1" topLeftCell="A1193" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1208" sqref="F1208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -44489,7 +44507,7 @@
         <v>127</v>
       </c>
       <c r="F1205" s="3" t="s">
-        <v>1179</v>
+        <v>1200</v>
       </c>
       <c r="G1205" s="8" t="s">
         <v>279</v>
@@ -44523,7 +44541,7 @@
         <v>127</v>
       </c>
       <c r="F1206" s="3" t="s">
-        <v>1179</v>
+        <v>1200</v>
       </c>
       <c r="G1206" s="8" t="s">
         <v>279</v>
@@ -45110,121 +45128,317 @@
         <v>279</v>
       </c>
       <c r="I1223" s="4">
-        <f t="shared" ref="I1223" si="340">YEAR(A1223)</f>
+        <f t="shared" ref="I1223:I1225" si="340">YEAR(A1223)</f>
         <v>2024</v>
       </c>
       <c r="J1223" s="4">
-        <f t="shared" ref="J1223" si="341">MONTH(A1223)</f>
+        <f t="shared" ref="J1223:J1225" si="341">MONTH(A1223)</f>
         <v>10</v>
       </c>
     </row>
     <row r="1224" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1224" s="3"/>
-      <c r="B1224" s="3"/>
-      <c r="C1224" s="3"/>
-      <c r="D1224" s="3"/>
-      <c r="E1224" s="3"/>
+      <c r="A1224" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B1224" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1224" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1224" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1224" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1224" s="3"/>
-      <c r="G1224" s="3"/>
-      <c r="H1224" s="3"/>
-      <c r="I1224" s="4"/>
-      <c r="J1224" s="4"/>
+      <c r="G1224" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1224" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1224" s="4">
+        <f t="shared" si="340"/>
+        <v>2024</v>
+      </c>
+      <c r="J1224" s="4">
+        <f t="shared" si="341"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1225" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1225" s="3"/>
-      <c r="B1225" s="3"/>
-      <c r="C1225" s="3"/>
-      <c r="D1225" s="3"/>
-      <c r="E1225" s="3"/>
-      <c r="F1225" s="3"/>
-      <c r="G1225" s="3"/>
-      <c r="H1225" s="3"/>
-      <c r="I1225" s="4"/>
-      <c r="J1225" s="4"/>
+      <c r="A1225" s="3" t="s">
+        <v>1195</v>
+      </c>
+      <c r="B1225" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1225" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1225" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1225" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1225" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1225" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1225" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1225" s="4">
+        <f t="shared" si="340"/>
+        <v>2024</v>
+      </c>
+      <c r="J1225" s="4">
+        <f t="shared" si="341"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1226" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1226" s="3"/>
-      <c r="B1226" s="3"/>
-      <c r="C1226" s="3"/>
-      <c r="D1226" s="3"/>
-      <c r="E1226" s="3"/>
-      <c r="F1226" s="3"/>
-      <c r="G1226" s="3"/>
-      <c r="H1226" s="3"/>
-      <c r="I1226" s="4"/>
-      <c r="J1226" s="4"/>
+      <c r="A1226" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B1226" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1226" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1226" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1226" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1226" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1226" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1226" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1226" s="4">
+        <f t="shared" ref="I1226:I1228" si="342">YEAR(A1226)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1226" s="4">
+        <f t="shared" ref="J1226:J1228" si="343">MONTH(A1226)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1227" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1227" s="3"/>
-      <c r="B1227" s="3"/>
-      <c r="C1227" s="3"/>
-      <c r="D1227" s="3"/>
-      <c r="E1227" s="3"/>
-      <c r="F1227" s="3"/>
-      <c r="G1227" s="3"/>
-      <c r="H1227" s="3"/>
-      <c r="I1227" s="4"/>
-      <c r="J1227" s="4"/>
+      <c r="A1227" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B1227" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1227" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1227" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1227" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1227" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1227" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1227" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1227" s="4">
+        <f t="shared" si="342"/>
+        <v>2024</v>
+      </c>
+      <c r="J1227" s="4">
+        <f t="shared" si="343"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1228" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1228" s="3"/>
-      <c r="B1228" s="3"/>
-      <c r="C1228" s="3"/>
-      <c r="D1228" s="3"/>
-      <c r="E1228" s="3"/>
-      <c r="F1228" s="3"/>
-      <c r="G1228" s="3"/>
-      <c r="H1228" s="3"/>
-      <c r="I1228" s="4"/>
-      <c r="J1228" s="4"/>
+      <c r="A1228" s="3" t="s">
+        <v>1196</v>
+      </c>
+      <c r="B1228" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1228" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1228" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1228" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1228" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1228" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1228" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1228" s="4">
+        <f t="shared" si="342"/>
+        <v>2024</v>
+      </c>
+      <c r="J1228" s="4">
+        <f t="shared" si="343"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1229" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1229" s="3"/>
-      <c r="B1229" s="3"/>
-      <c r="C1229" s="3"/>
-      <c r="D1229" s="3"/>
-      <c r="E1229" s="3"/>
-      <c r="F1229" s="3"/>
-      <c r="G1229" s="3"/>
-      <c r="H1229" s="3"/>
-      <c r="I1229" s="4"/>
-      <c r="J1229" s="4"/>
+      <c r="A1229" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B1229" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1229" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="D1229" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1229" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1229" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1229" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1229" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1229" s="4">
+        <f t="shared" ref="I1229:I1231" si="344">YEAR(A1229)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1229" s="4">
+        <f t="shared" ref="J1229:J1231" si="345">MONTH(A1229)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1230" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1230" s="3"/>
-      <c r="B1230" s="3"/>
-      <c r="C1230" s="3"/>
-      <c r="D1230" s="3"/>
-      <c r="E1230" s="3"/>
-      <c r="F1230" s="3"/>
-      <c r="G1230" s="3"/>
-      <c r="H1230" s="3"/>
-      <c r="I1230" s="4"/>
-      <c r="J1230" s="4"/>
+      <c r="A1230" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B1230" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1230" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1230" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1230" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1230" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1230" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1230" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1230" s="4">
+        <f t="shared" si="344"/>
+        <v>2024</v>
+      </c>
+      <c r="J1230" s="4">
+        <f t="shared" si="345"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1231" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1231" s="3"/>
-      <c r="B1231" s="3"/>
-      <c r="C1231" s="3"/>
-      <c r="D1231" s="3"/>
-      <c r="E1231" s="3"/>
-      <c r="F1231" s="3"/>
-      <c r="G1231" s="3"/>
-      <c r="H1231" s="3"/>
-      <c r="I1231" s="4"/>
-      <c r="J1231" s="4"/>
+      <c r="A1231" s="3" t="s">
+        <v>1197</v>
+      </c>
+      <c r="B1231" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1231" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1231" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1231" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1231" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1231" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1231" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1231" s="4">
+        <f t="shared" si="344"/>
+        <v>2024</v>
+      </c>
+      <c r="J1231" s="4">
+        <f t="shared" si="345"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1232" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1232" s="3"/>
-      <c r="B1232" s="3"/>
-      <c r="C1232" s="3"/>
-      <c r="D1232" s="3"/>
-      <c r="E1232" s="3"/>
-      <c r="F1232" s="3"/>
-      <c r="G1232" s="3"/>
-      <c r="H1232" s="3"/>
-      <c r="I1232" s="4"/>
-      <c r="J1232" s="4"/>
+      <c r="A1232" s="3" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B1232" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1232" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1232" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1232" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1232" s="3" t="s">
+        <v>1199</v>
+      </c>
+      <c r="G1232" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1232" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1232" s="4">
+        <f t="shared" ref="I1232" si="346">YEAR(A1232)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1232" s="4">
+        <f t="shared" ref="J1232" si="347">MONTH(A1232)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1233" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1233" s="3"/>
@@ -45262,6 +45476,222 @@
       <c r="I1235" s="4"/>
       <c r="J1235" s="4"/>
     </row>
+    <row r="1236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1236" s="3"/>
+      <c r="B1236" s="3"/>
+      <c r="C1236" s="3"/>
+      <c r="D1236" s="3"/>
+      <c r="E1236" s="3"/>
+      <c r="F1236" s="3"/>
+      <c r="G1236" s="3"/>
+      <c r="H1236" s="3"/>
+      <c r="I1236" s="4"/>
+      <c r="J1236" s="4"/>
+    </row>
+    <row r="1237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1237" s="3"/>
+      <c r="B1237" s="3"/>
+      <c r="C1237" s="3"/>
+      <c r="D1237" s="3"/>
+      <c r="E1237" s="3"/>
+      <c r="F1237" s="3"/>
+      <c r="G1237" s="3"/>
+      <c r="H1237" s="3"/>
+      <c r="I1237" s="4"/>
+      <c r="J1237" s="4"/>
+    </row>
+    <row r="1238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1238" s="3"/>
+      <c r="B1238" s="3"/>
+      <c r="C1238" s="3"/>
+      <c r="D1238" s="3"/>
+      <c r="E1238" s="3"/>
+      <c r="F1238" s="3"/>
+      <c r="G1238" s="3"/>
+      <c r="H1238" s="3"/>
+      <c r="I1238" s="4"/>
+      <c r="J1238" s="4"/>
+    </row>
+    <row r="1239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1239" s="3"/>
+      <c r="B1239" s="3"/>
+      <c r="C1239" s="3"/>
+      <c r="D1239" s="3"/>
+      <c r="E1239" s="3"/>
+      <c r="F1239" s="3"/>
+      <c r="G1239" s="3"/>
+      <c r="H1239" s="3"/>
+      <c r="I1239" s="4"/>
+      <c r="J1239" s="4"/>
+    </row>
+    <row r="1240" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1240" s="3"/>
+      <c r="B1240" s="3"/>
+      <c r="C1240" s="3"/>
+      <c r="D1240" s="3"/>
+      <c r="E1240" s="3"/>
+      <c r="F1240" s="3"/>
+      <c r="G1240" s="3"/>
+      <c r="H1240" s="3"/>
+      <c r="I1240" s="4"/>
+      <c r="J1240" s="4"/>
+    </row>
+    <row r="1241" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1241" s="3"/>
+      <c r="B1241" s="3"/>
+      <c r="C1241" s="3"/>
+      <c r="D1241" s="3"/>
+      <c r="E1241" s="3"/>
+      <c r="F1241" s="3"/>
+      <c r="G1241" s="3"/>
+      <c r="H1241" s="3"/>
+      <c r="I1241" s="4"/>
+      <c r="J1241" s="4"/>
+    </row>
+    <row r="1242" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1242" s="3"/>
+      <c r="B1242" s="3"/>
+      <c r="C1242" s="3"/>
+      <c r="D1242" s="3"/>
+      <c r="E1242" s="3"/>
+      <c r="F1242" s="3"/>
+      <c r="G1242" s="3"/>
+      <c r="H1242" s="3"/>
+      <c r="I1242" s="4"/>
+      <c r="J1242" s="4"/>
+    </row>
+    <row r="1243" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1243" s="3"/>
+      <c r="B1243" s="3"/>
+      <c r="C1243" s="3"/>
+      <c r="D1243" s="3"/>
+      <c r="E1243" s="3"/>
+      <c r="F1243" s="3"/>
+      <c r="G1243" s="3"/>
+      <c r="H1243" s="3"/>
+      <c r="I1243" s="4"/>
+      <c r="J1243" s="4"/>
+    </row>
+    <row r="1244" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1244" s="3"/>
+      <c r="B1244" s="3"/>
+      <c r="C1244" s="3"/>
+      <c r="D1244" s="3"/>
+      <c r="E1244" s="3"/>
+      <c r="F1244" s="3"/>
+      <c r="G1244" s="3"/>
+      <c r="H1244" s="3"/>
+      <c r="I1244" s="4"/>
+      <c r="J1244" s="4"/>
+    </row>
+    <row r="1245" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1245" s="3"/>
+      <c r="B1245" s="3"/>
+      <c r="C1245" s="3"/>
+      <c r="D1245" s="3"/>
+      <c r="E1245" s="3"/>
+      <c r="F1245" s="3"/>
+      <c r="G1245" s="3"/>
+      <c r="H1245" s="3"/>
+      <c r="I1245" s="4"/>
+      <c r="J1245" s="4"/>
+    </row>
+    <row r="1246" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1246" s="3"/>
+      <c r="B1246" s="3"/>
+      <c r="C1246" s="3"/>
+      <c r="D1246" s="3"/>
+      <c r="E1246" s="3"/>
+      <c r="F1246" s="3"/>
+      <c r="G1246" s="3"/>
+      <c r="H1246" s="3"/>
+      <c r="I1246" s="4"/>
+      <c r="J1246" s="4"/>
+    </row>
+    <row r="1247" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1247" s="3"/>
+      <c r="B1247" s="3"/>
+      <c r="C1247" s="3"/>
+      <c r="D1247" s="3"/>
+      <c r="E1247" s="3"/>
+      <c r="F1247" s="3"/>
+      <c r="G1247" s="3"/>
+      <c r="H1247" s="3"/>
+      <c r="I1247" s="4"/>
+      <c r="J1247" s="4"/>
+    </row>
+    <row r="1248" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1248" s="3"/>
+      <c r="B1248" s="3"/>
+      <c r="C1248" s="3"/>
+      <c r="D1248" s="3"/>
+      <c r="E1248" s="3"/>
+      <c r="F1248" s="3"/>
+      <c r="G1248" s="3"/>
+      <c r="H1248" s="3"/>
+      <c r="I1248" s="4"/>
+      <c r="J1248" s="4"/>
+    </row>
+    <row r="1249" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1249" s="3"/>
+      <c r="B1249" s="3"/>
+      <c r="C1249" s="3"/>
+      <c r="D1249" s="3"/>
+      <c r="E1249" s="3"/>
+      <c r="F1249" s="3"/>
+      <c r="G1249" s="3"/>
+      <c r="H1249" s="3"/>
+      <c r="I1249" s="4"/>
+      <c r="J1249" s="4"/>
+    </row>
+    <row r="1250" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1250" s="3"/>
+      <c r="B1250" s="3"/>
+      <c r="C1250" s="3"/>
+      <c r="D1250" s="3"/>
+      <c r="E1250" s="3"/>
+      <c r="F1250" s="3"/>
+      <c r="G1250" s="3"/>
+      <c r="H1250" s="3"/>
+      <c r="I1250" s="4"/>
+      <c r="J1250" s="4"/>
+    </row>
+    <row r="1251" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1251" s="3"/>
+      <c r="B1251" s="3"/>
+      <c r="C1251" s="3"/>
+      <c r="D1251" s="3"/>
+      <c r="E1251" s="3"/>
+      <c r="F1251" s="3"/>
+      <c r="G1251" s="3"/>
+      <c r="H1251" s="3"/>
+      <c r="I1251" s="4"/>
+      <c r="J1251" s="4"/>
+    </row>
+    <row r="1252" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1252" s="3"/>
+      <c r="B1252" s="3"/>
+      <c r="C1252" s="3"/>
+      <c r="D1252" s="3"/>
+      <c r="E1252" s="3"/>
+      <c r="F1252" s="3"/>
+      <c r="G1252" s="3"/>
+      <c r="H1252" s="3"/>
+      <c r="I1252" s="4"/>
+      <c r="J1252" s="4"/>
+    </row>
+    <row r="1253" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1253" s="3"/>
+      <c r="B1253" s="3"/>
+      <c r="C1253" s="3"/>
+      <c r="D1253" s="3"/>
+      <c r="E1253" s="3"/>
+      <c r="F1253" s="3"/>
+      <c r="G1253" s="3"/>
+      <c r="H1253" s="3"/>
+      <c r="I1253" s="4"/>
+      <c r="J1253" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#34 Time Tracking.xlsx: updated up to 2024-10-26.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9612" uniqueCount="1201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9691" uniqueCount="1207">
   <si>
     <t>Year</t>
   </si>
@@ -3625,6 +3625,24 @@
   </si>
   <si>
     <t>nwtimetracking v3.7.0</t>
+  </si>
+  <si>
+    <t>2024-10-22</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.1.0</t>
+  </si>
+  <si>
+    <t>nwshared v1.5.0</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.2.0</t>
+  </si>
+  <si>
+    <t>2024-10-24</t>
+  </si>
+  <si>
+    <t>2024-10-25</t>
   </si>
 </sst>
 </file>
@@ -4027,8 +4045,8 @@
   <dimension ref="A1:J1253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1208" sqref="F1208"/>
+      <pane ySplit="1" topLeftCell="A1214" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1244" sqref="G1244"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -45432,133 +45450,351 @@
         <v>279</v>
       </c>
       <c r="I1232" s="4">
-        <f t="shared" ref="I1232" si="346">YEAR(A1232)</f>
+        <f t="shared" ref="I1232:I1233" si="346">YEAR(A1232)</f>
         <v>2024</v>
       </c>
       <c r="J1232" s="4">
-        <f t="shared" ref="J1232" si="347">MONTH(A1232)</f>
+        <f t="shared" ref="J1232:J1233" si="347">MONTH(A1232)</f>
         <v>10</v>
       </c>
     </row>
     <row r="1233" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1233" s="3"/>
-      <c r="B1233" s="3"/>
-      <c r="C1233" s="3"/>
-      <c r="D1233" s="3"/>
-      <c r="E1233" s="3"/>
+      <c r="A1233" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B1233" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1233" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1233" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1233" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1233" s="3"/>
-      <c r="G1233" s="3"/>
-      <c r="H1233" s="3"/>
-      <c r="I1233" s="4"/>
-      <c r="J1233" s="4"/>
+      <c r="G1233" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1233" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1233" s="4">
+        <f t="shared" si="346"/>
+        <v>2024</v>
+      </c>
+      <c r="J1233" s="4">
+        <f t="shared" si="347"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1234" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1234" s="3"/>
-      <c r="B1234" s="3"/>
-      <c r="C1234" s="3"/>
-      <c r="D1234" s="3"/>
-      <c r="E1234" s="3"/>
-      <c r="F1234" s="3"/>
-      <c r="G1234" s="3"/>
-      <c r="H1234" s="3"/>
-      <c r="I1234" s="4"/>
-      <c r="J1234" s="4"/>
+      <c r="A1234" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B1234" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1234" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1234" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1234" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1234" s="3" t="s">
+        <v>1202</v>
+      </c>
+      <c r="G1234" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1234" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1234" s="4">
+        <f t="shared" ref="I1234" si="348">YEAR(A1234)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1234" s="4">
+        <f t="shared" ref="J1234" si="349">MONTH(A1234)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1235" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1235" s="3"/>
-      <c r="B1235" s="3"/>
-      <c r="C1235" s="3"/>
-      <c r="D1235" s="3"/>
-      <c r="E1235" s="3"/>
-      <c r="F1235" s="3"/>
-      <c r="G1235" s="3"/>
-      <c r="H1235" s="3"/>
-      <c r="I1235" s="4"/>
-      <c r="J1235" s="4"/>
+      <c r="A1235" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B1235" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1235" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1235" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1235" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1235" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G1235" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1235" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1235" s="4">
+        <f t="shared" ref="I1235" si="350">YEAR(A1235)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1235" s="4">
+        <f t="shared" ref="J1235" si="351">MONTH(A1235)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1236" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1236" s="3"/>
-      <c r="B1236" s="3"/>
-      <c r="C1236" s="3"/>
-      <c r="D1236" s="3"/>
-      <c r="E1236" s="3"/>
-      <c r="F1236" s="3"/>
-      <c r="G1236" s="3"/>
-      <c r="H1236" s="3"/>
-      <c r="I1236" s="4"/>
-      <c r="J1236" s="4"/>
+      <c r="A1236" s="3" t="s">
+        <v>1201</v>
+      </c>
+      <c r="B1236" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1236" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1236" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1236" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1236" s="3" t="s">
+        <v>1203</v>
+      </c>
+      <c r="G1236" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1236" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1236" s="4">
+        <f t="shared" ref="I1236:I1238" si="352">YEAR(A1236)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1236" s="4">
+        <f t="shared" ref="J1236:J1238" si="353">MONTH(A1236)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1237" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1237" s="3"/>
-      <c r="B1237" s="3"/>
-      <c r="C1237" s="3"/>
-      <c r="D1237" s="3"/>
-      <c r="E1237" s="3"/>
-      <c r="F1237" s="3"/>
-      <c r="G1237" s="3"/>
-      <c r="H1237" s="3"/>
-      <c r="I1237" s="4"/>
-      <c r="J1237" s="4"/>
+      <c r="A1237" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B1237" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1237" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1237" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1237" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1237" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G1237" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1237" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1237" s="4">
+        <f t="shared" si="352"/>
+        <v>2024</v>
+      </c>
+      <c r="J1237" s="4">
+        <f t="shared" si="353"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1238" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1238" s="3"/>
-      <c r="B1238" s="3"/>
-      <c r="C1238" s="3"/>
-      <c r="D1238" s="3"/>
-      <c r="E1238" s="3"/>
-      <c r="F1238" s="3"/>
-      <c r="G1238" s="3"/>
-      <c r="H1238" s="3"/>
-      <c r="I1238" s="4"/>
-      <c r="J1238" s="4"/>
+      <c r="A1238" s="3" t="s">
+        <v>1205</v>
+      </c>
+      <c r="B1238" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1238" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1238" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1238" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1238" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G1238" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1238" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1238" s="4">
+        <f t="shared" si="352"/>
+        <v>2024</v>
+      </c>
+      <c r="J1238" s="4">
+        <f t="shared" si="353"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1239" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1239" s="3"/>
-      <c r="B1239" s="3"/>
-      <c r="C1239" s="3"/>
-      <c r="D1239" s="3"/>
-      <c r="E1239" s="3"/>
-      <c r="F1239" s="3"/>
-      <c r="G1239" s="3"/>
-      <c r="H1239" s="3"/>
-      <c r="I1239" s="4"/>
-      <c r="J1239" s="4"/>
+      <c r="A1239" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1239" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1239" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1239" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1239" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1239" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G1239" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1239" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1239" s="4">
+        <f t="shared" ref="I1239:I1242" si="354">YEAR(A1239)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1239" s="4">
+        <f t="shared" ref="J1239:J1242" si="355">MONTH(A1239)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1240" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1240" s="3"/>
-      <c r="B1240" s="3"/>
-      <c r="C1240" s="3"/>
-      <c r="D1240" s="3"/>
-      <c r="E1240" s="3"/>
-      <c r="F1240" s="3"/>
-      <c r="G1240" s="3"/>
-      <c r="H1240" s="3"/>
-      <c r="I1240" s="4"/>
-      <c r="J1240" s="4"/>
+      <c r="A1240" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1240" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1240" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1240" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1240" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1240" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G1240" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1240" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1240" s="4">
+        <f t="shared" si="354"/>
+        <v>2024</v>
+      </c>
+      <c r="J1240" s="4">
+        <f t="shared" si="355"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1241" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1241" s="3"/>
-      <c r="B1241" s="3"/>
-      <c r="C1241" s="3"/>
-      <c r="D1241" s="3"/>
-      <c r="E1241" s="3"/>
-      <c r="F1241" s="3"/>
-      <c r="G1241" s="3"/>
-      <c r="H1241" s="3"/>
-      <c r="I1241" s="4"/>
-      <c r="J1241" s="4"/>
+      <c r="A1241" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1241" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1241" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1241" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1241" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1241" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G1241" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1241" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1241" s="4">
+        <f t="shared" si="354"/>
+        <v>2024</v>
+      </c>
+      <c r="J1241" s="4">
+        <f t="shared" si="355"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1242" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1242" s="3"/>
-      <c r="B1242" s="3"/>
-      <c r="C1242" s="3"/>
-      <c r="D1242" s="3"/>
-      <c r="E1242" s="3"/>
-      <c r="F1242" s="3"/>
-      <c r="G1242" s="3"/>
-      <c r="H1242" s="3"/>
-      <c r="I1242" s="4"/>
-      <c r="J1242" s="4"/>
+      <c r="A1242" s="3" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1242" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1242" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1242" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1242" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1242" s="3" t="s">
+        <v>1204</v>
+      </c>
+      <c r="G1242" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1242" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1242" s="4">
+        <f t="shared" si="354"/>
+        <v>2024</v>
+      </c>
+      <c r="J1242" s="4">
+        <f t="shared" si="355"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1243" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1243" s="3"/>

</xml_diff>

<commit_message>
#37 Time Tracking.xlsx: updated up to 2024-11-03.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9691" uniqueCount="1207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9819" uniqueCount="1220">
   <si>
     <t>Year</t>
   </si>
@@ -3643,6 +3643,45 @@
   </si>
   <si>
     <t>2024-10-25</t>
+  </si>
+  <si>
+    <t>2024-10-27</t>
+  </si>
+  <si>
+    <t>NB20230816, 58 -&gt; 94 (36 pp).</t>
+  </si>
+  <si>
+    <t>2024-10-28</t>
+  </si>
+  <si>
+    <t>NB20230816, 95 -&gt; 116 (21 pp).</t>
+  </si>
+  <si>
+    <t>nwshared v1.6.0</t>
+  </si>
+  <si>
+    <t>nwreadinglist v3.8.0</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.8.0</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.3.0</t>
+  </si>
+  <si>
+    <t>2024-10-29</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.6.0</t>
+  </si>
+  <si>
+    <t>2024-10-31</t>
+  </si>
+  <si>
+    <t>2024-11-01</t>
+  </si>
+  <si>
+    <t>2024-11-03</t>
   </si>
 </sst>
 </file>
@@ -4042,11 +4081,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1253"/>
+  <dimension ref="A1:J1275"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1214" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G1244" sqref="G1244"/>
+      <pane ySplit="1" topLeftCell="A1226" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1260" sqref="D1260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -45569,7 +45608,7 @@
         <v>203</v>
       </c>
       <c r="D1236" s="3" t="s">
-        <v>105</v>
+        <v>184</v>
       </c>
       <c r="E1236" s="3" t="s">
         <v>127</v>
@@ -45797,136 +45836,752 @@
       </c>
     </row>
     <row r="1243" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1243" s="3"/>
-      <c r="B1243" s="3"/>
-      <c r="C1243" s="3"/>
-      <c r="D1243" s="3"/>
-      <c r="E1243" s="3"/>
-      <c r="F1243" s="3"/>
-      <c r="G1243" s="3"/>
-      <c r="H1243" s="3"/>
-      <c r="I1243" s="4"/>
-      <c r="J1243" s="4"/>
+      <c r="A1243" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B1243" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1243" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1243" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1243" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1243" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G1243" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1243" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1243" s="4">
+        <f t="shared" ref="I1243" si="356">YEAR(A1243)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1243" s="4">
+        <f t="shared" ref="J1243" si="357">MONTH(A1243)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1244" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1244" s="3"/>
-      <c r="B1244" s="3"/>
-      <c r="C1244" s="3"/>
-      <c r="D1244" s="3"/>
-      <c r="E1244" s="3"/>
-      <c r="F1244" s="3"/>
-      <c r="G1244" s="3"/>
-      <c r="H1244" s="3"/>
-      <c r="I1244" s="4"/>
-      <c r="J1244" s="4"/>
+      <c r="A1244" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B1244" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1244" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1244" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1244" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1244" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G1244" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1244" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1244" s="4">
+        <f t="shared" ref="I1244:I1246" si="358">YEAR(A1244)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1244" s="4">
+        <f t="shared" ref="J1244:J1246" si="359">MONTH(A1244)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1245" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1245" s="3"/>
-      <c r="B1245" s="3"/>
-      <c r="C1245" s="3"/>
-      <c r="D1245" s="3"/>
-      <c r="E1245" s="3"/>
-      <c r="F1245" s="3"/>
-      <c r="G1245" s="3"/>
-      <c r="H1245" s="3"/>
-      <c r="I1245" s="4"/>
-      <c r="J1245" s="4"/>
+      <c r="A1245" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B1245" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1245" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1245" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1245" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1245" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G1245" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1245" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1245" s="4">
+        <f t="shared" si="358"/>
+        <v>2024</v>
+      </c>
+      <c r="J1245" s="4">
+        <f t="shared" si="359"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1246" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1246" s="3"/>
-      <c r="B1246" s="3"/>
-      <c r="C1246" s="3"/>
-      <c r="D1246" s="3"/>
-      <c r="E1246" s="3"/>
-      <c r="F1246" s="3"/>
-      <c r="G1246" s="3"/>
-      <c r="H1246" s="3"/>
-      <c r="I1246" s="4"/>
-      <c r="J1246" s="4"/>
+      <c r="A1246" s="3" t="s">
+        <v>1207</v>
+      </c>
+      <c r="B1246" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1246" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1246" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1246" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1246" s="3" t="s">
+        <v>1208</v>
+      </c>
+      <c r="G1246" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1246" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1246" s="4">
+        <f t="shared" si="358"/>
+        <v>2024</v>
+      </c>
+      <c r="J1246" s="4">
+        <f t="shared" si="359"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1247" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1247" s="3"/>
-      <c r="B1247" s="3"/>
-      <c r="C1247" s="3"/>
-      <c r="D1247" s="3"/>
-      <c r="E1247" s="3"/>
-      <c r="F1247" s="3"/>
-      <c r="G1247" s="3"/>
-      <c r="H1247" s="3"/>
-      <c r="I1247" s="4"/>
-      <c r="J1247" s="4"/>
+      <c r="A1247" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1247" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1247" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1247" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1247" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1247" s="3" t="s">
+        <v>1210</v>
+      </c>
+      <c r="G1247" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1247" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1247" s="4">
+        <f t="shared" ref="I1247:I1248" si="360">YEAR(A1247)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1247" s="4">
+        <f t="shared" ref="J1247:J1248" si="361">MONTH(A1247)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1248" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1248" s="3"/>
-      <c r="B1248" s="3"/>
-      <c r="C1248" s="3"/>
-      <c r="D1248" s="3"/>
-      <c r="E1248" s="3"/>
-      <c r="F1248" s="3"/>
-      <c r="G1248" s="3"/>
-      <c r="H1248" s="3"/>
-      <c r="I1248" s="4"/>
-      <c r="J1248" s="4"/>
+      <c r="A1248" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1248" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1248" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1248" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1248" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1248" s="3" t="s">
+        <v>1211</v>
+      </c>
+      <c r="G1248" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1248" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1248" s="4">
+        <f t="shared" si="360"/>
+        <v>2024</v>
+      </c>
+      <c r="J1248" s="4">
+        <f t="shared" si="361"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="1249" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1249" s="3"/>
-      <c r="B1249" s="3"/>
-      <c r="C1249" s="3"/>
-      <c r="D1249" s="3"/>
-      <c r="E1249" s="3"/>
-      <c r="F1249" s="3"/>
-      <c r="G1249" s="3"/>
-      <c r="H1249" s="3"/>
-      <c r="I1249" s="4"/>
-      <c r="J1249" s="4"/>
+      <c r="A1249" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1249" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1249" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1249" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1249" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1249" s="3" t="s">
+        <v>1212</v>
+      </c>
+      <c r="G1249" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1249" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1249" s="4">
+        <f t="shared" ref="I1249" si="362">YEAR(A1249)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1249" s="4">
+        <f t="shared" ref="J1249" si="363">MONTH(A1249)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1250" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1250" s="3"/>
-      <c r="B1250" s="3"/>
-      <c r="C1250" s="3"/>
-      <c r="D1250" s="3"/>
-      <c r="E1250" s="3"/>
-      <c r="F1250" s="3"/>
-      <c r="G1250" s="3"/>
-      <c r="H1250" s="3"/>
-      <c r="I1250" s="4"/>
-      <c r="J1250" s="4"/>
+      <c r="A1250" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1250" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1250" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1250" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1250" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1250" s="3" t="s">
+        <v>1213</v>
+      </c>
+      <c r="G1250" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1250" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1250" s="4">
+        <f t="shared" ref="I1250" si="364">YEAR(A1250)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1250" s="4">
+        <f t="shared" ref="J1250" si="365">MONTH(A1250)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1251" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1251" s="3"/>
-      <c r="B1251" s="3"/>
-      <c r="C1251" s="3"/>
-      <c r="D1251" s="3"/>
-      <c r="E1251" s="3"/>
-      <c r="F1251" s="3"/>
-      <c r="G1251" s="3"/>
-      <c r="H1251" s="3"/>
-      <c r="I1251" s="4"/>
-      <c r="J1251" s="4"/>
+      <c r="A1251" s="3" t="s">
+        <v>1209</v>
+      </c>
+      <c r="B1251" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1251" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1251" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1251" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1251" s="3" t="s">
+        <v>1214</v>
+      </c>
+      <c r="G1251" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1251" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1251" s="4">
+        <f t="shared" ref="I1251" si="366">YEAR(A1251)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1251" s="4">
+        <f t="shared" ref="J1251" si="367">MONTH(A1251)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1252" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1252" s="3"/>
-      <c r="B1252" s="3"/>
-      <c r="C1252" s="3"/>
-      <c r="D1252" s="3"/>
-      <c r="E1252" s="3"/>
-      <c r="F1252" s="3"/>
-      <c r="G1252" s="3"/>
-      <c r="H1252" s="3"/>
-      <c r="I1252" s="4"/>
-      <c r="J1252" s="4"/>
+      <c r="A1252" s="3" t="s">
+        <v>1215</v>
+      </c>
+      <c r="B1252" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1252" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1252" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1252" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1252" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1252" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1252" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1252" s="4">
+        <f t="shared" ref="I1252" si="368">YEAR(A1252)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1252" s="4">
+        <f t="shared" ref="J1252" si="369">MONTH(A1252)</f>
+        <v>10</v>
+      </c>
     </row>
     <row r="1253" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1253" s="3"/>
-      <c r="B1253" s="3"/>
-      <c r="C1253" s="3"/>
-      <c r="D1253" s="3"/>
-      <c r="E1253" s="3"/>
-      <c r="F1253" s="3"/>
-      <c r="G1253" s="3"/>
-      <c r="H1253" s="3"/>
-      <c r="I1253" s="4"/>
-      <c r="J1253" s="4"/>
+      <c r="A1253" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B1253" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1253" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1253" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1253" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1253" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1253" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1253" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1253" s="4">
+        <f t="shared" ref="I1253:I1254" si="370">YEAR(A1253)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1253" s="4">
+        <f t="shared" ref="J1253:J1254" si="371">MONTH(A1253)</f>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1254" s="3" t="s">
+        <v>1217</v>
+      </c>
+      <c r="B1254" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1254" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1254" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1254" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1254" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1254" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1254" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1254" s="4">
+        <f t="shared" si="370"/>
+        <v>2024</v>
+      </c>
+      <c r="J1254" s="4">
+        <f t="shared" si="371"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1255" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1255" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1255" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1255" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1255" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1255" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1255" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1255" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1255" s="4">
+        <f t="shared" ref="I1255:I1256" si="372">YEAR(A1255)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1255" s="4">
+        <f t="shared" ref="J1255:J1256" si="373">MONTH(A1255)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1256" s="3" t="s">
+        <v>1218</v>
+      </c>
+      <c r="B1256" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1256" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1256" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1256" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1256" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1256" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1256" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1256" s="4">
+        <f t="shared" si="372"/>
+        <v>2024</v>
+      </c>
+      <c r="J1256" s="4">
+        <f t="shared" si="373"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1257" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1257" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1257" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1257" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1257" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1257" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1257" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1257" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1257" s="4">
+        <f t="shared" ref="I1257:I1258" si="374">YEAR(A1257)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1257" s="4">
+        <f t="shared" ref="J1257:J1258" si="375">MONTH(A1257)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1258" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1258" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1258" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1258" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1258" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1258" s="3" t="s">
+        <v>1216</v>
+      </c>
+      <c r="G1258" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1258" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1258" s="4">
+        <f t="shared" si="374"/>
+        <v>2024</v>
+      </c>
+      <c r="J1258" s="4">
+        <f t="shared" si="375"/>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1259" s="3"/>
+      <c r="B1259" s="3"/>
+      <c r="C1259" s="3"/>
+      <c r="D1259" s="3"/>
+      <c r="E1259" s="3"/>
+      <c r="F1259" s="3"/>
+      <c r="G1259" s="3"/>
+      <c r="H1259" s="3"/>
+      <c r="I1259" s="4"/>
+      <c r="J1259" s="4"/>
+    </row>
+    <row r="1260" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1260" s="3"/>
+      <c r="B1260" s="3"/>
+      <c r="C1260" s="3"/>
+      <c r="D1260" s="3"/>
+      <c r="E1260" s="3"/>
+      <c r="F1260" s="3"/>
+      <c r="G1260" s="3"/>
+      <c r="H1260" s="3"/>
+      <c r="I1260" s="4"/>
+      <c r="J1260" s="4"/>
+    </row>
+    <row r="1261" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1261" s="3"/>
+      <c r="B1261" s="3"/>
+      <c r="C1261" s="3"/>
+      <c r="D1261" s="3"/>
+      <c r="E1261" s="3"/>
+      <c r="F1261" s="3"/>
+      <c r="G1261" s="3"/>
+      <c r="H1261" s="3"/>
+      <c r="I1261" s="4"/>
+      <c r="J1261" s="4"/>
+    </row>
+    <row r="1262" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1262" s="3"/>
+      <c r="B1262" s="3"/>
+      <c r="C1262" s="3"/>
+      <c r="D1262" s="3"/>
+      <c r="E1262" s="3"/>
+      <c r="F1262" s="3"/>
+      <c r="G1262" s="3"/>
+      <c r="H1262" s="3"/>
+      <c r="I1262" s="4"/>
+      <c r="J1262" s="4"/>
+    </row>
+    <row r="1263" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1263" s="3"/>
+      <c r="B1263" s="3"/>
+      <c r="C1263" s="3"/>
+      <c r="D1263" s="3"/>
+      <c r="E1263" s="3"/>
+      <c r="F1263" s="3"/>
+      <c r="G1263" s="3"/>
+      <c r="H1263" s="3"/>
+      <c r="I1263" s="4"/>
+      <c r="J1263" s="4"/>
+    </row>
+    <row r="1264" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1264" s="3"/>
+      <c r="B1264" s="3"/>
+      <c r="C1264" s="3"/>
+      <c r="D1264" s="3"/>
+      <c r="E1264" s="3"/>
+      <c r="F1264" s="3"/>
+      <c r="G1264" s="3"/>
+      <c r="H1264" s="3"/>
+      <c r="I1264" s="4"/>
+      <c r="J1264" s="4"/>
+    </row>
+    <row r="1265" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1265" s="3"/>
+      <c r="B1265" s="3"/>
+      <c r="C1265" s="3"/>
+      <c r="D1265" s="3"/>
+      <c r="E1265" s="3"/>
+      <c r="F1265" s="3"/>
+      <c r="G1265" s="3"/>
+      <c r="H1265" s="3"/>
+      <c r="I1265" s="4"/>
+      <c r="J1265" s="4"/>
+    </row>
+    <row r="1266" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1266" s="3"/>
+      <c r="B1266" s="3"/>
+      <c r="C1266" s="3"/>
+      <c r="D1266" s="3"/>
+      <c r="E1266" s="3"/>
+      <c r="F1266" s="3"/>
+      <c r="G1266" s="3"/>
+      <c r="H1266" s="3"/>
+      <c r="I1266" s="4"/>
+      <c r="J1266" s="4"/>
+    </row>
+    <row r="1267" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1267" s="3"/>
+      <c r="B1267" s="3"/>
+      <c r="C1267" s="3"/>
+      <c r="D1267" s="3"/>
+      <c r="E1267" s="3"/>
+      <c r="F1267" s="3"/>
+      <c r="G1267" s="3"/>
+      <c r="H1267" s="3"/>
+      <c r="I1267" s="4"/>
+      <c r="J1267" s="4"/>
+    </row>
+    <row r="1268" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1268" s="3"/>
+      <c r="B1268" s="3"/>
+      <c r="C1268" s="3"/>
+      <c r="D1268" s="3"/>
+      <c r="E1268" s="3"/>
+      <c r="F1268" s="3"/>
+      <c r="G1268" s="3"/>
+      <c r="H1268" s="3"/>
+      <c r="I1268" s="4"/>
+      <c r="J1268" s="4"/>
+    </row>
+    <row r="1269" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1269" s="3"/>
+      <c r="B1269" s="3"/>
+      <c r="C1269" s="3"/>
+      <c r="D1269" s="3"/>
+      <c r="E1269" s="3"/>
+      <c r="F1269" s="3"/>
+      <c r="G1269" s="3"/>
+      <c r="H1269" s="3"/>
+      <c r="I1269" s="4"/>
+      <c r="J1269" s="4"/>
+    </row>
+    <row r="1270" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1270" s="3"/>
+      <c r="B1270" s="3"/>
+      <c r="C1270" s="3"/>
+      <c r="D1270" s="3"/>
+      <c r="E1270" s="3"/>
+      <c r="F1270" s="3"/>
+      <c r="G1270" s="3"/>
+      <c r="H1270" s="3"/>
+      <c r="I1270" s="4"/>
+      <c r="J1270" s="4"/>
+    </row>
+    <row r="1271" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1271" s="3"/>
+      <c r="B1271" s="3"/>
+      <c r="C1271" s="3"/>
+      <c r="D1271" s="3"/>
+      <c r="E1271" s="3"/>
+      <c r="F1271" s="3"/>
+      <c r="G1271" s="3"/>
+      <c r="H1271" s="3"/>
+      <c r="I1271" s="4"/>
+      <c r="J1271" s="4"/>
+    </row>
+    <row r="1272" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1272" s="3"/>
+      <c r="B1272" s="3"/>
+      <c r="C1272" s="3"/>
+      <c r="D1272" s="3"/>
+      <c r="E1272" s="3"/>
+      <c r="F1272" s="3"/>
+      <c r="G1272" s="3"/>
+      <c r="H1272" s="3"/>
+      <c r="I1272" s="4"/>
+      <c r="J1272" s="4"/>
+    </row>
+    <row r="1273" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1273" s="3"/>
+      <c r="B1273" s="3"/>
+      <c r="C1273" s="3"/>
+      <c r="D1273" s="3"/>
+      <c r="E1273" s="3"/>
+      <c r="F1273" s="3"/>
+      <c r="G1273" s="3"/>
+      <c r="H1273" s="3"/>
+      <c r="I1273" s="4"/>
+      <c r="J1273" s="4"/>
+    </row>
+    <row r="1274" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1274" s="3"/>
+      <c r="B1274" s="3"/>
+      <c r="C1274" s="3"/>
+      <c r="D1274" s="3"/>
+      <c r="E1274" s="3"/>
+      <c r="F1274" s="3"/>
+      <c r="G1274" s="3"/>
+      <c r="H1274" s="3"/>
+      <c r="I1274" s="4"/>
+      <c r="J1274" s="4"/>
+    </row>
+    <row r="1275" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1275" s="3"/>
+      <c r="B1275" s="3"/>
+      <c r="C1275" s="3"/>
+      <c r="D1275" s="3"/>
+      <c r="E1275" s="3"/>
+      <c r="F1275" s="3"/>
+      <c r="G1275" s="3"/>
+      <c r="H1275" s="3"/>
+      <c r="I1275" s="4"/>
+      <c r="J1275" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#37 Time Tracking.xlsx: updated up to 2024-11-11.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9819" uniqueCount="1220">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9944" uniqueCount="1228">
   <si>
     <t>Year</t>
   </si>
@@ -3682,6 +3682,30 @@
   </si>
   <si>
     <t>2024-11-03</t>
+  </si>
+  <si>
+    <t>nwreadinglist v4.0.0</t>
+  </si>
+  <si>
+    <t>2024-11-04</t>
+  </si>
+  <si>
+    <t>2024-11-05</t>
+  </si>
+  <si>
+    <t>nwshared v1.7.0</t>
+  </si>
+  <si>
+    <t>2024-11-07</t>
+  </si>
+  <si>
+    <t>2024-11-08</t>
+  </si>
+  <si>
+    <t>2024-11-10</t>
+  </si>
+  <si>
+    <t>2024-11-11</t>
   </si>
 </sst>
 </file>
@@ -4081,11 +4105,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1275"/>
+  <dimension ref="A1:J1291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1226" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1260" sqref="D1260"/>
+      <pane ySplit="1" topLeftCell="A1253" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1278" sqref="H1278"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -46334,14 +46358,14 @@
         <v>279</v>
       </c>
       <c r="H1257" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I1257" s="4">
-        <f t="shared" ref="I1257:I1258" si="374">YEAR(A1257)</f>
+        <f t="shared" ref="I1257:I1259" si="374">YEAR(A1257)</f>
         <v>2024</v>
       </c>
       <c r="J1257" s="4">
-        <f t="shared" ref="J1257:J1258" si="375">MONTH(A1257)</f>
+        <f t="shared" ref="J1257:J1259" si="375">MONTH(A1257)</f>
         <v>11</v>
       </c>
     </row>
@@ -46368,7 +46392,7 @@
         <v>279</v>
       </c>
       <c r="H1258" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="I1258" s="4">
         <f t="shared" si="374"/>
@@ -46380,196 +46404,542 @@
       </c>
     </row>
     <row r="1259" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1259" s="3"/>
-      <c r="B1259" s="3"/>
-      <c r="C1259" s="3"/>
-      <c r="D1259" s="3"/>
-      <c r="E1259" s="3"/>
+      <c r="A1259" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1259" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1259" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1259" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1259" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1259" s="3"/>
-      <c r="G1259" s="3"/>
-      <c r="H1259" s="3"/>
-      <c r="I1259" s="4"/>
-      <c r="J1259" s="4"/>
+      <c r="G1259" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1259" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1259" s="4">
+        <f t="shared" si="374"/>
+        <v>2024</v>
+      </c>
+      <c r="J1259" s="4">
+        <f t="shared" si="375"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1260" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1260" s="3"/>
-      <c r="B1260" s="3"/>
-      <c r="C1260" s="3"/>
-      <c r="D1260" s="3"/>
-      <c r="E1260" s="3"/>
-      <c r="F1260" s="3"/>
-      <c r="G1260" s="3"/>
-      <c r="H1260" s="3"/>
-      <c r="I1260" s="4"/>
-      <c r="J1260" s="4"/>
+      <c r="A1260" s="3" t="s">
+        <v>1219</v>
+      </c>
+      <c r="B1260" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1260" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1260" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1260" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1260" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1260" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1260" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1260" s="4">
+        <f t="shared" ref="I1260:I1261" si="376">YEAR(A1260)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1260" s="4">
+        <f t="shared" ref="J1260:J1261" si="377">MONTH(A1260)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1261" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1261" s="3"/>
-      <c r="B1261" s="3"/>
-      <c r="C1261" s="3"/>
-      <c r="D1261" s="3"/>
-      <c r="E1261" s="3"/>
+      <c r="A1261" s="3" t="s">
+        <v>1221</v>
+      </c>
+      <c r="B1261" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1261" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1261" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1261" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1261" s="3"/>
-      <c r="G1261" s="3"/>
-      <c r="H1261" s="3"/>
-      <c r="I1261" s="4"/>
-      <c r="J1261" s="4"/>
+      <c r="G1261" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1261" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1261" s="4">
+        <f t="shared" si="376"/>
+        <v>2024</v>
+      </c>
+      <c r="J1261" s="4">
+        <f t="shared" si="377"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1262" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1262" s="3"/>
-      <c r="B1262" s="3"/>
-      <c r="C1262" s="3"/>
-      <c r="D1262" s="3"/>
-      <c r="E1262" s="3"/>
+      <c r="A1262" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B1262" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1262" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1262" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1262" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1262" s="3"/>
-      <c r="G1262" s="3"/>
-      <c r="H1262" s="3"/>
-      <c r="I1262" s="4"/>
-      <c r="J1262" s="4"/>
+      <c r="G1262" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1262" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1262" s="4">
+        <f t="shared" ref="I1262:I1265" si="378">YEAR(A1262)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1262" s="4">
+        <f t="shared" ref="J1262:J1265" si="379">MONTH(A1262)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1263" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1263" s="3"/>
-      <c r="B1263" s="3"/>
-      <c r="C1263" s="3"/>
-      <c r="D1263" s="3"/>
-      <c r="E1263" s="3"/>
-      <c r="F1263" s="3"/>
-      <c r="G1263" s="3"/>
-      <c r="H1263" s="3"/>
-      <c r="I1263" s="4"/>
-      <c r="J1263" s="4"/>
+      <c r="A1263" s="3" t="s">
+        <v>1222</v>
+      </c>
+      <c r="B1263" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1263" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1263" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1263" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1263" s="3" t="s">
+        <v>1223</v>
+      </c>
+      <c r="G1263" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1263" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1263" s="4">
+        <f t="shared" si="378"/>
+        <v>2024</v>
+      </c>
+      <c r="J1263" s="4">
+        <f t="shared" si="379"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1264" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1264" s="3"/>
-      <c r="B1264" s="3"/>
-      <c r="C1264" s="3"/>
-      <c r="D1264" s="3"/>
-      <c r="E1264" s="3"/>
-      <c r="F1264" s="3"/>
-      <c r="G1264" s="3"/>
-      <c r="H1264" s="3"/>
-      <c r="I1264" s="4"/>
-      <c r="J1264" s="4"/>
+      <c r="A1264" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B1264" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1264" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1264" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1264" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1264" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1264" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1264" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1264" s="4">
+        <f t="shared" si="378"/>
+        <v>2024</v>
+      </c>
+      <c r="J1264" s="4">
+        <f t="shared" si="379"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1265" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1265" s="3"/>
-      <c r="B1265" s="3"/>
-      <c r="C1265" s="3"/>
-      <c r="D1265" s="3"/>
-      <c r="E1265" s="3"/>
-      <c r="F1265" s="3"/>
-      <c r="G1265" s="3"/>
-      <c r="H1265" s="3"/>
-      <c r="I1265" s="4"/>
-      <c r="J1265" s="4"/>
+      <c r="A1265" s="3" t="s">
+        <v>1224</v>
+      </c>
+      <c r="B1265" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1265" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1265" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1265" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1265" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1265" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1265" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1265" s="4">
+        <f t="shared" si="378"/>
+        <v>2024</v>
+      </c>
+      <c r="J1265" s="4">
+        <f t="shared" si="379"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1266" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1266" s="3"/>
-      <c r="B1266" s="3"/>
-      <c r="C1266" s="3"/>
-      <c r="D1266" s="3"/>
-      <c r="E1266" s="3"/>
-      <c r="F1266" s="3"/>
-      <c r="G1266" s="3"/>
-      <c r="H1266" s="3"/>
-      <c r="I1266" s="4"/>
-      <c r="J1266" s="4"/>
+      <c r="A1266" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B1266" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1266" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1266" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1266" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1266" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1266" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1266" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1266" s="4">
+        <f t="shared" ref="I1266" si="380">YEAR(A1266)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1266" s="4">
+        <f t="shared" ref="J1266" si="381">MONTH(A1266)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1267" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1267" s="3"/>
-      <c r="B1267" s="3"/>
-      <c r="C1267" s="3"/>
-      <c r="D1267" s="3"/>
-      <c r="E1267" s="3"/>
-      <c r="F1267" s="3"/>
-      <c r="G1267" s="3"/>
-      <c r="H1267" s="3"/>
-      <c r="I1267" s="4"/>
-      <c r="J1267" s="4"/>
+      <c r="A1267" s="3" t="s">
+        <v>1225</v>
+      </c>
+      <c r="B1267" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1267" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1267" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1267" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1267" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1267" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1267" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1267" s="4">
+        <f t="shared" ref="I1267:I1270" si="382">YEAR(A1267)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1267" s="4">
+        <f t="shared" ref="J1267:J1270" si="383">MONTH(A1267)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1268" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1268" s="3"/>
-      <c r="B1268" s="3"/>
-      <c r="C1268" s="3"/>
-      <c r="D1268" s="3"/>
-      <c r="E1268" s="3"/>
-      <c r="F1268" s="3"/>
-      <c r="G1268" s="3"/>
-      <c r="H1268" s="3"/>
-      <c r="I1268" s="4"/>
-      <c r="J1268" s="4"/>
+      <c r="A1268" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1268" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1268" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1268" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1268" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1268" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1268" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1268" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1268" s="4">
+        <f t="shared" si="382"/>
+        <v>2024</v>
+      </c>
+      <c r="J1268" s="4">
+        <f t="shared" si="383"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1269" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1269" s="3"/>
-      <c r="B1269" s="3"/>
-      <c r="C1269" s="3"/>
-      <c r="D1269" s="3"/>
-      <c r="E1269" s="3"/>
-      <c r="F1269" s="3"/>
-      <c r="G1269" s="3"/>
-      <c r="H1269" s="3"/>
-      <c r="I1269" s="4"/>
-      <c r="J1269" s="4"/>
+      <c r="A1269" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1269" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1269" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1269" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1269" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1269" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1269" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1269" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1269" s="4">
+        <f t="shared" si="382"/>
+        <v>2024</v>
+      </c>
+      <c r="J1269" s="4">
+        <f t="shared" si="383"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1270" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1270" s="3"/>
-      <c r="B1270" s="3"/>
-      <c r="C1270" s="3"/>
-      <c r="D1270" s="3"/>
-      <c r="E1270" s="3"/>
-      <c r="F1270" s="3"/>
-      <c r="G1270" s="3"/>
-      <c r="H1270" s="3"/>
-      <c r="I1270" s="4"/>
-      <c r="J1270" s="4"/>
+      <c r="A1270" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1270" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1270" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1270" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1270" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1270" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1270" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1270" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1270" s="4">
+        <f t="shared" si="382"/>
+        <v>2024</v>
+      </c>
+      <c r="J1270" s="4">
+        <f t="shared" si="383"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1271" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1271" s="3"/>
-      <c r="B1271" s="3"/>
-      <c r="C1271" s="3"/>
-      <c r="D1271" s="3"/>
-      <c r="E1271" s="3"/>
-      <c r="F1271" s="3"/>
-      <c r="G1271" s="3"/>
-      <c r="H1271" s="3"/>
-      <c r="I1271" s="4"/>
-      <c r="J1271" s="4"/>
+      <c r="A1271" s="3" t="s">
+        <v>1226</v>
+      </c>
+      <c r="B1271" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1271" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1271" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1271" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1271" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1271" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1271" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1271" s="4">
+        <f t="shared" ref="I1271:I1273" si="384">YEAR(A1271)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1271" s="4">
+        <f t="shared" ref="J1271:J1273" si="385">MONTH(A1271)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1272" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1272" s="3"/>
-      <c r="B1272" s="3"/>
-      <c r="C1272" s="3"/>
-      <c r="D1272" s="3"/>
-      <c r="E1272" s="3"/>
-      <c r="F1272" s="3"/>
-      <c r="G1272" s="3"/>
-      <c r="H1272" s="3"/>
-      <c r="I1272" s="4"/>
-      <c r="J1272" s="4"/>
+      <c r="A1272" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B1272" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1272" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1272" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1272" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1272" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1272" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1272" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1272" s="4">
+        <f t="shared" si="384"/>
+        <v>2024</v>
+      </c>
+      <c r="J1272" s="4">
+        <f t="shared" si="385"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1273" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1273" s="3"/>
-      <c r="B1273" s="3"/>
-      <c r="C1273" s="3"/>
-      <c r="D1273" s="3"/>
-      <c r="E1273" s="3"/>
-      <c r="F1273" s="3"/>
-      <c r="G1273" s="3"/>
-      <c r="H1273" s="3"/>
-      <c r="I1273" s="4"/>
-      <c r="J1273" s="4"/>
+      <c r="A1273" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B1273" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1273" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1273" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1273" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1273" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1273" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1273" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1273" s="4">
+        <f t="shared" si="384"/>
+        <v>2024</v>
+      </c>
+      <c r="J1273" s="4">
+        <f t="shared" si="385"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1274" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1274" s="3"/>
-      <c r="B1274" s="3"/>
-      <c r="C1274" s="3"/>
-      <c r="D1274" s="3"/>
-      <c r="E1274" s="3"/>
-      <c r="F1274" s="3"/>
-      <c r="G1274" s="3"/>
-      <c r="H1274" s="3"/>
-      <c r="I1274" s="4"/>
-      <c r="J1274" s="4"/>
+      <c r="A1274" s="3" t="s">
+        <v>1227</v>
+      </c>
+      <c r="B1274" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1274" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1274" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1274" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1274" s="3" t="s">
+        <v>1220</v>
+      </c>
+      <c r="G1274" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1274" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1274" s="4">
+        <f t="shared" ref="I1274" si="386">YEAR(A1274)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1274" s="4">
+        <f t="shared" ref="J1274" si="387">MONTH(A1274)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1275" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1275" s="3"/>
@@ -46583,6 +46953,198 @@
       <c r="I1275" s="4"/>
       <c r="J1275" s="4"/>
     </row>
+    <row r="1276" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1276" s="3"/>
+      <c r="B1276" s="3"/>
+      <c r="C1276" s="3"/>
+      <c r="D1276" s="3"/>
+      <c r="E1276" s="3"/>
+      <c r="F1276" s="3"/>
+      <c r="G1276" s="3"/>
+      <c r="H1276" s="3"/>
+      <c r="I1276" s="4"/>
+      <c r="J1276" s="4"/>
+    </row>
+    <row r="1277" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1277" s="3"/>
+      <c r="B1277" s="3"/>
+      <c r="C1277" s="3"/>
+      <c r="D1277" s="3"/>
+      <c r="E1277" s="3"/>
+      <c r="F1277" s="3"/>
+      <c r="G1277" s="3"/>
+      <c r="H1277" s="3"/>
+      <c r="I1277" s="4"/>
+      <c r="J1277" s="4"/>
+    </row>
+    <row r="1278" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1278" s="3"/>
+      <c r="B1278" s="3"/>
+      <c r="C1278" s="3"/>
+      <c r="D1278" s="3"/>
+      <c r="E1278" s="3"/>
+      <c r="F1278" s="3"/>
+      <c r="G1278" s="3"/>
+      <c r="H1278" s="3"/>
+      <c r="I1278" s="4"/>
+      <c r="J1278" s="4"/>
+    </row>
+    <row r="1279" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1279" s="3"/>
+      <c r="B1279" s="3"/>
+      <c r="C1279" s="3"/>
+      <c r="D1279" s="3"/>
+      <c r="E1279" s="3"/>
+      <c r="F1279" s="3"/>
+      <c r="G1279" s="3"/>
+      <c r="H1279" s="3"/>
+      <c r="I1279" s="4"/>
+      <c r="J1279" s="4"/>
+    </row>
+    <row r="1280" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1280" s="3"/>
+      <c r="B1280" s="3"/>
+      <c r="C1280" s="3"/>
+      <c r="D1280" s="3"/>
+      <c r="E1280" s="3"/>
+      <c r="F1280" s="3"/>
+      <c r="G1280" s="3"/>
+      <c r="H1280" s="3"/>
+      <c r="I1280" s="4"/>
+      <c r="J1280" s="4"/>
+    </row>
+    <row r="1281" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1281" s="3"/>
+      <c r="B1281" s="3"/>
+      <c r="C1281" s="3"/>
+      <c r="D1281" s="3"/>
+      <c r="E1281" s="3"/>
+      <c r="F1281" s="3"/>
+      <c r="G1281" s="3"/>
+      <c r="H1281" s="3"/>
+      <c r="I1281" s="4"/>
+      <c r="J1281" s="4"/>
+    </row>
+    <row r="1282" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1282" s="3"/>
+      <c r="B1282" s="3"/>
+      <c r="C1282" s="3"/>
+      <c r="D1282" s="3"/>
+      <c r="E1282" s="3"/>
+      <c r="F1282" s="3"/>
+      <c r="G1282" s="3"/>
+      <c r="H1282" s="3"/>
+      <c r="I1282" s="4"/>
+      <c r="J1282" s="4"/>
+    </row>
+    <row r="1283" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1283" s="3"/>
+      <c r="B1283" s="3"/>
+      <c r="C1283" s="3"/>
+      <c r="D1283" s="3"/>
+      <c r="E1283" s="3"/>
+      <c r="F1283" s="3"/>
+      <c r="G1283" s="3"/>
+      <c r="H1283" s="3"/>
+      <c r="I1283" s="4"/>
+      <c r="J1283" s="4"/>
+    </row>
+    <row r="1284" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1284" s="3"/>
+      <c r="B1284" s="3"/>
+      <c r="C1284" s="3"/>
+      <c r="D1284" s="3"/>
+      <c r="E1284" s="3"/>
+      <c r="F1284" s="3"/>
+      <c r="G1284" s="3"/>
+      <c r="H1284" s="3"/>
+      <c r="I1284" s="4"/>
+      <c r="J1284" s="4"/>
+    </row>
+    <row r="1285" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1285" s="3"/>
+      <c r="B1285" s="3"/>
+      <c r="C1285" s="3"/>
+      <c r="D1285" s="3"/>
+      <c r="E1285" s="3"/>
+      <c r="F1285" s="3"/>
+      <c r="G1285" s="3"/>
+      <c r="H1285" s="3"/>
+      <c r="I1285" s="4"/>
+      <c r="J1285" s="4"/>
+    </row>
+    <row r="1286" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1286" s="3"/>
+      <c r="B1286" s="3"/>
+      <c r="C1286" s="3"/>
+      <c r="D1286" s="3"/>
+      <c r="E1286" s="3"/>
+      <c r="F1286" s="3"/>
+      <c r="G1286" s="3"/>
+      <c r="H1286" s="3"/>
+      <c r="I1286" s="4"/>
+      <c r="J1286" s="4"/>
+    </row>
+    <row r="1287" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1287" s="3"/>
+      <c r="B1287" s="3"/>
+      <c r="C1287" s="3"/>
+      <c r="D1287" s="3"/>
+      <c r="E1287" s="3"/>
+      <c r="F1287" s="3"/>
+      <c r="G1287" s="3"/>
+      <c r="H1287" s="3"/>
+      <c r="I1287" s="4"/>
+      <c r="J1287" s="4"/>
+    </row>
+    <row r="1288" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1288" s="3"/>
+      <c r="B1288" s="3"/>
+      <c r="C1288" s="3"/>
+      <c r="D1288" s="3"/>
+      <c r="E1288" s="3"/>
+      <c r="F1288" s="3"/>
+      <c r="G1288" s="3"/>
+      <c r="H1288" s="3"/>
+      <c r="I1288" s="4"/>
+      <c r="J1288" s="4"/>
+    </row>
+    <row r="1289" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1289" s="3"/>
+      <c r="B1289" s="3"/>
+      <c r="C1289" s="3"/>
+      <c r="D1289" s="3"/>
+      <c r="E1289" s="3"/>
+      <c r="F1289" s="3"/>
+      <c r="G1289" s="3"/>
+      <c r="H1289" s="3"/>
+      <c r="I1289" s="4"/>
+      <c r="J1289" s="4"/>
+    </row>
+    <row r="1290" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1290" s="3"/>
+      <c r="B1290" s="3"/>
+      <c r="C1290" s="3"/>
+      <c r="D1290" s="3"/>
+      <c r="E1290" s="3"/>
+      <c r="F1290" s="3"/>
+      <c r="G1290" s="3"/>
+      <c r="H1290" s="3"/>
+      <c r="I1290" s="4"/>
+      <c r="J1290" s="4"/>
+    </row>
+    <row r="1291" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1291" s="3"/>
+      <c r="B1291" s="3"/>
+      <c r="C1291" s="3"/>
+      <c r="D1291" s="3"/>
+      <c r="E1291" s="3"/>
+      <c r="F1291" s="3"/>
+      <c r="G1291" s="3"/>
+      <c r="H1291" s="3"/>
+      <c r="I1291" s="4"/>
+      <c r="J1291" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#37 Time Tracking.xlsx: updated up to 2024-11-18.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9944" uniqueCount="1228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9993" uniqueCount="1232">
   <si>
     <t>Year</t>
   </si>
@@ -3706,6 +3706,18 @@
   </si>
   <si>
     <t>2024-11-11</t>
+  </si>
+  <si>
+    <t>2024-11-12</t>
+  </si>
+  <si>
+    <t>2024-11-14</t>
+  </si>
+  <si>
+    <t>2024-11-17</t>
+  </si>
+  <si>
+    <t>2024-11-18</t>
   </si>
 </sst>
 </file>
@@ -4109,7 +4121,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1278" sqref="H1278"/>
+      <selection pane="bottomLeft" activeCell="D1283" sqref="D1283"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -46933,97 +46945,237 @@
         <v>279</v>
       </c>
       <c r="I1274" s="4">
-        <f t="shared" ref="I1274" si="386">YEAR(A1274)</f>
+        <f t="shared" ref="I1274:I1276" si="386">YEAR(A1274)</f>
         <v>2024</v>
       </c>
       <c r="J1274" s="4">
-        <f t="shared" ref="J1274" si="387">MONTH(A1274)</f>
+        <f t="shared" ref="J1274:J1276" si="387">MONTH(A1274)</f>
         <v>11</v>
       </c>
     </row>
     <row r="1275" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1275" s="3"/>
-      <c r="B1275" s="3"/>
-      <c r="C1275" s="3"/>
-      <c r="D1275" s="3"/>
-      <c r="E1275" s="3"/>
+      <c r="A1275" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B1275" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1275" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1275" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1275" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1275" s="3"/>
-      <c r="G1275" s="3"/>
-      <c r="H1275" s="3"/>
-      <c r="I1275" s="4"/>
-      <c r="J1275" s="4"/>
+      <c r="G1275" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1275" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1275" s="4">
+        <f t="shared" si="386"/>
+        <v>2024</v>
+      </c>
+      <c r="J1275" s="4">
+        <f t="shared" si="387"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1276" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1276" s="3"/>
-      <c r="B1276" s="3"/>
-      <c r="C1276" s="3"/>
-      <c r="D1276" s="3"/>
-      <c r="E1276" s="3"/>
+      <c r="A1276" s="3" t="s">
+        <v>1228</v>
+      </c>
+      <c r="B1276" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1276" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1276" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1276" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1276" s="3"/>
-      <c r="G1276" s="3"/>
-      <c r="H1276" s="3"/>
-      <c r="I1276" s="4"/>
-      <c r="J1276" s="4"/>
+      <c r="G1276" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1276" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1276" s="4">
+        <f t="shared" si="386"/>
+        <v>2024</v>
+      </c>
+      <c r="J1276" s="4">
+        <f t="shared" si="387"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1277" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1277" s="3"/>
-      <c r="B1277" s="3"/>
-      <c r="C1277" s="3"/>
-      <c r="D1277" s="3"/>
-      <c r="E1277" s="3"/>
+      <c r="A1277" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B1277" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1277" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1277" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1277" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1277" s="3"/>
-      <c r="G1277" s="3"/>
-      <c r="H1277" s="3"/>
-      <c r="I1277" s="4"/>
-      <c r="J1277" s="4"/>
+      <c r="G1277" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1277" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1277" s="4">
+        <f t="shared" ref="I1277:I1278" si="388">YEAR(A1277)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1277" s="4">
+        <f t="shared" ref="J1277:J1278" si="389">MONTH(A1277)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1278" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1278" s="3"/>
-      <c r="B1278" s="3"/>
-      <c r="C1278" s="3"/>
-      <c r="D1278" s="3"/>
-      <c r="E1278" s="3"/>
+      <c r="A1278" s="3" t="s">
+        <v>1229</v>
+      </c>
+      <c r="B1278" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1278" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1278" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1278" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1278" s="3"/>
-      <c r="G1278" s="3"/>
-      <c r="H1278" s="3"/>
-      <c r="I1278" s="4"/>
-      <c r="J1278" s="4"/>
+      <c r="G1278" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1278" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1278" s="4">
+        <f t="shared" si="388"/>
+        <v>2024</v>
+      </c>
+      <c r="J1278" s="4">
+        <f t="shared" si="389"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1279" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1279" s="3"/>
-      <c r="B1279" s="3"/>
-      <c r="C1279" s="3"/>
-      <c r="D1279" s="3"/>
-      <c r="E1279" s="3"/>
+      <c r="A1279" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B1279" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1279" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1279" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1279" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1279" s="3"/>
-      <c r="G1279" s="3"/>
-      <c r="H1279" s="3"/>
-      <c r="I1279" s="4"/>
-      <c r="J1279" s="4"/>
+      <c r="G1279" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1279" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1279" s="4">
+        <f t="shared" ref="I1279:I1280" si="390">YEAR(A1279)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1279" s="4">
+        <f t="shared" ref="J1279:J1280" si="391">MONTH(A1279)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1280" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1280" s="3"/>
-      <c r="B1280" s="3"/>
-      <c r="C1280" s="3"/>
-      <c r="D1280" s="3"/>
-      <c r="E1280" s="3"/>
+      <c r="A1280" s="3" t="s">
+        <v>1230</v>
+      </c>
+      <c r="B1280" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1280" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1280" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1280" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1280" s="3"/>
-      <c r="G1280" s="3"/>
-      <c r="H1280" s="3"/>
-      <c r="I1280" s="4"/>
-      <c r="J1280" s="4"/>
+      <c r="G1280" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1280" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1280" s="4">
+        <f t="shared" si="390"/>
+        <v>2024</v>
+      </c>
+      <c r="J1280" s="4">
+        <f t="shared" si="391"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1281" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1281" s="3"/>
-      <c r="B1281" s="3"/>
-      <c r="C1281" s="3"/>
-      <c r="D1281" s="3"/>
-      <c r="E1281" s="3"/>
+      <c r="A1281" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B1281" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1281" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1281" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1281" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1281" s="3"/>
-      <c r="G1281" s="3"/>
-      <c r="H1281" s="3"/>
-      <c r="I1281" s="4"/>
-      <c r="J1281" s="4"/>
+      <c r="G1281" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1281" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1281" s="4">
+        <f t="shared" ref="I1281" si="392">YEAR(A1281)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1281" s="4">
+        <f t="shared" ref="J1281" si="393">MONTH(A1281)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1282" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1282" s="3"/>

</xml_diff>

<commit_message>
#37 Time Tracking.xlsx: updated up to 2024-11-19.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9993" uniqueCount="1232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10014" uniqueCount="1233">
   <si>
     <t>Year</t>
   </si>
@@ -3718,6 +3718,9 @@
   </si>
   <si>
     <t>2024-11-18</t>
+  </si>
+  <si>
+    <t>2024-11-19</t>
   </si>
 </sst>
 </file>
@@ -4120,8 +4123,8 @@
   <dimension ref="A1:J1291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1253" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1283" sqref="D1283"/>
+      <pane ySplit="1" topLeftCell="A1259" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1286" sqref="C1286"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47178,40 +47181,100 @@
       </c>
     </row>
     <row r="1282" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1282" s="3"/>
-      <c r="B1282" s="3"/>
-      <c r="C1282" s="3"/>
-      <c r="D1282" s="3"/>
-      <c r="E1282" s="3"/>
+      <c r="A1282" s="3" t="s">
+        <v>1231</v>
+      </c>
+      <c r="B1282" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1282" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1282" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1282" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1282" s="3"/>
-      <c r="G1282" s="3"/>
-      <c r="H1282" s="3"/>
-      <c r="I1282" s="4"/>
-      <c r="J1282" s="4"/>
+      <c r="G1282" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1282" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1282" s="4">
+        <f t="shared" ref="I1282:I1283" si="394">YEAR(A1282)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1282" s="4">
+        <f t="shared" ref="J1282:J1283" si="395">MONTH(A1282)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1283" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1283" s="3"/>
-      <c r="B1283" s="3"/>
-      <c r="C1283" s="3"/>
-      <c r="D1283" s="3"/>
-      <c r="E1283" s="3"/>
+      <c r="A1283" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B1283" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1283" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="D1283" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E1283" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1283" s="3"/>
-      <c r="G1283" s="3"/>
-      <c r="H1283" s="3"/>
-      <c r="I1283" s="4"/>
-      <c r="J1283" s="4"/>
+      <c r="G1283" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1283" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1283" s="4">
+        <f t="shared" si="394"/>
+        <v>2024</v>
+      </c>
+      <c r="J1283" s="4">
+        <f t="shared" si="395"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1284" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1284" s="3"/>
-      <c r="B1284" s="3"/>
-      <c r="C1284" s="3"/>
-      <c r="D1284" s="3"/>
-      <c r="E1284" s="3"/>
+      <c r="A1284" s="3" t="s">
+        <v>1232</v>
+      </c>
+      <c r="B1284" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1284" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1284" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1284" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1284" s="3"/>
-      <c r="G1284" s="3"/>
-      <c r="H1284" s="3"/>
-      <c r="I1284" s="4"/>
-      <c r="J1284" s="4"/>
+      <c r="G1284" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1284" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1284" s="4">
+        <f t="shared" ref="I1284" si="396">YEAR(A1284)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1284" s="4">
+        <f t="shared" ref="J1284" si="397">MONTH(A1284)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1285" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1285" s="3"/>

</xml_diff>

<commit_message>
#37 Time Tracking.xlsx: updated up to 2024-11-27.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10014" uniqueCount="1233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10042" uniqueCount="1234">
   <si>
     <t>Year</t>
   </si>
@@ -3721,6 +3721,9 @@
   </si>
   <si>
     <t>2024-11-19</t>
+  </si>
+  <si>
+    <t>2024-11-24</t>
   </si>
 </sst>
 </file>
@@ -4120,11 +4123,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1291"/>
+  <dimension ref="A1:J1307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1259" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1286" sqref="C1286"/>
+      <selection pane="bottomLeft" activeCell="F1293" sqref="F1293"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47268,61 +47271,141 @@
         <v>280</v>
       </c>
       <c r="I1284" s="4">
-        <f t="shared" ref="I1284" si="396">YEAR(A1284)</f>
+        <f t="shared" ref="I1284:I1285" si="396">YEAR(A1284)</f>
         <v>2024</v>
       </c>
       <c r="J1284" s="4">
-        <f t="shared" ref="J1284" si="397">MONTH(A1284)</f>
+        <f t="shared" ref="J1284:J1285" si="397">MONTH(A1284)</f>
         <v>11</v>
       </c>
     </row>
     <row r="1285" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1285" s="3"/>
-      <c r="B1285" s="3"/>
-      <c r="C1285" s="3"/>
-      <c r="D1285" s="3"/>
-      <c r="E1285" s="3"/>
+      <c r="A1285" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1285" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1285" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1285" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1285" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1285" s="3"/>
-      <c r="G1285" s="3"/>
-      <c r="H1285" s="3"/>
-      <c r="I1285" s="4"/>
-      <c r="J1285" s="4"/>
+      <c r="G1285" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1285" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1285" s="4">
+        <f t="shared" si="396"/>
+        <v>2024</v>
+      </c>
+      <c r="J1285" s="4">
+        <f t="shared" si="397"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1286" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1286" s="3"/>
-      <c r="B1286" s="3"/>
-      <c r="C1286" s="3"/>
-      <c r="D1286" s="3"/>
-      <c r="E1286" s="3"/>
+      <c r="A1286" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1286" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1286" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1286" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1286" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1286" s="3"/>
-      <c r="G1286" s="3"/>
-      <c r="H1286" s="3"/>
-      <c r="I1286" s="4"/>
-      <c r="J1286" s="4"/>
+      <c r="G1286" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1286" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1286" s="4">
+        <f t="shared" ref="I1286:I1288" si="398">YEAR(A1286)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1286" s="4">
+        <f t="shared" ref="J1286:J1288" si="399">MONTH(A1286)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1287" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1287" s="3"/>
-      <c r="B1287" s="3"/>
-      <c r="C1287" s="3"/>
-      <c r="D1287" s="3"/>
-      <c r="E1287" s="3"/>
+      <c r="A1287" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1287" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1287" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1287" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1287" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1287" s="3"/>
-      <c r="G1287" s="3"/>
-      <c r="H1287" s="3"/>
-      <c r="I1287" s="4"/>
-      <c r="J1287" s="4"/>
+      <c r="G1287" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1287" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1287" s="4">
+        <f t="shared" si="398"/>
+        <v>2024</v>
+      </c>
+      <c r="J1287" s="4">
+        <f t="shared" si="399"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1288" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1288" s="3"/>
-      <c r="B1288" s="3"/>
-      <c r="C1288" s="3"/>
-      <c r="D1288" s="3"/>
-      <c r="E1288" s="3"/>
+      <c r="A1288" s="3" t="s">
+        <v>1233</v>
+      </c>
+      <c r="B1288" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1288" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1288" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1288" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1288" s="3"/>
-      <c r="G1288" s="3"/>
-      <c r="H1288" s="3"/>
-      <c r="I1288" s="4"/>
-      <c r="J1288" s="4"/>
+      <c r="G1288" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1288" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1288" s="4">
+        <f t="shared" si="398"/>
+        <v>2024</v>
+      </c>
+      <c r="J1288" s="4">
+        <f t="shared" si="399"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1289" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1289" s="3"/>
@@ -47360,6 +47443,198 @@
       <c r="I1291" s="4"/>
       <c r="J1291" s="4"/>
     </row>
+    <row r="1292" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1292" s="3"/>
+      <c r="B1292" s="3"/>
+      <c r="C1292" s="3"/>
+      <c r="D1292" s="3"/>
+      <c r="E1292" s="3"/>
+      <c r="F1292" s="3"/>
+      <c r="G1292" s="3"/>
+      <c r="H1292" s="3"/>
+      <c r="I1292" s="4"/>
+      <c r="J1292" s="4"/>
+    </row>
+    <row r="1293" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1293" s="3"/>
+      <c r="B1293" s="3"/>
+      <c r="C1293" s="3"/>
+      <c r="D1293" s="3"/>
+      <c r="E1293" s="3"/>
+      <c r="F1293" s="3"/>
+      <c r="G1293" s="3"/>
+      <c r="H1293" s="3"/>
+      <c r="I1293" s="4"/>
+      <c r="J1293" s="4"/>
+    </row>
+    <row r="1294" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1294" s="3"/>
+      <c r="B1294" s="3"/>
+      <c r="C1294" s="3"/>
+      <c r="D1294" s="3"/>
+      <c r="E1294" s="3"/>
+      <c r="F1294" s="3"/>
+      <c r="G1294" s="3"/>
+      <c r="H1294" s="3"/>
+      <c r="I1294" s="4"/>
+      <c r="J1294" s="4"/>
+    </row>
+    <row r="1295" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1295" s="3"/>
+      <c r="B1295" s="3"/>
+      <c r="C1295" s="3"/>
+      <c r="D1295" s="3"/>
+      <c r="E1295" s="3"/>
+      <c r="F1295" s="3"/>
+      <c r="G1295" s="3"/>
+      <c r="H1295" s="3"/>
+      <c r="I1295" s="4"/>
+      <c r="J1295" s="4"/>
+    </row>
+    <row r="1296" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1296" s="3"/>
+      <c r="B1296" s="3"/>
+      <c r="C1296" s="3"/>
+      <c r="D1296" s="3"/>
+      <c r="E1296" s="3"/>
+      <c r="F1296" s="3"/>
+      <c r="G1296" s="3"/>
+      <c r="H1296" s="3"/>
+      <c r="I1296" s="4"/>
+      <c r="J1296" s="4"/>
+    </row>
+    <row r="1297" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1297" s="3"/>
+      <c r="B1297" s="3"/>
+      <c r="C1297" s="3"/>
+      <c r="D1297" s="3"/>
+      <c r="E1297" s="3"/>
+      <c r="F1297" s="3"/>
+      <c r="G1297" s="3"/>
+      <c r="H1297" s="3"/>
+      <c r="I1297" s="4"/>
+      <c r="J1297" s="4"/>
+    </row>
+    <row r="1298" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1298" s="3"/>
+      <c r="B1298" s="3"/>
+      <c r="C1298" s="3"/>
+      <c r="D1298" s="3"/>
+      <c r="E1298" s="3"/>
+      <c r="F1298" s="3"/>
+      <c r="G1298" s="3"/>
+      <c r="H1298" s="3"/>
+      <c r="I1298" s="4"/>
+      <c r="J1298" s="4"/>
+    </row>
+    <row r="1299" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1299" s="3"/>
+      <c r="B1299" s="3"/>
+      <c r="C1299" s="3"/>
+      <c r="D1299" s="3"/>
+      <c r="E1299" s="3"/>
+      <c r="F1299" s="3"/>
+      <c r="G1299" s="3"/>
+      <c r="H1299" s="3"/>
+      <c r="I1299" s="4"/>
+      <c r="J1299" s="4"/>
+    </row>
+    <row r="1300" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1300" s="3"/>
+      <c r="B1300" s="3"/>
+      <c r="C1300" s="3"/>
+      <c r="D1300" s="3"/>
+      <c r="E1300" s="3"/>
+      <c r="F1300" s="3"/>
+      <c r="G1300" s="3"/>
+      <c r="H1300" s="3"/>
+      <c r="I1300" s="4"/>
+      <c r="J1300" s="4"/>
+    </row>
+    <row r="1301" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1301" s="3"/>
+      <c r="B1301" s="3"/>
+      <c r="C1301" s="3"/>
+      <c r="D1301" s="3"/>
+      <c r="E1301" s="3"/>
+      <c r="F1301" s="3"/>
+      <c r="G1301" s="3"/>
+      <c r="H1301" s="3"/>
+      <c r="I1301" s="4"/>
+      <c r="J1301" s="4"/>
+    </row>
+    <row r="1302" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1302" s="3"/>
+      <c r="B1302" s="3"/>
+      <c r="C1302" s="3"/>
+      <c r="D1302" s="3"/>
+      <c r="E1302" s="3"/>
+      <c r="F1302" s="3"/>
+      <c r="G1302" s="3"/>
+      <c r="H1302" s="3"/>
+      <c r="I1302" s="4"/>
+      <c r="J1302" s="4"/>
+    </row>
+    <row r="1303" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1303" s="3"/>
+      <c r="B1303" s="3"/>
+      <c r="C1303" s="3"/>
+      <c r="D1303" s="3"/>
+      <c r="E1303" s="3"/>
+      <c r="F1303" s="3"/>
+      <c r="G1303" s="3"/>
+      <c r="H1303" s="3"/>
+      <c r="I1303" s="4"/>
+      <c r="J1303" s="4"/>
+    </row>
+    <row r="1304" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1304" s="3"/>
+      <c r="B1304" s="3"/>
+      <c r="C1304" s="3"/>
+      <c r="D1304" s="3"/>
+      <c r="E1304" s="3"/>
+      <c r="F1304" s="3"/>
+      <c r="G1304" s="3"/>
+      <c r="H1304" s="3"/>
+      <c r="I1304" s="4"/>
+      <c r="J1304" s="4"/>
+    </row>
+    <row r="1305" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1305" s="3"/>
+      <c r="B1305" s="3"/>
+      <c r="C1305" s="3"/>
+      <c r="D1305" s="3"/>
+      <c r="E1305" s="3"/>
+      <c r="F1305" s="3"/>
+      <c r="G1305" s="3"/>
+      <c r="H1305" s="3"/>
+      <c r="I1305" s="4"/>
+      <c r="J1305" s="4"/>
+    </row>
+    <row r="1306" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1306" s="3"/>
+      <c r="B1306" s="3"/>
+      <c r="C1306" s="3"/>
+      <c r="D1306" s="3"/>
+      <c r="E1306" s="3"/>
+      <c r="F1306" s="3"/>
+      <c r="G1306" s="3"/>
+      <c r="H1306" s="3"/>
+      <c r="I1306" s="4"/>
+      <c r="J1306" s="4"/>
+    </row>
+    <row r="1307" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1307" s="3"/>
+      <c r="B1307" s="3"/>
+      <c r="C1307" s="3"/>
+      <c r="D1307" s="3"/>
+      <c r="E1307" s="3"/>
+      <c r="F1307" s="3"/>
+      <c r="G1307" s="3"/>
+      <c r="H1307" s="3"/>
+      <c r="I1307" s="4"/>
+      <c r="J1307" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#37 Time Tracking.xlsx: updated up to 2024-11-29.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10042" uniqueCount="1234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10090" uniqueCount="1239">
   <si>
     <t>Year</t>
   </si>
@@ -3724,6 +3724,21 @@
   </si>
   <si>
     <t>2024-11-24</t>
+  </si>
+  <si>
+    <t>2024-11-26</t>
+  </si>
+  <si>
+    <t>nwshared v1.7.1</t>
+  </si>
+  <si>
+    <t>nwshared v1.8.0</t>
+  </si>
+  <si>
+    <t>2024-11-28</t>
+  </si>
+  <si>
+    <t>2024-11-29</t>
   </si>
 </sst>
 </file>
@@ -4126,8 +4141,8 @@
   <dimension ref="A1:J1307"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1259" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1293" sqref="F1293"/>
+      <pane ySplit="1" topLeftCell="A1271" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1289" sqref="F1289"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47335,11 +47350,11 @@
         <v>280</v>
       </c>
       <c r="I1286" s="4">
-        <f t="shared" ref="I1286:I1288" si="398">YEAR(A1286)</f>
+        <f t="shared" ref="I1286:I1289" si="398">YEAR(A1286)</f>
         <v>2024</v>
       </c>
       <c r="J1286" s="4">
-        <f t="shared" ref="J1286:J1288" si="399">MONTH(A1286)</f>
+        <f t="shared" ref="J1286:J1289" si="399">MONTH(A1286)</f>
         <v>11</v>
       </c>
     </row>
@@ -47408,76 +47423,208 @@
       </c>
     </row>
     <row r="1289" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1289" s="3"/>
-      <c r="B1289" s="3"/>
-      <c r="C1289" s="3"/>
-      <c r="D1289" s="3"/>
-      <c r="E1289" s="3"/>
-      <c r="F1289" s="3"/>
-      <c r="G1289" s="3"/>
-      <c r="H1289" s="3"/>
-      <c r="I1289" s="4"/>
-      <c r="J1289" s="4"/>
+      <c r="A1289" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B1289" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1289" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1289" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1289" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1289" s="3" t="s">
+        <v>1235</v>
+      </c>
+      <c r="G1289" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1289" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1289" s="4">
+        <f t="shared" si="398"/>
+        <v>2024</v>
+      </c>
+      <c r="J1289" s="4">
+        <f t="shared" si="399"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1290" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1290" s="3"/>
-      <c r="B1290" s="3"/>
-      <c r="C1290" s="3"/>
-      <c r="D1290" s="3"/>
-      <c r="E1290" s="3"/>
-      <c r="F1290" s="3"/>
-      <c r="G1290" s="3"/>
-      <c r="H1290" s="3"/>
-      <c r="I1290" s="4"/>
-      <c r="J1290" s="4"/>
+      <c r="A1290" s="3" t="s">
+        <v>1234</v>
+      </c>
+      <c r="B1290" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1290" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1290" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1290" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1290" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1290" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1290" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1290" s="4">
+        <f>YEAR(A1290)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1290" s="4">
+        <f>MONTH(A1290)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1291" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1291" s="3"/>
-      <c r="B1291" s="3"/>
-      <c r="C1291" s="3"/>
-      <c r="D1291" s="3"/>
-      <c r="E1291" s="3"/>
-      <c r="F1291" s="3"/>
-      <c r="G1291" s="3"/>
-      <c r="H1291" s="3"/>
-      <c r="I1291" s="4"/>
-      <c r="J1291" s="4"/>
+      <c r="A1291" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B1291" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1291" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="D1291" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1291" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1291" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1291" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1291" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1291" s="4">
+        <f>YEAR(A1291)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1291" s="4">
+        <f>MONTH(A1291)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1292" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1292" s="3"/>
-      <c r="B1292" s="3"/>
-      <c r="C1292" s="3"/>
-      <c r="D1292" s="3"/>
-      <c r="E1292" s="3"/>
-      <c r="F1292" s="3"/>
-      <c r="G1292" s="3"/>
-      <c r="H1292" s="3"/>
-      <c r="I1292" s="4"/>
-      <c r="J1292" s="4"/>
+      <c r="A1292" s="3" t="s">
+        <v>1237</v>
+      </c>
+      <c r="B1292" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1292" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1292" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1292" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1292" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1292" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1292" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1292" s="4">
+        <f>YEAR(A1292)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1292" s="4">
+        <f>MONTH(A1292)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1293" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1293" s="3"/>
-      <c r="B1293" s="3"/>
-      <c r="C1293" s="3"/>
-      <c r="D1293" s="3"/>
-      <c r="E1293" s="3"/>
-      <c r="F1293" s="3"/>
-      <c r="G1293" s="3"/>
-      <c r="H1293" s="3"/>
-      <c r="I1293" s="4"/>
-      <c r="J1293" s="4"/>
+      <c r="A1293" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1293" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1293" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1293" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1293" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1293" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1293" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1293" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1293" s="4">
+        <f>YEAR(A1293)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1293" s="4">
+        <f>MONTH(A1293)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1294" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1294" s="3"/>
-      <c r="B1294" s="3"/>
-      <c r="C1294" s="3"/>
-      <c r="D1294" s="3"/>
-      <c r="E1294" s="3"/>
-      <c r="F1294" s="3"/>
-      <c r="G1294" s="3"/>
-      <c r="H1294" s="3"/>
-      <c r="I1294" s="4"/>
-      <c r="J1294" s="4"/>
+      <c r="A1294" s="3" t="s">
+        <v>1238</v>
+      </c>
+      <c r="B1294" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1294" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1294" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1294" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1294" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1294" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1294" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1294" s="4">
+        <f>YEAR(A1294)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1294" s="4">
+        <f>MONTH(A1294)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1295" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1295" s="3"/>

</xml_diff>

<commit_message>
#40 Time Tracking.xlsx: updated up to 2024-12-01.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10090" uniqueCount="1239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10146" uniqueCount="1245">
   <si>
     <t>Year</t>
   </si>
@@ -3739,6 +3739,24 @@
   </si>
   <si>
     <t>2024-11-29</t>
+  </si>
+  <si>
+    <t>2024-11-30</t>
+  </si>
+  <si>
+    <t>2024-12-01</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.8.0</t>
+  </si>
+  <si>
+    <t>nwreadinglist v4.1.0</t>
+  </si>
+  <si>
+    <t>nwtimetracking v3.9.0</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.4.0</t>
   </si>
 </sst>
 </file>
@@ -4138,11 +4156,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1307"/>
+  <dimension ref="A1:J1321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1271" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1289" sqref="F1289"/>
+      <pane ySplit="1" topLeftCell="A1289" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1304" sqref="D1304"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47627,88 +47645,242 @@
       </c>
     </row>
     <row r="1295" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1295" s="3"/>
-      <c r="B1295" s="3"/>
-      <c r="C1295" s="3"/>
-      <c r="D1295" s="3"/>
-      <c r="E1295" s="3"/>
-      <c r="F1295" s="3"/>
-      <c r="G1295" s="3"/>
-      <c r="H1295" s="3"/>
-      <c r="I1295" s="4"/>
-      <c r="J1295" s="4"/>
+      <c r="A1295" s="3" t="s">
+        <v>1239</v>
+      </c>
+      <c r="B1295" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1295" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1295" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1295" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1295" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1295" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1295" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1295" s="4">
+        <f>YEAR(A1295)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1295" s="4">
+        <f>MONTH(A1295)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1296" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1296" s="3"/>
-      <c r="B1296" s="3"/>
-      <c r="C1296" s="3"/>
-      <c r="D1296" s="3"/>
-      <c r="E1296" s="3"/>
-      <c r="F1296" s="3"/>
-      <c r="G1296" s="3"/>
-      <c r="H1296" s="3"/>
-      <c r="I1296" s="4"/>
-      <c r="J1296" s="4"/>
+      <c r="A1296" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1296" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1296" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1296" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1296" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1296" s="3" t="s">
+        <v>1236</v>
+      </c>
+      <c r="G1296" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1296" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1296" s="4">
+        <f>YEAR(A1296)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1296" s="4">
+        <f>MONTH(A1296)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1297" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1297" s="3"/>
-      <c r="B1297" s="3"/>
-      <c r="C1297" s="3"/>
-      <c r="D1297" s="3"/>
-      <c r="E1297" s="3"/>
-      <c r="F1297" s="3"/>
-      <c r="G1297" s="3"/>
-      <c r="H1297" s="3"/>
-      <c r="I1297" s="4"/>
-      <c r="J1297" s="4"/>
+      <c r="A1297" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1297" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1297" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="D1297" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1297" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1297" s="3" t="s">
+        <v>1241</v>
+      </c>
+      <c r="G1297" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1297" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1297" s="4">
+        <f>YEAR(A1297)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1297" s="4">
+        <f>MONTH(A1297)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1298" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1298" s="3"/>
-      <c r="B1298" s="3"/>
-      <c r="C1298" s="3"/>
-      <c r="D1298" s="3"/>
-      <c r="E1298" s="3"/>
-      <c r="F1298" s="3"/>
-      <c r="G1298" s="3"/>
-      <c r="H1298" s="3"/>
-      <c r="I1298" s="4"/>
-      <c r="J1298" s="4"/>
+      <c r="A1298" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1298" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1298" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1298" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1298" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1298" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G1298" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1298" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1298" s="4">
+        <f>YEAR(A1298)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1298" s="4">
+        <f>MONTH(A1298)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1299" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1299" s="3"/>
-      <c r="B1299" s="3"/>
-      <c r="C1299" s="3"/>
-      <c r="D1299" s="3"/>
-      <c r="E1299" s="3"/>
-      <c r="F1299" s="3"/>
-      <c r="G1299" s="3"/>
-      <c r="H1299" s="3"/>
-      <c r="I1299" s="4"/>
-      <c r="J1299" s="4"/>
+      <c r="A1299" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1299" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="C1299" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1299" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1299" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1299" s="3" t="s">
+        <v>1242</v>
+      </c>
+      <c r="G1299" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1299" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1299" s="4">
+        <f>YEAR(A1299)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1299" s="4">
+        <f>MONTH(A1299)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1300" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1300" s="3"/>
-      <c r="B1300" s="3"/>
-      <c r="C1300" s="3"/>
-      <c r="D1300" s="3"/>
-      <c r="E1300" s="3"/>
-      <c r="F1300" s="3"/>
-      <c r="G1300" s="3"/>
-      <c r="H1300" s="3"/>
-      <c r="I1300" s="4"/>
-      <c r="J1300" s="4"/>
+      <c r="A1300" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1300" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1300" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1300" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1300" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1300" s="3" t="s">
+        <v>1243</v>
+      </c>
+      <c r="G1300" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1300" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1300" s="4">
+        <f>YEAR(A1300)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1300" s="4">
+        <f>MONTH(A1300)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1301" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1301" s="3"/>
-      <c r="B1301" s="3"/>
-      <c r="C1301" s="3"/>
-      <c r="D1301" s="3"/>
-      <c r="E1301" s="3"/>
-      <c r="F1301" s="3"/>
-      <c r="G1301" s="3"/>
-      <c r="H1301" s="3"/>
-      <c r="I1301" s="4"/>
-      <c r="J1301" s="4"/>
+      <c r="A1301" s="3" t="s">
+        <v>1240</v>
+      </c>
+      <c r="B1301" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1301" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1301" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1301" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1301" s="3" t="s">
+        <v>1244</v>
+      </c>
+      <c r="G1301" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1301" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1301" s="4">
+        <f>YEAR(A1301)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1301" s="4">
+        <f>MONTH(A1301)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1302" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1302" s="3"/>
@@ -47782,6 +47954,174 @@
       <c r="I1307" s="4"/>
       <c r="J1307" s="4"/>
     </row>
+    <row r="1308" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1308" s="3"/>
+      <c r="B1308" s="3"/>
+      <c r="C1308" s="3"/>
+      <c r="D1308" s="3"/>
+      <c r="E1308" s="3"/>
+      <c r="F1308" s="3"/>
+      <c r="G1308" s="3"/>
+      <c r="H1308" s="3"/>
+      <c r="I1308" s="4"/>
+      <c r="J1308" s="4"/>
+    </row>
+    <row r="1309" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1309" s="3"/>
+      <c r="B1309" s="3"/>
+      <c r="C1309" s="3"/>
+      <c r="D1309" s="3"/>
+      <c r="E1309" s="3"/>
+      <c r="F1309" s="3"/>
+      <c r="G1309" s="3"/>
+      <c r="H1309" s="3"/>
+      <c r="I1309" s="4"/>
+      <c r="J1309" s="4"/>
+    </row>
+    <row r="1310" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1310" s="3"/>
+      <c r="B1310" s="3"/>
+      <c r="C1310" s="3"/>
+      <c r="D1310" s="3"/>
+      <c r="E1310" s="3"/>
+      <c r="F1310" s="3"/>
+      <c r="G1310" s="3"/>
+      <c r="H1310" s="3"/>
+      <c r="I1310" s="4"/>
+      <c r="J1310" s="4"/>
+    </row>
+    <row r="1311" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1311" s="3"/>
+      <c r="B1311" s="3"/>
+      <c r="C1311" s="3"/>
+      <c r="D1311" s="3"/>
+      <c r="E1311" s="3"/>
+      <c r="F1311" s="3"/>
+      <c r="G1311" s="3"/>
+      <c r="H1311" s="3"/>
+      <c r="I1311" s="4"/>
+      <c r="J1311" s="4"/>
+    </row>
+    <row r="1312" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1312" s="3"/>
+      <c r="B1312" s="3"/>
+      <c r="C1312" s="3"/>
+      <c r="D1312" s="3"/>
+      <c r="E1312" s="3"/>
+      <c r="F1312" s="3"/>
+      <c r="G1312" s="3"/>
+      <c r="H1312" s="3"/>
+      <c r="I1312" s="4"/>
+      <c r="J1312" s="4"/>
+    </row>
+    <row r="1313" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1313" s="3"/>
+      <c r="B1313" s="3"/>
+      <c r="C1313" s="3"/>
+      <c r="D1313" s="3"/>
+      <c r="E1313" s="3"/>
+      <c r="F1313" s="3"/>
+      <c r="G1313" s="3"/>
+      <c r="H1313" s="3"/>
+      <c r="I1313" s="4"/>
+      <c r="J1313" s="4"/>
+    </row>
+    <row r="1314" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1314" s="3"/>
+      <c r="B1314" s="3"/>
+      <c r="C1314" s="3"/>
+      <c r="D1314" s="3"/>
+      <c r="E1314" s="3"/>
+      <c r="F1314" s="3"/>
+      <c r="G1314" s="3"/>
+      <c r="H1314" s="3"/>
+      <c r="I1314" s="4"/>
+      <c r="J1314" s="4"/>
+    </row>
+    <row r="1315" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1315" s="3"/>
+      <c r="B1315" s="3"/>
+      <c r="C1315" s="3"/>
+      <c r="D1315" s="3"/>
+      <c r="E1315" s="3"/>
+      <c r="F1315" s="3"/>
+      <c r="G1315" s="3"/>
+      <c r="H1315" s="3"/>
+      <c r="I1315" s="4"/>
+      <c r="J1315" s="4"/>
+    </row>
+    <row r="1316" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1316" s="3"/>
+      <c r="B1316" s="3"/>
+      <c r="C1316" s="3"/>
+      <c r="D1316" s="3"/>
+      <c r="E1316" s="3"/>
+      <c r="F1316" s="3"/>
+      <c r="G1316" s="3"/>
+      <c r="H1316" s="3"/>
+      <c r="I1316" s="4"/>
+      <c r="J1316" s="4"/>
+    </row>
+    <row r="1317" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1317" s="3"/>
+      <c r="B1317" s="3"/>
+      <c r="C1317" s="3"/>
+      <c r="D1317" s="3"/>
+      <c r="E1317" s="3"/>
+      <c r="F1317" s="3"/>
+      <c r="G1317" s="3"/>
+      <c r="H1317" s="3"/>
+      <c r="I1317" s="4"/>
+      <c r="J1317" s="4"/>
+    </row>
+    <row r="1318" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1318" s="3"/>
+      <c r="B1318" s="3"/>
+      <c r="C1318" s="3"/>
+      <c r="D1318" s="3"/>
+      <c r="E1318" s="3"/>
+      <c r="F1318" s="3"/>
+      <c r="G1318" s="3"/>
+      <c r="H1318" s="3"/>
+      <c r="I1318" s="4"/>
+      <c r="J1318" s="4"/>
+    </row>
+    <row r="1319" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1319" s="3"/>
+      <c r="B1319" s="3"/>
+      <c r="C1319" s="3"/>
+      <c r="D1319" s="3"/>
+      <c r="E1319" s="3"/>
+      <c r="F1319" s="3"/>
+      <c r="G1319" s="3"/>
+      <c r="H1319" s="3"/>
+      <c r="I1319" s="4"/>
+      <c r="J1319" s="4"/>
+    </row>
+    <row r="1320" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1320" s="3"/>
+      <c r="B1320" s="3"/>
+      <c r="C1320" s="3"/>
+      <c r="D1320" s="3"/>
+      <c r="E1320" s="3"/>
+      <c r="F1320" s="3"/>
+      <c r="G1320" s="3"/>
+      <c r="H1320" s="3"/>
+      <c r="I1320" s="4"/>
+      <c r="J1320" s="4"/>
+    </row>
+    <row r="1321" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1321" s="3"/>
+      <c r="B1321" s="3"/>
+      <c r="C1321" s="3"/>
+      <c r="D1321" s="3"/>
+      <c r="E1321" s="3"/>
+      <c r="F1321" s="3"/>
+      <c r="G1321" s="3"/>
+      <c r="H1321" s="3"/>
+      <c r="I1321" s="4"/>
+      <c r="J1321" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#42 Time Tracking: updated to 2024-12-08.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10146" uniqueCount="1245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10233" uniqueCount="1251">
   <si>
     <t>Year</t>
   </si>
@@ -3757,6 +3757,24 @@
   </si>
   <si>
     <t>nwtraderaanalytics v4.4.0</t>
+  </si>
+  <si>
+    <t>2024-12-02</t>
+  </si>
+  <si>
+    <t>nwtimetracking v4.0.0</t>
+  </si>
+  <si>
+    <t>2024-12-03</t>
+  </si>
+  <si>
+    <t>2024-12-05</t>
+  </si>
+  <si>
+    <t>2024-12-06</t>
+  </si>
+  <si>
+    <t>2024-12-08</t>
   </si>
 </sst>
 </file>
@@ -4159,8 +4177,8 @@
   <dimension ref="A1:J1321"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1289" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1304" sqref="D1304"/>
+      <pane ySplit="1" topLeftCell="A1283" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1314" sqref="G1314"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -47500,11 +47518,11 @@
         <v>280</v>
       </c>
       <c r="I1290" s="4">
-        <f>YEAR(A1290)</f>
+        <f t="shared" ref="I1290:I1302" si="400">YEAR(A1290)</f>
         <v>2024</v>
       </c>
       <c r="J1290" s="4">
-        <f>MONTH(A1290)</f>
+        <f t="shared" ref="J1290:J1302" si="401">MONTH(A1290)</f>
         <v>11</v>
       </c>
     </row>
@@ -47534,11 +47552,11 @@
         <v>280</v>
       </c>
       <c r="I1291" s="4">
-        <f>YEAR(A1291)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1291" s="4">
-        <f>MONTH(A1291)</f>
+        <f t="shared" si="401"/>
         <v>11</v>
       </c>
     </row>
@@ -47568,11 +47586,11 @@
         <v>280</v>
       </c>
       <c r="I1292" s="4">
-        <f>YEAR(A1292)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1292" s="4">
-        <f>MONTH(A1292)</f>
+        <f t="shared" si="401"/>
         <v>11</v>
       </c>
     </row>
@@ -47602,11 +47620,11 @@
         <v>280</v>
       </c>
       <c r="I1293" s="4">
-        <f>YEAR(A1293)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1293" s="4">
-        <f>MONTH(A1293)</f>
+        <f t="shared" si="401"/>
         <v>11</v>
       </c>
     </row>
@@ -47636,11 +47654,11 @@
         <v>280</v>
       </c>
       <c r="I1294" s="4">
-        <f>YEAR(A1294)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1294" s="4">
-        <f>MONTH(A1294)</f>
+        <f t="shared" si="401"/>
         <v>11</v>
       </c>
     </row>
@@ -47670,11 +47688,11 @@
         <v>280</v>
       </c>
       <c r="I1295" s="4">
-        <f>YEAR(A1295)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1295" s="4">
-        <f>MONTH(A1295)</f>
+        <f t="shared" si="401"/>
         <v>11</v>
       </c>
     </row>
@@ -47704,11 +47722,11 @@
         <v>279</v>
       </c>
       <c r="I1296" s="4">
-        <f>YEAR(A1296)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1296" s="4">
-        <f>MONTH(A1296)</f>
+        <f t="shared" si="401"/>
         <v>12</v>
       </c>
     </row>
@@ -47738,11 +47756,11 @@
         <v>279</v>
       </c>
       <c r="I1297" s="4">
-        <f>YEAR(A1297)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1297" s="4">
-        <f>MONTH(A1297)</f>
+        <f t="shared" si="401"/>
         <v>12</v>
       </c>
     </row>
@@ -47772,11 +47790,11 @@
         <v>279</v>
       </c>
       <c r="I1298" s="4">
-        <f>YEAR(A1298)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1298" s="4">
-        <f>MONTH(A1298)</f>
+        <f t="shared" si="401"/>
         <v>12</v>
       </c>
     </row>
@@ -47806,11 +47824,11 @@
         <v>279</v>
       </c>
       <c r="I1299" s="4">
-        <f>YEAR(A1299)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1299" s="4">
-        <f>MONTH(A1299)</f>
+        <f t="shared" si="401"/>
         <v>12</v>
       </c>
     </row>
@@ -47840,11 +47858,11 @@
         <v>279</v>
       </c>
       <c r="I1300" s="4">
-        <f>YEAR(A1300)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1300" s="4">
-        <f>MONTH(A1300)</f>
+        <f t="shared" si="401"/>
         <v>12</v>
       </c>
     </row>
@@ -47874,145 +47892,385 @@
         <v>279</v>
       </c>
       <c r="I1301" s="4">
-        <f>YEAR(A1301)</f>
+        <f t="shared" si="400"/>
         <v>2024</v>
       </c>
       <c r="J1301" s="4">
-        <f>MONTH(A1301)</f>
+        <f t="shared" si="401"/>
         <v>12</v>
       </c>
     </row>
     <row r="1302" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1302" s="3"/>
-      <c r="B1302" s="3"/>
-      <c r="C1302" s="3"/>
-      <c r="D1302" s="3"/>
-      <c r="E1302" s="3"/>
+      <c r="A1302" s="3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B1302" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1302" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1302" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1302" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1302" s="3"/>
-      <c r="G1302" s="3"/>
-      <c r="H1302" s="3"/>
-      <c r="I1302" s="4"/>
-      <c r="J1302" s="4"/>
+      <c r="G1302" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1302" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1302" s="4">
+        <f t="shared" si="400"/>
+        <v>2024</v>
+      </c>
+      <c r="J1302" s="4">
+        <f t="shared" si="401"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1303" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1303" s="3"/>
-      <c r="B1303" s="3"/>
-      <c r="C1303" s="3"/>
-      <c r="D1303" s="3"/>
-      <c r="E1303" s="3"/>
-      <c r="F1303" s="3"/>
-      <c r="G1303" s="3"/>
-      <c r="H1303" s="3"/>
-      <c r="I1303" s="4"/>
-      <c r="J1303" s="4"/>
+      <c r="A1303" s="3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B1303" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1303" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1303" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1303" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1303" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1303" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1303" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1303" s="4">
+        <f t="shared" ref="I1303:I1304" si="402">YEAR(A1303)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1303" s="4">
+        <f t="shared" ref="J1303:J1304" si="403">MONTH(A1303)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1304" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1304" s="3"/>
-      <c r="B1304" s="3"/>
-      <c r="C1304" s="3"/>
-      <c r="D1304" s="3"/>
-      <c r="E1304" s="3"/>
-      <c r="F1304" s="3"/>
-      <c r="G1304" s="3"/>
-      <c r="H1304" s="3"/>
-      <c r="I1304" s="4"/>
-      <c r="J1304" s="4"/>
+      <c r="A1304" s="3" t="s">
+        <v>1245</v>
+      </c>
+      <c r="B1304" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1304" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1304" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1304" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1304" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1304" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1304" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1304" s="4">
+        <f t="shared" si="402"/>
+        <v>2024</v>
+      </c>
+      <c r="J1304" s="4">
+        <f t="shared" si="403"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1305" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1305" s="3"/>
-      <c r="B1305" s="3"/>
-      <c r="C1305" s="3"/>
-      <c r="D1305" s="3"/>
-      <c r="E1305" s="3"/>
-      <c r="F1305" s="3"/>
-      <c r="G1305" s="3"/>
-      <c r="H1305" s="3"/>
-      <c r="I1305" s="4"/>
-      <c r="J1305" s="4"/>
+      <c r="A1305" s="3" t="s">
+        <v>1247</v>
+      </c>
+      <c r="B1305" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1305" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1305" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1305" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1305" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1305" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1305" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1305" s="4">
+        <f t="shared" ref="I1305:I1306" si="404">YEAR(A1305)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1305" s="4">
+        <f t="shared" ref="J1305:J1306" si="405">MONTH(A1305)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1306" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1306" s="3"/>
-      <c r="B1306" s="3"/>
-      <c r="C1306" s="3"/>
-      <c r="D1306" s="3"/>
-      <c r="E1306" s="3"/>
-      <c r="F1306" s="3"/>
-      <c r="G1306" s="3"/>
-      <c r="H1306" s="3"/>
-      <c r="I1306" s="4"/>
-      <c r="J1306" s="4"/>
+      <c r="A1306" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B1306" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1306" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1306" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1306" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1306" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1306" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1306" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1306" s="4">
+        <f t="shared" si="404"/>
+        <v>2024</v>
+      </c>
+      <c r="J1306" s="4">
+        <f t="shared" si="405"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1307" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1307" s="3"/>
-      <c r="B1307" s="3"/>
-      <c r="C1307" s="3"/>
-      <c r="D1307" s="3"/>
-      <c r="E1307" s="3"/>
-      <c r="F1307" s="3"/>
-      <c r="G1307" s="3"/>
-      <c r="H1307" s="3"/>
-      <c r="I1307" s="4"/>
-      <c r="J1307" s="4"/>
+      <c r="A1307" s="3" t="s">
+        <v>1248</v>
+      </c>
+      <c r="B1307" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1307" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1307" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1307" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1307" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1307" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1307" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1307" s="4">
+        <f t="shared" ref="I1307" si="406">YEAR(A1307)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1307" s="4">
+        <f t="shared" ref="J1307" si="407">MONTH(A1307)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1308" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1308" s="3"/>
-      <c r="B1308" s="3"/>
-      <c r="C1308" s="3"/>
-      <c r="D1308" s="3"/>
-      <c r="E1308" s="3"/>
-      <c r="F1308" s="3"/>
-      <c r="G1308" s="3"/>
-      <c r="H1308" s="3"/>
-      <c r="I1308" s="4"/>
-      <c r="J1308" s="4"/>
+      <c r="A1308" s="3" t="s">
+        <v>1249</v>
+      </c>
+      <c r="B1308" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1308" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1308" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="E1308" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1308" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1308" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1308" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1308" s="4">
+        <f t="shared" ref="I1308:I1312" si="408">YEAR(A1308)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1308" s="4">
+        <f t="shared" ref="J1308:J1312" si="409">MONTH(A1308)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1309" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1309" s="3"/>
-      <c r="B1309" s="3"/>
-      <c r="C1309" s="3"/>
-      <c r="D1309" s="3"/>
-      <c r="E1309" s="3"/>
-      <c r="F1309" s="3"/>
-      <c r="G1309" s="3"/>
-      <c r="H1309" s="3"/>
-      <c r="I1309" s="4"/>
-      <c r="J1309" s="4"/>
+      <c r="A1309" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1309" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1309" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1309" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1309" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1309" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1309" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1309" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1309" s="4">
+        <f t="shared" si="408"/>
+        <v>2024</v>
+      </c>
+      <c r="J1309" s="4">
+        <f t="shared" si="409"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1310" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1310" s="3"/>
-      <c r="B1310" s="3"/>
-      <c r="C1310" s="3"/>
-      <c r="D1310" s="3"/>
-      <c r="E1310" s="3"/>
-      <c r="F1310" s="3"/>
-      <c r="G1310" s="3"/>
-      <c r="H1310" s="3"/>
-      <c r="I1310" s="4"/>
-      <c r="J1310" s="4"/>
+      <c r="A1310" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1310" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1310" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1310" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1310" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1310" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1310" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1310" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1310" s="4">
+        <f t="shared" si="408"/>
+        <v>2024</v>
+      </c>
+      <c r="J1310" s="4">
+        <f t="shared" si="409"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1311" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1311" s="3"/>
-      <c r="B1311" s="3"/>
-      <c r="C1311" s="3"/>
-      <c r="D1311" s="3"/>
-      <c r="E1311" s="3"/>
-      <c r="F1311" s="3"/>
-      <c r="G1311" s="3"/>
-      <c r="H1311" s="3"/>
-      <c r="I1311" s="4"/>
-      <c r="J1311" s="4"/>
+      <c r="A1311" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1311" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1311" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1311" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1311" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1311" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1311" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1311" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1311" s="4">
+        <f t="shared" si="408"/>
+        <v>2024</v>
+      </c>
+      <c r="J1311" s="4">
+        <f t="shared" si="409"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1312" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1312" s="3"/>
-      <c r="B1312" s="3"/>
-      <c r="C1312" s="3"/>
-      <c r="D1312" s="3"/>
-      <c r="E1312" s="3"/>
-      <c r="F1312" s="3"/>
-      <c r="G1312" s="3"/>
-      <c r="H1312" s="3"/>
-      <c r="I1312" s="4"/>
-      <c r="J1312" s="4"/>
+      <c r="A1312" s="3" t="s">
+        <v>1250</v>
+      </c>
+      <c r="B1312" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1312" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1312" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1312" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1312" s="3" t="s">
+        <v>1246</v>
+      </c>
+      <c r="G1312" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1312" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1312" s="4">
+        <f t="shared" si="408"/>
+        <v>2024</v>
+      </c>
+      <c r="J1312" s="4">
+        <f t="shared" si="409"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1313" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1313" s="3"/>

</xml_diff>

<commit_message>
#42 Time Tracking: updated to 2024-12-15.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10239" uniqueCount="1251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10318" uniqueCount="1259">
   <si>
     <t>Year</t>
   </si>
@@ -3775,6 +3775,30 @@
   </si>
   <si>
     <t>2024-12-08</t>
+  </si>
+  <si>
+    <t>2024-12-09</t>
+  </si>
+  <si>
+    <t>nwreadinglist v4.2.0</t>
+  </si>
+  <si>
+    <t>2024-12-10</t>
+  </si>
+  <si>
+    <t>2024-12-11</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.5.0</t>
+  </si>
+  <si>
+    <t>2024-12-12</t>
+  </si>
+  <si>
+    <t>2024-12-13</t>
+  </si>
+  <si>
+    <t>2024-12-15</t>
   </si>
 </sst>
 </file>
@@ -4174,11 +4198,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1321"/>
+  <dimension ref="A1:J1352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1283" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1315" sqref="F1315"/>
+      <pane ySplit="1" topLeftCell="A1300" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1327" sqref="H1327"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48303,100 +48327,690 @@
       </c>
     </row>
     <row r="1314" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1314" s="3"/>
-      <c r="B1314" s="3"/>
-      <c r="C1314" s="3"/>
-      <c r="D1314" s="3"/>
-      <c r="E1314" s="3"/>
-      <c r="F1314" s="3"/>
-      <c r="G1314" s="3"/>
-      <c r="H1314" s="3"/>
-      <c r="I1314" s="4"/>
-      <c r="J1314" s="4"/>
+      <c r="A1314" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B1314" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1314" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1314" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1314" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1314" s="3" t="s">
+        <v>1252</v>
+      </c>
+      <c r="G1314" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1314" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1314" s="4">
+        <f t="shared" ref="I1314:I1316" si="408">YEAR(A1314)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1314" s="4">
+        <f t="shared" ref="J1314:J1316" si="409">MONTH(A1314)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1315" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1315" s="3"/>
-      <c r="B1315" s="3"/>
-      <c r="C1315" s="3"/>
-      <c r="D1315" s="3"/>
-      <c r="E1315" s="3"/>
+      <c r="A1315" s="3" t="s">
+        <v>1251</v>
+      </c>
+      <c r="B1315" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1315" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1315" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1315" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1315" s="3"/>
-      <c r="G1315" s="3"/>
-      <c r="H1315" s="3"/>
-      <c r="I1315" s="4"/>
-      <c r="J1315" s="4"/>
+      <c r="G1315" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1315" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1315" s="4">
+        <f t="shared" si="408"/>
+        <v>2024</v>
+      </c>
+      <c r="J1315" s="4">
+        <f t="shared" si="409"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1316" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1316" s="3"/>
-      <c r="B1316" s="3"/>
-      <c r="C1316" s="3"/>
-      <c r="D1316" s="3"/>
-      <c r="E1316" s="3"/>
-      <c r="F1316" s="3"/>
-      <c r="G1316" s="3"/>
-      <c r="H1316" s="3"/>
-      <c r="I1316" s="4"/>
-      <c r="J1316" s="4"/>
+      <c r="A1316" s="3" t="s">
+        <v>1253</v>
+      </c>
+      <c r="B1316" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1316" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1316" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1316" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1316" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1316" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1316" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1316" s="4">
+        <f t="shared" si="408"/>
+        <v>2024</v>
+      </c>
+      <c r="J1316" s="4">
+        <f t="shared" si="409"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1317" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1317" s="3"/>
-      <c r="B1317" s="3"/>
-      <c r="C1317" s="3"/>
-      <c r="D1317" s="3"/>
-      <c r="E1317" s="3"/>
-      <c r="F1317" s="3"/>
-      <c r="G1317" s="3"/>
-      <c r="H1317" s="3"/>
-      <c r="I1317" s="4"/>
-      <c r="J1317" s="4"/>
+      <c r="A1317" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B1317" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1317" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1317" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1317" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1317" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1317" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1317" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1317" s="4">
+        <f t="shared" ref="I1317:I1318" si="410">YEAR(A1317)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1317" s="4">
+        <f t="shared" ref="J1317:J1318" si="411">MONTH(A1317)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1318" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1318" s="3"/>
-      <c r="B1318" s="3"/>
-      <c r="C1318" s="3"/>
-      <c r="D1318" s="3"/>
-      <c r="E1318" s="3"/>
-      <c r="F1318" s="3"/>
-      <c r="G1318" s="3"/>
-      <c r="H1318" s="3"/>
-      <c r="I1318" s="4"/>
-      <c r="J1318" s="4"/>
+      <c r="A1318" s="3" t="s">
+        <v>1254</v>
+      </c>
+      <c r="B1318" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1318" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1318" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1318" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1318" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1318" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1318" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1318" s="4">
+        <f t="shared" si="410"/>
+        <v>2024</v>
+      </c>
+      <c r="J1318" s="4">
+        <f t="shared" si="411"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1319" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1319" s="3"/>
-      <c r="B1319" s="3"/>
-      <c r="C1319" s="3"/>
-      <c r="D1319" s="3"/>
-      <c r="E1319" s="3"/>
-      <c r="F1319" s="3"/>
-      <c r="G1319" s="3"/>
-      <c r="H1319" s="3"/>
-      <c r="I1319" s="4"/>
-      <c r="J1319" s="4"/>
+      <c r="A1319" s="3" t="s">
+        <v>1256</v>
+      </c>
+      <c r="B1319" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="C1319" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="D1319" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1319" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1319" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1319" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1319" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1319" s="4">
+        <f t="shared" ref="I1319" si="412">YEAR(A1319)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1319" s="4">
+        <f t="shared" ref="J1319" si="413">MONTH(A1319)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1320" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1320" s="3"/>
-      <c r="B1320" s="3"/>
-      <c r="C1320" s="3"/>
-      <c r="D1320" s="3"/>
-      <c r="E1320" s="3"/>
-      <c r="F1320" s="3"/>
-      <c r="G1320" s="3"/>
-      <c r="H1320" s="3"/>
-      <c r="I1320" s="4"/>
-      <c r="J1320" s="4"/>
+      <c r="A1320" s="3" t="s">
+        <v>1257</v>
+      </c>
+      <c r="B1320" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1320" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1320" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1320" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1320" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1320" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1320" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1320" s="4">
+        <f t="shared" ref="I1320:I1322" si="414">YEAR(A1320)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1320" s="4">
+        <f t="shared" ref="J1320:J1322" si="415">MONTH(A1320)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1321" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1321" s="3"/>
-      <c r="B1321" s="3"/>
-      <c r="C1321" s="3"/>
-      <c r="D1321" s="3"/>
-      <c r="E1321" s="3"/>
-      <c r="F1321" s="3"/>
-      <c r="G1321" s="3"/>
-      <c r="H1321" s="3"/>
-      <c r="I1321" s="4"/>
-      <c r="J1321" s="4"/>
+      <c r="A1321" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B1321" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1321" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1321" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1321" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1321" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1321" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1321" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1321" s="4">
+        <f t="shared" si="414"/>
+        <v>2024</v>
+      </c>
+      <c r="J1321" s="4">
+        <f t="shared" si="415"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1322" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B1322" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1322" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1322" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1322" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1322" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1322" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1322" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1322" s="4">
+        <f t="shared" si="414"/>
+        <v>2024</v>
+      </c>
+      <c r="J1322" s="4">
+        <f t="shared" si="415"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1323" s="3" t="s">
+        <v>1258</v>
+      </c>
+      <c r="B1323" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1323" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1323" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1323" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1323" s="3" t="s">
+        <v>1255</v>
+      </c>
+      <c r="G1323" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1323" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1323" s="4">
+        <f t="shared" ref="I1323" si="416">YEAR(A1323)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1323" s="4">
+        <f t="shared" ref="J1323" si="417">MONTH(A1323)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1324" s="3"/>
+      <c r="B1324" s="3"/>
+      <c r="C1324" s="3"/>
+      <c r="D1324" s="3"/>
+      <c r="E1324" s="3"/>
+      <c r="F1324" s="3"/>
+      <c r="G1324" s="3"/>
+      <c r="H1324" s="3"/>
+      <c r="I1324" s="4"/>
+      <c r="J1324" s="4"/>
+    </row>
+    <row r="1325" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1325" s="3"/>
+      <c r="B1325" s="3"/>
+      <c r="C1325" s="3"/>
+      <c r="D1325" s="3"/>
+      <c r="E1325" s="3"/>
+      <c r="F1325" s="3"/>
+      <c r="G1325" s="3"/>
+      <c r="H1325" s="3"/>
+      <c r="I1325" s="4"/>
+      <c r="J1325" s="4"/>
+    </row>
+    <row r="1326" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1326" s="3"/>
+      <c r="B1326" s="3"/>
+      <c r="C1326" s="3"/>
+      <c r="D1326" s="3"/>
+      <c r="E1326" s="3"/>
+      <c r="F1326" s="3"/>
+      <c r="G1326" s="3"/>
+      <c r="H1326" s="3"/>
+      <c r="I1326" s="4"/>
+      <c r="J1326" s="4"/>
+    </row>
+    <row r="1327" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1327" s="3"/>
+      <c r="B1327" s="3"/>
+      <c r="C1327" s="3"/>
+      <c r="D1327" s="3"/>
+      <c r="E1327" s="3"/>
+      <c r="F1327" s="3"/>
+      <c r="G1327" s="3"/>
+      <c r="H1327" s="3"/>
+      <c r="I1327" s="4"/>
+      <c r="J1327" s="4"/>
+    </row>
+    <row r="1328" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1328" s="3"/>
+      <c r="B1328" s="3"/>
+      <c r="C1328" s="3"/>
+      <c r="D1328" s="3"/>
+      <c r="E1328" s="3"/>
+      <c r="F1328" s="3"/>
+      <c r="G1328" s="3"/>
+      <c r="H1328" s="3"/>
+      <c r="I1328" s="4"/>
+      <c r="J1328" s="4"/>
+    </row>
+    <row r="1329" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1329" s="3"/>
+      <c r="B1329" s="3"/>
+      <c r="C1329" s="3"/>
+      <c r="D1329" s="3"/>
+      <c r="E1329" s="3"/>
+      <c r="F1329" s="3"/>
+      <c r="G1329" s="3"/>
+      <c r="H1329" s="3"/>
+      <c r="I1329" s="4"/>
+      <c r="J1329" s="4"/>
+    </row>
+    <row r="1330" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1330" s="3"/>
+      <c r="B1330" s="3"/>
+      <c r="C1330" s="3"/>
+      <c r="D1330" s="3"/>
+      <c r="E1330" s="3"/>
+      <c r="F1330" s="3"/>
+      <c r="G1330" s="3"/>
+      <c r="H1330" s="3"/>
+      <c r="I1330" s="4"/>
+      <c r="J1330" s="4"/>
+    </row>
+    <row r="1331" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1331" s="3"/>
+      <c r="B1331" s="3"/>
+      <c r="C1331" s="3"/>
+      <c r="D1331" s="3"/>
+      <c r="E1331" s="3"/>
+      <c r="F1331" s="3"/>
+      <c r="G1331" s="3"/>
+      <c r="H1331" s="3"/>
+      <c r="I1331" s="4"/>
+      <c r="J1331" s="4"/>
+    </row>
+    <row r="1332" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1332" s="3"/>
+      <c r="B1332" s="3"/>
+      <c r="C1332" s="3"/>
+      <c r="D1332" s="3"/>
+      <c r="E1332" s="3"/>
+      <c r="F1332" s="3"/>
+      <c r="G1332" s="3"/>
+      <c r="H1332" s="3"/>
+      <c r="I1332" s="4"/>
+      <c r="J1332" s="4"/>
+    </row>
+    <row r="1333" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1333" s="3"/>
+      <c r="B1333" s="3"/>
+      <c r="C1333" s="3"/>
+      <c r="D1333" s="3"/>
+      <c r="E1333" s="3"/>
+      <c r="F1333" s="3"/>
+      <c r="G1333" s="3"/>
+      <c r="H1333" s="3"/>
+      <c r="I1333" s="4"/>
+      <c r="J1333" s="4"/>
+    </row>
+    <row r="1334" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1334" s="3"/>
+      <c r="B1334" s="3"/>
+      <c r="C1334" s="3"/>
+      <c r="D1334" s="3"/>
+      <c r="E1334" s="3"/>
+      <c r="F1334" s="3"/>
+      <c r="G1334" s="3"/>
+      <c r="H1334" s="3"/>
+      <c r="I1334" s="4"/>
+      <c r="J1334" s="4"/>
+    </row>
+    <row r="1335" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1335" s="3"/>
+      <c r="B1335" s="3"/>
+      <c r="C1335" s="3"/>
+      <c r="D1335" s="3"/>
+      <c r="E1335" s="3"/>
+      <c r="F1335" s="3"/>
+      <c r="G1335" s="3"/>
+      <c r="H1335" s="3"/>
+      <c r="I1335" s="4"/>
+      <c r="J1335" s="4"/>
+    </row>
+    <row r="1336" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1336" s="3"/>
+      <c r="B1336" s="3"/>
+      <c r="C1336" s="3"/>
+      <c r="D1336" s="3"/>
+      <c r="E1336" s="3"/>
+      <c r="F1336" s="3"/>
+      <c r="G1336" s="3"/>
+      <c r="H1336" s="3"/>
+      <c r="I1336" s="4"/>
+      <c r="J1336" s="4"/>
+    </row>
+    <row r="1337" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1337" s="3"/>
+      <c r="B1337" s="3"/>
+      <c r="C1337" s="3"/>
+      <c r="D1337" s="3"/>
+      <c r="E1337" s="3"/>
+      <c r="F1337" s="3"/>
+      <c r="G1337" s="3"/>
+      <c r="H1337" s="3"/>
+      <c r="I1337" s="4"/>
+      <c r="J1337" s="4"/>
+    </row>
+    <row r="1338" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1338" s="3"/>
+      <c r="B1338" s="3"/>
+      <c r="C1338" s="3"/>
+      <c r="D1338" s="3"/>
+      <c r="E1338" s="3"/>
+      <c r="F1338" s="3"/>
+      <c r="G1338" s="3"/>
+      <c r="H1338" s="3"/>
+      <c r="I1338" s="4"/>
+      <c r="J1338" s="4"/>
+    </row>
+    <row r="1339" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1339" s="3"/>
+      <c r="B1339" s="3"/>
+      <c r="C1339" s="3"/>
+      <c r="D1339" s="3"/>
+      <c r="E1339" s="3"/>
+      <c r="F1339" s="3"/>
+      <c r="G1339" s="3"/>
+      <c r="H1339" s="3"/>
+      <c r="I1339" s="4"/>
+      <c r="J1339" s="4"/>
+    </row>
+    <row r="1340" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1340" s="3"/>
+      <c r="B1340" s="3"/>
+      <c r="C1340" s="3"/>
+      <c r="D1340" s="3"/>
+      <c r="E1340" s="3"/>
+      <c r="F1340" s="3"/>
+      <c r="G1340" s="3"/>
+      <c r="H1340" s="3"/>
+      <c r="I1340" s="4"/>
+      <c r="J1340" s="4"/>
+    </row>
+    <row r="1341" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1341" s="3"/>
+      <c r="B1341" s="3"/>
+      <c r="C1341" s="3"/>
+      <c r="D1341" s="3"/>
+      <c r="E1341" s="3"/>
+      <c r="F1341" s="3"/>
+      <c r="G1341" s="3"/>
+      <c r="H1341" s="3"/>
+      <c r="I1341" s="4"/>
+      <c r="J1341" s="4"/>
+    </row>
+    <row r="1342" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1342" s="3"/>
+      <c r="B1342" s="3"/>
+      <c r="C1342" s="3"/>
+      <c r="D1342" s="3"/>
+      <c r="E1342" s="3"/>
+      <c r="F1342" s="3"/>
+      <c r="G1342" s="3"/>
+      <c r="H1342" s="3"/>
+      <c r="I1342" s="4"/>
+      <c r="J1342" s="4"/>
+    </row>
+    <row r="1343" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1343" s="3"/>
+      <c r="B1343" s="3"/>
+      <c r="C1343" s="3"/>
+      <c r="D1343" s="3"/>
+      <c r="E1343" s="3"/>
+      <c r="F1343" s="3"/>
+      <c r="G1343" s="3"/>
+      <c r="H1343" s="3"/>
+      <c r="I1343" s="4"/>
+      <c r="J1343" s="4"/>
+    </row>
+    <row r="1344" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1344" s="3"/>
+      <c r="B1344" s="3"/>
+      <c r="C1344" s="3"/>
+      <c r="D1344" s="3"/>
+      <c r="E1344" s="3"/>
+      <c r="F1344" s="3"/>
+      <c r="G1344" s="3"/>
+      <c r="H1344" s="3"/>
+      <c r="I1344" s="4"/>
+      <c r="J1344" s="4"/>
+    </row>
+    <row r="1345" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1345" s="3"/>
+      <c r="B1345" s="3"/>
+      <c r="C1345" s="3"/>
+      <c r="D1345" s="3"/>
+      <c r="E1345" s="3"/>
+      <c r="F1345" s="3"/>
+      <c r="G1345" s="3"/>
+      <c r="H1345" s="3"/>
+      <c r="I1345" s="4"/>
+      <c r="J1345" s="4"/>
+    </row>
+    <row r="1346" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1346" s="3"/>
+      <c r="B1346" s="3"/>
+      <c r="C1346" s="3"/>
+      <c r="D1346" s="3"/>
+      <c r="E1346" s="3"/>
+      <c r="F1346" s="3"/>
+      <c r="G1346" s="3"/>
+      <c r="H1346" s="3"/>
+      <c r="I1346" s="4"/>
+      <c r="J1346" s="4"/>
+    </row>
+    <row r="1347" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1347" s="3"/>
+      <c r="B1347" s="3"/>
+      <c r="C1347" s="3"/>
+      <c r="D1347" s="3"/>
+      <c r="E1347" s="3"/>
+      <c r="F1347" s="3"/>
+      <c r="G1347" s="3"/>
+      <c r="H1347" s="3"/>
+      <c r="I1347" s="4"/>
+      <c r="J1347" s="4"/>
+    </row>
+    <row r="1348" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1348" s="3"/>
+      <c r="B1348" s="3"/>
+      <c r="C1348" s="3"/>
+      <c r="D1348" s="3"/>
+      <c r="E1348" s="3"/>
+      <c r="F1348" s="3"/>
+      <c r="G1348" s="3"/>
+      <c r="H1348" s="3"/>
+      <c r="I1348" s="4"/>
+      <c r="J1348" s="4"/>
+    </row>
+    <row r="1349" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1349" s="3"/>
+      <c r="B1349" s="3"/>
+      <c r="C1349" s="3"/>
+      <c r="D1349" s="3"/>
+      <c r="E1349" s="3"/>
+      <c r="F1349" s="3"/>
+      <c r="G1349" s="3"/>
+      <c r="H1349" s="3"/>
+      <c r="I1349" s="4"/>
+      <c r="J1349" s="4"/>
+    </row>
+    <row r="1350" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1350" s="3"/>
+      <c r="B1350" s="3"/>
+      <c r="C1350" s="3"/>
+      <c r="D1350" s="3"/>
+      <c r="E1350" s="3"/>
+      <c r="F1350" s="3"/>
+      <c r="G1350" s="3"/>
+      <c r="H1350" s="3"/>
+      <c r="I1350" s="4"/>
+      <c r="J1350" s="4"/>
+    </row>
+    <row r="1351" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1351" s="3"/>
+      <c r="B1351" s="3"/>
+      <c r="C1351" s="3"/>
+      <c r="D1351" s="3"/>
+      <c r="E1351" s="3"/>
+      <c r="F1351" s="3"/>
+      <c r="G1351" s="3"/>
+      <c r="H1351" s="3"/>
+      <c r="I1351" s="4"/>
+      <c r="J1351" s="4"/>
+    </row>
+    <row r="1352" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1352" s="3"/>
+      <c r="B1352" s="3"/>
+      <c r="C1352" s="3"/>
+      <c r="D1352" s="3"/>
+      <c r="E1352" s="3"/>
+      <c r="F1352" s="3"/>
+      <c r="G1352" s="3"/>
+      <c r="H1352" s="3"/>
+      <c r="I1352" s="4"/>
+      <c r="J1352" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#42 Time Tracking: updated to 2024-12-16.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10318" uniqueCount="1259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10334" uniqueCount="1262">
   <si>
     <t>Year</t>
   </si>
@@ -3799,6 +3799,15 @@
   </si>
   <si>
     <t>2024-12-15</t>
+  </si>
+  <si>
+    <t>2024-12-16</t>
+  </si>
+  <si>
+    <t>10h 30m</t>
+  </si>
+  <si>
+    <t>nwtimetracking v4.5.0</t>
   </si>
 </sst>
 </file>
@@ -4202,7 +4211,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1300" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1327" sqref="H1327"/>
+      <selection pane="bottomLeft" activeCell="E1328" sqref="E1328"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48656,37 +48665,81 @@
         <v>279</v>
       </c>
       <c r="I1323" s="4">
-        <f t="shared" ref="I1323" si="416">YEAR(A1323)</f>
+        <f t="shared" ref="I1323:I1325" si="416">YEAR(A1323)</f>
         <v>2024</v>
       </c>
       <c r="J1323" s="4">
-        <f t="shared" ref="J1323" si="417">MONTH(A1323)</f>
+        <f t="shared" ref="J1323:J1325" si="417">MONTH(A1323)</f>
         <v>12</v>
       </c>
     </row>
     <row r="1324" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1324" s="3"/>
-      <c r="B1324" s="3"/>
-      <c r="C1324" s="3"/>
-      <c r="D1324" s="3"/>
-      <c r="E1324" s="3"/>
-      <c r="F1324" s="3"/>
-      <c r="G1324" s="3"/>
-      <c r="H1324" s="3"/>
-      <c r="I1324" s="4"/>
-      <c r="J1324" s="4"/>
+      <c r="A1324" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B1324" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1324" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1324" s="3" t="s">
+        <v>1260</v>
+      </c>
+      <c r="E1324" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1324" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G1324" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1324" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1324" s="4">
+        <f t="shared" si="416"/>
+        <v>2024</v>
+      </c>
+      <c r="J1324" s="4">
+        <f t="shared" si="417"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1325" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1325" s="3"/>
-      <c r="B1325" s="3"/>
-      <c r="C1325" s="3"/>
-      <c r="D1325" s="3"/>
-      <c r="E1325" s="3"/>
-      <c r="F1325" s="3"/>
-      <c r="G1325" s="3"/>
-      <c r="H1325" s="3"/>
-      <c r="I1325" s="4"/>
-      <c r="J1325" s="4"/>
+      <c r="A1325" s="3" t="s">
+        <v>1259</v>
+      </c>
+      <c r="B1325" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1325" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1325" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1325" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1325" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G1325" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1325" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1325" s="4">
+        <f t="shared" si="416"/>
+        <v>2024</v>
+      </c>
+      <c r="J1325" s="4">
+        <f t="shared" si="417"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1326" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1326" s="3"/>

</xml_diff>

<commit_message>
#42 Time Tracking: fixed some cells.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -9,6 +9,9 @@
   <sheets>
     <sheet name="Sessions" sheetId="8" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sessions!$A$1:$J$1325</definedName>
+  </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -4210,8 +4213,8 @@
   <dimension ref="A1:J1352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1300" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1328" sqref="E1328"/>
+      <pane ySplit="1" topLeftCell="A1301" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1329" sqref="E1329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -8295,13 +8298,13 @@
         <v>115</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F128" s="3" t="s">
         <v>669</v>
       </c>
       <c r="G128" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H128" s="8" t="s">
         <v>280</v>
@@ -8633,7 +8636,7 @@
         <v>105</v>
       </c>
       <c r="E138" s="3" t="s">
-        <v>155</v>
+        <v>728</v>
       </c>
       <c r="F138" s="3" t="s">
         <v>680</v>
@@ -8871,13 +8874,13 @@
         <v>105</v>
       </c>
       <c r="E145" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F145" s="3" t="s">
         <v>669</v>
       </c>
       <c r="G145" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H145" s="8" t="s">
         <v>280</v>
@@ -8905,13 +8908,13 @@
         <v>193</v>
       </c>
       <c r="E146" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>669</v>
       </c>
       <c r="G146" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H146" s="8" t="s">
         <v>280</v>
@@ -8939,13 +8942,13 @@
         <v>120</v>
       </c>
       <c r="E147" s="3" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="F147" s="3" t="s">
         <v>669</v>
       </c>
       <c r="G147" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H147" s="8" t="s">
         <v>280</v>
@@ -34955,13 +34958,13 @@
         <v>126</v>
       </c>
       <c r="E913" s="3" t="s">
-        <v>127</v>
+        <v>728</v>
       </c>
       <c r="F913" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="G913" s="8" t="s">
-        <v>279</v>
+      <c r="G913" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="H913" s="3" t="s">
         <v>280</v>
@@ -34989,13 +34992,13 @@
         <v>239</v>
       </c>
       <c r="E914" s="3" t="s">
-        <v>127</v>
+        <v>728</v>
       </c>
       <c r="F914" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="G914" s="8" t="s">
-        <v>279</v>
+      <c r="G914" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="H914" s="3" t="s">
         <v>280</v>
@@ -35023,13 +35026,13 @@
         <v>168</v>
       </c>
       <c r="E915" s="3" t="s">
-        <v>127</v>
+        <v>728</v>
       </c>
       <c r="F915" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="G915" s="8" t="s">
-        <v>279</v>
+      <c r="G915" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="H915" s="3" t="s">
         <v>280</v>
@@ -35057,13 +35060,13 @@
         <v>243</v>
       </c>
       <c r="E916" s="3" t="s">
-        <v>127</v>
+        <v>728</v>
       </c>
       <c r="F916" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="G916" s="8" t="s">
-        <v>279</v>
+      <c r="G916" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="H916" s="3" t="s">
         <v>280</v>
@@ -35091,13 +35094,13 @@
         <v>193</v>
       </c>
       <c r="E917" s="3" t="s">
-        <v>127</v>
+        <v>728</v>
       </c>
       <c r="F917" s="3" t="s">
         <v>991</v>
       </c>
-      <c r="G917" s="8" t="s">
-        <v>279</v>
+      <c r="G917" s="3" t="s">
+        <v>280</v>
       </c>
       <c r="H917" s="3" t="s">
         <v>280</v>
@@ -45641,7 +45644,7 @@
       </c>
       <c r="F1233" s="3"/>
       <c r="G1233" s="8" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="H1233" s="8" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
#42 Time Tracking: updated to 2024-12-17.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10334" uniqueCount="1262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10358" uniqueCount="1263">
   <si>
     <t>Year</t>
   </si>
@@ -3811,6 +3811,9 @@
   </si>
   <si>
     <t>nwtimetracking v4.5.0</t>
+  </si>
+  <si>
+    <t>2024-12-17</t>
   </si>
 </sst>
 </file>
@@ -4214,7 +4217,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1301" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1329" sqref="E1329"/>
+      <selection pane="bottomLeft" activeCell="F1332" sqref="F1332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48745,40 +48748,106 @@
       </c>
     </row>
     <row r="1326" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1326" s="3"/>
-      <c r="B1326" s="3"/>
-      <c r="C1326" s="3"/>
-      <c r="D1326" s="3"/>
-      <c r="E1326" s="3"/>
-      <c r="F1326" s="3"/>
-      <c r="G1326" s="3"/>
-      <c r="H1326" s="3"/>
-      <c r="I1326" s="4"/>
-      <c r="J1326" s="4"/>
+      <c r="A1326" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B1326" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1326" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1326" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1326" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1326" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G1326" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1326" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1326" s="4">
+        <f t="shared" ref="I1326:I1328" si="418">YEAR(A1326)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1326" s="4">
+        <f t="shared" ref="J1326:J1328" si="419">MONTH(A1326)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1327" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1327" s="3"/>
-      <c r="B1327" s="3"/>
-      <c r="C1327" s="3"/>
-      <c r="D1327" s="3"/>
-      <c r="E1327" s="3"/>
-      <c r="F1327" s="3"/>
-      <c r="G1327" s="3"/>
-      <c r="H1327" s="3"/>
-      <c r="I1327" s="4"/>
-      <c r="J1327" s="4"/>
+      <c r="A1327" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B1327" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1327" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1327" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1327" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1327" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G1327" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1327" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1327" s="4">
+        <f t="shared" si="418"/>
+        <v>2024</v>
+      </c>
+      <c r="J1327" s="4">
+        <f t="shared" si="419"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1328" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1328" s="3"/>
-      <c r="B1328" s="3"/>
-      <c r="C1328" s="3"/>
-      <c r="D1328" s="3"/>
-      <c r="E1328" s="3"/>
-      <c r="F1328" s="3"/>
-      <c r="G1328" s="3"/>
-      <c r="H1328" s="3"/>
-      <c r="I1328" s="4"/>
-      <c r="J1328" s="4"/>
+      <c r="A1328" s="3" t="s">
+        <v>1262</v>
+      </c>
+      <c r="B1328" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1328" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1328" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1328" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1328" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G1328" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1328" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1328" s="4">
+        <f t="shared" si="418"/>
+        <v>2024</v>
+      </c>
+      <c r="J1328" s="4">
+        <f t="shared" si="419"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1329" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1329" s="3"/>

</xml_diff>

<commit_message>
#44 Time Tracking: updated to 2024-12-21.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10358" uniqueCount="1263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10430" uniqueCount="1268">
   <si>
     <t>Year</t>
   </si>
@@ -3814,6 +3814,21 @@
   </si>
   <si>
     <t>2024-12-17</t>
+  </si>
+  <si>
+    <t>2024-12-18</t>
+  </si>
+  <si>
+    <t>nwtimetracking v4.6.0</t>
+  </si>
+  <si>
+    <t>2024-12-19</t>
+  </si>
+  <si>
+    <t>2024-12-20</t>
+  </si>
+  <si>
+    <t>2024-12-21</t>
   </si>
 </sst>
 </file>
@@ -4216,8 +4231,8 @@
   <dimension ref="A1:J1352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1301" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1332" sqref="F1332"/>
+      <pane ySplit="1" topLeftCell="A1312" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1338" sqref="A1338"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -48850,112 +48865,310 @@
       </c>
     </row>
     <row r="1329" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1329" s="3"/>
-      <c r="B1329" s="3"/>
-      <c r="C1329" s="3"/>
-      <c r="D1329" s="3"/>
-      <c r="E1329" s="3"/>
-      <c r="F1329" s="3"/>
-      <c r="G1329" s="3"/>
-      <c r="H1329" s="3"/>
-      <c r="I1329" s="4"/>
-      <c r="J1329" s="4"/>
+      <c r="A1329" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B1329" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1329" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1329" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1329" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1329" s="3" t="s">
+        <v>1261</v>
+      </c>
+      <c r="G1329" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1329" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1329" s="4">
+        <f t="shared" ref="I1329:I1330" si="420">YEAR(A1329)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1329" s="4">
+        <f t="shared" ref="J1329:J1330" si="421">MONTH(A1329)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1330" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1330" s="3"/>
-      <c r="B1330" s="3"/>
-      <c r="C1330" s="3"/>
-      <c r="D1330" s="3"/>
-      <c r="E1330" s="3"/>
-      <c r="F1330" s="3"/>
-      <c r="G1330" s="3"/>
-      <c r="H1330" s="3"/>
-      <c r="I1330" s="4"/>
-      <c r="J1330" s="4"/>
+      <c r="A1330" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B1330" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1330" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1330" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1330" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1330" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1330" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1330" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1330" s="4">
+        <f t="shared" si="420"/>
+        <v>2024</v>
+      </c>
+      <c r="J1330" s="4">
+        <f t="shared" si="421"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1331" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1331" s="3"/>
-      <c r="B1331" s="3"/>
-      <c r="C1331" s="3"/>
-      <c r="D1331" s="3"/>
-      <c r="E1331" s="3"/>
-      <c r="F1331" s="3"/>
-      <c r="G1331" s="3"/>
-      <c r="H1331" s="3"/>
-      <c r="I1331" s="4"/>
-      <c r="J1331" s="4"/>
+      <c r="A1331" s="3" t="s">
+        <v>1263</v>
+      </c>
+      <c r="B1331" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1331" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1331" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1331" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1331" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1331" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1331" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1331" s="4">
+        <f t="shared" ref="I1331:I1332" si="422">YEAR(A1331)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1331" s="4">
+        <f t="shared" ref="J1331:J1332" si="423">MONTH(A1331)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1332" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1332" s="3"/>
-      <c r="B1332" s="3"/>
-      <c r="C1332" s="3"/>
-      <c r="D1332" s="3"/>
-      <c r="E1332" s="3"/>
-      <c r="F1332" s="3"/>
-      <c r="G1332" s="3"/>
-      <c r="H1332" s="3"/>
-      <c r="I1332" s="4"/>
-      <c r="J1332" s="4"/>
+      <c r="A1332" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1332" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1332" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1332" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1332" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1332" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1332" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1332" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1332" s="4">
+        <f t="shared" si="422"/>
+        <v>2024</v>
+      </c>
+      <c r="J1332" s="4">
+        <f t="shared" si="423"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1333" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1333" s="3"/>
-      <c r="B1333" s="3"/>
-      <c r="C1333" s="3"/>
-      <c r="D1333" s="3"/>
-      <c r="E1333" s="3"/>
-      <c r="F1333" s="3"/>
-      <c r="G1333" s="3"/>
-      <c r="H1333" s="3"/>
-      <c r="I1333" s="4"/>
-      <c r="J1333" s="4"/>
+      <c r="A1333" s="3" t="s">
+        <v>1265</v>
+      </c>
+      <c r="B1333" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1333" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1333" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1333" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1333" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1333" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1333" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1333" s="4">
+        <f t="shared" ref="I1333" si="424">YEAR(A1333)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1333" s="4">
+        <f t="shared" ref="J1333" si="425">MONTH(A1333)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1334" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1334" s="3"/>
-      <c r="B1334" s="3"/>
-      <c r="C1334" s="3"/>
-      <c r="D1334" s="3"/>
-      <c r="E1334" s="3"/>
-      <c r="F1334" s="3"/>
-      <c r="G1334" s="3"/>
-      <c r="H1334" s="3"/>
-      <c r="I1334" s="4"/>
-      <c r="J1334" s="4"/>
+      <c r="A1334" s="3" t="s">
+        <v>1266</v>
+      </c>
+      <c r="B1334" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1334" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1334" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1334" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1334" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1334" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1334" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1334" s="4">
+        <f t="shared" ref="I1334:I1336" si="426">YEAR(A1334)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1334" s="4">
+        <f t="shared" ref="J1334:J1336" si="427">MONTH(A1334)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1335" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1335" s="3"/>
-      <c r="B1335" s="3"/>
-      <c r="C1335" s="3"/>
-      <c r="D1335" s="3"/>
-      <c r="E1335" s="3"/>
-      <c r="F1335" s="3"/>
-      <c r="G1335" s="3"/>
-      <c r="H1335" s="3"/>
-      <c r="I1335" s="4"/>
-      <c r="J1335" s="4"/>
+      <c r="A1335" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B1335" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1335" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1335" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1335" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1335" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1335" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1335" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1335" s="4">
+        <f t="shared" si="426"/>
+        <v>2024</v>
+      </c>
+      <c r="J1335" s="4">
+        <f t="shared" si="427"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1336" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1336" s="3"/>
-      <c r="B1336" s="3"/>
-      <c r="C1336" s="3"/>
-      <c r="D1336" s="3"/>
-      <c r="E1336" s="3"/>
-      <c r="F1336" s="3"/>
-      <c r="G1336" s="3"/>
-      <c r="H1336" s="3"/>
-      <c r="I1336" s="4"/>
-      <c r="J1336" s="4"/>
+      <c r="A1336" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B1336" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1336" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1336" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1336" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1336" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1336" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1336" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1336" s="4">
+        <f t="shared" si="426"/>
+        <v>2024</v>
+      </c>
+      <c r="J1336" s="4">
+        <f t="shared" si="427"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1337" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1337" s="3"/>
-      <c r="B1337" s="3"/>
-      <c r="C1337" s="3"/>
-      <c r="D1337" s="3"/>
-      <c r="E1337" s="3"/>
-      <c r="F1337" s="3"/>
-      <c r="G1337" s="3"/>
-      <c r="H1337" s="3"/>
-      <c r="I1337" s="4"/>
-      <c r="J1337" s="4"/>
+      <c r="A1337" s="3" t="s">
+        <v>1267</v>
+      </c>
+      <c r="B1337" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1337" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1337" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1337" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1337" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1337" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1337" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1337" s="4">
+        <f t="shared" ref="I1337" si="428">YEAR(A1337)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1337" s="4">
+        <f t="shared" ref="J1337" si="429">MONTH(A1337)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1338" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1338" s="3"/>

</xml_diff>

<commit_message>
#44 Time Tracking: updated to 2024-12-23.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10430" uniqueCount="1268">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10462" uniqueCount="1270">
   <si>
     <t>Year</t>
   </si>
@@ -3829,6 +3829,12 @@
   </si>
   <si>
     <t>2024-12-21</t>
+  </si>
+  <si>
+    <t>2024-12-22</t>
+  </si>
+  <si>
+    <t>2024-12-23</t>
   </si>
 </sst>
 </file>
@@ -4231,8 +4237,8 @@
   <dimension ref="A1:J1352"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1312" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1338" sqref="A1338"/>
+      <pane ySplit="1" topLeftCell="A1318" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1342" sqref="A1342"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -49162,61 +49168,149 @@
         <v>280</v>
       </c>
       <c r="I1337" s="4">
-        <f t="shared" ref="I1337" si="428">YEAR(A1337)</f>
+        <f t="shared" ref="I1337:I1338" si="428">YEAR(A1337)</f>
         <v>2024</v>
       </c>
       <c r="J1337" s="4">
-        <f t="shared" ref="J1337" si="429">MONTH(A1337)</f>
+        <f t="shared" ref="J1337:J1338" si="429">MONTH(A1337)</f>
         <v>12</v>
       </c>
     </row>
     <row r="1338" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1338" s="3"/>
-      <c r="B1338" s="3"/>
-      <c r="C1338" s="3"/>
-      <c r="D1338" s="3"/>
-      <c r="E1338" s="3"/>
-      <c r="F1338" s="3"/>
-      <c r="G1338" s="3"/>
-      <c r="H1338" s="3"/>
-      <c r="I1338" s="4"/>
-      <c r="J1338" s="4"/>
+      <c r="A1338" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B1338" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1338" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1338" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1338" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1338" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1338" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1338" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1338" s="4">
+        <f t="shared" si="428"/>
+        <v>2024</v>
+      </c>
+      <c r="J1338" s="4">
+        <f t="shared" si="429"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1339" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1339" s="3"/>
-      <c r="B1339" s="3"/>
-      <c r="C1339" s="3"/>
-      <c r="D1339" s="3"/>
-      <c r="E1339" s="3"/>
-      <c r="F1339" s="3"/>
-      <c r="G1339" s="3"/>
-      <c r="H1339" s="3"/>
-      <c r="I1339" s="4"/>
-      <c r="J1339" s="4"/>
+      <c r="A1339" s="3" t="s">
+        <v>1268</v>
+      </c>
+      <c r="B1339" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1339" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1339" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1339" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1339" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1339" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1339" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1339" s="4">
+        <f t="shared" ref="I1339:I1340" si="430">YEAR(A1339)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1339" s="4">
+        <f t="shared" ref="J1339:J1340" si="431">MONTH(A1339)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1340" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1340" s="3"/>
-      <c r="B1340" s="3"/>
-      <c r="C1340" s="3"/>
-      <c r="D1340" s="3"/>
-      <c r="E1340" s="3"/>
-      <c r="F1340" s="3"/>
-      <c r="G1340" s="3"/>
-      <c r="H1340" s="3"/>
-      <c r="I1340" s="4"/>
-      <c r="J1340" s="4"/>
+      <c r="A1340" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1340" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1340" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1340" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1340" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1340" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1340" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1340" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1340" s="4">
+        <f t="shared" si="430"/>
+        <v>2024</v>
+      </c>
+      <c r="J1340" s="4">
+        <f t="shared" si="431"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1341" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1341" s="3"/>
-      <c r="B1341" s="3"/>
-      <c r="C1341" s="3"/>
-      <c r="D1341" s="3"/>
-      <c r="E1341" s="3"/>
-      <c r="F1341" s="3"/>
-      <c r="G1341" s="3"/>
-      <c r="H1341" s="3"/>
-      <c r="I1341" s="4"/>
-      <c r="J1341" s="4"/>
+      <c r="A1341" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1341" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1341" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1341" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1341" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1341" s="3" t="s">
+        <v>1264</v>
+      </c>
+      <c r="G1341" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1341" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1341" s="4">
+        <f t="shared" ref="I1341" si="432">YEAR(A1341)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1341" s="4">
+        <f t="shared" ref="J1341" si="433">MONTH(A1341)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1342" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1342" s="3"/>

</xml_diff>

<commit_message>
#46 Time Tracking: updated to 2024-12-24.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10462" uniqueCount="1270">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10510" uniqueCount="1272">
   <si>
     <t>Year</t>
   </si>
@@ -3835,6 +3835,12 @@
   </si>
   <si>
     <t>2024-12-23</t>
+  </si>
+  <si>
+    <t>nwtimetracking v4.7.0</t>
+  </si>
+  <si>
+    <t>2024-12-24</t>
   </si>
 </sst>
 </file>
@@ -4234,11 +4240,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1352"/>
+  <dimension ref="A1:J1379"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1318" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1342" sqref="A1342"/>
+      <pane ySplit="1" topLeftCell="A1323" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1349" sqref="F1349"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -49304,85 +49310,217 @@
         <v>279</v>
       </c>
       <c r="I1341" s="4">
-        <f t="shared" ref="I1341" si="432">YEAR(A1341)</f>
+        <f t="shared" ref="I1341:I1344" si="432">YEAR(A1341)</f>
         <v>2024</v>
       </c>
       <c r="J1341" s="4">
-        <f t="shared" ref="J1341" si="433">MONTH(A1341)</f>
+        <f t="shared" ref="J1341:J1344" si="433">MONTH(A1341)</f>
         <v>12</v>
       </c>
     </row>
     <row r="1342" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1342" s="3"/>
-      <c r="B1342" s="3"/>
-      <c r="C1342" s="3"/>
-      <c r="D1342" s="3"/>
-      <c r="E1342" s="3"/>
-      <c r="F1342" s="3"/>
-      <c r="G1342" s="3"/>
-      <c r="H1342" s="3"/>
-      <c r="I1342" s="4"/>
-      <c r="J1342" s="4"/>
+      <c r="A1342" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1342" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1342" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1342" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1342" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1342" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G1342" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1342" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1342" s="4">
+        <f t="shared" si="432"/>
+        <v>2024</v>
+      </c>
+      <c r="J1342" s="4">
+        <f t="shared" si="433"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1343" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1343" s="3"/>
-      <c r="B1343" s="3"/>
-      <c r="C1343" s="3"/>
-      <c r="D1343" s="3"/>
-      <c r="E1343" s="3"/>
-      <c r="F1343" s="3"/>
-      <c r="G1343" s="3"/>
-      <c r="H1343" s="3"/>
-      <c r="I1343" s="4"/>
-      <c r="J1343" s="4"/>
+      <c r="A1343" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1343" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1343" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1343" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1343" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1343" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G1343" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1343" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1343" s="4">
+        <f t="shared" si="432"/>
+        <v>2024</v>
+      </c>
+      <c r="J1343" s="4">
+        <f t="shared" si="433"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1344" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1344" s="3"/>
-      <c r="B1344" s="3"/>
-      <c r="C1344" s="3"/>
-      <c r="D1344" s="3"/>
-      <c r="E1344" s="3"/>
-      <c r="F1344" s="3"/>
-      <c r="G1344" s="3"/>
-      <c r="H1344" s="3"/>
-      <c r="I1344" s="4"/>
-      <c r="J1344" s="4"/>
+      <c r="A1344" s="3" t="s">
+        <v>1269</v>
+      </c>
+      <c r="B1344" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1344" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1344" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1344" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1344" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G1344" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1344" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1344" s="4">
+        <f t="shared" si="432"/>
+        <v>2024</v>
+      </c>
+      <c r="J1344" s="4">
+        <f t="shared" si="433"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1345" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1345" s="3"/>
-      <c r="B1345" s="3"/>
-      <c r="C1345" s="3"/>
-      <c r="D1345" s="3"/>
-      <c r="E1345" s="3"/>
-      <c r="F1345" s="3"/>
-      <c r="G1345" s="3"/>
-      <c r="H1345" s="3"/>
-      <c r="I1345" s="4"/>
-      <c r="J1345" s="4"/>
+      <c r="A1345" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B1345" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1345" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1345" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1345" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1345" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G1345" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1345" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1345" s="4">
+        <f t="shared" ref="I1345:I1347" si="434">YEAR(A1345)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1345" s="4">
+        <f t="shared" ref="J1345:J1347" si="435">MONTH(A1345)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1346" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1346" s="3"/>
-      <c r="B1346" s="3"/>
-      <c r="C1346" s="3"/>
-      <c r="D1346" s="3"/>
-      <c r="E1346" s="3"/>
-      <c r="F1346" s="3"/>
-      <c r="G1346" s="3"/>
-      <c r="H1346" s="3"/>
-      <c r="I1346" s="4"/>
-      <c r="J1346" s="4"/>
+      <c r="A1346" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B1346" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1346" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1346" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1346" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1346" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G1346" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1346" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1346" s="4">
+        <f t="shared" si="434"/>
+        <v>2024</v>
+      </c>
+      <c r="J1346" s="4">
+        <f t="shared" si="435"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1347" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1347" s="3"/>
-      <c r="B1347" s="3"/>
-      <c r="C1347" s="3"/>
-      <c r="D1347" s="3"/>
-      <c r="E1347" s="3"/>
-      <c r="F1347" s="3"/>
-      <c r="G1347" s="3"/>
-      <c r="H1347" s="3"/>
-      <c r="I1347" s="4"/>
-      <c r="J1347" s="4"/>
+      <c r="A1347" s="3" t="s">
+        <v>1271</v>
+      </c>
+      <c r="B1347" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1347" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1347" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1347" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1347" s="3" t="s">
+        <v>1270</v>
+      </c>
+      <c r="G1347" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1347" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1347" s="4">
+        <f t="shared" si="434"/>
+        <v>2024</v>
+      </c>
+      <c r="J1347" s="4">
+        <f t="shared" si="435"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1348" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1348" s="3"/>
@@ -49444,6 +49582,330 @@
       <c r="I1352" s="4"/>
       <c r="J1352" s="4"/>
     </row>
+    <row r="1353" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1353" s="3"/>
+      <c r="B1353" s="3"/>
+      <c r="C1353" s="3"/>
+      <c r="D1353" s="3"/>
+      <c r="E1353" s="3"/>
+      <c r="F1353" s="3"/>
+      <c r="G1353" s="3"/>
+      <c r="H1353" s="3"/>
+      <c r="I1353" s="4"/>
+      <c r="J1353" s="4"/>
+    </row>
+    <row r="1354" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1354" s="3"/>
+      <c r="B1354" s="3"/>
+      <c r="C1354" s="3"/>
+      <c r="D1354" s="3"/>
+      <c r="E1354" s="3"/>
+      <c r="F1354" s="3"/>
+      <c r="G1354" s="3"/>
+      <c r="H1354" s="3"/>
+      <c r="I1354" s="4"/>
+      <c r="J1354" s="4"/>
+    </row>
+    <row r="1355" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1355" s="3"/>
+      <c r="B1355" s="3"/>
+      <c r="C1355" s="3"/>
+      <c r="D1355" s="3"/>
+      <c r="E1355" s="3"/>
+      <c r="F1355" s="3"/>
+      <c r="G1355" s="3"/>
+      <c r="H1355" s="3"/>
+      <c r="I1355" s="4"/>
+      <c r="J1355" s="4"/>
+    </row>
+    <row r="1356" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1356" s="3"/>
+      <c r="B1356" s="3"/>
+      <c r="C1356" s="3"/>
+      <c r="D1356" s="3"/>
+      <c r="E1356" s="3"/>
+      <c r="F1356" s="3"/>
+      <c r="G1356" s="3"/>
+      <c r="H1356" s="3"/>
+      <c r="I1356" s="4"/>
+      <c r="J1356" s="4"/>
+    </row>
+    <row r="1357" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1357" s="3"/>
+      <c r="B1357" s="3"/>
+      <c r="C1357" s="3"/>
+      <c r="D1357" s="3"/>
+      <c r="E1357" s="3"/>
+      <c r="F1357" s="3"/>
+      <c r="G1357" s="3"/>
+      <c r="H1357" s="3"/>
+      <c r="I1357" s="4"/>
+      <c r="J1357" s="4"/>
+    </row>
+    <row r="1358" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1358" s="3"/>
+      <c r="B1358" s="3"/>
+      <c r="C1358" s="3"/>
+      <c r="D1358" s="3"/>
+      <c r="E1358" s="3"/>
+      <c r="F1358" s="3"/>
+      <c r="G1358" s="3"/>
+      <c r="H1358" s="3"/>
+      <c r="I1358" s="4"/>
+      <c r="J1358" s="4"/>
+    </row>
+    <row r="1359" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1359" s="3"/>
+      <c r="B1359" s="3"/>
+      <c r="C1359" s="3"/>
+      <c r="D1359" s="3"/>
+      <c r="E1359" s="3"/>
+      <c r="F1359" s="3"/>
+      <c r="G1359" s="3"/>
+      <c r="H1359" s="3"/>
+      <c r="I1359" s="4"/>
+      <c r="J1359" s="4"/>
+    </row>
+    <row r="1360" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1360" s="3"/>
+      <c r="B1360" s="3"/>
+      <c r="C1360" s="3"/>
+      <c r="D1360" s="3"/>
+      <c r="E1360" s="3"/>
+      <c r="F1360" s="3"/>
+      <c r="G1360" s="3"/>
+      <c r="H1360" s="3"/>
+      <c r="I1360" s="4"/>
+      <c r="J1360" s="4"/>
+    </row>
+    <row r="1361" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1361" s="3"/>
+      <c r="B1361" s="3"/>
+      <c r="C1361" s="3"/>
+      <c r="D1361" s="3"/>
+      <c r="E1361" s="3"/>
+      <c r="F1361" s="3"/>
+      <c r="G1361" s="3"/>
+      <c r="H1361" s="3"/>
+      <c r="I1361" s="4"/>
+      <c r="J1361" s="4"/>
+    </row>
+    <row r="1362" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1362" s="3"/>
+      <c r="B1362" s="3"/>
+      <c r="C1362" s="3"/>
+      <c r="D1362" s="3"/>
+      <c r="E1362" s="3"/>
+      <c r="F1362" s="3"/>
+      <c r="G1362" s="3"/>
+      <c r="H1362" s="3"/>
+      <c r="I1362" s="4"/>
+      <c r="J1362" s="4"/>
+    </row>
+    <row r="1363" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1363" s="3"/>
+      <c r="B1363" s="3"/>
+      <c r="C1363" s="3"/>
+      <c r="D1363" s="3"/>
+      <c r="E1363" s="3"/>
+      <c r="F1363" s="3"/>
+      <c r="G1363" s="3"/>
+      <c r="H1363" s="3"/>
+      <c r="I1363" s="4"/>
+      <c r="J1363" s="4"/>
+    </row>
+    <row r="1364" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1364" s="3"/>
+      <c r="B1364" s="3"/>
+      <c r="C1364" s="3"/>
+      <c r="D1364" s="3"/>
+      <c r="E1364" s="3"/>
+      <c r="F1364" s="3"/>
+      <c r="G1364" s="3"/>
+      <c r="H1364" s="3"/>
+      <c r="I1364" s="4"/>
+      <c r="J1364" s="4"/>
+    </row>
+    <row r="1365" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1365" s="3"/>
+      <c r="B1365" s="3"/>
+      <c r="C1365" s="3"/>
+      <c r="D1365" s="3"/>
+      <c r="E1365" s="3"/>
+      <c r="F1365" s="3"/>
+      <c r="G1365" s="3"/>
+      <c r="H1365" s="3"/>
+      <c r="I1365" s="4"/>
+      <c r="J1365" s="4"/>
+    </row>
+    <row r="1366" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1366" s="3"/>
+      <c r="B1366" s="3"/>
+      <c r="C1366" s="3"/>
+      <c r="D1366" s="3"/>
+      <c r="E1366" s="3"/>
+      <c r="F1366" s="3"/>
+      <c r="G1366" s="3"/>
+      <c r="H1366" s="3"/>
+      <c r="I1366" s="4"/>
+      <c r="J1366" s="4"/>
+    </row>
+    <row r="1367" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1367" s="3"/>
+      <c r="B1367" s="3"/>
+      <c r="C1367" s="3"/>
+      <c r="D1367" s="3"/>
+      <c r="E1367" s="3"/>
+      <c r="F1367" s="3"/>
+      <c r="G1367" s="3"/>
+      <c r="H1367" s="3"/>
+      <c r="I1367" s="4"/>
+      <c r="J1367" s="4"/>
+    </row>
+    <row r="1368" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1368" s="3"/>
+      <c r="B1368" s="3"/>
+      <c r="C1368" s="3"/>
+      <c r="D1368" s="3"/>
+      <c r="E1368" s="3"/>
+      <c r="F1368" s="3"/>
+      <c r="G1368" s="3"/>
+      <c r="H1368" s="3"/>
+      <c r="I1368" s="4"/>
+      <c r="J1368" s="4"/>
+    </row>
+    <row r="1369" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1369" s="3"/>
+      <c r="B1369" s="3"/>
+      <c r="C1369" s="3"/>
+      <c r="D1369" s="3"/>
+      <c r="E1369" s="3"/>
+      <c r="F1369" s="3"/>
+      <c r="G1369" s="3"/>
+      <c r="H1369" s="3"/>
+      <c r="I1369" s="4"/>
+      <c r="J1369" s="4"/>
+    </row>
+    <row r="1370" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1370" s="3"/>
+      <c r="B1370" s="3"/>
+      <c r="C1370" s="3"/>
+      <c r="D1370" s="3"/>
+      <c r="E1370" s="3"/>
+      <c r="F1370" s="3"/>
+      <c r="G1370" s="3"/>
+      <c r="H1370" s="3"/>
+      <c r="I1370" s="4"/>
+      <c r="J1370" s="4"/>
+    </row>
+    <row r="1371" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1371" s="3"/>
+      <c r="B1371" s="3"/>
+      <c r="C1371" s="3"/>
+      <c r="D1371" s="3"/>
+      <c r="E1371" s="3"/>
+      <c r="F1371" s="3"/>
+      <c r="G1371" s="3"/>
+      <c r="H1371" s="3"/>
+      <c r="I1371" s="4"/>
+      <c r="J1371" s="4"/>
+    </row>
+    <row r="1372" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1372" s="3"/>
+      <c r="B1372" s="3"/>
+      <c r="C1372" s="3"/>
+      <c r="D1372" s="3"/>
+      <c r="E1372" s="3"/>
+      <c r="F1372" s="3"/>
+      <c r="G1372" s="3"/>
+      <c r="H1372" s="3"/>
+      <c r="I1372" s="4"/>
+      <c r="J1372" s="4"/>
+    </row>
+    <row r="1373" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1373" s="3"/>
+      <c r="B1373" s="3"/>
+      <c r="C1373" s="3"/>
+      <c r="D1373" s="3"/>
+      <c r="E1373" s="3"/>
+      <c r="F1373" s="3"/>
+      <c r="G1373" s="3"/>
+      <c r="H1373" s="3"/>
+      <c r="I1373" s="4"/>
+      <c r="J1373" s="4"/>
+    </row>
+    <row r="1374" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1374" s="3"/>
+      <c r="B1374" s="3"/>
+      <c r="C1374" s="3"/>
+      <c r="D1374" s="3"/>
+      <c r="E1374" s="3"/>
+      <c r="F1374" s="3"/>
+      <c r="G1374" s="3"/>
+      <c r="H1374" s="3"/>
+      <c r="I1374" s="4"/>
+      <c r="J1374" s="4"/>
+    </row>
+    <row r="1375" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1375" s="3"/>
+      <c r="B1375" s="3"/>
+      <c r="C1375" s="3"/>
+      <c r="D1375" s="3"/>
+      <c r="E1375" s="3"/>
+      <c r="F1375" s="3"/>
+      <c r="G1375" s="3"/>
+      <c r="H1375" s="3"/>
+      <c r="I1375" s="4"/>
+      <c r="J1375" s="4"/>
+    </row>
+    <row r="1376" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1376" s="3"/>
+      <c r="B1376" s="3"/>
+      <c r="C1376" s="3"/>
+      <c r="D1376" s="3"/>
+      <c r="E1376" s="3"/>
+      <c r="F1376" s="3"/>
+      <c r="G1376" s="3"/>
+      <c r="H1376" s="3"/>
+      <c r="I1376" s="4"/>
+      <c r="J1376" s="4"/>
+    </row>
+    <row r="1377" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1377" s="3"/>
+      <c r="B1377" s="3"/>
+      <c r="C1377" s="3"/>
+      <c r="D1377" s="3"/>
+      <c r="E1377" s="3"/>
+      <c r="F1377" s="3"/>
+      <c r="G1377" s="3"/>
+      <c r="H1377" s="3"/>
+      <c r="I1377" s="4"/>
+      <c r="J1377" s="4"/>
+    </row>
+    <row r="1378" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1378" s="3"/>
+      <c r="B1378" s="3"/>
+      <c r="C1378" s="3"/>
+      <c r="D1378" s="3"/>
+      <c r="E1378" s="3"/>
+      <c r="F1378" s="3"/>
+      <c r="G1378" s="3"/>
+      <c r="H1378" s="3"/>
+      <c r="I1378" s="4"/>
+      <c r="J1378" s="4"/>
+    </row>
+    <row r="1379" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1379" s="3"/>
+      <c r="B1379" s="3"/>
+      <c r="C1379" s="3"/>
+      <c r="D1379" s="3"/>
+      <c r="E1379" s="3"/>
+      <c r="F1379" s="3"/>
+      <c r="G1379" s="3"/>
+      <c r="H1379" s="3"/>
+      <c r="I1379" s="4"/>
+      <c r="J1379" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#48 Time Tracking: updated to 2024-12-26.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10510" uniqueCount="1272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10558" uniqueCount="1275">
   <si>
     <t>Year</t>
   </si>
@@ -3841,6 +3841,15 @@
   </si>
   <si>
     <t>2024-12-24</t>
+  </si>
+  <si>
+    <t>2024-12-25</t>
+  </si>
+  <si>
+    <t>nwtimetracking v4.8.0</t>
+  </si>
+  <si>
+    <t>2024-12-26</t>
   </si>
 </sst>
 </file>
@@ -4243,8 +4252,8 @@
   <dimension ref="A1:J1379"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1323" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1349" sqref="F1349"/>
+      <pane ySplit="1" topLeftCell="A1330" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1356" sqref="E1356"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -49446,11 +49455,11 @@
         <v>279</v>
       </c>
       <c r="I1345" s="4">
-        <f t="shared" ref="I1345:I1347" si="434">YEAR(A1345)</f>
+        <f t="shared" ref="I1345:I1348" si="434">YEAR(A1345)</f>
         <v>2024</v>
       </c>
       <c r="J1345" s="4">
-        <f t="shared" ref="J1345:J1347" si="435">MONTH(A1345)</f>
+        <f t="shared" ref="J1345:J1348" si="435">MONTH(A1345)</f>
         <v>12</v>
       </c>
     </row>
@@ -49523,76 +49532,208 @@
       </c>
     </row>
     <row r="1348" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1348" s="3"/>
-      <c r="B1348" s="3"/>
-      <c r="C1348" s="3"/>
-      <c r="D1348" s="3"/>
-      <c r="E1348" s="3"/>
-      <c r="F1348" s="3"/>
-      <c r="G1348" s="3"/>
-      <c r="H1348" s="3"/>
-      <c r="I1348" s="4"/>
-      <c r="J1348" s="4"/>
+      <c r="A1348" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B1348" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1348" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1348" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1348" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1348" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G1348" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1348" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1348" s="4">
+        <f t="shared" si="434"/>
+        <v>2024</v>
+      </c>
+      <c r="J1348" s="4">
+        <f t="shared" si="435"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1349" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1349" s="3"/>
-      <c r="B1349" s="3"/>
-      <c r="C1349" s="3"/>
-      <c r="D1349" s="3"/>
-      <c r="E1349" s="3"/>
-      <c r="F1349" s="3"/>
-      <c r="G1349" s="3"/>
-      <c r="H1349" s="3"/>
-      <c r="I1349" s="4"/>
-      <c r="J1349" s="4"/>
+      <c r="A1349" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B1349" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1349" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1349" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1349" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1349" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G1349" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1349" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1349" s="4">
+        <f t="shared" ref="I1349:I1351" si="436">YEAR(A1349)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1349" s="4">
+        <f t="shared" ref="J1349:J1351" si="437">MONTH(A1349)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1350" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1350" s="3"/>
-      <c r="B1350" s="3"/>
-      <c r="C1350" s="3"/>
-      <c r="D1350" s="3"/>
-      <c r="E1350" s="3"/>
-      <c r="F1350" s="3"/>
-      <c r="G1350" s="3"/>
-      <c r="H1350" s="3"/>
-      <c r="I1350" s="4"/>
-      <c r="J1350" s="4"/>
+      <c r="A1350" s="3" t="s">
+        <v>1272</v>
+      </c>
+      <c r="B1350" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1350" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1350" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1350" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1350" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G1350" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1350" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1350" s="4">
+        <f t="shared" si="436"/>
+        <v>2024</v>
+      </c>
+      <c r="J1350" s="4">
+        <f t="shared" si="437"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1351" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1351" s="3"/>
-      <c r="B1351" s="3"/>
-      <c r="C1351" s="3"/>
-      <c r="D1351" s="3"/>
-      <c r="E1351" s="3"/>
-      <c r="F1351" s="3"/>
-      <c r="G1351" s="3"/>
-      <c r="H1351" s="3"/>
-      <c r="I1351" s="4"/>
-      <c r="J1351" s="4"/>
+      <c r="A1351" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B1351" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1351" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1351" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1351" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1351" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G1351" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1351" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1351" s="4">
+        <f t="shared" si="436"/>
+        <v>2024</v>
+      </c>
+      <c r="J1351" s="4">
+        <f t="shared" si="437"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1352" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1352" s="3"/>
-      <c r="B1352" s="3"/>
-      <c r="C1352" s="3"/>
-      <c r="D1352" s="3"/>
-      <c r="E1352" s="3"/>
-      <c r="F1352" s="3"/>
-      <c r="G1352" s="3"/>
-      <c r="H1352" s="3"/>
-      <c r="I1352" s="4"/>
-      <c r="J1352" s="4"/>
+      <c r="A1352" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B1352" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1352" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1352" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1352" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1352" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G1352" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1352" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1352" s="4">
+        <f t="shared" ref="I1352:I1353" si="438">YEAR(A1352)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1352" s="4">
+        <f t="shared" ref="J1352:J1353" si="439">MONTH(A1352)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1353" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1353" s="3"/>
-      <c r="B1353" s="3"/>
-      <c r="C1353" s="3"/>
-      <c r="D1353" s="3"/>
-      <c r="E1353" s="3"/>
-      <c r="F1353" s="3"/>
-      <c r="G1353" s="3"/>
-      <c r="H1353" s="3"/>
-      <c r="I1353" s="4"/>
-      <c r="J1353" s="4"/>
+      <c r="A1353" s="3" t="s">
+        <v>1274</v>
+      </c>
+      <c r="B1353" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1353" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1353" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1353" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1353" s="3" t="s">
+        <v>1273</v>
+      </c>
+      <c r="G1353" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1353" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1353" s="4">
+        <f t="shared" si="438"/>
+        <v>2024</v>
+      </c>
+      <c r="J1353" s="4">
+        <f t="shared" si="439"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1354" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1354" s="3"/>

</xml_diff>

<commit_message>
#50 Time Tracking: updated to 2024-12-30.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10558" uniqueCount="1275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10644" uniqueCount="1282">
   <si>
     <t>Year</t>
   </si>
@@ -3850,6 +3850,27 @@
   </si>
   <si>
     <t>2024-12-26</t>
+  </si>
+  <si>
+    <t>2024-12-27</t>
+  </si>
+  <si>
+    <t>nwshared v1.8.1</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.8.1</t>
+  </si>
+  <si>
+    <t>2024-12-28</t>
+  </si>
+  <si>
+    <t>2024-12-29</t>
+  </si>
+  <si>
+    <t>nwtimetracking v5.0.0</t>
+  </si>
+  <si>
+    <t>2024-12-30</t>
   </si>
 </sst>
 </file>
@@ -4252,8 +4273,8 @@
   <dimension ref="A1:J1379"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1330" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1356" sqref="E1356"/>
+      <pane ySplit="1" topLeftCell="A1339" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1368" sqref="H1368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -49736,136 +49757,374 @@
       </c>
     </row>
     <row r="1354" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1354" s="3"/>
-      <c r="B1354" s="3"/>
-      <c r="C1354" s="3"/>
-      <c r="D1354" s="3"/>
-      <c r="E1354" s="3"/>
-      <c r="F1354" s="3"/>
-      <c r="G1354" s="3"/>
-      <c r="H1354" s="3"/>
-      <c r="I1354" s="4"/>
-      <c r="J1354" s="4"/>
+      <c r="A1354" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B1354" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1354" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1354" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1354" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1354" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1354" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1354" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1354" s="4">
+        <f t="shared" ref="I1354:I1359" si="440">YEAR(A1354)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1354" s="4">
+        <f t="shared" ref="J1354:J1359" si="441">MONTH(A1354)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1355" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1355" s="3"/>
-      <c r="B1355" s="3"/>
-      <c r="C1355" s="3"/>
-      <c r="D1355" s="3"/>
-      <c r="E1355" s="3"/>
-      <c r="F1355" s="3"/>
-      <c r="G1355" s="3"/>
-      <c r="H1355" s="3"/>
-      <c r="I1355" s="4"/>
-      <c r="J1355" s="4"/>
+      <c r="A1355" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B1355" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1355" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1355" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1355" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1355" s="3" t="s">
+        <v>1276</v>
+      </c>
+      <c r="G1355" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1355" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1355" s="4">
+        <f t="shared" si="440"/>
+        <v>2024</v>
+      </c>
+      <c r="J1355" s="4">
+        <f t="shared" si="441"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1356" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1356" s="3"/>
-      <c r="B1356" s="3"/>
-      <c r="C1356" s="3"/>
-      <c r="D1356" s="3"/>
-      <c r="E1356" s="3"/>
-      <c r="F1356" s="3"/>
-      <c r="G1356" s="3"/>
-      <c r="H1356" s="3"/>
-      <c r="I1356" s="4"/>
-      <c r="J1356" s="4"/>
+      <c r="A1356" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B1356" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1356" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1356" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1356" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1356" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="G1356" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1356" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1356" s="4">
+        <f t="shared" si="440"/>
+        <v>2024</v>
+      </c>
+      <c r="J1356" s="4">
+        <f t="shared" si="441"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1357" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1357" s="3"/>
-      <c r="B1357" s="3"/>
-      <c r="C1357" s="3"/>
-      <c r="D1357" s="3"/>
-      <c r="E1357" s="3"/>
-      <c r="F1357" s="3"/>
-      <c r="G1357" s="3"/>
-      <c r="H1357" s="3"/>
-      <c r="I1357" s="4"/>
-      <c r="J1357" s="4"/>
+      <c r="A1357" s="3" t="s">
+        <v>1275</v>
+      </c>
+      <c r="B1357" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1357" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1357" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1357" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1357" s="3" t="s">
+        <v>1277</v>
+      </c>
+      <c r="G1357" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1357" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1357" s="4">
+        <f t="shared" si="440"/>
+        <v>2024</v>
+      </c>
+      <c r="J1357" s="4">
+        <f t="shared" si="441"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1358" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1358" s="3"/>
-      <c r="B1358" s="3"/>
-      <c r="C1358" s="3"/>
-      <c r="D1358" s="3"/>
-      <c r="E1358" s="3"/>
+      <c r="A1358" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B1358" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1358" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1358" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1358" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1358" s="3"/>
-      <c r="G1358" s="3"/>
-      <c r="H1358" s="3"/>
-      <c r="I1358" s="4"/>
-      <c r="J1358" s="4"/>
+      <c r="G1358" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1358" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1358" s="4">
+        <f t="shared" si="440"/>
+        <v>2024</v>
+      </c>
+      <c r="J1358" s="4">
+        <f t="shared" si="441"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1359" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1359" s="3"/>
-      <c r="B1359" s="3"/>
-      <c r="C1359" s="3"/>
-      <c r="D1359" s="3"/>
-      <c r="E1359" s="3"/>
+      <c r="A1359" s="3" t="s">
+        <v>1278</v>
+      </c>
+      <c r="B1359" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C1359" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1359" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1359" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1359" s="3"/>
-      <c r="G1359" s="3"/>
-      <c r="H1359" s="3"/>
-      <c r="I1359" s="4"/>
-      <c r="J1359" s="4"/>
+      <c r="G1359" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1359" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1359" s="4">
+        <f t="shared" si="440"/>
+        <v>2024</v>
+      </c>
+      <c r="J1359" s="4">
+        <f t="shared" si="441"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1360" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1360" s="3"/>
-      <c r="B1360" s="3"/>
-      <c r="C1360" s="3"/>
-      <c r="D1360" s="3"/>
-      <c r="E1360" s="3"/>
-      <c r="F1360" s="3"/>
-      <c r="G1360" s="3"/>
-      <c r="H1360" s="3"/>
-      <c r="I1360" s="4"/>
-      <c r="J1360" s="4"/>
+      <c r="A1360" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B1360" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1360" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1360" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1360" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1360" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G1360" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1360" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1360" s="4">
+        <f t="shared" ref="I1360:I1363" si="442">YEAR(A1360)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1360" s="4">
+        <f t="shared" ref="J1360:J1363" si="443">MONTH(A1360)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1361" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1361" s="3"/>
-      <c r="B1361" s="3"/>
-      <c r="C1361" s="3"/>
-      <c r="D1361" s="3"/>
-      <c r="E1361" s="3"/>
-      <c r="F1361" s="3"/>
-      <c r="G1361" s="3"/>
-      <c r="H1361" s="3"/>
-      <c r="I1361" s="4"/>
-      <c r="J1361" s="4"/>
+      <c r="A1361" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B1361" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1361" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1361" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1361" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1361" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G1361" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1361" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1361" s="4">
+        <f t="shared" si="442"/>
+        <v>2024</v>
+      </c>
+      <c r="J1361" s="4">
+        <f t="shared" si="443"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1362" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1362" s="3"/>
-      <c r="B1362" s="3"/>
-      <c r="C1362" s="3"/>
-      <c r="D1362" s="3"/>
-      <c r="E1362" s="3"/>
-      <c r="F1362" s="3"/>
-      <c r="G1362" s="3"/>
-      <c r="H1362" s="3"/>
-      <c r="I1362" s="4"/>
-      <c r="J1362" s="4"/>
+      <c r="A1362" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B1362" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1362" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1362" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1362" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1362" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G1362" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1362" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1362" s="4">
+        <f t="shared" si="442"/>
+        <v>2024</v>
+      </c>
+      <c r="J1362" s="4">
+        <f t="shared" si="443"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1363" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1363" s="3"/>
-      <c r="B1363" s="3"/>
-      <c r="C1363" s="3"/>
-      <c r="D1363" s="3"/>
-      <c r="E1363" s="3"/>
-      <c r="F1363" s="3"/>
-      <c r="G1363" s="3"/>
-      <c r="H1363" s="3"/>
-      <c r="I1363" s="4"/>
-      <c r="J1363" s="4"/>
+      <c r="A1363" s="3" t="s">
+        <v>1279</v>
+      </c>
+      <c r="B1363" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1363" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="D1363" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1363" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1363" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G1363" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1363" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1363" s="4">
+        <f t="shared" si="442"/>
+        <v>2024</v>
+      </c>
+      <c r="J1363" s="4">
+        <f t="shared" si="443"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1364" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1364" s="3"/>
-      <c r="B1364" s="3"/>
-      <c r="C1364" s="3"/>
-      <c r="D1364" s="3"/>
-      <c r="E1364" s="3"/>
-      <c r="F1364" s="3"/>
-      <c r="G1364" s="3"/>
-      <c r="H1364" s="3"/>
-      <c r="I1364" s="4"/>
-      <c r="J1364" s="4"/>
+      <c r="A1364" s="3" t="s">
+        <v>1281</v>
+      </c>
+      <c r="B1364" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1364" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1364" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1364" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1364" s="3" t="s">
+        <v>1280</v>
+      </c>
+      <c r="G1364" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1364" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1364" s="4">
+        <f t="shared" ref="I1364" si="444">YEAR(A1364)</f>
+        <v>2024</v>
+      </c>
+      <c r="J1364" s="4">
+        <f t="shared" ref="J1364" si="445">MONTH(A1364)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1365" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1365" s="3"/>

</xml_diff>

<commit_message>
#52 Time Tracking: updated to 2024-01-01.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10644" uniqueCount="1282">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10658" uniqueCount="1284">
   <si>
     <t>Year</t>
   </si>
@@ -3871,6 +3871,12 @@
   </si>
   <si>
     <t>2024-12-30</t>
+  </si>
+  <si>
+    <t>2024-12-31</t>
+  </si>
+  <si>
+    <t>2025-01-01</t>
   </si>
 </sst>
 </file>
@@ -4274,7 +4280,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1339" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1367" sqref="D1367"/>
+      <selection pane="bottomLeft" activeCell="E1369" sqref="E1369"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -50118,37 +50124,77 @@
         <v>279</v>
       </c>
       <c r="I1364" s="4">
-        <f t="shared" ref="I1364" si="444">YEAR(A1364)</f>
+        <f t="shared" ref="I1364:I1366" si="444">YEAR(A1364)</f>
         <v>2024</v>
       </c>
       <c r="J1364" s="4">
-        <f t="shared" ref="J1364" si="445">MONTH(A1364)</f>
+        <f t="shared" ref="J1364:J1366" si="445">MONTH(A1364)</f>
         <v>12</v>
       </c>
     </row>
     <row r="1365" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1365" s="3"/>
-      <c r="B1365" s="3"/>
-      <c r="C1365" s="3"/>
-      <c r="D1365" s="3"/>
-      <c r="E1365" s="3"/>
+      <c r="A1365" s="3" t="s">
+        <v>1282</v>
+      </c>
+      <c r="B1365" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1365" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1365" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="E1365" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1365" s="3"/>
-      <c r="G1365" s="3"/>
-      <c r="H1365" s="3"/>
-      <c r="I1365" s="4"/>
-      <c r="J1365" s="4"/>
+      <c r="G1365" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1365" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1365" s="4">
+        <f t="shared" si="444"/>
+        <v>2024</v>
+      </c>
+      <c r="J1365" s="4">
+        <f t="shared" si="445"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1366" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1366" s="3"/>
-      <c r="B1366" s="3"/>
-      <c r="C1366" s="3"/>
-      <c r="D1366" s="3"/>
-      <c r="E1366" s="3"/>
+      <c r="A1366" s="3" t="s">
+        <v>1283</v>
+      </c>
+      <c r="B1366" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1366" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1366" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1366" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1366" s="3"/>
-      <c r="G1366" s="3"/>
-      <c r="H1366" s="3"/>
-      <c r="I1366" s="4"/>
-      <c r="J1366" s="4"/>
+      <c r="G1366" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1366" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1366" s="4">
+        <f t="shared" ref="I1366" si="446">YEAR(A1366)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1366" s="4">
+        <f t="shared" ref="J1366" si="447">MONTH(A1366)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="1367" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1367" s="3"/>

</xml_diff>

<commit_message>
#52 Time Tracking: updated to 2025-01-06.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10658" uniqueCount="1284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10705" uniqueCount="1289">
   <si>
     <t>Year</t>
   </si>
@@ -3877,6 +3877,21 @@
   </si>
   <si>
     <t>2025-01-01</t>
+  </si>
+  <si>
+    <t>2025-01-02</t>
+  </si>
+  <si>
+    <t>nwknowledgebase v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-01-05</t>
+  </si>
+  <si>
+    <t>nwtimetracking v5.0.1</t>
+  </si>
+  <si>
+    <t>2025-01-06</t>
   </si>
 </sst>
 </file>
@@ -4280,7 +4295,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1339" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1369" sqref="E1369"/>
+      <selection pane="bottomLeft" activeCell="H1375" sqref="H1375"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -50124,11 +50139,11 @@
         <v>279</v>
       </c>
       <c r="I1364" s="4">
-        <f t="shared" ref="I1364:I1366" si="444">YEAR(A1364)</f>
+        <f t="shared" ref="I1364:I1365" si="444">YEAR(A1364)</f>
         <v>2024</v>
       </c>
       <c r="J1364" s="4">
-        <f t="shared" ref="J1364:J1366" si="445">MONTH(A1364)</f>
+        <f t="shared" ref="J1364:J1365" si="445">MONTH(A1364)</f>
         <v>12</v>
       </c>
     </row>
@@ -50188,85 +50203,215 @@
         <v>280</v>
       </c>
       <c r="I1366" s="4">
-        <f t="shared" ref="I1366" si="446">YEAR(A1366)</f>
+        <f t="shared" ref="I1366:I1369" si="446">YEAR(A1366)</f>
         <v>2025</v>
       </c>
       <c r="J1366" s="4">
-        <f t="shared" ref="J1366" si="447">MONTH(A1366)</f>
+        <f t="shared" ref="J1366:J1369" si="447">MONTH(A1366)</f>
         <v>1</v>
       </c>
     </row>
     <row r="1367" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1367" s="3"/>
-      <c r="B1367" s="3"/>
-      <c r="C1367" s="3"/>
-      <c r="D1367" s="3"/>
-      <c r="E1367" s="3"/>
-      <c r="F1367" s="3"/>
-      <c r="G1367" s="3"/>
-      <c r="H1367" s="3"/>
-      <c r="I1367" s="4"/>
-      <c r="J1367" s="4"/>
+      <c r="A1367" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B1367" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1367" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1367" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1367" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1367" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1367" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1367" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1367" s="4">
+        <f t="shared" si="446"/>
+        <v>2025</v>
+      </c>
+      <c r="J1367" s="4">
+        <f t="shared" si="447"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1368" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1368" s="3"/>
-      <c r="B1368" s="3"/>
-      <c r="C1368" s="3"/>
-      <c r="D1368" s="3"/>
-      <c r="E1368" s="3"/>
-      <c r="F1368" s="3"/>
-      <c r="G1368" s="3"/>
-      <c r="H1368" s="3"/>
-      <c r="I1368" s="4"/>
-      <c r="J1368" s="4"/>
+      <c r="A1368" s="3" t="s">
+        <v>1284</v>
+      </c>
+      <c r="B1368" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1368" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1368" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1368" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1368" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1368" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1368" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1368" s="4">
+        <f t="shared" si="446"/>
+        <v>2025</v>
+      </c>
+      <c r="J1368" s="4">
+        <f t="shared" si="447"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1369" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1369" s="3"/>
-      <c r="B1369" s="3"/>
-      <c r="C1369" s="3"/>
-      <c r="D1369" s="3"/>
-      <c r="E1369" s="3"/>
+      <c r="A1369" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B1369" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1369" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1369" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1369" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1369" s="3"/>
-      <c r="G1369" s="3"/>
-      <c r="H1369" s="3"/>
-      <c r="I1369" s="4"/>
-      <c r="J1369" s="4"/>
+      <c r="G1369" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1369" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1369" s="4">
+        <f t="shared" si="446"/>
+        <v>2025</v>
+      </c>
+      <c r="J1369" s="4">
+        <f t="shared" si="447"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1370" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1370" s="3"/>
-      <c r="B1370" s="3"/>
-      <c r="C1370" s="3"/>
-      <c r="D1370" s="3"/>
-      <c r="E1370" s="3"/>
-      <c r="F1370" s="3"/>
-      <c r="G1370" s="3"/>
-      <c r="H1370" s="3"/>
-      <c r="I1370" s="4"/>
-      <c r="J1370" s="4"/>
+      <c r="A1370" s="3" t="s">
+        <v>1286</v>
+      </c>
+      <c r="B1370" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1370" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1370" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1370" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1370" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="G1370" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1370" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1370" s="4">
+        <f t="shared" ref="I1370:I1371" si="448">YEAR(A1370)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1370" s="4">
+        <f t="shared" ref="J1370:J1371" si="449">MONTH(A1370)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="1371" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1371" s="3"/>
-      <c r="B1371" s="3"/>
-      <c r="C1371" s="3"/>
-      <c r="D1371" s="3"/>
-      <c r="E1371" s="3"/>
-      <c r="F1371" s="3"/>
-      <c r="G1371" s="3"/>
-      <c r="H1371" s="3"/>
-      <c r="I1371" s="4"/>
-      <c r="J1371" s="4"/>
+      <c r="A1371" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B1371" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1371" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1371" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1371" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1371" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="G1371" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1371" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1371" s="4">
+        <f t="shared" si="448"/>
+        <v>2025</v>
+      </c>
+      <c r="J1371" s="4">
+        <f t="shared" si="449"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1372" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1372" s="3"/>
-      <c r="B1372" s="3"/>
-      <c r="C1372" s="3"/>
-      <c r="D1372" s="3"/>
-      <c r="E1372" s="3"/>
-      <c r="F1372" s="3"/>
-      <c r="G1372" s="3"/>
-      <c r="H1372" s="3"/>
-      <c r="I1372" s="4"/>
-      <c r="J1372" s="4"/>
+      <c r="A1372" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B1372" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1372" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1372" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1372" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1372" s="3" t="s">
+        <v>1287</v>
+      </c>
+      <c r="G1372" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1372" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1372" s="4">
+        <f t="shared" ref="I1372" si="450">YEAR(A1372)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1372" s="4">
+        <f t="shared" ref="J1372" si="451">MONTH(A1372)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="1373" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1373" s="3"/>

</xml_diff>

<commit_message>
#54 Time Tracking: updated to 2025-02-16.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10705" uniqueCount="1289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11041" uniqueCount="1317">
   <si>
     <t>Year</t>
   </si>
@@ -3892,6 +3892,90 @@
   </si>
   <si>
     <t>2025-01-06</t>
+  </si>
+  <si>
+    <t>2025-01-07</t>
+  </si>
+  <si>
+    <t>2025-01-13</t>
+  </si>
+  <si>
+    <t>2025-01-14</t>
+  </si>
+  <si>
+    <t>#duckdb</t>
+  </si>
+  <si>
+    <t>apolloanalytics v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-01-18</t>
+  </si>
+  <si>
+    <t>2025-01-19</t>
+  </si>
+  <si>
+    <t>2025-01-20</t>
+  </si>
+  <si>
+    <t>2025-01-21</t>
+  </si>
+  <si>
+    <t>2025-01-23</t>
+  </si>
+  <si>
+    <t>2025-01-25</t>
+  </si>
+  <si>
+    <t>2025-01-26</t>
+  </si>
+  <si>
+    <t>2025-01-27</t>
+  </si>
+  <si>
+    <t>2025-01-28</t>
+  </si>
+  <si>
+    <t>2025-01-29</t>
+  </si>
+  <si>
+    <t>2025-02-01</t>
+  </si>
+  <si>
+    <t>2025-02-02</t>
+  </si>
+  <si>
+    <t>6h 15m</t>
+  </si>
+  <si>
+    <t>2025-02-03</t>
+  </si>
+  <si>
+    <t>2025-02-04</t>
+  </si>
+  <si>
+    <t>2025-02-05</t>
+  </si>
+  <si>
+    <t>2025-02-06</t>
+  </si>
+  <si>
+    <t>2025-02-07</t>
+  </si>
+  <si>
+    <t>2025-02-11</t>
+  </si>
+  <si>
+    <t>2025-02-12</t>
+  </si>
+  <si>
+    <t>2025-02-13</t>
+  </si>
+  <si>
+    <t>2025-02-15</t>
+  </si>
+  <si>
+    <t>2025-02-16</t>
   </si>
 </sst>
 </file>
@@ -4291,11 +4375,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1379"/>
+  <dimension ref="A1:J1437"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1339" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1375" sqref="H1375"/>
+      <pane ySplit="1" topLeftCell="A1379" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1396" sqref="F1396"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -50405,97 +50489,1723 @@
         <v>279</v>
       </c>
       <c r="I1372" s="4">
-        <f t="shared" ref="I1372" si="450">YEAR(A1372)</f>
+        <f t="shared" ref="I1372:I1374" si="450">YEAR(A1372)</f>
         <v>2025</v>
       </c>
       <c r="J1372" s="4">
-        <f t="shared" ref="J1372" si="451">MONTH(A1372)</f>
+        <f t="shared" ref="J1372:J1374" si="451">MONTH(A1372)</f>
         <v>1</v>
       </c>
     </row>
     <row r="1373" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1373" s="3"/>
-      <c r="B1373" s="3"/>
-      <c r="C1373" s="3"/>
-      <c r="D1373" s="3"/>
-      <c r="E1373" s="3"/>
+      <c r="A1373" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B1373" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1373" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1373" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1373" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1373" s="3"/>
-      <c r="G1373" s="3"/>
-      <c r="H1373" s="3"/>
-      <c r="I1373" s="4"/>
-      <c r="J1373" s="4"/>
+      <c r="G1373" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1373" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1373" s="4">
+        <f t="shared" si="450"/>
+        <v>2025</v>
+      </c>
+      <c r="J1373" s="4">
+        <f t="shared" si="451"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1374" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1374" s="3"/>
-      <c r="B1374" s="3"/>
-      <c r="C1374" s="3"/>
-      <c r="D1374" s="3"/>
-      <c r="E1374" s="3"/>
+      <c r="A1374" s="3" t="s">
+        <v>1288</v>
+      </c>
+      <c r="B1374" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1374" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1374" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1374" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1374" s="3"/>
-      <c r="G1374" s="3"/>
-      <c r="H1374" s="3"/>
-      <c r="I1374" s="4"/>
-      <c r="J1374" s="4"/>
+      <c r="G1374" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1374" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1374" s="4">
+        <f t="shared" si="450"/>
+        <v>2025</v>
+      </c>
+      <c r="J1374" s="4">
+        <f t="shared" si="451"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1375" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1375" s="3"/>
-      <c r="B1375" s="3"/>
-      <c r="C1375" s="3"/>
-      <c r="D1375" s="3"/>
-      <c r="E1375" s="3"/>
+      <c r="A1375" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B1375" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1375" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1375" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1375" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1375" s="3"/>
-      <c r="G1375" s="3"/>
-      <c r="H1375" s="3"/>
-      <c r="I1375" s="4"/>
-      <c r="J1375" s="4"/>
+      <c r="G1375" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1375" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1375" s="4">
+        <f t="shared" ref="I1375:I1377" si="452">YEAR(A1375)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1375" s="4">
+        <f t="shared" ref="J1375:J1377" si="453">MONTH(A1375)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="1376" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1376" s="3"/>
-      <c r="B1376" s="3"/>
-      <c r="C1376" s="3"/>
-      <c r="D1376" s="3"/>
-      <c r="E1376" s="3"/>
+      <c r="A1376" s="3" t="s">
+        <v>1289</v>
+      </c>
+      <c r="B1376" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1376" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1376" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1376" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1376" s="3"/>
-      <c r="G1376" s="3"/>
-      <c r="H1376" s="3"/>
-      <c r="I1376" s="4"/>
-      <c r="J1376" s="4"/>
+      <c r="G1376" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1376" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1376" s="4">
+        <f t="shared" si="452"/>
+        <v>2025</v>
+      </c>
+      <c r="J1376" s="4">
+        <f t="shared" si="453"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1377" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1377" s="3"/>
-      <c r="B1377" s="3"/>
-      <c r="C1377" s="3"/>
-      <c r="D1377" s="3"/>
-      <c r="E1377" s="3"/>
-      <c r="F1377" s="3"/>
-      <c r="G1377" s="3"/>
-      <c r="H1377" s="3"/>
-      <c r="I1377" s="4"/>
-      <c r="J1377" s="4"/>
+      <c r="A1377" s="3" t="s">
+        <v>1290</v>
+      </c>
+      <c r="B1377" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1377" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1377" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1377" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1377" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1377" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1377" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1377" s="4">
+        <f t="shared" si="452"/>
+        <v>2025</v>
+      </c>
+      <c r="J1377" s="4">
+        <f t="shared" si="453"/>
+        <v>1</v>
+      </c>
     </row>
     <row r="1378" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1378" s="3"/>
-      <c r="B1378" s="3"/>
-      <c r="C1378" s="3"/>
-      <c r="D1378" s="3"/>
-      <c r="E1378" s="3"/>
-      <c r="F1378" s="3"/>
-      <c r="G1378" s="3"/>
-      <c r="H1378" s="3"/>
-      <c r="I1378" s="4"/>
-      <c r="J1378" s="4"/>
+      <c r="A1378" s="3" t="s">
+        <v>1291</v>
+      </c>
+      <c r="B1378" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1378" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1378" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1378" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1378" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1378" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1378" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1378" s="4">
+        <f t="shared" ref="I1378" si="454">YEAR(A1378)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1378" s="4">
+        <f t="shared" ref="J1378" si="455">MONTH(A1378)</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="1379" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1379" s="3"/>
-      <c r="B1379" s="3"/>
-      <c r="C1379" s="3"/>
-      <c r="D1379" s="3"/>
-      <c r="E1379" s="3"/>
-      <c r="F1379" s="3"/>
-      <c r="G1379" s="3"/>
-      <c r="H1379" s="3"/>
-      <c r="I1379" s="4"/>
-      <c r="J1379" s="4"/>
+      <c r="A1379" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B1379" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1379" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1379" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1379" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1379" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1379" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1379" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1379" s="4">
+        <f t="shared" ref="I1379:I1380" si="456">YEAR(A1379)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1379" s="4">
+        <f t="shared" ref="J1379:J1380" si="457">MONTH(A1379)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1380" s="3" t="s">
+        <v>1294</v>
+      </c>
+      <c r="B1380" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1380" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1380" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1380" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1380" s="3"/>
+      <c r="G1380" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1380" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1380" s="4">
+        <f t="shared" si="456"/>
+        <v>2025</v>
+      </c>
+      <c r="J1380" s="4">
+        <f t="shared" si="457"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1381" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B1381" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1381" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1381" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1381" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1381" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1381" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1381" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1381" s="4">
+        <f t="shared" ref="I1381:I1383" si="458">YEAR(A1381)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1381" s="4">
+        <f t="shared" ref="J1381:J1383" si="459">MONTH(A1381)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1382" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B1382" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1382" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1382" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1382" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1382" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1382" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1382" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1382" s="4">
+        <f t="shared" si="458"/>
+        <v>2025</v>
+      </c>
+      <c r="J1382" s="4">
+        <f t="shared" si="459"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1383" s="3" t="s">
+        <v>1295</v>
+      </c>
+      <c r="B1383" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1383" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1383" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1383" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1383" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1383" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1383" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1383" s="4">
+        <f t="shared" si="458"/>
+        <v>2025</v>
+      </c>
+      <c r="J1383" s="4">
+        <f t="shared" si="459"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1384" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B1384" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1384" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1384" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1384" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1384" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1384" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1384" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1384" s="4">
+        <f t="shared" ref="I1384:I1385" si="460">YEAR(A1384)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1384" s="4">
+        <f t="shared" ref="J1384:J1385" si="461">MONTH(A1384)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1385" s="3" t="s">
+        <v>1296</v>
+      </c>
+      <c r="B1385" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1385" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="D1385" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1385" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1385" s="3"/>
+      <c r="G1385" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1385" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1385" s="4">
+        <f t="shared" si="460"/>
+        <v>2025</v>
+      </c>
+      <c r="J1385" s="4">
+        <f t="shared" si="461"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1386" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B1386" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1386" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1386" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1386" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1386" s="3"/>
+      <c r="G1386" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1386" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1386" s="4">
+        <f t="shared" ref="I1386:I1389" si="462">YEAR(A1386)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1386" s="4">
+        <f t="shared" ref="J1386:J1389" si="463">MONTH(A1386)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1387" s="3" t="s">
+        <v>1297</v>
+      </c>
+      <c r="B1387" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1387" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1387" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1387" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1387" s="3"/>
+      <c r="G1387" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1387" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1387" s="4">
+        <f t="shared" si="462"/>
+        <v>2025</v>
+      </c>
+      <c r="J1387" s="4">
+        <f t="shared" si="463"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1388" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B1388" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1388" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1388" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1388" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1388" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1388" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1388" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1388" s="4">
+        <f t="shared" si="462"/>
+        <v>2025</v>
+      </c>
+      <c r="J1388" s="4">
+        <f t="shared" si="463"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1389" s="3" t="s">
+        <v>1298</v>
+      </c>
+      <c r="B1389" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1389" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1389" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1389" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1389" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1389" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1389" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1389" s="4">
+        <f t="shared" si="462"/>
+        <v>2025</v>
+      </c>
+      <c r="J1389" s="4">
+        <f t="shared" si="463"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1390" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B1390" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1390" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1390" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="E1390" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1390" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1390" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1390" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1390" s="4">
+        <f t="shared" ref="I1390:I1393" si="464">YEAR(A1390)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1390" s="4">
+        <f t="shared" ref="J1390:J1393" si="465">MONTH(A1390)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1391" s="3" t="s">
+        <v>1299</v>
+      </c>
+      <c r="B1391" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1391" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1391" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1391" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1391" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1391" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1391" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1391" s="4">
+        <f t="shared" si="464"/>
+        <v>2025</v>
+      </c>
+      <c r="J1391" s="4">
+        <f t="shared" si="465"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1392" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B1392" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1392" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1392" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1392" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1392" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1392" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1392" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1392" s="4">
+        <f t="shared" si="464"/>
+        <v>2025</v>
+      </c>
+      <c r="J1392" s="4">
+        <f t="shared" si="465"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1393" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1393" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B1393" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1393" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1393" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1393" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1393" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1393" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1393" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1393" s="4">
+        <f t="shared" si="464"/>
+        <v>2025</v>
+      </c>
+      <c r="J1393" s="4">
+        <f t="shared" si="465"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1394" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B1394" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1394" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1394" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1394" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1394" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1394" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1394" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1394" s="4">
+        <f t="shared" ref="I1394:I1395" si="466">YEAR(A1394)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1394" s="4">
+        <f t="shared" ref="J1394:J1395" si="467">MONTH(A1394)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1395" s="3" t="s">
+        <v>1300</v>
+      </c>
+      <c r="B1395" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1395" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1395" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1395" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1395" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1395" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1395" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1395" s="4">
+        <f t="shared" si="466"/>
+        <v>2025</v>
+      </c>
+      <c r="J1395" s="4">
+        <f t="shared" si="467"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1396" s="3" t="s">
+        <v>1301</v>
+      </c>
+      <c r="B1396" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1396" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1396" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1396" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1396" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1396" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1396" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1396" s="4">
+        <f t="shared" ref="I1396:I1397" si="468">YEAR(A1396)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1396" s="4">
+        <f t="shared" ref="J1396:J1397" si="469">MONTH(A1396)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1397" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B1397" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1397" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1397" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1397" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1397" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1397" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1397" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1397" s="4">
+        <f t="shared" si="468"/>
+        <v>2025</v>
+      </c>
+      <c r="J1397" s="4">
+        <f t="shared" si="469"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1398" s="3" t="s">
+        <v>1302</v>
+      </c>
+      <c r="B1398" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1398" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1398" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1398" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1398" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1398" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1398" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1398" s="4">
+        <f t="shared" ref="I1398" si="470">YEAR(A1398)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1398" s="4">
+        <f t="shared" ref="J1398" si="471">MONTH(A1398)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1399" s="3" t="s">
+        <v>1303</v>
+      </c>
+      <c r="B1399" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1399" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1399" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1399" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1399" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1399" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1399" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1399" s="4">
+        <f t="shared" ref="I1399" si="472">YEAR(A1399)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1399" s="4">
+        <f t="shared" ref="J1399" si="473">MONTH(A1399)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1400" s="3" t="s">
+        <v>1304</v>
+      </c>
+      <c r="B1400" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1400" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1400" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1400" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1400" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1400" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1400" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1400" s="4">
+        <f t="shared" ref="I1400:I1402" si="474">YEAR(A1400)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1400" s="4">
+        <f t="shared" ref="J1400:J1402" si="475">MONTH(A1400)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1401" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1401" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1401" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1401" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1401" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1401" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1401" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1401" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1401" s="4">
+        <f t="shared" si="474"/>
+        <v>2025</v>
+      </c>
+      <c r="J1401" s="4">
+        <f t="shared" si="475"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1402" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1402" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1402" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1402" s="3" t="s">
+        <v>1306</v>
+      </c>
+      <c r="E1402" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1402" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1402" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1402" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1402" s="4">
+        <f t="shared" si="474"/>
+        <v>2025</v>
+      </c>
+      <c r="J1402" s="4">
+        <f t="shared" si="475"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1403" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="B1403" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1403" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1403" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1403" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1403" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1403" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1403" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1403" s="4">
+        <f t="shared" ref="I1403:I1404" si="476">YEAR(A1403)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1403" s="4">
+        <f t="shared" ref="J1403:J1404" si="477">MONTH(A1403)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1404" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B1404" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1404" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1404" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1404" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1404" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1404" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1404" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1404" s="4">
+        <f t="shared" si="476"/>
+        <v>2025</v>
+      </c>
+      <c r="J1404" s="4">
+        <f t="shared" si="477"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1405" s="3" t="s">
+        <v>1307</v>
+      </c>
+      <c r="B1405" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1405" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1405" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1405" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1405" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1405" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1405" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1405" s="4">
+        <f t="shared" ref="I1405" si="478">YEAR(A1405)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1405" s="4">
+        <f t="shared" ref="J1405" si="479">MONTH(A1405)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1406" s="3" t="s">
+        <v>1308</v>
+      </c>
+      <c r="B1406" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1406" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1406" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1406" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1406" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1406" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1406" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1406" s="4">
+        <f t="shared" ref="I1406" si="480">YEAR(A1406)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1406" s="4">
+        <f t="shared" ref="J1406" si="481">MONTH(A1406)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1407" s="3" t="s">
+        <v>1309</v>
+      </c>
+      <c r="B1407" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1407" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1407" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1407" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1407" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1407" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1407" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1407" s="4">
+        <f t="shared" ref="I1407" si="482">YEAR(A1407)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1407" s="4">
+        <f t="shared" ref="J1407" si="483">MONTH(A1407)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1408" s="3" t="s">
+        <v>1310</v>
+      </c>
+      <c r="B1408" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1408" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1408" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1408" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1408" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1408" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1408" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1408" s="4">
+        <f t="shared" ref="I1408:I1409" si="484">YEAR(A1408)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1408" s="4">
+        <f t="shared" ref="J1408:J1409" si="485">MONTH(A1408)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1409" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B1409" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1409" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1409" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1409" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1409" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1409" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1409" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1409" s="4">
+        <f t="shared" si="484"/>
+        <v>2025</v>
+      </c>
+      <c r="J1409" s="4">
+        <f t="shared" si="485"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1410" s="3" t="s">
+        <v>1311</v>
+      </c>
+      <c r="B1410" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1410" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1410" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1410" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1410" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1410" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1410" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1410" s="4">
+        <f t="shared" ref="I1410" si="486">YEAR(A1410)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1410" s="4">
+        <f t="shared" ref="J1410" si="487">MONTH(A1410)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1411" s="3" t="s">
+        <v>1312</v>
+      </c>
+      <c r="B1411" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1411" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1411" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1411" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1411" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1411" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1411" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1411" s="4">
+        <f t="shared" ref="I1411" si="488">YEAR(A1411)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1411" s="4">
+        <f t="shared" ref="J1411" si="489">MONTH(A1411)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1412" s="3" t="s">
+        <v>1313</v>
+      </c>
+      <c r="B1412" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1412" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1412" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1412" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1412" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1412" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1412" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1412" s="4">
+        <f t="shared" ref="I1412" si="490">YEAR(A1412)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1412" s="4">
+        <f t="shared" ref="J1412" si="491">MONTH(A1412)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1413" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1413" s="3" t="s">
+        <v>1314</v>
+      </c>
+      <c r="B1413" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1413" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1413" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1413" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1413" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1413" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1413" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1413" s="4">
+        <f t="shared" ref="I1413:I1414" si="492">YEAR(A1413)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1413" s="4">
+        <f t="shared" ref="J1413:J1414" si="493">MONTH(A1413)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1414" s="3" t="s">
+        <v>1315</v>
+      </c>
+      <c r="B1414" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1414" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1414" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1414" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1414" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1414" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1414" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1414" s="4">
+        <f t="shared" si="492"/>
+        <v>2025</v>
+      </c>
+      <c r="J1414" s="4">
+        <f t="shared" si="493"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1415" s="3" t="s">
+        <v>1316</v>
+      </c>
+      <c r="B1415" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1415" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1415" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1415" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1415" s="3" t="s">
+        <v>1293</v>
+      </c>
+      <c r="G1415" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1415" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1415" s="4">
+        <f t="shared" ref="I1415" si="494">YEAR(A1415)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1415" s="4">
+        <f t="shared" ref="J1415" si="495">MONTH(A1415)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1416" s="3"/>
+      <c r="B1416" s="3"/>
+      <c r="C1416" s="3"/>
+      <c r="D1416" s="3"/>
+      <c r="E1416" s="3"/>
+      <c r="F1416" s="3"/>
+      <c r="G1416" s="3"/>
+      <c r="H1416" s="3"/>
+      <c r="I1416" s="4"/>
+      <c r="J1416" s="4"/>
+    </row>
+    <row r="1417" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1417" s="3"/>
+      <c r="B1417" s="3"/>
+      <c r="C1417" s="3"/>
+      <c r="D1417" s="3"/>
+      <c r="E1417" s="3"/>
+      <c r="F1417" s="3"/>
+      <c r="G1417" s="3"/>
+      <c r="H1417" s="3"/>
+      <c r="I1417" s="4"/>
+      <c r="J1417" s="4"/>
+    </row>
+    <row r="1418" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1418" s="3"/>
+      <c r="B1418" s="3"/>
+      <c r="C1418" s="3"/>
+      <c r="D1418" s="3"/>
+      <c r="E1418" s="3"/>
+      <c r="F1418" s="3"/>
+      <c r="G1418" s="3"/>
+      <c r="H1418" s="3"/>
+      <c r="I1418" s="4"/>
+      <c r="J1418" s="4"/>
+    </row>
+    <row r="1419" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1419" s="3"/>
+      <c r="B1419" s="3"/>
+      <c r="C1419" s="3"/>
+      <c r="D1419" s="3"/>
+      <c r="E1419" s="3"/>
+      <c r="F1419" s="3"/>
+      <c r="G1419" s="3"/>
+      <c r="H1419" s="3"/>
+      <c r="I1419" s="4"/>
+      <c r="J1419" s="4"/>
+    </row>
+    <row r="1420" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1420" s="3"/>
+      <c r="B1420" s="3"/>
+      <c r="C1420" s="3"/>
+      <c r="D1420" s="3"/>
+      <c r="E1420" s="3"/>
+      <c r="F1420" s="3"/>
+      <c r="G1420" s="3"/>
+      <c r="H1420" s="3"/>
+      <c r="I1420" s="4"/>
+      <c r="J1420" s="4"/>
+    </row>
+    <row r="1421" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1421" s="3"/>
+      <c r="B1421" s="3"/>
+      <c r="C1421" s="3"/>
+      <c r="D1421" s="3"/>
+      <c r="E1421" s="3"/>
+      <c r="F1421" s="3"/>
+      <c r="G1421" s="3"/>
+      <c r="H1421" s="3"/>
+      <c r="I1421" s="4"/>
+      <c r="J1421" s="4"/>
+    </row>
+    <row r="1422" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1422" s="3"/>
+      <c r="B1422" s="3"/>
+      <c r="C1422" s="3"/>
+      <c r="D1422" s="3"/>
+      <c r="E1422" s="3"/>
+      <c r="F1422" s="3"/>
+      <c r="G1422" s="3"/>
+      <c r="H1422" s="3"/>
+      <c r="I1422" s="4"/>
+      <c r="J1422" s="4"/>
+    </row>
+    <row r="1423" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1423" s="3"/>
+      <c r="B1423" s="3"/>
+      <c r="C1423" s="3"/>
+      <c r="D1423" s="3"/>
+      <c r="E1423" s="3"/>
+      <c r="F1423" s="3"/>
+      <c r="G1423" s="3"/>
+      <c r="H1423" s="3"/>
+      <c r="I1423" s="4"/>
+      <c r="J1423" s="4"/>
+    </row>
+    <row r="1424" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1424" s="3"/>
+      <c r="B1424" s="3"/>
+      <c r="C1424" s="3"/>
+      <c r="D1424" s="3"/>
+      <c r="E1424" s="3"/>
+      <c r="F1424" s="3"/>
+      <c r="G1424" s="3"/>
+      <c r="H1424" s="3"/>
+      <c r="I1424" s="4"/>
+      <c r="J1424" s="4"/>
+    </row>
+    <row r="1425" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1425" s="3"/>
+      <c r="B1425" s="3"/>
+      <c r="C1425" s="3"/>
+      <c r="D1425" s="3"/>
+      <c r="E1425" s="3"/>
+      <c r="F1425" s="3"/>
+      <c r="G1425" s="3"/>
+      <c r="H1425" s="3"/>
+      <c r="I1425" s="4"/>
+      <c r="J1425" s="4"/>
+    </row>
+    <row r="1426" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1426" s="3"/>
+      <c r="B1426" s="3"/>
+      <c r="C1426" s="3"/>
+      <c r="D1426" s="3"/>
+      <c r="E1426" s="3"/>
+      <c r="F1426" s="3"/>
+      <c r="G1426" s="3"/>
+      <c r="H1426" s="3"/>
+      <c r="I1426" s="4"/>
+      <c r="J1426" s="4"/>
+    </row>
+    <row r="1427" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1427" s="3"/>
+      <c r="B1427" s="3"/>
+      <c r="C1427" s="3"/>
+      <c r="D1427" s="3"/>
+      <c r="E1427" s="3"/>
+      <c r="F1427" s="3"/>
+      <c r="G1427" s="3"/>
+      <c r="H1427" s="3"/>
+      <c r="I1427" s="4"/>
+      <c r="J1427" s="4"/>
+    </row>
+    <row r="1428" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1428" s="3"/>
+      <c r="B1428" s="3"/>
+      <c r="C1428" s="3"/>
+      <c r="D1428" s="3"/>
+      <c r="E1428" s="3"/>
+      <c r="F1428" s="3"/>
+      <c r="G1428" s="3"/>
+      <c r="H1428" s="3"/>
+      <c r="I1428" s="4"/>
+      <c r="J1428" s="4"/>
+    </row>
+    <row r="1429" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1429" s="3"/>
+      <c r="B1429" s="3"/>
+      <c r="C1429" s="3"/>
+      <c r="D1429" s="3"/>
+      <c r="E1429" s="3"/>
+      <c r="F1429" s="3"/>
+      <c r="G1429" s="3"/>
+      <c r="H1429" s="3"/>
+      <c r="I1429" s="4"/>
+      <c r="J1429" s="4"/>
+    </row>
+    <row r="1430" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1430" s="3"/>
+      <c r="B1430" s="3"/>
+      <c r="C1430" s="3"/>
+      <c r="D1430" s="3"/>
+      <c r="E1430" s="3"/>
+      <c r="F1430" s="3"/>
+      <c r="G1430" s="3"/>
+      <c r="H1430" s="3"/>
+      <c r="I1430" s="4"/>
+      <c r="J1430" s="4"/>
+    </row>
+    <row r="1431" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1431" s="3"/>
+      <c r="B1431" s="3"/>
+      <c r="C1431" s="3"/>
+      <c r="D1431" s="3"/>
+      <c r="E1431" s="3"/>
+      <c r="F1431" s="3"/>
+      <c r="G1431" s="3"/>
+      <c r="H1431" s="3"/>
+      <c r="I1431" s="4"/>
+      <c r="J1431" s="4"/>
+    </row>
+    <row r="1432" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1432" s="3"/>
+      <c r="B1432" s="3"/>
+      <c r="C1432" s="3"/>
+      <c r="D1432" s="3"/>
+      <c r="E1432" s="3"/>
+      <c r="F1432" s="3"/>
+      <c r="G1432" s="3"/>
+      <c r="H1432" s="3"/>
+      <c r="I1432" s="4"/>
+      <c r="J1432" s="4"/>
+    </row>
+    <row r="1433" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1433" s="3"/>
+      <c r="B1433" s="3"/>
+      <c r="C1433" s="3"/>
+      <c r="D1433" s="3"/>
+      <c r="E1433" s="3"/>
+      <c r="F1433" s="3"/>
+      <c r="G1433" s="3"/>
+      <c r="H1433" s="3"/>
+      <c r="I1433" s="4"/>
+      <c r="J1433" s="4"/>
+    </row>
+    <row r="1434" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1434" s="3"/>
+      <c r="B1434" s="3"/>
+      <c r="C1434" s="3"/>
+      <c r="D1434" s="3"/>
+      <c r="E1434" s="3"/>
+      <c r="F1434" s="3"/>
+      <c r="G1434" s="3"/>
+      <c r="H1434" s="3"/>
+      <c r="I1434" s="4"/>
+      <c r="J1434" s="4"/>
+    </row>
+    <row r="1435" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1435" s="3"/>
+      <c r="B1435" s="3"/>
+      <c r="C1435" s="3"/>
+      <c r="D1435" s="3"/>
+      <c r="E1435" s="3"/>
+      <c r="F1435" s="3"/>
+      <c r="G1435" s="3"/>
+      <c r="H1435" s="3"/>
+      <c r="I1435" s="4"/>
+      <c r="J1435" s="4"/>
+    </row>
+    <row r="1436" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1436" s="3"/>
+      <c r="B1436" s="3"/>
+      <c r="C1436" s="3"/>
+      <c r="D1436" s="3"/>
+      <c r="E1436" s="3"/>
+      <c r="F1436" s="3"/>
+      <c r="G1436" s="3"/>
+      <c r="H1436" s="3"/>
+      <c r="I1436" s="4"/>
+      <c r="J1436" s="4"/>
+    </row>
+    <row r="1437" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1437" s="3"/>
+      <c r="B1437" s="3"/>
+      <c r="C1437" s="3"/>
+      <c r="D1437" s="3"/>
+      <c r="E1437" s="3"/>
+      <c r="F1437" s="3"/>
+      <c r="G1437" s="3"/>
+      <c r="H1437" s="3"/>
+      <c r="I1437" s="4"/>
+      <c r="J1437" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#54 Time Tracking: updated to 2025-04-07.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11235" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11327" uniqueCount="1337">
   <si>
     <t>Year</t>
   </si>
@@ -4015,6 +4015,27 @@
   </si>
   <si>
     <t>nwapolloanalytics v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-03-25</t>
+  </si>
+  <si>
+    <t>2025-04-01</t>
+  </si>
+  <si>
+    <t>2025-04-03</t>
+  </si>
+  <si>
+    <t>2025-04-04</t>
+  </si>
+  <si>
+    <t>2025-04-05</t>
+  </si>
+  <si>
+    <t>2025-04-06</t>
+  </si>
+  <si>
+    <t>2025-04-07</t>
   </si>
 </sst>
 </file>
@@ -4414,11 +4435,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1455"/>
+  <dimension ref="A1:J1470"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1420" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1440" sqref="F1440"/>
+      <pane ySplit="1" topLeftCell="A1429" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1441" sqref="F1441"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -52821,148 +52842,404 @@
       </c>
     </row>
     <row r="1441" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1441" s="3"/>
-      <c r="B1441" s="3"/>
-      <c r="C1441" s="3"/>
-      <c r="D1441" s="3"/>
-      <c r="E1441" s="3"/>
+      <c r="A1441" s="3" t="s">
+        <v>1330</v>
+      </c>
+      <c r="B1441" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1441" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1441" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1441" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1441" s="3"/>
-      <c r="G1441" s="3"/>
-      <c r="H1441" s="3"/>
-      <c r="I1441" s="4"/>
-      <c r="J1441" s="4"/>
+      <c r="G1441" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1441" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1441" s="4">
+        <f t="shared" ref="I1441" si="512">YEAR(A1441)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1441" s="4">
+        <f t="shared" ref="J1441" si="513">MONTH(A1441)</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="1442" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1442" s="3"/>
-      <c r="B1442" s="3"/>
-      <c r="C1442" s="3"/>
-      <c r="D1442" s="3"/>
-      <c r="E1442" s="3"/>
+      <c r="A1442" s="3" t="s">
+        <v>1331</v>
+      </c>
+      <c r="B1442" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1442" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1442" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1442" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1442" s="3"/>
-      <c r="G1442" s="3"/>
-      <c r="H1442" s="3"/>
-      <c r="I1442" s="4"/>
-      <c r="J1442" s="4"/>
+      <c r="G1442" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1442" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1442" s="4">
+        <f t="shared" ref="I1442" si="514">YEAR(A1442)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1442" s="4">
+        <f t="shared" ref="J1442" si="515">MONTH(A1442)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1443" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1443" s="3"/>
-      <c r="B1443" s="3"/>
-      <c r="C1443" s="3"/>
-      <c r="D1443" s="3"/>
-      <c r="E1443" s="3"/>
+      <c r="A1443" s="3" t="s">
+        <v>1332</v>
+      </c>
+      <c r="B1443" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1443" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1443" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1443" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1443" s="3"/>
-      <c r="G1443" s="3"/>
-      <c r="H1443" s="3"/>
-      <c r="I1443" s="4"/>
-      <c r="J1443" s="4"/>
+      <c r="G1443" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1443" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1443" s="4">
+        <f t="shared" ref="I1443" si="516">YEAR(A1443)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1443" s="4">
+        <f t="shared" ref="J1443" si="517">MONTH(A1443)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1444" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1444" s="3"/>
-      <c r="B1444" s="3"/>
-      <c r="C1444" s="3"/>
-      <c r="D1444" s="3"/>
-      <c r="E1444" s="3"/>
+      <c r="A1444" s="3" t="s">
+        <v>1333</v>
+      </c>
+      <c r="B1444" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1444" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1444" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1444" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1444" s="3"/>
-      <c r="G1444" s="3"/>
-      <c r="H1444" s="3"/>
-      <c r="I1444" s="4"/>
-      <c r="J1444" s="4"/>
+      <c r="G1444" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1444" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1444" s="4">
+        <f t="shared" ref="I1444" si="518">YEAR(A1444)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1444" s="4">
+        <f t="shared" ref="J1444" si="519">MONTH(A1444)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1445" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1445" s="3"/>
-      <c r="B1445" s="3"/>
-      <c r="C1445" s="3"/>
-      <c r="D1445" s="3"/>
-      <c r="E1445" s="3"/>
-      <c r="F1445" s="3"/>
-      <c r="G1445" s="3"/>
-      <c r="H1445" s="3"/>
-      <c r="I1445" s="4"/>
-      <c r="J1445" s="4"/>
+      <c r="A1445" s="3" t="s">
+        <v>1334</v>
+      </c>
+      <c r="B1445" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1445" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1445" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1445" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1445" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1445" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1445" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1445" s="4">
+        <f t="shared" ref="I1445:I1452" si="520">YEAR(A1445)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1445" s="4">
+        <f t="shared" ref="J1445:J1452" si="521">MONTH(A1445)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1446" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1446" s="3"/>
-      <c r="B1446" s="3"/>
-      <c r="C1446" s="3"/>
-      <c r="D1446" s="3"/>
-      <c r="E1446" s="3"/>
-      <c r="F1446" s="3"/>
-      <c r="G1446" s="3"/>
-      <c r="H1446" s="3"/>
-      <c r="I1446" s="4"/>
-      <c r="J1446" s="4"/>
+      <c r="A1446" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B1446" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1446" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1446" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1446" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1446" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1446" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1446" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1446" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1446" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1447" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1447" s="3"/>
-      <c r="B1447" s="3"/>
-      <c r="C1447" s="3"/>
-      <c r="D1447" s="3"/>
-      <c r="E1447" s="3"/>
-      <c r="F1447" s="3"/>
-      <c r="G1447" s="3"/>
-      <c r="H1447" s="3"/>
-      <c r="I1447" s="4"/>
-      <c r="J1447" s="4"/>
+      <c r="A1447" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B1447" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1447" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1447" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1447" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1447" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1447" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1447" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1447" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1447" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1448" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1448" s="3"/>
-      <c r="B1448" s="3"/>
-      <c r="C1448" s="3"/>
-      <c r="D1448" s="3"/>
-      <c r="E1448" s="3"/>
-      <c r="F1448" s="3"/>
-      <c r="G1448" s="3"/>
-      <c r="H1448" s="3"/>
-      <c r="I1448" s="4"/>
-      <c r="J1448" s="4"/>
+      <c r="A1448" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B1448" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1448" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1448" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1448" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1448" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1448" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1448" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1448" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1448" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1449" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1449" s="3"/>
-      <c r="B1449" s="3"/>
-      <c r="C1449" s="3"/>
-      <c r="D1449" s="3"/>
-      <c r="E1449" s="3"/>
-      <c r="F1449" s="3"/>
-      <c r="G1449" s="3"/>
-      <c r="H1449" s="3"/>
-      <c r="I1449" s="4"/>
-      <c r="J1449" s="4"/>
+      <c r="A1449" s="3" t="s">
+        <v>1335</v>
+      </c>
+      <c r="B1449" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1449" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1449" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1449" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1449" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1449" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1449" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1449" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1449" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1450" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1450" s="3"/>
-      <c r="B1450" s="3"/>
-      <c r="C1450" s="3"/>
-      <c r="D1450" s="3"/>
-      <c r="E1450" s="3"/>
-      <c r="F1450" s="3"/>
-      <c r="G1450" s="3"/>
-      <c r="H1450" s="3"/>
-      <c r="I1450" s="4"/>
-      <c r="J1450" s="4"/>
+      <c r="A1450" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B1450" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1450" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1450" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1450" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1450" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1450" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1450" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1450" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1450" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1451" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1451" s="3"/>
-      <c r="B1451" s="3"/>
-      <c r="C1451" s="3"/>
-      <c r="D1451" s="3"/>
-      <c r="E1451" s="3"/>
-      <c r="F1451" s="3"/>
-      <c r="G1451" s="3"/>
-      <c r="H1451" s="3"/>
-      <c r="I1451" s="4"/>
-      <c r="J1451" s="4"/>
+      <c r="A1451" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B1451" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1451" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1451" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1451" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1451" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1451" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1451" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1451" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1451" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1452" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1452" s="3"/>
-      <c r="B1452" s="3"/>
-      <c r="C1452" s="3"/>
-      <c r="D1452" s="3"/>
-      <c r="E1452" s="3"/>
-      <c r="F1452" s="3"/>
-      <c r="G1452" s="3"/>
-      <c r="H1452" s="3"/>
-      <c r="I1452" s="4"/>
-      <c r="J1452" s="4"/>
+      <c r="A1452" s="3" t="s">
+        <v>1336</v>
+      </c>
+      <c r="B1452" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1452" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1452" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1452" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1452" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1452" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1452" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1452" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1452" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1453" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1453" s="3"/>
@@ -53000,6 +53277,186 @@
       <c r="I1455" s="4"/>
       <c r="J1455" s="4"/>
     </row>
+    <row r="1456" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1456" s="3"/>
+      <c r="B1456" s="3"/>
+      <c r="C1456" s="3"/>
+      <c r="D1456" s="3"/>
+      <c r="E1456" s="3"/>
+      <c r="F1456" s="3"/>
+      <c r="G1456" s="3"/>
+      <c r="H1456" s="3"/>
+      <c r="I1456" s="4"/>
+      <c r="J1456" s="4"/>
+    </row>
+    <row r="1457" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1457" s="3"/>
+      <c r="B1457" s="3"/>
+      <c r="C1457" s="3"/>
+      <c r="D1457" s="3"/>
+      <c r="E1457" s="3"/>
+      <c r="F1457" s="3"/>
+      <c r="G1457" s="3"/>
+      <c r="H1457" s="3"/>
+      <c r="I1457" s="4"/>
+      <c r="J1457" s="4"/>
+    </row>
+    <row r="1458" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1458" s="3"/>
+      <c r="B1458" s="3"/>
+      <c r="C1458" s="3"/>
+      <c r="D1458" s="3"/>
+      <c r="E1458" s="3"/>
+      <c r="F1458" s="3"/>
+      <c r="G1458" s="3"/>
+      <c r="H1458" s="3"/>
+      <c r="I1458" s="4"/>
+      <c r="J1458" s="4"/>
+    </row>
+    <row r="1459" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1459" s="3"/>
+      <c r="B1459" s="3"/>
+      <c r="C1459" s="3"/>
+      <c r="D1459" s="3"/>
+      <c r="E1459" s="3"/>
+      <c r="F1459" s="3"/>
+      <c r="G1459" s="3"/>
+      <c r="H1459" s="3"/>
+      <c r="I1459" s="4"/>
+      <c r="J1459" s="4"/>
+    </row>
+    <row r="1460" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1460" s="3"/>
+      <c r="B1460" s="3"/>
+      <c r="C1460" s="3"/>
+      <c r="D1460" s="3"/>
+      <c r="E1460" s="3"/>
+      <c r="F1460" s="3"/>
+      <c r="G1460" s="3"/>
+      <c r="H1460" s="3"/>
+      <c r="I1460" s="4"/>
+      <c r="J1460" s="4"/>
+    </row>
+    <row r="1461" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1461" s="3"/>
+      <c r="B1461" s="3"/>
+      <c r="C1461" s="3"/>
+      <c r="D1461" s="3"/>
+      <c r="E1461" s="3"/>
+      <c r="F1461" s="3"/>
+      <c r="G1461" s="3"/>
+      <c r="H1461" s="3"/>
+      <c r="I1461" s="4"/>
+      <c r="J1461" s="4"/>
+    </row>
+    <row r="1462" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1462" s="3"/>
+      <c r="B1462" s="3"/>
+      <c r="C1462" s="3"/>
+      <c r="D1462" s="3"/>
+      <c r="E1462" s="3"/>
+      <c r="F1462" s="3"/>
+      <c r="G1462" s="3"/>
+      <c r="H1462" s="3"/>
+      <c r="I1462" s="4"/>
+      <c r="J1462" s="4"/>
+    </row>
+    <row r="1463" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1463" s="3"/>
+      <c r="B1463" s="3"/>
+      <c r="C1463" s="3"/>
+      <c r="D1463" s="3"/>
+      <c r="E1463" s="3"/>
+      <c r="F1463" s="3"/>
+      <c r="G1463" s="3"/>
+      <c r="H1463" s="3"/>
+      <c r="I1463" s="4"/>
+      <c r="J1463" s="4"/>
+    </row>
+    <row r="1464" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1464" s="3"/>
+      <c r="B1464" s="3"/>
+      <c r="C1464" s="3"/>
+      <c r="D1464" s="3"/>
+      <c r="E1464" s="3"/>
+      <c r="F1464" s="3"/>
+      <c r="G1464" s="3"/>
+      <c r="H1464" s="3"/>
+      <c r="I1464" s="4"/>
+      <c r="J1464" s="4"/>
+    </row>
+    <row r="1465" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1465" s="3"/>
+      <c r="B1465" s="3"/>
+      <c r="C1465" s="3"/>
+      <c r="D1465" s="3"/>
+      <c r="E1465" s="3"/>
+      <c r="F1465" s="3"/>
+      <c r="G1465" s="3"/>
+      <c r="H1465" s="3"/>
+      <c r="I1465" s="4"/>
+      <c r="J1465" s="4"/>
+    </row>
+    <row r="1466" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1466" s="3"/>
+      <c r="B1466" s="3"/>
+      <c r="C1466" s="3"/>
+      <c r="D1466" s="3"/>
+      <c r="E1466" s="3"/>
+      <c r="F1466" s="3"/>
+      <c r="G1466" s="3"/>
+      <c r="H1466" s="3"/>
+      <c r="I1466" s="4"/>
+      <c r="J1466" s="4"/>
+    </row>
+    <row r="1467" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1467" s="3"/>
+      <c r="B1467" s="3"/>
+      <c r="C1467" s="3"/>
+      <c r="D1467" s="3"/>
+      <c r="E1467" s="3"/>
+      <c r="F1467" s="3"/>
+      <c r="G1467" s="3"/>
+      <c r="H1467" s="3"/>
+      <c r="I1467" s="4"/>
+      <c r="J1467" s="4"/>
+    </row>
+    <row r="1468" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1468" s="3"/>
+      <c r="B1468" s="3"/>
+      <c r="C1468" s="3"/>
+      <c r="D1468" s="3"/>
+      <c r="E1468" s="3"/>
+      <c r="F1468" s="3"/>
+      <c r="G1468" s="3"/>
+      <c r="H1468" s="3"/>
+      <c r="I1468" s="4"/>
+      <c r="J1468" s="4"/>
+    </row>
+    <row r="1469" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1469" s="3"/>
+      <c r="B1469" s="3"/>
+      <c r="C1469" s="3"/>
+      <c r="D1469" s="3"/>
+      <c r="E1469" s="3"/>
+      <c r="F1469" s="3"/>
+      <c r="G1469" s="3"/>
+      <c r="H1469" s="3"/>
+      <c r="I1469" s="4"/>
+      <c r="J1469" s="4"/>
+    </row>
+    <row r="1470" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1470" s="3"/>
+      <c r="B1470" s="3"/>
+      <c r="C1470" s="3"/>
+      <c r="D1470" s="3"/>
+      <c r="E1470" s="3"/>
+      <c r="F1470" s="3"/>
+      <c r="G1470" s="3"/>
+      <c r="H1470" s="3"/>
+      <c r="I1470" s="4"/>
+      <c r="J1470" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#54 Time Tracking: updated to 2025-04-29.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11327" uniqueCount="1337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11580" uniqueCount="1358">
   <si>
     <t>Year</t>
   </si>
@@ -4036,6 +4036,69 @@
   </si>
   <si>
     <t>2025-04-07</t>
+  </si>
+  <si>
+    <t>2025-04-08</t>
+  </si>
+  <si>
+    <t>2025-04-09</t>
+  </si>
+  <si>
+    <t>2025-04-10</t>
+  </si>
+  <si>
+    <t>2025-04-11</t>
+  </si>
+  <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
+    <t>2025-04-13</t>
+  </si>
+  <si>
+    <t>2025-04-14</t>
+  </si>
+  <si>
+    <t>#asciidoc</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>2025-04-16</t>
+  </si>
+  <si>
+    <t>2025-04-17</t>
+  </si>
+  <si>
+    <t>2025-04-18</t>
+  </si>
+  <si>
+    <t>2025-04-19</t>
+  </si>
+  <si>
+    <t>2025-04-20</t>
+  </si>
+  <si>
+    <t>2025-04-21</t>
+  </si>
+  <si>
+    <t>2025-04-24</t>
+  </si>
+  <si>
+    <t>2025-04-25</t>
+  </si>
+  <si>
+    <t>2025-04-26</t>
+  </si>
+  <si>
+    <t>2025-04-27</t>
+  </si>
+  <si>
+    <t>2025-04-28</t>
+  </si>
+  <si>
+    <t>2025-04-29</t>
   </si>
 </sst>
 </file>
@@ -4435,11 +4498,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1470"/>
+  <dimension ref="A1:J1508"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1429" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1441" sqref="F1441"/>
+      <pane ySplit="1" topLeftCell="A1460" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1488" sqref="E1488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -52995,11 +53058,11 @@
         <v>280</v>
       </c>
       <c r="I1445" s="4">
-        <f t="shared" ref="I1445:I1452" si="520">YEAR(A1445)</f>
+        <f t="shared" ref="I1445:I1453" si="520">YEAR(A1445)</f>
         <v>2025</v>
       </c>
       <c r="J1445" s="4">
-        <f t="shared" ref="J1445:J1452" si="521">MONTH(A1445)</f>
+        <f t="shared" ref="J1445:J1453" si="521">MONTH(A1445)</f>
         <v>4</v>
       </c>
     </row>
@@ -53242,220 +53305,1386 @@
       </c>
     </row>
     <row r="1453" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1453" s="3"/>
-      <c r="B1453" s="3"/>
-      <c r="C1453" s="3"/>
-      <c r="D1453" s="3"/>
-      <c r="E1453" s="3"/>
+      <c r="A1453" s="3" t="s">
+        <v>1337</v>
+      </c>
+      <c r="B1453" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1453" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1453" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1453" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1453" s="3"/>
-      <c r="G1453" s="3"/>
-      <c r="H1453" s="3"/>
-      <c r="I1453" s="4"/>
-      <c r="J1453" s="4"/>
+      <c r="G1453" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1453" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1453" s="4">
+        <f t="shared" si="520"/>
+        <v>2025</v>
+      </c>
+      <c r="J1453" s="4">
+        <f t="shared" si="521"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1454" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1454" s="3"/>
-      <c r="B1454" s="3"/>
-      <c r="C1454" s="3"/>
-      <c r="D1454" s="3"/>
-      <c r="E1454" s="3"/>
-      <c r="F1454" s="3"/>
-      <c r="G1454" s="3"/>
-      <c r="H1454" s="3"/>
-      <c r="I1454" s="4"/>
-      <c r="J1454" s="4"/>
+      <c r="A1454" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B1454" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1454" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1454" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1454" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1454" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1454" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1454" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1454" s="4">
+        <f t="shared" ref="I1454:I1455" si="522">YEAR(A1454)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1454" s="4">
+        <f t="shared" ref="J1454:J1455" si="523">MONTH(A1454)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1455" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1455" s="3"/>
-      <c r="B1455" s="3"/>
-      <c r="C1455" s="3"/>
-      <c r="D1455" s="3"/>
-      <c r="E1455" s="3"/>
-      <c r="F1455" s="3"/>
-      <c r="G1455" s="3"/>
-      <c r="H1455" s="3"/>
-      <c r="I1455" s="4"/>
-      <c r="J1455" s="4"/>
+      <c r="A1455" s="3" t="s">
+        <v>1338</v>
+      </c>
+      <c r="B1455" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1455" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1455" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1455" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1455" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1455" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1455" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1455" s="4">
+        <f t="shared" si="522"/>
+        <v>2025</v>
+      </c>
+      <c r="J1455" s="4">
+        <f t="shared" si="523"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1456" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1456" s="3"/>
-      <c r="B1456" s="3"/>
-      <c r="C1456" s="3"/>
-      <c r="D1456" s="3"/>
-      <c r="E1456" s="3"/>
-      <c r="F1456" s="3"/>
-      <c r="G1456" s="3"/>
-      <c r="H1456" s="3"/>
-      <c r="I1456" s="4"/>
-      <c r="J1456" s="4"/>
+      <c r="A1456" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B1456" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1456" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1456" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1456" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1456" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1456" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1456" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1456" s="4">
+        <f t="shared" ref="I1456:I1458" si="524">YEAR(A1456)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1456" s="4">
+        <f t="shared" ref="J1456:J1458" si="525">MONTH(A1456)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1457" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1457" s="3"/>
-      <c r="B1457" s="3"/>
-      <c r="C1457" s="3"/>
-      <c r="D1457" s="3"/>
-      <c r="E1457" s="3"/>
-      <c r="F1457" s="3"/>
-      <c r="G1457" s="3"/>
-      <c r="H1457" s="3"/>
-      <c r="I1457" s="4"/>
-      <c r="J1457" s="4"/>
+      <c r="A1457" s="3" t="s">
+        <v>1339</v>
+      </c>
+      <c r="B1457" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1457" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1457" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1457" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1457" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1457" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1457" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1457" s="4">
+        <f t="shared" si="524"/>
+        <v>2025</v>
+      </c>
+      <c r="J1457" s="4">
+        <f t="shared" si="525"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1458" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1458" s="3"/>
-      <c r="B1458" s="3"/>
-      <c r="C1458" s="3"/>
-      <c r="D1458" s="3"/>
-      <c r="E1458" s="3"/>
+      <c r="A1458" s="3" t="s">
+        <v>1340</v>
+      </c>
+      <c r="B1458" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1458" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1458" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1458" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1458" s="3"/>
-      <c r="G1458" s="3"/>
-      <c r="H1458" s="3"/>
-      <c r="I1458" s="4"/>
-      <c r="J1458" s="4"/>
+      <c r="G1458" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1458" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1458" s="4">
+        <f t="shared" si="524"/>
+        <v>2025</v>
+      </c>
+      <c r="J1458" s="4">
+        <f t="shared" si="525"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1459" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1459" s="3"/>
-      <c r="B1459" s="3"/>
-      <c r="C1459" s="3"/>
-      <c r="D1459" s="3"/>
-      <c r="E1459" s="3"/>
+      <c r="A1459" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B1459" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1459" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1459" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1459" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1459" s="3"/>
-      <c r="G1459" s="3"/>
-      <c r="H1459" s="3"/>
-      <c r="I1459" s="4"/>
-      <c r="J1459" s="4"/>
+      <c r="G1459" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1459" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1459" s="4">
+        <f t="shared" ref="I1459:I1461" si="526">YEAR(A1459)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1459" s="4">
+        <f t="shared" ref="J1459:J1461" si="527">MONTH(A1459)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1460" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1460" s="3"/>
-      <c r="B1460" s="3"/>
-      <c r="C1460" s="3"/>
-      <c r="D1460" s="3"/>
-      <c r="E1460" s="3"/>
+      <c r="A1460" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B1460" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1460" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1460" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1460" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1460" s="3"/>
-      <c r="G1460" s="3"/>
-      <c r="H1460" s="3"/>
-      <c r="I1460" s="4"/>
-      <c r="J1460" s="4"/>
+      <c r="G1460" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1460" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1460" s="4">
+        <f t="shared" si="526"/>
+        <v>2025</v>
+      </c>
+      <c r="J1460" s="4">
+        <f t="shared" si="527"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1461" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1461" s="3"/>
-      <c r="B1461" s="3"/>
-      <c r="C1461" s="3"/>
-      <c r="D1461" s="3"/>
-      <c r="E1461" s="3"/>
+      <c r="A1461" s="3" t="s">
+        <v>1341</v>
+      </c>
+      <c r="B1461" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1461" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1461" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1461" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1461" s="3"/>
-      <c r="G1461" s="3"/>
-      <c r="H1461" s="3"/>
-      <c r="I1461" s="4"/>
-      <c r="J1461" s="4"/>
+      <c r="G1461" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1461" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1461" s="4">
+        <f t="shared" si="526"/>
+        <v>2025</v>
+      </c>
+      <c r="J1461" s="4">
+        <f t="shared" si="527"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1462" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1462" s="3"/>
-      <c r="B1462" s="3"/>
-      <c r="C1462" s="3"/>
-      <c r="D1462" s="3"/>
-      <c r="E1462" s="3"/>
+      <c r="A1462" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B1462" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1462" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1462" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1462" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1462" s="3"/>
-      <c r="G1462" s="3"/>
-      <c r="H1462" s="3"/>
-      <c r="I1462" s="4"/>
-      <c r="J1462" s="4"/>
+      <c r="G1462" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1462" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1462" s="4">
+        <f t="shared" ref="I1462:I1466" si="528">YEAR(A1462)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1462" s="4">
+        <f t="shared" ref="J1462:J1466" si="529">MONTH(A1462)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1463" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1463" s="3"/>
-      <c r="B1463" s="3"/>
-      <c r="C1463" s="3"/>
-      <c r="D1463" s="3"/>
-      <c r="E1463" s="3"/>
+      <c r="A1463" s="3" t="s">
+        <v>1342</v>
+      </c>
+      <c r="B1463" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1463" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1463" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1463" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1463" s="3"/>
-      <c r="G1463" s="3"/>
-      <c r="H1463" s="3"/>
-      <c r="I1463" s="4"/>
-      <c r="J1463" s="4"/>
+      <c r="G1463" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1463" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1463" s="4">
+        <f t="shared" si="528"/>
+        <v>2025</v>
+      </c>
+      <c r="J1463" s="4">
+        <f t="shared" si="529"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1464" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1464" s="3"/>
-      <c r="B1464" s="3"/>
-      <c r="C1464" s="3"/>
-      <c r="D1464" s="3"/>
-      <c r="E1464" s="3"/>
-      <c r="F1464" s="3"/>
-      <c r="G1464" s="3"/>
-      <c r="H1464" s="3"/>
-      <c r="I1464" s="4"/>
-      <c r="J1464" s="4"/>
+      <c r="A1464" s="3" t="s">
+        <v>1343</v>
+      </c>
+      <c r="B1464" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1464" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1464" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1464" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F1464" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1464" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1464" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1464" s="4">
+        <f t="shared" si="528"/>
+        <v>2025</v>
+      </c>
+      <c r="J1464" s="4">
+        <f t="shared" si="529"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1465" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1465" s="3"/>
-      <c r="B1465" s="3"/>
-      <c r="C1465" s="3"/>
-      <c r="D1465" s="3"/>
-      <c r="E1465" s="3"/>
+      <c r="A1465" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B1465" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1465" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1465" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1465" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1465" s="3"/>
-      <c r="G1465" s="3"/>
-      <c r="H1465" s="3"/>
-      <c r="I1465" s="4"/>
-      <c r="J1465" s="4"/>
+      <c r="G1465" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1465" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1465" s="4">
+        <f t="shared" si="528"/>
+        <v>2025</v>
+      </c>
+      <c r="J1465" s="4">
+        <f t="shared" si="529"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1466" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1466" s="3"/>
-      <c r="B1466" s="3"/>
-      <c r="C1466" s="3"/>
-      <c r="D1466" s="3"/>
-      <c r="E1466" s="3"/>
-      <c r="F1466" s="3"/>
-      <c r="G1466" s="3"/>
-      <c r="H1466" s="3"/>
-      <c r="I1466" s="4"/>
-      <c r="J1466" s="4"/>
+      <c r="A1466" s="3" t="s">
+        <v>1345</v>
+      </c>
+      <c r="B1466" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1466" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1466" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1466" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1466" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1466" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1466" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1466" s="4">
+        <f t="shared" si="528"/>
+        <v>2025</v>
+      </c>
+      <c r="J1466" s="4">
+        <f t="shared" si="529"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1467" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1467" s="3"/>
-      <c r="B1467" s="3"/>
-      <c r="C1467" s="3"/>
-      <c r="D1467" s="3"/>
-      <c r="E1467" s="3"/>
-      <c r="F1467" s="3"/>
-      <c r="G1467" s="3"/>
-      <c r="H1467" s="3"/>
-      <c r="I1467" s="4"/>
-      <c r="J1467" s="4"/>
+      <c r="A1467" s="3" t="s">
+        <v>1346</v>
+      </c>
+      <c r="B1467" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1467" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1467" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1467" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1467" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1467" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1467" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1467" s="4">
+        <f t="shared" ref="I1467:I1470" si="530">YEAR(A1467)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1467" s="4">
+        <f t="shared" ref="J1467:J1470" si="531">MONTH(A1467)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="1468" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1468" s="3"/>
-      <c r="B1468" s="3"/>
-      <c r="C1468" s="3"/>
-      <c r="D1468" s="3"/>
-      <c r="E1468" s="3"/>
-      <c r="F1468" s="3"/>
-      <c r="G1468" s="3"/>
-      <c r="H1468" s="3"/>
-      <c r="I1468" s="4"/>
-      <c r="J1468" s="4"/>
+      <c r="A1468" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B1468" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1468" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1468" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1468" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F1468" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1468" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1468" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1468" s="4">
+        <f t="shared" si="530"/>
+        <v>2025</v>
+      </c>
+      <c r="J1468" s="4">
+        <f t="shared" si="531"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1469" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1469" s="3"/>
-      <c r="B1469" s="3"/>
-      <c r="C1469" s="3"/>
-      <c r="D1469" s="3"/>
-      <c r="E1469" s="3"/>
-      <c r="F1469" s="3"/>
-      <c r="G1469" s="3"/>
-      <c r="H1469" s="3"/>
-      <c r="I1469" s="4"/>
-      <c r="J1469" s="4"/>
+      <c r="A1469" s="3" t="s">
+        <v>1347</v>
+      </c>
+      <c r="B1469" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1469" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1469" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1469" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F1469" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1469" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1469" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1469" s="4">
+        <f t="shared" si="530"/>
+        <v>2025</v>
+      </c>
+      <c r="J1469" s="4">
+        <f t="shared" si="531"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1470" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1470" s="3"/>
-      <c r="B1470" s="3"/>
-      <c r="C1470" s="3"/>
-      <c r="D1470" s="3"/>
-      <c r="E1470" s="3"/>
+      <c r="A1470" s="3" t="s">
+        <v>1348</v>
+      </c>
+      <c r="B1470" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1470" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1470" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1470" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1470" s="3"/>
-      <c r="G1470" s="3"/>
-      <c r="H1470" s="3"/>
-      <c r="I1470" s="4"/>
-      <c r="J1470" s="4"/>
+      <c r="G1470" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1470" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1470" s="4">
+        <f t="shared" si="530"/>
+        <v>2025</v>
+      </c>
+      <c r="J1470" s="4">
+        <f t="shared" si="531"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1471" s="3" t="s">
+        <v>1349</v>
+      </c>
+      <c r="B1471" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1471" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1471" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1471" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F1471" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1471" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1471" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1471" s="4">
+        <f t="shared" ref="I1471" si="532">YEAR(A1471)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1471" s="4">
+        <f t="shared" ref="J1471" si="533">MONTH(A1471)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1472" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B1472" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1472" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1472" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1472" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F1472" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1472" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1472" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1472" s="4">
+        <f t="shared" ref="I1472:I1475" si="534">YEAR(A1472)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1472" s="4">
+        <f t="shared" ref="J1472:J1475" si="535">MONTH(A1472)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1473" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1473" s="3" t="s">
+        <v>1350</v>
+      </c>
+      <c r="B1473" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1473" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1473" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1473" s="3" t="s">
+        <v>1344</v>
+      </c>
+      <c r="F1473" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1473" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1473" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1473" s="4">
+        <f t="shared" si="534"/>
+        <v>2025</v>
+      </c>
+      <c r="J1473" s="4">
+        <f t="shared" si="535"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1474" s="3" t="s">
+        <v>1351</v>
+      </c>
+      <c r="B1474" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1474" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1474" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1474" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1474" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1474" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1474" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1474" s="4">
+        <f t="shared" si="534"/>
+        <v>2025</v>
+      </c>
+      <c r="J1474" s="4">
+        <f t="shared" si="535"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1475" s="3" t="s">
+        <v>1352</v>
+      </c>
+      <c r="B1475" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1475" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1475" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1475" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1475" s="3"/>
+      <c r="G1475" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1475" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1475" s="4">
+        <f t="shared" si="534"/>
+        <v>2025</v>
+      </c>
+      <c r="J1475" s="4">
+        <f t="shared" si="535"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1476" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B1476" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1476" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1476" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1476" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1476" s="3"/>
+      <c r="G1476" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1476" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1476" s="4">
+        <f t="shared" ref="I1476:I1480" si="536">YEAR(A1476)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1476" s="4">
+        <f t="shared" ref="J1476:J1480" si="537">MONTH(A1476)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1477" s="3" t="s">
+        <v>1353</v>
+      </c>
+      <c r="B1477" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1477" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1477" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1477" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1477" s="3"/>
+      <c r="G1477" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1477" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1477" s="4">
+        <f t="shared" si="536"/>
+        <v>2025</v>
+      </c>
+      <c r="J1477" s="4">
+        <f t="shared" si="537"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1478" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B1478" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1478" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1478" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1478" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1478" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1478" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1478" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1478" s="4">
+        <f t="shared" si="536"/>
+        <v>2025</v>
+      </c>
+      <c r="J1478" s="4">
+        <f t="shared" si="537"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1479" s="3" t="s">
+        <v>1354</v>
+      </c>
+      <c r="B1479" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1479" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1479" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1479" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1479" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1479" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1479" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1479" s="4">
+        <f t="shared" si="536"/>
+        <v>2025</v>
+      </c>
+      <c r="J1479" s="4">
+        <f t="shared" si="537"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1480" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B1480" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1480" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1480" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1480" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1480" s="3"/>
+      <c r="G1480" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1480" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1480" s="4">
+        <f t="shared" si="536"/>
+        <v>2025</v>
+      </c>
+      <c r="J1480" s="4">
+        <f t="shared" si="537"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1481" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B1481" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1481" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1481" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1481" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1481" s="3"/>
+      <c r="G1481" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1481" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1481" s="4">
+        <f t="shared" ref="I1481:I1482" si="538">YEAR(A1481)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1481" s="4">
+        <f t="shared" ref="J1481:J1482" si="539">MONTH(A1481)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1482" s="3" t="s">
+        <v>1355</v>
+      </c>
+      <c r="B1482" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1482" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1482" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1482" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1482" s="3"/>
+      <c r="G1482" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1482" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1482" s="4">
+        <f t="shared" si="538"/>
+        <v>2025</v>
+      </c>
+      <c r="J1482" s="4">
+        <f t="shared" si="539"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1483" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B1483" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1483" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1483" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1483" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1483" s="3"/>
+      <c r="G1483" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1483" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1483" s="4">
+        <f t="shared" ref="I1483:I1484" si="540">YEAR(A1483)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1483" s="4">
+        <f t="shared" ref="J1483:J1484" si="541">MONTH(A1483)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1484" s="3" t="s">
+        <v>1356</v>
+      </c>
+      <c r="B1484" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1484" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1484" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1484" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1484" s="3"/>
+      <c r="G1484" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1484" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1484" s="4">
+        <f t="shared" si="540"/>
+        <v>2025</v>
+      </c>
+      <c r="J1484" s="4">
+        <f t="shared" si="541"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1485" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B1485" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1485" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1485" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1485" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1485" s="3"/>
+      <c r="G1485" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1485" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1485" s="4">
+        <f t="shared" ref="I1485:I1486" si="542">YEAR(A1485)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1485" s="4">
+        <f t="shared" ref="J1485:J1486" si="543">MONTH(A1485)</f>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1486" s="3" t="s">
+        <v>1357</v>
+      </c>
+      <c r="B1486" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1486" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1486" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1486" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1486" s="3"/>
+      <c r="G1486" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1486" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1486" s="4">
+        <f t="shared" si="542"/>
+        <v>2025</v>
+      </c>
+      <c r="J1486" s="4">
+        <f t="shared" si="543"/>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1487" s="3"/>
+      <c r="B1487" s="3"/>
+      <c r="C1487" s="3"/>
+      <c r="D1487" s="3"/>
+      <c r="E1487" s="3"/>
+      <c r="F1487" s="3"/>
+      <c r="G1487" s="3"/>
+      <c r="H1487" s="3"/>
+      <c r="I1487" s="4"/>
+      <c r="J1487" s="4"/>
+    </row>
+    <row r="1488" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1488" s="3"/>
+      <c r="B1488" s="3"/>
+      <c r="C1488" s="3"/>
+      <c r="D1488" s="3"/>
+      <c r="E1488" s="3"/>
+      <c r="F1488" s="3"/>
+      <c r="G1488" s="3"/>
+      <c r="H1488" s="3"/>
+      <c r="I1488" s="4"/>
+      <c r="J1488" s="4"/>
+    </row>
+    <row r="1489" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1489" s="3"/>
+      <c r="B1489" s="3"/>
+      <c r="C1489" s="3"/>
+      <c r="D1489" s="3"/>
+      <c r="E1489" s="3"/>
+      <c r="F1489" s="3"/>
+      <c r="G1489" s="3"/>
+      <c r="H1489" s="3"/>
+      <c r="I1489" s="4"/>
+      <c r="J1489" s="4"/>
+    </row>
+    <row r="1490" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1490" s="3"/>
+      <c r="B1490" s="3"/>
+      <c r="C1490" s="3"/>
+      <c r="D1490" s="3"/>
+      <c r="E1490" s="3"/>
+      <c r="F1490" s="3"/>
+      <c r="G1490" s="3"/>
+      <c r="H1490" s="3"/>
+      <c r="I1490" s="4"/>
+      <c r="J1490" s="4"/>
+    </row>
+    <row r="1491" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1491" s="3"/>
+      <c r="B1491" s="3"/>
+      <c r="C1491" s="3"/>
+      <c r="D1491" s="3"/>
+      <c r="E1491" s="3"/>
+      <c r="F1491" s="3"/>
+      <c r="G1491" s="3"/>
+      <c r="H1491" s="3"/>
+      <c r="I1491" s="4"/>
+      <c r="J1491" s="4"/>
+    </row>
+    <row r="1492" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1492" s="3"/>
+      <c r="B1492" s="3"/>
+      <c r="C1492" s="3"/>
+      <c r="D1492" s="3"/>
+      <c r="E1492" s="3"/>
+      <c r="F1492" s="3"/>
+      <c r="G1492" s="3"/>
+      <c r="H1492" s="3"/>
+      <c r="I1492" s="4"/>
+      <c r="J1492" s="4"/>
+    </row>
+    <row r="1493" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1493" s="3"/>
+      <c r="B1493" s="3"/>
+      <c r="C1493" s="3"/>
+      <c r="D1493" s="3"/>
+      <c r="E1493" s="3"/>
+      <c r="F1493" s="3"/>
+      <c r="G1493" s="3"/>
+      <c r="H1493" s="3"/>
+      <c r="I1493" s="4"/>
+      <c r="J1493" s="4"/>
+    </row>
+    <row r="1494" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1494" s="3"/>
+      <c r="B1494" s="3"/>
+      <c r="C1494" s="3"/>
+      <c r="D1494" s="3"/>
+      <c r="E1494" s="3"/>
+      <c r="F1494" s="3"/>
+      <c r="G1494" s="3"/>
+      <c r="H1494" s="3"/>
+      <c r="I1494" s="4"/>
+      <c r="J1494" s="4"/>
+    </row>
+    <row r="1495" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1495" s="3"/>
+      <c r="B1495" s="3"/>
+      <c r="C1495" s="3"/>
+      <c r="D1495" s="3"/>
+      <c r="E1495" s="3"/>
+      <c r="F1495" s="3"/>
+      <c r="G1495" s="3"/>
+      <c r="H1495" s="3"/>
+      <c r="I1495" s="4"/>
+      <c r="J1495" s="4"/>
+    </row>
+    <row r="1496" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1496" s="3"/>
+      <c r="B1496" s="3"/>
+      <c r="C1496" s="3"/>
+      <c r="D1496" s="3"/>
+      <c r="E1496" s="3"/>
+      <c r="F1496" s="3"/>
+      <c r="G1496" s="3"/>
+      <c r="H1496" s="3"/>
+      <c r="I1496" s="4"/>
+      <c r="J1496" s="4"/>
+    </row>
+    <row r="1497" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1497" s="3"/>
+      <c r="B1497" s="3"/>
+      <c r="C1497" s="3"/>
+      <c r="D1497" s="3"/>
+      <c r="E1497" s="3"/>
+      <c r="F1497" s="3"/>
+      <c r="G1497" s="3"/>
+      <c r="H1497" s="3"/>
+      <c r="I1497" s="4"/>
+      <c r="J1497" s="4"/>
+    </row>
+    <row r="1498" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1498" s="3"/>
+      <c r="B1498" s="3"/>
+      <c r="C1498" s="3"/>
+      <c r="D1498" s="3"/>
+      <c r="E1498" s="3"/>
+      <c r="F1498" s="3"/>
+      <c r="G1498" s="3"/>
+      <c r="H1498" s="3"/>
+      <c r="I1498" s="4"/>
+      <c r="J1498" s="4"/>
+    </row>
+    <row r="1499" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1499" s="3"/>
+      <c r="B1499" s="3"/>
+      <c r="C1499" s="3"/>
+      <c r="D1499" s="3"/>
+      <c r="E1499" s="3"/>
+      <c r="F1499" s="3"/>
+      <c r="G1499" s="3"/>
+      <c r="H1499" s="3"/>
+      <c r="I1499" s="4"/>
+      <c r="J1499" s="4"/>
+    </row>
+    <row r="1500" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1500" s="3"/>
+      <c r="B1500" s="3"/>
+      <c r="C1500" s="3"/>
+      <c r="D1500" s="3"/>
+      <c r="E1500" s="3"/>
+      <c r="F1500" s="3"/>
+      <c r="G1500" s="3"/>
+      <c r="H1500" s="3"/>
+      <c r="I1500" s="4"/>
+      <c r="J1500" s="4"/>
+    </row>
+    <row r="1501" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1501" s="3"/>
+      <c r="B1501" s="3"/>
+      <c r="C1501" s="3"/>
+      <c r="D1501" s="3"/>
+      <c r="E1501" s="3"/>
+      <c r="F1501" s="3"/>
+      <c r="G1501" s="3"/>
+      <c r="H1501" s="3"/>
+      <c r="I1501" s="4"/>
+      <c r="J1501" s="4"/>
+    </row>
+    <row r="1502" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1502" s="3"/>
+      <c r="B1502" s="3"/>
+      <c r="C1502" s="3"/>
+      <c r="D1502" s="3"/>
+      <c r="E1502" s="3"/>
+      <c r="F1502" s="3"/>
+      <c r="G1502" s="3"/>
+      <c r="H1502" s="3"/>
+      <c r="I1502" s="4"/>
+      <c r="J1502" s="4"/>
+    </row>
+    <row r="1503" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1503" s="3"/>
+      <c r="B1503" s="3"/>
+      <c r="C1503" s="3"/>
+      <c r="D1503" s="3"/>
+      <c r="E1503" s="3"/>
+      <c r="F1503" s="3"/>
+      <c r="G1503" s="3"/>
+      <c r="H1503" s="3"/>
+      <c r="I1503" s="4"/>
+      <c r="J1503" s="4"/>
+    </row>
+    <row r="1504" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1504" s="3"/>
+      <c r="B1504" s="3"/>
+      <c r="C1504" s="3"/>
+      <c r="D1504" s="3"/>
+      <c r="E1504" s="3"/>
+      <c r="F1504" s="3"/>
+      <c r="G1504" s="3"/>
+      <c r="H1504" s="3"/>
+      <c r="I1504" s="4"/>
+      <c r="J1504" s="4"/>
+    </row>
+    <row r="1505" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1505" s="3"/>
+      <c r="B1505" s="3"/>
+      <c r="C1505" s="3"/>
+      <c r="D1505" s="3"/>
+      <c r="E1505" s="3"/>
+      <c r="F1505" s="3"/>
+      <c r="G1505" s="3"/>
+      <c r="H1505" s="3"/>
+      <c r="I1505" s="4"/>
+      <c r="J1505" s="4"/>
+    </row>
+    <row r="1506" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1506" s="3"/>
+      <c r="B1506" s="3"/>
+      <c r="C1506" s="3"/>
+      <c r="D1506" s="3"/>
+      <c r="E1506" s="3"/>
+      <c r="F1506" s="3"/>
+      <c r="G1506" s="3"/>
+      <c r="H1506" s="3"/>
+      <c r="I1506" s="4"/>
+      <c r="J1506" s="4"/>
+    </row>
+    <row r="1507" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1507" s="3"/>
+      <c r="B1507" s="3"/>
+      <c r="C1507" s="3"/>
+      <c r="D1507" s="3"/>
+      <c r="E1507" s="3"/>
+      <c r="F1507" s="3"/>
+      <c r="G1507" s="3"/>
+      <c r="H1507" s="3"/>
+      <c r="I1507" s="4"/>
+      <c r="J1507" s="4"/>
+    </row>
+    <row r="1508" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1508" s="3"/>
+      <c r="B1508" s="3"/>
+      <c r="C1508" s="3"/>
+      <c r="D1508" s="3"/>
+      <c r="E1508" s="3"/>
+      <c r="F1508" s="3"/>
+      <c r="G1508" s="3"/>
+      <c r="H1508" s="3"/>
+      <c r="I1508" s="4"/>
+      <c r="J1508" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#54 Time Tracking: updated to 2025-05-05.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11580" uniqueCount="1358">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11630" uniqueCount="1362">
   <si>
     <t>Year</t>
   </si>
@@ -4099,6 +4099,18 @@
   </si>
   <si>
     <t>2025-04-29</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
+  </si>
+  <si>
+    <t>2025-05-01</t>
+  </si>
+  <si>
+    <t>2025-05-02</t>
+  </si>
+  <si>
+    <t>2025-05-05</t>
   </si>
 </sst>
 </file>
@@ -4501,8 +4513,8 @@
   <dimension ref="A1:J1508"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1460" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1488" sqref="E1488"/>
+      <pane ySplit="1" topLeftCell="A1469" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1495" sqref="F1495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -54011,7 +54023,7 @@
         <v>271</v>
       </c>
       <c r="D1474" s="3" t="s">
-        <v>217</v>
+        <v>136</v>
       </c>
       <c r="E1474" s="3" t="s">
         <v>1292</v>
@@ -54382,11 +54394,11 @@
         <v>280</v>
       </c>
       <c r="I1485" s="4">
-        <f t="shared" ref="I1485:I1486" si="542">YEAR(A1485)</f>
+        <f t="shared" ref="I1485:I1488" si="542">YEAR(A1485)</f>
         <v>2025</v>
       </c>
       <c r="J1485" s="4">
-        <f t="shared" ref="J1485:J1486" si="543">MONTH(A1485)</f>
+        <f t="shared" ref="J1485:J1488" si="543">MONTH(A1485)</f>
         <v>4</v>
       </c>
     </row>
@@ -54423,88 +54435,230 @@
       </c>
     </row>
     <row r="1487" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1487" s="3"/>
-      <c r="B1487" s="3"/>
-      <c r="C1487" s="3"/>
-      <c r="D1487" s="3"/>
-      <c r="E1487" s="3"/>
-      <c r="F1487" s="3"/>
-      <c r="G1487" s="3"/>
-      <c r="H1487" s="3"/>
-      <c r="I1487" s="4"/>
-      <c r="J1487" s="4"/>
+      <c r="A1487" s="3" t="s">
+        <v>1358</v>
+      </c>
+      <c r="B1487" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1487" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1487" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1487" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1487" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1487" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1487" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1487" s="4">
+        <f t="shared" si="542"/>
+        <v>2025</v>
+      </c>
+      <c r="J1487" s="4">
+        <f t="shared" si="543"/>
+        <v>4</v>
+      </c>
     </row>
     <row r="1488" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1488" s="3"/>
-      <c r="B1488" s="3"/>
-      <c r="C1488" s="3"/>
-      <c r="D1488" s="3"/>
-      <c r="E1488" s="3"/>
+      <c r="A1488" s="3" t="s">
+        <v>1359</v>
+      </c>
+      <c r="B1488" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1488" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1488" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1488" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1488" s="3"/>
-      <c r="G1488" s="3"/>
-      <c r="H1488" s="3"/>
-      <c r="I1488" s="4"/>
-      <c r="J1488" s="4"/>
+      <c r="G1488" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1488" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1488" s="4">
+        <f t="shared" si="542"/>
+        <v>2025</v>
+      </c>
+      <c r="J1488" s="4">
+        <f t="shared" si="543"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1489" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1489" s="3"/>
-      <c r="B1489" s="3"/>
-      <c r="C1489" s="3"/>
-      <c r="D1489" s="3"/>
-      <c r="E1489" s="3"/>
+      <c r="A1489" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B1489" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1489" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1489" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1489" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1489" s="3"/>
-      <c r="G1489" s="3"/>
-      <c r="H1489" s="3"/>
-      <c r="I1489" s="4"/>
-      <c r="J1489" s="4"/>
+      <c r="G1489" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1489" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1489" s="4">
+        <f t="shared" ref="I1489:I1491" si="544">YEAR(A1489)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1489" s="4">
+        <f t="shared" ref="J1489:J1491" si="545">MONTH(A1489)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1490" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1490" s="3"/>
-      <c r="B1490" s="3"/>
-      <c r="C1490" s="3"/>
-      <c r="D1490" s="3"/>
-      <c r="E1490" s="3"/>
+      <c r="A1490" s="3" t="s">
+        <v>1360</v>
+      </c>
+      <c r="B1490" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1490" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1490" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1490" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1490" s="3"/>
-      <c r="G1490" s="3"/>
-      <c r="H1490" s="3"/>
-      <c r="I1490" s="4"/>
-      <c r="J1490" s="4"/>
+      <c r="G1490" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1490" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1490" s="4">
+        <f t="shared" si="544"/>
+        <v>2025</v>
+      </c>
+      <c r="J1490" s="4">
+        <f t="shared" si="545"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1491" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1491" s="3"/>
-      <c r="B1491" s="3"/>
-      <c r="C1491" s="3"/>
-      <c r="D1491" s="3"/>
-      <c r="E1491" s="3"/>
+      <c r="A1491" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B1491" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1491" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="D1491" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1491" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1491" s="3"/>
-      <c r="G1491" s="3"/>
-      <c r="H1491" s="3"/>
-      <c r="I1491" s="4"/>
-      <c r="J1491" s="4"/>
+      <c r="G1491" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1491" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1491" s="4">
+        <f t="shared" si="544"/>
+        <v>2025</v>
+      </c>
+      <c r="J1491" s="4">
+        <f t="shared" si="545"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1492" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1492" s="3"/>
-      <c r="B1492" s="3"/>
-      <c r="C1492" s="3"/>
-      <c r="D1492" s="3"/>
-      <c r="E1492" s="3"/>
+      <c r="A1492" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B1492" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1492" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1492" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1492" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1492" s="3"/>
-      <c r="G1492" s="3"/>
-      <c r="H1492" s="3"/>
-      <c r="I1492" s="4"/>
-      <c r="J1492" s="4"/>
+      <c r="G1492" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1492" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1492" s="4">
+        <f t="shared" ref="I1492:I1493" si="546">YEAR(A1492)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1492" s="4">
+        <f t="shared" ref="J1492:J1493" si="547">MONTH(A1492)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1493" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1493" s="3"/>
-      <c r="B1493" s="3"/>
-      <c r="C1493" s="3"/>
-      <c r="D1493" s="3"/>
-      <c r="E1493" s="3"/>
+      <c r="A1493" s="3" t="s">
+        <v>1361</v>
+      </c>
+      <c r="B1493" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1493" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1493" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1493" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1493" s="3"/>
-      <c r="G1493" s="3"/>
-      <c r="H1493" s="3"/>
-      <c r="I1493" s="4"/>
-      <c r="J1493" s="4"/>
+      <c r="G1493" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1493" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1493" s="4">
+        <f t="shared" si="546"/>
+        <v>2025</v>
+      </c>
+      <c r="J1493" s="4">
+        <f t="shared" si="547"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1494" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1494" s="3"/>

</xml_diff>

<commit_message>
#54 Time Tracking: updated to 2025-05-23.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11630" uniqueCount="1362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11843" uniqueCount="1384">
   <si>
     <t>Year</t>
   </si>
@@ -4111,6 +4111,72 @@
   </si>
   <si>
     <t>2025-05-05</t>
+  </si>
+  <si>
+    <t>2025-05-06</t>
+  </si>
+  <si>
+    <t>2025-05-07</t>
+  </si>
+  <si>
+    <t>2025-05-08</t>
+  </si>
+  <si>
+    <t>nwreadinglist v4.3.0</t>
+  </si>
+  <si>
+    <t>2025-05-09</t>
+  </si>
+  <si>
+    <t>2025-05-11</t>
+  </si>
+  <si>
+    <t>2025-05-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nuitka/pyinstaller. </t>
+  </si>
+  <si>
+    <t>2025-05-13</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.5.1</t>
+  </si>
+  <si>
+    <t>2025-05-14</t>
+  </si>
+  <si>
+    <t>HackberryPi configuration.</t>
+  </si>
+  <si>
+    <t>2025-05-15</t>
+  </si>
+  <si>
+    <t>2025-05-17</t>
+  </si>
+  <si>
+    <t>2025-05-16</t>
+  </si>
+  <si>
+    <t>2025-05-18</t>
+  </si>
+  <si>
+    <t>nwdocstringchecking v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-05-19</t>
+  </si>
+  <si>
+    <t>nwcommitaverages v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-05-20</t>
+  </si>
+  <si>
+    <t>2025-05-22</t>
+  </si>
+  <si>
+    <t>2025-05-23</t>
   </si>
 </sst>
 </file>
@@ -4510,11 +4576,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1508"/>
+  <dimension ref="A1:J1559"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1469" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1495" sqref="F1495"/>
+      <pane ySplit="1" topLeftCell="A1496" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1523" sqref="E1523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -54620,11 +54686,11 @@
         <v>280</v>
       </c>
       <c r="I1492" s="4">
-        <f t="shared" ref="I1492:I1493" si="546">YEAR(A1492)</f>
+        <f t="shared" ref="I1492:I1494" si="546">YEAR(A1492)</f>
         <v>2025</v>
       </c>
       <c r="J1492" s="4">
-        <f t="shared" ref="J1492:J1493" si="547">MONTH(A1492)</f>
+        <f t="shared" ref="J1492:J1494" si="547">MONTH(A1492)</f>
         <v>5</v>
       </c>
     </row>
@@ -54661,184 +54727,1390 @@
       </c>
     </row>
     <row r="1494" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1494" s="3"/>
-      <c r="B1494" s="3"/>
-      <c r="C1494" s="3"/>
-      <c r="D1494" s="3"/>
-      <c r="E1494" s="3"/>
+      <c r="A1494" s="3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B1494" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1494" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="D1494" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1494" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1494" s="3"/>
-      <c r="G1494" s="3"/>
-      <c r="H1494" s="3"/>
-      <c r="I1494" s="4"/>
-      <c r="J1494" s="4"/>
+      <c r="G1494" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1494" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1494" s="4">
+        <f t="shared" si="546"/>
+        <v>2025</v>
+      </c>
+      <c r="J1494" s="4">
+        <f t="shared" si="547"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1495" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1495" s="3"/>
-      <c r="B1495" s="3"/>
-      <c r="C1495" s="3"/>
-      <c r="D1495" s="3"/>
-      <c r="E1495" s="3"/>
+      <c r="A1495" s="3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B1495" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1495" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1495" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1495" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1495" s="3"/>
-      <c r="G1495" s="3"/>
-      <c r="H1495" s="3"/>
-      <c r="I1495" s="4"/>
-      <c r="J1495" s="4"/>
+      <c r="G1495" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1495" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1495" s="4">
+        <f t="shared" ref="I1495:I1496" si="548">YEAR(A1495)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1495" s="4">
+        <f t="shared" ref="J1495:J1496" si="549">MONTH(A1495)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1496" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1496" s="3"/>
-      <c r="B1496" s="3"/>
-      <c r="C1496" s="3"/>
-      <c r="D1496" s="3"/>
-      <c r="E1496" s="3"/>
+      <c r="A1496" s="3" t="s">
+        <v>1362</v>
+      </c>
+      <c r="B1496" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1496" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1496" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1496" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1496" s="3"/>
-      <c r="G1496" s="3"/>
-      <c r="H1496" s="3"/>
-      <c r="I1496" s="4"/>
-      <c r="J1496" s="4"/>
+      <c r="G1496" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1496" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1496" s="4">
+        <f t="shared" si="548"/>
+        <v>2025</v>
+      </c>
+      <c r="J1496" s="4">
+        <f t="shared" si="549"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1497" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1497" s="3"/>
-      <c r="B1497" s="3"/>
-      <c r="C1497" s="3"/>
-      <c r="D1497" s="3"/>
-      <c r="E1497" s="3"/>
+      <c r="A1497" s="3" t="s">
+        <v>1363</v>
+      </c>
+      <c r="B1497" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1497" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1497" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1497" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1497" s="3"/>
-      <c r="G1497" s="3"/>
-      <c r="H1497" s="3"/>
-      <c r="I1497" s="4"/>
-      <c r="J1497" s="4"/>
+      <c r="G1497" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1497" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1497" s="4">
+        <f t="shared" ref="I1497:I1499" si="550">YEAR(A1497)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1497" s="4">
+        <f t="shared" ref="J1497:J1499" si="551">MONTH(A1497)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1498" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1498" s="3"/>
-      <c r="B1498" s="3"/>
-      <c r="C1498" s="3"/>
-      <c r="D1498" s="3"/>
-      <c r="E1498" s="3"/>
-      <c r="F1498" s="3"/>
-      <c r="G1498" s="3"/>
-      <c r="H1498" s="3"/>
-      <c r="I1498" s="4"/>
-      <c r="J1498" s="4"/>
+      <c r="A1498" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B1498" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1498" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1498" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1498" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1498" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G1498" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1498" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1498" s="4">
+        <f t="shared" si="550"/>
+        <v>2025</v>
+      </c>
+      <c r="J1498" s="4">
+        <f t="shared" si="551"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1499" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1499" s="3"/>
-      <c r="B1499" s="3"/>
-      <c r="C1499" s="3"/>
-      <c r="D1499" s="3"/>
-      <c r="E1499" s="3"/>
-      <c r="F1499" s="3"/>
-      <c r="G1499" s="3"/>
-      <c r="H1499" s="3"/>
-      <c r="I1499" s="4"/>
-      <c r="J1499" s="4"/>
+      <c r="A1499" s="3" t="s">
+        <v>1364</v>
+      </c>
+      <c r="B1499" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1499" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1499" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1499" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1499" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G1499" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1499" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1499" s="4">
+        <f t="shared" si="550"/>
+        <v>2025</v>
+      </c>
+      <c r="J1499" s="4">
+        <f t="shared" si="551"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1500" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1500" s="3"/>
-      <c r="B1500" s="3"/>
-      <c r="C1500" s="3"/>
-      <c r="D1500" s="3"/>
-      <c r="E1500" s="3"/>
-      <c r="F1500" s="3"/>
-      <c r="G1500" s="3"/>
-      <c r="H1500" s="3"/>
-      <c r="I1500" s="4"/>
-      <c r="J1500" s="4"/>
+      <c r="A1500" s="3" t="s">
+        <v>1366</v>
+      </c>
+      <c r="B1500" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1500" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1500" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1500" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1500" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G1500" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1500" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1500" s="4">
+        <f t="shared" ref="I1500" si="552">YEAR(A1500)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1500" s="4">
+        <f t="shared" ref="J1500" si="553">MONTH(A1500)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1501" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1501" s="3"/>
-      <c r="B1501" s="3"/>
-      <c r="C1501" s="3"/>
-      <c r="D1501" s="3"/>
-      <c r="E1501" s="3"/>
-      <c r="F1501" s="3"/>
-      <c r="G1501" s="3"/>
-      <c r="H1501" s="3"/>
-      <c r="I1501" s="4"/>
-      <c r="J1501" s="4"/>
+      <c r="A1501" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B1501" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1501" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1501" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1501" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1501" s="3" t="s">
+        <v>1365</v>
+      </c>
+      <c r="G1501" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1501" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1501" s="4">
+        <f t="shared" ref="I1501:I1503" si="554">YEAR(A1501)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1501" s="4">
+        <f t="shared" ref="J1501:J1503" si="555">MONTH(A1501)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1502" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1502" s="3"/>
-      <c r="B1502" s="3"/>
-      <c r="C1502" s="3"/>
-      <c r="D1502" s="3"/>
-      <c r="E1502" s="3"/>
+      <c r="A1502" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B1502" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1502" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1502" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1502" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1502" s="3"/>
-      <c r="G1502" s="3"/>
-      <c r="H1502" s="3"/>
-      <c r="I1502" s="4"/>
-      <c r="J1502" s="4"/>
+      <c r="G1502" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1502" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1502" s="4">
+        <f t="shared" si="554"/>
+        <v>2025</v>
+      </c>
+      <c r="J1502" s="4">
+        <f t="shared" si="555"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1503" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1503" s="3"/>
-      <c r="B1503" s="3"/>
-      <c r="C1503" s="3"/>
-      <c r="D1503" s="3"/>
-      <c r="E1503" s="3"/>
+      <c r="A1503" s="3" t="s">
+        <v>1367</v>
+      </c>
+      <c r="B1503" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="C1503" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1503" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="E1503" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1503" s="3"/>
-      <c r="G1503" s="3"/>
-      <c r="H1503" s="3"/>
-      <c r="I1503" s="4"/>
-      <c r="J1503" s="4"/>
+      <c r="G1503" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1503" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1503" s="4">
+        <f t="shared" si="554"/>
+        <v>2025</v>
+      </c>
+      <c r="J1503" s="4">
+        <f t="shared" si="555"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1504" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1504" s="3"/>
-      <c r="B1504" s="3"/>
-      <c r="C1504" s="3"/>
-      <c r="D1504" s="3"/>
-      <c r="E1504" s="3"/>
-      <c r="F1504" s="3"/>
-      <c r="G1504" s="3"/>
-      <c r="H1504" s="3"/>
-      <c r="I1504" s="4"/>
-      <c r="J1504" s="4"/>
+      <c r="A1504" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B1504" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1504" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1504" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1504" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1504" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G1504" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1504" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1504" s="4">
+        <f t="shared" ref="I1504:I1505" si="556">YEAR(A1504)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1504" s="4">
+        <f t="shared" ref="J1504:J1505" si="557">MONTH(A1504)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1505" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1505" s="3"/>
-      <c r="B1505" s="3"/>
-      <c r="C1505" s="3"/>
-      <c r="D1505" s="3"/>
-      <c r="E1505" s="3"/>
-      <c r="F1505" s="3"/>
-      <c r="G1505" s="3"/>
-      <c r="H1505" s="3"/>
-      <c r="I1505" s="4"/>
-      <c r="J1505" s="4"/>
+      <c r="A1505" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B1505" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1505" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1505" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1505" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1505" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G1505" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1505" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1505" s="4">
+        <f t="shared" si="556"/>
+        <v>2025</v>
+      </c>
+      <c r="J1505" s="4">
+        <f t="shared" si="557"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1506" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1506" s="3"/>
-      <c r="B1506" s="3"/>
-      <c r="C1506" s="3"/>
-      <c r="D1506" s="3"/>
-      <c r="E1506" s="3"/>
-      <c r="F1506" s="3"/>
-      <c r="G1506" s="3"/>
-      <c r="H1506" s="3"/>
-      <c r="I1506" s="4"/>
-      <c r="J1506" s="4"/>
+      <c r="A1506" s="3" t="s">
+        <v>1368</v>
+      </c>
+      <c r="B1506" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1506" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1506" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1506" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1506" s="3" t="s">
+        <v>1369</v>
+      </c>
+      <c r="G1506" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1506" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1506" s="4">
+        <f t="shared" ref="I1506:I1508" si="558">YEAR(A1506)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1506" s="4">
+        <f t="shared" ref="J1506:J1508" si="559">MONTH(A1506)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1507" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1507" s="3"/>
-      <c r="B1507" s="3"/>
-      <c r="C1507" s="3"/>
-      <c r="D1507" s="3"/>
-      <c r="E1507" s="3"/>
-      <c r="F1507" s="3"/>
-      <c r="G1507" s="3"/>
-      <c r="H1507" s="3"/>
-      <c r="I1507" s="4"/>
-      <c r="J1507" s="4"/>
+      <c r="A1507" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B1507" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1507" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1507" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1507" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1507" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="G1507" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1507" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1507" s="4">
+        <f t="shared" si="558"/>
+        <v>2025</v>
+      </c>
+      <c r="J1507" s="4">
+        <f t="shared" si="559"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1508" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1508" s="3"/>
-      <c r="B1508" s="3"/>
-      <c r="C1508" s="3"/>
-      <c r="D1508" s="3"/>
-      <c r="E1508" s="3"/>
-      <c r="F1508" s="3"/>
-      <c r="G1508" s="3"/>
-      <c r="H1508" s="3"/>
-      <c r="I1508" s="4"/>
-      <c r="J1508" s="4"/>
+      <c r="A1508" s="3" t="s">
+        <v>1370</v>
+      </c>
+      <c r="B1508" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1508" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1508" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1508" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1508" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="G1508" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1508" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1508" s="4">
+        <f t="shared" si="558"/>
+        <v>2025</v>
+      </c>
+      <c r="J1508" s="4">
+        <f t="shared" si="559"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1509" s="3" t="s">
+        <v>1372</v>
+      </c>
+      <c r="B1509" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="C1509" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1509" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1509" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1509" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G1509" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1509" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1509" s="4">
+        <f t="shared" ref="I1509" si="560">YEAR(A1509)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1509" s="4">
+        <f t="shared" ref="J1509" si="561">MONTH(A1509)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1510" s="3" t="s">
+        <v>1374</v>
+      </c>
+      <c r="B1510" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1510" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1510" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1510" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1510" s="3"/>
+      <c r="G1510" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1510" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1510" s="4">
+        <f t="shared" ref="I1510" si="562">YEAR(A1510)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1510" s="4">
+        <f t="shared" ref="J1510" si="563">MONTH(A1510)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1511" s="3" t="s">
+        <v>1376</v>
+      </c>
+      <c r="B1511" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1511" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1511" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1511" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1511" s="3"/>
+      <c r="G1511" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1511" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1511" s="4">
+        <f t="shared" ref="I1511" si="564">YEAR(A1511)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1511" s="4">
+        <f t="shared" ref="J1511" si="565">MONTH(A1511)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1512" s="3" t="s">
+        <v>1375</v>
+      </c>
+      <c r="B1512" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1512" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1512" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1512" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1512" s="3" t="s">
+        <v>1373</v>
+      </c>
+      <c r="G1512" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1512" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1512" s="4">
+        <f t="shared" ref="I1512:I1514" si="566">YEAR(A1512)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1512" s="4">
+        <f t="shared" ref="J1512:J1514" si="567">MONTH(A1512)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1513" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1513" s="3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B1513" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1513" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1513" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1513" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1513" s="3" t="s">
+        <v>1371</v>
+      </c>
+      <c r="G1513" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1513" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1513" s="4">
+        <f t="shared" si="566"/>
+        <v>2025</v>
+      </c>
+      <c r="J1513" s="4">
+        <f t="shared" si="567"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1514" s="3" t="s">
+        <v>1377</v>
+      </c>
+      <c r="B1514" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1514" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1514" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1514" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1514" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G1514" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1514" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1514" s="4">
+        <f t="shared" si="566"/>
+        <v>2025</v>
+      </c>
+      <c r="J1514" s="4">
+        <f t="shared" si="567"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1515" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B1515" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1515" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1515" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1515" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1515" s="3" t="s">
+        <v>1378</v>
+      </c>
+      <c r="G1515" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1515" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1515" s="4">
+        <f t="shared" ref="I1515:I1516" si="568">YEAR(A1515)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1515" s="4">
+        <f t="shared" ref="J1515:J1516" si="569">MONTH(A1515)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1516" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B1516" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1516" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1516" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1516" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1516" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G1516" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1516" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1516" s="4">
+        <f t="shared" si="568"/>
+        <v>2025</v>
+      </c>
+      <c r="J1516" s="4">
+        <f t="shared" si="569"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1517" s="3" t="s">
+        <v>1379</v>
+      </c>
+      <c r="B1517" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1517" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1517" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1517" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1517" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G1517" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1517" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1517" s="4">
+        <f>YEAR(A1517)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1517" s="4">
+        <f>MONTH(A1517)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1518" s="3" t="s">
+        <v>1381</v>
+      </c>
+      <c r="B1518" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1518" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1518" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1518" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1518" s="3" t="s">
+        <v>1380</v>
+      </c>
+      <c r="G1518" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1518" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1518" s="4">
+        <f>YEAR(A1518)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1518" s="4">
+        <f>MONTH(A1518)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1519" s="3" t="s">
+        <v>1382</v>
+      </c>
+      <c r="B1519" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1519" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1519" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1519" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1519" s="3"/>
+      <c r="G1519" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1519" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1519" s="4">
+        <f t="shared" ref="I1519:I1521" si="570">YEAR(A1519)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1519" s="4">
+        <f t="shared" ref="J1519:J1521" si="571">MONTH(A1519)</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1520" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B1520" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1520" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1520" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1520" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1520" s="3"/>
+      <c r="G1520" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1520" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1520" s="4">
+        <f t="shared" si="570"/>
+        <v>2025</v>
+      </c>
+      <c r="J1520" s="4">
+        <f t="shared" si="571"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1521" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B1521" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1521" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1521" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1521" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1521" s="3"/>
+      <c r="G1521" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1521" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1521" s="4">
+        <f t="shared" si="570"/>
+        <v>2025</v>
+      </c>
+      <c r="J1521" s="4">
+        <f t="shared" si="571"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1522" s="3"/>
+      <c r="B1522" s="3"/>
+      <c r="C1522" s="3"/>
+      <c r="D1522" s="3"/>
+      <c r="E1522" s="3"/>
+      <c r="F1522" s="3"/>
+      <c r="G1522" s="3"/>
+      <c r="H1522" s="3"/>
+      <c r="I1522" s="4"/>
+      <c r="J1522" s="4"/>
+    </row>
+    <row r="1523" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1523" s="3"/>
+      <c r="B1523" s="3"/>
+      <c r="C1523" s="3"/>
+      <c r="D1523" s="3"/>
+      <c r="E1523" s="3"/>
+      <c r="F1523" s="3"/>
+      <c r="G1523" s="3"/>
+      <c r="H1523" s="3"/>
+      <c r="I1523" s="4"/>
+      <c r="J1523" s="4"/>
+    </row>
+    <row r="1524" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1524" s="3"/>
+      <c r="B1524" s="3"/>
+      <c r="C1524" s="3"/>
+      <c r="D1524" s="3"/>
+      <c r="E1524" s="3"/>
+      <c r="F1524" s="3"/>
+      <c r="G1524" s="3"/>
+      <c r="H1524" s="3"/>
+      <c r="I1524" s="4"/>
+      <c r="J1524" s="4"/>
+    </row>
+    <row r="1525" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1525" s="3"/>
+      <c r="B1525" s="3"/>
+      <c r="C1525" s="3"/>
+      <c r="D1525" s="3"/>
+      <c r="E1525" s="3"/>
+      <c r="F1525" s="3"/>
+      <c r="G1525" s="3"/>
+      <c r="H1525" s="3"/>
+      <c r="I1525" s="4"/>
+      <c r="J1525" s="4"/>
+    </row>
+    <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1526" s="3"/>
+      <c r="B1526" s="3"/>
+      <c r="C1526" s="3"/>
+      <c r="D1526" s="3"/>
+      <c r="E1526" s="3"/>
+      <c r="F1526" s="3"/>
+      <c r="G1526" s="3"/>
+      <c r="H1526" s="3"/>
+      <c r="I1526" s="4"/>
+      <c r="J1526" s="4"/>
+    </row>
+    <row r="1527" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1527" s="3"/>
+      <c r="B1527" s="3"/>
+      <c r="C1527" s="3"/>
+      <c r="D1527" s="3"/>
+      <c r="E1527" s="3"/>
+      <c r="F1527" s="3"/>
+      <c r="G1527" s="3"/>
+      <c r="H1527" s="3"/>
+      <c r="I1527" s="4"/>
+      <c r="J1527" s="4"/>
+    </row>
+    <row r="1528" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1528" s="3"/>
+      <c r="B1528" s="3"/>
+      <c r="C1528" s="3"/>
+      <c r="D1528" s="3"/>
+      <c r="E1528" s="3"/>
+      <c r="F1528" s="3"/>
+      <c r="G1528" s="3"/>
+      <c r="H1528" s="3"/>
+      <c r="I1528" s="4"/>
+      <c r="J1528" s="4"/>
+    </row>
+    <row r="1529" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1529" s="3"/>
+      <c r="B1529" s="3"/>
+      <c r="C1529" s="3"/>
+      <c r="D1529" s="3"/>
+      <c r="E1529" s="3"/>
+      <c r="F1529" s="3"/>
+      <c r="G1529" s="3"/>
+      <c r="H1529" s="3"/>
+      <c r="I1529" s="4"/>
+      <c r="J1529" s="4"/>
+    </row>
+    <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1530" s="3"/>
+      <c r="B1530" s="3"/>
+      <c r="C1530" s="3"/>
+      <c r="D1530" s="3"/>
+      <c r="E1530" s="3"/>
+      <c r="F1530" s="3"/>
+      <c r="G1530" s="3"/>
+      <c r="H1530" s="3"/>
+      <c r="I1530" s="4"/>
+      <c r="J1530" s="4"/>
+    </row>
+    <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1531" s="3"/>
+      <c r="B1531" s="3"/>
+      <c r="C1531" s="3"/>
+      <c r="D1531" s="3"/>
+      <c r="E1531" s="3"/>
+      <c r="F1531" s="3"/>
+      <c r="G1531" s="3"/>
+      <c r="H1531" s="3"/>
+      <c r="I1531" s="4"/>
+      <c r="J1531" s="4"/>
+    </row>
+    <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1532" s="3"/>
+      <c r="B1532" s="3"/>
+      <c r="C1532" s="3"/>
+      <c r="D1532" s="3"/>
+      <c r="E1532" s="3"/>
+      <c r="F1532" s="3"/>
+      <c r="G1532" s="3"/>
+      <c r="H1532" s="3"/>
+      <c r="I1532" s="4"/>
+      <c r="J1532" s="4"/>
+    </row>
+    <row r="1533" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1533" s="3"/>
+      <c r="B1533" s="3"/>
+      <c r="C1533" s="3"/>
+      <c r="D1533" s="3"/>
+      <c r="E1533" s="3"/>
+      <c r="F1533" s="3"/>
+      <c r="G1533" s="3"/>
+      <c r="H1533" s="3"/>
+      <c r="I1533" s="4"/>
+      <c r="J1533" s="4"/>
+    </row>
+    <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1534" s="3"/>
+      <c r="B1534" s="3"/>
+      <c r="C1534" s="3"/>
+      <c r="D1534" s="3"/>
+      <c r="E1534" s="3"/>
+      <c r="F1534" s="3"/>
+      <c r="G1534" s="3"/>
+      <c r="H1534" s="3"/>
+      <c r="I1534" s="4"/>
+      <c r="J1534" s="4"/>
+    </row>
+    <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1535" s="3"/>
+      <c r="B1535" s="3"/>
+      <c r="C1535" s="3"/>
+      <c r="D1535" s="3"/>
+      <c r="E1535" s="3"/>
+      <c r="F1535" s="3"/>
+      <c r="G1535" s="3"/>
+      <c r="H1535" s="3"/>
+      <c r="I1535" s="4"/>
+      <c r="J1535" s="4"/>
+    </row>
+    <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1536" s="3"/>
+      <c r="B1536" s="3"/>
+      <c r="C1536" s="3"/>
+      <c r="D1536" s="3"/>
+      <c r="E1536" s="3"/>
+      <c r="F1536" s="3"/>
+      <c r="G1536" s="3"/>
+      <c r="H1536" s="3"/>
+      <c r="I1536" s="4"/>
+      <c r="J1536" s="4"/>
+    </row>
+    <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1537" s="3"/>
+      <c r="B1537" s="3"/>
+      <c r="C1537" s="3"/>
+      <c r="D1537" s="3"/>
+      <c r="E1537" s="3"/>
+      <c r="F1537" s="3"/>
+      <c r="G1537" s="3"/>
+      <c r="H1537" s="3"/>
+      <c r="I1537" s="4"/>
+      <c r="J1537" s="4"/>
+    </row>
+    <row r="1538" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1538" s="3"/>
+      <c r="B1538" s="3"/>
+      <c r="C1538" s="3"/>
+      <c r="D1538" s="3"/>
+      <c r="E1538" s="3"/>
+      <c r="F1538" s="3"/>
+      <c r="G1538" s="3"/>
+      <c r="H1538" s="3"/>
+      <c r="I1538" s="4"/>
+      <c r="J1538" s="4"/>
+    </row>
+    <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1539" s="3"/>
+      <c r="B1539" s="3"/>
+      <c r="C1539" s="3"/>
+      <c r="D1539" s="3"/>
+      <c r="E1539" s="3"/>
+      <c r="F1539" s="3"/>
+      <c r="G1539" s="3"/>
+      <c r="H1539" s="3"/>
+      <c r="I1539" s="4"/>
+      <c r="J1539" s="4"/>
+    </row>
+    <row r="1540" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1540" s="3"/>
+      <c r="B1540" s="3"/>
+      <c r="C1540" s="3"/>
+      <c r="D1540" s="3"/>
+      <c r="E1540" s="3"/>
+      <c r="F1540" s="3"/>
+      <c r="G1540" s="3"/>
+      <c r="H1540" s="3"/>
+      <c r="I1540" s="4"/>
+      <c r="J1540" s="4"/>
+    </row>
+    <row r="1541" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1541" s="3"/>
+      <c r="B1541" s="3"/>
+      <c r="C1541" s="3"/>
+      <c r="D1541" s="3"/>
+      <c r="E1541" s="3"/>
+      <c r="F1541" s="3"/>
+      <c r="G1541" s="3"/>
+      <c r="H1541" s="3"/>
+      <c r="I1541" s="4"/>
+      <c r="J1541" s="4"/>
+    </row>
+    <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1542" s="3"/>
+      <c r="B1542" s="3"/>
+      <c r="C1542" s="3"/>
+      <c r="D1542" s="3"/>
+      <c r="E1542" s="3"/>
+      <c r="F1542" s="3"/>
+      <c r="G1542" s="3"/>
+      <c r="H1542" s="3"/>
+      <c r="I1542" s="4"/>
+      <c r="J1542" s="4"/>
+    </row>
+    <row r="1543" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1543" s="3"/>
+      <c r="B1543" s="3"/>
+      <c r="C1543" s="3"/>
+      <c r="D1543" s="3"/>
+      <c r="E1543" s="3"/>
+      <c r="F1543" s="3"/>
+      <c r="G1543" s="3"/>
+      <c r="H1543" s="3"/>
+      <c r="I1543" s="4"/>
+      <c r="J1543" s="4"/>
+    </row>
+    <row r="1544" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1544" s="3"/>
+      <c r="B1544" s="3"/>
+      <c r="C1544" s="3"/>
+      <c r="D1544" s="3"/>
+      <c r="E1544" s="3"/>
+      <c r="F1544" s="3"/>
+      <c r="G1544" s="3"/>
+      <c r="H1544" s="3"/>
+      <c r="I1544" s="4"/>
+      <c r="J1544" s="4"/>
+    </row>
+    <row r="1545" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1545" s="3"/>
+      <c r="B1545" s="3"/>
+      <c r="C1545" s="3"/>
+      <c r="D1545" s="3"/>
+      <c r="E1545" s="3"/>
+      <c r="F1545" s="3"/>
+      <c r="G1545" s="3"/>
+      <c r="H1545" s="3"/>
+      <c r="I1545" s="4"/>
+      <c r="J1545" s="4"/>
+    </row>
+    <row r="1546" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1546" s="3"/>
+      <c r="B1546" s="3"/>
+      <c r="C1546" s="3"/>
+      <c r="D1546" s="3"/>
+      <c r="E1546" s="3"/>
+      <c r="F1546" s="3"/>
+      <c r="G1546" s="3"/>
+      <c r="H1546" s="3"/>
+      <c r="I1546" s="4"/>
+      <c r="J1546" s="4"/>
+    </row>
+    <row r="1547" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1547" s="3"/>
+      <c r="B1547" s="3"/>
+      <c r="C1547" s="3"/>
+      <c r="D1547" s="3"/>
+      <c r="E1547" s="3"/>
+      <c r="F1547" s="3"/>
+      <c r="G1547" s="3"/>
+      <c r="H1547" s="3"/>
+      <c r="I1547" s="4"/>
+      <c r="J1547" s="4"/>
+    </row>
+    <row r="1548" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1548" s="3"/>
+      <c r="B1548" s="3"/>
+      <c r="C1548" s="3"/>
+      <c r="D1548" s="3"/>
+      <c r="E1548" s="3"/>
+      <c r="F1548" s="3"/>
+      <c r="G1548" s="3"/>
+      <c r="H1548" s="3"/>
+      <c r="I1548" s="4"/>
+      <c r="J1548" s="4"/>
+    </row>
+    <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1549" s="3"/>
+      <c r="B1549" s="3"/>
+      <c r="C1549" s="3"/>
+      <c r="D1549" s="3"/>
+      <c r="E1549" s="3"/>
+      <c r="F1549" s="3"/>
+      <c r="G1549" s="3"/>
+      <c r="H1549" s="3"/>
+      <c r="I1549" s="4"/>
+      <c r="J1549" s="4"/>
+    </row>
+    <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1550" s="3"/>
+      <c r="B1550" s="3"/>
+      <c r="C1550" s="3"/>
+      <c r="D1550" s="3"/>
+      <c r="E1550" s="3"/>
+      <c r="F1550" s="3"/>
+      <c r="G1550" s="3"/>
+      <c r="H1550" s="3"/>
+      <c r="I1550" s="4"/>
+      <c r="J1550" s="4"/>
+    </row>
+    <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1551" s="3"/>
+      <c r="B1551" s="3"/>
+      <c r="C1551" s="3"/>
+      <c r="D1551" s="3"/>
+      <c r="E1551" s="3"/>
+      <c r="F1551" s="3"/>
+      <c r="G1551" s="3"/>
+      <c r="H1551" s="3"/>
+      <c r="I1551" s="4"/>
+      <c r="J1551" s="4"/>
+    </row>
+    <row r="1552" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1552" s="3"/>
+      <c r="B1552" s="3"/>
+      <c r="C1552" s="3"/>
+      <c r="D1552" s="3"/>
+      <c r="E1552" s="3"/>
+      <c r="F1552" s="3"/>
+      <c r="G1552" s="3"/>
+      <c r="H1552" s="3"/>
+      <c r="I1552" s="4"/>
+      <c r="J1552" s="4"/>
+    </row>
+    <row r="1553" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1553" s="3"/>
+      <c r="B1553" s="3"/>
+      <c r="C1553" s="3"/>
+      <c r="D1553" s="3"/>
+      <c r="E1553" s="3"/>
+      <c r="F1553" s="3"/>
+      <c r="G1553" s="3"/>
+      <c r="H1553" s="3"/>
+      <c r="I1553" s="4"/>
+      <c r="J1553" s="4"/>
+    </row>
+    <row r="1554" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1554" s="3"/>
+      <c r="B1554" s="3"/>
+      <c r="C1554" s="3"/>
+      <c r="D1554" s="3"/>
+      <c r="E1554" s="3"/>
+      <c r="F1554" s="3"/>
+      <c r="G1554" s="3"/>
+      <c r="H1554" s="3"/>
+      <c r="I1554" s="4"/>
+      <c r="J1554" s="4"/>
+    </row>
+    <row r="1555" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1555" s="3"/>
+      <c r="B1555" s="3"/>
+      <c r="C1555" s="3"/>
+      <c r="D1555" s="3"/>
+      <c r="E1555" s="3"/>
+      <c r="F1555" s="3"/>
+      <c r="G1555" s="3"/>
+      <c r="H1555" s="3"/>
+      <c r="I1555" s="4"/>
+      <c r="J1555" s="4"/>
+    </row>
+    <row r="1556" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1556" s="3"/>
+      <c r="B1556" s="3"/>
+      <c r="C1556" s="3"/>
+      <c r="D1556" s="3"/>
+      <c r="E1556" s="3"/>
+      <c r="F1556" s="3"/>
+      <c r="G1556" s="3"/>
+      <c r="H1556" s="3"/>
+      <c r="I1556" s="4"/>
+      <c r="J1556" s="4"/>
+    </row>
+    <row r="1557" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1557" s="3"/>
+      <c r="B1557" s="3"/>
+      <c r="C1557" s="3"/>
+      <c r="D1557" s="3"/>
+      <c r="E1557" s="3"/>
+      <c r="F1557" s="3"/>
+      <c r="G1557" s="3"/>
+      <c r="H1557" s="3"/>
+      <c r="I1557" s="4"/>
+      <c r="J1557" s="4"/>
+    </row>
+    <row r="1558" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1558" s="3"/>
+      <c r="B1558" s="3"/>
+      <c r="C1558" s="3"/>
+      <c r="D1558" s="3"/>
+      <c r="E1558" s="3"/>
+      <c r="F1558" s="3"/>
+      <c r="G1558" s="3"/>
+      <c r="H1558" s="3"/>
+      <c r="I1558" s="4"/>
+      <c r="J1558" s="4"/>
+    </row>
+    <row r="1559" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1559" s="3"/>
+      <c r="B1559" s="3"/>
+      <c r="C1559" s="3"/>
+      <c r="D1559" s="3"/>
+      <c r="E1559" s="3"/>
+      <c r="F1559" s="3"/>
+      <c r="G1559" s="3"/>
+      <c r="H1559" s="3"/>
+      <c r="I1559" s="4"/>
+      <c r="J1559" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#54 Time Tracking: updated to 2025-05-25.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11843" uniqueCount="1384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11867" uniqueCount="1385">
   <si>
     <t>Year</t>
   </si>
@@ -4134,9 +4134,6 @@
     <t>2025-05-12</t>
   </si>
   <si>
-    <t xml:space="preserve">Nuitka/pyinstaller. </t>
-  </si>
-  <si>
     <t>2025-05-13</t>
   </si>
   <si>
@@ -4177,6 +4174,12 @@
   </si>
   <si>
     <t>2025-05-23</t>
+  </si>
+  <si>
+    <t>2025-05-25</t>
+  </si>
+  <si>
+    <t>nwbuild v1.0.0</t>
   </si>
 </sst>
 </file>
@@ -4580,7 +4583,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1496" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1523" sqref="E1523"/>
+      <selection pane="bottomLeft" activeCell="F1527" sqref="F1527"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -55068,13 +55071,13 @@
         <v>239</v>
       </c>
       <c r="E1504" s="3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="F1504" s="3" t="s">
-        <v>1369</v>
+        <v>1384</v>
       </c>
       <c r="G1504" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H1504" s="8" t="s">
         <v>280</v>
@@ -55102,13 +55105,13 @@
         <v>168</v>
       </c>
       <c r="E1505" s="3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="F1505" s="3" t="s">
-        <v>1369</v>
+        <v>1384</v>
       </c>
       <c r="G1505" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H1505" s="8" t="s">
         <v>280</v>
@@ -55136,13 +55139,13 @@
         <v>111</v>
       </c>
       <c r="E1506" s="3" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="F1506" s="3" t="s">
-        <v>1369</v>
+        <v>1384</v>
       </c>
       <c r="G1506" s="8" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="H1506" s="8" t="s">
         <v>280</v>
@@ -55158,7 +55161,7 @@
     </row>
     <row r="1507" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1507" s="3" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B1507" s="3" t="s">
         <v>331</v>
@@ -55173,7 +55176,7 @@
         <v>127</v>
       </c>
       <c r="F1507" s="3" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="G1507" s="8" t="s">
         <v>279</v>
@@ -55192,7 +55195,7 @@
     </row>
     <row r="1508" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1508" s="3" t="s">
-        <v>1370</v>
+        <v>1369</v>
       </c>
       <c r="B1508" s="3" t="s">
         <v>160</v>
@@ -55207,7 +55210,7 @@
         <v>127</v>
       </c>
       <c r="F1508" s="3" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="G1508" s="8" t="s">
         <v>279</v>
@@ -55226,7 +55229,7 @@
     </row>
     <row r="1509" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1509" s="3" t="s">
-        <v>1372</v>
+        <v>1371</v>
       </c>
       <c r="B1509" s="3" t="s">
         <v>267</v>
@@ -55241,7 +55244,7 @@
         <v>140</v>
       </c>
       <c r="F1509" s="3" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="G1509" s="8" t="s">
         <v>280</v>
@@ -55260,7 +55263,7 @@
     </row>
     <row r="1510" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1510" s="3" t="s">
-        <v>1374</v>
+        <v>1373</v>
       </c>
       <c r="B1510" s="3" t="s">
         <v>149</v>
@@ -55292,7 +55295,7 @@
     </row>
     <row r="1511" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1511" s="3" t="s">
-        <v>1376</v>
+        <v>1375</v>
       </c>
       <c r="B1511" s="3" t="s">
         <v>248</v>
@@ -55324,7 +55327,7 @@
     </row>
     <row r="1512" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1512" s="3" t="s">
-        <v>1375</v>
+        <v>1374</v>
       </c>
       <c r="B1512" s="3" t="s">
         <v>123</v>
@@ -55339,7 +55342,7 @@
         <v>140</v>
       </c>
       <c r="F1512" s="3" t="s">
-        <v>1373</v>
+        <v>1372</v>
       </c>
       <c r="G1512" s="8" t="s">
         <v>280</v>
@@ -55358,7 +55361,7 @@
     </row>
     <row r="1513" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1513" s="3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B1513" s="3" t="s">
         <v>174</v>
@@ -55373,7 +55376,7 @@
         <v>127</v>
       </c>
       <c r="F1513" s="3" t="s">
-        <v>1371</v>
+        <v>1370</v>
       </c>
       <c r="G1513" s="8" t="s">
         <v>279</v>
@@ -55392,7 +55395,7 @@
     </row>
     <row r="1514" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1514" s="3" t="s">
-        <v>1377</v>
+        <v>1376</v>
       </c>
       <c r="B1514" s="3" t="s">
         <v>271</v>
@@ -55407,7 +55410,7 @@
         <v>127</v>
       </c>
       <c r="F1514" s="3" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="G1514" s="8" t="s">
         <v>279</v>
@@ -55426,7 +55429,7 @@
     </row>
     <row r="1515" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1515" s="3" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B1515" s="3" t="s">
         <v>355</v>
@@ -55441,7 +55444,7 @@
         <v>127</v>
       </c>
       <c r="F1515" s="3" t="s">
-        <v>1378</v>
+        <v>1377</v>
       </c>
       <c r="G1515" s="8" t="s">
         <v>279</v>
@@ -55460,7 +55463,7 @@
     </row>
     <row r="1516" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1516" s="3" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B1516" s="3" t="s">
         <v>219</v>
@@ -55475,7 +55478,7 @@
         <v>127</v>
       </c>
       <c r="F1516" s="3" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G1516" s="8" t="s">
         <v>279</v>
@@ -55494,7 +55497,7 @@
     </row>
     <row r="1517" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1517" s="3" t="s">
-        <v>1379</v>
+        <v>1378</v>
       </c>
       <c r="B1517" s="3" t="s">
         <v>114</v>
@@ -55509,7 +55512,7 @@
         <v>127</v>
       </c>
       <c r="F1517" s="3" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G1517" s="8" t="s">
         <v>279</v>
@@ -55528,7 +55531,7 @@
     </row>
     <row r="1518" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1518" s="3" t="s">
-        <v>1381</v>
+        <v>1380</v>
       </c>
       <c r="B1518" s="3" t="s">
         <v>180</v>
@@ -55543,7 +55546,7 @@
         <v>127</v>
       </c>
       <c r="F1518" s="3" t="s">
-        <v>1380</v>
+        <v>1379</v>
       </c>
       <c r="G1518" s="8" t="s">
         <v>279</v>
@@ -55562,7 +55565,7 @@
     </row>
     <row r="1519" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1519" s="3" t="s">
-        <v>1382</v>
+        <v>1381</v>
       </c>
       <c r="B1519" s="3" t="s">
         <v>248</v>
@@ -55584,17 +55587,17 @@
         <v>280</v>
       </c>
       <c r="I1519" s="4">
-        <f t="shared" ref="I1519:I1521" si="570">YEAR(A1519)</f>
+        <f t="shared" ref="I1519:I1522" si="570">YEAR(A1519)</f>
         <v>2025</v>
       </c>
       <c r="J1519" s="4">
-        <f t="shared" ref="J1519:J1521" si="571">MONTH(A1519)</f>
+        <f t="shared" ref="J1519:J1522" si="571">MONTH(A1519)</f>
         <v>5</v>
       </c>
     </row>
     <row r="1520" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1520" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B1520" s="3" t="s">
         <v>248</v>
@@ -55626,7 +55629,7 @@
     </row>
     <row r="1521" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1521" s="3" t="s">
-        <v>1383</v>
+        <v>1382</v>
       </c>
       <c r="B1521" s="3" t="s">
         <v>219</v>
@@ -55657,40 +55660,106 @@
       </c>
     </row>
     <row r="1522" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1522" s="3"/>
-      <c r="B1522" s="3"/>
-      <c r="C1522" s="3"/>
-      <c r="D1522" s="3"/>
-      <c r="E1522" s="3"/>
-      <c r="F1522" s="3"/>
-      <c r="G1522" s="3"/>
-      <c r="H1522" s="3"/>
-      <c r="I1522" s="4"/>
-      <c r="J1522" s="4"/>
+      <c r="A1522" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B1522" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1522" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1522" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1522" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1522" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G1522" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1522" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1522" s="4">
+        <f t="shared" si="570"/>
+        <v>2025</v>
+      </c>
+      <c r="J1522" s="4">
+        <f t="shared" si="571"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1523" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1523" s="3"/>
-      <c r="B1523" s="3"/>
-      <c r="C1523" s="3"/>
-      <c r="D1523" s="3"/>
-      <c r="E1523" s="3"/>
-      <c r="F1523" s="3"/>
-      <c r="G1523" s="3"/>
-      <c r="H1523" s="3"/>
-      <c r="I1523" s="4"/>
-      <c r="J1523" s="4"/>
+      <c r="A1523" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B1523" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1523" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1523" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E1523" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1523" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G1523" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1523" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1523" s="4">
+        <f>YEAR(A1523)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1523" s="4">
+        <f>MONTH(A1523)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1524" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1524" s="3"/>
-      <c r="B1524" s="3"/>
-      <c r="C1524" s="3"/>
-      <c r="D1524" s="3"/>
-      <c r="E1524" s="3"/>
-      <c r="F1524" s="3"/>
-      <c r="G1524" s="3"/>
-      <c r="H1524" s="3"/>
-      <c r="I1524" s="4"/>
-      <c r="J1524" s="4"/>
+      <c r="A1524" s="3" t="s">
+        <v>1383</v>
+      </c>
+      <c r="B1524" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1524" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1524" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1524" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1524" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G1524" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1524" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1524" s="4">
+        <f>YEAR(A1524)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1524" s="4">
+        <f>MONTH(A1524)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1525" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1525" s="3"/>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-06-23.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11867" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12210" uniqueCount="1411">
   <si>
     <t>Year</t>
   </si>
@@ -4180,6 +4180,84 @@
   </si>
   <si>
     <t>nwbuild v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-05-26</t>
+  </si>
+  <si>
+    <t>nwtimetracking v5.0.2</t>
+  </si>
+  <si>
+    <t>nwreadinglist v4.3.2</t>
+  </si>
+  <si>
+    <t>nwtraderaanalytics v4.5.2</t>
+  </si>
+  <si>
+    <t>nwshared v1.8.2</t>
+  </si>
+  <si>
+    <t>nwpackageversions v1.8.2</t>
+  </si>
+  <si>
+    <t>2025-05-27</t>
+  </si>
+  <si>
+    <t>nwtraderanalytics v?</t>
+  </si>
+  <si>
+    <t>2025-05-29</t>
+  </si>
+  <si>
+    <t>2025-05-30</t>
+  </si>
+  <si>
+    <t>2025-05-31</t>
+  </si>
+  <si>
+    <t>2025-06-01</t>
+  </si>
+  <si>
+    <t>2025-06-02</t>
+  </si>
+  <si>
+    <t>2025-06-03</t>
+  </si>
+  <si>
+    <t>nwdatamarkadanalytics v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-06-05</t>
+  </si>
+  <si>
+    <t>2025-06-06</t>
+  </si>
+  <si>
+    <t>2025-06-07</t>
+  </si>
+  <si>
+    <t>2025-06-08</t>
+  </si>
+  <si>
+    <t>2025-06-10</t>
+  </si>
+  <si>
+    <t>2025-06-11</t>
+  </si>
+  <si>
+    <t>2025-06-12</t>
+  </si>
+  <si>
+    <t>2025-06-13</t>
+  </si>
+  <si>
+    <t>2025-06-21</t>
+  </si>
+  <si>
+    <t>2025-06-22</t>
+  </si>
+  <si>
+    <t>2025-06-23</t>
   </si>
 </sst>
 </file>
@@ -4210,7 +4288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4220,6 +4298,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4251,7 +4335,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4273,6 +4357,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -4579,11 +4666,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1559"/>
+  <dimension ref="A1:J1627"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1496" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1527" sqref="F1527"/>
+      <pane ySplit="1" topLeftCell="A1502" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1531" sqref="F1531"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -55719,11 +55806,11 @@
         <v>280</v>
       </c>
       <c r="I1523" s="4">
-        <f>YEAR(A1523)</f>
+        <f t="shared" ref="I1523:I1531" si="572">YEAR(A1523)</f>
         <v>2025</v>
       </c>
       <c r="J1523" s="4">
-        <f>MONTH(A1523)</f>
+        <f t="shared" ref="J1523:J1531" si="573">MONTH(A1523)</f>
         <v>5</v>
       </c>
     </row>
@@ -55753,433 +55840,2205 @@
         <v>280</v>
       </c>
       <c r="I1524" s="4">
-        <f>YEAR(A1524)</f>
+        <f t="shared" si="572"/>
         <v>2025</v>
       </c>
       <c r="J1524" s="4">
-        <f>MONTH(A1524)</f>
+        <f t="shared" si="573"/>
         <v>5</v>
       </c>
     </row>
     <row r="1525" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1525" s="3"/>
-      <c r="B1525" s="3"/>
-      <c r="C1525" s="3"/>
-      <c r="D1525" s="3"/>
-      <c r="E1525" s="3"/>
-      <c r="F1525" s="3"/>
-      <c r="G1525" s="3"/>
-      <c r="H1525" s="3"/>
-      <c r="I1525" s="4"/>
-      <c r="J1525" s="4"/>
+      <c r="A1525" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B1525" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C1525" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1525" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1525" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1525" s="3" t="s">
+        <v>1384</v>
+      </c>
+      <c r="G1525" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1525" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1525" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1525" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1526" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1526" s="3"/>
-      <c r="B1526" s="3"/>
-      <c r="C1526" s="3"/>
-      <c r="D1526" s="3"/>
-      <c r="E1526" s="3"/>
-      <c r="F1526" s="3"/>
-      <c r="G1526" s="3"/>
-      <c r="H1526" s="3"/>
-      <c r="I1526" s="4"/>
-      <c r="J1526" s="4"/>
+      <c r="A1526" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B1526" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1526" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1526" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1526" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1526" s="3" t="s">
+        <v>1386</v>
+      </c>
+      <c r="G1526" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1526" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1526" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1526" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1527" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1527" s="3"/>
-      <c r="B1527" s="3"/>
-      <c r="C1527" s="3"/>
-      <c r="D1527" s="3"/>
-      <c r="E1527" s="3"/>
-      <c r="F1527" s="3"/>
-      <c r="G1527" s="3"/>
-      <c r="H1527" s="3"/>
-      <c r="I1527" s="4"/>
-      <c r="J1527" s="4"/>
+      <c r="A1527" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B1527" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="C1527" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1527" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1527" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1527" s="3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="G1527" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1527" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1527" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1527" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1528" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1528" s="3"/>
-      <c r="B1528" s="3"/>
-      <c r="C1528" s="3"/>
-      <c r="D1528" s="3"/>
-      <c r="E1528" s="3"/>
-      <c r="F1528" s="3"/>
-      <c r="G1528" s="3"/>
-      <c r="H1528" s="3"/>
-      <c r="I1528" s="4"/>
-      <c r="J1528" s="4"/>
+      <c r="A1528" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B1528" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1528" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1528" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1528" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1528" s="3" t="s">
+        <v>1388</v>
+      </c>
+      <c r="G1528" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1528" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1528" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1528" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1529" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1529" s="3"/>
-      <c r="B1529" s="3"/>
-      <c r="C1529" s="3"/>
-      <c r="D1529" s="3"/>
-      <c r="E1529" s="3"/>
-      <c r="F1529" s="3"/>
-      <c r="G1529" s="3"/>
-      <c r="H1529" s="3"/>
-      <c r="I1529" s="4"/>
-      <c r="J1529" s="4"/>
+      <c r="A1529" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B1529" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1529" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1529" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1529" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1529" s="3" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G1529" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1529" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1529" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1529" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1530" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1530" s="3"/>
-      <c r="B1530" s="3"/>
-      <c r="C1530" s="3"/>
-      <c r="D1530" s="3"/>
-      <c r="E1530" s="3"/>
-      <c r="F1530" s="3"/>
-      <c r="G1530" s="3"/>
-      <c r="H1530" s="3"/>
-      <c r="I1530" s="4"/>
-      <c r="J1530" s="4"/>
+      <c r="A1530" s="3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="B1530" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1530" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1530" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1530" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1530" s="3" t="s">
+        <v>1390</v>
+      </c>
+      <c r="G1530" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1530" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1530" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1530" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1531" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1531" s="3"/>
-      <c r="B1531" s="3"/>
-      <c r="C1531" s="3"/>
-      <c r="D1531" s="3"/>
-      <c r="E1531" s="3"/>
-      <c r="F1531" s="3"/>
-      <c r="G1531" s="3"/>
-      <c r="H1531" s="3"/>
-      <c r="I1531" s="4"/>
-      <c r="J1531" s="4"/>
+      <c r="A1531" s="3" t="s">
+        <v>1391</v>
+      </c>
+      <c r="B1531" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1531" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1531" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1531" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1531" s="9" t="s">
+        <v>1392</v>
+      </c>
+      <c r="G1531" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1531" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1531" s="4">
+        <f t="shared" si="572"/>
+        <v>2025</v>
+      </c>
+      <c r="J1531" s="4">
+        <f t="shared" si="573"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1532" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1532" s="3"/>
-      <c r="B1532" s="3"/>
-      <c r="C1532" s="3"/>
-      <c r="D1532" s="3"/>
-      <c r="E1532" s="3"/>
+      <c r="A1532" s="3" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B1532" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1532" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1532" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1532" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1532" s="3"/>
-      <c r="G1532" s="3"/>
-      <c r="H1532" s="3"/>
-      <c r="I1532" s="4"/>
-      <c r="J1532" s="4"/>
+      <c r="G1532" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1532" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1532" s="4">
+        <f t="shared" ref="I1532:I1533" si="574">YEAR(A1532)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1532" s="4">
+        <f t="shared" ref="J1532:J1533" si="575">MONTH(A1532)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1533" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1533" s="3"/>
-      <c r="B1533" s="3"/>
-      <c r="C1533" s="3"/>
-      <c r="D1533" s="3"/>
-      <c r="E1533" s="3"/>
+      <c r="A1533" s="3" t="s">
+        <v>1393</v>
+      </c>
+      <c r="B1533" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1533" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1533" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1533" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1533" s="3"/>
-      <c r="G1533" s="3"/>
-      <c r="H1533" s="3"/>
-      <c r="I1533" s="4"/>
-      <c r="J1533" s="4"/>
+      <c r="G1533" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1533" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1533" s="4">
+        <f t="shared" si="574"/>
+        <v>2025</v>
+      </c>
+      <c r="J1533" s="4">
+        <f t="shared" si="575"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1534" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1534" s="3"/>
-      <c r="B1534" s="3"/>
-      <c r="C1534" s="3"/>
-      <c r="D1534" s="3"/>
-      <c r="E1534" s="3"/>
+      <c r="A1534" s="3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B1534" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1534" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1534" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1534" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1534" s="3"/>
-      <c r="G1534" s="3"/>
-      <c r="H1534" s="3"/>
-      <c r="I1534" s="4"/>
-      <c r="J1534" s="4"/>
+      <c r="G1534" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1534" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1534" s="4">
+        <f t="shared" ref="I1534:I1535" si="576">YEAR(A1534)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1534" s="4">
+        <f t="shared" ref="J1534:J1535" si="577">MONTH(A1534)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1535" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1535" s="3"/>
-      <c r="B1535" s="3"/>
-      <c r="C1535" s="3"/>
-      <c r="D1535" s="3"/>
-      <c r="E1535" s="3"/>
+      <c r="A1535" s="3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="B1535" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1535" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1535" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1535" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1535" s="3"/>
-      <c r="G1535" s="3"/>
-      <c r="H1535" s="3"/>
-      <c r="I1535" s="4"/>
-      <c r="J1535" s="4"/>
+      <c r="G1535" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1535" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1535" s="4">
+        <f t="shared" si="576"/>
+        <v>2025</v>
+      </c>
+      <c r="J1535" s="4">
+        <f t="shared" si="577"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1536" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1536" s="3"/>
-      <c r="B1536" s="3"/>
-      <c r="C1536" s="3"/>
-      <c r="D1536" s="3"/>
-      <c r="E1536" s="3"/>
-      <c r="F1536" s="3"/>
-      <c r="G1536" s="3"/>
-      <c r="H1536" s="3"/>
-      <c r="I1536" s="4"/>
-      <c r="J1536" s="4"/>
+      <c r="A1536" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B1536" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1536" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1536" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1536" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1536" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1536" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1536" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1536" s="4">
+        <f t="shared" ref="I1536:I1546" si="578">YEAR(A1536)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1536" s="4">
+        <f t="shared" ref="J1536:J1546" si="579">MONTH(A1536)</f>
+        <v>5</v>
+      </c>
     </row>
     <row r="1537" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1537" s="3"/>
-      <c r="B1537" s="3"/>
-      <c r="C1537" s="3"/>
-      <c r="D1537" s="3"/>
-      <c r="E1537" s="3"/>
-      <c r="F1537" s="3"/>
-      <c r="G1537" s="3"/>
-      <c r="H1537" s="3"/>
-      <c r="I1537" s="4"/>
-      <c r="J1537" s="4"/>
+      <c r="A1537" s="3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="B1537" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1537" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1537" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1537" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1537" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1537" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1537" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1537" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1537" s="4">
+        <f t="shared" si="579"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="1538" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1538" s="3"/>
-      <c r="B1538" s="3"/>
-      <c r="C1538" s="3"/>
-      <c r="D1538" s="3"/>
-      <c r="E1538" s="3"/>
-      <c r="F1538" s="3"/>
-      <c r="G1538" s="3"/>
-      <c r="H1538" s="3"/>
-      <c r="I1538" s="4"/>
-      <c r="J1538" s="4"/>
+      <c r="A1538" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B1538" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1538" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1538" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1538" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1538" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1538" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1538" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1538" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1538" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1539" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1539" s="3"/>
-      <c r="B1539" s="3"/>
-      <c r="C1539" s="3"/>
-      <c r="D1539" s="3"/>
-      <c r="E1539" s="3"/>
-      <c r="F1539" s="3"/>
-      <c r="G1539" s="3"/>
-      <c r="H1539" s="3"/>
-      <c r="I1539" s="4"/>
-      <c r="J1539" s="4"/>
+      <c r="A1539" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B1539" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1539" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="D1539" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1539" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1539" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1539" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1539" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1539" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1539" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1540" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1540" s="3"/>
-      <c r="B1540" s="3"/>
-      <c r="C1540" s="3"/>
-      <c r="D1540" s="3"/>
-      <c r="E1540" s="3"/>
-      <c r="F1540" s="3"/>
-      <c r="G1540" s="3"/>
-      <c r="H1540" s="3"/>
-      <c r="I1540" s="4"/>
-      <c r="J1540" s="4"/>
+      <c r="A1540" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B1540" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C1540" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1540" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1540" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1540" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1540" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1540" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1540" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1540" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1541" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1541" s="3"/>
-      <c r="B1541" s="3"/>
-      <c r="C1541" s="3"/>
-      <c r="D1541" s="3"/>
-      <c r="E1541" s="3"/>
-      <c r="F1541" s="3"/>
-      <c r="G1541" s="3"/>
-      <c r="H1541" s="3"/>
-      <c r="I1541" s="4"/>
-      <c r="J1541" s="4"/>
+      <c r="A1541" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B1541" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1541" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1541" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1541" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1541" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1541" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1541" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1541" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1541" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1542" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1542" s="3"/>
-      <c r="B1542" s="3"/>
-      <c r="C1542" s="3"/>
-      <c r="D1542" s="3"/>
-      <c r="E1542" s="3"/>
-      <c r="F1542" s="3"/>
-      <c r="G1542" s="3"/>
-      <c r="H1542" s="3"/>
-      <c r="I1542" s="4"/>
-      <c r="J1542" s="4"/>
+      <c r="A1542" s="3" t="s">
+        <v>1396</v>
+      </c>
+      <c r="B1542" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="C1542" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1542" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1542" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1542" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1542" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1542" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1542" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1542" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1543" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1543" s="3"/>
-      <c r="B1543" s="3"/>
-      <c r="C1543" s="3"/>
-      <c r="D1543" s="3"/>
-      <c r="E1543" s="3"/>
-      <c r="F1543" s="3"/>
-      <c r="G1543" s="3"/>
-      <c r="H1543" s="3"/>
-      <c r="I1543" s="4"/>
-      <c r="J1543" s="4"/>
+      <c r="A1543" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B1543" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1543" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1543" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1543" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1543" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1543" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1543" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1543" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1543" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1544" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1544" s="3"/>
-      <c r="B1544" s="3"/>
-      <c r="C1544" s="3"/>
-      <c r="D1544" s="3"/>
-      <c r="E1544" s="3"/>
-      <c r="F1544" s="3"/>
-      <c r="G1544" s="3"/>
-      <c r="H1544" s="3"/>
-      <c r="I1544" s="4"/>
-      <c r="J1544" s="4"/>
+      <c r="A1544" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B1544" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1544" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1544" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1544" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1544" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1544" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1544" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1544" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1544" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1545" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1545" s="3"/>
-      <c r="B1545" s="3"/>
-      <c r="C1545" s="3"/>
-      <c r="D1545" s="3"/>
-      <c r="E1545" s="3"/>
-      <c r="F1545" s="3"/>
-      <c r="G1545" s="3"/>
-      <c r="H1545" s="3"/>
-      <c r="I1545" s="4"/>
-      <c r="J1545" s="4"/>
+      <c r="A1545" s="3" t="s">
+        <v>1397</v>
+      </c>
+      <c r="B1545" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1545" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1545" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1545" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1545" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1545" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1545" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1545" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1545" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1546" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1546" s="3"/>
-      <c r="B1546" s="3"/>
-      <c r="C1546" s="3"/>
-      <c r="D1546" s="3"/>
-      <c r="E1546" s="3"/>
-      <c r="F1546" s="3"/>
-      <c r="G1546" s="3"/>
-      <c r="H1546" s="3"/>
-      <c r="I1546" s="4"/>
-      <c r="J1546" s="4"/>
+      <c r="A1546" s="3" t="s">
+        <v>1398</v>
+      </c>
+      <c r="B1546" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1546" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1546" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1546" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1546" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1546" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1546" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1546" s="4">
+        <f t="shared" si="578"/>
+        <v>2025</v>
+      </c>
+      <c r="J1546" s="4">
+        <f t="shared" si="579"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1547" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1547" s="3"/>
-      <c r="B1547" s="3"/>
-      <c r="C1547" s="3"/>
-      <c r="D1547" s="3"/>
-      <c r="E1547" s="3"/>
+      <c r="A1547" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B1547" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1547" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1547" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1547" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1547" s="3"/>
-      <c r="G1547" s="3"/>
-      <c r="H1547" s="3"/>
-      <c r="I1547" s="4"/>
-      <c r="J1547" s="4"/>
+      <c r="G1547" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1547" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1547" s="4">
+        <f t="shared" ref="I1547:I1549" si="580">YEAR(A1547)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1547" s="4">
+        <f t="shared" ref="J1547:J1549" si="581">MONTH(A1547)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1548" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1548" s="3"/>
-      <c r="B1548" s="3"/>
-      <c r="C1548" s="3"/>
-      <c r="D1548" s="3"/>
-      <c r="E1548" s="3"/>
+      <c r="A1548" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B1548" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1548" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1548" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1548" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1548" s="3"/>
-      <c r="G1548" s="3"/>
-      <c r="H1548" s="3"/>
-      <c r="I1548" s="4"/>
-      <c r="J1548" s="4"/>
+      <c r="G1548" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1548" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1548" s="4">
+        <f t="shared" si="580"/>
+        <v>2025</v>
+      </c>
+      <c r="J1548" s="4">
+        <f t="shared" si="581"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1549" s="3"/>
-      <c r="B1549" s="3"/>
-      <c r="C1549" s="3"/>
-      <c r="D1549" s="3"/>
-      <c r="E1549" s="3"/>
+      <c r="A1549" s="3" t="s">
+        <v>1400</v>
+      </c>
+      <c r="B1549" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1549" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1549" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1549" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1549" s="3"/>
-      <c r="G1549" s="3"/>
-      <c r="H1549" s="3"/>
-      <c r="I1549" s="4"/>
-      <c r="J1549" s="4"/>
+      <c r="G1549" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1549" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1549" s="4">
+        <f t="shared" si="580"/>
+        <v>2025</v>
+      </c>
+      <c r="J1549" s="4">
+        <f t="shared" si="581"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1550" s="3"/>
-      <c r="B1550" s="3"/>
-      <c r="C1550" s="3"/>
-      <c r="D1550" s="3"/>
-      <c r="E1550" s="3"/>
+      <c r="A1550" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B1550" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="C1550" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1550" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1550" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1550" s="3"/>
-      <c r="G1550" s="3"/>
-      <c r="H1550" s="3"/>
-      <c r="I1550" s="4"/>
-      <c r="J1550" s="4"/>
+      <c r="G1550" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1550" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1550" s="4">
+        <f t="shared" ref="I1550:I1554" si="582">YEAR(A1550)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1550" s="4">
+        <f t="shared" ref="J1550:J1554" si="583">MONTH(A1550)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1551" s="3"/>
-      <c r="B1551" s="3"/>
-      <c r="C1551" s="3"/>
-      <c r="D1551" s="3"/>
-      <c r="E1551" s="3"/>
+      <c r="A1551" s="3" t="s">
+        <v>1401</v>
+      </c>
+      <c r="B1551" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1551" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1551" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1551" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1551" s="3"/>
-      <c r="G1551" s="3"/>
-      <c r="H1551" s="3"/>
-      <c r="I1551" s="4"/>
-      <c r="J1551" s="4"/>
+      <c r="G1551" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1551" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1551" s="4">
+        <f t="shared" si="582"/>
+        <v>2025</v>
+      </c>
+      <c r="J1551" s="4">
+        <f t="shared" si="583"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1552" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1552" s="3"/>
-      <c r="B1552" s="3"/>
-      <c r="C1552" s="3"/>
-      <c r="D1552" s="3"/>
-      <c r="E1552" s="3"/>
+      <c r="A1552" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B1552" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1552" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1552" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1552" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1552" s="3"/>
-      <c r="G1552" s="3"/>
-      <c r="H1552" s="3"/>
-      <c r="I1552" s="4"/>
-      <c r="J1552" s="4"/>
+      <c r="G1552" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1552" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1552" s="4">
+        <f t="shared" si="582"/>
+        <v>2025</v>
+      </c>
+      <c r="J1552" s="4">
+        <f t="shared" si="583"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1553" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1553" s="3"/>
-      <c r="B1553" s="3"/>
-      <c r="C1553" s="3"/>
-      <c r="D1553" s="3"/>
-      <c r="E1553" s="3"/>
+      <c r="A1553" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B1553" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1553" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1553" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1553" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1553" s="3"/>
-      <c r="G1553" s="3"/>
-      <c r="H1553" s="3"/>
-      <c r="I1553" s="4"/>
-      <c r="J1553" s="4"/>
+      <c r="G1553" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1553" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1553" s="4">
+        <f t="shared" si="582"/>
+        <v>2025</v>
+      </c>
+      <c r="J1553" s="4">
+        <f t="shared" si="583"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1554" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1554" s="3"/>
-      <c r="B1554" s="3"/>
-      <c r="C1554" s="3"/>
-      <c r="D1554" s="3"/>
-      <c r="E1554" s="3"/>
+      <c r="A1554" s="3" t="s">
+        <v>1402</v>
+      </c>
+      <c r="B1554" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1554" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1554" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1554" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1554" s="3"/>
-      <c r="G1554" s="3"/>
-      <c r="H1554" s="3"/>
-      <c r="I1554" s="4"/>
-      <c r="J1554" s="4"/>
+      <c r="G1554" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1554" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1554" s="4">
+        <f t="shared" si="582"/>
+        <v>2025</v>
+      </c>
+      <c r="J1554" s="4">
+        <f t="shared" si="583"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1555" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1555" s="3"/>
-      <c r="B1555" s="3"/>
-      <c r="C1555" s="3"/>
-      <c r="D1555" s="3"/>
-      <c r="E1555" s="3"/>
+      <c r="A1555" s="3" t="s">
+        <v>1403</v>
+      </c>
+      <c r="B1555" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1555" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1555" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1555" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1555" s="3"/>
-      <c r="G1555" s="3"/>
-      <c r="H1555" s="3"/>
-      <c r="I1555" s="4"/>
-      <c r="J1555" s="4"/>
+      <c r="G1555" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1555" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1555" s="4">
+        <f t="shared" ref="I1555" si="584">YEAR(A1555)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1555" s="4">
+        <f t="shared" ref="J1555" si="585">MONTH(A1555)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1556" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1556" s="3"/>
-      <c r="B1556" s="3"/>
-      <c r="C1556" s="3"/>
-      <c r="D1556" s="3"/>
-      <c r="E1556" s="3"/>
-      <c r="F1556" s="3"/>
-      <c r="G1556" s="3"/>
-      <c r="H1556" s="3"/>
-      <c r="I1556" s="4"/>
-      <c r="J1556" s="4"/>
+      <c r="A1556" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B1556" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1556" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1556" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1556" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1556" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1556" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1556" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1556" s="4">
+        <f>YEAR(A1556)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1556" s="4">
+        <f>MONTH(A1556)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1557" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1557" s="3"/>
-      <c r="B1557" s="3"/>
-      <c r="C1557" s="3"/>
-      <c r="D1557" s="3"/>
-      <c r="E1557" s="3"/>
-      <c r="F1557" s="3"/>
-      <c r="G1557" s="3"/>
-      <c r="H1557" s="3"/>
-      <c r="I1557" s="4"/>
-      <c r="J1557" s="4"/>
+      <c r="A1557" s="3" t="s">
+        <v>1404</v>
+      </c>
+      <c r="B1557" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1557" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1557" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1557" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1557" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1557" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1557" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1557" s="4">
+        <f>YEAR(A1557)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1557" s="4">
+        <f>MONTH(A1557)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1558" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1558" s="3"/>
-      <c r="B1558" s="3"/>
-      <c r="C1558" s="3"/>
-      <c r="D1558" s="3"/>
-      <c r="E1558" s="3"/>
-      <c r="F1558" s="3"/>
-      <c r="G1558" s="3"/>
-      <c r="H1558" s="3"/>
-      <c r="I1558" s="4"/>
-      <c r="J1558" s="4"/>
+      <c r="A1558" s="3" t="s">
+        <v>1405</v>
+      </c>
+      <c r="B1558" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1558" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1558" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1558" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1558" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1558" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1558" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1558" s="4">
+        <f>YEAR(A1558)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1558" s="4">
+        <f>MONTH(A1558)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1559" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1559" s="3"/>
-      <c r="B1559" s="3"/>
-      <c r="C1559" s="3"/>
-      <c r="D1559" s="3"/>
-      <c r="E1559" s="3"/>
+      <c r="A1559" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1559" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1559" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1559" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1559" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1559" s="3"/>
-      <c r="G1559" s="3"/>
-      <c r="H1559" s="3"/>
-      <c r="I1559" s="4"/>
-      <c r="J1559" s="4"/>
+      <c r="G1559" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1559" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1559" s="4">
+        <f t="shared" ref="I1559:I1560" si="586">YEAR(A1559)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1559" s="4">
+        <f t="shared" ref="J1559:J1560" si="587">MONTH(A1559)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1560" s="3" t="s">
+        <v>1406</v>
+      </c>
+      <c r="B1560" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1560" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1560" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1560" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1560" s="3"/>
+      <c r="G1560" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1560" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1560" s="4">
+        <f t="shared" si="586"/>
+        <v>2025</v>
+      </c>
+      <c r="J1560" s="4">
+        <f t="shared" si="587"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1561" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1561" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1561" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="D1561" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1561" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1561" s="3"/>
+      <c r="G1561" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1561" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1561" s="4">
+        <f t="shared" ref="I1561:I1562" si="588">YEAR(A1561)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1561" s="4">
+        <f t="shared" ref="J1561:J1562" si="589">MONTH(A1561)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1562" s="3" t="s">
+        <v>1407</v>
+      </c>
+      <c r="B1562" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1562" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1562" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1562" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F1562" s="3"/>
+      <c r="G1562" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1562" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1562" s="4">
+        <f t="shared" si="588"/>
+        <v>2025</v>
+      </c>
+      <c r="J1562" s="4">
+        <f t="shared" si="589"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1563" s="3" t="s">
+        <v>1408</v>
+      </c>
+      <c r="B1563" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="C1563" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1563" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1563" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1563" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1563" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1563" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1563" s="4">
+        <f t="shared" ref="I1563:I1569" si="590">YEAR(A1563)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1563" s="4">
+        <f t="shared" ref="J1563:J1569" si="591">MONTH(A1563)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1564" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B1564" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1564" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1564" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1564" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1564" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1564" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1564" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1564" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1564" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1565" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B1565" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1565" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1565" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1565" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1565" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1565" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1565" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1565" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1565" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1566" s="3" t="s">
+        <v>1409</v>
+      </c>
+      <c r="B1566" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1566" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1566" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1566" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1566" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1566" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1566" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1566" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1566" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1567" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1567" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1567" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="D1567" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1567" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1567" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1567" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1567" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1567" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1567" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1568" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1568" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1568" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1568" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1568" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1568" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1568" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1568" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1568" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1568" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1569" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1569" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1569" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1569" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1569" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1569" s="3" t="s">
+        <v>1399</v>
+      </c>
+      <c r="G1569" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1569" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1569" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1569" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1570" s="3"/>
+      <c r="B1570" s="3"/>
+      <c r="C1570" s="3"/>
+      <c r="D1570" s="3"/>
+      <c r="E1570" s="3"/>
+      <c r="F1570" s="3"/>
+      <c r="G1570" s="3"/>
+      <c r="H1570" s="3"/>
+      <c r="I1570" s="4"/>
+      <c r="J1570" s="4"/>
+    </row>
+    <row r="1571" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1571" s="3"/>
+      <c r="B1571" s="3"/>
+      <c r="C1571" s="3"/>
+      <c r="D1571" s="3"/>
+      <c r="E1571" s="3"/>
+      <c r="F1571" s="3"/>
+      <c r="G1571" s="3"/>
+      <c r="H1571" s="3"/>
+      <c r="I1571" s="4"/>
+      <c r="J1571" s="4"/>
+    </row>
+    <row r="1572" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1572" s="3"/>
+      <c r="B1572" s="3"/>
+      <c r="C1572" s="3"/>
+      <c r="D1572" s="3"/>
+      <c r="E1572" s="3"/>
+      <c r="F1572" s="3"/>
+      <c r="G1572" s="3"/>
+      <c r="H1572" s="3"/>
+      <c r="I1572" s="4"/>
+      <c r="J1572" s="4"/>
+    </row>
+    <row r="1573" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1573" s="3"/>
+      <c r="B1573" s="3"/>
+      <c r="C1573" s="3"/>
+      <c r="D1573" s="3"/>
+      <c r="E1573" s="3"/>
+      <c r="F1573" s="3"/>
+      <c r="G1573" s="3"/>
+      <c r="H1573" s="3"/>
+      <c r="I1573" s="4"/>
+      <c r="J1573" s="4"/>
+    </row>
+    <row r="1574" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1574" s="3"/>
+      <c r="B1574" s="3"/>
+      <c r="C1574" s="3"/>
+      <c r="D1574" s="3"/>
+      <c r="E1574" s="3"/>
+      <c r="F1574" s="3"/>
+      <c r="G1574" s="3"/>
+      <c r="H1574" s="3"/>
+      <c r="I1574" s="4"/>
+      <c r="J1574" s="4"/>
+    </row>
+    <row r="1575" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1575" s="3"/>
+      <c r="B1575" s="3"/>
+      <c r="C1575" s="3"/>
+      <c r="D1575" s="3"/>
+      <c r="E1575" s="3"/>
+      <c r="F1575" s="3"/>
+      <c r="G1575" s="3"/>
+      <c r="H1575" s="3"/>
+      <c r="I1575" s="4"/>
+      <c r="J1575" s="4"/>
+    </row>
+    <row r="1576" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1576" s="3"/>
+      <c r="B1576" s="3"/>
+      <c r="C1576" s="3"/>
+      <c r="D1576" s="3"/>
+      <c r="E1576" s="3"/>
+      <c r="F1576" s="3"/>
+      <c r="G1576" s="3"/>
+      <c r="H1576" s="3"/>
+      <c r="I1576" s="4"/>
+      <c r="J1576" s="4"/>
+    </row>
+    <row r="1577" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1577" s="3"/>
+      <c r="B1577" s="3"/>
+      <c r="C1577" s="3"/>
+      <c r="D1577" s="3"/>
+      <c r="E1577" s="3"/>
+      <c r="F1577" s="3"/>
+      <c r="G1577" s="3"/>
+      <c r="H1577" s="3"/>
+      <c r="I1577" s="4"/>
+      <c r="J1577" s="4"/>
+    </row>
+    <row r="1578" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1578" s="3"/>
+      <c r="B1578" s="3"/>
+      <c r="C1578" s="3"/>
+      <c r="D1578" s="3"/>
+      <c r="E1578" s="3"/>
+      <c r="F1578" s="3"/>
+      <c r="G1578" s="3"/>
+      <c r="H1578" s="3"/>
+      <c r="I1578" s="4"/>
+      <c r="J1578" s="4"/>
+    </row>
+    <row r="1579" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1579" s="3"/>
+      <c r="B1579" s="3"/>
+      <c r="C1579" s="3"/>
+      <c r="D1579" s="3"/>
+      <c r="E1579" s="3"/>
+      <c r="F1579" s="3"/>
+      <c r="G1579" s="3"/>
+      <c r="H1579" s="3"/>
+      <c r="I1579" s="4"/>
+      <c r="J1579" s="4"/>
+    </row>
+    <row r="1580" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1580" s="3"/>
+      <c r="B1580" s="3"/>
+      <c r="C1580" s="3"/>
+      <c r="D1580" s="3"/>
+      <c r="E1580" s="3"/>
+      <c r="F1580" s="3"/>
+      <c r="G1580" s="3"/>
+      <c r="H1580" s="3"/>
+      <c r="I1580" s="4"/>
+      <c r="J1580" s="4"/>
+    </row>
+    <row r="1581" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1581" s="3"/>
+      <c r="B1581" s="3"/>
+      <c r="C1581" s="3"/>
+      <c r="D1581" s="3"/>
+      <c r="E1581" s="3"/>
+      <c r="F1581" s="3"/>
+      <c r="G1581" s="3"/>
+      <c r="H1581" s="3"/>
+      <c r="I1581" s="4"/>
+      <c r="J1581" s="4"/>
+    </row>
+    <row r="1582" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1582" s="3"/>
+      <c r="B1582" s="3"/>
+      <c r="C1582" s="3"/>
+      <c r="D1582" s="3"/>
+      <c r="E1582" s="3"/>
+      <c r="F1582" s="3"/>
+      <c r="G1582" s="3"/>
+      <c r="H1582" s="3"/>
+      <c r="I1582" s="4"/>
+      <c r="J1582" s="4"/>
+    </row>
+    <row r="1583" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1583" s="3"/>
+      <c r="B1583" s="3"/>
+      <c r="C1583" s="3"/>
+      <c r="D1583" s="3"/>
+      <c r="E1583" s="3"/>
+      <c r="F1583" s="3"/>
+      <c r="G1583" s="3"/>
+      <c r="H1583" s="3"/>
+      <c r="I1583" s="4"/>
+      <c r="J1583" s="4"/>
+    </row>
+    <row r="1584" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1584" s="3"/>
+      <c r="B1584" s="3"/>
+      <c r="C1584" s="3"/>
+      <c r="D1584" s="3"/>
+      <c r="E1584" s="3"/>
+      <c r="F1584" s="3"/>
+      <c r="G1584" s="3"/>
+      <c r="H1584" s="3"/>
+      <c r="I1584" s="4"/>
+      <c r="J1584" s="4"/>
+    </row>
+    <row r="1585" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1585" s="3"/>
+      <c r="B1585" s="3"/>
+      <c r="C1585" s="3"/>
+      <c r="D1585" s="3"/>
+      <c r="E1585" s="3"/>
+      <c r="F1585" s="3"/>
+      <c r="G1585" s="3"/>
+      <c r="H1585" s="3"/>
+      <c r="I1585" s="4"/>
+      <c r="J1585" s="4"/>
+    </row>
+    <row r="1586" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1586" s="3"/>
+      <c r="B1586" s="3"/>
+      <c r="C1586" s="3"/>
+      <c r="D1586" s="3"/>
+      <c r="E1586" s="3"/>
+      <c r="F1586" s="3"/>
+      <c r="G1586" s="3"/>
+      <c r="H1586" s="3"/>
+      <c r="I1586" s="4"/>
+      <c r="J1586" s="4"/>
+    </row>
+    <row r="1587" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1587" s="3"/>
+      <c r="B1587" s="3"/>
+      <c r="C1587" s="3"/>
+      <c r="D1587" s="3"/>
+      <c r="E1587" s="3"/>
+      <c r="F1587" s="3"/>
+      <c r="G1587" s="3"/>
+      <c r="H1587" s="3"/>
+      <c r="I1587" s="4"/>
+      <c r="J1587" s="4"/>
+    </row>
+    <row r="1588" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1588" s="3"/>
+      <c r="B1588" s="3"/>
+      <c r="C1588" s="3"/>
+      <c r="D1588" s="3"/>
+      <c r="E1588" s="3"/>
+      <c r="F1588" s="3"/>
+      <c r="G1588" s="3"/>
+      <c r="H1588" s="3"/>
+      <c r="I1588" s="4"/>
+      <c r="J1588" s="4"/>
+    </row>
+    <row r="1589" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1589" s="3"/>
+      <c r="B1589" s="3"/>
+      <c r="C1589" s="3"/>
+      <c r="D1589" s="3"/>
+      <c r="E1589" s="3"/>
+      <c r="F1589" s="3"/>
+      <c r="G1589" s="3"/>
+      <c r="H1589" s="3"/>
+      <c r="I1589" s="4"/>
+      <c r="J1589" s="4"/>
+    </row>
+    <row r="1590" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1590" s="3"/>
+      <c r="B1590" s="3"/>
+      <c r="C1590" s="3"/>
+      <c r="D1590" s="3"/>
+      <c r="E1590" s="3"/>
+      <c r="F1590" s="3"/>
+      <c r="G1590" s="3"/>
+      <c r="H1590" s="3"/>
+      <c r="I1590" s="4"/>
+      <c r="J1590" s="4"/>
+    </row>
+    <row r="1591" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1591" s="3"/>
+      <c r="B1591" s="3"/>
+      <c r="C1591" s="3"/>
+      <c r="D1591" s="3"/>
+      <c r="E1591" s="3"/>
+      <c r="F1591" s="3"/>
+      <c r="G1591" s="3"/>
+      <c r="H1591" s="3"/>
+      <c r="I1591" s="4"/>
+      <c r="J1591" s="4"/>
+    </row>
+    <row r="1592" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1592" s="3"/>
+      <c r="B1592" s="3"/>
+      <c r="C1592" s="3"/>
+      <c r="D1592" s="3"/>
+      <c r="E1592" s="3"/>
+      <c r="F1592" s="3"/>
+      <c r="G1592" s="3"/>
+      <c r="H1592" s="3"/>
+      <c r="I1592" s="4"/>
+      <c r="J1592" s="4"/>
+    </row>
+    <row r="1593" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1593" s="3"/>
+      <c r="B1593" s="3"/>
+      <c r="C1593" s="3"/>
+      <c r="D1593" s="3"/>
+      <c r="E1593" s="3"/>
+      <c r="F1593" s="3"/>
+      <c r="G1593" s="3"/>
+      <c r="H1593" s="3"/>
+      <c r="I1593" s="4"/>
+      <c r="J1593" s="4"/>
+    </row>
+    <row r="1594" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1594" s="3"/>
+      <c r="B1594" s="3"/>
+      <c r="C1594" s="3"/>
+      <c r="D1594" s="3"/>
+      <c r="E1594" s="3"/>
+      <c r="F1594" s="3"/>
+      <c r="G1594" s="3"/>
+      <c r="H1594" s="3"/>
+      <c r="I1594" s="4"/>
+      <c r="J1594" s="4"/>
+    </row>
+    <row r="1595" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1595" s="3"/>
+      <c r="B1595" s="3"/>
+      <c r="C1595" s="3"/>
+      <c r="D1595" s="3"/>
+      <c r="E1595" s="3"/>
+      <c r="F1595" s="3"/>
+      <c r="G1595" s="3"/>
+      <c r="H1595" s="3"/>
+      <c r="I1595" s="4"/>
+      <c r="J1595" s="4"/>
+    </row>
+    <row r="1596" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1596" s="3"/>
+      <c r="B1596" s="3"/>
+      <c r="C1596" s="3"/>
+      <c r="D1596" s="3"/>
+      <c r="E1596" s="3"/>
+      <c r="F1596" s="3"/>
+      <c r="G1596" s="3"/>
+      <c r="H1596" s="3"/>
+      <c r="I1596" s="4"/>
+      <c r="J1596" s="4"/>
+    </row>
+    <row r="1597" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1597" s="3"/>
+      <c r="B1597" s="3"/>
+      <c r="C1597" s="3"/>
+      <c r="D1597" s="3"/>
+      <c r="E1597" s="3"/>
+      <c r="F1597" s="3"/>
+      <c r="G1597" s="3"/>
+      <c r="H1597" s="3"/>
+      <c r="I1597" s="4"/>
+      <c r="J1597" s="4"/>
+    </row>
+    <row r="1598" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1598" s="3"/>
+      <c r="B1598" s="3"/>
+      <c r="C1598" s="3"/>
+      <c r="D1598" s="3"/>
+      <c r="E1598" s="3"/>
+      <c r="F1598" s="3"/>
+      <c r="G1598" s="3"/>
+      <c r="H1598" s="3"/>
+      <c r="I1598" s="4"/>
+      <c r="J1598" s="4"/>
+    </row>
+    <row r="1599" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1599" s="3"/>
+      <c r="B1599" s="3"/>
+      <c r="C1599" s="3"/>
+      <c r="D1599" s="3"/>
+      <c r="E1599" s="3"/>
+      <c r="F1599" s="3"/>
+      <c r="G1599" s="3"/>
+      <c r="H1599" s="3"/>
+      <c r="I1599" s="4"/>
+      <c r="J1599" s="4"/>
+    </row>
+    <row r="1600" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1600" s="3"/>
+      <c r="B1600" s="3"/>
+      <c r="C1600" s="3"/>
+      <c r="D1600" s="3"/>
+      <c r="E1600" s="3"/>
+      <c r="F1600" s="3"/>
+      <c r="G1600" s="3"/>
+      <c r="H1600" s="3"/>
+      <c r="I1600" s="4"/>
+      <c r="J1600" s="4"/>
+    </row>
+    <row r="1601" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1601" s="3"/>
+      <c r="B1601" s="3"/>
+      <c r="C1601" s="3"/>
+      <c r="D1601" s="3"/>
+      <c r="E1601" s="3"/>
+      <c r="F1601" s="3"/>
+      <c r="G1601" s="3"/>
+      <c r="H1601" s="3"/>
+      <c r="I1601" s="4"/>
+      <c r="J1601" s="4"/>
+    </row>
+    <row r="1602" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1602" s="3"/>
+      <c r="B1602" s="3"/>
+      <c r="C1602" s="3"/>
+      <c r="D1602" s="3"/>
+      <c r="E1602" s="3"/>
+      <c r="F1602" s="3"/>
+      <c r="G1602" s="3"/>
+      <c r="H1602" s="3"/>
+      <c r="I1602" s="4"/>
+      <c r="J1602" s="4"/>
+    </row>
+    <row r="1603" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1603" s="3"/>
+      <c r="B1603" s="3"/>
+      <c r="C1603" s="3"/>
+      <c r="D1603" s="3"/>
+      <c r="E1603" s="3"/>
+      <c r="F1603" s="3"/>
+      <c r="G1603" s="3"/>
+      <c r="H1603" s="3"/>
+      <c r="I1603" s="4"/>
+      <c r="J1603" s="4"/>
+    </row>
+    <row r="1604" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1604" s="3"/>
+      <c r="B1604" s="3"/>
+      <c r="C1604" s="3"/>
+      <c r="D1604" s="3"/>
+      <c r="E1604" s="3"/>
+      <c r="F1604" s="3"/>
+      <c r="G1604" s="3"/>
+      <c r="H1604" s="3"/>
+      <c r="I1604" s="4"/>
+      <c r="J1604" s="4"/>
+    </row>
+    <row r="1605" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1605" s="3"/>
+      <c r="B1605" s="3"/>
+      <c r="C1605" s="3"/>
+      <c r="D1605" s="3"/>
+      <c r="E1605" s="3"/>
+      <c r="F1605" s="3"/>
+      <c r="G1605" s="3"/>
+      <c r="H1605" s="3"/>
+      <c r="I1605" s="4"/>
+      <c r="J1605" s="4"/>
+    </row>
+    <row r="1606" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1606" s="3"/>
+      <c r="B1606" s="3"/>
+      <c r="C1606" s="3"/>
+      <c r="D1606" s="3"/>
+      <c r="E1606" s="3"/>
+      <c r="F1606" s="3"/>
+      <c r="G1606" s="3"/>
+      <c r="H1606" s="3"/>
+      <c r="I1606" s="4"/>
+      <c r="J1606" s="4"/>
+    </row>
+    <row r="1607" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1607" s="3"/>
+      <c r="B1607" s="3"/>
+      <c r="C1607" s="3"/>
+      <c r="D1607" s="3"/>
+      <c r="E1607" s="3"/>
+      <c r="F1607" s="3"/>
+      <c r="G1607" s="3"/>
+      <c r="H1607" s="3"/>
+      <c r="I1607" s="4"/>
+      <c r="J1607" s="4"/>
+    </row>
+    <row r="1608" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1608" s="3"/>
+      <c r="B1608" s="3"/>
+      <c r="C1608" s="3"/>
+      <c r="D1608" s="3"/>
+      <c r="E1608" s="3"/>
+      <c r="F1608" s="3"/>
+      <c r="G1608" s="3"/>
+      <c r="H1608" s="3"/>
+      <c r="I1608" s="4"/>
+      <c r="J1608" s="4"/>
+    </row>
+    <row r="1609" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1609" s="3"/>
+      <c r="B1609" s="3"/>
+      <c r="C1609" s="3"/>
+      <c r="D1609" s="3"/>
+      <c r="E1609" s="3"/>
+      <c r="F1609" s="3"/>
+      <c r="G1609" s="3"/>
+      <c r="H1609" s="3"/>
+      <c r="I1609" s="4"/>
+      <c r="J1609" s="4"/>
+    </row>
+    <row r="1610" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1610" s="3"/>
+      <c r="B1610" s="3"/>
+      <c r="C1610" s="3"/>
+      <c r="D1610" s="3"/>
+      <c r="E1610" s="3"/>
+      <c r="F1610" s="3"/>
+      <c r="G1610" s="3"/>
+      <c r="H1610" s="3"/>
+      <c r="I1610" s="4"/>
+      <c r="J1610" s="4"/>
+    </row>
+    <row r="1611" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1611" s="3"/>
+      <c r="B1611" s="3"/>
+      <c r="C1611" s="3"/>
+      <c r="D1611" s="3"/>
+      <c r="E1611" s="3"/>
+      <c r="F1611" s="3"/>
+      <c r="G1611" s="3"/>
+      <c r="H1611" s="3"/>
+      <c r="I1611" s="4"/>
+      <c r="J1611" s="4"/>
+    </row>
+    <row r="1612" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1612" s="3"/>
+      <c r="B1612" s="3"/>
+      <c r="C1612" s="3"/>
+      <c r="D1612" s="3"/>
+      <c r="E1612" s="3"/>
+      <c r="F1612" s="3"/>
+      <c r="G1612" s="3"/>
+      <c r="H1612" s="3"/>
+      <c r="I1612" s="4"/>
+      <c r="J1612" s="4"/>
+    </row>
+    <row r="1613" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1613" s="3"/>
+      <c r="B1613" s="3"/>
+      <c r="C1613" s="3"/>
+      <c r="D1613" s="3"/>
+      <c r="E1613" s="3"/>
+      <c r="F1613" s="3"/>
+      <c r="G1613" s="3"/>
+      <c r="H1613" s="3"/>
+      <c r="I1613" s="4"/>
+      <c r="J1613" s="4"/>
+    </row>
+    <row r="1614" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1614" s="3"/>
+      <c r="B1614" s="3"/>
+      <c r="C1614" s="3"/>
+      <c r="D1614" s="3"/>
+      <c r="E1614" s="3"/>
+      <c r="F1614" s="3"/>
+      <c r="G1614" s="3"/>
+      <c r="H1614" s="3"/>
+      <c r="I1614" s="4"/>
+      <c r="J1614" s="4"/>
+    </row>
+    <row r="1615" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1615" s="3"/>
+      <c r="B1615" s="3"/>
+      <c r="C1615" s="3"/>
+      <c r="D1615" s="3"/>
+      <c r="E1615" s="3"/>
+      <c r="F1615" s="3"/>
+      <c r="G1615" s="3"/>
+      <c r="H1615" s="3"/>
+      <c r="I1615" s="4"/>
+      <c r="J1615" s="4"/>
+    </row>
+    <row r="1616" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1616" s="3"/>
+      <c r="B1616" s="3"/>
+      <c r="C1616" s="3"/>
+      <c r="D1616" s="3"/>
+      <c r="E1616" s="3"/>
+      <c r="F1616" s="3"/>
+      <c r="G1616" s="3"/>
+      <c r="H1616" s="3"/>
+      <c r="I1616" s="4"/>
+      <c r="J1616" s="4"/>
+    </row>
+    <row r="1617" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1617" s="3"/>
+      <c r="B1617" s="3"/>
+      <c r="C1617" s="3"/>
+      <c r="D1617" s="3"/>
+      <c r="E1617" s="3"/>
+      <c r="F1617" s="3"/>
+      <c r="G1617" s="3"/>
+      <c r="H1617" s="3"/>
+      <c r="I1617" s="4"/>
+      <c r="J1617" s="4"/>
+    </row>
+    <row r="1618" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1618" s="3"/>
+      <c r="B1618" s="3"/>
+      <c r="C1618" s="3"/>
+      <c r="D1618" s="3"/>
+      <c r="E1618" s="3"/>
+      <c r="F1618" s="3"/>
+      <c r="G1618" s="3"/>
+      <c r="H1618" s="3"/>
+      <c r="I1618" s="4"/>
+      <c r="J1618" s="4"/>
+    </row>
+    <row r="1619" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1619" s="3"/>
+      <c r="B1619" s="3"/>
+      <c r="C1619" s="3"/>
+      <c r="D1619" s="3"/>
+      <c r="E1619" s="3"/>
+      <c r="F1619" s="3"/>
+      <c r="G1619" s="3"/>
+      <c r="H1619" s="3"/>
+      <c r="I1619" s="4"/>
+      <c r="J1619" s="4"/>
+    </row>
+    <row r="1620" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1620" s="3"/>
+      <c r="B1620" s="3"/>
+      <c r="C1620" s="3"/>
+      <c r="D1620" s="3"/>
+      <c r="E1620" s="3"/>
+      <c r="F1620" s="3"/>
+      <c r="G1620" s="3"/>
+      <c r="H1620" s="3"/>
+      <c r="I1620" s="4"/>
+      <c r="J1620" s="4"/>
+    </row>
+    <row r="1621" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1621" s="3"/>
+      <c r="B1621" s="3"/>
+      <c r="C1621" s="3"/>
+      <c r="D1621" s="3"/>
+      <c r="E1621" s="3"/>
+      <c r="F1621" s="3"/>
+      <c r="G1621" s="3"/>
+      <c r="H1621" s="3"/>
+      <c r="I1621" s="4"/>
+      <c r="J1621" s="4"/>
+    </row>
+    <row r="1622" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1622" s="3"/>
+      <c r="B1622" s="3"/>
+      <c r="C1622" s="3"/>
+      <c r="D1622" s="3"/>
+      <c r="E1622" s="3"/>
+      <c r="F1622" s="3"/>
+      <c r="G1622" s="3"/>
+      <c r="H1622" s="3"/>
+      <c r="I1622" s="4"/>
+      <c r="J1622" s="4"/>
+    </row>
+    <row r="1623" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1623" s="3"/>
+      <c r="B1623" s="3"/>
+      <c r="C1623" s="3"/>
+      <c r="D1623" s="3"/>
+      <c r="E1623" s="3"/>
+      <c r="F1623" s="3"/>
+      <c r="G1623" s="3"/>
+      <c r="H1623" s="3"/>
+      <c r="I1623" s="4"/>
+      <c r="J1623" s="4"/>
+    </row>
+    <row r="1624" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1624" s="3"/>
+      <c r="B1624" s="3"/>
+      <c r="C1624" s="3"/>
+      <c r="D1624" s="3"/>
+      <c r="E1624" s="3"/>
+      <c r="F1624" s="3"/>
+      <c r="G1624" s="3"/>
+      <c r="H1624" s="3"/>
+      <c r="I1624" s="4"/>
+      <c r="J1624" s="4"/>
+    </row>
+    <row r="1625" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1625" s="3"/>
+      <c r="B1625" s="3"/>
+      <c r="C1625" s="3"/>
+      <c r="D1625" s="3"/>
+      <c r="E1625" s="3"/>
+      <c r="F1625" s="3"/>
+      <c r="G1625" s="3"/>
+      <c r="H1625" s="3"/>
+      <c r="I1625" s="4"/>
+      <c r="J1625" s="4"/>
+    </row>
+    <row r="1626" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1626" s="3"/>
+      <c r="B1626" s="3"/>
+      <c r="C1626" s="3"/>
+      <c r="D1626" s="3"/>
+      <c r="E1626" s="3"/>
+      <c r="F1626" s="3"/>
+      <c r="G1626" s="3"/>
+      <c r="H1626" s="3"/>
+      <c r="I1626" s="4"/>
+      <c r="J1626" s="4"/>
+    </row>
+    <row r="1627" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1627" s="3"/>
+      <c r="B1627" s="3"/>
+      <c r="C1627" s="3"/>
+      <c r="D1627" s="3"/>
+      <c r="E1627" s="3"/>
+      <c r="F1627" s="3"/>
+      <c r="G1627" s="3"/>
+      <c r="H1627" s="3"/>
+      <c r="I1627" s="4"/>
+      <c r="J1627" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-07-13.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12210" uniqueCount="1411">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12518" uniqueCount="1429">
   <si>
     <t>Year</t>
   </si>
@@ -4224,9 +4224,6 @@
     <t>2025-06-03</t>
   </si>
   <si>
-    <t>nwdatamarkadanalytics v1.0.0</t>
-  </si>
-  <si>
     <t>2025-06-05</t>
   </si>
   <si>
@@ -4258,6 +4255,63 @@
   </si>
   <si>
     <t>2025-06-23</t>
+  </si>
+  <si>
+    <t>2025-06-24</t>
+  </si>
+  <si>
+    <t>nwrefurbishedanalytics v1.0.0</t>
+  </si>
+  <si>
+    <t>2025-06-25</t>
+  </si>
+  <si>
+    <t>2025-06-26</t>
+  </si>
+  <si>
+    <t>2025-06-27</t>
+  </si>
+  <si>
+    <t>2025-06-28</t>
+  </si>
+  <si>
+    <t>2025-06-29</t>
+  </si>
+  <si>
+    <t>2025-07-01</t>
+  </si>
+  <si>
+    <t>2025-07-03</t>
+  </si>
+  <si>
+    <t>2025-07-04</t>
+  </si>
+  <si>
+    <t>2025-07-05</t>
+  </si>
+  <si>
+    <t>2025-07-06</t>
+  </si>
+  <si>
+    <t>2025-07-07</t>
+  </si>
+  <si>
+    <t>2025-07-08</t>
+  </si>
+  <si>
+    <t>2025-07-09</t>
+  </si>
+  <si>
+    <t>2025-07-10</t>
+  </si>
+  <si>
+    <t>2025-07-11</t>
+  </si>
+  <si>
+    <t>2025-07-12</t>
+  </si>
+  <si>
+    <t>2025-07-13</t>
   </si>
 </sst>
 </file>
@@ -4666,11 +4720,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1627"/>
+  <dimension ref="A1:J1667"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1502" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F1531" sqref="F1531"/>
+      <pane ySplit="1" topLeftCell="A1583" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D1612" sqref="D1612"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -56571,7 +56625,7 @@
         <v>127</v>
       </c>
       <c r="F1546" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1546" s="8" t="s">
         <v>279</v>
@@ -56590,7 +56644,7 @@
     </row>
     <row r="1547" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1547" s="3" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B1547" s="3" t="s">
         <v>248</v>
@@ -56622,7 +56676,7 @@
     </row>
     <row r="1548" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1548" s="3" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B1548" s="3" t="s">
         <v>149</v>
@@ -56654,7 +56708,7 @@
     </row>
     <row r="1549" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1549" s="3" t="s">
-        <v>1400</v>
+        <v>1399</v>
       </c>
       <c r="B1549" s="3" t="s">
         <v>174</v>
@@ -56686,7 +56740,7 @@
     </row>
     <row r="1550" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1550" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B1550" s="3" t="s">
         <v>249</v>
@@ -56718,7 +56772,7 @@
     </row>
     <row r="1551" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1551" s="3" t="s">
-        <v>1401</v>
+        <v>1400</v>
       </c>
       <c r="B1551" s="3" t="s">
         <v>149</v>
@@ -56750,7 +56804,7 @@
     </row>
     <row r="1552" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1552" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B1552" s="3" t="s">
         <v>132</v>
@@ -56782,7 +56836,7 @@
     </row>
     <row r="1553" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1553" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B1553" s="3" t="s">
         <v>161</v>
@@ -56814,7 +56868,7 @@
     </row>
     <row r="1554" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1554" s="3" t="s">
-        <v>1402</v>
+        <v>1401</v>
       </c>
       <c r="B1554" s="3" t="s">
         <v>124</v>
@@ -56846,7 +56900,7 @@
     </row>
     <row r="1555" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1555" s="3" t="s">
-        <v>1403</v>
+        <v>1402</v>
       </c>
       <c r="B1555" s="3" t="s">
         <v>327</v>
@@ -56878,7 +56932,7 @@
     </row>
     <row r="1556" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1556" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B1556" s="3" t="s">
         <v>355</v>
@@ -56893,7 +56947,7 @@
         <v>127</v>
       </c>
       <c r="F1556" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1556" s="8" t="s">
         <v>279</v>
@@ -56912,7 +56966,7 @@
     </row>
     <row r="1557" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1557" s="3" t="s">
-        <v>1404</v>
+        <v>1403</v>
       </c>
       <c r="B1557" s="3" t="s">
         <v>114</v>
@@ -56927,7 +56981,7 @@
         <v>127</v>
       </c>
       <c r="F1557" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1557" s="8" t="s">
         <v>279</v>
@@ -56946,7 +57000,7 @@
     </row>
     <row r="1558" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1558" s="3" t="s">
-        <v>1405</v>
+        <v>1404</v>
       </c>
       <c r="B1558" s="3" t="s">
         <v>134</v>
@@ -56961,7 +57015,7 @@
         <v>127</v>
       </c>
       <c r="F1558" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1558" s="8" t="s">
         <v>279</v>
@@ -56980,7 +57034,7 @@
     </row>
     <row r="1559" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1559" s="3" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="B1559" s="3" t="s">
         <v>248</v>
@@ -57012,7 +57066,7 @@
     </row>
     <row r="1560" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1560" s="3" t="s">
-        <v>1406</v>
+        <v>1405</v>
       </c>
       <c r="B1560" s="3" t="s">
         <v>171</v>
@@ -57044,7 +57098,7 @@
     </row>
     <row r="1561" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1561" s="3" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B1561" s="3" t="s">
         <v>248</v>
@@ -57076,7 +57130,7 @@
     </row>
     <row r="1562" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1562" s="3" t="s">
-        <v>1407</v>
+        <v>1406</v>
       </c>
       <c r="B1562" s="3" t="s">
         <v>118</v>
@@ -57108,7 +57162,7 @@
     </row>
     <row r="1563" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1563" s="3" t="s">
-        <v>1408</v>
+        <v>1407</v>
       </c>
       <c r="B1563" s="3" t="s">
         <v>395</v>
@@ -57123,7 +57177,7 @@
         <v>127</v>
       </c>
       <c r="F1563" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1563" s="8" t="s">
         <v>279</v>
@@ -57132,17 +57186,17 @@
         <v>280</v>
       </c>
       <c r="I1563" s="4">
-        <f t="shared" ref="I1563:I1569" si="590">YEAR(A1563)</f>
+        <f t="shared" ref="I1563:I1572" si="590">YEAR(A1563)</f>
         <v>2025</v>
       </c>
       <c r="J1563" s="4">
-        <f t="shared" ref="J1563:J1569" si="591">MONTH(A1563)</f>
+        <f t="shared" ref="J1563:J1572" si="591">MONTH(A1563)</f>
         <v>6</v>
       </c>
     </row>
     <row r="1564" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1564" s="3" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B1564" s="3" t="s">
         <v>327</v>
@@ -57157,7 +57211,7 @@
         <v>127</v>
       </c>
       <c r="F1564" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1564" s="8" t="s">
         <v>279</v>
@@ -57176,7 +57230,7 @@
     </row>
     <row r="1565" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1565" s="3" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B1565" s="3" t="s">
         <v>174</v>
@@ -57191,7 +57245,7 @@
         <v>127</v>
       </c>
       <c r="F1565" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1565" s="8" t="s">
         <v>279</v>
@@ -57210,7 +57264,7 @@
     </row>
     <row r="1566" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1566" s="3" t="s">
-        <v>1409</v>
+        <v>1408</v>
       </c>
       <c r="B1566" s="3" t="s">
         <v>271</v>
@@ -57225,7 +57279,7 @@
         <v>127</v>
       </c>
       <c r="F1566" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1566" s="8" t="s">
         <v>279</v>
@@ -57244,7 +57298,7 @@
     </row>
     <row r="1567" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1567" s="3" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B1567" s="3" t="s">
         <v>287</v>
@@ -57259,7 +57313,7 @@
         <v>127</v>
       </c>
       <c r="F1567" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1567" s="8" t="s">
         <v>279</v>
@@ -57278,7 +57332,7 @@
     </row>
     <row r="1568" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1568" s="3" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B1568" s="3" t="s">
         <v>191</v>
@@ -57293,7 +57347,7 @@
         <v>127</v>
       </c>
       <c r="F1568" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1568" s="8" t="s">
         <v>279</v>
@@ -57312,7 +57366,7 @@
     </row>
     <row r="1569" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1569" s="3" t="s">
-        <v>1410</v>
+        <v>1409</v>
       </c>
       <c r="B1569" s="3" t="s">
         <v>134</v>
@@ -57327,7 +57381,7 @@
         <v>127</v>
       </c>
       <c r="F1569" s="3" t="s">
-        <v>1399</v>
+        <v>1411</v>
       </c>
       <c r="G1569" s="8" t="s">
         <v>279</v>
@@ -57345,484 +57399,1340 @@
       </c>
     </row>
     <row r="1570" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1570" s="3"/>
-      <c r="B1570" s="3"/>
-      <c r="C1570" s="3"/>
-      <c r="D1570" s="3"/>
-      <c r="E1570" s="3"/>
+      <c r="A1570" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1570" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1570" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1570" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1570" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1570" s="3"/>
-      <c r="G1570" s="3"/>
-      <c r="H1570" s="3"/>
-      <c r="I1570" s="4"/>
-      <c r="J1570" s="4"/>
+      <c r="G1570" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1570" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1570" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1570" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1571" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1571" s="3"/>
-      <c r="B1571" s="3"/>
-      <c r="C1571" s="3"/>
-      <c r="D1571" s="3"/>
-      <c r="E1571" s="3"/>
+      <c r="A1571" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1571" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1571" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1571" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1571" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1571" s="3"/>
-      <c r="G1571" s="3"/>
-      <c r="H1571" s="3"/>
-      <c r="I1571" s="4"/>
-      <c r="J1571" s="4"/>
+      <c r="G1571" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1571" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1571" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1571" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1572" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1572" s="3"/>
-      <c r="B1572" s="3"/>
-      <c r="C1572" s="3"/>
-      <c r="D1572" s="3"/>
-      <c r="E1572" s="3"/>
+      <c r="A1572" s="3" t="s">
+        <v>1410</v>
+      </c>
+      <c r="B1572" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1572" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1572" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1572" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1572" s="3"/>
-      <c r="G1572" s="3"/>
-      <c r="H1572" s="3"/>
-      <c r="I1572" s="4"/>
-      <c r="J1572" s="4"/>
+      <c r="G1572" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1572" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1572" s="4">
+        <f t="shared" si="590"/>
+        <v>2025</v>
+      </c>
+      <c r="J1572" s="4">
+        <f t="shared" si="591"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1573" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1573" s="3"/>
-      <c r="B1573" s="3"/>
-      <c r="C1573" s="3"/>
-      <c r="D1573" s="3"/>
-      <c r="E1573" s="3"/>
-      <c r="F1573" s="3"/>
-      <c r="G1573" s="3"/>
-      <c r="H1573" s="3"/>
-      <c r="I1573" s="4"/>
-      <c r="J1573" s="4"/>
+      <c r="A1573" s="3" t="s">
+        <v>1412</v>
+      </c>
+      <c r="B1573" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C1573" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1573" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1573" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1573" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1573" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1573" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1573" s="4">
+        <f t="shared" ref="I1573:I1575" si="592">YEAR(A1573)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1573" s="4">
+        <f t="shared" ref="J1573:J1575" si="593">MONTH(A1573)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1574" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1574" s="3"/>
-      <c r="B1574" s="3"/>
-      <c r="C1574" s="3"/>
-      <c r="D1574" s="3"/>
-      <c r="E1574" s="3"/>
+      <c r="A1574" s="3" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B1574" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1574" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1574" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1574" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1574" s="3"/>
-      <c r="G1574" s="3"/>
-      <c r="H1574" s="3"/>
-      <c r="I1574" s="4"/>
-      <c r="J1574" s="4"/>
+      <c r="G1574" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1574" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1574" s="4">
+        <f t="shared" si="592"/>
+        <v>2025</v>
+      </c>
+      <c r="J1574" s="4">
+        <f t="shared" si="593"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1575" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1575" s="3"/>
-      <c r="B1575" s="3"/>
-      <c r="C1575" s="3"/>
-      <c r="D1575" s="3"/>
-      <c r="E1575" s="3"/>
+      <c r="A1575" s="3" t="s">
+        <v>1413</v>
+      </c>
+      <c r="B1575" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1575" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1575" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1575" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1575" s="3"/>
-      <c r="G1575" s="3"/>
-      <c r="H1575" s="3"/>
-      <c r="I1575" s="4"/>
-      <c r="J1575" s="4"/>
+      <c r="G1575" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1575" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1575" s="4">
+        <f t="shared" si="592"/>
+        <v>2025</v>
+      </c>
+      <c r="J1575" s="4">
+        <f t="shared" si="593"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1576" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1576" s="3"/>
-      <c r="B1576" s="3"/>
-      <c r="C1576" s="3"/>
-      <c r="D1576" s="3"/>
-      <c r="E1576" s="3"/>
+      <c r="A1576" s="3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B1576" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1576" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1576" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1576" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1576" s="3"/>
-      <c r="G1576" s="3"/>
-      <c r="H1576" s="3"/>
-      <c r="I1576" s="4"/>
-      <c r="J1576" s="4"/>
+      <c r="G1576" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1576" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1576" s="4">
+        <f t="shared" ref="I1576:I1581" si="594">YEAR(A1576)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1576" s="4">
+        <f t="shared" ref="J1576:J1581" si="595">MONTH(A1576)</f>
+        <v>6</v>
+      </c>
     </row>
     <row r="1577" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1577" s="3"/>
-      <c r="B1577" s="3"/>
-      <c r="C1577" s="3"/>
-      <c r="D1577" s="3"/>
-      <c r="E1577" s="3"/>
+      <c r="A1577" s="3" t="s">
+        <v>1414</v>
+      </c>
+      <c r="B1577" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="C1577" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1577" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1577" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1577" s="3"/>
-      <c r="G1577" s="3"/>
-      <c r="H1577" s="3"/>
-      <c r="I1577" s="4"/>
-      <c r="J1577" s="4"/>
+      <c r="G1577" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1577" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1577" s="4">
+        <f t="shared" si="594"/>
+        <v>2025</v>
+      </c>
+      <c r="J1577" s="4">
+        <f t="shared" si="595"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1578" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1578" s="3"/>
-      <c r="B1578" s="3"/>
-      <c r="C1578" s="3"/>
-      <c r="D1578" s="3"/>
-      <c r="E1578" s="3"/>
-      <c r="F1578" s="3"/>
-      <c r="G1578" s="3"/>
-      <c r="H1578" s="3"/>
-      <c r="I1578" s="4"/>
-      <c r="J1578" s="4"/>
+      <c r="A1578" s="3" t="s">
+        <v>1415</v>
+      </c>
+      <c r="B1578" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1578" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="D1578" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1578" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1578" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1578" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1578" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1578" s="4">
+        <f t="shared" si="594"/>
+        <v>2025</v>
+      </c>
+      <c r="J1578" s="4">
+        <f t="shared" si="595"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1579" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1579" s="3"/>
-      <c r="B1579" s="3"/>
-      <c r="C1579" s="3"/>
-      <c r="D1579" s="3"/>
-      <c r="E1579" s="3"/>
-      <c r="F1579" s="3"/>
-      <c r="G1579" s="3"/>
-      <c r="H1579" s="3"/>
-      <c r="I1579" s="4"/>
-      <c r="J1579" s="4"/>
+      <c r="A1579" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1579" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1579" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="D1579" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1579" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1579" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1579" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1579" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1579" s="4">
+        <f t="shared" si="594"/>
+        <v>2025</v>
+      </c>
+      <c r="J1579" s="4">
+        <f t="shared" si="595"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1580" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1580" s="3"/>
-      <c r="B1580" s="3"/>
-      <c r="C1580" s="3"/>
-      <c r="D1580" s="3"/>
-      <c r="E1580" s="3"/>
-      <c r="F1580" s="3"/>
-      <c r="G1580" s="3"/>
-      <c r="H1580" s="3"/>
-      <c r="I1580" s="4"/>
-      <c r="J1580" s="4"/>
+      <c r="A1580" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1580" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1580" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1580" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E1580" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1580" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1580" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1580" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1580" s="4">
+        <f t="shared" si="594"/>
+        <v>2025</v>
+      </c>
+      <c r="J1580" s="4">
+        <f t="shared" si="595"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1581" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1581" s="3"/>
-      <c r="B1581" s="3"/>
-      <c r="C1581" s="3"/>
-      <c r="D1581" s="3"/>
-      <c r="E1581" s="3"/>
-      <c r="F1581" s="3"/>
-      <c r="G1581" s="3"/>
-      <c r="H1581" s="3"/>
-      <c r="I1581" s="4"/>
-      <c r="J1581" s="4"/>
+      <c r="A1581" s="3" t="s">
+        <v>1416</v>
+      </c>
+      <c r="B1581" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1581" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1581" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E1581" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1581" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1581" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1581" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1581" s="4">
+        <f t="shared" si="594"/>
+        <v>2025</v>
+      </c>
+      <c r="J1581" s="4">
+        <f t="shared" si="595"/>
+        <v>6</v>
+      </c>
     </row>
     <row r="1582" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1582" s="3"/>
-      <c r="B1582" s="3"/>
-      <c r="C1582" s="3"/>
-      <c r="D1582" s="3"/>
-      <c r="E1582" s="3"/>
-      <c r="F1582" s="3"/>
-      <c r="G1582" s="3"/>
-      <c r="H1582" s="3"/>
-      <c r="I1582" s="4"/>
-      <c r="J1582" s="4"/>
+      <c r="A1582" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1582" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1582" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1582" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="E1582" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1582" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1582" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1582" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1582" s="4">
+        <f t="shared" ref="I1582:I1584" si="596">YEAR(A1582)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1582" s="4">
+        <f t="shared" ref="J1582:J1584" si="597">MONTH(A1582)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1583" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1583" s="3"/>
-      <c r="B1583" s="3"/>
-      <c r="C1583" s="3"/>
-      <c r="D1583" s="3"/>
-      <c r="E1583" s="3"/>
-      <c r="F1583" s="3"/>
-      <c r="G1583" s="3"/>
-      <c r="H1583" s="3"/>
-      <c r="I1583" s="4"/>
-      <c r="J1583" s="4"/>
+      <c r="A1583" s="3" t="s">
+        <v>1417</v>
+      </c>
+      <c r="B1583" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1583" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1583" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1583" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1583" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1583" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1583" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1583" s="4">
+        <f t="shared" si="596"/>
+        <v>2025</v>
+      </c>
+      <c r="J1583" s="4">
+        <f t="shared" si="597"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1584" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1584" s="3"/>
-      <c r="B1584" s="3"/>
-      <c r="C1584" s="3"/>
-      <c r="D1584" s="3"/>
-      <c r="E1584" s="3"/>
+      <c r="A1584" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B1584" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1584" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1584" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1584" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1584" s="3"/>
-      <c r="G1584" s="3"/>
-      <c r="H1584" s="3"/>
-      <c r="I1584" s="4"/>
-      <c r="J1584" s="4"/>
+      <c r="G1584" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1584" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1584" s="4">
+        <f t="shared" si="596"/>
+        <v>2025</v>
+      </c>
+      <c r="J1584" s="4">
+        <f t="shared" si="597"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1585" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1585" s="3"/>
-      <c r="B1585" s="3"/>
-      <c r="C1585" s="3"/>
-      <c r="D1585" s="3"/>
-      <c r="E1585" s="3"/>
-      <c r="F1585" s="3"/>
-      <c r="G1585" s="3"/>
-      <c r="H1585" s="3"/>
-      <c r="I1585" s="4"/>
-      <c r="J1585" s="4"/>
+      <c r="A1585" s="3" t="s">
+        <v>1418</v>
+      </c>
+      <c r="B1585" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1585" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1585" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1585" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1585" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1585" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1585" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1585" s="4">
+        <f t="shared" ref="I1585:I1588" si="598">YEAR(A1585)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1585" s="4">
+        <f t="shared" ref="J1585:J1588" si="599">MONTH(A1585)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1586" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1586" s="3"/>
-      <c r="B1586" s="3"/>
-      <c r="C1586" s="3"/>
-      <c r="D1586" s="3"/>
-      <c r="E1586" s="3"/>
+      <c r="A1586" s="3" t="s">
+        <v>1419</v>
+      </c>
+      <c r="B1586" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1586" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1586" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1586" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1586" s="3"/>
-      <c r="G1586" s="3"/>
-      <c r="H1586" s="3"/>
-      <c r="I1586" s="4"/>
-      <c r="J1586" s="4"/>
+      <c r="G1586" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1586" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1586" s="4">
+        <f t="shared" si="598"/>
+        <v>2025</v>
+      </c>
+      <c r="J1586" s="4">
+        <f t="shared" si="599"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1587" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1587" s="3"/>
-      <c r="B1587" s="3"/>
-      <c r="C1587" s="3"/>
-      <c r="D1587" s="3"/>
-      <c r="E1587" s="3"/>
-      <c r="F1587" s="3"/>
-      <c r="G1587" s="3"/>
-      <c r="H1587" s="3"/>
-      <c r="I1587" s="4"/>
-      <c r="J1587" s="4"/>
+      <c r="A1587" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B1587" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1587" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1587" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1587" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1587" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1587" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1587" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1587" s="4">
+        <f t="shared" si="598"/>
+        <v>2025</v>
+      </c>
+      <c r="J1587" s="4">
+        <f t="shared" si="599"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1588" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1588" s="3"/>
-      <c r="B1588" s="3"/>
-      <c r="C1588" s="3"/>
-      <c r="D1588" s="3"/>
-      <c r="E1588" s="3"/>
-      <c r="F1588" s="3"/>
-      <c r="G1588" s="3"/>
-      <c r="H1588" s="3"/>
-      <c r="I1588" s="4"/>
-      <c r="J1588" s="4"/>
+      <c r="A1588" s="3" t="s">
+        <v>1420</v>
+      </c>
+      <c r="B1588" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1588" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D1588" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="E1588" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1588" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1588" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1588" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1588" s="4">
+        <f t="shared" si="598"/>
+        <v>2025</v>
+      </c>
+      <c r="J1588" s="4">
+        <f t="shared" si="599"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1589" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1589" s="3"/>
-      <c r="B1589" s="3"/>
-      <c r="C1589" s="3"/>
-      <c r="D1589" s="3"/>
-      <c r="E1589" s="3"/>
-      <c r="F1589" s="3"/>
-      <c r="G1589" s="3"/>
-      <c r="H1589" s="3"/>
-      <c r="I1589" s="4"/>
-      <c r="J1589" s="4"/>
+      <c r="A1589" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B1589" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1589" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1589" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1589" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1589" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1589" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1589" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1589" s="4">
+        <f t="shared" ref="I1589:I1590" si="600">YEAR(A1589)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1589" s="4">
+        <f t="shared" ref="J1589:J1590" si="601">MONTH(A1589)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1590" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1590" s="3"/>
-      <c r="B1590" s="3"/>
-      <c r="C1590" s="3"/>
-      <c r="D1590" s="3"/>
-      <c r="E1590" s="3"/>
-      <c r="F1590" s="3"/>
-      <c r="G1590" s="3"/>
-      <c r="H1590" s="3"/>
-      <c r="I1590" s="4"/>
-      <c r="J1590" s="4"/>
+      <c r="A1590" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B1590" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1590" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1590" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1590" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1590" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1590" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1590" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1590" s="4">
+        <f t="shared" si="600"/>
+        <v>2025</v>
+      </c>
+      <c r="J1590" s="4">
+        <f t="shared" si="601"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1591" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1591" s="3"/>
-      <c r="B1591" s="3"/>
-      <c r="C1591" s="3"/>
-      <c r="D1591" s="3"/>
-      <c r="E1591" s="3"/>
-      <c r="F1591" s="3"/>
-      <c r="G1591" s="3"/>
-      <c r="H1591" s="3"/>
-      <c r="I1591" s="4"/>
-      <c r="J1591" s="4"/>
+      <c r="A1591" s="3" t="s">
+        <v>1421</v>
+      </c>
+      <c r="B1591" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1591" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1591" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1591" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1591" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1591" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1591" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1591" s="4">
+        <f t="shared" ref="I1591:I1592" si="602">YEAR(A1591)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1591" s="4">
+        <f t="shared" ref="J1591:J1592" si="603">MONTH(A1591)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1592" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1592" s="3"/>
-      <c r="B1592" s="3"/>
-      <c r="C1592" s="3"/>
-      <c r="D1592" s="3"/>
-      <c r="E1592" s="3"/>
-      <c r="F1592" s="3"/>
-      <c r="G1592" s="3"/>
-      <c r="H1592" s="3"/>
-      <c r="I1592" s="4"/>
-      <c r="J1592" s="4"/>
+      <c r="A1592" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B1592" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1592" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="D1592" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1592" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1592" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1592" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1592" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1592" s="4">
+        <f t="shared" si="602"/>
+        <v>2025</v>
+      </c>
+      <c r="J1592" s="4">
+        <f t="shared" si="603"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1593" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1593" s="3"/>
-      <c r="B1593" s="3"/>
-      <c r="C1593" s="3"/>
-      <c r="D1593" s="3"/>
-      <c r="E1593" s="3"/>
-      <c r="F1593" s="3"/>
-      <c r="G1593" s="3"/>
-      <c r="H1593" s="3"/>
-      <c r="I1593" s="4"/>
-      <c r="J1593" s="4"/>
+      <c r="A1593" s="3" t="s">
+        <v>1422</v>
+      </c>
+      <c r="B1593" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1593" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1593" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1593" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1593" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1593" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1593" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1593" s="4">
+        <f t="shared" ref="I1593" si="604">YEAR(A1593)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1593" s="4">
+        <f t="shared" ref="J1593" si="605">MONTH(A1593)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1594" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1594" s="3"/>
-      <c r="B1594" s="3"/>
-      <c r="C1594" s="3"/>
-      <c r="D1594" s="3"/>
-      <c r="E1594" s="3"/>
-      <c r="F1594" s="3"/>
-      <c r="G1594" s="3"/>
-      <c r="H1594" s="3"/>
-      <c r="I1594" s="4"/>
-      <c r="J1594" s="4"/>
+      <c r="A1594" s="3" t="s">
+        <v>1423</v>
+      </c>
+      <c r="B1594" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="C1594" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1594" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1594" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1594" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1594" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1594" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1594" s="4">
+        <f t="shared" ref="I1594:I1598" si="606">YEAR(A1594)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1594" s="4">
+        <f t="shared" ref="J1594:J1598" si="607">MONTH(A1594)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1595" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1595" s="3"/>
-      <c r="B1595" s="3"/>
-      <c r="C1595" s="3"/>
-      <c r="D1595" s="3"/>
-      <c r="E1595" s="3"/>
+      <c r="A1595" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B1595" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1595" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1595" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1595" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1595" s="3"/>
-      <c r="G1595" s="3"/>
-      <c r="H1595" s="3"/>
-      <c r="I1595" s="4"/>
-      <c r="J1595" s="4"/>
+      <c r="G1595" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1595" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1595" s="4">
+        <f t="shared" si="606"/>
+        <v>2025</v>
+      </c>
+      <c r="J1595" s="4">
+        <f t="shared" si="607"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1596" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1596" s="3"/>
-      <c r="B1596" s="3"/>
-      <c r="C1596" s="3"/>
-      <c r="D1596" s="3"/>
-      <c r="E1596" s="3"/>
+      <c r="A1596" s="3" t="s">
+        <v>1424</v>
+      </c>
+      <c r="B1596" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1596" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1596" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1596" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1596" s="3"/>
-      <c r="G1596" s="3"/>
-      <c r="H1596" s="3"/>
-      <c r="I1596" s="4"/>
-      <c r="J1596" s="4"/>
+      <c r="G1596" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1596" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1596" s="4">
+        <f t="shared" si="606"/>
+        <v>2025</v>
+      </c>
+      <c r="J1596" s="4">
+        <f t="shared" si="607"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1597" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1597" s="3"/>
-      <c r="B1597" s="3"/>
-      <c r="C1597" s="3"/>
-      <c r="D1597" s="3"/>
-      <c r="E1597" s="3"/>
-      <c r="F1597" s="3"/>
-      <c r="G1597" s="3"/>
-      <c r="H1597" s="3"/>
-      <c r="I1597" s="4"/>
-      <c r="J1597" s="4"/>
+      <c r="A1597" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B1597" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1597" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1597" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1597" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1597" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1597" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1597" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1597" s="4">
+        <f t="shared" si="606"/>
+        <v>2025</v>
+      </c>
+      <c r="J1597" s="4">
+        <f t="shared" si="607"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1598" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1598" s="3"/>
-      <c r="B1598" s="3"/>
-      <c r="C1598" s="3"/>
-      <c r="D1598" s="3"/>
-      <c r="E1598" s="3"/>
-      <c r="F1598" s="3"/>
-      <c r="G1598" s="3"/>
-      <c r="H1598" s="3"/>
-      <c r="I1598" s="4"/>
-      <c r="J1598" s="4"/>
+      <c r="A1598" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B1598" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1598" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1598" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1598" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1598" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1598" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1598" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1598" s="4">
+        <f t="shared" si="606"/>
+        <v>2025</v>
+      </c>
+      <c r="J1598" s="4">
+        <f t="shared" si="607"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1599" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1599" s="3"/>
-      <c r="B1599" s="3"/>
-      <c r="C1599" s="3"/>
-      <c r="D1599" s="3"/>
-      <c r="E1599" s="3"/>
-      <c r="F1599" s="3"/>
-      <c r="G1599" s="3"/>
-      <c r="H1599" s="3"/>
-      <c r="I1599" s="4"/>
-      <c r="J1599" s="4"/>
+      <c r="A1599" s="3" t="s">
+        <v>1425</v>
+      </c>
+      <c r="B1599" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1599" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1599" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1599" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1599" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1599" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1599" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1599" s="4">
+        <f t="shared" ref="I1599" si="608">YEAR(A1599)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1599" s="4">
+        <f t="shared" ref="J1599" si="609">MONTH(A1599)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1600" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1600" s="3"/>
-      <c r="B1600" s="3"/>
-      <c r="C1600" s="3"/>
-      <c r="D1600" s="3"/>
-      <c r="E1600" s="3"/>
-      <c r="F1600" s="3"/>
-      <c r="G1600" s="3"/>
-      <c r="H1600" s="3"/>
-      <c r="I1600" s="4"/>
-      <c r="J1600" s="4"/>
+      <c r="A1600" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B1600" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1600" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D1600" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1600" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1600" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1600" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1600" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1600" s="4">
+        <f t="shared" ref="I1600:I1603" si="610">YEAR(A1600)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1600" s="4">
+        <f t="shared" ref="J1600:J1603" si="611">MONTH(A1600)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1601" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1601" s="3"/>
-      <c r="B1601" s="3"/>
-      <c r="C1601" s="3"/>
-      <c r="D1601" s="3"/>
-      <c r="E1601" s="3"/>
+      <c r="A1601" s="3" t="s">
+        <v>1426</v>
+      </c>
+      <c r="B1601" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1601" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="D1601" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1601" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1601" s="3"/>
-      <c r="G1601" s="3"/>
-      <c r="H1601" s="3"/>
-      <c r="I1601" s="4"/>
-      <c r="J1601" s="4"/>
+      <c r="G1601" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1601" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1601" s="4">
+        <f t="shared" si="610"/>
+        <v>2025</v>
+      </c>
+      <c r="J1601" s="4">
+        <f t="shared" si="611"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1602" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1602" s="3"/>
-      <c r="B1602" s="3"/>
-      <c r="C1602" s="3"/>
-      <c r="D1602" s="3"/>
-      <c r="E1602" s="3"/>
-      <c r="F1602" s="3"/>
-      <c r="G1602" s="3"/>
-      <c r="H1602" s="3"/>
-      <c r="I1602" s="4"/>
-      <c r="J1602" s="4"/>
+      <c r="A1602" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B1602" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1602" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1602" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1602" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1602" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1602" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1602" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1602" s="4">
+        <f t="shared" si="610"/>
+        <v>2025</v>
+      </c>
+      <c r="J1602" s="4">
+        <f t="shared" si="611"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1603" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1603" s="3"/>
-      <c r="B1603" s="3"/>
-      <c r="C1603" s="3"/>
-      <c r="D1603" s="3"/>
-      <c r="E1603" s="3"/>
-      <c r="F1603" s="3"/>
-      <c r="G1603" s="3"/>
-      <c r="H1603" s="3"/>
-      <c r="I1603" s="4"/>
-      <c r="J1603" s="4"/>
+      <c r="A1603" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B1603" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1603" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1603" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1603" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1603" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1603" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1603" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1603" s="4">
+        <f t="shared" si="610"/>
+        <v>2025</v>
+      </c>
+      <c r="J1603" s="4">
+        <f t="shared" si="611"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1604" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1604" s="3"/>
-      <c r="B1604" s="3"/>
-      <c r="C1604" s="3"/>
-      <c r="D1604" s="3"/>
-      <c r="E1604" s="3"/>
-      <c r="F1604" s="3"/>
-      <c r="G1604" s="3"/>
-      <c r="H1604" s="3"/>
-      <c r="I1604" s="4"/>
-      <c r="J1604" s="4"/>
+      <c r="A1604" s="3" t="s">
+        <v>1427</v>
+      </c>
+      <c r="B1604" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1604" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="D1604" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1604" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1604" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1604" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1604" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1604" s="4">
+        <f t="shared" ref="I1604:I1606" si="612">YEAR(A1604)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1604" s="4">
+        <f t="shared" ref="J1604:J1606" si="613">MONTH(A1604)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1605" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1605" s="3"/>
-      <c r="B1605" s="3"/>
-      <c r="C1605" s="3"/>
-      <c r="D1605" s="3"/>
-      <c r="E1605" s="3"/>
-      <c r="F1605" s="3"/>
-      <c r="G1605" s="3"/>
-      <c r="H1605" s="3"/>
-      <c r="I1605" s="4"/>
-      <c r="J1605" s="4"/>
+      <c r="A1605" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1605" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1605" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1605" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1605" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1605" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1605" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1605" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1605" s="4">
+        <f t="shared" si="612"/>
+        <v>2025</v>
+      </c>
+      <c r="J1605" s="4">
+        <f t="shared" si="613"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1606" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1606" s="3"/>
-      <c r="B1606" s="3"/>
-      <c r="C1606" s="3"/>
-      <c r="D1606" s="3"/>
-      <c r="E1606" s="3"/>
-      <c r="F1606" s="3"/>
-      <c r="G1606" s="3"/>
-      <c r="H1606" s="3"/>
-      <c r="I1606" s="4"/>
-      <c r="J1606" s="4"/>
+      <c r="A1606" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1606" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1606" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1606" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1606" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1606" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1606" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1606" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1606" s="4">
+        <f t="shared" si="612"/>
+        <v>2025</v>
+      </c>
+      <c r="J1606" s="4">
+        <f t="shared" si="613"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1607" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1607" s="3"/>
-      <c r="B1607" s="3"/>
-      <c r="C1607" s="3"/>
-      <c r="D1607" s="3"/>
-      <c r="E1607" s="3"/>
-      <c r="F1607" s="3"/>
-      <c r="G1607" s="3"/>
-      <c r="H1607" s="3"/>
-      <c r="I1607" s="4"/>
-      <c r="J1607" s="4"/>
+      <c r="A1607" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1607" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1607" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="D1607" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1607" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1607" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1607" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1607" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1607" s="4">
+        <f t="shared" ref="I1607:I1608" si="614">YEAR(A1607)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1607" s="4">
+        <f t="shared" ref="J1607:J1608" si="615">MONTH(A1607)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1608" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1608" s="3"/>
-      <c r="B1608" s="3"/>
-      <c r="C1608" s="3"/>
-      <c r="D1608" s="3"/>
-      <c r="E1608" s="3"/>
-      <c r="F1608" s="3"/>
-      <c r="G1608" s="3"/>
-      <c r="H1608" s="3"/>
-      <c r="I1608" s="4"/>
-      <c r="J1608" s="4"/>
+      <c r="A1608" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1608" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1608" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1608" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1608" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1608" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1608" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1608" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1608" s="4">
+        <f t="shared" si="614"/>
+        <v>2025</v>
+      </c>
+      <c r="J1608" s="4">
+        <f t="shared" si="615"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1609" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1609" s="3"/>
-      <c r="B1609" s="3"/>
-      <c r="C1609" s="3"/>
-      <c r="D1609" s="3"/>
-      <c r="E1609" s="3"/>
-      <c r="F1609" s="3"/>
-      <c r="G1609" s="3"/>
-      <c r="H1609" s="3"/>
-      <c r="I1609" s="4"/>
-      <c r="J1609" s="4"/>
+      <c r="A1609" s="3" t="s">
+        <v>1428</v>
+      </c>
+      <c r="B1609" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1609" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1609" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1609" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1609" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1609" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1609" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1609" s="4">
+        <f t="shared" ref="I1609" si="616">YEAR(A1609)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1609" s="4">
+        <f t="shared" ref="J1609" si="617">MONTH(A1609)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1610" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1610" s="3"/>
@@ -58040,6 +58950,486 @@
       <c r="I1627" s="4"/>
       <c r="J1627" s="4"/>
     </row>
+    <row r="1628" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1628" s="3"/>
+      <c r="B1628" s="3"/>
+      <c r="C1628" s="3"/>
+      <c r="D1628" s="3"/>
+      <c r="E1628" s="3"/>
+      <c r="F1628" s="3"/>
+      <c r="G1628" s="3"/>
+      <c r="H1628" s="3"/>
+      <c r="I1628" s="4"/>
+      <c r="J1628" s="4"/>
+    </row>
+    <row r="1629" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1629" s="3"/>
+      <c r="B1629" s="3"/>
+      <c r="C1629" s="3"/>
+      <c r="D1629" s="3"/>
+      <c r="E1629" s="3"/>
+      <c r="F1629" s="3"/>
+      <c r="G1629" s="3"/>
+      <c r="H1629" s="3"/>
+      <c r="I1629" s="4"/>
+      <c r="J1629" s="4"/>
+    </row>
+    <row r="1630" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1630" s="3"/>
+      <c r="B1630" s="3"/>
+      <c r="C1630" s="3"/>
+      <c r="D1630" s="3"/>
+      <c r="E1630" s="3"/>
+      <c r="F1630" s="3"/>
+      <c r="G1630" s="3"/>
+      <c r="H1630" s="3"/>
+      <c r="I1630" s="4"/>
+      <c r="J1630" s="4"/>
+    </row>
+    <row r="1631" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1631" s="3"/>
+      <c r="B1631" s="3"/>
+      <c r="C1631" s="3"/>
+      <c r="D1631" s="3"/>
+      <c r="E1631" s="3"/>
+      <c r="F1631" s="3"/>
+      <c r="G1631" s="3"/>
+      <c r="H1631" s="3"/>
+      <c r="I1631" s="4"/>
+      <c r="J1631" s="4"/>
+    </row>
+    <row r="1632" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1632" s="3"/>
+      <c r="B1632" s="3"/>
+      <c r="C1632" s="3"/>
+      <c r="D1632" s="3"/>
+      <c r="E1632" s="3"/>
+      <c r="F1632" s="3"/>
+      <c r="G1632" s="3"/>
+      <c r="H1632" s="3"/>
+      <c r="I1632" s="4"/>
+      <c r="J1632" s="4"/>
+    </row>
+    <row r="1633" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1633" s="3"/>
+      <c r="B1633" s="3"/>
+      <c r="C1633" s="3"/>
+      <c r="D1633" s="3"/>
+      <c r="E1633" s="3"/>
+      <c r="F1633" s="3"/>
+      <c r="G1633" s="3"/>
+      <c r="H1633" s="3"/>
+      <c r="I1633" s="4"/>
+      <c r="J1633" s="4"/>
+    </row>
+    <row r="1634" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1634" s="3"/>
+      <c r="B1634" s="3"/>
+      <c r="C1634" s="3"/>
+      <c r="D1634" s="3"/>
+      <c r="E1634" s="3"/>
+      <c r="F1634" s="3"/>
+      <c r="G1634" s="3"/>
+      <c r="H1634" s="3"/>
+      <c r="I1634" s="4"/>
+      <c r="J1634" s="4"/>
+    </row>
+    <row r="1635" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1635" s="3"/>
+      <c r="B1635" s="3"/>
+      <c r="C1635" s="3"/>
+      <c r="D1635" s="3"/>
+      <c r="E1635" s="3"/>
+      <c r="F1635" s="3"/>
+      <c r="G1635" s="3"/>
+      <c r="H1635" s="3"/>
+      <c r="I1635" s="4"/>
+      <c r="J1635" s="4"/>
+    </row>
+    <row r="1636" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1636" s="3"/>
+      <c r="B1636" s="3"/>
+      <c r="C1636" s="3"/>
+      <c r="D1636" s="3"/>
+      <c r="E1636" s="3"/>
+      <c r="F1636" s="3"/>
+      <c r="G1636" s="3"/>
+      <c r="H1636" s="3"/>
+      <c r="I1636" s="4"/>
+      <c r="J1636" s="4"/>
+    </row>
+    <row r="1637" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1637" s="3"/>
+      <c r="B1637" s="3"/>
+      <c r="C1637" s="3"/>
+      <c r="D1637" s="3"/>
+      <c r="E1637" s="3"/>
+      <c r="F1637" s="3"/>
+      <c r="G1637" s="3"/>
+      <c r="H1637" s="3"/>
+      <c r="I1637" s="4"/>
+      <c r="J1637" s="4"/>
+    </row>
+    <row r="1638" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1638" s="3"/>
+      <c r="B1638" s="3"/>
+      <c r="C1638" s="3"/>
+      <c r="D1638" s="3"/>
+      <c r="E1638" s="3"/>
+      <c r="F1638" s="3"/>
+      <c r="G1638" s="3"/>
+      <c r="H1638" s="3"/>
+      <c r="I1638" s="4"/>
+      <c r="J1638" s="4"/>
+    </row>
+    <row r="1639" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1639" s="3"/>
+      <c r="B1639" s="3"/>
+      <c r="C1639" s="3"/>
+      <c r="D1639" s="3"/>
+      <c r="E1639" s="3"/>
+      <c r="F1639" s="3"/>
+      <c r="G1639" s="3"/>
+      <c r="H1639" s="3"/>
+      <c r="I1639" s="4"/>
+      <c r="J1639" s="4"/>
+    </row>
+    <row r="1640" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1640" s="3"/>
+      <c r="B1640" s="3"/>
+      <c r="C1640" s="3"/>
+      <c r="D1640" s="3"/>
+      <c r="E1640" s="3"/>
+      <c r="F1640" s="3"/>
+      <c r="G1640" s="3"/>
+      <c r="H1640" s="3"/>
+      <c r="I1640" s="4"/>
+      <c r="J1640" s="4"/>
+    </row>
+    <row r="1641" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1641" s="3"/>
+      <c r="B1641" s="3"/>
+      <c r="C1641" s="3"/>
+      <c r="D1641" s="3"/>
+      <c r="E1641" s="3"/>
+      <c r="F1641" s="3"/>
+      <c r="G1641" s="3"/>
+      <c r="H1641" s="3"/>
+      <c r="I1641" s="4"/>
+      <c r="J1641" s="4"/>
+    </row>
+    <row r="1642" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1642" s="3"/>
+      <c r="B1642" s="3"/>
+      <c r="C1642" s="3"/>
+      <c r="D1642" s="3"/>
+      <c r="E1642" s="3"/>
+      <c r="F1642" s="3"/>
+      <c r="G1642" s="3"/>
+      <c r="H1642" s="3"/>
+      <c r="I1642" s="4"/>
+      <c r="J1642" s="4"/>
+    </row>
+    <row r="1643" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1643" s="3"/>
+      <c r="B1643" s="3"/>
+      <c r="C1643" s="3"/>
+      <c r="D1643" s="3"/>
+      <c r="E1643" s="3"/>
+      <c r="F1643" s="3"/>
+      <c r="G1643" s="3"/>
+      <c r="H1643" s="3"/>
+      <c r="I1643" s="4"/>
+      <c r="J1643" s="4"/>
+    </row>
+    <row r="1644" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1644" s="3"/>
+      <c r="B1644" s="3"/>
+      <c r="C1644" s="3"/>
+      <c r="D1644" s="3"/>
+      <c r="E1644" s="3"/>
+      <c r="F1644" s="3"/>
+      <c r="G1644" s="3"/>
+      <c r="H1644" s="3"/>
+      <c r="I1644" s="4"/>
+      <c r="J1644" s="4"/>
+    </row>
+    <row r="1645" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1645" s="3"/>
+      <c r="B1645" s="3"/>
+      <c r="C1645" s="3"/>
+      <c r="D1645" s="3"/>
+      <c r="E1645" s="3"/>
+      <c r="F1645" s="3"/>
+      <c r="G1645" s="3"/>
+      <c r="H1645" s="3"/>
+      <c r="I1645" s="4"/>
+      <c r="J1645" s="4"/>
+    </row>
+    <row r="1646" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1646" s="3"/>
+      <c r="B1646" s="3"/>
+      <c r="C1646" s="3"/>
+      <c r="D1646" s="3"/>
+      <c r="E1646" s="3"/>
+      <c r="F1646" s="3"/>
+      <c r="G1646" s="3"/>
+      <c r="H1646" s="3"/>
+      <c r="I1646" s="4"/>
+      <c r="J1646" s="4"/>
+    </row>
+    <row r="1647" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1647" s="3"/>
+      <c r="B1647" s="3"/>
+      <c r="C1647" s="3"/>
+      <c r="D1647" s="3"/>
+      <c r="E1647" s="3"/>
+      <c r="F1647" s="3"/>
+      <c r="G1647" s="3"/>
+      <c r="H1647" s="3"/>
+      <c r="I1647" s="4"/>
+      <c r="J1647" s="4"/>
+    </row>
+    <row r="1648" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1648" s="3"/>
+      <c r="B1648" s="3"/>
+      <c r="C1648" s="3"/>
+      <c r="D1648" s="3"/>
+      <c r="E1648" s="3"/>
+      <c r="F1648" s="3"/>
+      <c r="G1648" s="3"/>
+      <c r="H1648" s="3"/>
+      <c r="I1648" s="4"/>
+      <c r="J1648" s="4"/>
+    </row>
+    <row r="1649" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1649" s="3"/>
+      <c r="B1649" s="3"/>
+      <c r="C1649" s="3"/>
+      <c r="D1649" s="3"/>
+      <c r="E1649" s="3"/>
+      <c r="F1649" s="3"/>
+      <c r="G1649" s="3"/>
+      <c r="H1649" s="3"/>
+      <c r="I1649" s="4"/>
+      <c r="J1649" s="4"/>
+    </row>
+    <row r="1650" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1650" s="3"/>
+      <c r="B1650" s="3"/>
+      <c r="C1650" s="3"/>
+      <c r="D1650" s="3"/>
+      <c r="E1650" s="3"/>
+      <c r="F1650" s="3"/>
+      <c r="G1650" s="3"/>
+      <c r="H1650" s="3"/>
+      <c r="I1650" s="4"/>
+      <c r="J1650" s="4"/>
+    </row>
+    <row r="1651" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1651" s="3"/>
+      <c r="B1651" s="3"/>
+      <c r="C1651" s="3"/>
+      <c r="D1651" s="3"/>
+      <c r="E1651" s="3"/>
+      <c r="F1651" s="3"/>
+      <c r="G1651" s="3"/>
+      <c r="H1651" s="3"/>
+      <c r="I1651" s="4"/>
+      <c r="J1651" s="4"/>
+    </row>
+    <row r="1652" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1652" s="3"/>
+      <c r="B1652" s="3"/>
+      <c r="C1652" s="3"/>
+      <c r="D1652" s="3"/>
+      <c r="E1652" s="3"/>
+      <c r="F1652" s="3"/>
+      <c r="G1652" s="3"/>
+      <c r="H1652" s="3"/>
+      <c r="I1652" s="4"/>
+      <c r="J1652" s="4"/>
+    </row>
+    <row r="1653" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1653" s="3"/>
+      <c r="B1653" s="3"/>
+      <c r="C1653" s="3"/>
+      <c r="D1653" s="3"/>
+      <c r="E1653" s="3"/>
+      <c r="F1653" s="3"/>
+      <c r="G1653" s="3"/>
+      <c r="H1653" s="3"/>
+      <c r="I1653" s="4"/>
+      <c r="J1653" s="4"/>
+    </row>
+    <row r="1654" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1654" s="3"/>
+      <c r="B1654" s="3"/>
+      <c r="C1654" s="3"/>
+      <c r="D1654" s="3"/>
+      <c r="E1654" s="3"/>
+      <c r="F1654" s="3"/>
+      <c r="G1654" s="3"/>
+      <c r="H1654" s="3"/>
+      <c r="I1654" s="4"/>
+      <c r="J1654" s="4"/>
+    </row>
+    <row r="1655" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1655" s="3"/>
+      <c r="B1655" s="3"/>
+      <c r="C1655" s="3"/>
+      <c r="D1655" s="3"/>
+      <c r="E1655" s="3"/>
+      <c r="F1655" s="3"/>
+      <c r="G1655" s="3"/>
+      <c r="H1655" s="3"/>
+      <c r="I1655" s="4"/>
+      <c r="J1655" s="4"/>
+    </row>
+    <row r="1656" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1656" s="3"/>
+      <c r="B1656" s="3"/>
+      <c r="C1656" s="3"/>
+      <c r="D1656" s="3"/>
+      <c r="E1656" s="3"/>
+      <c r="F1656" s="3"/>
+      <c r="G1656" s="3"/>
+      <c r="H1656" s="3"/>
+      <c r="I1656" s="4"/>
+      <c r="J1656" s="4"/>
+    </row>
+    <row r="1657" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1657" s="3"/>
+      <c r="B1657" s="3"/>
+      <c r="C1657" s="3"/>
+      <c r="D1657" s="3"/>
+      <c r="E1657" s="3"/>
+      <c r="F1657" s="3"/>
+      <c r="G1657" s="3"/>
+      <c r="H1657" s="3"/>
+      <c r="I1657" s="4"/>
+      <c r="J1657" s="4"/>
+    </row>
+    <row r="1658" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1658" s="3"/>
+      <c r="B1658" s="3"/>
+      <c r="C1658" s="3"/>
+      <c r="D1658" s="3"/>
+      <c r="E1658" s="3"/>
+      <c r="F1658" s="3"/>
+      <c r="G1658" s="3"/>
+      <c r="H1658" s="3"/>
+      <c r="I1658" s="4"/>
+      <c r="J1658" s="4"/>
+    </row>
+    <row r="1659" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1659" s="3"/>
+      <c r="B1659" s="3"/>
+      <c r="C1659" s="3"/>
+      <c r="D1659" s="3"/>
+      <c r="E1659" s="3"/>
+      <c r="F1659" s="3"/>
+      <c r="G1659" s="3"/>
+      <c r="H1659" s="3"/>
+      <c r="I1659" s="4"/>
+      <c r="J1659" s="4"/>
+    </row>
+    <row r="1660" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1660" s="3"/>
+      <c r="B1660" s="3"/>
+      <c r="C1660" s="3"/>
+      <c r="D1660" s="3"/>
+      <c r="E1660" s="3"/>
+      <c r="F1660" s="3"/>
+      <c r="G1660" s="3"/>
+      <c r="H1660" s="3"/>
+      <c r="I1660" s="4"/>
+      <c r="J1660" s="4"/>
+    </row>
+    <row r="1661" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1661" s="3"/>
+      <c r="B1661" s="3"/>
+      <c r="C1661" s="3"/>
+      <c r="D1661" s="3"/>
+      <c r="E1661" s="3"/>
+      <c r="F1661" s="3"/>
+      <c r="G1661" s="3"/>
+      <c r="H1661" s="3"/>
+      <c r="I1661" s="4"/>
+      <c r="J1661" s="4"/>
+    </row>
+    <row r="1662" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1662" s="3"/>
+      <c r="B1662" s="3"/>
+      <c r="C1662" s="3"/>
+      <c r="D1662" s="3"/>
+      <c r="E1662" s="3"/>
+      <c r="F1662" s="3"/>
+      <c r="G1662" s="3"/>
+      <c r="H1662" s="3"/>
+      <c r="I1662" s="4"/>
+      <c r="J1662" s="4"/>
+    </row>
+    <row r="1663" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1663" s="3"/>
+      <c r="B1663" s="3"/>
+      <c r="C1663" s="3"/>
+      <c r="D1663" s="3"/>
+      <c r="E1663" s="3"/>
+      <c r="F1663" s="3"/>
+      <c r="G1663" s="3"/>
+      <c r="H1663" s="3"/>
+      <c r="I1663" s="4"/>
+      <c r="J1663" s="4"/>
+    </row>
+    <row r="1664" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1664" s="3"/>
+      <c r="B1664" s="3"/>
+      <c r="C1664" s="3"/>
+      <c r="D1664" s="3"/>
+      <c r="E1664" s="3"/>
+      <c r="F1664" s="3"/>
+      <c r="G1664" s="3"/>
+      <c r="H1664" s="3"/>
+      <c r="I1664" s="4"/>
+      <c r="J1664" s="4"/>
+    </row>
+    <row r="1665" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1665" s="3"/>
+      <c r="B1665" s="3"/>
+      <c r="C1665" s="3"/>
+      <c r="D1665" s="3"/>
+      <c r="E1665" s="3"/>
+      <c r="F1665" s="3"/>
+      <c r="G1665" s="3"/>
+      <c r="H1665" s="3"/>
+      <c r="I1665" s="4"/>
+      <c r="J1665" s="4"/>
+    </row>
+    <row r="1666" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1666" s="3"/>
+      <c r="B1666" s="3"/>
+      <c r="C1666" s="3"/>
+      <c r="D1666" s="3"/>
+      <c r="E1666" s="3"/>
+      <c r="F1666" s="3"/>
+      <c r="G1666" s="3"/>
+      <c r="H1666" s="3"/>
+      <c r="I1666" s="4"/>
+      <c r="J1666" s="4"/>
+    </row>
+    <row r="1667" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1667" s="3"/>
+      <c r="B1667" s="3"/>
+      <c r="C1667" s="3"/>
+      <c r="D1667" s="3"/>
+      <c r="E1667" s="3"/>
+      <c r="F1667" s="3"/>
+      <c r="G1667" s="3"/>
+      <c r="H1667" s="3"/>
+      <c r="I1667" s="4"/>
+      <c r="J1667" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-08-11.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12518" uniqueCount="1429">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12784" uniqueCount="1454">
   <si>
     <t>Year</t>
   </si>
@@ -4312,6 +4312,81 @@
   </si>
   <si>
     <t>2025-07-13</t>
+  </si>
+  <si>
+    <t>2025-07-14</t>
+  </si>
+  <si>
+    <t>2025-07-15</t>
+  </si>
+  <si>
+    <t>2025-07-16</t>
+  </si>
+  <si>
+    <t>2025-07-17</t>
+  </si>
+  <si>
+    <t>2025-07-18</t>
+  </si>
+  <si>
+    <t>2025-07-20</t>
+  </si>
+  <si>
+    <t>2025-07-21</t>
+  </si>
+  <si>
+    <t>2025-07-22</t>
+  </si>
+  <si>
+    <t>2025-07-24</t>
+  </si>
+  <si>
+    <t>2025-07-25</t>
+  </si>
+  <si>
+    <t>2025-07-27</t>
+  </si>
+  <si>
+    <t>Resume update.</t>
+  </si>
+  <si>
+    <t>2025-07-28</t>
+  </si>
+  <si>
+    <t>2025-07-29</t>
+  </si>
+  <si>
+    <t>2025-07-31</t>
+  </si>
+  <si>
+    <t>2025-08-01</t>
+  </si>
+  <si>
+    <t>2025-08-04</t>
+  </si>
+  <si>
+    <t>2025-08-05</t>
+  </si>
+  <si>
+    <t>Hackberry Pi stuff.</t>
+  </si>
+  <si>
+    <t>2025-08-06</t>
+  </si>
+  <si>
+    <t>2025-08-07</t>
+  </si>
+  <si>
+    <t>2025-08-08</t>
+  </si>
+  <si>
+    <t>2025-08-09</t>
+  </si>
+  <si>
+    <t>2025-08-11</t>
+  </si>
+  <si>
+    <t>Debian 13 preseed.cfg.</t>
   </si>
 </sst>
 </file>
@@ -4723,8 +4798,8 @@
   <dimension ref="A1:J1667"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1583" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1612" sqref="D1612"/>
+      <pane ySplit="1" topLeftCell="A1624" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F1647" sqref="F1647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -58726,433 +58801,1175 @@
         <v>280</v>
       </c>
       <c r="I1609" s="4">
-        <f t="shared" ref="I1609" si="616">YEAR(A1609)</f>
+        <f t="shared" ref="I1609:I1611" si="616">YEAR(A1609)</f>
         <v>2025</v>
       </c>
       <c r="J1609" s="4">
-        <f t="shared" ref="J1609" si="617">MONTH(A1609)</f>
+        <f t="shared" ref="J1609:J1611" si="617">MONTH(A1609)</f>
         <v>7</v>
       </c>
     </row>
     <row r="1610" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1610" s="3"/>
-      <c r="B1610" s="3"/>
-      <c r="C1610" s="3"/>
-      <c r="D1610" s="3"/>
-      <c r="E1610" s="3"/>
+      <c r="A1610" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B1610" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1610" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1610" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1610" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1610" s="3"/>
-      <c r="G1610" s="3"/>
-      <c r="H1610" s="3"/>
-      <c r="I1610" s="4"/>
-      <c r="J1610" s="4"/>
+      <c r="G1610" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1610" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1610" s="4">
+        <f t="shared" si="616"/>
+        <v>2025</v>
+      </c>
+      <c r="J1610" s="4">
+        <f t="shared" si="617"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1611" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1611" s="3"/>
-      <c r="B1611" s="3"/>
-      <c r="C1611" s="3"/>
-      <c r="D1611" s="3"/>
-      <c r="E1611" s="3"/>
+      <c r="A1611" s="3" t="s">
+        <v>1429</v>
+      </c>
+      <c r="B1611" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1611" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="D1611" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1611" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1611" s="3"/>
-      <c r="G1611" s="3"/>
-      <c r="H1611" s="3"/>
-      <c r="I1611" s="4"/>
-      <c r="J1611" s="4"/>
+      <c r="G1611" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1611" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1611" s="4">
+        <f t="shared" si="616"/>
+        <v>2025</v>
+      </c>
+      <c r="J1611" s="4">
+        <f t="shared" si="617"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1612" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1612" s="3"/>
-      <c r="B1612" s="3"/>
-      <c r="C1612" s="3"/>
-      <c r="D1612" s="3"/>
-      <c r="E1612" s="3"/>
-      <c r="F1612" s="3"/>
-      <c r="G1612" s="3"/>
-      <c r="H1612" s="3"/>
-      <c r="I1612" s="4"/>
-      <c r="J1612" s="4"/>
+      <c r="A1612" s="3" t="s">
+        <v>1430</v>
+      </c>
+      <c r="B1612" s="3" t="s">
+        <v>564</v>
+      </c>
+      <c r="C1612" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1612" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1612" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1612" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1612" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1612" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1612" s="4">
+        <f t="shared" ref="I1612" si="618">YEAR(A1612)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1612" s="4">
+        <f t="shared" ref="J1612" si="619">MONTH(A1612)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1613" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1613" s="3"/>
-      <c r="B1613" s="3"/>
-      <c r="C1613" s="3"/>
-      <c r="D1613" s="3"/>
-      <c r="E1613" s="3"/>
-      <c r="F1613" s="3"/>
-      <c r="G1613" s="3"/>
-      <c r="H1613" s="3"/>
-      <c r="I1613" s="4"/>
-      <c r="J1613" s="4"/>
+      <c r="A1613" s="3" t="s">
+        <v>1431</v>
+      </c>
+      <c r="B1613" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1613" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1613" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1613" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1613" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1613" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1613" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1613" s="4">
+        <f t="shared" ref="I1613:I1615" si="620">YEAR(A1613)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1613" s="4">
+        <f t="shared" ref="J1613:J1615" si="621">MONTH(A1613)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1614" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1614" s="3"/>
-      <c r="B1614" s="3"/>
-      <c r="C1614" s="3"/>
-      <c r="D1614" s="3"/>
-      <c r="E1614" s="3"/>
+      <c r="A1614" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B1614" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1614" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1614" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1614" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1614" s="3"/>
-      <c r="G1614" s="3"/>
-      <c r="H1614" s="3"/>
-      <c r="I1614" s="4"/>
-      <c r="J1614" s="4"/>
+      <c r="G1614" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1614" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1614" s="4">
+        <f t="shared" si="620"/>
+        <v>2025</v>
+      </c>
+      <c r="J1614" s="4">
+        <f t="shared" si="621"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1615" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1615" s="3"/>
-      <c r="B1615" s="3"/>
-      <c r="C1615" s="3"/>
-      <c r="D1615" s="3"/>
-      <c r="E1615" s="3"/>
+      <c r="A1615" s="3" t="s">
+        <v>1432</v>
+      </c>
+      <c r="B1615" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1615" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1615" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1615" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1615" s="3"/>
-      <c r="G1615" s="3"/>
-      <c r="H1615" s="3"/>
-      <c r="I1615" s="4"/>
-      <c r="J1615" s="4"/>
+      <c r="G1615" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1615" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1615" s="4">
+        <f t="shared" si="620"/>
+        <v>2025</v>
+      </c>
+      <c r="J1615" s="4">
+        <f t="shared" si="621"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1616" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1616" s="3"/>
-      <c r="B1616" s="3"/>
-      <c r="C1616" s="3"/>
-      <c r="D1616" s="3"/>
-      <c r="E1616" s="3"/>
+      <c r="A1616" s="3" t="s">
+        <v>1433</v>
+      </c>
+      <c r="B1616" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1616" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1616" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1616" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1616" s="3"/>
-      <c r="G1616" s="3"/>
-      <c r="H1616" s="3"/>
-      <c r="I1616" s="4"/>
-      <c r="J1616" s="4"/>
+      <c r="G1616" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1616" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1616" s="4">
+        <f t="shared" ref="I1616:I1620" si="622">YEAR(A1616)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1616" s="4">
+        <f t="shared" ref="J1616:J1620" si="623">MONTH(A1616)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1617" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1617" s="3"/>
-      <c r="B1617" s="3"/>
-      <c r="C1617" s="3"/>
-      <c r="D1617" s="3"/>
-      <c r="E1617" s="3"/>
-      <c r="F1617" s="3"/>
-      <c r="G1617" s="3"/>
-      <c r="H1617" s="3"/>
-      <c r="I1617" s="4"/>
-      <c r="J1617" s="4"/>
+      <c r="A1617" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B1617" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1617" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="D1617" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1617" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1617" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1617" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1617" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1617" s="4">
+        <f t="shared" si="622"/>
+        <v>2025</v>
+      </c>
+      <c r="J1617" s="4">
+        <f t="shared" si="623"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1618" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1618" s="3"/>
-      <c r="B1618" s="3"/>
-      <c r="C1618" s="3"/>
-      <c r="D1618" s="3"/>
-      <c r="E1618" s="3"/>
-      <c r="F1618" s="3"/>
-      <c r="G1618" s="3"/>
-      <c r="H1618" s="3"/>
-      <c r="I1618" s="4"/>
-      <c r="J1618" s="4"/>
+      <c r="A1618" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B1618" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1618" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1618" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1618" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1618" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1618" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1618" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1618" s="4">
+        <f t="shared" si="622"/>
+        <v>2025</v>
+      </c>
+      <c r="J1618" s="4">
+        <f t="shared" si="623"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1619" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1619" s="3"/>
-      <c r="B1619" s="3"/>
-      <c r="C1619" s="3"/>
-      <c r="D1619" s="3"/>
-      <c r="E1619" s="3"/>
-      <c r="F1619" s="3"/>
-      <c r="G1619" s="3"/>
-      <c r="H1619" s="3"/>
-      <c r="I1619" s="4"/>
-      <c r="J1619" s="4"/>
+      <c r="A1619" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B1619" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="C1619" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1619" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1619" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1619" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1619" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1619" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1619" s="4">
+        <f t="shared" si="622"/>
+        <v>2025</v>
+      </c>
+      <c r="J1619" s="4">
+        <f t="shared" si="623"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1620" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1620" s="3"/>
-      <c r="B1620" s="3"/>
-      <c r="C1620" s="3"/>
-      <c r="D1620" s="3"/>
-      <c r="E1620" s="3"/>
-      <c r="F1620" s="3"/>
-      <c r="G1620" s="3"/>
-      <c r="H1620" s="3"/>
-      <c r="I1620" s="4"/>
-      <c r="J1620" s="4"/>
+      <c r="A1620" s="3" t="s">
+        <v>1434</v>
+      </c>
+      <c r="B1620" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1620" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1620" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1620" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1620" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1620" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1620" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1620" s="4">
+        <f t="shared" si="622"/>
+        <v>2025</v>
+      </c>
+      <c r="J1620" s="4">
+        <f t="shared" si="623"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1621" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1621" s="3"/>
-      <c r="B1621" s="3"/>
-      <c r="C1621" s="3"/>
-      <c r="D1621" s="3"/>
-      <c r="E1621" s="3"/>
-      <c r="F1621" s="3"/>
-      <c r="G1621" s="3"/>
-      <c r="H1621" s="3"/>
-      <c r="I1621" s="4"/>
-      <c r="J1621" s="4"/>
+      <c r="A1621" s="3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B1621" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1621" s="3" t="s">
+        <v>790</v>
+      </c>
+      <c r="D1621" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1621" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1621" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1621" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1621" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1621" s="4">
+        <f t="shared" ref="I1621:I1622" si="624">YEAR(A1621)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1621" s="4">
+        <f t="shared" ref="J1621:J1622" si="625">MONTH(A1621)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1622" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1622" s="3"/>
-      <c r="B1622" s="3"/>
-      <c r="C1622" s="3"/>
-      <c r="D1622" s="3"/>
-      <c r="E1622" s="3"/>
-      <c r="F1622" s="3"/>
-      <c r="G1622" s="3"/>
-      <c r="H1622" s="3"/>
-      <c r="I1622" s="4"/>
-      <c r="J1622" s="4"/>
+      <c r="A1622" s="3" t="s">
+        <v>1435</v>
+      </c>
+      <c r="B1622" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1622" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1622" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1622" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1622" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1622" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1622" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1622" s="4">
+        <f t="shared" si="624"/>
+        <v>2025</v>
+      </c>
+      <c r="J1622" s="4">
+        <f t="shared" si="625"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1623" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1623" s="3"/>
-      <c r="B1623" s="3"/>
-      <c r="C1623" s="3"/>
-      <c r="D1623" s="3"/>
-      <c r="E1623" s="3"/>
-      <c r="F1623" s="3"/>
-      <c r="G1623" s="3"/>
-      <c r="H1623" s="3"/>
-      <c r="I1623" s="4"/>
-      <c r="J1623" s="4"/>
+      <c r="A1623" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B1623" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="C1623" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D1623" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1623" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1623" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1623" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1623" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1623" s="4">
+        <f t="shared" ref="I1623:I1625" si="626">YEAR(A1623)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1623" s="4">
+        <f t="shared" ref="J1623:J1625" si="627">MONTH(A1623)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1624" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1624" s="3"/>
-      <c r="B1624" s="3"/>
-      <c r="C1624" s="3"/>
-      <c r="D1624" s="3"/>
-      <c r="E1624" s="3"/>
-      <c r="F1624" s="3"/>
-      <c r="G1624" s="3"/>
-      <c r="H1624" s="3"/>
-      <c r="I1624" s="4"/>
-      <c r="J1624" s="4"/>
+      <c r="A1624" s="3" t="s">
+        <v>1436</v>
+      </c>
+      <c r="B1624" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1624" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1624" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1624" s="3" t="s">
+        <v>1292</v>
+      </c>
+      <c r="F1624" s="3" t="s">
+        <v>1329</v>
+      </c>
+      <c r="G1624" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1624" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1624" s="4">
+        <f t="shared" si="626"/>
+        <v>2025</v>
+      </c>
+      <c r="J1624" s="4">
+        <f t="shared" si="627"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1625" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1625" s="3"/>
-      <c r="B1625" s="3"/>
-      <c r="C1625" s="3"/>
-      <c r="D1625" s="3"/>
-      <c r="E1625" s="3"/>
-      <c r="F1625" s="3"/>
-      <c r="G1625" s="3"/>
-      <c r="H1625" s="3"/>
-      <c r="I1625" s="4"/>
-      <c r="J1625" s="4"/>
+      <c r="A1625" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B1625" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1625" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1625" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1625" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1625" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1625" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1625" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1625" s="4">
+        <f t="shared" si="626"/>
+        <v>2025</v>
+      </c>
+      <c r="J1625" s="4">
+        <f t="shared" si="627"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1626" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1626" s="3"/>
-      <c r="B1626" s="3"/>
-      <c r="C1626" s="3"/>
-      <c r="D1626" s="3"/>
-      <c r="E1626" s="3"/>
-      <c r="F1626" s="3"/>
-      <c r="G1626" s="3"/>
-      <c r="H1626" s="3"/>
-      <c r="I1626" s="4"/>
-      <c r="J1626" s="4"/>
+      <c r="A1626" s="3" t="s">
+        <v>1437</v>
+      </c>
+      <c r="B1626" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1626" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1626" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1626" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1626" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1626" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1626" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1626" s="4">
+        <f t="shared" ref="I1626:I1628" si="628">YEAR(A1626)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1626" s="4">
+        <f t="shared" ref="J1626:J1628" si="629">MONTH(A1626)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1627" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1627" s="3"/>
-      <c r="B1627" s="3"/>
-      <c r="C1627" s="3"/>
-      <c r="D1627" s="3"/>
-      <c r="E1627" s="3"/>
-      <c r="F1627" s="3"/>
-      <c r="G1627" s="3"/>
-      <c r="H1627" s="3"/>
-      <c r="I1627" s="4"/>
-      <c r="J1627" s="4"/>
+      <c r="A1627" s="3" t="s">
+        <v>1438</v>
+      </c>
+      <c r="B1627" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1627" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1627" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1627" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1627" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1627" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1627" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1627" s="4">
+        <f t="shared" si="628"/>
+        <v>2025</v>
+      </c>
+      <c r="J1627" s="4">
+        <f t="shared" si="629"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1628" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1628" s="3"/>
-      <c r="B1628" s="3"/>
-      <c r="C1628" s="3"/>
-      <c r="D1628" s="3"/>
-      <c r="E1628" s="3"/>
-      <c r="F1628" s="3"/>
-      <c r="G1628" s="3"/>
-      <c r="H1628" s="3"/>
-      <c r="I1628" s="4"/>
-      <c r="J1628" s="4"/>
+      <c r="A1628" s="3" t="s">
+        <v>1439</v>
+      </c>
+      <c r="B1628" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1628" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="D1628" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1628" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1628" s="3" t="s">
+        <v>1440</v>
+      </c>
+      <c r="G1628" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1628" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1628" s="4">
+        <f t="shared" si="628"/>
+        <v>2025</v>
+      </c>
+      <c r="J1628" s="4">
+        <f t="shared" si="629"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1629" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1629" s="3"/>
-      <c r="B1629" s="3"/>
-      <c r="C1629" s="3"/>
-      <c r="D1629" s="3"/>
-      <c r="E1629" s="3"/>
-      <c r="F1629" s="3"/>
-      <c r="G1629" s="3"/>
-      <c r="H1629" s="3"/>
-      <c r="I1629" s="4"/>
-      <c r="J1629" s="4"/>
+      <c r="A1629" s="3" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B1629" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1629" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D1629" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1629" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1629" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1629" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1629" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1629" s="4">
+        <f t="shared" ref="I1629:I1630" si="630">YEAR(A1629)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1629" s="4">
+        <f t="shared" ref="J1629:J1630" si="631">MONTH(A1629)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1630" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1630" s="3"/>
-      <c r="B1630" s="3"/>
-      <c r="C1630" s="3"/>
-      <c r="D1630" s="3"/>
-      <c r="E1630" s="3"/>
-      <c r="F1630" s="3"/>
-      <c r="G1630" s="3"/>
-      <c r="H1630" s="3"/>
-      <c r="I1630" s="4"/>
-      <c r="J1630" s="4"/>
+      <c r="A1630" s="3" t="s">
+        <v>1441</v>
+      </c>
+      <c r="B1630" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="C1630" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="D1630" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1630" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1630" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1630" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1630" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1630" s="4">
+        <f t="shared" si="630"/>
+        <v>2025</v>
+      </c>
+      <c r="J1630" s="4">
+        <f t="shared" si="631"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1631" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1631" s="3"/>
-      <c r="B1631" s="3"/>
-      <c r="C1631" s="3"/>
-      <c r="D1631" s="3"/>
-      <c r="E1631" s="3"/>
-      <c r="F1631" s="3"/>
-      <c r="G1631" s="3"/>
-      <c r="H1631" s="3"/>
-      <c r="I1631" s="4"/>
-      <c r="J1631" s="4"/>
+      <c r="A1631" s="3" t="s">
+        <v>1442</v>
+      </c>
+      <c r="B1631" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1631" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1631" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1631" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1631" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1631" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1631" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1631" s="4">
+        <f t="shared" ref="I1631:I1632" si="632">YEAR(A1631)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1631" s="4">
+        <f t="shared" ref="J1631:J1632" si="633">MONTH(A1631)</f>
+        <v>7</v>
+      </c>
     </row>
     <row r="1632" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1632" s="3"/>
-      <c r="B1632" s="3"/>
-      <c r="C1632" s="3"/>
-      <c r="D1632" s="3"/>
-      <c r="E1632" s="3"/>
+      <c r="A1632" s="3" t="s">
+        <v>1443</v>
+      </c>
+      <c r="B1632" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1632" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1632" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1632" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1632" s="3"/>
-      <c r="G1632" s="3"/>
-      <c r="H1632" s="3"/>
-      <c r="I1632" s="4"/>
-      <c r="J1632" s="4"/>
+      <c r="G1632" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1632" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1632" s="4">
+        <f t="shared" si="632"/>
+        <v>2025</v>
+      </c>
+      <c r="J1632" s="4">
+        <f t="shared" si="633"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="1633" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1633" s="3"/>
-      <c r="B1633" s="3"/>
-      <c r="C1633" s="3"/>
-      <c r="D1633" s="3"/>
-      <c r="E1633" s="3"/>
-      <c r="F1633" s="3"/>
-      <c r="G1633" s="3"/>
-      <c r="H1633" s="3"/>
-      <c r="I1633" s="4"/>
-      <c r="J1633" s="4"/>
+      <c r="A1633" s="3" t="s">
+        <v>1444</v>
+      </c>
+      <c r="B1633" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1633" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1633" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1633" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1633" s="3" t="s">
+        <v>1411</v>
+      </c>
+      <c r="G1633" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1633" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1633" s="4">
+        <f t="shared" ref="I1633:I1635" si="634">YEAR(A1633)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1633" s="4">
+        <f t="shared" ref="J1633:J1635" si="635">MONTH(A1633)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1634" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1634" s="3"/>
-      <c r="B1634" s="3"/>
-      <c r="C1634" s="3"/>
-      <c r="D1634" s="3"/>
-      <c r="E1634" s="3"/>
+      <c r="A1634" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B1634" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1634" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1634" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1634" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1634" s="3"/>
-      <c r="G1634" s="3"/>
-      <c r="H1634" s="3"/>
-      <c r="I1634" s="4"/>
-      <c r="J1634" s="4"/>
+      <c r="G1634" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1634" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1634" s="4">
+        <f t="shared" si="634"/>
+        <v>2025</v>
+      </c>
+      <c r="J1634" s="4">
+        <f t="shared" si="635"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1635" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1635" s="3"/>
-      <c r="B1635" s="3"/>
-      <c r="C1635" s="3"/>
-      <c r="D1635" s="3"/>
-      <c r="E1635" s="3"/>
+      <c r="A1635" s="3" t="s">
+        <v>1445</v>
+      </c>
+      <c r="B1635" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1635" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1635" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1635" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1635" s="3"/>
-      <c r="G1635" s="3"/>
-      <c r="H1635" s="3"/>
-      <c r="I1635" s="4"/>
-      <c r="J1635" s="4"/>
+      <c r="G1635" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1635" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1635" s="4">
+        <f t="shared" si="634"/>
+        <v>2025</v>
+      </c>
+      <c r="J1635" s="4">
+        <f t="shared" si="635"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1636" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1636" s="3"/>
-      <c r="B1636" s="3"/>
-      <c r="C1636" s="3"/>
-      <c r="D1636" s="3"/>
-      <c r="E1636" s="3"/>
-      <c r="F1636" s="3"/>
-      <c r="G1636" s="3"/>
-      <c r="H1636" s="3"/>
-      <c r="I1636" s="4"/>
-      <c r="J1636" s="4"/>
+      <c r="A1636" s="3" t="s">
+        <v>1446</v>
+      </c>
+      <c r="B1636" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1636" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1636" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1636" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1636" s="3" t="s">
+        <v>1447</v>
+      </c>
+      <c r="G1636" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1636" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1636" s="4">
+        <f t="shared" ref="I1636:I1638" si="636">YEAR(A1636)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1636" s="4">
+        <f t="shared" ref="J1636:J1638" si="637">MONTH(A1636)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1637" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1637" s="3"/>
-      <c r="B1637" s="3"/>
-      <c r="C1637" s="3"/>
-      <c r="D1637" s="3"/>
-      <c r="E1637" s="3"/>
+      <c r="A1637" s="3" t="s">
+        <v>1448</v>
+      </c>
+      <c r="B1637" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1637" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1637" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1637" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1637" s="3"/>
-      <c r="G1637" s="3"/>
-      <c r="H1637" s="3"/>
-      <c r="I1637" s="4"/>
-      <c r="J1637" s="4"/>
+      <c r="G1637" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1637" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1637" s="4">
+        <f t="shared" si="636"/>
+        <v>2025</v>
+      </c>
+      <c r="J1637" s="4">
+        <f t="shared" si="637"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1638" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1638" s="3"/>
-      <c r="B1638" s="3"/>
-      <c r="C1638" s="3"/>
-      <c r="D1638" s="3"/>
-      <c r="E1638" s="3"/>
+      <c r="A1638" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B1638" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1638" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1638" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1638" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1638" s="3"/>
-      <c r="G1638" s="3"/>
-      <c r="H1638" s="3"/>
-      <c r="I1638" s="4"/>
-      <c r="J1638" s="4"/>
+      <c r="G1638" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1638" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1638" s="4">
+        <f t="shared" si="636"/>
+        <v>2025</v>
+      </c>
+      <c r="J1638" s="4">
+        <f t="shared" si="637"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1639" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1639" s="3"/>
-      <c r="B1639" s="3"/>
-      <c r="C1639" s="3"/>
-      <c r="D1639" s="3"/>
-      <c r="E1639" s="3"/>
+      <c r="A1639" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B1639" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="C1639" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1639" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1639" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1639" s="3"/>
-      <c r="G1639" s="3"/>
-      <c r="H1639" s="3"/>
-      <c r="I1639" s="4"/>
-      <c r="J1639" s="4"/>
+      <c r="G1639" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1639" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1639" s="4">
+        <f t="shared" ref="I1639:I1640" si="638">YEAR(A1639)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1639" s="4">
+        <f t="shared" ref="J1639:J1640" si="639">MONTH(A1639)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1640" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1640" s="3"/>
-      <c r="B1640" s="3"/>
-      <c r="C1640" s="3"/>
-      <c r="D1640" s="3"/>
-      <c r="E1640" s="3"/>
+      <c r="A1640" s="3" t="s">
+        <v>1449</v>
+      </c>
+      <c r="B1640" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C1640" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1640" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1640" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1640" s="3"/>
-      <c r="G1640" s="3"/>
-      <c r="H1640" s="3"/>
-      <c r="I1640" s="4"/>
-      <c r="J1640" s="4"/>
+      <c r="G1640" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1640" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1640" s="4">
+        <f t="shared" si="638"/>
+        <v>2025</v>
+      </c>
+      <c r="J1640" s="4">
+        <f t="shared" si="639"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1641" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1641" s="3"/>
-      <c r="B1641" s="3"/>
-      <c r="C1641" s="3"/>
-      <c r="D1641" s="3"/>
-      <c r="E1641" s="3"/>
+      <c r="A1641" s="3" t="s">
+        <v>1450</v>
+      </c>
+      <c r="B1641" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="C1641" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1641" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1641" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1641" s="3"/>
-      <c r="G1641" s="3"/>
-      <c r="H1641" s="3"/>
-      <c r="I1641" s="4"/>
-      <c r="J1641" s="4"/>
+      <c r="G1641" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1641" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1641" s="4">
+        <f t="shared" ref="I1641:I1644" si="640">YEAR(A1641)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1641" s="4">
+        <f t="shared" ref="J1641:J1644" si="641">MONTH(A1641)</f>
+        <v>8</v>
+      </c>
     </row>
     <row r="1642" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1642" s="3"/>
-      <c r="B1642" s="3"/>
-      <c r="C1642" s="3"/>
-      <c r="D1642" s="3"/>
-      <c r="E1642" s="3"/>
+      <c r="A1642" s="3" t="s">
+        <v>1451</v>
+      </c>
+      <c r="B1642" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1642" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1642" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="E1642" s="3" t="s">
+        <v>140</v>
+      </c>
       <c r="F1642" s="3"/>
-      <c r="G1642" s="3"/>
-      <c r="H1642" s="3"/>
-      <c r="I1642" s="4"/>
-      <c r="J1642" s="4"/>
+      <c r="G1642" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1642" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1642" s="4">
+        <f t="shared" si="640"/>
+        <v>2025</v>
+      </c>
+      <c r="J1642" s="4">
+        <f t="shared" si="641"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1643" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1643" s="3"/>
-      <c r="B1643" s="3"/>
-      <c r="C1643" s="3"/>
-      <c r="D1643" s="3"/>
-      <c r="E1643" s="3"/>
-      <c r="F1643" s="3"/>
-      <c r="G1643" s="3"/>
-      <c r="H1643" s="3"/>
-      <c r="I1643" s="4"/>
-      <c r="J1643" s="4"/>
+      <c r="A1643" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B1643" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1643" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1643" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="E1643" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1643" s="3" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G1643" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1643" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1643" s="4">
+        <f t="shared" si="640"/>
+        <v>2025</v>
+      </c>
+      <c r="J1643" s="4">
+        <f t="shared" si="641"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1644" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1644" s="3"/>
-      <c r="B1644" s="3"/>
-      <c r="C1644" s="3"/>
-      <c r="D1644" s="3"/>
-      <c r="E1644" s="3"/>
-      <c r="F1644" s="3"/>
-      <c r="G1644" s="3"/>
-      <c r="H1644" s="3"/>
-      <c r="I1644" s="4"/>
-      <c r="J1644" s="4"/>
+      <c r="A1644" s="3" t="s">
+        <v>1452</v>
+      </c>
+      <c r="B1644" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1644" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1644" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1644" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="F1644" s="3" t="s">
+        <v>1453</v>
+      </c>
+      <c r="G1644" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1644" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1644" s="4">
+        <f t="shared" si="640"/>
+        <v>2025</v>
+      </c>
+      <c r="J1644" s="4">
+        <f t="shared" si="641"/>
+        <v>8</v>
+      </c>
     </row>
     <row r="1645" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1645" s="3"/>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-12-09.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13575" uniqueCount="1514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13858" uniqueCount="1532">
   <si>
     <t>Year</t>
   </si>
@@ -4567,6 +4567,60 @@
   </si>
   <si>
     <t>2025-11-16</t>
+  </si>
+  <si>
+    <t>2025-11-17</t>
+  </si>
+  <si>
+    <t>2025-11-18</t>
+  </si>
+  <si>
+    <t>2025-11-20</t>
+  </si>
+  <si>
+    <t>2025-11-22</t>
+  </si>
+  <si>
+    <t>2025-11-23</t>
+  </si>
+  <si>
+    <t>2025-11-25</t>
+  </si>
+  <si>
+    <t>2025-11-26</t>
+  </si>
+  <si>
+    <t>2025-11-27</t>
+  </si>
+  <si>
+    <t>2025-11-28</t>
+  </si>
+  <si>
+    <t>2025-11-30</t>
+  </si>
+  <si>
+    <t>2025-12-01</t>
+  </si>
+  <si>
+    <t>2025-12-02</t>
+  </si>
+  <si>
+    <t>2025-12-03</t>
+  </si>
+  <si>
+    <t>2025-12-04</t>
+  </si>
+  <si>
+    <t>2025-12-05</t>
+  </si>
+  <si>
+    <t>2025-12-07</t>
+  </si>
+  <si>
+    <t>2025-12-08</t>
+  </si>
+  <si>
+    <t>2025-12-09</t>
   </si>
 </sst>
 </file>
@@ -4975,11 +5029,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1768"/>
+  <dimension ref="A1:J1811"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1630" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1659" sqref="D1659"/>
+      <pane ySplit="1" topLeftCell="A1760" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E1787" sqref="E1787"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -63543,289 +63597,1593 @@
         <v>280</v>
       </c>
       <c r="I1745" s="4">
-        <f t="shared" ref="I1745" si="732">YEAR(A1745)</f>
+        <f t="shared" ref="I1745:I1747" si="732">YEAR(A1745)</f>
         <v>2025</v>
       </c>
       <c r="J1745" s="4">
-        <f t="shared" ref="J1745" si="733">MONTH(A1745)</f>
+        <f t="shared" ref="J1745:J1747" si="733">MONTH(A1745)</f>
         <v>11</v>
       </c>
     </row>
     <row r="1746" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1746" s="3"/>
-      <c r="B1746" s="3"/>
-      <c r="C1746" s="3"/>
-      <c r="D1746" s="3"/>
-      <c r="E1746" s="3"/>
+      <c r="A1746" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B1746" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="C1746" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1746" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="E1746" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1746" s="3"/>
-      <c r="G1746" s="3"/>
-      <c r="H1746" s="3"/>
-      <c r="I1746" s="4"/>
-      <c r="J1746" s="4"/>
+      <c r="G1746" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1746" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1746" s="4">
+        <f t="shared" si="732"/>
+        <v>2025</v>
+      </c>
+      <c r="J1746" s="4">
+        <f t="shared" si="733"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1747" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1747" s="3"/>
-      <c r="B1747" s="3"/>
-      <c r="C1747" s="3"/>
-      <c r="D1747" s="3"/>
-      <c r="E1747" s="3"/>
+      <c r="A1747" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B1747" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1747" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1747" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1747" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1747" s="3"/>
-      <c r="G1747" s="3"/>
-      <c r="H1747" s="3"/>
-      <c r="I1747" s="4"/>
-      <c r="J1747" s="4"/>
+      <c r="G1747" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1747" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1747" s="4">
+        <f t="shared" si="732"/>
+        <v>2025</v>
+      </c>
+      <c r="J1747" s="4">
+        <f t="shared" si="733"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1748" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1748" s="3"/>
-      <c r="B1748" s="3"/>
-      <c r="C1748" s="3"/>
-      <c r="D1748" s="3"/>
-      <c r="E1748" s="3"/>
+      <c r="A1748" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="B1748" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1748" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1748" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1748" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1748" s="3"/>
-      <c r="G1748" s="3"/>
-      <c r="H1748" s="3"/>
-      <c r="I1748" s="4"/>
-      <c r="J1748" s="4"/>
+      <c r="G1748" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1748" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1748" s="4">
+        <f t="shared" ref="I1748" si="734">YEAR(A1748)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1748" s="4">
+        <f t="shared" ref="J1748" si="735">MONTH(A1748)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1749" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1749" s="3"/>
-      <c r="B1749" s="3"/>
-      <c r="C1749" s="3"/>
-      <c r="D1749" s="3"/>
-      <c r="E1749" s="3"/>
+      <c r="A1749" s="3" t="s">
+        <v>1515</v>
+      </c>
+      <c r="B1749" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1749" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1749" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1749" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1749" s="3"/>
-      <c r="G1749" s="3"/>
-      <c r="H1749" s="3"/>
-      <c r="I1749" s="4"/>
-      <c r="J1749" s="4"/>
+      <c r="G1749" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1749" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1749" s="4">
+        <f t="shared" ref="I1749" si="736">YEAR(A1749)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1749" s="4">
+        <f t="shared" ref="J1749" si="737">MONTH(A1749)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1750" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1750" s="3"/>
-      <c r="B1750" s="3"/>
-      <c r="C1750" s="3"/>
-      <c r="D1750" s="3"/>
-      <c r="E1750" s="3"/>
+      <c r="A1750" s="3" t="s">
+        <v>1516</v>
+      </c>
+      <c r="B1750" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1750" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1750" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1750" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1750" s="3"/>
-      <c r="G1750" s="3"/>
-      <c r="H1750" s="3"/>
-      <c r="I1750" s="4"/>
-      <c r="J1750" s="4"/>
+      <c r="G1750" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1750" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1750" s="4">
+        <f t="shared" ref="I1750:I1751" si="738">YEAR(A1750)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1750" s="4">
+        <f t="shared" ref="J1750:J1751" si="739">MONTH(A1750)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1751" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1751" s="3"/>
-      <c r="B1751" s="3"/>
-      <c r="C1751" s="3"/>
-      <c r="D1751" s="3"/>
-      <c r="E1751" s="3"/>
+      <c r="A1751" s="3" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B1751" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1751" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1751" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1751" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1751" s="3"/>
-      <c r="G1751" s="3"/>
-      <c r="H1751" s="3"/>
-      <c r="I1751" s="4"/>
-      <c r="J1751" s="4"/>
+      <c r="G1751" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1751" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1751" s="4">
+        <f t="shared" si="738"/>
+        <v>2025</v>
+      </c>
+      <c r="J1751" s="4">
+        <f t="shared" si="739"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1752" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1752" s="3"/>
-      <c r="B1752" s="3"/>
-      <c r="C1752" s="3"/>
-      <c r="D1752" s="3"/>
-      <c r="E1752" s="3"/>
+      <c r="A1752" s="3" t="s">
+        <v>1517</v>
+      </c>
+      <c r="B1752" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1752" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1752" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1752" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1752" s="3"/>
-      <c r="G1752" s="3"/>
-      <c r="H1752" s="3"/>
-      <c r="I1752" s="4"/>
-      <c r="J1752" s="4"/>
+      <c r="G1752" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1752" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1752" s="4">
+        <f t="shared" ref="I1752:I1753" si="740">YEAR(A1752)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1752" s="4">
+        <f t="shared" ref="J1752:J1753" si="741">MONTH(A1752)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1753" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1753" s="3"/>
-      <c r="B1753" s="3"/>
-      <c r="C1753" s="3"/>
-      <c r="D1753" s="3"/>
-      <c r="E1753" s="3"/>
+      <c r="A1753" s="3" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B1753" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1753" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="D1753" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1753" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1753" s="3"/>
-      <c r="G1753" s="3"/>
-      <c r="H1753" s="3"/>
-      <c r="I1753" s="4"/>
-      <c r="J1753" s="4"/>
+      <c r="G1753" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1753" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1753" s="4">
+        <f t="shared" si="740"/>
+        <v>2025</v>
+      </c>
+      <c r="J1753" s="4">
+        <f t="shared" si="741"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1754" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1754" s="3"/>
-      <c r="B1754" s="3"/>
-      <c r="C1754" s="3"/>
-      <c r="D1754" s="3"/>
-      <c r="E1754" s="3"/>
+      <c r="A1754" s="3" t="s">
+        <v>1518</v>
+      </c>
+      <c r="B1754" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1754" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1754" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1754" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1754" s="3"/>
-      <c r="G1754" s="3"/>
-      <c r="H1754" s="3"/>
-      <c r="I1754" s="4"/>
-      <c r="J1754" s="4"/>
+      <c r="G1754" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1754" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1754" s="4">
+        <f t="shared" ref="I1754" si="742">YEAR(A1754)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1754" s="4">
+        <f t="shared" ref="J1754" si="743">MONTH(A1754)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1755" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1755" s="3"/>
-      <c r="B1755" s="3"/>
-      <c r="C1755" s="3"/>
-      <c r="D1755" s="3"/>
-      <c r="E1755" s="3"/>
-      <c r="F1755" s="3"/>
-      <c r="G1755" s="3"/>
-      <c r="H1755" s="3"/>
-      <c r="I1755" s="4"/>
-      <c r="J1755" s="4"/>
+      <c r="A1755" s="3" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B1755" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1755" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D1755" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="E1755" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1755" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1755" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1755" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1755" s="4">
+        <f>YEAR(A1755)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1755" s="4">
+        <f>MONTH(A1755)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1756" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1756" s="3"/>
-      <c r="B1756" s="3"/>
-      <c r="C1756" s="3"/>
-      <c r="D1756" s="3"/>
-      <c r="E1756" s="3"/>
+      <c r="A1756" s="3" t="s">
+        <v>1519</v>
+      </c>
+      <c r="B1756" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1756" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1756" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1756" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1756" s="3"/>
-      <c r="G1756" s="3"/>
-      <c r="H1756" s="3"/>
-      <c r="I1756" s="4"/>
-      <c r="J1756" s="4"/>
+      <c r="G1756" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1756" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1756" s="4">
+        <f t="shared" ref="I1756:I1757" si="744">YEAR(A1756)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1756" s="4">
+        <f t="shared" ref="J1756:J1757" si="745">MONTH(A1756)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1757" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1757" s="3"/>
-      <c r="B1757" s="3"/>
-      <c r="C1757" s="3"/>
-      <c r="D1757" s="3"/>
-      <c r="E1757" s="3"/>
+      <c r="A1757" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B1757" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1757" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1757" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1757" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1757" s="3"/>
-      <c r="G1757" s="3"/>
-      <c r="H1757" s="3"/>
-      <c r="I1757" s="4"/>
-      <c r="J1757" s="4"/>
+      <c r="G1757" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1757" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1757" s="4">
+        <f t="shared" si="744"/>
+        <v>2025</v>
+      </c>
+      <c r="J1757" s="4">
+        <f t="shared" si="745"/>
+        <v>11</v>
+      </c>
     </row>
     <row r="1758" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1758" s="3"/>
-      <c r="B1758" s="3"/>
-      <c r="C1758" s="3"/>
-      <c r="D1758" s="3"/>
-      <c r="E1758" s="3"/>
+      <c r="A1758" s="3" t="s">
+        <v>1520</v>
+      </c>
+      <c r="B1758" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1758" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1758" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1758" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1758" s="3"/>
-      <c r="G1758" s="3"/>
-      <c r="H1758" s="3"/>
-      <c r="I1758" s="4"/>
-      <c r="J1758" s="4"/>
+      <c r="G1758" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1758" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1758" s="4">
+        <f t="shared" ref="I1758" si="746">YEAR(A1758)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1758" s="4">
+        <f t="shared" ref="J1758" si="747">MONTH(A1758)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1759" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1759" s="3"/>
-      <c r="B1759" s="3"/>
-      <c r="C1759" s="3"/>
-      <c r="D1759" s="3"/>
-      <c r="E1759" s="3"/>
+      <c r="A1759" s="3" t="s">
+        <v>1521</v>
+      </c>
+      <c r="B1759" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="C1759" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="D1759" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1759" s="3" t="s">
+        <v>151</v>
+      </c>
       <c r="F1759" s="3"/>
-      <c r="G1759" s="3"/>
-      <c r="H1759" s="3"/>
-      <c r="I1759" s="4"/>
-      <c r="J1759" s="4"/>
+      <c r="G1759" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="H1759" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1759" s="4">
+        <f t="shared" ref="I1759" si="748">YEAR(A1759)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1759" s="4">
+        <f t="shared" ref="J1759" si="749">MONTH(A1759)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1760" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1760" s="3"/>
-      <c r="B1760" s="3"/>
-      <c r="C1760" s="3"/>
-      <c r="D1760" s="3"/>
-      <c r="E1760" s="3"/>
-      <c r="F1760" s="3"/>
-      <c r="G1760" s="3"/>
-      <c r="H1760" s="3"/>
-      <c r="I1760" s="4"/>
-      <c r="J1760" s="4"/>
+      <c r="A1760" s="3" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B1760" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1760" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D1760" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1760" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1760" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1760" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1760" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1760" s="4">
+        <f>YEAR(A1760)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1760" s="4">
+        <f>MONTH(A1760)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1761" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1761" s="3"/>
-      <c r="B1761" s="3"/>
-      <c r="C1761" s="3"/>
-      <c r="D1761" s="3"/>
-      <c r="E1761" s="3"/>
-      <c r="F1761" s="3"/>
-      <c r="G1761" s="3"/>
-      <c r="H1761" s="3"/>
-      <c r="I1761" s="4"/>
-      <c r="J1761" s="4"/>
+      <c r="A1761" s="3" t="s">
+        <v>1522</v>
+      </c>
+      <c r="B1761" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C1761" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1761" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="E1761" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1761" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1761" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1761" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1761" s="4">
+        <f>YEAR(A1761)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1761" s="4">
+        <f>MONTH(A1761)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1762" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1762" s="3"/>
-      <c r="B1762" s="3"/>
-      <c r="C1762" s="3"/>
-      <c r="D1762" s="3"/>
-      <c r="E1762" s="3"/>
-      <c r="F1762" s="3"/>
-      <c r="G1762" s="3"/>
-      <c r="H1762" s="3"/>
-      <c r="I1762" s="4"/>
-      <c r="J1762" s="4"/>
+      <c r="A1762" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1762" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1762" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D1762" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1762" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1762" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1762" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1762" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1762" s="4">
+        <f>YEAR(A1762)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1762" s="4">
+        <f>MONTH(A1762)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1763" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1763" s="3"/>
-      <c r="B1763" s="3"/>
-      <c r="C1763" s="3"/>
-      <c r="D1763" s="3"/>
-      <c r="E1763" s="3"/>
-      <c r="F1763" s="3"/>
-      <c r="G1763" s="3"/>
-      <c r="H1763" s="3"/>
-      <c r="I1763" s="4"/>
-      <c r="J1763" s="4"/>
+      <c r="A1763" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1763" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1763" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1763" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1763" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1763" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1763" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1763" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1763" s="4">
+        <f>YEAR(A1763)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1763" s="4">
+        <f>MONTH(A1763)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1764" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1764" s="3"/>
-      <c r="B1764" s="3"/>
-      <c r="C1764" s="3"/>
-      <c r="D1764" s="3"/>
-      <c r="E1764" s="3"/>
-      <c r="F1764" s="3"/>
-      <c r="G1764" s="3"/>
-      <c r="H1764" s="3"/>
-      <c r="I1764" s="4"/>
-      <c r="J1764" s="4"/>
+      <c r="A1764" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1764" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1764" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D1764" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1764" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1764" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1764" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1764" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1764" s="4">
+        <f>YEAR(A1764)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1764" s="4">
+        <f>MONTH(A1764)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1765" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1765" s="3"/>
-      <c r="B1765" s="3"/>
-      <c r="C1765" s="3"/>
-      <c r="D1765" s="3"/>
-      <c r="E1765" s="3"/>
-      <c r="F1765" s="3"/>
-      <c r="G1765" s="3"/>
-      <c r="H1765" s="3"/>
-      <c r="I1765" s="4"/>
-      <c r="J1765" s="4"/>
+      <c r="A1765" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1765" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1765" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1765" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1765" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1765" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1765" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1765" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1765" s="4">
+        <f>YEAR(A1765)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1765" s="4">
+        <f>MONTH(A1765)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1766" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1766" s="3"/>
-      <c r="B1766" s="3"/>
-      <c r="C1766" s="3"/>
-      <c r="D1766" s="3"/>
-      <c r="E1766" s="3"/>
-      <c r="F1766" s="3"/>
-      <c r="G1766" s="3"/>
-      <c r="H1766" s="3"/>
-      <c r="I1766" s="4"/>
-      <c r="J1766" s="4"/>
+      <c r="A1766" s="3" t="s">
+        <v>1523</v>
+      </c>
+      <c r="B1766" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1766" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1766" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1766" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1766" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1766" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1766" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1766" s="4">
+        <f>YEAR(A1766)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1766" s="4">
+        <f>MONTH(A1766)</f>
+        <v>11</v>
+      </c>
     </row>
     <row r="1767" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1767" s="3"/>
-      <c r="B1767" s="3"/>
-      <c r="C1767" s="3"/>
-      <c r="D1767" s="3"/>
-      <c r="E1767" s="3"/>
-      <c r="F1767" s="3"/>
-      <c r="G1767" s="3"/>
-      <c r="H1767" s="3"/>
-      <c r="I1767" s="4"/>
-      <c r="J1767" s="4"/>
+      <c r="A1767" s="3" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B1767" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="C1767" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="D1767" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1767" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1767" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1767" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1767" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1767" s="4">
+        <f>YEAR(A1767)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1767" s="4">
+        <f>MONTH(A1767)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1768" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1768" s="3"/>
-      <c r="B1768" s="3"/>
-      <c r="C1768" s="3"/>
-      <c r="D1768" s="3"/>
-      <c r="E1768" s="3"/>
-      <c r="F1768" s="3"/>
-      <c r="G1768" s="3"/>
-      <c r="H1768" s="3"/>
-      <c r="I1768" s="4"/>
-      <c r="J1768" s="4"/>
+      <c r="A1768" s="3" t="s">
+        <v>1524</v>
+      </c>
+      <c r="B1768" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1768" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="D1768" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1768" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1768" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1768" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1768" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1768" s="4">
+        <f>YEAR(A1768)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1768" s="4">
+        <f>MONTH(A1768)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1769" s="3" t="s">
+        <v>1525</v>
+      </c>
+      <c r="B1769" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="C1769" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1769" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1769" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1769" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1769" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1769" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1769" s="4">
+        <f>YEAR(A1769)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1769" s="4">
+        <f>MONTH(A1769)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1770" s="3" t="s">
+        <v>1526</v>
+      </c>
+      <c r="B1770" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1770" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1770" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1770" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1770" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1770" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1770" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1770" s="4">
+        <f>YEAR(A1770)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1770" s="4">
+        <f>MONTH(A1770)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1771" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B1771" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C1771" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D1771" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="E1771" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1771" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1771" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1771" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1771" s="4">
+        <f>YEAR(A1771)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1771" s="4">
+        <f>MONTH(A1771)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1772" s="3" t="s">
+        <v>1527</v>
+      </c>
+      <c r="B1772" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1772" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1772" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1772" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1772" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1772" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1772" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1772" s="4">
+        <f>YEAR(A1772)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1772" s="4">
+        <f>MONTH(A1772)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1773" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1773" s="3" t="s">
+        <v>1528</v>
+      </c>
+      <c r="B1773" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1773" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1773" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1773" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1773" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1773" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1773" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1773" s="4">
+        <f>YEAR(A1773)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1773" s="4">
+        <f>MONTH(A1773)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1774" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B1774" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="C1774" s="3" t="s">
+        <v>333</v>
+      </c>
+      <c r="D1774" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1774" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1774" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1774" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1774" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1774" s="4">
+        <f>YEAR(A1774)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1774" s="4">
+        <f>MONTH(A1774)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1775" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B1775" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1775" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="D1775" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="E1775" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1775" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1775" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1775" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1775" s="4">
+        <f>YEAR(A1775)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1775" s="4">
+        <f>MONTH(A1775)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1776" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B1776" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="C1776" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1776" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1776" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1776" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1776" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1776" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1776" s="4">
+        <f>YEAR(A1776)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1776" s="4">
+        <f>MONTH(A1776)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1777" s="3" t="s">
+        <v>1529</v>
+      </c>
+      <c r="B1777" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1777" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1777" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1777" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1777" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1777" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1777" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1777" s="4">
+        <f>YEAR(A1777)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1777" s="4">
+        <f>MONTH(A1777)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1778" s="3" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B1778" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="C1778" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1778" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="E1778" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1778" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1778" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1778" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1778" s="4">
+        <f>YEAR(A1778)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1778" s="4">
+        <f>MONTH(A1778)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1779" s="3" t="s">
+        <v>1530</v>
+      </c>
+      <c r="B1779" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C1779" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1779" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1779" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1779" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1779" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1779" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1779" s="4">
+        <f>YEAR(A1779)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1779" s="4">
+        <f>MONTH(A1779)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1780" s="3" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B1780" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1780" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1780" s="3" t="s">
+        <v>1305</v>
+      </c>
+      <c r="E1780" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1780" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1780" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1780" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1780" s="4">
+        <f>YEAR(A1780)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1780" s="4">
+        <f>MONTH(A1780)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1781" s="3" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B1781" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C1781" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1781" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1781" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1781" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1781" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1781" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1781" s="4">
+        <f>YEAR(A1781)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1781" s="4">
+        <f>MONTH(A1781)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1782" s="3" t="s">
+        <v>1531</v>
+      </c>
+      <c r="B1782" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1782" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="D1782" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1782" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1782" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1782" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1782" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1782" s="4">
+        <f>YEAR(A1782)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1782" s="4">
+        <f>MONTH(A1782)</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1783" s="3"/>
+      <c r="B1783" s="3"/>
+      <c r="C1783" s="3"/>
+      <c r="D1783" s="3"/>
+      <c r="E1783" s="3"/>
+      <c r="F1783" s="3"/>
+      <c r="G1783" s="3"/>
+      <c r="H1783" s="3"/>
+      <c r="I1783" s="4"/>
+      <c r="J1783" s="4"/>
+    </row>
+    <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1784" s="3"/>
+      <c r="B1784" s="3"/>
+      <c r="C1784" s="3"/>
+      <c r="D1784" s="3"/>
+      <c r="E1784" s="3"/>
+      <c r="F1784" s="3"/>
+      <c r="G1784" s="3"/>
+      <c r="H1784" s="3"/>
+      <c r="I1784" s="4"/>
+      <c r="J1784" s="4"/>
+    </row>
+    <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1785" s="3"/>
+      <c r="B1785" s="3"/>
+      <c r="C1785" s="3"/>
+      <c r="D1785" s="3"/>
+      <c r="E1785" s="3"/>
+      <c r="F1785" s="3"/>
+      <c r="G1785" s="3"/>
+      <c r="H1785" s="3"/>
+      <c r="I1785" s="4"/>
+      <c r="J1785" s="4"/>
+    </row>
+    <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1786" s="3"/>
+      <c r="B1786" s="3"/>
+      <c r="C1786" s="3"/>
+      <c r="D1786" s="3"/>
+      <c r="E1786" s="3"/>
+      <c r="F1786" s="3"/>
+      <c r="G1786" s="3"/>
+      <c r="H1786" s="3"/>
+      <c r="I1786" s="4"/>
+      <c r="J1786" s="4"/>
+    </row>
+    <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1787" s="3"/>
+      <c r="B1787" s="3"/>
+      <c r="C1787" s="3"/>
+      <c r="D1787" s="3"/>
+      <c r="E1787" s="3"/>
+      <c r="F1787" s="3"/>
+      <c r="G1787" s="3"/>
+      <c r="H1787" s="3"/>
+      <c r="I1787" s="4"/>
+      <c r="J1787" s="4"/>
+    </row>
+    <row r="1788" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1788" s="3"/>
+      <c r="B1788" s="3"/>
+      <c r="C1788" s="3"/>
+      <c r="D1788" s="3"/>
+      <c r="E1788" s="3"/>
+      <c r="F1788" s="3"/>
+      <c r="G1788" s="3"/>
+      <c r="H1788" s="3"/>
+      <c r="I1788" s="4"/>
+      <c r="J1788" s="4"/>
+    </row>
+    <row r="1789" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1789" s="3"/>
+      <c r="B1789" s="3"/>
+      <c r="C1789" s="3"/>
+      <c r="D1789" s="3"/>
+      <c r="E1789" s="3"/>
+      <c r="F1789" s="3"/>
+      <c r="G1789" s="3"/>
+      <c r="H1789" s="3"/>
+      <c r="I1789" s="4"/>
+      <c r="J1789" s="4"/>
+    </row>
+    <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1790" s="3"/>
+      <c r="B1790" s="3"/>
+      <c r="C1790" s="3"/>
+      <c r="D1790" s="3"/>
+      <c r="E1790" s="3"/>
+      <c r="F1790" s="3"/>
+      <c r="G1790" s="3"/>
+      <c r="H1790" s="3"/>
+      <c r="I1790" s="4"/>
+      <c r="J1790" s="4"/>
+    </row>
+    <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1791" s="3"/>
+      <c r="B1791" s="3"/>
+      <c r="C1791" s="3"/>
+      <c r="D1791" s="3"/>
+      <c r="E1791" s="3"/>
+      <c r="F1791" s="3"/>
+      <c r="G1791" s="3"/>
+      <c r="H1791" s="3"/>
+      <c r="I1791" s="4"/>
+      <c r="J1791" s="4"/>
+    </row>
+    <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1792" s="3"/>
+      <c r="B1792" s="3"/>
+      <c r="C1792" s="3"/>
+      <c r="D1792" s="3"/>
+      <c r="E1792" s="3"/>
+      <c r="F1792" s="3"/>
+      <c r="G1792" s="3"/>
+      <c r="H1792" s="3"/>
+      <c r="I1792" s="4"/>
+      <c r="J1792" s="4"/>
+    </row>
+    <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1793" s="3"/>
+      <c r="B1793" s="3"/>
+      <c r="C1793" s="3"/>
+      <c r="D1793" s="3"/>
+      <c r="E1793" s="3"/>
+      <c r="F1793" s="3"/>
+      <c r="G1793" s="3"/>
+      <c r="H1793" s="3"/>
+      <c r="I1793" s="4"/>
+      <c r="J1793" s="4"/>
+    </row>
+    <row r="1794" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1794" s="3"/>
+      <c r="B1794" s="3"/>
+      <c r="C1794" s="3"/>
+      <c r="D1794" s="3"/>
+      <c r="E1794" s="3"/>
+      <c r="F1794" s="3"/>
+      <c r="G1794" s="3"/>
+      <c r="H1794" s="3"/>
+      <c r="I1794" s="4"/>
+      <c r="J1794" s="4"/>
+    </row>
+    <row r="1795" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1795" s="3"/>
+      <c r="B1795" s="3"/>
+      <c r="C1795" s="3"/>
+      <c r="D1795" s="3"/>
+      <c r="E1795" s="3"/>
+      <c r="F1795" s="3"/>
+      <c r="G1795" s="3"/>
+      <c r="H1795" s="3"/>
+      <c r="I1795" s="4"/>
+      <c r="J1795" s="4"/>
+    </row>
+    <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1796" s="3"/>
+      <c r="B1796" s="3"/>
+      <c r="C1796" s="3"/>
+      <c r="D1796" s="3"/>
+      <c r="E1796" s="3"/>
+      <c r="F1796" s="3"/>
+      <c r="G1796" s="3"/>
+      <c r="H1796" s="3"/>
+      <c r="I1796" s="4"/>
+      <c r="J1796" s="4"/>
+    </row>
+    <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1797" s="3"/>
+      <c r="B1797" s="3"/>
+      <c r="C1797" s="3"/>
+      <c r="D1797" s="3"/>
+      <c r="E1797" s="3"/>
+      <c r="F1797" s="3"/>
+      <c r="G1797" s="3"/>
+      <c r="H1797" s="3"/>
+      <c r="I1797" s="4"/>
+      <c r="J1797" s="4"/>
+    </row>
+    <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1798" s="3"/>
+      <c r="B1798" s="3"/>
+      <c r="C1798" s="3"/>
+      <c r="D1798" s="3"/>
+      <c r="E1798" s="3"/>
+      <c r="F1798" s="3"/>
+      <c r="G1798" s="3"/>
+      <c r="H1798" s="3"/>
+      <c r="I1798" s="4"/>
+      <c r="J1798" s="4"/>
+    </row>
+    <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1799" s="3"/>
+      <c r="B1799" s="3"/>
+      <c r="C1799" s="3"/>
+      <c r="D1799" s="3"/>
+      <c r="E1799" s="3"/>
+      <c r="F1799" s="3"/>
+      <c r="G1799" s="3"/>
+      <c r="H1799" s="3"/>
+      <c r="I1799" s="4"/>
+      <c r="J1799" s="4"/>
+    </row>
+    <row r="1800" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1800" s="3"/>
+      <c r="B1800" s="3"/>
+      <c r="C1800" s="3"/>
+      <c r="D1800" s="3"/>
+      <c r="E1800" s="3"/>
+      <c r="F1800" s="3"/>
+      <c r="G1800" s="3"/>
+      <c r="H1800" s="3"/>
+      <c r="I1800" s="4"/>
+      <c r="J1800" s="4"/>
+    </row>
+    <row r="1801" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1801" s="3"/>
+      <c r="B1801" s="3"/>
+      <c r="C1801" s="3"/>
+      <c r="D1801" s="3"/>
+      <c r="E1801" s="3"/>
+      <c r="F1801" s="3"/>
+      <c r="G1801" s="3"/>
+      <c r="H1801" s="3"/>
+      <c r="I1801" s="4"/>
+      <c r="J1801" s="4"/>
+    </row>
+    <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1802" s="3"/>
+      <c r="B1802" s="3"/>
+      <c r="C1802" s="3"/>
+      <c r="D1802" s="3"/>
+      <c r="E1802" s="3"/>
+      <c r="F1802" s="3"/>
+      <c r="G1802" s="3"/>
+      <c r="H1802" s="3"/>
+      <c r="I1802" s="4"/>
+      <c r="J1802" s="4"/>
+    </row>
+    <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1803" s="3"/>
+      <c r="B1803" s="3"/>
+      <c r="C1803" s="3"/>
+      <c r="D1803" s="3"/>
+      <c r="E1803" s="3"/>
+      <c r="F1803" s="3"/>
+      <c r="G1803" s="3"/>
+      <c r="H1803" s="3"/>
+      <c r="I1803" s="4"/>
+      <c r="J1803" s="4"/>
+    </row>
+    <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1804" s="3"/>
+      <c r="B1804" s="3"/>
+      <c r="C1804" s="3"/>
+      <c r="D1804" s="3"/>
+      <c r="E1804" s="3"/>
+      <c r="F1804" s="3"/>
+      <c r="G1804" s="3"/>
+      <c r="H1804" s="3"/>
+      <c r="I1804" s="4"/>
+      <c r="J1804" s="4"/>
+    </row>
+    <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1805" s="3"/>
+      <c r="B1805" s="3"/>
+      <c r="C1805" s="3"/>
+      <c r="D1805" s="3"/>
+      <c r="E1805" s="3"/>
+      <c r="F1805" s="3"/>
+      <c r="G1805" s="3"/>
+      <c r="H1805" s="3"/>
+      <c r="I1805" s="4"/>
+      <c r="J1805" s="4"/>
+    </row>
+    <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1806" s="3"/>
+      <c r="B1806" s="3"/>
+      <c r="C1806" s="3"/>
+      <c r="D1806" s="3"/>
+      <c r="E1806" s="3"/>
+      <c r="F1806" s="3"/>
+      <c r="G1806" s="3"/>
+      <c r="H1806" s="3"/>
+      <c r="I1806" s="4"/>
+      <c r="J1806" s="4"/>
+    </row>
+    <row r="1807" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1807" s="3"/>
+      <c r="B1807" s="3"/>
+      <c r="C1807" s="3"/>
+      <c r="D1807" s="3"/>
+      <c r="E1807" s="3"/>
+      <c r="F1807" s="3"/>
+      <c r="G1807" s="3"/>
+      <c r="H1807" s="3"/>
+      <c r="I1807" s="4"/>
+      <c r="J1807" s="4"/>
+    </row>
+    <row r="1808" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1808" s="3"/>
+      <c r="B1808" s="3"/>
+      <c r="C1808" s="3"/>
+      <c r="D1808" s="3"/>
+      <c r="E1808" s="3"/>
+      <c r="F1808" s="3"/>
+      <c r="G1808" s="3"/>
+      <c r="H1808" s="3"/>
+      <c r="I1808" s="4"/>
+      <c r="J1808" s="4"/>
+    </row>
+    <row r="1809" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1809" s="3"/>
+      <c r="B1809" s="3"/>
+      <c r="C1809" s="3"/>
+      <c r="D1809" s="3"/>
+      <c r="E1809" s="3"/>
+      <c r="F1809" s="3"/>
+      <c r="G1809" s="3"/>
+      <c r="H1809" s="3"/>
+      <c r="I1809" s="4"/>
+      <c r="J1809" s="4"/>
+    </row>
+    <row r="1810" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1810" s="3"/>
+      <c r="B1810" s="3"/>
+      <c r="C1810" s="3"/>
+      <c r="D1810" s="3"/>
+      <c r="E1810" s="3"/>
+      <c r="F1810" s="3"/>
+      <c r="G1810" s="3"/>
+      <c r="H1810" s="3"/>
+      <c r="I1810" s="4"/>
+      <c r="J1810" s="4"/>
+    </row>
+    <row r="1811" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1811" s="3"/>
+      <c r="B1811" s="3"/>
+      <c r="C1811" s="3"/>
+      <c r="D1811" s="3"/>
+      <c r="E1811" s="3"/>
+      <c r="F1811" s="3"/>
+      <c r="G1811" s="3"/>
+      <c r="H1811" s="3"/>
+      <c r="I1811" s="4"/>
+      <c r="J1811" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-12-22.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13858" uniqueCount="1532">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14034" uniqueCount="1544">
   <si>
     <t>Year</t>
   </si>
@@ -4621,6 +4621,42 @@
   </si>
   <si>
     <t>2025-12-09</t>
+  </si>
+  <si>
+    <t>2025-12-10</t>
+  </si>
+  <si>
+    <t>2025-12-11</t>
+  </si>
+  <si>
+    <t>2025-12-12</t>
+  </si>
+  <si>
+    <t>2025-12-14</t>
+  </si>
+  <si>
+    <t>2025-12-15</t>
+  </si>
+  <si>
+    <t>2025-12-16</t>
+  </si>
+  <si>
+    <t>2025-12-17</t>
+  </si>
+  <si>
+    <t>2025-12-18</t>
+  </si>
+  <si>
+    <t>nwreadinglist v4.4.0</t>
+  </si>
+  <si>
+    <t>2025-12-19</t>
+  </si>
+  <si>
+    <t>2025-12-21</t>
+  </si>
+  <si>
+    <t>2025-12-22</t>
   </si>
 </sst>
 </file>
@@ -5029,11 +5065,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J1811"/>
+  <dimension ref="A1:J1841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1760" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1787" sqref="E1787"/>
+      <pane ySplit="1" topLeftCell="A1778" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G1809" sqref="G1809"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -64081,11 +64117,11 @@
         <v>280</v>
       </c>
       <c r="I1760" s="4">
-        <f>YEAR(A1760)</f>
+        <f t="shared" ref="I1760:I1782" si="750">YEAR(A1760)</f>
         <v>2025</v>
       </c>
       <c r="J1760" s="4">
-        <f>MONTH(A1760)</f>
+        <f t="shared" ref="J1760:J1782" si="751">MONTH(A1760)</f>
         <v>11</v>
       </c>
     </row>
@@ -64115,11 +64151,11 @@
         <v>280</v>
       </c>
       <c r="I1761" s="4">
-        <f>YEAR(A1761)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1761" s="4">
-        <f>MONTH(A1761)</f>
+        <f t="shared" si="751"/>
         <v>11</v>
       </c>
     </row>
@@ -64149,11 +64185,11 @@
         <v>280</v>
       </c>
       <c r="I1762" s="4">
-        <f>YEAR(A1762)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1762" s="4">
-        <f>MONTH(A1762)</f>
+        <f t="shared" si="751"/>
         <v>11</v>
       </c>
     </row>
@@ -64183,11 +64219,11 @@
         <v>280</v>
       </c>
       <c r="I1763" s="4">
-        <f>YEAR(A1763)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1763" s="4">
-        <f>MONTH(A1763)</f>
+        <f t="shared" si="751"/>
         <v>11</v>
       </c>
     </row>
@@ -64217,11 +64253,11 @@
         <v>280</v>
       </c>
       <c r="I1764" s="4">
-        <f>YEAR(A1764)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1764" s="4">
-        <f>MONTH(A1764)</f>
+        <f t="shared" si="751"/>
         <v>11</v>
       </c>
     </row>
@@ -64251,11 +64287,11 @@
         <v>280</v>
       </c>
       <c r="I1765" s="4">
-        <f>YEAR(A1765)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1765" s="4">
-        <f>MONTH(A1765)</f>
+        <f t="shared" si="751"/>
         <v>11</v>
       </c>
     </row>
@@ -64285,11 +64321,11 @@
         <v>280</v>
       </c>
       <c r="I1766" s="4">
-        <f>YEAR(A1766)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1766" s="4">
-        <f>MONTH(A1766)</f>
+        <f t="shared" si="751"/>
         <v>11</v>
       </c>
     </row>
@@ -64319,11 +64355,11 @@
         <v>280</v>
       </c>
       <c r="I1767" s="4">
-        <f>YEAR(A1767)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1767" s="4">
-        <f>MONTH(A1767)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64353,11 +64389,11 @@
         <v>280</v>
       </c>
       <c r="I1768" s="4">
-        <f>YEAR(A1768)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1768" s="4">
-        <f>MONTH(A1768)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64387,11 +64423,11 @@
         <v>280</v>
       </c>
       <c r="I1769" s="4">
-        <f>YEAR(A1769)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1769" s="4">
-        <f>MONTH(A1769)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64421,11 +64457,11 @@
         <v>280</v>
       </c>
       <c r="I1770" s="4">
-        <f>YEAR(A1770)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1770" s="4">
-        <f>MONTH(A1770)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64455,11 +64491,11 @@
         <v>280</v>
       </c>
       <c r="I1771" s="4">
-        <f>YEAR(A1771)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1771" s="4">
-        <f>MONTH(A1771)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64489,11 +64525,11 @@
         <v>280</v>
       </c>
       <c r="I1772" s="4">
-        <f>YEAR(A1772)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1772" s="4">
-        <f>MONTH(A1772)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64523,11 +64559,11 @@
         <v>280</v>
       </c>
       <c r="I1773" s="4">
-        <f>YEAR(A1773)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1773" s="4">
-        <f>MONTH(A1773)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64557,11 +64593,11 @@
         <v>280</v>
       </c>
       <c r="I1774" s="4">
-        <f>YEAR(A1774)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1774" s="4">
-        <f>MONTH(A1774)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64591,11 +64627,11 @@
         <v>280</v>
       </c>
       <c r="I1775" s="4">
-        <f>YEAR(A1775)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1775" s="4">
-        <f>MONTH(A1775)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64625,11 +64661,11 @@
         <v>280</v>
       </c>
       <c r="I1776" s="4">
-        <f>YEAR(A1776)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1776" s="4">
-        <f>MONTH(A1776)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64659,11 +64695,11 @@
         <v>280</v>
       </c>
       <c r="I1777" s="4">
-        <f>YEAR(A1777)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1777" s="4">
-        <f>MONTH(A1777)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64693,11 +64729,11 @@
         <v>280</v>
       </c>
       <c r="I1778" s="4">
-        <f>YEAR(A1778)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1778" s="4">
-        <f>MONTH(A1778)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64727,11 +64763,11 @@
         <v>280</v>
       </c>
       <c r="I1779" s="4">
-        <f>YEAR(A1779)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1779" s="4">
-        <f>MONTH(A1779)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64761,11 +64797,11 @@
         <v>280</v>
       </c>
       <c r="I1780" s="4">
-        <f>YEAR(A1780)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1780" s="4">
-        <f>MONTH(A1780)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64795,11 +64831,11 @@
         <v>280</v>
       </c>
       <c r="I1781" s="4">
-        <f>YEAR(A1781)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1781" s="4">
-        <f>MONTH(A1781)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
@@ -64829,277 +64865,761 @@
         <v>280</v>
       </c>
       <c r="I1782" s="4">
-        <f>YEAR(A1782)</f>
+        <f t="shared" si="750"/>
         <v>2025</v>
       </c>
       <c r="J1782" s="4">
-        <f>MONTH(A1782)</f>
+        <f t="shared" si="751"/>
         <v>12</v>
       </c>
     </row>
     <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1783" s="3"/>
-      <c r="B1783" s="3"/>
-      <c r="C1783" s="3"/>
-      <c r="D1783" s="3"/>
-      <c r="E1783" s="3"/>
-      <c r="F1783" s="3"/>
-      <c r="G1783" s="3"/>
-      <c r="H1783" s="3"/>
-      <c r="I1783" s="4"/>
-      <c r="J1783" s="4"/>
+      <c r="A1783" s="3" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B1783" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1783" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1783" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E1783" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1783" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1783" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1783" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1783" s="4">
+        <f t="shared" ref="I1783:I1785" si="752">YEAR(A1783)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1783" s="4">
+        <f t="shared" ref="J1783:J1785" si="753">MONTH(A1783)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1784" s="3"/>
-      <c r="B1784" s="3"/>
-      <c r="C1784" s="3"/>
-      <c r="D1784" s="3"/>
-      <c r="E1784" s="3"/>
-      <c r="F1784" s="3"/>
-      <c r="G1784" s="3"/>
-      <c r="H1784" s="3"/>
-      <c r="I1784" s="4"/>
-      <c r="J1784" s="4"/>
+      <c r="A1784" s="3" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B1784" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1784" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D1784" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="E1784" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1784" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1784" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1784" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1784" s="4">
+        <f t="shared" si="752"/>
+        <v>2025</v>
+      </c>
+      <c r="J1784" s="4">
+        <f t="shared" si="753"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1785" s="3"/>
-      <c r="B1785" s="3"/>
-      <c r="C1785" s="3"/>
-      <c r="D1785" s="3"/>
-      <c r="E1785" s="3"/>
-      <c r="F1785" s="3"/>
-      <c r="G1785" s="3"/>
-      <c r="H1785" s="3"/>
-      <c r="I1785" s="4"/>
-      <c r="J1785" s="4"/>
+      <c r="A1785" s="3" t="s">
+        <v>1532</v>
+      </c>
+      <c r="B1785" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="C1785" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1785" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1785" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1785" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1785" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1785" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1785" s="4">
+        <f t="shared" si="752"/>
+        <v>2025</v>
+      </c>
+      <c r="J1785" s="4">
+        <f t="shared" si="753"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1786" s="3"/>
-      <c r="B1786" s="3"/>
-      <c r="C1786" s="3"/>
-      <c r="D1786" s="3"/>
-      <c r="E1786" s="3"/>
-      <c r="F1786" s="3"/>
-      <c r="G1786" s="3"/>
-      <c r="H1786" s="3"/>
-      <c r="I1786" s="4"/>
-      <c r="J1786" s="4"/>
+      <c r="A1786" s="3" t="s">
+        <v>1533</v>
+      </c>
+      <c r="B1786" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="C1786" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1786" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="E1786" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1786" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1786" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1786" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1786" s="4">
+        <f t="shared" ref="I1786:I1787" si="754">YEAR(A1786)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1786" s="4">
+        <f t="shared" ref="J1786:J1787" si="755">MONTH(A1786)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1787" s="3"/>
-      <c r="B1787" s="3"/>
-      <c r="C1787" s="3"/>
-      <c r="D1787" s="3"/>
-      <c r="E1787" s="3"/>
-      <c r="F1787" s="3"/>
-      <c r="G1787" s="3"/>
-      <c r="H1787" s="3"/>
-      <c r="I1787" s="4"/>
-      <c r="J1787" s="4"/>
+      <c r="A1787" s="3" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B1787" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1787" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="D1787" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1787" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1787" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1787" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1787" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1787" s="4">
+        <f t="shared" si="754"/>
+        <v>2025</v>
+      </c>
+      <c r="J1787" s="4">
+        <f t="shared" si="755"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1788" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1788" s="3"/>
-      <c r="B1788" s="3"/>
-      <c r="C1788" s="3"/>
-      <c r="D1788" s="3"/>
-      <c r="E1788" s="3"/>
-      <c r="F1788" s="3"/>
-      <c r="G1788" s="3"/>
-      <c r="H1788" s="3"/>
-      <c r="I1788" s="4"/>
-      <c r="J1788" s="4"/>
+      <c r="A1788" s="3" t="s">
+        <v>1534</v>
+      </c>
+      <c r="B1788" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1788" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1788" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1788" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1788" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1788" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1788" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1788" s="4">
+        <f t="shared" ref="I1788:I1790" si="756">YEAR(A1788)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1788" s="4">
+        <f t="shared" ref="J1788:J1790" si="757">MONTH(A1788)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1789" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1789" s="3"/>
-      <c r="B1789" s="3"/>
-      <c r="C1789" s="3"/>
-      <c r="D1789" s="3"/>
-      <c r="E1789" s="3"/>
-      <c r="F1789" s="3"/>
-      <c r="G1789" s="3"/>
-      <c r="H1789" s="3"/>
-      <c r="I1789" s="4"/>
-      <c r="J1789" s="4"/>
+      <c r="A1789" s="3" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B1789" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1789" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1789" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1789" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1789" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1789" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1789" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1789" s="4">
+        <f t="shared" si="756"/>
+        <v>2025</v>
+      </c>
+      <c r="J1789" s="4">
+        <f t="shared" si="757"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1790" s="3"/>
-      <c r="B1790" s="3"/>
-      <c r="C1790" s="3"/>
-      <c r="D1790" s="3"/>
-      <c r="E1790" s="3"/>
-      <c r="F1790" s="3"/>
-      <c r="G1790" s="3"/>
-      <c r="H1790" s="3"/>
-      <c r="I1790" s="4"/>
-      <c r="J1790" s="4"/>
+      <c r="A1790" s="3" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B1790" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1790" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D1790" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1790" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1790" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1790" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1790" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1790" s="4">
+        <f t="shared" si="756"/>
+        <v>2025</v>
+      </c>
+      <c r="J1790" s="4">
+        <f t="shared" si="757"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1791" s="3"/>
-      <c r="B1791" s="3"/>
-      <c r="C1791" s="3"/>
-      <c r="D1791" s="3"/>
-      <c r="E1791" s="3"/>
-      <c r="F1791" s="3"/>
-      <c r="G1791" s="3"/>
-      <c r="H1791" s="3"/>
-      <c r="I1791" s="4"/>
-      <c r="J1791" s="4"/>
+      <c r="A1791" s="3" t="s">
+        <v>1535</v>
+      </c>
+      <c r="B1791" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="C1791" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="D1791" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1791" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1791" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1791" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1791" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1791" s="4">
+        <f t="shared" ref="I1791:I1792" si="758">YEAR(A1791)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1791" s="4">
+        <f t="shared" ref="J1791:J1792" si="759">MONTH(A1791)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1792" s="3"/>
-      <c r="B1792" s="3"/>
-      <c r="C1792" s="3"/>
-      <c r="D1792" s="3"/>
-      <c r="E1792" s="3"/>
-      <c r="F1792" s="3"/>
-      <c r="G1792" s="3"/>
-      <c r="H1792" s="3"/>
-      <c r="I1792" s="4"/>
-      <c r="J1792" s="4"/>
+      <c r="A1792" s="3" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B1792" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C1792" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1792" s="3" t="s">
+        <v>875</v>
+      </c>
+      <c r="E1792" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1792" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1792" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1792" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1792" s="4">
+        <f t="shared" si="758"/>
+        <v>2025</v>
+      </c>
+      <c r="J1792" s="4">
+        <f t="shared" si="759"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1793" s="3"/>
-      <c r="B1793" s="3"/>
-      <c r="C1793" s="3"/>
-      <c r="D1793" s="3"/>
-      <c r="E1793" s="3"/>
-      <c r="F1793" s="3"/>
-      <c r="G1793" s="3"/>
-      <c r="H1793" s="3"/>
-      <c r="I1793" s="4"/>
-      <c r="J1793" s="4"/>
+      <c r="A1793" s="3" t="s">
+        <v>1536</v>
+      </c>
+      <c r="B1793" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1793" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="D1793" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1793" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1793" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1793" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1793" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1793" s="4">
+        <f t="shared" ref="I1793" si="760">YEAR(A1793)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1793" s="4">
+        <f t="shared" ref="J1793" si="761">MONTH(A1793)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1794" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1794" s="3"/>
-      <c r="B1794" s="3"/>
-      <c r="C1794" s="3"/>
-      <c r="D1794" s="3"/>
-      <c r="E1794" s="3"/>
-      <c r="F1794" s="3"/>
-      <c r="G1794" s="3"/>
-      <c r="H1794" s="3"/>
-      <c r="I1794" s="4"/>
-      <c r="J1794" s="4"/>
+      <c r="A1794" s="3" t="s">
+        <v>1537</v>
+      </c>
+      <c r="B1794" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="C1794" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1794" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="E1794" s="3" t="s">
+        <v>1463</v>
+      </c>
+      <c r="F1794" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1794" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1794" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1794" s="4">
+        <f t="shared" ref="I1794" si="762">YEAR(A1794)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1794" s="4">
+        <f t="shared" ref="J1794" si="763">MONTH(A1794)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1795" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1795" s="3"/>
-      <c r="B1795" s="3"/>
-      <c r="C1795" s="3"/>
-      <c r="D1795" s="3"/>
-      <c r="E1795" s="3"/>
-      <c r="F1795" s="3"/>
-      <c r="G1795" s="3"/>
-      <c r="H1795" s="3"/>
-      <c r="I1795" s="4"/>
-      <c r="J1795" s="4"/>
+      <c r="A1795" s="3" t="s">
+        <v>1538</v>
+      </c>
+      <c r="B1795" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1795" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1795" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1795" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1795" s="3" t="s">
+        <v>1285</v>
+      </c>
+      <c r="G1795" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1795" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1795" s="4">
+        <f t="shared" ref="I1795:I1796" si="764">YEAR(A1795)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1795" s="4">
+        <f t="shared" ref="J1795:J1796" si="765">MONTH(A1795)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1796" s="3"/>
-      <c r="B1796" s="3"/>
-      <c r="C1796" s="3"/>
-      <c r="D1796" s="3"/>
-      <c r="E1796" s="3"/>
-      <c r="F1796" s="3"/>
-      <c r="G1796" s="3"/>
-      <c r="H1796" s="3"/>
-      <c r="I1796" s="4"/>
-      <c r="J1796" s="4"/>
+      <c r="A1796" s="3" t="s">
+        <v>1539</v>
+      </c>
+      <c r="B1796" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C1796" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1796" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1796" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1796" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1796" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1796" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1796" s="4">
+        <f t="shared" si="764"/>
+        <v>2025</v>
+      </c>
+      <c r="J1796" s="4">
+        <f t="shared" si="765"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1797" s="3"/>
-      <c r="B1797" s="3"/>
-      <c r="C1797" s="3"/>
-      <c r="D1797" s="3"/>
-      <c r="E1797" s="3"/>
-      <c r="F1797" s="3"/>
-      <c r="G1797" s="3"/>
-      <c r="H1797" s="3"/>
-      <c r="I1797" s="4"/>
-      <c r="J1797" s="4"/>
+      <c r="A1797" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B1797" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C1797" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1797" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1797" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1797" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1797" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1797" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1797" s="4">
+        <f t="shared" ref="I1797:I1798" si="766">YEAR(A1797)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1797" s="4">
+        <f t="shared" ref="J1797:J1798" si="767">MONTH(A1797)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1798" s="3"/>
-      <c r="B1798" s="3"/>
-      <c r="C1798" s="3"/>
-      <c r="D1798" s="3"/>
-      <c r="E1798" s="3"/>
-      <c r="F1798" s="3"/>
-      <c r="G1798" s="3"/>
-      <c r="H1798" s="3"/>
-      <c r="I1798" s="4"/>
-      <c r="J1798" s="4"/>
+      <c r="A1798" s="3" t="s">
+        <v>1541</v>
+      </c>
+      <c r="B1798" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C1798" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="D1798" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1798" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1798" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1798" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1798" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1798" s="4">
+        <f t="shared" si="766"/>
+        <v>2025</v>
+      </c>
+      <c r="J1798" s="4">
+        <f t="shared" si="767"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1799" s="3"/>
-      <c r="B1799" s="3"/>
-      <c r="C1799" s="3"/>
-      <c r="D1799" s="3"/>
-      <c r="E1799" s="3"/>
-      <c r="F1799" s="3"/>
-      <c r="G1799" s="3"/>
-      <c r="H1799" s="3"/>
-      <c r="I1799" s="4"/>
-      <c r="J1799" s="4"/>
+      <c r="A1799" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B1799" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="C1799" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="D1799" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1799" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1799" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1799" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1799" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1799" s="4">
+        <f t="shared" ref="I1799:I1802" si="768">YEAR(A1799)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1799" s="4">
+        <f t="shared" ref="J1799:J1802" si="769">MONTH(A1799)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1800" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1800" s="3"/>
-      <c r="B1800" s="3"/>
-      <c r="C1800" s="3"/>
-      <c r="D1800" s="3"/>
-      <c r="E1800" s="3"/>
-      <c r="F1800" s="3"/>
-      <c r="G1800" s="3"/>
-      <c r="H1800" s="3"/>
-      <c r="I1800" s="4"/>
-      <c r="J1800" s="4"/>
+      <c r="A1800" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B1800" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1800" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="D1800" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1800" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1800" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1800" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1800" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1800" s="4">
+        <f t="shared" si="768"/>
+        <v>2025</v>
+      </c>
+      <c r="J1800" s="4">
+        <f t="shared" si="769"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1801" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1801" s="3"/>
-      <c r="B1801" s="3"/>
-      <c r="C1801" s="3"/>
-      <c r="D1801" s="3"/>
-      <c r="E1801" s="3"/>
-      <c r="F1801" s="3"/>
-      <c r="G1801" s="3"/>
-      <c r="H1801" s="3"/>
-      <c r="I1801" s="4"/>
-      <c r="J1801" s="4"/>
+      <c r="A1801" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B1801" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="C1801" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="D1801" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="E1801" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1801" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1801" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1801" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1801" s="4">
+        <f t="shared" si="768"/>
+        <v>2025</v>
+      </c>
+      <c r="J1801" s="4">
+        <f t="shared" si="769"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1802" s="3"/>
-      <c r="B1802" s="3"/>
-      <c r="C1802" s="3"/>
-      <c r="D1802" s="3"/>
-      <c r="E1802" s="3"/>
-      <c r="F1802" s="3"/>
-      <c r="G1802" s="3"/>
-      <c r="H1802" s="3"/>
-      <c r="I1802" s="4"/>
-      <c r="J1802" s="4"/>
+      <c r="A1802" s="3" t="s">
+        <v>1542</v>
+      </c>
+      <c r="B1802" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="C1802" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="D1802" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="E1802" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1802" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1802" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1802" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1802" s="4">
+        <f t="shared" si="768"/>
+        <v>2025</v>
+      </c>
+      <c r="J1802" s="4">
+        <f t="shared" si="769"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1803" s="3"/>
-      <c r="B1803" s="3"/>
-      <c r="C1803" s="3"/>
-      <c r="D1803" s="3"/>
-      <c r="E1803" s="3"/>
-      <c r="F1803" s="3"/>
-      <c r="G1803" s="3"/>
-      <c r="H1803" s="3"/>
-      <c r="I1803" s="4"/>
-      <c r="J1803" s="4"/>
+      <c r="A1803" s="3" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B1803" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1803" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="D1803" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E1803" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1803" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1803" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1803" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1803" s="4">
+        <f t="shared" ref="I1803:I1804" si="770">YEAR(A1803)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1803" s="4">
+        <f t="shared" ref="J1803:J1804" si="771">MONTH(A1803)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1804" s="3"/>
-      <c r="B1804" s="3"/>
-      <c r="C1804" s="3"/>
-      <c r="D1804" s="3"/>
-      <c r="E1804" s="3"/>
-      <c r="F1804" s="3"/>
-      <c r="G1804" s="3"/>
-      <c r="H1804" s="3"/>
-      <c r="I1804" s="4"/>
-      <c r="J1804" s="4"/>
+      <c r="A1804" s="3" t="s">
+        <v>1543</v>
+      </c>
+      <c r="B1804" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C1804" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1804" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1804" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1804" s="3" t="s">
+        <v>1540</v>
+      </c>
+      <c r="G1804" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1804" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1804" s="4">
+        <f t="shared" si="770"/>
+        <v>2025</v>
+      </c>
+      <c r="J1804" s="4">
+        <f t="shared" si="771"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1805" s="3"/>
@@ -65185,6 +65705,366 @@
       <c r="I1811" s="4"/>
       <c r="J1811" s="4"/>
     </row>
+    <row r="1812" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1812" s="3"/>
+      <c r="B1812" s="3"/>
+      <c r="C1812" s="3"/>
+      <c r="D1812" s="3"/>
+      <c r="E1812" s="3"/>
+      <c r="F1812" s="3"/>
+      <c r="G1812" s="3"/>
+      <c r="H1812" s="3"/>
+      <c r="I1812" s="4"/>
+      <c r="J1812" s="4"/>
+    </row>
+    <row r="1813" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1813" s="3"/>
+      <c r="B1813" s="3"/>
+      <c r="C1813" s="3"/>
+      <c r="D1813" s="3"/>
+      <c r="E1813" s="3"/>
+      <c r="F1813" s="3"/>
+      <c r="G1813" s="3"/>
+      <c r="H1813" s="3"/>
+      <c r="I1813" s="4"/>
+      <c r="J1813" s="4"/>
+    </row>
+    <row r="1814" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1814" s="3"/>
+      <c r="B1814" s="3"/>
+      <c r="C1814" s="3"/>
+      <c r="D1814" s="3"/>
+      <c r="E1814" s="3"/>
+      <c r="F1814" s="3"/>
+      <c r="G1814" s="3"/>
+      <c r="H1814" s="3"/>
+      <c r="I1814" s="4"/>
+      <c r="J1814" s="4"/>
+    </row>
+    <row r="1815" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1815" s="3"/>
+      <c r="B1815" s="3"/>
+      <c r="C1815" s="3"/>
+      <c r="D1815" s="3"/>
+      <c r="E1815" s="3"/>
+      <c r="F1815" s="3"/>
+      <c r="G1815" s="3"/>
+      <c r="H1815" s="3"/>
+      <c r="I1815" s="4"/>
+      <c r="J1815" s="4"/>
+    </row>
+    <row r="1816" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1816" s="3"/>
+      <c r="B1816" s="3"/>
+      <c r="C1816" s="3"/>
+      <c r="D1816" s="3"/>
+      <c r="E1816" s="3"/>
+      <c r="F1816" s="3"/>
+      <c r="G1816" s="3"/>
+      <c r="H1816" s="3"/>
+      <c r="I1816" s="4"/>
+      <c r="J1816" s="4"/>
+    </row>
+    <row r="1817" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1817" s="3"/>
+      <c r="B1817" s="3"/>
+      <c r="C1817" s="3"/>
+      <c r="D1817" s="3"/>
+      <c r="E1817" s="3"/>
+      <c r="F1817" s="3"/>
+      <c r="G1817" s="3"/>
+      <c r="H1817" s="3"/>
+      <c r="I1817" s="4"/>
+      <c r="J1817" s="4"/>
+    </row>
+    <row r="1818" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1818" s="3"/>
+      <c r="B1818" s="3"/>
+      <c r="C1818" s="3"/>
+      <c r="D1818" s="3"/>
+      <c r="E1818" s="3"/>
+      <c r="F1818" s="3"/>
+      <c r="G1818" s="3"/>
+      <c r="H1818" s="3"/>
+      <c r="I1818" s="4"/>
+      <c r="J1818" s="4"/>
+    </row>
+    <row r="1819" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1819" s="3"/>
+      <c r="B1819" s="3"/>
+      <c r="C1819" s="3"/>
+      <c r="D1819" s="3"/>
+      <c r="E1819" s="3"/>
+      <c r="F1819" s="3"/>
+      <c r="G1819" s="3"/>
+      <c r="H1819" s="3"/>
+      <c r="I1819" s="4"/>
+      <c r="J1819" s="4"/>
+    </row>
+    <row r="1820" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1820" s="3"/>
+      <c r="B1820" s="3"/>
+      <c r="C1820" s="3"/>
+      <c r="D1820" s="3"/>
+      <c r="E1820" s="3"/>
+      <c r="F1820" s="3"/>
+      <c r="G1820" s="3"/>
+      <c r="H1820" s="3"/>
+      <c r="I1820" s="4"/>
+      <c r="J1820" s="4"/>
+    </row>
+    <row r="1821" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1821" s="3"/>
+      <c r="B1821" s="3"/>
+      <c r="C1821" s="3"/>
+      <c r="D1821" s="3"/>
+      <c r="E1821" s="3"/>
+      <c r="F1821" s="3"/>
+      <c r="G1821" s="3"/>
+      <c r="H1821" s="3"/>
+      <c r="I1821" s="4"/>
+      <c r="J1821" s="4"/>
+    </row>
+    <row r="1822" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1822" s="3"/>
+      <c r="B1822" s="3"/>
+      <c r="C1822" s="3"/>
+      <c r="D1822" s="3"/>
+      <c r="E1822" s="3"/>
+      <c r="F1822" s="3"/>
+      <c r="G1822" s="3"/>
+      <c r="H1822" s="3"/>
+      <c r="I1822" s="4"/>
+      <c r="J1822" s="4"/>
+    </row>
+    <row r="1823" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1823" s="3"/>
+      <c r="B1823" s="3"/>
+      <c r="C1823" s="3"/>
+      <c r="D1823" s="3"/>
+      <c r="E1823" s="3"/>
+      <c r="F1823" s="3"/>
+      <c r="G1823" s="3"/>
+      <c r="H1823" s="3"/>
+      <c r="I1823" s="4"/>
+      <c r="J1823" s="4"/>
+    </row>
+    <row r="1824" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1824" s="3"/>
+      <c r="B1824" s="3"/>
+      <c r="C1824" s="3"/>
+      <c r="D1824" s="3"/>
+      <c r="E1824" s="3"/>
+      <c r="F1824" s="3"/>
+      <c r="G1824" s="3"/>
+      <c r="H1824" s="3"/>
+      <c r="I1824" s="4"/>
+      <c r="J1824" s="4"/>
+    </row>
+    <row r="1825" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1825" s="3"/>
+      <c r="B1825" s="3"/>
+      <c r="C1825" s="3"/>
+      <c r="D1825" s="3"/>
+      <c r="E1825" s="3"/>
+      <c r="F1825" s="3"/>
+      <c r="G1825" s="3"/>
+      <c r="H1825" s="3"/>
+      <c r="I1825" s="4"/>
+      <c r="J1825" s="4"/>
+    </row>
+    <row r="1826" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1826" s="3"/>
+      <c r="B1826" s="3"/>
+      <c r="C1826" s="3"/>
+      <c r="D1826" s="3"/>
+      <c r="E1826" s="3"/>
+      <c r="F1826" s="3"/>
+      <c r="G1826" s="3"/>
+      <c r="H1826" s="3"/>
+      <c r="I1826" s="4"/>
+      <c r="J1826" s="4"/>
+    </row>
+    <row r="1827" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1827" s="3"/>
+      <c r="B1827" s="3"/>
+      <c r="C1827" s="3"/>
+      <c r="D1827" s="3"/>
+      <c r="E1827" s="3"/>
+      <c r="F1827" s="3"/>
+      <c r="G1827" s="3"/>
+      <c r="H1827" s="3"/>
+      <c r="I1827" s="4"/>
+      <c r="J1827" s="4"/>
+    </row>
+    <row r="1828" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1828" s="3"/>
+      <c r="B1828" s="3"/>
+      <c r="C1828" s="3"/>
+      <c r="D1828" s="3"/>
+      <c r="E1828" s="3"/>
+      <c r="F1828" s="3"/>
+      <c r="G1828" s="3"/>
+      <c r="H1828" s="3"/>
+      <c r="I1828" s="4"/>
+      <c r="J1828" s="4"/>
+    </row>
+    <row r="1829" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1829" s="3"/>
+      <c r="B1829" s="3"/>
+      <c r="C1829" s="3"/>
+      <c r="D1829" s="3"/>
+      <c r="E1829" s="3"/>
+      <c r="F1829" s="3"/>
+      <c r="G1829" s="3"/>
+      <c r="H1829" s="3"/>
+      <c r="I1829" s="4"/>
+      <c r="J1829" s="4"/>
+    </row>
+    <row r="1830" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1830" s="3"/>
+      <c r="B1830" s="3"/>
+      <c r="C1830" s="3"/>
+      <c r="D1830" s="3"/>
+      <c r="E1830" s="3"/>
+      <c r="F1830" s="3"/>
+      <c r="G1830" s="3"/>
+      <c r="H1830" s="3"/>
+      <c r="I1830" s="4"/>
+      <c r="J1830" s="4"/>
+    </row>
+    <row r="1831" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1831" s="3"/>
+      <c r="B1831" s="3"/>
+      <c r="C1831" s="3"/>
+      <c r="D1831" s="3"/>
+      <c r="E1831" s="3"/>
+      <c r="F1831" s="3"/>
+      <c r="G1831" s="3"/>
+      <c r="H1831" s="3"/>
+      <c r="I1831" s="4"/>
+      <c r="J1831" s="4"/>
+    </row>
+    <row r="1832" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1832" s="3"/>
+      <c r="B1832" s="3"/>
+      <c r="C1832" s="3"/>
+      <c r="D1832" s="3"/>
+      <c r="E1832" s="3"/>
+      <c r="F1832" s="3"/>
+      <c r="G1832" s="3"/>
+      <c r="H1832" s="3"/>
+      <c r="I1832" s="4"/>
+      <c r="J1832" s="4"/>
+    </row>
+    <row r="1833" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1833" s="3"/>
+      <c r="B1833" s="3"/>
+      <c r="C1833" s="3"/>
+      <c r="D1833" s="3"/>
+      <c r="E1833" s="3"/>
+      <c r="F1833" s="3"/>
+      <c r="G1833" s="3"/>
+      <c r="H1833" s="3"/>
+      <c r="I1833" s="4"/>
+      <c r="J1833" s="4"/>
+    </row>
+    <row r="1834" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1834" s="3"/>
+      <c r="B1834" s="3"/>
+      <c r="C1834" s="3"/>
+      <c r="D1834" s="3"/>
+      <c r="E1834" s="3"/>
+      <c r="F1834" s="3"/>
+      <c r="G1834" s="3"/>
+      <c r="H1834" s="3"/>
+      <c r="I1834" s="4"/>
+      <c r="J1834" s="4"/>
+    </row>
+    <row r="1835" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1835" s="3"/>
+      <c r="B1835" s="3"/>
+      <c r="C1835" s="3"/>
+      <c r="D1835" s="3"/>
+      <c r="E1835" s="3"/>
+      <c r="F1835" s="3"/>
+      <c r="G1835" s="3"/>
+      <c r="H1835" s="3"/>
+      <c r="I1835" s="4"/>
+      <c r="J1835" s="4"/>
+    </row>
+    <row r="1836" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1836" s="3"/>
+      <c r="B1836" s="3"/>
+      <c r="C1836" s="3"/>
+      <c r="D1836" s="3"/>
+      <c r="E1836" s="3"/>
+      <c r="F1836" s="3"/>
+      <c r="G1836" s="3"/>
+      <c r="H1836" s="3"/>
+      <c r="I1836" s="4"/>
+      <c r="J1836" s="4"/>
+    </row>
+    <row r="1837" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1837" s="3"/>
+      <c r="B1837" s="3"/>
+      <c r="C1837" s="3"/>
+      <c r="D1837" s="3"/>
+      <c r="E1837" s="3"/>
+      <c r="F1837" s="3"/>
+      <c r="G1837" s="3"/>
+      <c r="H1837" s="3"/>
+      <c r="I1837" s="4"/>
+      <c r="J1837" s="4"/>
+    </row>
+    <row r="1838" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1838" s="3"/>
+      <c r="B1838" s="3"/>
+      <c r="C1838" s="3"/>
+      <c r="D1838" s="3"/>
+      <c r="E1838" s="3"/>
+      <c r="F1838" s="3"/>
+      <c r="G1838" s="3"/>
+      <c r="H1838" s="3"/>
+      <c r="I1838" s="4"/>
+      <c r="J1838" s="4"/>
+    </row>
+    <row r="1839" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1839" s="3"/>
+      <c r="B1839" s="3"/>
+      <c r="C1839" s="3"/>
+      <c r="D1839" s="3"/>
+      <c r="E1839" s="3"/>
+      <c r="F1839" s="3"/>
+      <c r="G1839" s="3"/>
+      <c r="H1839" s="3"/>
+      <c r="I1839" s="4"/>
+      <c r="J1839" s="4"/>
+    </row>
+    <row r="1840" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1840" s="3"/>
+      <c r="B1840" s="3"/>
+      <c r="C1840" s="3"/>
+      <c r="D1840" s="3"/>
+      <c r="E1840" s="3"/>
+      <c r="F1840" s="3"/>
+      <c r="G1840" s="3"/>
+      <c r="H1840" s="3"/>
+      <c r="I1840" s="4"/>
+      <c r="J1840" s="4"/>
+    </row>
+    <row r="1841" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1841" s="3"/>
+      <c r="B1841" s="3"/>
+      <c r="C1841" s="3"/>
+      <c r="D1841" s="3"/>
+      <c r="E1841" s="3"/>
+      <c r="F1841" s="3"/>
+      <c r="G1841" s="3"/>
+      <c r="H1841" s="3"/>
+      <c r="I1841" s="4"/>
+      <c r="J1841" s="4"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-12-26.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14034" uniqueCount="1545">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14082" uniqueCount="1549">
   <si>
     <t>Year</t>
   </si>
@@ -4660,6 +4660,18 @@
   </si>
   <si>
     <t>8h 45m</t>
+  </si>
+  <si>
+    <t>2025-12-23</t>
+  </si>
+  <si>
+    <t>nwtimetracking v5.1.0</t>
+  </si>
+  <si>
+    <t>2025-12-25</t>
+  </si>
+  <si>
+    <t>2025-12-26</t>
   </si>
 </sst>
 </file>
@@ -5071,8 +5083,8 @@
   <dimension ref="A1:J1841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1766" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1805" sqref="D1805"/>
+      <pane ySplit="1" topLeftCell="A1784" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1811" sqref="A1811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -65582,11 +65594,11 @@
         <v>279</v>
       </c>
       <c r="I1803" s="4">
-        <f t="shared" ref="I1803:I1804" si="770">YEAR(A1803)</f>
+        <f t="shared" ref="I1803:I1805" si="770">YEAR(A1803)</f>
         <v>2025</v>
       </c>
       <c r="J1803" s="4">
-        <f t="shared" ref="J1803:J1804" si="771">MONTH(A1803)</f>
+        <f t="shared" ref="J1803:J1805" si="771">MONTH(A1803)</f>
         <v>12</v>
       </c>
     </row>
@@ -65625,76 +65637,208 @@
       </c>
     </row>
     <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1805" s="3"/>
-      <c r="B1805" s="3"/>
-      <c r="C1805" s="3"/>
-      <c r="D1805" s="3"/>
-      <c r="E1805" s="3"/>
-      <c r="F1805" s="3"/>
-      <c r="G1805" s="3"/>
-      <c r="H1805" s="3"/>
-      <c r="I1805" s="4"/>
-      <c r="J1805" s="4"/>
+      <c r="A1805" s="3" t="s">
+        <v>1545</v>
+      </c>
+      <c r="B1805" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C1805" s="3" t="s">
+        <v>285</v>
+      </c>
+      <c r="D1805" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="E1805" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1805" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1805" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1805" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1805" s="4">
+        <f t="shared" si="770"/>
+        <v>2025</v>
+      </c>
+      <c r="J1805" s="4">
+        <f t="shared" si="771"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1806" s="3"/>
-      <c r="B1806" s="3"/>
-      <c r="C1806" s="3"/>
-      <c r="D1806" s="3"/>
-      <c r="E1806" s="3"/>
-      <c r="F1806" s="3"/>
-      <c r="G1806" s="3"/>
-      <c r="H1806" s="3"/>
-      <c r="I1806" s="4"/>
-      <c r="J1806" s="4"/>
+      <c r="A1806" s="3" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B1806" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C1806" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1806" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="E1806" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1806" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1806" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1806" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1806" s="4">
+        <f t="shared" ref="I1806:I1808" si="772">YEAR(A1806)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1806" s="4">
+        <f t="shared" ref="J1806:J1808" si="773">MONTH(A1806)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1807" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1807" s="3"/>
-      <c r="B1807" s="3"/>
-      <c r="C1807" s="3"/>
-      <c r="D1807" s="3"/>
-      <c r="E1807" s="3"/>
-      <c r="F1807" s="3"/>
-      <c r="G1807" s="3"/>
-      <c r="H1807" s="3"/>
-      <c r="I1807" s="4"/>
-      <c r="J1807" s="4"/>
+      <c r="A1807" s="3" t="s">
+        <v>1547</v>
+      </c>
+      <c r="B1807" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="C1807" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="D1807" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1807" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1807" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1807" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1807" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1807" s="4">
+        <f t="shared" si="772"/>
+        <v>2025</v>
+      </c>
+      <c r="J1807" s="4">
+        <f t="shared" si="773"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1808" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1808" s="3"/>
-      <c r="B1808" s="3"/>
-      <c r="C1808" s="3"/>
-      <c r="D1808" s="3"/>
-      <c r="E1808" s="3"/>
-      <c r="F1808" s="3"/>
-      <c r="G1808" s="3"/>
-      <c r="H1808" s="3"/>
-      <c r="I1808" s="4"/>
-      <c r="J1808" s="4"/>
+      <c r="A1808" s="3" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B1808" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C1808" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1808" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="E1808" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1808" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1808" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1808" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1808" s="4">
+        <f t="shared" si="772"/>
+        <v>2025</v>
+      </c>
+      <c r="J1808" s="4">
+        <f t="shared" si="773"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1809" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1809" s="3"/>
-      <c r="B1809" s="3"/>
-      <c r="C1809" s="3"/>
-      <c r="D1809" s="3"/>
-      <c r="E1809" s="3"/>
-      <c r="F1809" s="3"/>
-      <c r="G1809" s="3"/>
-      <c r="H1809" s="3"/>
-      <c r="I1809" s="4"/>
-      <c r="J1809" s="4"/>
+      <c r="A1809" s="3" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B1809" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C1809" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1809" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1809" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1809" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1809" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1809" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1809" s="4">
+        <f t="shared" ref="I1809:I1810" si="774">YEAR(A1809)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1809" s="4">
+        <f t="shared" ref="J1809:J1810" si="775">MONTH(A1809)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1810" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1810" s="3"/>
-      <c r="B1810" s="3"/>
-      <c r="C1810" s="3"/>
-      <c r="D1810" s="3"/>
-      <c r="E1810" s="3"/>
-      <c r="F1810" s="3"/>
-      <c r="G1810" s="3"/>
-      <c r="H1810" s="3"/>
-      <c r="I1810" s="4"/>
-      <c r="J1810" s="4"/>
+      <c r="A1810" s="3" t="s">
+        <v>1548</v>
+      </c>
+      <c r="B1810" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C1810" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="D1810" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="E1810" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1810" s="3" t="s">
+        <v>1546</v>
+      </c>
+      <c r="G1810" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1810" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1810" s="4">
+        <f t="shared" si="774"/>
+        <v>2025</v>
+      </c>
+      <c r="J1810" s="4">
+        <f t="shared" si="775"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1811" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1811" s="3"/>

</xml_diff>

<commit_message>
#56 Time Tracking: fixed 1807.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -5084,7 +5084,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A1784" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1811" sqref="A1811"/>
+      <selection pane="bottomLeft" activeCell="D1807" sqref="D1807"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -65715,7 +65715,7 @@
         <v>139</v>
       </c>
       <c r="D1807" s="3" t="s">
-        <v>347</v>
+        <v>298</v>
       </c>
       <c r="E1807" s="3" t="s">
         <v>127</v>

</xml_diff>

<commit_message>
#56 Time Tracking: #adoc -> #asciidoc.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -4416,9 +4416,6 @@
     <t>2025-08-25</t>
   </si>
   <si>
-    <t>#adoc</t>
-  </si>
-  <si>
     <t>2025-08-26</t>
   </si>
   <si>
@@ -4672,6 +4669,9 @@
   </si>
   <si>
     <t>2025-12-26</t>
+  </si>
+  <si>
+    <t>#asciidoc</t>
   </si>
 </sst>
 </file>
@@ -5083,8 +5083,8 @@
   <dimension ref="A1:J1841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1784" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1807" sqref="D1807"/>
+      <pane ySplit="1" topLeftCell="A1779" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1811" sqref="C1811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -54260,7 +54260,7 @@
         <v>389</v>
       </c>
       <c r="E1464" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1464" s="3" t="s">
         <v>1285</v>
@@ -54394,7 +54394,7 @@
         <v>94</v>
       </c>
       <c r="E1468" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1468" s="3" t="s">
         <v>1285</v>
@@ -54428,7 +54428,7 @@
         <v>105</v>
       </c>
       <c r="E1469" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1469" s="3" t="s">
         <v>1285</v>
@@ -54494,7 +54494,7 @@
         <v>243</v>
       </c>
       <c r="E1471" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1471" s="3" t="s">
         <v>1285</v>
@@ -54528,7 +54528,7 @@
         <v>220</v>
       </c>
       <c r="E1472" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1472" s="3" t="s">
         <v>1285</v>
@@ -54562,7 +54562,7 @@
         <v>239</v>
       </c>
       <c r="E1473" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1473" s="3" t="s">
         <v>1285</v>
@@ -60666,7 +60666,7 @@
         <v>167</v>
       </c>
       <c r="E1657" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1657" s="3" t="s">
         <v>1285</v>
@@ -60700,7 +60700,7 @@
         <v>115</v>
       </c>
       <c r="E1658" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1658" s="3" t="s">
         <v>1285</v>
@@ -60722,7 +60722,7 @@
     </row>
     <row r="1659" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1659" s="3" t="s">
-        <v>1464</v>
+        <v>1463</v>
       </c>
       <c r="B1659" s="3" t="s">
         <v>329</v>
@@ -60734,7 +60734,7 @@
         <v>972</v>
       </c>
       <c r="E1659" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1659" s="3" t="s">
         <v>1285</v>
@@ -60756,7 +60756,7 @@
     </row>
     <row r="1660" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1660" s="3" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B1660" s="3" t="s">
         <v>248</v>
@@ -60768,7 +60768,7 @@
         <v>184</v>
       </c>
       <c r="E1660" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1660" s="3" t="s">
         <v>1285</v>
@@ -60790,7 +60790,7 @@
     </row>
     <row r="1661" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1661" s="3" t="s">
-        <v>1465</v>
+        <v>1464</v>
       </c>
       <c r="B1661" s="3" t="s">
         <v>149</v>
@@ -60802,7 +60802,7 @@
         <v>193</v>
       </c>
       <c r="E1661" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1661" s="3" t="s">
         <v>1285</v>
@@ -60824,7 +60824,7 @@
     </row>
     <row r="1662" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1662" s="3" t="s">
-        <v>1466</v>
+        <v>1465</v>
       </c>
       <c r="B1662" s="3" t="s">
         <v>355</v>
@@ -60836,7 +60836,7 @@
         <v>193</v>
       </c>
       <c r="E1662" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1662" s="3" t="s">
         <v>1285</v>
@@ -60858,7 +60858,7 @@
     </row>
     <row r="1663" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1663" s="3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B1663" s="3" t="s">
         <v>200</v>
@@ -60870,7 +60870,7 @@
         <v>136</v>
       </c>
       <c r="E1663" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1663" s="3" t="s">
         <v>1285</v>
@@ -60892,7 +60892,7 @@
     </row>
     <row r="1664" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1664" s="3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B1664" s="3" t="s">
         <v>375</v>
@@ -60904,7 +60904,7 @@
         <v>120</v>
       </c>
       <c r="E1664" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1664" s="3" t="s">
         <v>1285</v>
@@ -60926,7 +60926,7 @@
     </row>
     <row r="1665" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1665" s="3" t="s">
-        <v>1467</v>
+        <v>1466</v>
       </c>
       <c r="B1665" s="3" t="s">
         <v>149</v>
@@ -60938,7 +60938,7 @@
         <v>239</v>
       </c>
       <c r="E1665" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1665" s="3" t="s">
         <v>1285</v>
@@ -60960,7 +60960,7 @@
     </row>
     <row r="1666" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1666" s="3" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B1666" s="3" t="s">
         <v>180</v>
@@ -60969,10 +60969,10 @@
         <v>267</v>
       </c>
       <c r="D1666" s="3" t="s">
-        <v>1469</v>
+        <v>1468</v>
       </c>
       <c r="E1666" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1666" s="3" t="s">
         <v>1285</v>
@@ -60994,7 +60994,7 @@
     </row>
     <row r="1667" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1667" s="3" t="s">
-        <v>1468</v>
+        <v>1467</v>
       </c>
       <c r="B1667" s="3" t="s">
         <v>233</v>
@@ -61006,7 +61006,7 @@
         <v>120</v>
       </c>
       <c r="E1667" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1667" s="3" t="s">
         <v>1285</v>
@@ -61028,7 +61028,7 @@
     </row>
     <row r="1668" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1668" s="3" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B1668" s="3" t="s">
         <v>359</v>
@@ -61040,7 +61040,7 @@
         <v>298</v>
       </c>
       <c r="E1668" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1668" s="3" t="s">
         <v>1285</v>
@@ -61062,7 +61062,7 @@
     </row>
     <row r="1669" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1669" s="3" t="s">
-        <v>1470</v>
+        <v>1469</v>
       </c>
       <c r="B1669" s="3" t="s">
         <v>171</v>
@@ -61074,7 +61074,7 @@
         <v>120</v>
       </c>
       <c r="E1669" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1669" s="3" t="s">
         <v>1285</v>
@@ -61096,7 +61096,7 @@
     </row>
     <row r="1670" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1670" s="3" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B1670" s="3" t="s">
         <v>248</v>
@@ -61108,7 +61108,7 @@
         <v>184</v>
       </c>
       <c r="E1670" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1670" s="3" t="s">
         <v>1285</v>
@@ -61130,7 +61130,7 @@
     </row>
     <row r="1671" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1671" s="3" t="s">
-        <v>1471</v>
+        <v>1470</v>
       </c>
       <c r="B1671" s="3" t="s">
         <v>149</v>
@@ -61142,7 +61142,7 @@
         <v>193</v>
       </c>
       <c r="E1671" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1671" s="3" t="s">
         <v>1285</v>
@@ -61164,7 +61164,7 @@
     </row>
     <row r="1672" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1672" s="3" t="s">
-        <v>1472</v>
+        <v>1471</v>
       </c>
       <c r="B1672" s="3" t="s">
         <v>248</v>
@@ -61176,7 +61176,7 @@
         <v>184</v>
       </c>
       <c r="E1672" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1672" s="3" t="s">
         <v>1285</v>
@@ -61198,7 +61198,7 @@
     </row>
     <row r="1673" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1673" s="3" t="s">
-        <v>1473</v>
+        <v>1472</v>
       </c>
       <c r="B1673" s="3" t="s">
         <v>179</v>
@@ -61210,7 +61210,7 @@
         <v>1051</v>
       </c>
       <c r="E1673" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1673" s="3" t="s">
         <v>1285</v>
@@ -61232,7 +61232,7 @@
     </row>
     <row r="1674" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1674" s="3" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B1674" s="3" t="s">
         <v>248</v>
@@ -61244,7 +61244,7 @@
         <v>184</v>
       </c>
       <c r="E1674" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1674" s="3" t="s">
         <v>1285</v>
@@ -61266,7 +61266,7 @@
     </row>
     <row r="1675" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1675" s="3" t="s">
-        <v>1474</v>
+        <v>1473</v>
       </c>
       <c r="B1675" s="3" t="s">
         <v>149</v>
@@ -61278,7 +61278,7 @@
         <v>193</v>
       </c>
       <c r="E1675" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1675" s="3" t="s">
         <v>1285</v>
@@ -61300,7 +61300,7 @@
     </row>
     <row r="1676" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1676" s="3" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B1676" s="3" t="s">
         <v>331</v>
@@ -61312,7 +61312,7 @@
         <v>126</v>
       </c>
       <c r="E1676" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1676" s="3" t="s">
         <v>1285</v>
@@ -61334,7 +61334,7 @@
     </row>
     <row r="1677" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1677" s="3" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B1677" s="3" t="s">
         <v>333</v>
@@ -61346,7 +61346,7 @@
         <v>167</v>
       </c>
       <c r="E1677" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1677" s="3" t="s">
         <v>1285</v>
@@ -61368,7 +61368,7 @@
     </row>
     <row r="1678" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1678" s="3" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B1678" s="3" t="s">
         <v>192</v>
@@ -61380,7 +61380,7 @@
         <v>115</v>
       </c>
       <c r="E1678" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1678" s="3" t="s">
         <v>1285</v>
@@ -61402,7 +61402,7 @@
     </row>
     <row r="1679" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1679" s="3" t="s">
-        <v>1475</v>
+        <v>1474</v>
       </c>
       <c r="B1679" s="3" t="s">
         <v>271</v>
@@ -61414,7 +61414,7 @@
         <v>136</v>
       </c>
       <c r="E1679" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1679" s="3" t="s">
         <v>1285</v>
@@ -61436,7 +61436,7 @@
     </row>
     <row r="1680" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1680" s="3" t="s">
-        <v>1476</v>
+        <v>1475</v>
       </c>
       <c r="B1680" s="3" t="s">
         <v>133</v>
@@ -61448,7 +61448,7 @@
         <v>875</v>
       </c>
       <c r="E1680" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1680" s="3" t="s">
         <v>1285</v>
@@ -61470,7 +61470,7 @@
     </row>
     <row r="1681" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1681" s="3" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B1681" s="3" t="s">
         <v>253</v>
@@ -61482,7 +61482,7 @@
         <v>193</v>
       </c>
       <c r="E1681" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1681" s="3" t="s">
         <v>1285</v>
@@ -61504,7 +61504,7 @@
     </row>
     <row r="1682" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1682" s="3" t="s">
-        <v>1477</v>
+        <v>1476</v>
       </c>
       <c r="B1682" s="3" t="s">
         <v>149</v>
@@ -61516,7 +61516,7 @@
         <v>193</v>
       </c>
       <c r="E1682" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1682" s="3" t="s">
         <v>1285</v>
@@ -61538,7 +61538,7 @@
     </row>
     <row r="1683" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1683" s="3" t="s">
-        <v>1478</v>
+        <v>1477</v>
       </c>
       <c r="B1683" s="3" t="s">
         <v>253</v>
@@ -61550,7 +61550,7 @@
         <v>193</v>
       </c>
       <c r="E1683" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1683" s="3" t="s">
         <v>1285</v>
@@ -61572,7 +61572,7 @@
     </row>
     <row r="1684" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1684" s="3" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B1684" s="3" t="s">
         <v>253</v>
@@ -61584,7 +61584,7 @@
         <v>193</v>
       </c>
       <c r="E1684" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1684" s="3" t="s">
         <v>1285</v>
@@ -61606,7 +61606,7 @@
     </row>
     <row r="1685" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1685" s="3" t="s">
-        <v>1479</v>
+        <v>1478</v>
       </c>
       <c r="B1685" s="3" t="s">
         <v>209</v>
@@ -61618,7 +61618,7 @@
         <v>120</v>
       </c>
       <c r="E1685" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1685" s="3" t="s">
         <v>1285</v>
@@ -61640,7 +61640,7 @@
     </row>
     <row r="1686" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1686" s="3" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B1686" s="3" t="s">
         <v>179</v>
@@ -61652,7 +61652,7 @@
         <v>184</v>
       </c>
       <c r="E1686" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1686" s="3" t="s">
         <v>1285</v>
@@ -61674,7 +61674,7 @@
     </row>
     <row r="1687" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1687" s="3" t="s">
-        <v>1480</v>
+        <v>1479</v>
       </c>
       <c r="B1687" s="3" t="s">
         <v>241</v>
@@ -61686,7 +61686,7 @@
         <v>184</v>
       </c>
       <c r="E1687" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1687" s="3" t="s">
         <v>1285</v>
@@ -61708,7 +61708,7 @@
     </row>
     <row r="1688" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1688" s="3" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B1688" s="3" t="s">
         <v>179</v>
@@ -61720,7 +61720,7 @@
         <v>184</v>
       </c>
       <c r="E1688" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1688" s="3" t="s">
         <v>1285</v>
@@ -61742,7 +61742,7 @@
     </row>
     <row r="1689" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1689" s="3" t="s">
-        <v>1481</v>
+        <v>1480</v>
       </c>
       <c r="B1689" s="3" t="s">
         <v>132</v>
@@ -61754,7 +61754,7 @@
         <v>184</v>
       </c>
       <c r="E1689" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1689" s="3" t="s">
         <v>1285</v>
@@ -61776,7 +61776,7 @@
     </row>
     <row r="1690" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1690" s="3" t="s">
-        <v>1482</v>
+        <v>1481</v>
       </c>
       <c r="B1690" s="3" t="s">
         <v>355</v>
@@ -61788,7 +61788,7 @@
         <v>105</v>
       </c>
       <c r="E1690" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1690" s="3" t="s">
         <v>1285</v>
@@ -61810,7 +61810,7 @@
     </row>
     <row r="1691" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1691" s="3" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B1691" s="3" t="s">
         <v>253</v>
@@ -61822,7 +61822,7 @@
         <v>193</v>
       </c>
       <c r="E1691" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1691" s="3" t="s">
         <v>1285</v>
@@ -61844,7 +61844,7 @@
     </row>
     <row r="1692" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1692" s="3" t="s">
-        <v>1483</v>
+        <v>1482</v>
       </c>
       <c r="B1692" s="3" t="s">
         <v>157</v>
@@ -61876,7 +61876,7 @@
     </row>
     <row r="1693" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1693" s="3" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B1693" s="3" t="s">
         <v>249</v>
@@ -61888,7 +61888,7 @@
         <v>251</v>
       </c>
       <c r="E1693" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1693" s="3" t="s">
         <v>1285</v>
@@ -61910,7 +61910,7 @@
     </row>
     <row r="1694" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1694" s="3" t="s">
-        <v>1484</v>
+        <v>1483</v>
       </c>
       <c r="B1694" s="3" t="s">
         <v>171</v>
@@ -61922,7 +61922,7 @@
         <v>251</v>
       </c>
       <c r="E1694" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1694" s="3" t="s">
         <v>1285</v>
@@ -61944,7 +61944,7 @@
     </row>
     <row r="1695" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1695" s="3" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B1695" s="3" t="s">
         <v>200</v>
@@ -61976,7 +61976,7 @@
     </row>
     <row r="1696" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1696" s="3" t="s">
-        <v>1485</v>
+        <v>1484</v>
       </c>
       <c r="B1696" s="3" t="s">
         <v>150</v>
@@ -61988,7 +61988,7 @@
         <v>115</v>
       </c>
       <c r="E1696" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1696" s="3" t="s">
         <v>1285</v>
@@ -62010,7 +62010,7 @@
     </row>
     <row r="1697" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1697" s="3" t="s">
-        <v>1486</v>
+        <v>1485</v>
       </c>
       <c r="B1697" s="5" t="s">
         <v>200</v>
@@ -62022,7 +62022,7 @@
         <v>167</v>
       </c>
       <c r="E1697" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1697" s="3" t="s">
         <v>1285</v>
@@ -62044,7 +62044,7 @@
     </row>
     <row r="1698" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1698" s="3" t="s">
-        <v>1487</v>
+        <v>1486</v>
       </c>
       <c r="B1698" s="3" t="s">
         <v>329</v>
@@ -62056,7 +62056,7 @@
         <v>144</v>
       </c>
       <c r="E1698" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1698" s="3" t="s">
         <v>1285</v>
@@ -62078,7 +62078,7 @@
     </row>
     <row r="1699" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1699" s="3" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B1699" s="3" t="s">
         <v>248</v>
@@ -62090,7 +62090,7 @@
         <v>184</v>
       </c>
       <c r="E1699" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1699" s="3" t="s">
         <v>1285</v>
@@ -62112,7 +62112,7 @@
     </row>
     <row r="1700" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1700" s="3" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B1700" s="3" t="s">
         <v>219</v>
@@ -62124,7 +62124,7 @@
         <v>193</v>
       </c>
       <c r="E1700" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1700" s="3" t="s">
         <v>1285</v>
@@ -62146,7 +62146,7 @@
     </row>
     <row r="1701" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1701" s="3" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B1701" s="3" t="s">
         <v>196</v>
@@ -62158,7 +62158,7 @@
         <v>193</v>
       </c>
       <c r="E1701" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1701" s="3" t="s">
         <v>1285</v>
@@ -62180,7 +62180,7 @@
     </row>
     <row r="1702" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1702" s="3" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B1702" s="3" t="s">
         <v>157</v>
@@ -62192,7 +62192,7 @@
         <v>193</v>
       </c>
       <c r="E1702" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1702" s="3" t="s">
         <v>1285</v>
@@ -62214,7 +62214,7 @@
     </row>
     <row r="1703" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1703" s="3" t="s">
-        <v>1488</v>
+        <v>1487</v>
       </c>
       <c r="B1703" s="3" t="s">
         <v>114</v>
@@ -62226,7 +62226,7 @@
         <v>193</v>
       </c>
       <c r="E1703" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1703" s="3" t="s">
         <v>1285</v>
@@ -62248,7 +62248,7 @@
     </row>
     <row r="1704" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1704" s="3" t="s">
-        <v>1489</v>
+        <v>1488</v>
       </c>
       <c r="B1704" s="3" t="s">
         <v>248</v>
@@ -62260,7 +62260,7 @@
         <v>184</v>
       </c>
       <c r="E1704" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1704" s="3" t="s">
         <v>1285</v>
@@ -62282,7 +62282,7 @@
     </row>
     <row r="1705" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1705" s="3" t="s">
-        <v>1490</v>
+        <v>1489</v>
       </c>
       <c r="B1705" s="3" t="s">
         <v>154</v>
@@ -62294,7 +62294,7 @@
         <v>168</v>
       </c>
       <c r="E1705" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1705" s="3" t="s">
         <v>1285</v>
@@ -62316,7 +62316,7 @@
     </row>
     <row r="1706" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1706" s="3" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B1706" s="3" t="s">
         <v>338</v>
@@ -62328,7 +62328,7 @@
         <v>272</v>
       </c>
       <c r="E1706" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1706" s="3" t="s">
         <v>1285</v>
@@ -62350,7 +62350,7 @@
     </row>
     <row r="1707" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1707" s="3" t="s">
-        <v>1491</v>
+        <v>1490</v>
       </c>
       <c r="B1707" s="3" t="s">
         <v>161</v>
@@ -62362,7 +62362,7 @@
         <v>184</v>
       </c>
       <c r="E1707" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1707" s="3" t="s">
         <v>1285</v>
@@ -62384,7 +62384,7 @@
     </row>
     <row r="1708" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1708" s="3" t="s">
-        <v>1492</v>
+        <v>1491</v>
       </c>
       <c r="B1708" s="3" t="s">
         <v>248</v>
@@ -62396,7 +62396,7 @@
         <v>184</v>
       </c>
       <c r="E1708" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1708" s="3" t="s">
         <v>1285</v>
@@ -62418,7 +62418,7 @@
     </row>
     <row r="1709" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1709" s="3" t="s">
-        <v>1493</v>
+        <v>1492</v>
       </c>
       <c r="B1709" s="3" t="s">
         <v>219</v>
@@ -62430,7 +62430,7 @@
         <v>184</v>
       </c>
       <c r="E1709" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1709" s="3" t="s">
         <v>1285</v>
@@ -62452,7 +62452,7 @@
     </row>
     <row r="1710" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1710" s="3" t="s">
-        <v>1494</v>
+        <v>1493</v>
       </c>
       <c r="B1710" s="3" t="s">
         <v>355</v>
@@ -62464,7 +62464,7 @@
         <v>220</v>
       </c>
       <c r="E1710" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1710" s="3" t="s">
         <v>1285</v>
@@ -62486,7 +62486,7 @@
     </row>
     <row r="1711" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1711" s="3" t="s">
-        <v>1495</v>
+        <v>1494</v>
       </c>
       <c r="B1711" s="3" t="s">
         <v>209</v>
@@ -62498,7 +62498,7 @@
         <v>167</v>
       </c>
       <c r="E1711" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1711" s="3" t="s">
         <v>1285</v>
@@ -62520,7 +62520,7 @@
     </row>
     <row r="1712" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1712" s="3" t="s">
-        <v>1496</v>
+        <v>1495</v>
       </c>
       <c r="B1712" s="3" t="s">
         <v>340</v>
@@ -62532,7 +62532,7 @@
         <v>347</v>
       </c>
       <c r="E1712" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1712" s="3" t="s">
         <v>1285</v>
@@ -62554,7 +62554,7 @@
     </row>
     <row r="1713" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1713" s="3" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B1713" s="3" t="s">
         <v>202</v>
@@ -62566,7 +62566,7 @@
         <v>168</v>
       </c>
       <c r="E1713" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1713" s="3" t="s">
         <v>1285</v>
@@ -62588,7 +62588,7 @@
     </row>
     <row r="1714" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1714" s="3" t="s">
-        <v>1497</v>
+        <v>1496</v>
       </c>
       <c r="B1714" s="3" t="s">
         <v>171</v>
@@ -62600,7 +62600,7 @@
         <v>120</v>
       </c>
       <c r="E1714" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1714" s="3" t="s">
         <v>1285</v>
@@ -62622,10 +62622,10 @@
     </row>
     <row r="1715" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1715" s="3" t="s">
+        <v>1497</v>
+      </c>
+      <c r="B1715" s="3" t="s">
         <v>1498</v>
-      </c>
-      <c r="B1715" s="3" t="s">
-        <v>1499</v>
       </c>
       <c r="C1715" s="3" t="s">
         <v>249</v>
@@ -62634,7 +62634,7 @@
         <v>184</v>
       </c>
       <c r="E1715" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1715" s="3" t="s">
         <v>1285</v>
@@ -62656,7 +62656,7 @@
     </row>
     <row r="1716" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1716" s="3" t="s">
-        <v>1498</v>
+        <v>1497</v>
       </c>
       <c r="B1716" s="3" t="s">
         <v>171</v>
@@ -62668,7 +62668,7 @@
         <v>184</v>
       </c>
       <c r="E1716" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1716" s="3" t="s">
         <v>1285</v>
@@ -62690,7 +62690,7 @@
     </row>
     <row r="1717" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1717" s="3" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="B1717" s="3" t="s">
         <v>200</v>
@@ -62702,7 +62702,7 @@
         <v>105</v>
       </c>
       <c r="E1717" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1717" s="3" t="s">
         <v>1285</v>
@@ -62724,7 +62724,7 @@
     </row>
     <row r="1718" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1718" s="3" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="B1718" s="3" t="s">
         <v>160</v>
@@ -62736,7 +62736,7 @@
         <v>217</v>
       </c>
       <c r="E1718" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1718" s="3" t="s">
         <v>1285</v>
@@ -62758,7 +62758,7 @@
     </row>
     <row r="1719" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1719" s="3" t="s">
-        <v>1500</v>
+        <v>1499</v>
       </c>
       <c r="B1719" s="3" t="s">
         <v>196</v>
@@ -62770,7 +62770,7 @@
         <v>115</v>
       </c>
       <c r="E1719" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1719" s="3" t="s">
         <v>1285</v>
@@ -62792,7 +62792,7 @@
     </row>
     <row r="1720" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1720" s="3" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B1720" s="3" t="s">
         <v>329</v>
@@ -62804,7 +62804,7 @@
         <v>584</v>
       </c>
       <c r="E1720" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1720" s="3" t="s">
         <v>1285</v>
@@ -62826,7 +62826,7 @@
     </row>
     <row r="1721" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1721" s="3" t="s">
-        <v>1501</v>
+        <v>1500</v>
       </c>
       <c r="B1721" s="3" t="s">
         <v>119</v>
@@ -62838,7 +62838,7 @@
         <v>193</v>
       </c>
       <c r="E1721" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1721" s="3" t="s">
         <v>1285</v>
@@ -62860,7 +62860,7 @@
     </row>
     <row r="1722" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1722" s="3" t="s">
-        <v>1502</v>
+        <v>1501</v>
       </c>
       <c r="B1722" s="3" t="s">
         <v>114</v>
@@ -62872,7 +62872,7 @@
         <v>193</v>
       </c>
       <c r="E1722" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1722" s="3" t="s">
         <v>1285</v>
@@ -62894,7 +62894,7 @@
     </row>
     <row r="1723" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1723" s="3" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B1723" s="3" t="s">
         <v>331</v>
@@ -62906,7 +62906,7 @@
         <v>125</v>
       </c>
       <c r="E1723" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1723" s="3" t="s">
         <v>1285</v>
@@ -62928,7 +62928,7 @@
     </row>
     <row r="1724" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1724" s="3" t="s">
-        <v>1503</v>
+        <v>1502</v>
       </c>
       <c r="B1724" s="3" t="s">
         <v>242</v>
@@ -62940,7 +62940,7 @@
         <v>272</v>
       </c>
       <c r="E1724" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1724" s="3" t="s">
         <v>1285</v>
@@ -62962,7 +62962,7 @@
     </row>
     <row r="1725" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1725" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B1725" s="3" t="s">
         <v>287</v>
@@ -62974,7 +62974,7 @@
         <v>272</v>
       </c>
       <c r="E1725" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1725" s="3" t="s">
         <v>1285</v>
@@ -62996,7 +62996,7 @@
     </row>
     <row r="1726" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1726" s="3" t="s">
-        <v>1504</v>
+        <v>1503</v>
       </c>
       <c r="B1726" s="3" t="s">
         <v>149</v>
@@ -63008,7 +63008,7 @@
         <v>126</v>
       </c>
       <c r="E1726" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1726" s="3" t="s">
         <v>1285</v>
@@ -63030,7 +63030,7 @@
     </row>
     <row r="1727" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1727" s="3" t="s">
-        <v>1505</v>
+        <v>1504</v>
       </c>
       <c r="B1727" s="3" t="s">
         <v>359</v>
@@ -63042,7 +63042,7 @@
         <v>94</v>
       </c>
       <c r="E1727" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1727" s="3" t="s">
         <v>1285</v>
@@ -63064,7 +63064,7 @@
     </row>
     <row r="1728" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1728" s="3" t="s">
-        <v>1506</v>
+        <v>1505</v>
       </c>
       <c r="B1728" s="3" t="s">
         <v>248</v>
@@ -63076,7 +63076,7 @@
         <v>184</v>
       </c>
       <c r="E1728" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1728" s="3" t="s">
         <v>1285</v>
@@ -63098,7 +63098,7 @@
     </row>
     <row r="1729" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1729" s="3" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B1729" s="3" t="s">
         <v>248</v>
@@ -63110,7 +63110,7 @@
         <v>184</v>
       </c>
       <c r="E1729" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1729" s="3" t="s">
         <v>1285</v>
@@ -63132,7 +63132,7 @@
     </row>
     <row r="1730" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1730" s="3" t="s">
-        <v>1507</v>
+        <v>1506</v>
       </c>
       <c r="B1730" s="3" t="s">
         <v>171</v>
@@ -63144,7 +63144,7 @@
         <v>184</v>
       </c>
       <c r="E1730" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1730" s="3" t="s">
         <v>1285</v>
@@ -63166,7 +63166,7 @@
     </row>
     <row r="1731" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1731" s="3" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B1731" s="3" t="s">
         <v>359</v>
@@ -63178,7 +63178,7 @@
         <v>111</v>
       </c>
       <c r="E1731" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1731" s="3" t="s">
         <v>1285</v>
@@ -63200,7 +63200,7 @@
     </row>
     <row r="1732" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1732" s="3" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B1732" s="3" t="s">
         <v>375</v>
@@ -63212,7 +63212,7 @@
         <v>94</v>
       </c>
       <c r="E1732" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1732" s="3" t="s">
         <v>1285</v>
@@ -63234,7 +63234,7 @@
     </row>
     <row r="1733" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1733" s="3" t="s">
-        <v>1508</v>
+        <v>1507</v>
       </c>
       <c r="B1733" s="3" t="s">
         <v>174</v>
@@ -63246,7 +63246,7 @@
         <v>105</v>
       </c>
       <c r="E1733" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1733" s="3" t="s">
         <v>1285</v>
@@ -63268,7 +63268,7 @@
     </row>
     <row r="1734" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1734" s="3" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B1734" s="3" t="s">
         <v>564</v>
@@ -63280,7 +63280,7 @@
         <v>870</v>
       </c>
       <c r="E1734" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1734" s="3" t="s">
         <v>1285</v>
@@ -63302,7 +63302,7 @@
     </row>
     <row r="1735" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1735" s="3" t="s">
-        <v>1509</v>
+        <v>1508</v>
       </c>
       <c r="B1735" s="3" t="s">
         <v>154</v>
@@ -63314,7 +63314,7 @@
         <v>120</v>
       </c>
       <c r="E1735" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1735" s="3" t="s">
         <v>1285</v>
@@ -63336,7 +63336,7 @@
     </row>
     <row r="1736" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1736" s="3" t="s">
-        <v>1510</v>
+        <v>1509</v>
       </c>
       <c r="B1736" s="3" t="s">
         <v>287</v>
@@ -63348,7 +63348,7 @@
         <v>1051</v>
       </c>
       <c r="E1736" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1736" s="3" t="s">
         <v>1285</v>
@@ -63370,7 +63370,7 @@
     </row>
     <row r="1737" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1737" s="3" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B1737" s="3" t="s">
         <v>171</v>
@@ -63402,7 +63402,7 @@
     </row>
     <row r="1738" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1738" s="3" t="s">
-        <v>1511</v>
+        <v>1510</v>
       </c>
       <c r="B1738" s="3" t="s">
         <v>353</v>
@@ -63434,7 +63434,7 @@
     </row>
     <row r="1739" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1739" s="3" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B1739" s="3" t="s">
         <v>248</v>
@@ -63466,7 +63466,7 @@
     </row>
     <row r="1740" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1740" s="3" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B1740" s="3" t="s">
         <v>171</v>
@@ -63498,7 +63498,7 @@
     </row>
     <row r="1741" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1741" s="3" t="s">
-        <v>1512</v>
+        <v>1511</v>
       </c>
       <c r="B1741" s="3" t="s">
         <v>196</v>
@@ -63530,7 +63530,7 @@
     </row>
     <row r="1742" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1742" s="3" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B1742" s="3" t="s">
         <v>359</v>
@@ -63562,7 +63562,7 @@
     </row>
     <row r="1743" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1743" s="3" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B1743" s="3" t="s">
         <v>375</v>
@@ -63594,7 +63594,7 @@
     </row>
     <row r="1744" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1744" s="3" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B1744" s="3" t="s">
         <v>191</v>
@@ -63626,7 +63626,7 @@
     </row>
     <row r="1745" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1745" s="3" t="s">
-        <v>1513</v>
+        <v>1512</v>
       </c>
       <c r="B1745" s="3" t="s">
         <v>353</v>
@@ -63658,7 +63658,7 @@
     </row>
     <row r="1746" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1746" s="3" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B1746" s="3" t="s">
         <v>287</v>
@@ -63690,7 +63690,7 @@
     </row>
     <row r="1747" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1747" s="3" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B1747" s="3" t="s">
         <v>288</v>
@@ -63722,7 +63722,7 @@
     </row>
     <row r="1748" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1748" s="3" t="s">
-        <v>1514</v>
+        <v>1513</v>
       </c>
       <c r="B1748" s="3" t="s">
         <v>353</v>
@@ -63754,7 +63754,7 @@
     </row>
     <row r="1749" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1749" s="3" t="s">
-        <v>1515</v>
+        <v>1514</v>
       </c>
       <c r="B1749" s="3" t="s">
         <v>233</v>
@@ -63786,7 +63786,7 @@
     </row>
     <row r="1750" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1750" s="3" t="s">
-        <v>1516</v>
+        <v>1515</v>
       </c>
       <c r="B1750" s="3" t="s">
         <v>149</v>
@@ -63818,7 +63818,7 @@
     </row>
     <row r="1751" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1751" s="3" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B1751" s="3" t="s">
         <v>361</v>
@@ -63850,7 +63850,7 @@
     </row>
     <row r="1752" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1752" s="3" t="s">
-        <v>1517</v>
+        <v>1516</v>
       </c>
       <c r="B1752" s="3" t="s">
         <v>134</v>
@@ -63882,7 +63882,7 @@
     </row>
     <row r="1753" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1753" s="3" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B1753" s="3" t="s">
         <v>200</v>
@@ -63914,7 +63914,7 @@
     </row>
     <row r="1754" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1754" s="3" t="s">
-        <v>1518</v>
+        <v>1517</v>
       </c>
       <c r="B1754" s="3" t="s">
         <v>459</v>
@@ -63946,7 +63946,7 @@
     </row>
     <row r="1755" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1755" s="3" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B1755" s="3" t="s">
         <v>200</v>
@@ -63958,7 +63958,7 @@
         <v>870</v>
       </c>
       <c r="E1755" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1755" s="3" t="s">
         <v>1285</v>
@@ -63980,7 +63980,7 @@
     </row>
     <row r="1756" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1756" s="3" t="s">
-        <v>1519</v>
+        <v>1518</v>
       </c>
       <c r="B1756" s="3" t="s">
         <v>233</v>
@@ -64012,7 +64012,7 @@
     </row>
     <row r="1757" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1757" s="3" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="B1757" s="3" t="s">
         <v>253</v>
@@ -64044,7 +64044,7 @@
     </row>
     <row r="1758" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1758" s="3" t="s">
-        <v>1520</v>
+        <v>1519</v>
       </c>
       <c r="B1758" s="3" t="s">
         <v>149</v>
@@ -64076,7 +64076,7 @@
     </row>
     <row r="1759" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1759" s="3" t="s">
-        <v>1521</v>
+        <v>1520</v>
       </c>
       <c r="B1759" s="3" t="s">
         <v>253</v>
@@ -64108,7 +64108,7 @@
     </row>
     <row r="1760" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1760" s="3" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B1760" s="3" t="s">
         <v>202</v>
@@ -64120,7 +64120,7 @@
         <v>94</v>
       </c>
       <c r="E1760" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1760" s="3" t="s">
         <v>1285</v>
@@ -64142,7 +64142,7 @@
     </row>
     <row r="1761" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1761" s="3" t="s">
-        <v>1522</v>
+        <v>1521</v>
       </c>
       <c r="B1761" s="3" t="s">
         <v>154</v>
@@ -64154,7 +64154,7 @@
         <v>184</v>
       </c>
       <c r="E1761" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1761" s="3" t="s">
         <v>1285</v>
@@ -64176,7 +64176,7 @@
     </row>
     <row r="1762" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1762" s="3" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B1762" s="3" t="s">
         <v>202</v>
@@ -64188,7 +64188,7 @@
         <v>220</v>
       </c>
       <c r="E1762" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1762" s="3" t="s">
         <v>1285</v>
@@ -64210,7 +64210,7 @@
     </row>
     <row r="1763" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1763" s="3" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B1763" s="3" t="s">
         <v>209</v>
@@ -64222,7 +64222,7 @@
         <v>111</v>
       </c>
       <c r="E1763" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1763" s="3" t="s">
         <v>1285</v>
@@ -64244,7 +64244,7 @@
     </row>
     <row r="1764" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1764" s="3" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B1764" s="3" t="s">
         <v>119</v>
@@ -64256,7 +64256,7 @@
         <v>220</v>
       </c>
       <c r="E1764" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1764" s="3" t="s">
         <v>1285</v>
@@ -64278,7 +64278,7 @@
     </row>
     <row r="1765" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1765" s="3" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B1765" s="3" t="s">
         <v>124</v>
@@ -64290,7 +64290,7 @@
         <v>193</v>
       </c>
       <c r="E1765" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1765" s="3" t="s">
         <v>1285</v>
@@ -64312,7 +64312,7 @@
     </row>
     <row r="1766" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1766" s="3" t="s">
-        <v>1523</v>
+        <v>1522</v>
       </c>
       <c r="B1766" s="3" t="s">
         <v>135</v>
@@ -64324,7 +64324,7 @@
         <v>115</v>
       </c>
       <c r="E1766" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1766" s="3" t="s">
         <v>1285</v>
@@ -64346,7 +64346,7 @@
     </row>
     <row r="1767" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1767" s="3" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B1767" s="3" t="s">
         <v>355</v>
@@ -64358,7 +64358,7 @@
         <v>9</v>
       </c>
       <c r="E1767" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1767" s="3" t="s">
         <v>1285</v>
@@ -64380,7 +64380,7 @@
     </row>
     <row r="1768" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1768" s="3" t="s">
-        <v>1524</v>
+        <v>1523</v>
       </c>
       <c r="B1768" s="3" t="s">
         <v>124</v>
@@ -64392,7 +64392,7 @@
         <v>251</v>
       </c>
       <c r="E1768" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1768" s="3" t="s">
         <v>1285</v>
@@ -64414,7 +64414,7 @@
     </row>
     <row r="1769" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1769" s="3" t="s">
-        <v>1525</v>
+        <v>1524</v>
       </c>
       <c r="B1769" s="3" t="s">
         <v>331</v>
@@ -64426,7 +64426,7 @@
         <v>9</v>
       </c>
       <c r="E1769" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1769" s="3" t="s">
         <v>1285</v>
@@ -64448,7 +64448,7 @@
     </row>
     <row r="1770" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1770" s="3" t="s">
-        <v>1526</v>
+        <v>1525</v>
       </c>
       <c r="B1770" s="3" t="s">
         <v>209</v>
@@ -64460,7 +64460,7 @@
         <v>167</v>
       </c>
       <c r="E1770" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1770" s="3" t="s">
         <v>1285</v>
@@ -64482,7 +64482,7 @@
     </row>
     <row r="1771" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1771" s="3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B1771" s="3" t="s">
         <v>132</v>
@@ -64494,7 +64494,7 @@
         <v>875</v>
       </c>
       <c r="E1771" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1771" s="3" t="s">
         <v>1285</v>
@@ -64516,7 +64516,7 @@
     </row>
     <row r="1772" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1772" s="3" t="s">
-        <v>1527</v>
+        <v>1526</v>
       </c>
       <c r="B1772" s="3" t="s">
         <v>353</v>
@@ -64528,7 +64528,7 @@
         <v>136</v>
       </c>
       <c r="E1772" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1772" s="3" t="s">
         <v>1285</v>
@@ -64550,7 +64550,7 @@
     </row>
     <row r="1773" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1773" s="3" t="s">
-        <v>1528</v>
+        <v>1527</v>
       </c>
       <c r="B1773" s="3" t="s">
         <v>288</v>
@@ -64562,7 +64562,7 @@
         <v>272</v>
       </c>
       <c r="E1773" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1773" s="3" t="s">
         <v>1285</v>
@@ -64584,7 +64584,7 @@
     </row>
     <row r="1774" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1774" s="3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B1774" s="3" t="s">
         <v>241</v>
@@ -64596,7 +64596,7 @@
         <v>136</v>
       </c>
       <c r="E1774" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1774" s="3" t="s">
         <v>1285</v>
@@ -64618,7 +64618,7 @@
     </row>
     <row r="1775" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1775" s="3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B1775" s="3" t="s">
         <v>160</v>
@@ -64630,7 +64630,7 @@
         <v>136</v>
       </c>
       <c r="E1775" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1775" s="3" t="s">
         <v>1285</v>
@@ -64652,7 +64652,7 @@
     </row>
     <row r="1776" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1776" s="3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B1776" s="3" t="s">
         <v>134</v>
@@ -64664,7 +64664,7 @@
         <v>105</v>
       </c>
       <c r="E1776" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1776" s="3" t="s">
         <v>1285</v>
@@ -64686,7 +64686,7 @@
     </row>
     <row r="1777" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1777" s="3" t="s">
-        <v>1529</v>
+        <v>1528</v>
       </c>
       <c r="B1777" s="3" t="s">
         <v>203</v>
@@ -64698,7 +64698,7 @@
         <v>115</v>
       </c>
       <c r="E1777" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1777" s="3" t="s">
         <v>1285</v>
@@ -64720,7 +64720,7 @@
     </row>
     <row r="1778" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1778" s="3" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B1778" s="3" t="s">
         <v>133</v>
@@ -64732,7 +64732,7 @@
         <v>870</v>
       </c>
       <c r="E1778" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1778" s="3" t="s">
         <v>1285</v>
@@ -64754,7 +64754,7 @@
     </row>
     <row r="1779" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1779" s="3" t="s">
-        <v>1530</v>
+        <v>1529</v>
       </c>
       <c r="B1779" s="3" t="s">
         <v>124</v>
@@ -64766,7 +64766,7 @@
         <v>217</v>
       </c>
       <c r="E1779" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1779" s="3" t="s">
         <v>1285</v>
@@ -64788,7 +64788,7 @@
     </row>
     <row r="1780" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1780" s="3" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B1780" s="3" t="s">
         <v>336</v>
@@ -64800,7 +64800,7 @@
         <v>1305</v>
       </c>
       <c r="E1780" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1780" s="3" t="s">
         <v>1285</v>
@@ -64822,7 +64822,7 @@
     </row>
     <row r="1781" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1781" s="3" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B1781" s="3" t="s">
         <v>157</v>
@@ -64834,7 +64834,7 @@
         <v>105</v>
       </c>
       <c r="E1781" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1781" s="3" t="s">
         <v>1285</v>
@@ -64856,7 +64856,7 @@
     </row>
     <row r="1782" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1782" s="3" t="s">
-        <v>1531</v>
+        <v>1530</v>
       </c>
       <c r="B1782" s="3" t="s">
         <v>304</v>
@@ -64868,7 +64868,7 @@
         <v>115</v>
       </c>
       <c r="E1782" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1782" s="3" t="s">
         <v>1285</v>
@@ -64890,7 +64890,7 @@
     </row>
     <row r="1783" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1783" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B1783" s="3" t="s">
         <v>200</v>
@@ -64902,7 +64902,7 @@
         <v>94</v>
       </c>
       <c r="E1783" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1783" s="3" t="s">
         <v>1285</v>
@@ -64924,7 +64924,7 @@
     </row>
     <row r="1784" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1784" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B1784" s="3" t="s">
         <v>191</v>
@@ -64936,7 +64936,7 @@
         <v>193</v>
       </c>
       <c r="E1784" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1784" s="3" t="s">
         <v>1285</v>
@@ -64958,7 +64958,7 @@
     </row>
     <row r="1785" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1785" s="3" t="s">
-        <v>1532</v>
+        <v>1531</v>
       </c>
       <c r="B1785" s="3" t="s">
         <v>387</v>
@@ -64970,7 +64970,7 @@
         <v>220</v>
       </c>
       <c r="E1785" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1785" s="3" t="s">
         <v>1285</v>
@@ -64992,7 +64992,7 @@
     </row>
     <row r="1786" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1786" s="3" t="s">
-        <v>1533</v>
+        <v>1532</v>
       </c>
       <c r="B1786" s="3" t="s">
         <v>459</v>
@@ -65004,7 +65004,7 @@
         <v>272</v>
       </c>
       <c r="E1786" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1786" s="3" t="s">
         <v>1285</v>
@@ -65026,7 +65026,7 @@
     </row>
     <row r="1787" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1787" s="3" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B1787" s="3" t="s">
         <v>160</v>
@@ -65038,7 +65038,7 @@
         <v>239</v>
       </c>
       <c r="E1787" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1787" s="3" t="s">
         <v>1285</v>
@@ -65060,7 +65060,7 @@
     </row>
     <row r="1788" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1788" s="3" t="s">
-        <v>1534</v>
+        <v>1533</v>
       </c>
       <c r="B1788" s="3" t="s">
         <v>203</v>
@@ -65072,7 +65072,7 @@
         <v>115</v>
       </c>
       <c r="E1788" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1788" s="3" t="s">
         <v>1285</v>
@@ -65094,7 +65094,7 @@
     </row>
     <row r="1789" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1789" s="3" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B1789" s="3" t="s">
         <v>209</v>
@@ -65106,7 +65106,7 @@
         <v>167</v>
       </c>
       <c r="E1789" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1789" s="3" t="s">
         <v>1285</v>
@@ -65128,7 +65128,7 @@
     </row>
     <row r="1790" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1790" s="3" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B1790" s="3" t="s">
         <v>114</v>
@@ -65140,7 +65140,7 @@
         <v>126</v>
       </c>
       <c r="E1790" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1790" s="3" t="s">
         <v>1285</v>
@@ -65162,7 +65162,7 @@
     </row>
     <row r="1791" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1791" s="3" t="s">
-        <v>1535</v>
+        <v>1534</v>
       </c>
       <c r="B1791" s="3" t="s">
         <v>271</v>
@@ -65174,7 +65174,7 @@
         <v>105</v>
       </c>
       <c r="E1791" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1791" s="3" t="s">
         <v>1285</v>
@@ -65196,7 +65196,7 @@
     </row>
     <row r="1792" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1792" s="3" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="B1792" s="3" t="s">
         <v>340</v>
@@ -65208,7 +65208,7 @@
         <v>875</v>
       </c>
       <c r="E1792" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1792" s="3" t="s">
         <v>1285</v>
@@ -65230,7 +65230,7 @@
     </row>
     <row r="1793" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1793" s="3" t="s">
-        <v>1536</v>
+        <v>1535</v>
       </c>
       <c r="B1793" s="3" t="s">
         <v>114</v>
@@ -65242,7 +65242,7 @@
         <v>105</v>
       </c>
       <c r="E1793" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1793" s="3" t="s">
         <v>1285</v>
@@ -65264,7 +65264,7 @@
     </row>
     <row r="1794" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1794" s="3" t="s">
-        <v>1537</v>
+        <v>1536</v>
       </c>
       <c r="B1794" s="3" t="s">
         <v>122</v>
@@ -65276,7 +65276,7 @@
         <v>389</v>
       </c>
       <c r="E1794" s="3" t="s">
-        <v>1463</v>
+        <v>1548</v>
       </c>
       <c r="F1794" s="3" t="s">
         <v>1285</v>
@@ -65298,7 +65298,7 @@
     </row>
     <row r="1795" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1795" s="3" t="s">
-        <v>1538</v>
+        <v>1537</v>
       </c>
       <c r="B1795" s="3" t="s">
         <v>200</v>
@@ -65332,7 +65332,7 @@
     </row>
     <row r="1796" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1796" s="3" t="s">
-        <v>1539</v>
+        <v>1538</v>
       </c>
       <c r="B1796" s="3" t="s">
         <v>210</v>
@@ -65347,7 +65347,7 @@
         <v>127</v>
       </c>
       <c r="F1796" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1796" s="8" t="s">
         <v>279</v>
@@ -65366,7 +65366,7 @@
     </row>
     <row r="1797" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1797" s="3" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B1797" s="3" t="s">
         <v>336</v>
@@ -65381,7 +65381,7 @@
         <v>127</v>
       </c>
       <c r="F1797" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1797" s="8" t="s">
         <v>279</v>
@@ -65400,7 +65400,7 @@
     </row>
     <row r="1798" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1798" s="3" t="s">
-        <v>1541</v>
+        <v>1540</v>
       </c>
       <c r="B1798" s="3" t="s">
         <v>135</v>
@@ -65415,7 +65415,7 @@
         <v>127</v>
       </c>
       <c r="F1798" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1798" s="8" t="s">
         <v>279</v>
@@ -65434,7 +65434,7 @@
     </row>
     <row r="1799" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1799" s="3" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B1799" s="3" t="s">
         <v>361</v>
@@ -65449,7 +65449,7 @@
         <v>127</v>
       </c>
       <c r="F1799" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1799" s="8" t="s">
         <v>279</v>
@@ -65468,7 +65468,7 @@
     </row>
     <row r="1800" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1800" s="3" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B1800" s="3" t="s">
         <v>119</v>
@@ -65483,7 +65483,7 @@
         <v>127</v>
       </c>
       <c r="F1800" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1800" s="8" t="s">
         <v>279</v>
@@ -65502,7 +65502,7 @@
     </row>
     <row r="1801" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1801" s="3" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B1801" s="3" t="s">
         <v>285</v>
@@ -65517,7 +65517,7 @@
         <v>127</v>
       </c>
       <c r="F1801" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1801" s="8" t="s">
         <v>279</v>
@@ -65536,7 +65536,7 @@
     </row>
     <row r="1802" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1802" s="3" t="s">
-        <v>1542</v>
+        <v>1541</v>
       </c>
       <c r="B1802" s="3" t="s">
         <v>147</v>
@@ -65551,7 +65551,7 @@
         <v>127</v>
       </c>
       <c r="F1802" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1802" s="8" t="s">
         <v>279</v>
@@ -65570,7 +65570,7 @@
     </row>
     <row r="1803" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1803" s="3" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B1803" s="3" t="s">
         <v>288</v>
@@ -65579,13 +65579,13 @@
         <v>124</v>
       </c>
       <c r="D1803" s="3" t="s">
-        <v>1544</v>
+        <v>1543</v>
       </c>
       <c r="E1803" s="3" t="s">
         <v>127</v>
       </c>
       <c r="F1803" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1803" s="8" t="s">
         <v>279</v>
@@ -65604,7 +65604,7 @@
     </row>
     <row r="1804" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1804" s="3" t="s">
-        <v>1543</v>
+        <v>1542</v>
       </c>
       <c r="B1804" s="3" t="s">
         <v>203</v>
@@ -65619,7 +65619,7 @@
         <v>127</v>
       </c>
       <c r="F1804" s="3" t="s">
-        <v>1540</v>
+        <v>1539</v>
       </c>
       <c r="G1804" s="8" t="s">
         <v>279</v>
@@ -65638,7 +65638,7 @@
     </row>
     <row r="1805" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1805" s="3" t="s">
-        <v>1545</v>
+        <v>1544</v>
       </c>
       <c r="B1805" s="3" t="s">
         <v>150</v>
@@ -65653,7 +65653,7 @@
         <v>127</v>
       </c>
       <c r="F1805" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G1805" s="8" t="s">
         <v>279</v>
@@ -65672,7 +65672,7 @@
     </row>
     <row r="1806" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1806" s="3" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="B1806" s="3" t="s">
         <v>160</v>
@@ -65687,7 +65687,7 @@
         <v>127</v>
       </c>
       <c r="F1806" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G1806" s="8" t="s">
         <v>279</v>
@@ -65706,7 +65706,7 @@
     </row>
     <row r="1807" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1807" s="3" t="s">
-        <v>1547</v>
+        <v>1546</v>
       </c>
       <c r="B1807" s="3" t="s">
         <v>353</v>
@@ -65721,7 +65721,7 @@
         <v>127</v>
       </c>
       <c r="F1807" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G1807" s="8" t="s">
         <v>279</v>
@@ -65740,7 +65740,7 @@
     </row>
     <row r="1808" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1808" s="3" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B1808" s="3" t="s">
         <v>288</v>
@@ -65755,7 +65755,7 @@
         <v>127</v>
       </c>
       <c r="F1808" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G1808" s="8" t="s">
         <v>279</v>
@@ -65774,7 +65774,7 @@
     </row>
     <row r="1809" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1809" s="3" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B1809" s="3" t="s">
         <v>233</v>
@@ -65789,7 +65789,7 @@
         <v>127</v>
       </c>
       <c r="F1809" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G1809" s="8" t="s">
         <v>279</v>
@@ -65808,7 +65808,7 @@
     </row>
     <row r="1810" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1810" s="3" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
       <c r="B1810" s="3" t="s">
         <v>304</v>
@@ -65823,7 +65823,7 @@
         <v>127</v>
       </c>
       <c r="F1810" s="3" t="s">
-        <v>1546</v>
+        <v>1545</v>
       </c>
       <c r="G1810" s="8" t="s">
         <v>279</v>

</xml_diff>

<commit_message>
#56 Time Tracking: updated to 2025-12-28.
</commit_message>
<xml_diff>
--- a/data/Time Tracking.xlsx
+++ b/data/Time Tracking.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14082" uniqueCount="1549">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14106" uniqueCount="1551">
   <si>
     <t>Year</t>
   </si>
@@ -4672,6 +4672,12 @@
   </si>
   <si>
     <t>#asciidoc</t>
+  </si>
+  <si>
+    <t>2025-12-27</t>
+  </si>
+  <si>
+    <t>2025-12-28</t>
   </si>
 </sst>
 </file>
@@ -5083,8 +5089,8 @@
   <dimension ref="A1:J1841"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1779" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1811" sqref="C1811"/>
+      <pane ySplit="1" topLeftCell="A1794" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H1817" sqref="H1817"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12" x14ac:dyDescent="0.2"/>
@@ -65841,40 +65847,106 @@
       </c>
     </row>
     <row r="1811" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1811" s="3"/>
-      <c r="B1811" s="3"/>
-      <c r="C1811" s="3"/>
-      <c r="D1811" s="3"/>
-      <c r="E1811" s="3"/>
-      <c r="F1811" s="3"/>
-      <c r="G1811" s="3"/>
-      <c r="H1811" s="3"/>
-      <c r="I1811" s="4"/>
-      <c r="J1811" s="4"/>
+      <c r="A1811" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B1811" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1811" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="D1811" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="E1811" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1811" s="3" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G1811" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1811" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1811" s="4">
+        <f t="shared" ref="I1811:I1812" si="776">YEAR(A1811)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1811" s="4">
+        <f t="shared" ref="J1811:J1812" si="777">MONTH(A1811)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1812" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1812" s="3"/>
-      <c r="B1812" s="3"/>
-      <c r="C1812" s="3"/>
-      <c r="D1812" s="3"/>
-      <c r="E1812" s="3"/>
-      <c r="F1812" s="3"/>
-      <c r="G1812" s="3"/>
-      <c r="H1812" s="3"/>
-      <c r="I1812" s="4"/>
-      <c r="J1812" s="4"/>
+      <c r="A1812" s="3" t="s">
+        <v>1549</v>
+      </c>
+      <c r="B1812" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C1812" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D1812" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1812" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1812" s="3" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G1812" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1812" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="I1812" s="4">
+        <f t="shared" si="776"/>
+        <v>2025</v>
+      </c>
+      <c r="J1812" s="4">
+        <f t="shared" si="777"/>
+        <v>12</v>
+      </c>
     </row>
     <row r="1813" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1813" s="3"/>
-      <c r="B1813" s="3"/>
-      <c r="C1813" s="3"/>
-      <c r="D1813" s="3"/>
-      <c r="E1813" s="3"/>
-      <c r="F1813" s="3"/>
-      <c r="G1813" s="3"/>
-      <c r="H1813" s="3"/>
-      <c r="I1813" s="4"/>
-      <c r="J1813" s="4"/>
+      <c r="A1813" s="3" t="s">
+        <v>1550</v>
+      </c>
+      <c r="B1813" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C1813" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D1813" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E1813" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F1813" s="3" t="s">
+        <v>1545</v>
+      </c>
+      <c r="G1813" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="H1813" s="8" t="s">
+        <v>279</v>
+      </c>
+      <c r="I1813" s="4">
+        <f t="shared" ref="I1813" si="778">YEAR(A1813)</f>
+        <v>2025</v>
+      </c>
+      <c r="J1813" s="4">
+        <f t="shared" ref="J1813" si="779">MONTH(A1813)</f>
+        <v>12</v>
+      </c>
     </row>
     <row r="1814" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1814" s="3"/>

</xml_diff>